<commit_message>
Rerunning 2023_TM152_IPA_15; updated param slightly
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\travel-model-one-v1.6_develop\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5AE300A-36FC-43DD-B4E6-EA69B6A725E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4B7AAFD-CF9C-4F38-A535-8256408D4B0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="795" windowWidth="21600" windowHeight="10440" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
+    <workbookView xWindow="1080" yWindow="2730" windowWidth="21600" windowHeight="10440" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelRuns" sheetId="1" r:id="rId1"/>
@@ -347,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -378,7 +378,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -696,7 +695,7 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1500,7 +1499,7 @@
       <c r="J18" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="K18" s="14" t="s">
+      <c r="K18" s="3" t="s">
         <v>69</v>
       </c>
       <c r="L18" s="8">
@@ -1510,7 +1509,7 @@
         <v>-0.75</v>
       </c>
       <c r="N18" s="9">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="O18" s="9">
         <v>0</v>

</xml_diff>

<commit_message>
Reframe "Sharing preferences adjustment" as "Transit Hesitance"
This is mostly renaming but it also included removing the application of these constants to TNC modes
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\travel-model-one-v1.6_develop\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4B7AAFD-CF9C-4F38-A535-8256408D4B0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E2DDD83-F897-4B62-9BE0-9B1633DC092E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="2730" windowWidth="21600" windowHeight="10440" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
+    <workbookView xWindow="2070" yWindow="2130" windowWidth="32115" windowHeight="16455" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelRuns" sheetId="1" r:id="rId1"/>
@@ -158,12 +158,6 @@
     <t>Telecommute_constant_PT</t>
   </si>
   <si>
-    <t>Work_Sharing_Pref_Factor</t>
-  </si>
-  <si>
-    <t>NonWork_Sharing_Pref_Factor</t>
-  </si>
-  <si>
     <t>2023_TM152_IPA_05</t>
   </si>
   <si>
@@ -255,6 +249,12 @@
   </si>
   <si>
     <t>2023_TM152_IPA_15</t>
+  </si>
+  <si>
+    <t>Work_Transit_Hesitance</t>
+  </si>
+  <si>
+    <t>NonWork_Transit_Hesitance</t>
   </si>
 </sst>
 </file>
@@ -695,7 +695,7 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -714,7 +714,7 @@
     <col min="12" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="7" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="7" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -755,10 +755,10 @@
         <v>39</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -1033,7 +1033,7 @@
         <v>2023</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>18</v>
@@ -1042,7 +1042,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>10</v>
@@ -1054,10 +1054,10 @@
         <v>33</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L8" s="8">
         <v>-1.25</v>
@@ -1077,7 +1077,7 @@
         <v>2023</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>18</v>
@@ -1086,7 +1086,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>10</v>
@@ -1098,10 +1098,10 @@
         <v>33</v>
       </c>
       <c r="J9" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="K9" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="L9" s="8">
         <v>-1.25</v>
@@ -1121,7 +1121,7 @@
         <v>2023</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>18</v>
@@ -1130,7 +1130,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>10</v>
@@ -1142,10 +1142,10 @@
         <v>33</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L10" s="8">
         <v>-1.25</v>
@@ -1165,31 +1165,31 @@
         <v>2023</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="3" t="s">
+      <c r="J11" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="K11" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="L11" s="8">
         <v>-1.25</v>
@@ -1209,31 +1209,31 @@
         <v>2023</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="J12" s="12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L12" s="8">
         <v>-1.25</v>
@@ -1253,31 +1253,31 @@
         <v>2023</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="K13" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="J13" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="L13" s="8">
         <v>-1.25</v>
@@ -1297,31 +1297,31 @@
         <v>2023</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="3" t="s">
+      <c r="J14" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="K14" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="J14" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="L14" s="8">
         <v>-1.25</v>
@@ -1341,7 +1341,7 @@
         <v>2023</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>18</v>
@@ -1350,22 +1350,22 @@
         <v>7</v>
       </c>
       <c r="E15" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J15" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="K15" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="J15" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="L15" s="8">
         <v>-1.25</v>
@@ -1385,7 +1385,7 @@
         <v>2023</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>18</v>
@@ -1394,22 +1394,22 @@
         <v>7</v>
       </c>
       <c r="E16" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="K16" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="J16" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="L16" s="8">
         <v>-1.25</v>
@@ -1429,7 +1429,7 @@
         <v>2023</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>18</v>
@@ -1438,22 +1438,22 @@
         <v>7</v>
       </c>
       <c r="E17" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="K17" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="J17" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="L17" s="8">
         <v>-1.25</v>
@@ -1473,7 +1473,7 @@
         <v>2023</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>18</v>
@@ -1482,7 +1482,7 @@
         <v>7</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>10</v>
@@ -1494,13 +1494,13 @@
         <v>12</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J18" s="12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L18" s="8">
         <v>-1.25</v>

</xml_diff>

<commit_message>
added 5 runs to the model run log
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\travel-model-one-v1.6_develop\utilities\RTP\config_RTP2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB2AD889-F1A0-4C3A-936A-AFFE3E3EB1CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8343B26F-7C1E-4919-8E81-D255224121B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6075" yWindow="2340" windowWidth="28800" windowHeight="11385" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelRuns" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="115">
   <si>
     <t>year</t>
   </si>
@@ -321,6 +321,66 @@
   </si>
   <si>
     <t>https://app.asana.com/0/1204085012544660/1205470723787170/f</t>
+  </si>
+  <si>
+    <t>2023_TM160_IPA_20</t>
+  </si>
+  <si>
+    <t>2023_TM160_IPA_21</t>
+  </si>
+  <si>
+    <t>Set WFH factors to be 0.5x of v19's</t>
+  </si>
+  <si>
+    <t>Set WFH factors to be 0.75x of v19's</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1205555270932662/f</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1205555270932665/f</t>
+  </si>
+  <si>
+    <t>2035_TM160_IPA_01</t>
+  </si>
+  <si>
+    <t>2035_TM160_IPA_02</t>
+  </si>
+  <si>
+    <t>2035_TM160_IPA_03</t>
+  </si>
+  <si>
+    <t>Future year</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1205533462992294/f</t>
+  </si>
+  <si>
+    <t>M:\Application\Model One\RTP2021\Blueprint\INPUT_DEVELOPMENT\Networks\BlueprintNetworks_64\net_2035_Blueprint_tollscsv</t>
+  </si>
+  <si>
+    <t>Initial 2035 IPA run with PBA50 AOC, WFH &amp; trn hesistance from 2023 v19</t>
+  </si>
+  <si>
+    <t>Same as v1 but with draft PBA50+ AOC</t>
+  </si>
+  <si>
+    <t>Same as v2 but with trn hesistance set to 0</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1205555270932668/f</t>
+  </si>
+  <si>
+    <t>model3-a</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>model2-c</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1205555270932675/f</t>
   </si>
 </sst>
 </file>
@@ -413,7 +473,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -444,7 +504,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -759,30 +818,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9564CC59-3725-4FDA-8BF2-0F68CB1B6F5A}">
-  <dimension ref="A1:R25"/>
+  <dimension ref="A1:R30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
+      <selection pane="bottomLeft" activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="6.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.140625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" style="12" customWidth="1"/>
-    <col min="11" max="11" width="17.5703125" style="3" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="3"/>
+    <col min="2" max="2" width="17.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="28.6328125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="11.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.1796875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="6.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.1796875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="11.26953125" style="12" customWidth="1"/>
+    <col min="11" max="11" width="17.54296875" style="3" customWidth="1"/>
+    <col min="12" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="7" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="7" customFormat="1" ht="39" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -838,7 +897,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>2015</v>
       </c>
@@ -887,7 +946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2023</v>
       </c>
@@ -933,7 +992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>2023</v>
       </c>
@@ -979,7 +1038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>2023</v>
       </c>
@@ -1025,7 +1084,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>2023</v>
       </c>
@@ -1071,7 +1130,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>2023</v>
       </c>
@@ -1117,7 +1176,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>2023</v>
       </c>
@@ -1163,7 +1222,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>2023</v>
       </c>
@@ -1209,7 +1268,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>2023</v>
       </c>
@@ -1255,7 +1314,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>2023</v>
       </c>
@@ -1301,7 +1360,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>2023</v>
       </c>
@@ -1347,7 +1406,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>2023</v>
       </c>
@@ -1393,7 +1452,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>2023</v>
       </c>
@@ -1439,7 +1498,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>2023</v>
       </c>
@@ -1485,7 +1544,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>2023</v>
       </c>
@@ -1531,7 +1590,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>2023</v>
       </c>
@@ -1577,7 +1636,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>2023</v>
       </c>
@@ -1623,7 +1682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>2023</v>
       </c>
@@ -1669,7 +1728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>2023</v>
       </c>
@@ -1715,7 +1774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>2023</v>
       </c>
@@ -1759,7 +1818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>2023</v>
       </c>
@@ -1808,7 +1867,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>2023</v>
       </c>
@@ -1855,7 +1914,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>2023</v>
       </c>
@@ -1886,7 +1945,7 @@
       <c r="J24" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="K24" s="14" t="s">
+      <c r="K24" s="3" t="s">
         <v>94</v>
       </c>
       <c r="L24" s="8">
@@ -1905,7 +1964,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>2023</v>
       </c>
@@ -1936,8 +1995,14 @@
       <c r="J25" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="K25" s="14" t="s">
+      <c r="K25" s="3" t="s">
         <v>94</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M25" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="N25" s="8">
         <v>1.27</v>
@@ -1953,6 +2018,286 @@
       </c>
       <c r="R25" s="9">
         <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>2023</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="J26" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M26" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="N26" s="3">
+        <v>0.64</v>
+      </c>
+      <c r="O26" s="3">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="P26" s="9">
+        <v>120</v>
+      </c>
+      <c r="Q26" s="9">
+        <v>0</v>
+      </c>
+      <c r="R26" s="9">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
+        <v>2023</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="J27" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="L27" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M27" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="N27" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="O27" s="3">
+        <v>0.86</v>
+      </c>
+      <c r="P27" s="9">
+        <v>120</v>
+      </c>
+      <c r="Q27" s="9">
+        <v>0</v>
+      </c>
+      <c r="R27" s="9">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <v>2035</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="J28" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M28" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="N28" s="8">
+        <v>1.27</v>
+      </c>
+      <c r="O28" s="8">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="P28" s="9">
+        <v>120</v>
+      </c>
+      <c r="Q28" s="9">
+        <v>0</v>
+      </c>
+      <c r="R28" s="9">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
+        <v>2035</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="J29" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M29" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="N29" s="8">
+        <v>1.27</v>
+      </c>
+      <c r="O29" s="8">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="P29" s="9">
+        <v>120</v>
+      </c>
+      <c r="Q29" s="9">
+        <v>0</v>
+      </c>
+      <c r="R29" s="9">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
+        <v>2035</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="J30" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M30" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="N30" s="8">
+        <v>1.27</v>
+      </c>
+      <c r="O30" s="8">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="P30" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="9">
+        <v>0</v>
+      </c>
+      <c r="R30" s="9">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added 2035 from RTP2021 to the model run log; also added a AOC column
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-v1.6_develop\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8343B26F-7C1E-4919-8E81-D255224121B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8AA8DDB-2306-40A1-8A47-615995AC8840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="123">
   <si>
     <t>year</t>
   </si>
@@ -381,6 +381,30 @@
   </si>
   <si>
     <t>https://app.asana.com/0/1204085012544660/1205555270932675/f</t>
+  </si>
+  <si>
+    <t>2035_TM152_FBP_Plus_24</t>
+  </si>
+  <si>
+    <t>RTP2021</t>
+  </si>
+  <si>
+    <t>Plan</t>
+  </si>
+  <si>
+    <t>RTP21 adopted run</t>
+  </si>
+  <si>
+    <t>M:\Application\Model One\RTP2021\Blueprint\INPUT_DEVELOPMENT\Networks\BlueprintNetworks_64\net_2035_Blueprint</t>
+  </si>
+  <si>
+    <t>run182</t>
+  </si>
+  <si>
+    <t>"Final Blueprint runs\Final Blueprint (s24)\BAUS v2.25 - FINAL VERSION"</t>
+  </si>
+  <si>
+    <t>AOC_CentsPerMile</t>
   </si>
 </sst>
 </file>
@@ -429,7 +453,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -439,6 +463,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -473,7 +509,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -504,6 +540,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -818,17 +872,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9564CC59-3725-4FDA-8BF2-0F68CB1B6F5A}">
-  <dimension ref="A1:R30"/>
+  <dimension ref="A1:S31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I34" sqref="I34"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.1796875" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.81640625" style="3" customWidth="1"/>
     <col min="4" max="4" width="9.81640625" style="3" customWidth="1"/>
     <col min="5" max="5" width="28.6328125" style="3" customWidth="1"/>
@@ -838,10 +892,11 @@
     <col min="9" max="9" width="22.1796875" style="3" customWidth="1"/>
     <col min="10" max="10" width="11.26953125" style="12" customWidth="1"/>
     <col min="11" max="11" width="17.54296875" style="3" customWidth="1"/>
-    <col min="12" max="16384" width="9.1796875" style="3"/>
+    <col min="12" max="12" width="5.36328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="7" customFormat="1" ht="39" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="7" customFormat="1" ht="52" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -876,28 +931,31 @@
         <v>23</v>
       </c>
       <c r="L1" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="S1" s="6" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>2015</v>
       </c>
@@ -931,22 +989,22 @@
       <c r="K2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="8">
+      <c r="M2" s="8">
         <v>-0.09</v>
       </c>
-      <c r="M2" s="8">
+      <c r="N2" s="8">
         <v>0.9</v>
       </c>
-      <c r="N2" s="8"/>
       <c r="O2" s="8"/>
-      <c r="P2" s="8">
-        <v>0</v>
-      </c>
+      <c r="P2" s="8"/>
       <c r="Q2" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="R2" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2023</v>
       </c>
@@ -977,22 +1035,22 @@
       <c r="K3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="8">
+      <c r="M3" s="8">
         <v>-0.44</v>
       </c>
-      <c r="M3" s="8">
+      <c r="N3" s="8">
         <v>-0.23</v>
       </c>
-      <c r="N3" s="8"/>
       <c r="O3" s="8"/>
-      <c r="P3" s="8">
-        <v>0</v>
-      </c>
+      <c r="P3" s="8"/>
       <c r="Q3" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="R3" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>2023</v>
       </c>
@@ -1023,22 +1081,22 @@
       <c r="K4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L4" s="8">
+      <c r="M4" s="8">
         <v>-1.25</v>
       </c>
-      <c r="M4" s="8">
+      <c r="N4" s="8">
         <v>-0.75</v>
       </c>
-      <c r="N4" s="8"/>
       <c r="O4" s="8"/>
-      <c r="P4" s="8">
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8">
         <v>30</v>
       </c>
-      <c r="Q4" s="8">
+      <c r="R4" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>2023</v>
       </c>
@@ -1069,22 +1127,22 @@
       <c r="K5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="L5" s="8">
+      <c r="M5" s="8">
         <v>-1.25</v>
       </c>
-      <c r="M5" s="8">
+      <c r="N5" s="8">
         <v>-0.75</v>
       </c>
-      <c r="N5" s="8"/>
       <c r="O5" s="8"/>
-      <c r="P5" s="8">
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8">
         <v>45</v>
       </c>
-      <c r="Q5" s="8">
+      <c r="R5" s="8">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>2023</v>
       </c>
@@ -1115,22 +1173,22 @@
       <c r="K6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="L6" s="8">
+      <c r="M6" s="8">
         <v>-1.25</v>
       </c>
-      <c r="M6" s="8">
+      <c r="N6" s="8">
         <v>-0.75</v>
       </c>
-      <c r="N6" s="8"/>
       <c r="O6" s="8"/>
-      <c r="P6" s="8">
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8">
         <v>75</v>
       </c>
-      <c r="Q6" s="8">
+      <c r="R6" s="8">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>2023</v>
       </c>
@@ -1161,22 +1219,22 @@
       <c r="K7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="L7" s="8">
+      <c r="M7" s="8">
         <v>-1.25</v>
       </c>
-      <c r="M7" s="8">
+      <c r="N7" s="8">
         <v>-0.75</v>
       </c>
-      <c r="N7" s="8"/>
       <c r="O7" s="8"/>
-      <c r="P7" s="13">
+      <c r="P7" s="8"/>
+      <c r="Q7" s="13">
         <v>75</v>
       </c>
-      <c r="Q7" s="13">
+      <c r="R7" s="13">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>2023</v>
       </c>
@@ -1207,22 +1265,22 @@
       <c r="K8" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="L8" s="8">
+      <c r="M8" s="8">
         <v>-1.25</v>
       </c>
-      <c r="M8" s="8">
+      <c r="N8" s="8">
         <v>-0.75</v>
       </c>
-      <c r="N8" s="8"/>
       <c r="O8" s="8"/>
-      <c r="P8" s="9">
+      <c r="P8" s="8"/>
+      <c r="Q8" s="9">
         <v>85</v>
       </c>
-      <c r="Q8" s="9">
+      <c r="R8" s="9">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>2023</v>
       </c>
@@ -1253,22 +1311,22 @@
       <c r="K9" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="L9" s="8">
+      <c r="M9" s="8">
         <v>-1.25</v>
       </c>
-      <c r="M9" s="8">
+      <c r="N9" s="8">
         <v>-0.75</v>
       </c>
-      <c r="N9" s="8"/>
       <c r="O9" s="8"/>
-      <c r="P9" s="9">
+      <c r="P9" s="8"/>
+      <c r="Q9" s="9">
         <v>95</v>
       </c>
-      <c r="Q9" s="9">
+      <c r="R9" s="9">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>2023</v>
       </c>
@@ -1299,22 +1357,22 @@
       <c r="K10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="L10" s="8">
+      <c r="M10" s="8">
         <v>-1.25</v>
       </c>
-      <c r="M10" s="8">
+      <c r="N10" s="8">
         <v>-0.75</v>
       </c>
-      <c r="N10" s="8"/>
       <c r="O10" s="8"/>
-      <c r="P10" s="9">
+      <c r="P10" s="8"/>
+      <c r="Q10" s="9">
         <v>85</v>
       </c>
-      <c r="Q10" s="9">
+      <c r="R10" s="9">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>2023</v>
       </c>
@@ -1345,22 +1403,22 @@
       <c r="K11" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="L11" s="8">
+      <c r="M11" s="8">
         <v>-1.25</v>
       </c>
-      <c r="M11" s="8">
+      <c r="N11" s="8">
         <v>-0.75</v>
       </c>
-      <c r="N11" s="8"/>
       <c r="O11" s="8"/>
-      <c r="P11" s="9">
+      <c r="P11" s="8"/>
+      <c r="Q11" s="9">
         <v>85</v>
       </c>
-      <c r="Q11" s="9">
+      <c r="R11" s="9">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>2023</v>
       </c>
@@ -1391,22 +1449,22 @@
       <c r="K12" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="L12" s="8">
+      <c r="M12" s="8">
         <v>-1.25</v>
       </c>
-      <c r="M12" s="8">
+      <c r="N12" s="8">
         <v>-0.75</v>
       </c>
-      <c r="N12" s="8"/>
       <c r="O12" s="8"/>
-      <c r="P12" s="9">
+      <c r="P12" s="8"/>
+      <c r="Q12" s="9">
         <v>95</v>
       </c>
-      <c r="Q12" s="9">
+      <c r="R12" s="9">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>2023</v>
       </c>
@@ -1437,22 +1495,22 @@
       <c r="K13" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="L13" s="8">
+      <c r="M13" s="8">
         <v>-1.25</v>
       </c>
-      <c r="M13" s="8">
+      <c r="N13" s="8">
         <v>-0.75</v>
       </c>
-      <c r="N13" s="8"/>
       <c r="O13" s="8"/>
-      <c r="P13" s="9">
+      <c r="P13" s="8"/>
+      <c r="Q13" s="9">
         <v>120</v>
       </c>
-      <c r="Q13" s="9">
+      <c r="R13" s="9">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>2023</v>
       </c>
@@ -1483,22 +1541,22 @@
       <c r="K14" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="L14" s="8">
+      <c r="M14" s="8">
         <v>-1.25</v>
       </c>
-      <c r="M14" s="8">
+      <c r="N14" s="8">
         <v>-0.75</v>
       </c>
-      <c r="N14" s="8"/>
       <c r="O14" s="8"/>
-      <c r="P14" s="9">
+      <c r="P14" s="8"/>
+      <c r="Q14" s="9">
         <v>180</v>
       </c>
-      <c r="Q14" s="9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="R14" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>2023</v>
       </c>
@@ -1529,22 +1587,22 @@
       <c r="K15" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="L15" s="8">
+      <c r="M15" s="8">
         <v>-1.25</v>
       </c>
-      <c r="M15" s="8">
+      <c r="N15" s="8">
         <v>-0.75</v>
       </c>
-      <c r="N15" s="8"/>
       <c r="O15" s="8"/>
-      <c r="P15" s="9">
+      <c r="P15" s="8"/>
+      <c r="Q15" s="9">
         <v>300</v>
       </c>
-      <c r="Q15" s="9">
+      <c r="R15" s="9">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>2023</v>
       </c>
@@ -1575,22 +1633,22 @@
       <c r="K16" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="L16" s="8">
+      <c r="M16" s="8">
         <v>-1.25</v>
       </c>
-      <c r="M16" s="8">
+      <c r="N16" s="8">
         <v>-0.75</v>
       </c>
-      <c r="N16" s="8"/>
       <c r="O16" s="8"/>
-      <c r="P16" s="9">
+      <c r="P16" s="8"/>
+      <c r="Q16" s="9">
         <v>250</v>
       </c>
-      <c r="Q16" s="9">
+      <c r="R16" s="9">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>2023</v>
       </c>
@@ -1621,22 +1679,22 @@
       <c r="K17" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="L17" s="8">
+      <c r="M17" s="8">
         <v>-1.25</v>
       </c>
-      <c r="M17" s="8">
+      <c r="N17" s="8">
         <v>-0.75</v>
       </c>
-      <c r="N17" s="8"/>
       <c r="O17" s="8"/>
-      <c r="P17" s="9">
+      <c r="P17" s="8"/>
+      <c r="Q17" s="9">
         <v>200</v>
       </c>
-      <c r="Q17" s="9">
+      <c r="R17" s="9">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>2023</v>
       </c>
@@ -1667,22 +1725,22 @@
       <c r="K18" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="L18" s="8">
+      <c r="M18" s="8">
         <v>-1.25</v>
       </c>
-      <c r="M18" s="8">
+      <c r="N18" s="8">
         <v>-0.75</v>
       </c>
-      <c r="N18" s="8"/>
       <c r="O18" s="8"/>
-      <c r="P18" s="9">
+      <c r="P18" s="8"/>
+      <c r="Q18" s="9">
         <v>120</v>
       </c>
-      <c r="Q18" s="9">
+      <c r="R18" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>2023</v>
       </c>
@@ -1713,22 +1771,22 @@
       <c r="K19" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="L19" s="8">
+      <c r="M19" s="8">
         <v>-1.25</v>
       </c>
-      <c r="M19" s="8">
+      <c r="N19" s="8">
         <v>-0.75</v>
       </c>
-      <c r="N19" s="8"/>
       <c r="O19" s="8"/>
-      <c r="P19" s="9">
+      <c r="P19" s="8"/>
+      <c r="Q19" s="9">
         <v>120</v>
       </c>
-      <c r="Q19" s="9">
+      <c r="R19" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>2023</v>
       </c>
@@ -1759,22 +1817,22 @@
       <c r="K20" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="L20" s="8">
+      <c r="M20" s="8">
         <v>-1.25</v>
       </c>
-      <c r="M20" s="8">
+      <c r="N20" s="8">
         <v>-0.75</v>
       </c>
-      <c r="N20" s="8"/>
       <c r="O20" s="8"/>
-      <c r="P20" s="9">
+      <c r="P20" s="8"/>
+      <c r="Q20" s="9">
         <v>120</v>
       </c>
-      <c r="Q20" s="9">
+      <c r="R20" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>2023</v>
       </c>
@@ -1805,20 +1863,20 @@
       <c r="K21" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="N21" s="8">
+      <c r="O21" s="8">
         <v>1.27</v>
       </c>
-      <c r="O21" s="8">
+      <c r="P21" s="8">
         <v>1.1499999999999999</v>
       </c>
-      <c r="P21" s="9">
+      <c r="Q21" s="9">
         <v>120</v>
       </c>
-      <c r="Q21" s="9">
+      <c r="R21" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>2023</v>
       </c>
@@ -1849,25 +1907,25 @@
       <c r="K22" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="L22" s="8">
+      <c r="M22" s="8">
         <v>-1.25</v>
       </c>
-      <c r="M22" s="8">
+      <c r="N22" s="8">
         <v>-0.75</v>
       </c>
-      <c r="N22" s="8"/>
       <c r="O22" s="8"/>
-      <c r="P22" s="9">
+      <c r="P22" s="8"/>
+      <c r="Q22" s="9">
         <v>120</v>
       </c>
-      <c r="Q22" s="9">
+      <c r="R22" s="9">
         <v>0</v>
       </c>
-      <c r="R22" s="9">
+      <c r="S22" s="9">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>2023</v>
       </c>
@@ -1898,23 +1956,23 @@
       <c r="K23" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="N23" s="8">
+      <c r="O23" s="8">
         <v>1.27</v>
       </c>
-      <c r="O23" s="8">
+      <c r="P23" s="8">
         <v>1.1499999999999999</v>
       </c>
-      <c r="P23" s="9">
+      <c r="Q23" s="9">
         <v>120</v>
       </c>
-      <c r="Q23" s="9">
+      <c r="R23" s="9">
         <v>0</v>
       </c>
-      <c r="R23" s="9">
+      <c r="S23" s="9">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>2023</v>
       </c>
@@ -1948,23 +2006,23 @@
       <c r="K24" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="L24" s="8">
+      <c r="M24" s="8">
         <v>-1.25</v>
       </c>
-      <c r="M24" s="8">
+      <c r="N24" s="8">
         <v>-0.75</v>
       </c>
-      <c r="P24" s="9">
+      <c r="Q24" s="9">
         <v>120</v>
       </c>
-      <c r="Q24" s="9">
+      <c r="R24" s="9">
         <v>0</v>
       </c>
-      <c r="R24" s="9">
+      <c r="S24" s="9">
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>2023</v>
       </c>
@@ -1998,29 +2056,32 @@
       <c r="K25" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="L25" s="3" t="s">
-        <v>112</v>
+      <c r="L25" s="3">
+        <v>17.77</v>
       </c>
       <c r="M25" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="N25" s="8">
+      <c r="N25" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="O25" s="8">
         <v>1.27</v>
       </c>
-      <c r="O25" s="8">
+      <c r="P25" s="8">
         <v>1.1499999999999999</v>
       </c>
-      <c r="P25" s="9">
+      <c r="Q25" s="9">
         <v>120</v>
       </c>
-      <c r="Q25" s="9">
+      <c r="R25" s="9">
         <v>0</v>
       </c>
-      <c r="R25" s="9">
+      <c r="S25" s="9">
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>2023</v>
       </c>
@@ -2054,255 +2115,329 @@
       <c r="K26" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="L26" s="3" t="s">
-        <v>112</v>
+      <c r="L26" s="3">
+        <v>17.77</v>
       </c>
       <c r="M26" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="N26" s="3">
+      <c r="N26" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="O26" s="3">
         <v>0.64</v>
       </c>
-      <c r="O26" s="3">
+      <c r="P26" s="3">
         <v>0.57999999999999996</v>
       </c>
-      <c r="P26" s="9">
+      <c r="Q26" s="9">
         <v>120</v>
       </c>
-      <c r="Q26" s="9">
+      <c r="R26" s="9">
         <v>0</v>
       </c>
-      <c r="R26" s="9">
+      <c r="S26" s="9">
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A27" s="3">
+    <row r="27" spans="1:19" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="17">
         <v>2023</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="3" t="s">
+      <c r="C27" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="F27" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H27" s="3" t="s">
+      <c r="F27" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H27" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="I27" s="3" t="s">
+      <c r="I27" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="J27" s="12" t="s">
+      <c r="J27" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="K27" s="3" t="s">
+      <c r="K27" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="L27" s="3" t="s">
+      <c r="L27" s="17">
+        <v>17.77</v>
+      </c>
+      <c r="M27" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="M27" s="3" t="s">
+      <c r="N27" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="N27" s="3">
+      <c r="O27" s="17">
         <v>0.95</v>
       </c>
-      <c r="O27" s="3">
+      <c r="P27" s="17">
         <v>0.86</v>
       </c>
-      <c r="P27" s="9">
+      <c r="Q27" s="19">
         <v>120</v>
       </c>
-      <c r="Q27" s="9">
+      <c r="R27" s="19">
         <v>0</v>
       </c>
-      <c r="R27" s="9">
+      <c r="S27" s="19">
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A28" s="3">
+    <row r="28" spans="1:19" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="20">
         <v>2035</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="D28" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="E28" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="F28" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="G28" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="H28" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="I28" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="J28" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="K28" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="L28" s="20">
+        <v>15.85</v>
+      </c>
+      <c r="M28" s="20">
+        <v>-0.27</v>
+      </c>
+      <c r="N28" s="20">
+        <v>0</v>
+      </c>
+      <c r="O28" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="P28" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q28" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="R28" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="S28" s="22" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="14">
+        <v>2035</v>
+      </c>
+      <c r="B29" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D28" s="3" t="s">
+      <c r="C29" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E29" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="F28" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H28" s="3" t="s">
+      <c r="F29" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H29" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I28" s="3" t="s">
+      <c r="I29" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="J28" s="12" t="s">
+      <c r="J29" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="K28" s="3" t="s">
+      <c r="K29" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="L28" s="3" t="s">
+      <c r="L29" s="14">
+        <v>15.85</v>
+      </c>
+      <c r="M29" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="M28" s="3" t="s">
+      <c r="N29" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="N28" s="8">
+      <c r="O29" s="16">
         <v>1.27</v>
       </c>
-      <c r="O28" s="8">
+      <c r="P29" s="16">
         <v>1.1499999999999999</v>
       </c>
-      <c r="P28" s="9">
+      <c r="Q29" s="16">
         <v>120</v>
       </c>
-      <c r="Q28" s="9">
+      <c r="R29" s="16">
         <v>0</v>
       </c>
-      <c r="R28" s="9">
+      <c r="S29" s="16">
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A29" s="3">
+    <row r="30" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="14">
         <v>2035</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B30" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D29" s="3" t="s">
+      <c r="C30" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E30" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="F29" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H29" s="3" t="s">
+      <c r="F30" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I29" s="3" t="s">
+      <c r="I30" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="J29" s="12" t="s">
+      <c r="J30" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="K29" s="3" t="s">
+      <c r="K30" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="L29" s="3" t="s">
+      <c r="L30" s="14">
+        <v>18.64</v>
+      </c>
+      <c r="M30" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="M29" s="3" t="s">
+      <c r="N30" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="N29" s="8">
+      <c r="O30" s="16">
         <v>1.27</v>
       </c>
-      <c r="O29" s="8">
+      <c r="P30" s="16">
         <v>1.1499999999999999</v>
       </c>
-      <c r="P29" s="9">
+      <c r="Q30" s="16">
         <v>120</v>
       </c>
-      <c r="Q29" s="9">
+      <c r="R30" s="16">
         <v>0</v>
       </c>
-      <c r="R29" s="9">
+      <c r="S30" s="16">
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A30" s="3">
+    <row r="31" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="14">
         <v>2035</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B31" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D30" s="3" t="s">
+      <c r="C31" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="E31" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="F30" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H30" s="3" t="s">
+      <c r="F31" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G31" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H31" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I30" s="3" t="s">
+      <c r="I31" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="J30" s="12" t="s">
+      <c r="J31" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="K30" s="3" t="s">
+      <c r="K31" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="L30" s="3" t="s">
+      <c r="L31" s="14">
+        <v>18.64</v>
+      </c>
+      <c r="M31" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="M30" s="3" t="s">
+      <c r="N31" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="N30" s="8">
+      <c r="O31" s="16">
         <v>1.27</v>
       </c>
-      <c r="O30" s="8">
+      <c r="P31" s="16">
         <v>1.1499999999999999</v>
       </c>
-      <c r="P30" s="9">
+      <c r="Q31" s="16">
         <v>0</v>
       </c>
-      <c r="Q30" s="9">
+      <c r="R31" s="16">
         <v>0</v>
       </c>
-      <c r="R30" s="9">
+      <c r="S31" s="16">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added a pair of 2035 IPA run in which the WFH rate are lowered to match 2022 ACS.
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-v1.6_develop\utilities\RTP\config_RTP2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8AA8DDB-2306-40A1-8A47-615995AC8840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B25A27A-23D9-4F9D-BE32-AB5D2A23185E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="129">
   <si>
     <t>year</t>
   </si>
@@ -405,6 +405,24 @@
   </si>
   <si>
     <t>AOC_CentsPerMile</t>
+  </si>
+  <si>
+    <t>2035_TM160_IPA_04</t>
+  </si>
+  <si>
+    <t>2035_TM160_IPA_05</t>
+  </si>
+  <si>
+    <t>WFH rate at 25%, with trn hesistance on</t>
+  </si>
+  <si>
+    <t>WFH rate at 25%, with trn hesistance off</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1205561944199034/f</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1205561944199029/f</t>
   </si>
 </sst>
 </file>
@@ -509,7 +527,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -545,11 +563,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -872,11 +885,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9564CC59-3725-4FDA-8BF2-0F68CB1B6F5A}">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L25" sqref="L25"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -2140,121 +2153,121 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:19" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="17">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
         <v>2023</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C27" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27" s="17" t="s">
+      <c r="C27" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E27" s="17" t="s">
+      <c r="E27" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="F27" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="G27" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="H27" s="17" t="s">
+      <c r="F27" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H27" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I27" s="17" t="s">
+      <c r="I27" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="J27" s="18" t="s">
+      <c r="J27" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="K27" s="17" t="s">
+      <c r="K27" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="L27" s="17">
+      <c r="L27" s="3">
         <v>17.77</v>
       </c>
-      <c r="M27" s="17" t="s">
+      <c r="M27" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="N27" s="17" t="s">
+      <c r="N27" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="O27" s="17">
+      <c r="O27" s="3">
         <v>0.95</v>
       </c>
-      <c r="P27" s="17">
+      <c r="P27" s="3">
         <v>0.86</v>
       </c>
-      <c r="Q27" s="19">
+      <c r="Q27" s="8">
         <v>120</v>
       </c>
-      <c r="R27" s="19">
+      <c r="R27" s="8">
         <v>0</v>
       </c>
-      <c r="S27" s="19">
+      <c r="S27" s="8">
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:19" s="20" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="20">
+    <row r="28" spans="1:19" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="17">
         <v>2035</v>
       </c>
-      <c r="B28" s="20" t="s">
+      <c r="B28" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="C28" s="20" t="s">
+      <c r="C28" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="D28" s="20" t="s">
+      <c r="D28" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="E28" s="20" t="s">
+      <c r="E28" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="F28" s="20" t="s">
+      <c r="F28" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="G28" s="23" t="s">
+      <c r="G28" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="H28" s="20" t="s">
+      <c r="H28" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="I28" s="20" t="s">
+      <c r="I28" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="J28" s="21" t="s">
+      <c r="J28" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="K28" s="20" t="s">
+      <c r="K28" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="L28" s="20">
+      <c r="L28" s="17">
         <v>15.85</v>
       </c>
-      <c r="M28" s="20">
+      <c r="M28" s="17">
         <v>-0.27</v>
       </c>
-      <c r="N28" s="20">
+      <c r="N28" s="17">
         <v>0</v>
       </c>
-      <c r="O28" s="20" t="s">
+      <c r="O28" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="P28" s="20" t="s">
+      <c r="P28" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="Q28" s="22" t="s">
+      <c r="Q28" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="R28" s="22" t="s">
+      <c r="R28" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="S28" s="22" t="s">
+      <c r="S28" s="19" t="s">
         <v>112</v>
       </c>
     </row>
@@ -2432,6 +2445,124 @@
         <v>0</v>
       </c>
       <c r="S31" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="14">
+        <v>2035</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G32" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H32" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="I32" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="J32" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="K32" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="L32" s="14">
+        <v>18.64</v>
+      </c>
+      <c r="M32" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="N32" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="O32" s="14">
+        <v>0.95</v>
+      </c>
+      <c r="P32" s="14">
+        <v>0.86</v>
+      </c>
+      <c r="Q32" s="16">
+        <v>120</v>
+      </c>
+      <c r="R32" s="16">
+        <v>0</v>
+      </c>
+      <c r="S32" s="16">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="14">
+        <v>2035</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G33" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H33" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="I33" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="J33" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="K33" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="L33" s="14">
+        <v>18.64</v>
+      </c>
+      <c r="M33" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="N33" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="O33" s="14">
+        <v>0.95</v>
+      </c>
+      <c r="P33" s="14">
+        <v>0.86</v>
+      </c>
+      <c r="Q33" s="16">
+        <v>0</v>
+      </c>
+      <c r="R33" s="16">
+        <v>0</v>
+      </c>
+      <c r="S33" s="16">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added 2005 and 2050 from the last Plan to the list of model runs
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B25A27A-23D9-4F9D-BE32-AB5D2A23185E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECEFF8EC-F77E-40CD-AE77-11BC685F8369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="134">
   <si>
     <t>year</t>
   </si>
@@ -423,6 +423,21 @@
   </si>
   <si>
     <t>https://app.asana.com/0/1204085012544660/1205561944199029/f</t>
+  </si>
+  <si>
+    <t>2005_TM152_IPA_03</t>
+  </si>
+  <si>
+    <t>RTP21 2005 run</t>
+  </si>
+  <si>
+    <t>2050_TM152_FBP_PlusCrossing_24</t>
+  </si>
+  <si>
+    <t>M:\Application\Model One\RTP2021\Blueprint\INPUT_DEVELOPMENT\Networks\BlueprintNetworks_64\net_2050_Blueprint</t>
+  </si>
+  <si>
+    <t>model2-a</t>
   </si>
 </sst>
 </file>
@@ -471,7 +486,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -493,6 +508,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -527,12 +554,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -571,6 +594,23 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -885,1685 +925,1770 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9564CC59-3725-4FDA-8BF2-0F68CB1B6F5A}">
-  <dimension ref="A1:S33"/>
+  <dimension ref="A1:S35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A33" sqref="A33"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.81640625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="9.81640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="28.6328125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="11.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.1796875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="6.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.1796875" style="3" customWidth="1"/>
-    <col min="10" max="10" width="11.26953125" style="12" customWidth="1"/>
-    <col min="11" max="11" width="17.54296875" style="3" customWidth="1"/>
-    <col min="12" max="12" width="5.36328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.1796875" style="3"/>
+    <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="28.6328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.1796875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="6.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.1796875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.26953125" style="10" customWidth="1"/>
+    <col min="11" max="11" width="17.54296875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="5.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="7" customFormat="1" ht="52" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:19" s="5" customFormat="1" ht="52" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q1" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="S1" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+    <row r="2" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="19">
+        <v>2005</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="22"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="10">
         <v>2015</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="8">
+      <c r="M3" s="6">
         <v>-0.09</v>
       </c>
-      <c r="N2" s="8">
+      <c r="N3" s="6">
         <v>0.9</v>
       </c>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8">
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6">
         <v>0</v>
       </c>
-      <c r="R2" s="8">
+      <c r="R3" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
         <v>2023</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="3" t="s">
+      <c r="F4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M3" s="8">
+      <c r="M4" s="6">
         <v>-0.44</v>
       </c>
-      <c r="N3" s="8">
+      <c r="N4" s="6">
         <v>-0.23</v>
       </c>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8">
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6">
         <v>0</v>
       </c>
-      <c r="R3" s="8">
+      <c r="R4" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
         <v>2023</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="3" t="s">
+      <c r="F5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="J5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="M4" s="8">
+      <c r="M5" s="6">
         <v>-1.25</v>
       </c>
-      <c r="N4" s="8">
+      <c r="N5" s="6">
         <v>-0.75</v>
       </c>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8">
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6">
         <v>30</v>
       </c>
-      <c r="R4" s="8">
+      <c r="R5" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
         <v>2023</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="3" t="s">
+      <c r="F6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="J6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="K6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M5" s="8">
+      <c r="M6" s="6">
         <v>-1.25</v>
       </c>
-      <c r="N5" s="8">
+      <c r="N6" s="6">
         <v>-0.75</v>
       </c>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8">
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6">
         <v>45</v>
       </c>
-      <c r="R5" s="8">
+      <c r="R6" s="6">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
         <v>2023</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="3" t="s">
+      <c r="F7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="J7" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="K7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="M6" s="8">
+      <c r="M7" s="6">
         <v>-1.25</v>
       </c>
-      <c r="N6" s="8">
+      <c r="N7" s="6">
         <v>-0.75</v>
       </c>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8">
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6">
         <v>75</v>
       </c>
-      <c r="R6" s="8">
+      <c r="R7" s="6">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
         <v>2023</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="C8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="3" t="s">
+      <c r="F8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J7" s="11" t="s">
+      <c r="J8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="K8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M7" s="8">
+      <c r="M8" s="6">
         <v>-1.25</v>
       </c>
-      <c r="N7" s="8">
+      <c r="N8" s="6">
         <v>-0.75</v>
       </c>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="13">
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="11">
         <v>75</v>
       </c>
-      <c r="R7" s="13">
+      <c r="R8" s="11">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
         <v>2023</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="C9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E9" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8" s="3" t="s">
+      <c r="F9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J8" s="11" t="s">
+      <c r="J9" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="K9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="M8" s="8">
+      <c r="M9" s="6">
         <v>-1.25</v>
       </c>
-      <c r="N8" s="8">
+      <c r="N9" s="6">
         <v>-0.75</v>
       </c>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="9">
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="7">
         <v>85</v>
       </c>
-      <c r="R8" s="9">
+      <c r="R9" s="7">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
         <v>2023</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="3" t="s">
+      <c r="C10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I9" s="3" t="s">
+      <c r="F10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J9" s="11" t="s">
+      <c r="J10" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="K10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="M9" s="8">
+      <c r="M10" s="6">
         <v>-1.25</v>
       </c>
-      <c r="N9" s="8">
+      <c r="N10" s="6">
         <v>-0.75</v>
       </c>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="9">
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="7">
         <v>95</v>
       </c>
-      <c r="R9" s="9">
+      <c r="R10" s="7">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
         <v>2023</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B11" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="3" t="s">
+      <c r="C11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E11" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I10" s="3" t="s">
+      <c r="F11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J10" s="11" t="s">
+      <c r="J11" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="K10" s="3" t="s">
+      <c r="K11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="M10" s="8">
+      <c r="M11" s="6">
         <v>-1.25</v>
       </c>
-      <c r="N10" s="8">
+      <c r="N11" s="6">
         <v>-0.75</v>
       </c>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="9">
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="7">
         <v>85</v>
       </c>
-      <c r="R10" s="9">
+      <c r="R11" s="7">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
         <v>2023</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B12" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="3" t="s">
+      <c r="C12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E12" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I11" s="3" t="s">
+      <c r="F12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J11" s="12" t="s">
+      <c r="J12" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="K11" s="3" t="s">
+      <c r="K12" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="M11" s="8">
+      <c r="M12" s="6">
         <v>-1.25</v>
       </c>
-      <c r="N11" s="8">
+      <c r="N12" s="6">
         <v>-0.75</v>
       </c>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="9">
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="7">
         <v>85</v>
       </c>
-      <c r="R11" s="9">
+      <c r="R12" s="7">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
         <v>2023</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B13" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="3" t="s">
+      <c r="C13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E13" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I12" s="3" t="s">
+      <c r="F13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="J12" s="12" t="s">
+      <c r="J13" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="K12" s="3" t="s">
+      <c r="K13" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="M12" s="8">
+      <c r="M13" s="6">
         <v>-1.25</v>
       </c>
-      <c r="N12" s="8">
+      <c r="N13" s="6">
         <v>-0.75</v>
       </c>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="9">
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="7">
         <v>95</v>
       </c>
-      <c r="R12" s="9">
+      <c r="R13" s="7">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A13" s="3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
         <v>2023</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B14" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="3" t="s">
+      <c r="C14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E14" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I13" s="3" t="s">
+      <c r="F14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="J13" s="12" t="s">
+      <c r="J14" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="K13" s="3" t="s">
+      <c r="K14" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="M13" s="8">
+      <c r="M14" s="6">
         <v>-1.25</v>
       </c>
-      <c r="N13" s="8">
+      <c r="N14" s="6">
         <v>-0.75</v>
       </c>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="9">
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="7">
         <v>120</v>
       </c>
-      <c r="R13" s="9">
+      <c r="R14" s="7">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A14" s="3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
         <v>2023</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B15" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="3" t="s">
+      <c r="C15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E15" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I14" s="3" t="s">
+      <c r="F15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="J14" s="12" t="s">
+      <c r="J15" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="K14" s="3" t="s">
+      <c r="K15" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="M14" s="8">
+      <c r="M15" s="6">
         <v>-1.25</v>
       </c>
-      <c r="N14" s="8">
+      <c r="N15" s="6">
         <v>-0.75</v>
       </c>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
-      <c r="Q14" s="9">
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="7">
         <v>180</v>
       </c>
-      <c r="R14" s="9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A15" s="3">
+      <c r="R15" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
         <v>2023</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B16" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="3" t="s">
+      <c r="C16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E16" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I15" s="3" t="s">
+      <c r="F16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="J15" s="12" t="s">
+      <c r="J16" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="K15" s="3" t="s">
+      <c r="K16" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="M15" s="8">
+      <c r="M16" s="6">
         <v>-1.25</v>
       </c>
-      <c r="N15" s="8">
+      <c r="N16" s="6">
         <v>-0.75</v>
       </c>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
-      <c r="Q15" s="9">
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="7">
         <v>300</v>
       </c>
-      <c r="R15" s="9">
+      <c r="R16" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A16" s="3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
         <v>2023</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B17" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="3" t="s">
+      <c r="C17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E17" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F16" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I16" s="3" t="s">
+      <c r="F17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I17" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="J16" s="12" t="s">
+      <c r="J17" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="K16" s="3" t="s">
+      <c r="K17" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="M16" s="8">
+      <c r="M17" s="6">
         <v>-1.25</v>
       </c>
-      <c r="N16" s="8">
+      <c r="N17" s="6">
         <v>-0.75</v>
       </c>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
-      <c r="Q16" s="9">
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="7">
         <v>250</v>
       </c>
-      <c r="R16" s="9">
+      <c r="R17" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A17" s="3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
         <v>2023</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B18" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="3" t="s">
+      <c r="C18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E18" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I17" s="3" t="s">
+      <c r="F18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I18" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="J17" s="12" t="s">
+      <c r="J18" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="K17" s="3" t="s">
+      <c r="K18" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="M17" s="8">
+      <c r="M18" s="6">
         <v>-1.25</v>
       </c>
-      <c r="N17" s="8">
+      <c r="N18" s="6">
         <v>-0.75</v>
       </c>
-      <c r="O17" s="8"/>
-      <c r="P17" s="8"/>
-      <c r="Q17" s="9">
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="7">
         <v>200</v>
       </c>
-      <c r="R17" s="9">
+      <c r="R18" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A18" s="3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
         <v>2023</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B19" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="3" t="s">
+      <c r="C19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E19" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I18" s="3" t="s">
+      <c r="F19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I19" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="J18" s="12" t="s">
+      <c r="J19" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="K18" s="3" t="s">
+      <c r="K19" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="M18" s="8">
+      <c r="M19" s="6">
         <v>-1.25</v>
       </c>
-      <c r="N18" s="8">
+      <c r="N19" s="6">
         <v>-0.75</v>
       </c>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
-      <c r="Q18" s="9">
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="7">
         <v>120</v>
       </c>
-      <c r="R18" s="9">
+      <c r="R19" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A19" s="3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
         <v>2023</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B20" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="3" t="s">
+      <c r="C20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E20" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I19" s="3" t="s">
+      <c r="F20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="J19" s="12" t="s">
+      <c r="J20" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="K19" s="3" t="s">
+      <c r="K20" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="M19" s="8">
+      <c r="M20" s="6">
         <v>-1.25</v>
       </c>
-      <c r="N19" s="8">
+      <c r="N20" s="6">
         <v>-0.75</v>
       </c>
-      <c r="O19" s="8"/>
-      <c r="P19" s="8"/>
-      <c r="Q19" s="9">
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="7">
         <v>120</v>
       </c>
-      <c r="R19" s="9">
+      <c r="R20" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A20" s="3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
         <v>2023</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B21" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" s="3" t="s">
+      <c r="C21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E21" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F20" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I20" s="3" t="s">
+      <c r="F21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J20" s="12" t="s">
+      <c r="J21" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="K20" s="3" t="s">
+      <c r="K21" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="M20" s="8">
+      <c r="M21" s="6">
         <v>-1.25</v>
       </c>
-      <c r="N20" s="8">
+      <c r="N21" s="6">
         <v>-0.75</v>
       </c>
-      <c r="O20" s="8"/>
-      <c r="P20" s="8"/>
-      <c r="Q20" s="9">
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="7">
         <v>120</v>
       </c>
-      <c r="R20" s="9">
+      <c r="R21" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A21" s="3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
         <v>2023</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B22" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" s="3" t="s">
+      <c r="C22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E22" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F21" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I21" s="3" t="s">
+      <c r="F22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I22" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J21" s="12" t="s">
+      <c r="J22" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="K21" s="3" t="s">
+      <c r="K22" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="O21" s="8">
+      <c r="O22" s="6">
         <v>1.27</v>
       </c>
-      <c r="P21" s="8">
+      <c r="P22" s="6">
         <v>1.1499999999999999</v>
       </c>
-      <c r="Q21" s="9">
+      <c r="Q22" s="7">
         <v>120</v>
       </c>
-      <c r="R21" s="9">
+      <c r="R22" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A22" s="3">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
         <v>2023</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B23" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" s="3" t="s">
+      <c r="C23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E23" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F22" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I22" s="3" t="s">
+      <c r="F23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I23" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J22" s="12" t="s">
+      <c r="J23" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="K22" s="3" t="s">
+      <c r="K23" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="M22" s="8">
+      <c r="M23" s="6">
         <v>-1.25</v>
       </c>
-      <c r="N22" s="8">
+      <c r="N23" s="6">
         <v>-0.75</v>
       </c>
-      <c r="O22" s="8"/>
-      <c r="P22" s="8"/>
-      <c r="Q22" s="9">
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="7">
         <v>120</v>
       </c>
-      <c r="R22" s="9">
+      <c r="R23" s="7">
         <v>0</v>
       </c>
-      <c r="S22" s="9">
+      <c r="S23" s="7">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A23" s="3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
         <v>2023</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B24" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" s="3" t="s">
+      <c r="C24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E24" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F23" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I23" s="3" t="s">
+      <c r="F24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I24" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J23" s="12" t="s">
+      <c r="J24" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="K23" s="3" t="s">
+      <c r="K24" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="O23" s="8">
+      <c r="O24" s="6">
         <v>1.27</v>
       </c>
-      <c r="P23" s="8">
+      <c r="P24" s="6">
         <v>1.1499999999999999</v>
       </c>
-      <c r="Q23" s="9">
+      <c r="Q24" s="7">
         <v>120</v>
       </c>
-      <c r="R23" s="9">
+      <c r="R24" s="7">
         <v>0</v>
       </c>
-      <c r="S23" s="9">
+      <c r="S24" s="7">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A24" s="3">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
         <v>2023</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B25" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" s="3" t="s">
+      <c r="C25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E25" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F24" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H24" s="3" t="s">
+      <c r="F25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I24" s="3" t="s">
+      <c r="I25" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J24" s="12" t="s">
+      <c r="J25" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="K24" s="3" t="s">
+      <c r="K25" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="M24" s="8">
+      <c r="M25" s="6">
         <v>-1.25</v>
       </c>
-      <c r="N24" s="8">
+      <c r="N25" s="6">
         <v>-0.75</v>
       </c>
-      <c r="Q24" s="9">
+      <c r="Q25" s="7">
         <v>120</v>
       </c>
-      <c r="R24" s="9">
+      <c r="R25" s="7">
         <v>0</v>
       </c>
-      <c r="S24" s="9">
+      <c r="S25" s="7">
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A25" s="3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
         <v>2023</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B26" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25" s="3" t="s">
+      <c r="C26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E26" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F25" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H25" s="3" t="s">
+      <c r="F26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I25" s="3" t="s">
+      <c r="I26" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J25" s="12" t="s">
+      <c r="J26" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="K25" s="3" t="s">
+      <c r="K26" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="L25" s="3">
+      <c r="L26" s="1">
         <v>17.77</v>
       </c>
-      <c r="M25" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="N25" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="O25" s="8">
+      <c r="M26" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="O26" s="6">
         <v>1.27</v>
       </c>
-      <c r="P25" s="8">
+      <c r="P26" s="6">
         <v>1.1499999999999999</v>
       </c>
-      <c r="Q25" s="9">
+      <c r="Q26" s="7">
         <v>120</v>
       </c>
-      <c r="R25" s="9">
+      <c r="R26" s="7">
         <v>0</v>
       </c>
-      <c r="S25" s="9">
+      <c r="S26" s="7">
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A26" s="3">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
         <v>2023</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B27" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D26" s="3" t="s">
+      <c r="C27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E27" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F26" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H26" s="3" t="s">
+      <c r="F27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H27" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I26" s="3" t="s">
+      <c r="I27" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J26" s="12" t="s">
+      <c r="J27" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="K26" s="3" t="s">
+      <c r="K27" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="L26" s="3">
+      <c r="L27" s="1">
         <v>17.77</v>
       </c>
-      <c r="M26" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="N26" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="O26" s="3">
+      <c r="M27" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="O27" s="1">
         <v>0.64</v>
       </c>
-      <c r="P26" s="3">
+      <c r="P27" s="1">
         <v>0.57999999999999996</v>
       </c>
-      <c r="Q26" s="9">
+      <c r="Q27" s="7">
         <v>120</v>
       </c>
-      <c r="R26" s="9">
+      <c r="R27" s="7">
         <v>0</v>
       </c>
-      <c r="S26" s="9">
+      <c r="S27" s="7">
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A27" s="3">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
         <v>2023</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B28" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27" s="3" t="s">
+      <c r="C28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E28" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="F27" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H27" s="3" t="s">
+      <c r="F28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H28" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I27" s="3" t="s">
+      <c r="I28" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J27" s="12" t="s">
+      <c r="J28" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="K27" s="3" t="s">
+      <c r="K28" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="L27" s="3">
+      <c r="L28" s="1">
         <v>17.77</v>
       </c>
-      <c r="M27" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="N27" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="O27" s="3">
+      <c r="M28" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="O28" s="1">
         <v>0.95</v>
       </c>
-      <c r="P27" s="3">
+      <c r="P28" s="1">
         <v>0.86</v>
       </c>
-      <c r="Q27" s="8">
+      <c r="Q28" s="6">
         <v>120</v>
       </c>
-      <c r="R27" s="8">
+      <c r="R28" s="6">
         <v>0</v>
       </c>
-      <c r="S27" s="8">
+      <c r="S28" s="6">
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:19" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="17">
+    <row r="29" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="15">
         <v>2035</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B29" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C29" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="D28" s="17" t="s">
+      <c r="D29" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="E28" s="17" t="s">
+      <c r="E29" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="F28" s="17" t="s">
+      <c r="F29" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="G28" s="20" t="s">
+      <c r="G29" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="H28" s="17" t="s">
+      <c r="H29" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I28" s="17" t="s">
+      <c r="I29" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="J28" s="18" t="s">
+      <c r="J29" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="K28" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="L28" s="17">
+      <c r="K29" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="L29" s="15">
         <v>15.85</v>
       </c>
-      <c r="M28" s="17">
+      <c r="M29" s="15">
         <v>-0.27</v>
       </c>
-      <c r="N28" s="17">
+      <c r="N29" s="15">
         <v>0</v>
       </c>
-      <c r="O28" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="P28" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q28" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="R28" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="S28" s="19" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="14">
+      <c r="O29" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="P29" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q29" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="R29" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="S29" s="17" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="12">
         <v>2035</v>
       </c>
-      <c r="B29" s="14" t="s">
+      <c r="B30" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="C29" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D29" s="14" t="s">
+      <c r="C30" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="E29" s="14" t="s">
+      <c r="E30" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="F29" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G29" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H29" s="14" t="s">
+      <c r="F30" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="I29" s="14" t="s">
+      <c r="I30" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="J29" s="15" t="s">
+      <c r="J30" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="K29" s="14" t="s">
+      <c r="K30" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="L29" s="14">
+      <c r="L30" s="12">
         <v>15.85</v>
       </c>
-      <c r="M29" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="N29" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="O29" s="16">
+      <c r="M30" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="N30" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="O30" s="14">
         <v>1.27</v>
       </c>
-      <c r="P29" s="16">
+      <c r="P30" s="14">
         <v>1.1499999999999999</v>
       </c>
-      <c r="Q29" s="16">
+      <c r="Q30" s="14">
         <v>120</v>
       </c>
-      <c r="R29" s="16">
+      <c r="R30" s="14">
         <v>0</v>
       </c>
-      <c r="S29" s="16">
+      <c r="S30" s="14">
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="14">
+    <row r="31" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="12">
         <v>2035</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="B31" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="C30" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D30" s="14" t="s">
+      <c r="C31" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="E30" s="14" t="s">
+      <c r="E31" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="F30" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G30" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H30" s="14" t="s">
+      <c r="F31" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H31" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="I30" s="14" t="s">
+      <c r="I31" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="J30" s="15" t="s">
+      <c r="J31" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="K30" s="14" t="s">
+      <c r="K31" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="L30" s="14">
+      <c r="L31" s="12">
         <v>18.64</v>
       </c>
-      <c r="M30" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="N30" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="O30" s="16">
+      <c r="M31" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="N31" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="O31" s="14">
         <v>1.27</v>
       </c>
-      <c r="P30" s="16">
+      <c r="P31" s="14">
         <v>1.1499999999999999</v>
       </c>
-      <c r="Q30" s="16">
+      <c r="Q31" s="14">
         <v>120</v>
       </c>
-      <c r="R30" s="16">
+      <c r="R31" s="14">
         <v>0</v>
       </c>
-      <c r="S30" s="16">
+      <c r="S31" s="14">
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="14">
+    <row r="32" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="12">
         <v>2035</v>
       </c>
-      <c r="B31" s="14" t="s">
+      <c r="B32" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="C31" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D31" s="14" t="s">
+      <c r="C32" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="E31" s="14" t="s">
+      <c r="E32" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="F31" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G31" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H31" s="14" t="s">
+      <c r="F32" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H32" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="I31" s="14" t="s">
+      <c r="I32" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="J31" s="15" t="s">
+      <c r="J32" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="K31" s="14" t="s">
+      <c r="K32" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="L31" s="14">
+      <c r="L32" s="12">
         <v>18.64</v>
       </c>
-      <c r="M31" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="N31" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="O31" s="16">
+      <c r="M32" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="N32" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="O32" s="14">
         <v>1.27</v>
       </c>
-      <c r="P31" s="16">
+      <c r="P32" s="14">
         <v>1.1499999999999999</v>
       </c>
-      <c r="Q31" s="16">
+      <c r="Q32" s="14">
         <v>0</v>
       </c>
-      <c r="R31" s="16">
+      <c r="R32" s="14">
         <v>0</v>
       </c>
-      <c r="S31" s="16">
+      <c r="S32" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="14">
+    <row r="33" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="12">
         <v>2035</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B33" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="C32" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D32" s="14" t="s">
+      <c r="C33" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="E32" s="14" t="s">
+      <c r="E33" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="F32" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G32" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H32" s="14" t="s">
+      <c r="F33" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G33" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H33" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="I32" s="14" t="s">
+      <c r="I33" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="J32" s="15" t="s">
+      <c r="J33" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="K32" s="14" t="s">
+      <c r="K33" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="L32" s="14">
+      <c r="L33" s="12">
         <v>18.64</v>
       </c>
-      <c r="M32" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="N32" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="O32" s="14">
+      <c r="M33" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="N33" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="O33" s="12">
         <v>0.95</v>
       </c>
-      <c r="P32" s="14">
+      <c r="P33" s="12">
         <v>0.86</v>
       </c>
-      <c r="Q32" s="16">
+      <c r="Q33" s="14">
         <v>120</v>
       </c>
-      <c r="R32" s="16">
+      <c r="R33" s="14">
         <v>0</v>
       </c>
-      <c r="S32" s="16">
+      <c r="S33" s="14">
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="14">
+    <row r="34" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="12">
         <v>2035</v>
       </c>
-      <c r="B33" s="14" t="s">
+      <c r="B34" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="C33" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D33" s="14" t="s">
+      <c r="C34" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="E33" s="14" t="s">
+      <c r="E34" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="F33" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G33" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H33" s="14" t="s">
+      <c r="F34" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G34" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H34" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="I33" s="14" t="s">
+      <c r="I34" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="J33" s="15" t="s">
+      <c r="J34" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="K33" s="14" t="s">
+      <c r="K34" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="L33" s="14">
+      <c r="L34" s="12">
         <v>18.64</v>
       </c>
-      <c r="M33" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="N33" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="O33" s="14">
+      <c r="M34" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="N34" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="O34" s="12">
         <v>0.95</v>
       </c>
-      <c r="P33" s="14">
+      <c r="P34" s="12">
         <v>0.86</v>
       </c>
-      <c r="Q33" s="16">
+      <c r="Q34" s="14">
         <v>0</v>
       </c>
-      <c r="R33" s="16">
+      <c r="R34" s="14">
         <v>0</v>
       </c>
-      <c r="S33" s="16">
+      <c r="S34" s="14">
         <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="24">
+        <v>2050</v>
+      </c>
+      <c r="B35" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="C35" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="D35" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="E35" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="F35" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="G35" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="I35" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="J35" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="K35" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="L35" s="24">
+        <v>17.440000000000001</v>
+      </c>
+      <c r="M35" s="24">
+        <v>-0.33</v>
+      </c>
+      <c r="N35" s="24">
+        <v>0</v>
+      </c>
+      <c r="O35" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="P35" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q35" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="R35" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="S35" s="27" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding RTP21 2025 model run to the list of runs
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECEFF8EC-F77E-40CD-AE77-11BC685F8369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63C60C66-6A53-45D2-8515-87BB61464FC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="137">
   <si>
     <t>year</t>
   </si>
@@ -438,6 +438,15 @@
   </si>
   <si>
     <t>model2-a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025_TM152_FBP_Plus_22 </t>
+  </si>
+  <si>
+    <t>RTP21 2025 run</t>
+  </si>
+  <si>
+    <t>BlueprintNetworks_62\net_2025_Blueprint_TransitCuts_v01</t>
   </si>
 </sst>
 </file>
@@ -925,11 +934,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9564CC59-3725-4FDA-8BF2-0F68CB1B6F5A}">
-  <dimension ref="A1:S35"/>
+  <dimension ref="A1:S36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
+      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -2281,122 +2290,92 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="15">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>2025</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="J29" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="6"/>
+      <c r="S29" s="6"/>
+    </row>
+    <row r="30" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="15">
         <v>2035</v>
       </c>
-      <c r="B29" s="15" t="s">
+      <c r="B30" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="C29" s="15" t="s">
+      <c r="C30" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="D29" s="15" t="s">
+      <c r="D30" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="E29" s="15" t="s">
+      <c r="E30" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="F29" s="15" t="s">
+      <c r="F30" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="G29" s="18" t="s">
+      <c r="G30" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="H29" s="15" t="s">
+      <c r="H30" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I29" s="15" t="s">
+      <c r="I30" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="J29" s="16" t="s">
+      <c r="J30" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="K29" s="15" t="s">
+      <c r="K30" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="L29" s="15">
+      <c r="L30" s="15">
         <v>15.85</v>
       </c>
-      <c r="M29" s="15">
+      <c r="M30" s="15">
         <v>-0.27</v>
       </c>
-      <c r="N29" s="15">
+      <c r="N30" s="15">
         <v>0</v>
       </c>
-      <c r="O29" s="15" t="s">
+      <c r="O30" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="P29" s="15" t="s">
+      <c r="P30" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="Q29" s="17" t="s">
+      <c r="Q30" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="R29" s="17" t="s">
+      <c r="R30" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="S29" s="17" t="s">
+      <c r="S30" s="17" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="12">
-        <v>2035</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="F30" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G30" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H30" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I30" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="J30" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="K30" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="L30" s="12">
-        <v>15.85</v>
-      </c>
-      <c r="M30" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="N30" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="O30" s="14">
-        <v>1.27</v>
-      </c>
-      <c r="P30" s="14">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="Q30" s="14">
-        <v>120</v>
-      </c>
-      <c r="R30" s="14">
-        <v>0</v>
-      </c>
-      <c r="S30" s="14">
-        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -2404,7 +2383,7 @@
         <v>2035</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C31" s="12" t="s">
         <v>18</v>
@@ -2413,7 +2392,7 @@
         <v>104</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F31" s="12" t="s">
         <v>10</v>
@@ -2428,13 +2407,13 @@
         <v>106</v>
       </c>
       <c r="J31" s="13" t="s">
-        <v>111</v>
+        <v>44</v>
       </c>
       <c r="K31" s="12" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="L31" s="12">
-        <v>18.64</v>
+        <v>15.85</v>
       </c>
       <c r="M31" s="12" t="s">
         <v>112</v>
@@ -2463,7 +2442,7 @@
         <v>2035</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C32" s="12" t="s">
         <v>18</v>
@@ -2472,7 +2451,7 @@
         <v>104</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F32" s="12" t="s">
         <v>10</v>
@@ -2487,10 +2466,10 @@
         <v>106</v>
       </c>
       <c r="J32" s="13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K32" s="12" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="L32" s="12">
         <v>18.64</v>
@@ -2508,13 +2487,13 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="Q32" s="14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="R32" s="14">
         <v>0</v>
       </c>
       <c r="S32" s="14">
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -2522,7 +2501,7 @@
         <v>2035</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="C33" s="12" t="s">
         <v>18</v>
@@ -2531,7 +2510,7 @@
         <v>104</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="F33" s="12" t="s">
         <v>10</v>
@@ -2546,10 +2525,10 @@
         <v>106</v>
       </c>
       <c r="J33" s="13" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="K33" s="12" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="L33" s="12">
         <v>18.64</v>
@@ -2560,20 +2539,20 @@
       <c r="N33" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="O33" s="12">
-        <v>0.95</v>
-      </c>
-      <c r="P33" s="12">
-        <v>0.86</v>
+      <c r="O33" s="14">
+        <v>1.27</v>
+      </c>
+      <c r="P33" s="14">
+        <v>1.1499999999999999</v>
       </c>
       <c r="Q33" s="14">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="R33" s="14">
         <v>0</v>
       </c>
       <c r="S33" s="14">
-        <v>45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -2581,7 +2560,7 @@
         <v>2035</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C34" s="12" t="s">
         <v>18</v>
@@ -2590,7 +2569,7 @@
         <v>104</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F34" s="12" t="s">
         <v>10</v>
@@ -2605,10 +2584,10 @@
         <v>106</v>
       </c>
       <c r="J34" s="13" t="s">
-        <v>43</v>
+        <v>111</v>
       </c>
       <c r="K34" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="L34" s="12">
         <v>18.64</v>
@@ -2626,68 +2605,127 @@
         <v>0.86</v>
       </c>
       <c r="Q34" s="14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="R34" s="14">
         <v>0</v>
       </c>
       <c r="S34" s="14">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G35" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H35" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I35" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="J35" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K35" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="L35" s="12">
+        <v>18.64</v>
+      </c>
+      <c r="M35" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="N35" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="O35" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="P35" s="12">
+        <v>0.86</v>
+      </c>
+      <c r="Q35" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="24">
+      <c r="R35" s="14">
+        <v>0</v>
+      </c>
+      <c r="S35" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="24">
         <v>2050</v>
       </c>
-      <c r="B35" s="24" t="s">
+      <c r="B36" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="C35" s="24" t="s">
+      <c r="C36" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D35" s="24" t="s">
+      <c r="D36" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="E35" s="24" t="s">
+      <c r="E36" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="F35" s="24" t="s">
+      <c r="F36" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="G35" s="25" t="s">
+      <c r="G36" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="I35" s="24" t="s">
+      <c r="I36" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="J35" s="26" t="s">
+      <c r="J36" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="K35" s="24" t="s">
+      <c r="K36" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="L35" s="24">
+      <c r="L36" s="24">
         <v>17.440000000000001</v>
       </c>
-      <c r="M35" s="24">
+      <c r="M36" s="24">
         <v>-0.33</v>
       </c>
-      <c r="N35" s="24">
+      <c r="N36" s="24">
         <v>0</v>
       </c>
-      <c r="O35" s="24" t="s">
+      <c r="O36" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="P35" s="24" t="s">
+      <c r="P36" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="Q35" s="27" t="s">
+      <c r="Q36" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="R35" s="27" t="s">
+      <c r="R36" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="S35" s="27" t="s">
+      <c r="S36" s="27" t="s">
         <v>112</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added three more 2023 test runs with different WFH or Transit Hesitance factors
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63C60C66-6A53-45D2-8515-87BB61464FC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{986A8FC1-D5C3-4CA8-B285-149D143D1C2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="146">
   <si>
     <t>year</t>
   </si>
@@ -447,6 +447,33 @@
   </si>
   <si>
     <t>BlueprintNetworks_62\net_2025_Blueprint_TransitCuts_v01</t>
+  </si>
+  <si>
+    <t>WFH at 25%, trn hes=200, 0, 50</t>
+  </si>
+  <si>
+    <t>WFH at 25%, trn hes=300, 0, 50</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1205620374882148/f</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1205606356917109/f</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1205620374882150/f</t>
+  </si>
+  <si>
+    <t>2023_TM160_IPA_22</t>
+  </si>
+  <si>
+    <t>2023_TM160_IPA_23</t>
+  </si>
+  <si>
+    <t>2023_TM160_IPA_24</t>
+  </si>
+  <si>
+    <t>WFH at 10%, trn hes=300, 0, 50</t>
   </si>
 </sst>
 </file>
@@ -495,7 +522,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -532,6 +559,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -563,7 +596,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -620,6 +653,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -934,11 +977,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9564CC59-3725-4FDA-8BF2-0F68CB1B6F5A}">
-  <dimension ref="A1:S36"/>
+  <dimension ref="A1:S39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -2290,269 +2333,260 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A29" s="1">
+    <row r="29" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="31">
+        <v>2023</v>
+      </c>
+      <c r="B29" s="31" t="s">
+        <v>142</v>
+      </c>
+      <c r="C29" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="31" t="s">
+        <v>137</v>
+      </c>
+      <c r="F29" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="H29" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="I29" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="J29" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="K29" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="M29" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="N29" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="O29" s="31">
+        <v>0.95</v>
+      </c>
+      <c r="P29" s="31">
+        <v>0.86</v>
+      </c>
+      <c r="Q29" s="33">
+        <v>200</v>
+      </c>
+      <c r="R29" s="33">
+        <v>0</v>
+      </c>
+      <c r="S29" s="33">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="31">
+        <v>2023</v>
+      </c>
+      <c r="B30" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="C30" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="F30" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="I30" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="J30" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="K30" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="M30" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="N30" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="O30" s="31">
+        <v>0.95</v>
+      </c>
+      <c r="P30" s="31">
+        <v>0.86</v>
+      </c>
+      <c r="Q30" s="33">
+        <v>300</v>
+      </c>
+      <c r="R30" s="33">
+        <v>0</v>
+      </c>
+      <c r="S30" s="33">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="31">
+        <v>2023</v>
+      </c>
+      <c r="B31" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="C31" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="F31" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="G31" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="H31" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="I31" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="J31" s="32" t="s">
+        <v>133</v>
+      </c>
+      <c r="K31" s="31" t="s">
+        <v>141</v>
+      </c>
+      <c r="M31" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="N31" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="O31" s="31">
+        <v>0.39</v>
+      </c>
+      <c r="P31" s="31">
+        <v>0.35</v>
+      </c>
+      <c r="Q31" s="33">
+        <v>300</v>
+      </c>
+      <c r="R31" s="33">
+        <v>0</v>
+      </c>
+      <c r="S31" s="33">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="28">
         <v>2025</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B32" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C32" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D32" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E32" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="H32" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="I29" s="1" t="s">
+      <c r="I32" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="J29" s="10" t="s">
+      <c r="J32" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="Q29" s="6"/>
-      <c r="R29" s="6"/>
-      <c r="S29" s="6"/>
-    </row>
-    <row r="30" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="15">
+      <c r="Q32" s="30"/>
+      <c r="R32" s="30"/>
+      <c r="S32" s="30"/>
+    </row>
+    <row r="33" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="15">
         <v>2035</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B33" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="C30" s="15" t="s">
+      <c r="C33" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="D30" s="15" t="s">
+      <c r="D33" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="E30" s="15" t="s">
+      <c r="E33" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="F30" s="15" t="s">
+      <c r="F33" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="G30" s="18" t="s">
+      <c r="G33" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="H30" s="15" t="s">
+      <c r="H33" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I30" s="15" t="s">
+      <c r="I33" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="J30" s="16" t="s">
+      <c r="J33" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="K30" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="L30" s="15">
+      <c r="K33" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="L33" s="15">
         <v>15.85</v>
       </c>
-      <c r="M30" s="15">
+      <c r="M33" s="15">
         <v>-0.27</v>
       </c>
-      <c r="N30" s="15">
+      <c r="N33" s="15">
         <v>0</v>
       </c>
-      <c r="O30" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="P30" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q30" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="R30" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="S30" s="17" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="12">
-        <v>2035</v>
-      </c>
-      <c r="B31" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="C31" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="F31" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G31" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H31" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I31" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="J31" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="K31" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="L31" s="12">
-        <v>15.85</v>
-      </c>
-      <c r="M31" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="N31" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="O31" s="14">
-        <v>1.27</v>
-      </c>
-      <c r="P31" s="14">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="Q31" s="14">
-        <v>120</v>
-      </c>
-      <c r="R31" s="14">
-        <v>0</v>
-      </c>
-      <c r="S31" s="14">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="12">
-        <v>2035</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="E32" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="F32" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G32" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H32" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I32" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="J32" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="K32" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="L32" s="12">
-        <v>18.64</v>
-      </c>
-      <c r="M32" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="N32" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="O32" s="14">
-        <v>1.27</v>
-      </c>
-      <c r="P32" s="14">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="Q32" s="14">
-        <v>120</v>
-      </c>
-      <c r="R32" s="14">
-        <v>0</v>
-      </c>
-      <c r="S32" s="14">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="12">
-        <v>2035</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="F33" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G33" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H33" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I33" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="J33" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="K33" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="L33" s="12">
-        <v>18.64</v>
-      </c>
-      <c r="M33" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="N33" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="O33" s="14">
-        <v>1.27</v>
-      </c>
-      <c r="P33" s="14">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="Q33" s="14">
-        <v>0</v>
-      </c>
-      <c r="R33" s="14">
-        <v>0</v>
-      </c>
-      <c r="S33" s="14">
-        <v>0</v>
+      <c r="O33" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="P33" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q33" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="R33" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="S33" s="17" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="34" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -2560,7 +2594,7 @@
         <v>2035</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="C34" s="12" t="s">
         <v>18</v>
@@ -2569,7 +2603,7 @@
         <v>104</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="F34" s="12" t="s">
         <v>10</v>
@@ -2584,13 +2618,13 @@
         <v>106</v>
       </c>
       <c r="J34" s="13" t="s">
-        <v>111</v>
+        <v>44</v>
       </c>
       <c r="K34" s="12" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="L34" s="12">
-        <v>18.64</v>
+        <v>15.85</v>
       </c>
       <c r="M34" s="12" t="s">
         <v>112</v>
@@ -2598,11 +2632,11 @@
       <c r="N34" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="O34" s="12">
-        <v>0.95</v>
-      </c>
-      <c r="P34" s="12">
-        <v>0.86</v>
+      <c r="O34" s="14">
+        <v>1.27</v>
+      </c>
+      <c r="P34" s="14">
+        <v>1.1499999999999999</v>
       </c>
       <c r="Q34" s="14">
         <v>120</v>
@@ -2619,7 +2653,7 @@
         <v>2035</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="C35" s="12" t="s">
         <v>18</v>
@@ -2628,7 +2662,7 @@
         <v>104</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="F35" s="12" t="s">
         <v>10</v>
@@ -2643,10 +2677,10 @@
         <v>106</v>
       </c>
       <c r="J35" s="13" t="s">
-        <v>43</v>
+        <v>111</v>
       </c>
       <c r="K35" s="12" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="L35" s="12">
         <v>18.64</v>
@@ -2657,75 +2691,252 @@
       <c r="N35" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="O35" s="12">
-        <v>0.95</v>
-      </c>
-      <c r="P35" s="12">
-        <v>0.86</v>
+      <c r="O35" s="14">
+        <v>1.27</v>
+      </c>
+      <c r="P35" s="14">
+        <v>1.1499999999999999</v>
       </c>
       <c r="Q35" s="14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="R35" s="14">
         <v>0</v>
       </c>
       <c r="S35" s="14">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G36" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H36" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I36" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="J36" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="K36" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="L36" s="12">
+        <v>18.64</v>
+      </c>
+      <c r="M36" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="N36" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="O36" s="14">
+        <v>1.27</v>
+      </c>
+      <c r="P36" s="14">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="Q36" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="24">
+      <c r="R36" s="14">
+        <v>0</v>
+      </c>
+      <c r="S36" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G37" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H37" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I37" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="J37" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="K37" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="L37" s="12">
+        <v>18.64</v>
+      </c>
+      <c r="M37" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="N37" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="O37" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="P37" s="12">
+        <v>0.86</v>
+      </c>
+      <c r="Q37" s="14">
+        <v>120</v>
+      </c>
+      <c r="R37" s="14">
+        <v>0</v>
+      </c>
+      <c r="S37" s="14">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H38" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I38" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="J38" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K38" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="L38" s="12">
+        <v>18.64</v>
+      </c>
+      <c r="M38" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="N38" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="O38" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="P38" s="12">
+        <v>0.86</v>
+      </c>
+      <c r="Q38" s="14">
+        <v>0</v>
+      </c>
+      <c r="R38" s="14">
+        <v>0</v>
+      </c>
+      <c r="S38" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="24">
         <v>2050</v>
       </c>
-      <c r="B36" s="24" t="s">
+      <c r="B39" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="C36" s="24" t="s">
+      <c r="C39" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D36" s="24" t="s">
+      <c r="D39" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="E36" s="24" t="s">
+      <c r="E39" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="F36" s="24" t="s">
+      <c r="F39" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="G36" s="25" t="s">
+      <c r="G39" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="I36" s="24" t="s">
+      <c r="I39" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="J36" s="26" t="s">
+      <c r="J39" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="K36" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="L36" s="24">
+      <c r="K39" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="L39" s="24">
         <v>17.440000000000001</v>
       </c>
-      <c r="M36" s="24">
+      <c r="M39" s="24">
         <v>-0.33</v>
       </c>
-      <c r="N36" s="24">
+      <c r="N39" s="24">
         <v>0</v>
       </c>
-      <c r="O36" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="P36" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q36" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="R36" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="S36" s="27" t="s">
+      <c r="O39" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="P39" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q39" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="R39" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="S39" s="27" t="s">
         <v>112</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added a new run to the log - 2023 v25 (WFH at 20%, trn hes=400, 0, 40)
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{986A8FC1-D5C3-4CA8-B285-149D143D1C2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F87356E-53FC-4A56-8C58-032639D85C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="149">
   <si>
     <t>year</t>
   </si>
@@ -474,6 +474,15 @@
   </si>
   <si>
     <t>WFH at 10%, trn hes=300, 0, 50</t>
+  </si>
+  <si>
+    <t>WFH at 20%, trn hes=400, 0, 40</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1205620374882153/f</t>
+  </si>
+  <si>
+    <t>2023_TM160_IPA_25</t>
   </si>
 </sst>
 </file>
@@ -596,7 +605,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -658,11 +667,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -977,11 +981,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9564CC59-3725-4FDA-8BF2-0F68CB1B6F5A}">
-  <dimension ref="A1:S39"/>
+  <dimension ref="A1:S40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -2333,319 +2337,328 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="31">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
         <v>2023</v>
       </c>
-      <c r="B29" s="31" t="s">
+      <c r="B29" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C29" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="D29" s="31" t="s">
+      <c r="C29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E29" s="31" t="s">
+      <c r="E29" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="F29" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="G29" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="H29" s="31" t="s">
+      <c r="F29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H29" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I29" s="31" t="s">
+      <c r="I29" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J29" s="32" t="s">
+      <c r="J29" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="K29" s="31" t="s">
+      <c r="K29" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="M29" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="N29" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="O29" s="31">
+      <c r="L29" s="1">
+        <v>17.77</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="O29" s="1">
         <v>0.95</v>
       </c>
-      <c r="P29" s="31">
+      <c r="P29" s="1">
         <v>0.86</v>
       </c>
-      <c r="Q29" s="33">
+      <c r="Q29" s="6">
         <v>200</v>
       </c>
-      <c r="R29" s="33">
+      <c r="R29" s="6">
         <v>0</v>
       </c>
-      <c r="S29" s="33">
+      <c r="S29" s="6">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="31">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
         <v>2023</v>
       </c>
-      <c r="B30" s="31" t="s">
+      <c r="B30" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C30" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="D30" s="31" t="s">
+      <c r="C30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E30" s="31" t="s">
+      <c r="E30" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="F30" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="G30" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="H30" s="31" t="s">
+      <c r="F30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I30" s="31" t="s">
+      <c r="I30" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J30" s="32" t="s">
+      <c r="J30" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="K30" s="31" t="s">
+      <c r="K30" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="M30" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="N30" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="O30" s="31">
+      <c r="L30" s="1">
+        <v>17.77</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="O30" s="1">
         <v>0.95</v>
       </c>
-      <c r="P30" s="31">
+      <c r="P30" s="1">
         <v>0.86</v>
       </c>
-      <c r="Q30" s="33">
+      <c r="Q30" s="6">
         <v>300</v>
       </c>
-      <c r="R30" s="33">
+      <c r="R30" s="6">
         <v>0</v>
       </c>
-      <c r="S30" s="33">
+      <c r="S30" s="6">
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="31">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
         <v>2023</v>
       </c>
-      <c r="B31" s="31" t="s">
+      <c r="B31" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C31" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="D31" s="31" t="s">
+      <c r="C31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E31" s="31" t="s">
+      <c r="E31" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="F31" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="G31" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="H31" s="31" t="s">
+      <c r="F31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H31" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I31" s="31" t="s">
+      <c r="I31" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J31" s="32" t="s">
+      <c r="J31" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="K31" s="31" t="s">
+      <c r="K31" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="M31" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="N31" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="O31" s="31">
+      <c r="L31" s="1">
+        <v>17.77</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="O31" s="1">
         <v>0.39</v>
       </c>
-      <c r="P31" s="31">
+      <c r="P31" s="1">
         <v>0.35</v>
       </c>
-      <c r="Q31" s="33">
+      <c r="Q31" s="6">
         <v>300</v>
       </c>
-      <c r="R31" s="33">
+      <c r="R31" s="6">
         <v>0</v>
       </c>
-      <c r="S31" s="33">
+      <c r="S31" s="6">
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="28">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J32" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="L32" s="1">
+        <v>17.77</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="O32" s="1">
+        <v>0.77</v>
+      </c>
+      <c r="P32" s="1">
+        <v>0.69</v>
+      </c>
+      <c r="Q32" s="6">
+        <v>400</v>
+      </c>
+      <c r="R32" s="6">
+        <v>0</v>
+      </c>
+      <c r="S32" s="6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="28">
         <v>2025</v>
       </c>
-      <c r="B32" s="28" t="s">
+      <c r="B33" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="C32" s="28" t="s">
+      <c r="C33" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="D32" s="28" t="s">
+      <c r="D33" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="E32" s="28" t="s">
+      <c r="E33" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="H32" s="28" t="s">
+      <c r="H33" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="I32" s="28" t="s">
+      <c r="I33" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="J32" s="29" t="s">
+      <c r="J33" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="Q32" s="30"/>
-      <c r="R32" s="30"/>
-      <c r="S32" s="30"/>
-    </row>
-    <row r="33" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="15">
+      <c r="Q33" s="30"/>
+      <c r="R33" s="30"/>
+      <c r="S33" s="30"/>
+    </row>
+    <row r="34" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="15">
         <v>2035</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B34" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="C33" s="15" t="s">
+      <c r="C34" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="D33" s="15" t="s">
+      <c r="D34" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="E33" s="15" t="s">
+      <c r="E34" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="F33" s="15" t="s">
+      <c r="F34" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="G33" s="18" t="s">
+      <c r="G34" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="H33" s="15" t="s">
+      <c r="H34" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I33" s="15" t="s">
+      <c r="I34" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="J33" s="16" t="s">
+      <c r="J34" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="K33" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="L33" s="15">
+      <c r="K34" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="L34" s="15">
         <v>15.85</v>
       </c>
-      <c r="M33" s="15">
+      <c r="M34" s="15">
         <v>-0.27</v>
       </c>
-      <c r="N33" s="15">
+      <c r="N34" s="15">
         <v>0</v>
       </c>
-      <c r="O33" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="P33" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q33" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="R33" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="S33" s="17" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="12">
-        <v>2035</v>
-      </c>
-      <c r="B34" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D34" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="E34" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="F34" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G34" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H34" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I34" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="J34" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="K34" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="L34" s="12">
-        <v>15.85</v>
-      </c>
-      <c r="M34" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="N34" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="O34" s="14">
-        <v>1.27</v>
-      </c>
-      <c r="P34" s="14">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="Q34" s="14">
-        <v>120</v>
-      </c>
-      <c r="R34" s="14">
-        <v>0</v>
-      </c>
-      <c r="S34" s="14">
-        <v>45</v>
+      <c r="O34" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="P34" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q34" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="R34" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="S34" s="17" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="35" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -2653,7 +2666,7 @@
         <v>2035</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C35" s="12" t="s">
         <v>18</v>
@@ -2662,7 +2675,7 @@
         <v>104</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F35" s="12" t="s">
         <v>10</v>
@@ -2677,13 +2690,13 @@
         <v>106</v>
       </c>
       <c r="J35" s="13" t="s">
-        <v>111</v>
+        <v>44</v>
       </c>
       <c r="K35" s="12" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="L35" s="12">
-        <v>18.64</v>
+        <v>15.85</v>
       </c>
       <c r="M35" s="12" t="s">
         <v>112</v>
@@ -2712,7 +2725,7 @@
         <v>2035</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C36" s="12" t="s">
         <v>18</v>
@@ -2721,7 +2734,7 @@
         <v>104</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F36" s="12" t="s">
         <v>10</v>
@@ -2736,10 +2749,10 @@
         <v>106</v>
       </c>
       <c r="J36" s="13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K36" s="12" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="L36" s="12">
         <v>18.64</v>
@@ -2757,13 +2770,13 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="Q36" s="14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="R36" s="14">
         <v>0</v>
       </c>
       <c r="S36" s="14">
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -2771,7 +2784,7 @@
         <v>2035</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="C37" s="12" t="s">
         <v>18</v>
@@ -2780,7 +2793,7 @@
         <v>104</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="F37" s="12" t="s">
         <v>10</v>
@@ -2795,10 +2808,10 @@
         <v>106</v>
       </c>
       <c r="J37" s="13" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="K37" s="12" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="L37" s="12">
         <v>18.64</v>
@@ -2809,20 +2822,20 @@
       <c r="N37" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="O37" s="12">
-        <v>0.95</v>
-      </c>
-      <c r="P37" s="12">
-        <v>0.86</v>
+      <c r="O37" s="14">
+        <v>1.27</v>
+      </c>
+      <c r="P37" s="14">
+        <v>1.1499999999999999</v>
       </c>
       <c r="Q37" s="14">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="R37" s="14">
         <v>0</v>
       </c>
       <c r="S37" s="14">
-        <v>45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -2830,7 +2843,7 @@
         <v>2035</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C38" s="12" t="s">
         <v>18</v>
@@ -2839,7 +2852,7 @@
         <v>104</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F38" s="12" t="s">
         <v>10</v>
@@ -2854,10 +2867,10 @@
         <v>106</v>
       </c>
       <c r="J38" s="13" t="s">
-        <v>43</v>
+        <v>111</v>
       </c>
       <c r="K38" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="L38" s="12">
         <v>18.64</v>
@@ -2875,68 +2888,127 @@
         <v>0.86</v>
       </c>
       <c r="Q38" s="14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="R38" s="14">
         <v>0</v>
       </c>
       <c r="S38" s="14">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G39" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H39" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I39" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="J39" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K39" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="L39" s="12">
+        <v>18.64</v>
+      </c>
+      <c r="M39" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="N39" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="O39" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="P39" s="12">
+        <v>0.86</v>
+      </c>
+      <c r="Q39" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="24">
+      <c r="R39" s="14">
+        <v>0</v>
+      </c>
+      <c r="S39" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="24">
         <v>2050</v>
       </c>
-      <c r="B39" s="24" t="s">
+      <c r="B40" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="C39" s="24" t="s">
+      <c r="C40" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D39" s="24" t="s">
+      <c r="D40" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="E39" s="24" t="s">
+      <c r="E40" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="F39" s="24" t="s">
+      <c r="F40" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="G39" s="25" t="s">
+      <c r="G40" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="I39" s="24" t="s">
+      <c r="I40" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="J39" s="26" t="s">
+      <c r="J40" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="K39" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="L39" s="24">
+      <c r="K40" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="L40" s="24">
         <v>17.440000000000001</v>
       </c>
-      <c r="M39" s="24">
+      <c r="M40" s="24">
         <v>-0.33</v>
       </c>
-      <c r="N39" s="24">
+      <c r="N40" s="24">
         <v>0</v>
       </c>
-      <c r="O39" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="P39" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q39" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="R39" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="S39" s="27" t="s">
+      <c r="O40" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="P40" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q40" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="R40" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="S40" s="27" t="s">
         <v>112</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add Initial TM160 runs for 2005 and 2015
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F87356E-53FC-4A56-8C58-032639D85C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D8D906-C16F-4756-8160-2DCF5880FB72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="157">
   <si>
     <t>year</t>
   </si>
@@ -483,6 +483,30 @@
   </si>
   <si>
     <t>2023_TM160_IPA_25</t>
+  </si>
+  <si>
+    <t>2015_TM160_IPA_01</t>
+  </si>
+  <si>
+    <t>BlueprintNetworks_v09\net_2015_Blueprint</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1205634764978037/f</t>
+  </si>
+  <si>
+    <t>2005_TM160_IPA_01</t>
+  </si>
+  <si>
+    <t>Initial TM160 2015 run</t>
+  </si>
+  <si>
+    <t>Initial TM160 2005 run</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1205634764978035/f</t>
+  </si>
+  <si>
+    <t>\RTP2021\IncrementalProgress\2005_TM152_IPA_03\INPUT</t>
   </si>
 </sst>
 </file>
@@ -531,7 +555,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -574,6 +598,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -605,7 +641,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -667,6 +703,53 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -981,11 +1064,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9564CC59-3725-4FDA-8BF2-0F68CB1B6F5A}">
-  <dimension ref="A1:S40"/>
+  <dimension ref="A1:S42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K32" sqref="K32"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1002,7 +1085,8 @@
     <col min="10" max="10" width="11.26953125" style="10" customWidth="1"/>
     <col min="11" max="11" width="17.54296875" style="1" customWidth="1"/>
     <col min="12" max="12" width="5.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.1796875" style="1"/>
+    <col min="13" max="14" width="9.1796875" style="45"/>
+    <col min="15" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="5" customFormat="1" ht="52" x14ac:dyDescent="0.3">
@@ -1042,10 +1126,10 @@
       <c r="L1" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="40" t="s">
         <v>39</v>
       </c>
       <c r="O1" s="4" t="s">
@@ -1086,151 +1170,170 @@
         <v>12</v>
       </c>
       <c r="J2" s="22"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
       <c r="O2" s="23"/>
       <c r="P2" s="23"/>
       <c r="Q2" s="23"/>
       <c r="R2" s="23"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="10">
+    <row r="3" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="31">
+        <v>2005</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="J3" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="K3" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="L3" s="33">
+        <v>14.87</v>
+      </c>
+      <c r="M3" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="N3" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="O3" s="35">
+        <v>0</v>
+      </c>
+      <c r="P3" s="35">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="35">
+        <v>0</v>
+      </c>
+      <c r="R3" s="35">
+        <v>0</v>
+      </c>
+      <c r="S3" s="35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="36">
         <v>2015</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="C4" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E4" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="F4" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I4" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J4" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K4" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="M3" s="6">
+      <c r="M4" s="43">
         <v>-0.09</v>
       </c>
-      <c r="N3" s="6">
+      <c r="N4" s="43">
         <v>0.9</v>
       </c>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6">
-        <v>0</v>
-      </c>
-      <c r="R3" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>2023</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="O4" s="39"/>
+      <c r="P4" s="39"/>
+      <c r="Q4" s="39">
+        <v>0</v>
+      </c>
+      <c r="R4" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="36">
+        <v>2015</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>149</v>
+      </c>
+      <c r="C5" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M4" s="6">
-        <v>-0.44</v>
-      </c>
-      <c r="N4" s="6">
-        <v>-0.23</v>
-      </c>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6">
-        <v>0</v>
-      </c>
-      <c r="R4" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>2023</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="M5" s="6">
-        <v>-1.25</v>
-      </c>
-      <c r="N5" s="6">
-        <v>-0.75</v>
-      </c>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6">
-        <v>30</v>
-      </c>
-      <c r="R5" s="6">
+      <c r="E5" s="37" t="s">
+        <v>153</v>
+      </c>
+      <c r="F5" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="37" t="s">
+        <v>150</v>
+      </c>
+      <c r="J5" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="M5" s="43" t="s">
+        <v>112</v>
+      </c>
+      <c r="N5" s="43" t="s">
+        <v>112</v>
+      </c>
+      <c r="O5" s="39">
+        <v>0</v>
+      </c>
+      <c r="P5" s="39">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="39">
+        <v>0</v>
+      </c>
+      <c r="R5" s="39">
+        <v>0</v>
+      </c>
+      <c r="S5" s="39">
         <v>0</v>
       </c>
     </row>
@@ -1239,7 +1342,7 @@
         <v>2023</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>18</v>
@@ -1248,7 +1351,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>10</v>
@@ -1257,27 +1360,27 @@
         <v>11</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="J6" s="9" t="s">
         <v>17</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M6" s="6">
-        <v>-1.25</v>
-      </c>
-      <c r="N6" s="6">
-        <v>-0.75</v>
+        <v>25</v>
+      </c>
+      <c r="M6" s="44">
+        <v>-0.44</v>
+      </c>
+      <c r="N6" s="44">
+        <v>-0.23</v>
       </c>
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
       <c r="Q6" s="6">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="R6" s="6">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
@@ -1285,7 +1388,7 @@
         <v>2023</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>18</v>
@@ -1294,7 +1397,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>10</v>
@@ -1303,27 +1406,27 @@
         <v>11</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="J7" s="9" t="s">
         <v>17</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M7" s="6">
+        <v>26</v>
+      </c>
+      <c r="M7" s="44">
         <v>-1.25</v>
       </c>
-      <c r="N7" s="6">
+      <c r="N7" s="44">
         <v>-0.75</v>
       </c>
       <c r="O7" s="6"/>
       <c r="P7" s="6"/>
       <c r="Q7" s="6">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="R7" s="6">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
@@ -1331,7 +1434,7 @@
         <v>2023</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>18</v>
@@ -1340,7 +1443,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>10</v>
@@ -1349,26 +1452,26 @@
         <v>11</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J8" s="9" t="s">
         <v>17</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="M8" s="6">
+        <v>30</v>
+      </c>
+      <c r="M8" s="44">
         <v>-1.25</v>
       </c>
-      <c r="N8" s="6">
+      <c r="N8" s="44">
         <v>-0.75</v>
       </c>
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
-      <c r="Q8" s="11">
-        <v>75</v>
-      </c>
-      <c r="R8" s="11">
+      <c r="Q8" s="6">
+        <v>45</v>
+      </c>
+      <c r="R8" s="6">
         <v>15</v>
       </c>
     </row>
@@ -1377,7 +1480,7 @@
         <v>2023</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>18</v>
@@ -1386,7 +1489,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>10</v>
@@ -1398,23 +1501,23 @@
         <v>33</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="M9" s="6">
+        <v>32</v>
+      </c>
+      <c r="M9" s="44">
         <v>-1.25</v>
       </c>
-      <c r="N9" s="6">
+      <c r="N9" s="44">
         <v>-0.75</v>
       </c>
       <c r="O9" s="6"/>
       <c r="P9" s="6"/>
-      <c r="Q9" s="7">
-        <v>85</v>
-      </c>
-      <c r="R9" s="7">
+      <c r="Q9" s="6">
+        <v>75</v>
+      </c>
+      <c r="R9" s="6">
         <v>15</v>
       </c>
     </row>
@@ -1423,7 +1526,7 @@
         <v>2023</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>18</v>
@@ -1432,7 +1535,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>10</v>
@@ -1444,23 +1547,23 @@
         <v>33</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="M10" s="6">
+        <v>35</v>
+      </c>
+      <c r="M10" s="44">
         <v>-1.25</v>
       </c>
-      <c r="N10" s="6">
+      <c r="N10" s="44">
         <v>-0.75</v>
       </c>
       <c r="O10" s="6"/>
       <c r="P10" s="6"/>
-      <c r="Q10" s="7">
-        <v>95</v>
-      </c>
-      <c r="R10" s="7">
+      <c r="Q10" s="11">
+        <v>75</v>
+      </c>
+      <c r="R10" s="11">
         <v>15</v>
       </c>
     </row>
@@ -1469,7 +1572,7 @@
         <v>2023</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>18</v>
@@ -1490,15 +1593,15 @@
         <v>33</v>
       </c>
       <c r="J11" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="M11" s="6">
+      <c r="M11" s="44">
         <v>-1.25</v>
       </c>
-      <c r="N11" s="6">
+      <c r="N11" s="44">
         <v>-0.75</v>
       </c>
       <c r="O11" s="6"/>
@@ -1507,7 +1610,7 @@
         <v>85</v>
       </c>
       <c r="R11" s="7">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
@@ -1515,7 +1618,7 @@
         <v>2023</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>18</v>
@@ -1524,7 +1627,7 @@
         <v>7</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>10</v>
@@ -1533,27 +1636,27 @@
         <v>11</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J12" s="10" t="s">
-        <v>43</v>
+        <v>33</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="M12" s="6">
+        <v>46</v>
+      </c>
+      <c r="M12" s="44">
         <v>-1.25</v>
       </c>
-      <c r="N12" s="6">
+      <c r="N12" s="44">
         <v>-0.75</v>
       </c>
       <c r="O12" s="6"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="7">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="R12" s="7">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
@@ -1561,7 +1664,7 @@
         <v>2023</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>18</v>
@@ -1570,7 +1673,7 @@
         <v>7</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>10</v>
@@ -1579,24 +1682,24 @@
         <v>11</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J13" s="10" t="s">
-        <v>43</v>
+        <v>33</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>45</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="M13" s="6">
+        <v>46</v>
+      </c>
+      <c r="M13" s="44">
         <v>-1.25</v>
       </c>
-      <c r="N13" s="6">
+      <c r="N13" s="44">
         <v>-0.75</v>
       </c>
       <c r="O13" s="6"/>
       <c r="P13" s="6"/>
       <c r="Q13" s="7">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="R13" s="7">
         <v>30</v>
@@ -1607,7 +1710,7 @@
         <v>2023</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>18</v>
@@ -1616,7 +1719,7 @@
         <v>7</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>10</v>
@@ -1625,24 +1728,24 @@
         <v>11</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="M14" s="6">
+        <v>51</v>
+      </c>
+      <c r="M14" s="44">
         <v>-1.25</v>
       </c>
-      <c r="N14" s="6">
+      <c r="N14" s="44">
         <v>-0.75</v>
       </c>
       <c r="O14" s="6"/>
       <c r="P14" s="6"/>
       <c r="Q14" s="7">
-        <v>120</v>
+        <v>85</v>
       </c>
       <c r="R14" s="7">
         <v>30</v>
@@ -1653,7 +1756,7 @@
         <v>2023</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>18</v>
@@ -1662,7 +1765,7 @@
         <v>7</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>10</v>
@@ -1671,27 +1774,27 @@
         <v>11</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="J15" s="10" t="s">
         <v>43</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="M15" s="6">
+        <v>57</v>
+      </c>
+      <c r="M15" s="44">
         <v>-1.25</v>
       </c>
-      <c r="N15" s="6">
+      <c r="N15" s="44">
         <v>-0.75</v>
       </c>
       <c r="O15" s="6"/>
       <c r="P15" s="6"/>
       <c r="Q15" s="7">
-        <v>180</v>
+        <v>95</v>
       </c>
       <c r="R15" s="7">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
@@ -1699,7 +1802,7 @@
         <v>2023</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>18</v>
@@ -1708,7 +1811,7 @@
         <v>7</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>10</v>
@@ -1717,27 +1820,27 @@
         <v>11</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="M16" s="6">
+        <v>57</v>
+      </c>
+      <c r="M16" s="44">
         <v>-1.25</v>
       </c>
-      <c r="N16" s="6">
+      <c r="N16" s="44">
         <v>-0.75</v>
       </c>
       <c r="O16" s="6"/>
       <c r="P16" s="6"/>
       <c r="Q16" s="7">
-        <v>300</v>
+        <v>120</v>
       </c>
       <c r="R16" s="7">
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
@@ -1745,7 +1848,7 @@
         <v>2023</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>18</v>
@@ -1754,7 +1857,7 @@
         <v>7</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>10</v>
@@ -1769,21 +1872,21 @@
         <v>43</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="M17" s="6">
+        <v>61</v>
+      </c>
+      <c r="M17" s="44">
         <v>-1.25</v>
       </c>
-      <c r="N17" s="6">
+      <c r="N17" s="44">
         <v>-0.75</v>
       </c>
       <c r="O17" s="6"/>
       <c r="P17" s="6"/>
       <c r="Q17" s="7">
-        <v>250</v>
+        <v>180</v>
       </c>
       <c r="R17" s="7">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
@@ -1791,7 +1894,7 @@
         <v>2023</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>18</v>
@@ -1817,16 +1920,16 @@
       <c r="K18" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="M18" s="6">
+      <c r="M18" s="44">
         <v>-1.25</v>
       </c>
-      <c r="N18" s="6">
+      <c r="N18" s="44">
         <v>-0.75</v>
       </c>
       <c r="O18" s="6"/>
       <c r="P18" s="6"/>
       <c r="Q18" s="7">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="R18" s="7">
         <v>5</v>
@@ -1837,7 +1940,7 @@
         <v>2023</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>18</v>
@@ -1846,7 +1949,7 @@
         <v>7</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>10</v>
@@ -1855,27 +1958,27 @@
         <v>11</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="J19" s="10" t="s">
         <v>43</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="M19" s="6">
+        <v>65</v>
+      </c>
+      <c r="M19" s="44">
         <v>-1.25</v>
       </c>
-      <c r="N19" s="6">
+      <c r="N19" s="44">
         <v>-0.75</v>
       </c>
       <c r="O19" s="6"/>
       <c r="P19" s="6"/>
       <c r="Q19" s="7">
-        <v>120</v>
+        <v>250</v>
       </c>
       <c r="R19" s="7">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
@@ -1883,7 +1986,7 @@
         <v>2023</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>18</v>
@@ -1892,7 +1995,7 @@
         <v>7</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>10</v>
@@ -1901,27 +2004,27 @@
         <v>11</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="J20" s="10" t="s">
         <v>43</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="M20" s="6">
+        <v>65</v>
+      </c>
+      <c r="M20" s="44">
         <v>-1.25</v>
       </c>
-      <c r="N20" s="6">
+      <c r="N20" s="44">
         <v>-0.75</v>
       </c>
       <c r="O20" s="6"/>
       <c r="P20" s="6"/>
       <c r="Q20" s="7">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="R20" s="7">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
@@ -1929,7 +2032,7 @@
         <v>2023</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>18</v>
@@ -1938,7 +2041,7 @@
         <v>7</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>10</v>
@@ -1947,18 +2050,18 @@
         <v>11</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="J21" s="10" t="s">
         <v>43</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="M21" s="6">
+        <v>67</v>
+      </c>
+      <c r="M21" s="44">
         <v>-1.25</v>
       </c>
-      <c r="N21" s="6">
+      <c r="N21" s="44">
         <v>-0.75</v>
       </c>
       <c r="O21" s="6"/>
@@ -1975,7 +2078,7 @@
         <v>2023</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>18</v>
@@ -1984,7 +2087,7 @@
         <v>7</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>10</v>
@@ -1993,20 +2096,22 @@
         <v>11</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>89</v>
+        <v>43</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="O22" s="6">
-        <v>1.27</v>
-      </c>
-      <c r="P22" s="6">
-        <v>1.1499999999999999</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="M22" s="44">
+        <v>-1.25</v>
+      </c>
+      <c r="N22" s="44">
+        <v>-0.75</v>
+      </c>
+      <c r="O22" s="6"/>
+      <c r="P22" s="6"/>
       <c r="Q22" s="7">
         <v>120</v>
       </c>
@@ -2019,7 +2124,7 @@
         <v>2023</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>18</v>
@@ -2028,7 +2133,7 @@
         <v>7</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>10</v>
@@ -2043,12 +2148,12 @@
         <v>43</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="M23" s="6">
+        <v>82</v>
+      </c>
+      <c r="M23" s="44">
         <v>-1.25</v>
       </c>
-      <c r="N23" s="6">
+      <c r="N23" s="44">
         <v>-0.75</v>
       </c>
       <c r="O23" s="6"/>
@@ -2059,16 +2164,13 @@
       <c r="R23" s="7">
         <v>0</v>
       </c>
-      <c r="S23" s="7">
-        <v>30</v>
-      </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>2023</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>18</v>
@@ -2077,7 +2179,7 @@
         <v>7</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>10</v>
@@ -2092,7 +2194,7 @@
         <v>89</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="O24" s="6">
         <v>1.27</v>
@@ -2105,9 +2207,6 @@
       </c>
       <c r="R24" s="7">
         <v>0</v>
-      </c>
-      <c r="S24" s="7">
-        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
@@ -2115,7 +2214,7 @@
         <v>2023</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>18</v>
@@ -2124,16 +2223,13 @@
         <v>7</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>80</v>
@@ -2142,14 +2238,16 @@
         <v>43</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="M25" s="6">
+        <v>90</v>
+      </c>
+      <c r="M25" s="44">
         <v>-1.25</v>
       </c>
-      <c r="N25" s="6">
+      <c r="N25" s="44">
         <v>-0.75</v>
       </c>
+      <c r="O25" s="6"/>
+      <c r="P25" s="6"/>
       <c r="Q25" s="7">
         <v>120</v>
       </c>
@@ -2157,7 +2255,7 @@
         <v>0</v>
       </c>
       <c r="S25" s="7">
-        <v>45</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
@@ -2165,7 +2263,7 @@
         <v>2023</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>18</v>
@@ -2174,16 +2272,13 @@
         <v>7</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>80</v>
@@ -2192,16 +2287,7 @@
         <v>89</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="L26" s="1">
-        <v>17.77</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="N26" s="1" t="s">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="O26" s="6">
         <v>1.27</v>
@@ -2216,7 +2302,7 @@
         <v>0</v>
       </c>
       <c r="S26" s="7">
-        <v>45</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
@@ -2224,7 +2310,7 @@
         <v>2023</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>18</v>
@@ -2233,7 +2319,7 @@
         <v>7</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>10</v>
@@ -2251,22 +2337,13 @@
         <v>43</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="L27" s="1">
-        <v>17.77</v>
-      </c>
-      <c r="M27" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="N27" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="O27" s="1">
-        <v>0.64</v>
-      </c>
-      <c r="P27" s="1">
-        <v>0.57999999999999996</v>
+        <v>94</v>
+      </c>
+      <c r="M27" s="44">
+        <v>-1.25</v>
+      </c>
+      <c r="N27" s="44">
+        <v>-0.75</v>
       </c>
       <c r="Q27" s="7">
         <v>120</v>
@@ -2283,7 +2360,7 @@
         <v>2023</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>18</v>
@@ -2292,7 +2369,7 @@
         <v>7</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>10</v>
@@ -2310,30 +2387,30 @@
         <v>89</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="L28" s="1">
         <v>17.77</v>
       </c>
-      <c r="M28" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="N28" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="O28" s="1">
-        <v>0.95</v>
-      </c>
-      <c r="P28" s="1">
-        <v>0.86</v>
-      </c>
-      <c r="Q28" s="6">
+      <c r="M28" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="N28" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="O28" s="6">
+        <v>1.27</v>
+      </c>
+      <c r="P28" s="6">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="Q28" s="7">
         <v>120</v>
       </c>
-      <c r="R28" s="6">
-        <v>0</v>
-      </c>
-      <c r="S28" s="6">
+      <c r="R28" s="7">
+        <v>0</v>
+      </c>
+      <c r="S28" s="7">
         <v>45</v>
       </c>
     </row>
@@ -2342,7 +2419,7 @@
         <v>2023</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>142</v>
+        <v>95</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>18</v>
@@ -2351,7 +2428,7 @@
         <v>7</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>137</v>
+        <v>97</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>10</v>
@@ -2366,34 +2443,34 @@
         <v>80</v>
       </c>
       <c r="J29" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>140</v>
+        <v>99</v>
       </c>
       <c r="L29" s="1">
         <v>17.77</v>
       </c>
-      <c r="M29" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="N29" s="1" t="s">
+      <c r="M29" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="N29" s="45" t="s">
         <v>112</v>
       </c>
       <c r="O29" s="1">
-        <v>0.95</v>
+        <v>0.64</v>
       </c>
       <c r="P29" s="1">
-        <v>0.86</v>
-      </c>
-      <c r="Q29" s="6">
-        <v>200</v>
-      </c>
-      <c r="R29" s="6">
-        <v>0</v>
-      </c>
-      <c r="S29" s="6">
-        <v>50</v>
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="Q29" s="7">
+        <v>120</v>
+      </c>
+      <c r="R29" s="7">
+        <v>0</v>
+      </c>
+      <c r="S29" s="7">
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
@@ -2401,7 +2478,7 @@
         <v>2023</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>143</v>
+        <v>96</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>18</v>
@@ -2410,7 +2487,7 @@
         <v>7</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>138</v>
+        <v>98</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>10</v>
@@ -2428,15 +2505,15 @@
         <v>89</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>139</v>
+        <v>100</v>
       </c>
       <c r="L30" s="1">
         <v>17.77</v>
       </c>
-      <c r="M30" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="N30" s="1" t="s">
+      <c r="M30" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="N30" s="45" t="s">
         <v>112</v>
       </c>
       <c r="O30" s="1">
@@ -2446,13 +2523,13 @@
         <v>0.86</v>
       </c>
       <c r="Q30" s="6">
-        <v>300</v>
+        <v>120</v>
       </c>
       <c r="R30" s="6">
         <v>0</v>
       </c>
       <c r="S30" s="6">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
@@ -2460,7 +2537,7 @@
         <v>2023</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>18</v>
@@ -2469,7 +2546,7 @@
         <v>7</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>10</v>
@@ -2484,28 +2561,28 @@
         <v>80</v>
       </c>
       <c r="J31" s="10" t="s">
-        <v>133</v>
+        <v>44</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L31" s="1">
         <v>17.77</v>
       </c>
-      <c r="M31" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="N31" s="1" t="s">
+      <c r="M31" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="N31" s="45" t="s">
         <v>112</v>
       </c>
       <c r="O31" s="1">
-        <v>0.39</v>
+        <v>0.95</v>
       </c>
       <c r="P31" s="1">
-        <v>0.35</v>
+        <v>0.86</v>
       </c>
       <c r="Q31" s="6">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="R31" s="6">
         <v>0</v>
@@ -2519,7 +2596,7 @@
         <v>2023</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>18</v>
@@ -2528,7 +2605,7 @@
         <v>7</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>10</v>
@@ -2543,240 +2620,242 @@
         <v>80</v>
       </c>
       <c r="J32" s="10" t="s">
-        <v>44</v>
+        <v>89</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="L32" s="1">
         <v>17.77</v>
       </c>
-      <c r="M32" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="N32" s="1" t="s">
+      <c r="M32" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="N32" s="45" t="s">
         <v>112</v>
       </c>
       <c r="O32" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="P32" s="1">
+        <v>0.86</v>
+      </c>
+      <c r="Q32" s="6">
+        <v>300</v>
+      </c>
+      <c r="R32" s="6">
+        <v>0</v>
+      </c>
+      <c r="S32" s="6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J33" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="L33" s="1">
+        <v>17.77</v>
+      </c>
+      <c r="M33" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="N33" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="O33" s="1">
+        <v>0.39</v>
+      </c>
+      <c r="P33" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="Q33" s="6">
+        <v>300</v>
+      </c>
+      <c r="R33" s="6">
+        <v>0</v>
+      </c>
+      <c r="S33" s="6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J34" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="L34" s="1">
+        <v>17.77</v>
+      </c>
+      <c r="M34" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="N34" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="O34" s="1">
         <v>0.77</v>
       </c>
-      <c r="P32" s="1">
+      <c r="P34" s="1">
         <v>0.69</v>
       </c>
-      <c r="Q32" s="6">
+      <c r="Q34" s="6">
         <v>400</v>
       </c>
-      <c r="R32" s="6">
-        <v>0</v>
-      </c>
-      <c r="S32" s="6">
+      <c r="R34" s="6">
+        <v>0</v>
+      </c>
+      <c r="S34" s="6">
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="28">
+    <row r="35" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="28">
         <v>2025</v>
       </c>
-      <c r="B33" s="28" t="s">
+      <c r="B35" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="C33" s="28" t="s">
+      <c r="C35" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="D33" s="28" t="s">
+      <c r="D35" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="E33" s="28" t="s">
+      <c r="E35" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="H33" s="28" t="s">
+      <c r="H35" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="I33" s="28" t="s">
+      <c r="I35" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="J33" s="29" t="s">
+      <c r="J35" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="Q33" s="30"/>
-      <c r="R33" s="30"/>
-      <c r="S33" s="30"/>
-    </row>
-    <row r="34" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="15">
+      <c r="M35" s="46"/>
+      <c r="N35" s="46"/>
+      <c r="Q35" s="30"/>
+      <c r="R35" s="30"/>
+      <c r="S35" s="30"/>
+    </row>
+    <row r="36" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="15">
         <v>2035</v>
       </c>
-      <c r="B34" s="15" t="s">
+      <c r="B36" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="C34" s="15" t="s">
+      <c r="C36" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="D34" s="15" t="s">
+      <c r="D36" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="E34" s="15" t="s">
+      <c r="E36" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="F34" s="15" t="s">
+      <c r="F36" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="G34" s="18" t="s">
+      <c r="G36" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="H34" s="15" t="s">
+      <c r="H36" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I34" s="15" t="s">
+      <c r="I36" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="J34" s="16" t="s">
+      <c r="J36" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="K34" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="L34" s="15">
+      <c r="K36" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="L36" s="15">
         <v>15.85</v>
       </c>
-      <c r="M34" s="15">
+      <c r="M36" s="47">
         <v>-0.27</v>
       </c>
-      <c r="N34" s="15">
-        <v>0</v>
-      </c>
-      <c r="O34" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="P34" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q34" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="R34" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="S34" s="17" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="12">
-        <v>2035</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D35" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="E35" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="F35" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G35" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H35" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I35" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="J35" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="K35" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="L35" s="12">
-        <v>15.85</v>
-      </c>
-      <c r="M35" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="N35" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="O35" s="14">
-        <v>1.27</v>
-      </c>
-      <c r="P35" s="14">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="Q35" s="14">
-        <v>120</v>
-      </c>
-      <c r="R35" s="14">
-        <v>0</v>
-      </c>
-      <c r="S35" s="14">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="12">
-        <v>2035</v>
-      </c>
-      <c r="B36" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D36" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="E36" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="F36" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G36" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H36" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I36" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="J36" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="K36" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="L36" s="12">
-        <v>18.64</v>
-      </c>
-      <c r="M36" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="N36" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="O36" s="14">
-        <v>1.27</v>
-      </c>
-      <c r="P36" s="14">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="Q36" s="14">
-        <v>120</v>
-      </c>
-      <c r="R36" s="14">
-        <v>0</v>
-      </c>
-      <c r="S36" s="14">
-        <v>45</v>
+      <c r="N36" s="47">
+        <v>0</v>
+      </c>
+      <c r="O36" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="P36" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q36" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="R36" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="S36" s="17" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="37" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -2784,7 +2863,7 @@
         <v>2035</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C37" s="12" t="s">
         <v>18</v>
@@ -2793,7 +2872,7 @@
         <v>104</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F37" s="12" t="s">
         <v>10</v>
@@ -2808,18 +2887,18 @@
         <v>106</v>
       </c>
       <c r="J37" s="13" t="s">
-        <v>113</v>
+        <v>44</v>
       </c>
       <c r="K37" s="12" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="L37" s="12">
-        <v>18.64</v>
-      </c>
-      <c r="M37" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="N37" s="12" t="s">
+        <v>15.85</v>
+      </c>
+      <c r="M37" s="48" t="s">
+        <v>112</v>
+      </c>
+      <c r="N37" s="48" t="s">
         <v>112</v>
       </c>
       <c r="O37" s="14">
@@ -2829,13 +2908,13 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="Q37" s="14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="R37" s="14">
         <v>0</v>
       </c>
       <c r="S37" s="14">
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -2843,7 +2922,7 @@
         <v>2035</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="C38" s="12" t="s">
         <v>18</v>
@@ -2852,7 +2931,7 @@
         <v>104</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="F38" s="12" t="s">
         <v>10</v>
@@ -2870,22 +2949,22 @@
         <v>111</v>
       </c>
       <c r="K38" s="12" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="L38" s="12">
         <v>18.64</v>
       </c>
-      <c r="M38" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="N38" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="O38" s="12">
-        <v>0.95</v>
-      </c>
-      <c r="P38" s="12">
-        <v>0.86</v>
+      <c r="M38" s="48" t="s">
+        <v>112</v>
+      </c>
+      <c r="N38" s="48" t="s">
+        <v>112</v>
+      </c>
+      <c r="O38" s="14">
+        <v>1.27</v>
+      </c>
+      <c r="P38" s="14">
+        <v>1.1499999999999999</v>
       </c>
       <c r="Q38" s="14">
         <v>120</v>
@@ -2902,7 +2981,7 @@
         <v>2035</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="C39" s="12" t="s">
         <v>18</v>
@@ -2911,7 +2990,7 @@
         <v>104</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="F39" s="12" t="s">
         <v>10</v>
@@ -2926,95 +3005,216 @@
         <v>106</v>
       </c>
       <c r="J39" s="13" t="s">
-        <v>43</v>
+        <v>113</v>
       </c>
       <c r="K39" s="12" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="L39" s="12">
         <v>18.64</v>
       </c>
-      <c r="M39" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="N39" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="O39" s="12">
+      <c r="M39" s="48" t="s">
+        <v>112</v>
+      </c>
+      <c r="N39" s="48" t="s">
+        <v>112</v>
+      </c>
+      <c r="O39" s="14">
+        <v>1.27</v>
+      </c>
+      <c r="P39" s="14">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="Q39" s="14">
+        <v>0</v>
+      </c>
+      <c r="R39" s="14">
+        <v>0</v>
+      </c>
+      <c r="S39" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="F40" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G40" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H40" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I40" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="J40" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="K40" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="L40" s="12">
+        <v>18.64</v>
+      </c>
+      <c r="M40" s="48" t="s">
+        <v>112</v>
+      </c>
+      <c r="N40" s="48" t="s">
+        <v>112</v>
+      </c>
+      <c r="O40" s="12">
         <v>0.95</v>
       </c>
-      <c r="P39" s="12">
+      <c r="P40" s="12">
         <v>0.86</v>
       </c>
-      <c r="Q39" s="14">
-        <v>0</v>
-      </c>
-      <c r="R39" s="14">
-        <v>0</v>
-      </c>
-      <c r="S39" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="24">
+      <c r="Q40" s="14">
+        <v>120</v>
+      </c>
+      <c r="R40" s="14">
+        <v>0</v>
+      </c>
+      <c r="S40" s="14">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="F41" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G41" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H41" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I41" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="J41" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K41" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="L41" s="12">
+        <v>18.64</v>
+      </c>
+      <c r="M41" s="48" t="s">
+        <v>112</v>
+      </c>
+      <c r="N41" s="48" t="s">
+        <v>112</v>
+      </c>
+      <c r="O41" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="P41" s="12">
+        <v>0.86</v>
+      </c>
+      <c r="Q41" s="14">
+        <v>0</v>
+      </c>
+      <c r="R41" s="14">
+        <v>0</v>
+      </c>
+      <c r="S41" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="24">
         <v>2050</v>
       </c>
-      <c r="B40" s="24" t="s">
+      <c r="B42" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="C40" s="24" t="s">
+      <c r="C42" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D40" s="24" t="s">
+      <c r="D42" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="E40" s="24" t="s">
+      <c r="E42" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="F40" s="24" t="s">
+      <c r="F42" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="G40" s="25" t="s">
+      <c r="G42" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="I40" s="24" t="s">
+      <c r="I42" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="J40" s="26" t="s">
+      <c r="J42" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="K40" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="L40" s="24">
+      <c r="K42" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="L42" s="24">
         <v>17.440000000000001</v>
       </c>
-      <c r="M40" s="24">
+      <c r="M42" s="49">
         <v>-0.33</v>
       </c>
-      <c r="N40" s="24">
-        <v>0</v>
-      </c>
-      <c r="O40" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="P40" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q40" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="R40" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="S40" s="27" t="s">
+      <c r="N42" s="49">
+        <v>0</v>
+      </c>
+      <c r="O42" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="P42" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q42" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="R42" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="S42" s="27" t="s">
         <v>112</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="K5" r:id="rId1" xr:uid="{1BE7DD4C-B567-4320-9B69-E8B55CE41797}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding 2015_TM160_IPA_02 (WFH at ~11%)
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D8D906-C16F-4756-8160-2DCF5880FB72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BFFE05C-A11B-4B1B-97CF-62A6BB4FBF7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="158">
   <si>
     <t>year</t>
   </si>
@@ -332,9 +332,6 @@
     <t>Set WFH factors to be 0.5x of v19's</t>
   </si>
   <si>
-    <t>Set WFH factors to be 0.75x of v19's</t>
-  </si>
-  <si>
     <t>https://app.asana.com/0/1204085012544660/1205555270932662/f</t>
   </si>
   <si>
@@ -507,6 +504,12 @@
   </si>
   <si>
     <t>\RTP2021\IncrementalProgress\2005_TM152_IPA_03\INPUT</t>
+  </si>
+  <si>
+    <t>WFH at 25%, trn hes=120, 0, 45</t>
+  </si>
+  <si>
+    <t>WFH rate at ~11%</t>
   </si>
 </sst>
 </file>
@@ -641,7 +644,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -703,10 +706,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1064,11 +1066,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9564CC59-3725-4FDA-8BF2-0F68CB1B6F5A}">
-  <dimension ref="A1:S42"/>
+  <dimension ref="A1:S43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1085,7 +1087,7 @@
     <col min="10" max="10" width="11.26953125" style="10" customWidth="1"/>
     <col min="11" max="11" width="17.54296875" style="1" customWidth="1"/>
     <col min="12" max="12" width="5.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="9.1796875" style="45"/>
+    <col min="13" max="14" width="9.1796875" style="44"/>
     <col min="15" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
@@ -1124,12 +1126,12 @@
         <v>23</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="M1" s="40" t="s">
+        <v>121</v>
+      </c>
+      <c r="M1" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="40" t="s">
+      <c r="N1" s="39" t="s">
         <v>39</v>
       </c>
       <c r="O1" s="4" t="s">
@@ -1153,16 +1155,16 @@
         <v>2005</v>
       </c>
       <c r="B2" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="20" t="s">
         <v>129</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>130</v>
       </c>
       <c r="F2" s="20"/>
       <c r="G2" s="20"/>
@@ -1170,216 +1172,224 @@
         <v>12</v>
       </c>
       <c r="J2" s="22"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
       <c r="O2" s="23"/>
       <c r="P2" s="23"/>
       <c r="Q2" s="23"/>
       <c r="R2" s="23"/>
     </row>
-    <row r="3" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="31">
         <v>2005</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>152</v>
-      </c>
-      <c r="C3" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3" s="32" t="s">
         <v>18</v>
       </c>
       <c r="D3" s="32" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="32" t="s">
-        <v>154</v>
-      </c>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
+        <v>153</v>
+      </c>
       <c r="H3" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="33" t="s">
-        <v>156</v>
-      </c>
-      <c r="J3" s="34" t="s">
+      <c r="I3" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="J3" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="K3" s="33" t="s">
-        <v>155</v>
-      </c>
-      <c r="L3" s="33">
+      <c r="K3" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="L3" s="32">
         <v>14.87</v>
       </c>
-      <c r="M3" s="42" t="s">
-        <v>112</v>
-      </c>
-      <c r="N3" s="42" t="s">
-        <v>112</v>
-      </c>
-      <c r="O3" s="35">
-        <v>0</v>
-      </c>
-      <c r="P3" s="35">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="35">
-        <v>0</v>
-      </c>
-      <c r="R3" s="35">
-        <v>0</v>
-      </c>
-      <c r="S3" s="35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="36">
+      <c r="M3" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="N3" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="O3" s="34">
+        <v>0</v>
+      </c>
+      <c r="P3" s="34">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="34">
+        <v>0</v>
+      </c>
+      <c r="R3" s="34">
+        <v>0</v>
+      </c>
+      <c r="S3" s="34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="35">
         <v>2015</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="37" t="s">
+      <c r="C4" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="37" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="37" t="s">
+      <c r="F4" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="37" t="s">
+      <c r="I4" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="38" t="s">
+      <c r="J4" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="37" t="s">
+      <c r="K4" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="M4" s="43">
+      <c r="M4" s="42">
         <v>-0.09</v>
       </c>
-      <c r="N4" s="43">
+      <c r="N4" s="42">
         <v>0.9</v>
       </c>
-      <c r="O4" s="39"/>
-      <c r="P4" s="39"/>
-      <c r="Q4" s="39">
-        <v>0</v>
-      </c>
-      <c r="R4" s="39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="36">
+      <c r="O4" s="38"/>
+      <c r="P4" s="38"/>
+      <c r="Q4" s="38">
+        <v>0</v>
+      </c>
+      <c r="R4" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="35">
         <v>2015</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="36" t="s">
+        <v>148</v>
+      </c>
+      <c r="C5" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="36" t="s">
+        <v>152</v>
+      </c>
+      <c r="F5" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="36" t="s">
         <v>149</v>
       </c>
-      <c r="C5" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="37" t="s">
-        <v>153</v>
-      </c>
-      <c r="F5" s="37" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="37" t="s">
+      <c r="J5" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="M5" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="N5" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="O5" s="38">
+        <v>0</v>
+      </c>
+      <c r="P5" s="38">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="38">
+        <v>0</v>
+      </c>
+      <c r="R5" s="38">
+        <v>0</v>
+      </c>
+      <c r="S5" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="35">
+        <v>2015</v>
+      </c>
+      <c r="B6" s="36" t="s">
+        <v>148</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="36" t="s">
+        <v>157</v>
+      </c>
+      <c r="F6" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="37" t="s">
+      <c r="I6" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="J6" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="K6" s="36" t="s">
         <v>150</v>
       </c>
-      <c r="J5" s="38" t="s">
-        <v>44</v>
-      </c>
-      <c r="K5" s="37" t="s">
-        <v>151</v>
-      </c>
-      <c r="M5" s="43" t="s">
-        <v>112</v>
-      </c>
-      <c r="N5" s="43" t="s">
-        <v>112</v>
-      </c>
-      <c r="O5" s="39">
-        <v>0</v>
-      </c>
-      <c r="P5" s="39">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="39">
-        <v>0</v>
-      </c>
-      <c r="R5" s="39">
-        <v>0</v>
-      </c>
-      <c r="S5" s="39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>2023</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M6" s="44">
-        <v>-0.44</v>
-      </c>
-      <c r="N6" s="44">
-        <v>-0.23</v>
-      </c>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6">
-        <v>0</v>
-      </c>
-      <c r="R6" s="6">
+      <c r="M6" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="N6" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="O6" s="38">
+        <v>0.32</v>
+      </c>
+      <c r="P6" s="38">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="Q6" s="38">
+        <v>0</v>
+      </c>
+      <c r="R6" s="38">
+        <v>0</v>
+      </c>
+      <c r="S6" s="38">
         <v>0</v>
       </c>
     </row>
@@ -1388,7 +1398,7 @@
         <v>2023</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>18</v>
@@ -1397,7 +1407,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>10</v>
@@ -1412,18 +1422,18 @@
         <v>17</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="M7" s="44">
-        <v>-1.25</v>
-      </c>
-      <c r="N7" s="44">
-        <v>-0.75</v>
+        <v>25</v>
+      </c>
+      <c r="M7" s="43">
+        <v>-0.44</v>
+      </c>
+      <c r="N7" s="43">
+        <v>-0.23</v>
       </c>
       <c r="O7" s="6"/>
       <c r="P7" s="6"/>
       <c r="Q7" s="6">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="R7" s="6">
         <v>0</v>
@@ -1434,7 +1444,7 @@
         <v>2023</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>18</v>
@@ -1443,7 +1453,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>10</v>
@@ -1452,27 +1462,27 @@
         <v>11</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="J8" s="9" t="s">
         <v>17</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M8" s="44">
+        <v>26</v>
+      </c>
+      <c r="M8" s="43">
         <v>-1.25</v>
       </c>
-      <c r="N8" s="44">
+      <c r="N8" s="43">
         <v>-0.75</v>
       </c>
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
       <c r="Q8" s="6">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="R8" s="6">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
@@ -1480,7 +1490,7 @@
         <v>2023</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>18</v>
@@ -1489,7 +1499,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>10</v>
@@ -1498,24 +1508,24 @@
         <v>11</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J9" s="9" t="s">
         <v>17</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M9" s="44">
+        <v>30</v>
+      </c>
+      <c r="M9" s="43">
         <v>-1.25</v>
       </c>
-      <c r="N9" s="44">
+      <c r="N9" s="43">
         <v>-0.75</v>
       </c>
       <c r="O9" s="6"/>
       <c r="P9" s="6"/>
       <c r="Q9" s="6">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="R9" s="6">
         <v>15</v>
@@ -1526,7 +1536,7 @@
         <v>2023</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>18</v>
@@ -1535,7 +1545,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>10</v>
@@ -1550,20 +1560,20 @@
         <v>17</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="M10" s="44">
+        <v>32</v>
+      </c>
+      <c r="M10" s="43">
         <v>-1.25</v>
       </c>
-      <c r="N10" s="44">
+      <c r="N10" s="43">
         <v>-0.75</v>
       </c>
       <c r="O10" s="6"/>
       <c r="P10" s="6"/>
-      <c r="Q10" s="11">
+      <c r="Q10" s="6">
         <v>75</v>
       </c>
-      <c r="R10" s="11">
+      <c r="R10" s="6">
         <v>15</v>
       </c>
     </row>
@@ -1572,7 +1582,7 @@
         <v>2023</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>18</v>
@@ -1581,7 +1591,7 @@
         <v>7</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>10</v>
@@ -1593,23 +1603,23 @@
         <v>33</v>
       </c>
       <c r="J11" s="9" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="M11" s="44">
+        <v>35</v>
+      </c>
+      <c r="M11" s="43">
         <v>-1.25</v>
       </c>
-      <c r="N11" s="44">
+      <c r="N11" s="43">
         <v>-0.75</v>
       </c>
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
-      <c r="Q11" s="7">
-        <v>85</v>
-      </c>
-      <c r="R11" s="7">
+      <c r="Q11" s="11">
+        <v>75</v>
+      </c>
+      <c r="R11" s="11">
         <v>15</v>
       </c>
     </row>
@@ -1618,7 +1628,7 @@
         <v>2023</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>18</v>
@@ -1639,21 +1649,21 @@
         <v>33</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="M12" s="44">
+      <c r="M12" s="43">
         <v>-1.25</v>
       </c>
-      <c r="N12" s="44">
+      <c r="N12" s="43">
         <v>-0.75</v>
       </c>
       <c r="O12" s="6"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="7">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="R12" s="7">
         <v>15</v>
@@ -1664,7 +1674,7 @@
         <v>2023</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>18</v>
@@ -1685,24 +1695,24 @@
         <v>33</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="M13" s="44">
+      <c r="M13" s="43">
         <v>-1.25</v>
       </c>
-      <c r="N13" s="44">
+      <c r="N13" s="43">
         <v>-0.75</v>
       </c>
       <c r="O13" s="6"/>
       <c r="P13" s="6"/>
       <c r="Q13" s="7">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="R13" s="7">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
@@ -1710,7 +1720,7 @@
         <v>2023</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>18</v>
@@ -1719,7 +1729,7 @@
         <v>7</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>10</v>
@@ -1728,18 +1738,18 @@
         <v>11</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J14" s="10" t="s">
-        <v>43</v>
+        <v>33</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>45</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="M14" s="44">
+        <v>46</v>
+      </c>
+      <c r="M14" s="43">
         <v>-1.25</v>
       </c>
-      <c r="N14" s="44">
+      <c r="N14" s="43">
         <v>-0.75</v>
       </c>
       <c r="O14" s="6"/>
@@ -1756,7 +1766,7 @@
         <v>2023</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>18</v>
@@ -1765,7 +1775,7 @@
         <v>7</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>10</v>
@@ -1774,24 +1784,24 @@
         <v>11</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="J15" s="10" t="s">
         <v>43</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="M15" s="44">
+        <v>51</v>
+      </c>
+      <c r="M15" s="43">
         <v>-1.25</v>
       </c>
-      <c r="N15" s="44">
+      <c r="N15" s="43">
         <v>-0.75</v>
       </c>
       <c r="O15" s="6"/>
       <c r="P15" s="6"/>
       <c r="Q15" s="7">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="R15" s="7">
         <v>30</v>
@@ -1802,7 +1812,7 @@
         <v>2023</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>18</v>
@@ -1811,7 +1821,7 @@
         <v>7</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>10</v>
@@ -1823,21 +1833,21 @@
         <v>54</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="M16" s="44">
+      <c r="M16" s="43">
         <v>-1.25</v>
       </c>
-      <c r="N16" s="44">
+      <c r="N16" s="43">
         <v>-0.75</v>
       </c>
       <c r="O16" s="6"/>
       <c r="P16" s="6"/>
       <c r="Q16" s="7">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="R16" s="7">
         <v>30</v>
@@ -1848,7 +1858,7 @@
         <v>2023</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>18</v>
@@ -1857,7 +1867,7 @@
         <v>7</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>10</v>
@@ -1866,27 +1876,27 @@
         <v>11</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="M17" s="44">
+        <v>57</v>
+      </c>
+      <c r="M17" s="43">
         <v>-1.25</v>
       </c>
-      <c r="N17" s="44">
+      <c r="N17" s="43">
         <v>-0.75</v>
       </c>
       <c r="O17" s="6"/>
       <c r="P17" s="6"/>
       <c r="Q17" s="7">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="R17" s="7">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
@@ -1894,7 +1904,7 @@
         <v>2023</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>18</v>
@@ -1903,7 +1913,7 @@
         <v>7</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>10</v>
@@ -1918,21 +1928,21 @@
         <v>43</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="M18" s="44">
+        <v>61</v>
+      </c>
+      <c r="M18" s="43">
         <v>-1.25</v>
       </c>
-      <c r="N18" s="44">
+      <c r="N18" s="43">
         <v>-0.75</v>
       </c>
       <c r="O18" s="6"/>
       <c r="P18" s="6"/>
       <c r="Q18" s="7">
-        <v>300</v>
+        <v>180</v>
       </c>
       <c r="R18" s="7">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
@@ -1940,7 +1950,7 @@
         <v>2023</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>18</v>
@@ -1966,16 +1976,16 @@
       <c r="K19" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="M19" s="44">
+      <c r="M19" s="43">
         <v>-1.25</v>
       </c>
-      <c r="N19" s="44">
+      <c r="N19" s="43">
         <v>-0.75</v>
       </c>
       <c r="O19" s="6"/>
       <c r="P19" s="6"/>
       <c r="Q19" s="7">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="R19" s="7">
         <v>5</v>
@@ -1986,7 +1996,7 @@
         <v>2023</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>18</v>
@@ -2012,16 +2022,16 @@
       <c r="K20" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="M20" s="44">
+      <c r="M20" s="43">
         <v>-1.25</v>
       </c>
-      <c r="N20" s="44">
+      <c r="N20" s="43">
         <v>-0.75</v>
       </c>
       <c r="O20" s="6"/>
       <c r="P20" s="6"/>
       <c r="Q20" s="7">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="R20" s="7">
         <v>5</v>
@@ -2032,7 +2042,7 @@
         <v>2023</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>18</v>
@@ -2041,7 +2051,7 @@
         <v>7</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>10</v>
@@ -2050,27 +2060,27 @@
         <v>11</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="J21" s="10" t="s">
         <v>43</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="M21" s="44">
+        <v>65</v>
+      </c>
+      <c r="M21" s="43">
         <v>-1.25</v>
       </c>
-      <c r="N21" s="44">
+      <c r="N21" s="43">
         <v>-0.75</v>
       </c>
       <c r="O21" s="6"/>
       <c r="P21" s="6"/>
       <c r="Q21" s="7">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="R21" s="7">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
@@ -2078,7 +2088,7 @@
         <v>2023</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>18</v>
@@ -2087,7 +2097,7 @@
         <v>7</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>10</v>
@@ -2096,18 +2106,18 @@
         <v>11</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="J22" s="10" t="s">
         <v>43</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="M22" s="44">
+        <v>67</v>
+      </c>
+      <c r="M22" s="43">
         <v>-1.25</v>
       </c>
-      <c r="N22" s="44">
+      <c r="N22" s="43">
         <v>-0.75</v>
       </c>
       <c r="O22" s="6"/>
@@ -2124,7 +2134,7 @@
         <v>2023</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>18</v>
@@ -2133,7 +2143,7 @@
         <v>7</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>10</v>
@@ -2142,18 +2152,18 @@
         <v>11</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="J23" s="10" t="s">
         <v>43</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="M23" s="44">
+        <v>76</v>
+      </c>
+      <c r="M23" s="43">
         <v>-1.25</v>
       </c>
-      <c r="N23" s="44">
+      <c r="N23" s="43">
         <v>-0.75</v>
       </c>
       <c r="O23" s="6"/>
@@ -2170,7 +2180,7 @@
         <v>2023</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>18</v>
@@ -2179,7 +2189,7 @@
         <v>7</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>10</v>
@@ -2191,17 +2201,19 @@
         <v>80</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>89</v>
+        <v>43</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="O24" s="6">
-        <v>1.27</v>
-      </c>
-      <c r="P24" s="6">
-        <v>1.1499999999999999</v>
-      </c>
+      <c r="M24" s="43">
+        <v>-1.25</v>
+      </c>
+      <c r="N24" s="43">
+        <v>-0.75</v>
+      </c>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
       <c r="Q24" s="7">
         <v>120</v>
       </c>
@@ -2214,7 +2226,7 @@
         <v>2023</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>18</v>
@@ -2223,7 +2235,7 @@
         <v>7</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>10</v>
@@ -2235,27 +2247,22 @@
         <v>80</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>43</v>
+        <v>89</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="M25" s="44">
-        <v>-1.25</v>
-      </c>
-      <c r="N25" s="44">
-        <v>-0.75</v>
-      </c>
-      <c r="O25" s="6"/>
-      <c r="P25" s="6"/>
+        <v>82</v>
+      </c>
+      <c r="O25" s="6">
+        <v>1.27</v>
+      </c>
+      <c r="P25" s="6">
+        <v>1.1499999999999999</v>
+      </c>
       <c r="Q25" s="7">
         <v>120</v>
       </c>
       <c r="R25" s="7">
         <v>0</v>
-      </c>
-      <c r="S25" s="7">
-        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
@@ -2263,7 +2270,7 @@
         <v>2023</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>18</v>
@@ -2284,17 +2291,19 @@
         <v>80</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>89</v>
+        <v>43</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="O26" s="6">
-        <v>1.27</v>
-      </c>
-      <c r="P26" s="6">
-        <v>1.1499999999999999</v>
-      </c>
+      <c r="M26" s="43">
+        <v>-1.25</v>
+      </c>
+      <c r="N26" s="43">
+        <v>-0.75</v>
+      </c>
+      <c r="O26" s="6"/>
+      <c r="P26" s="6"/>
       <c r="Q26" s="7">
         <v>120</v>
       </c>
@@ -2310,7 +2319,7 @@
         <v>2023</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>18</v>
@@ -2319,31 +2328,28 @@
         <v>7</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>80</v>
       </c>
       <c r="J27" s="10" t="s">
-        <v>43</v>
+        <v>89</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="M27" s="44">
-        <v>-1.25</v>
-      </c>
-      <c r="N27" s="44">
-        <v>-0.75</v>
+        <v>90</v>
+      </c>
+      <c r="O27" s="6">
+        <v>1.27</v>
+      </c>
+      <c r="P27" s="6">
+        <v>1.1499999999999999</v>
       </c>
       <c r="Q27" s="7">
         <v>120</v>
@@ -2352,7 +2358,7 @@
         <v>0</v>
       </c>
       <c r="S27" s="7">
-        <v>45</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
@@ -2360,7 +2366,7 @@
         <v>2023</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>18</v>
@@ -2384,25 +2390,16 @@
         <v>80</v>
       </c>
       <c r="J28" s="10" t="s">
-        <v>89</v>
+        <v>43</v>
       </c>
       <c r="K28" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="L28" s="1">
-        <v>17.77</v>
-      </c>
-      <c r="M28" s="45" t="s">
-        <v>112</v>
-      </c>
-      <c r="N28" s="45" t="s">
-        <v>112</v>
-      </c>
-      <c r="O28" s="6">
-        <v>1.27</v>
-      </c>
-      <c r="P28" s="6">
-        <v>1.1499999999999999</v>
+      <c r="M28" s="43">
+        <v>-1.25</v>
+      </c>
+      <c r="N28" s="43">
+        <v>-0.75</v>
       </c>
       <c r="Q28" s="7">
         <v>120</v>
@@ -2419,7 +2416,7 @@
         <v>2023</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>18</v>
@@ -2428,7 +2425,7 @@
         <v>7</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>10</v>
@@ -2443,25 +2440,25 @@
         <v>80</v>
       </c>
       <c r="J29" s="10" t="s">
-        <v>43</v>
+        <v>89</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="L29" s="1">
         <v>17.77</v>
       </c>
-      <c r="M29" s="45" t="s">
-        <v>112</v>
-      </c>
-      <c r="N29" s="45" t="s">
-        <v>112</v>
-      </c>
-      <c r="O29" s="1">
-        <v>0.64</v>
-      </c>
-      <c r="P29" s="1">
-        <v>0.57999999999999996</v>
+      <c r="M29" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="N29" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="O29" s="6">
+        <v>1.27</v>
+      </c>
+      <c r="P29" s="6">
+        <v>1.1499999999999999</v>
       </c>
       <c r="Q29" s="7">
         <v>120</v>
@@ -2478,7 +2475,7 @@
         <v>2023</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>18</v>
@@ -2487,7 +2484,7 @@
         <v>7</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>10</v>
@@ -2502,33 +2499,33 @@
         <v>80</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>89</v>
+        <v>43</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="L30" s="1">
         <v>17.77</v>
       </c>
-      <c r="M30" s="45" t="s">
-        <v>112</v>
-      </c>
-      <c r="N30" s="45" t="s">
-        <v>112</v>
+      <c r="M30" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="N30" s="44" t="s">
+        <v>111</v>
       </c>
       <c r="O30" s="1">
-        <v>0.95</v>
+        <v>0.64</v>
       </c>
       <c r="P30" s="1">
-        <v>0.86</v>
-      </c>
-      <c r="Q30" s="6">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="Q30" s="7">
         <v>120</v>
       </c>
-      <c r="R30" s="6">
-        <v>0</v>
-      </c>
-      <c r="S30" s="6">
+      <c r="R30" s="7">
+        <v>0</v>
+      </c>
+      <c r="S30" s="7">
         <v>45</v>
       </c>
     </row>
@@ -2537,7 +2534,7 @@
         <v>2023</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>142</v>
+        <v>96</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>18</v>
@@ -2546,7 +2543,7 @@
         <v>7</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>137</v>
+        <v>156</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>10</v>
@@ -2561,19 +2558,19 @@
         <v>80</v>
       </c>
       <c r="J31" s="10" t="s">
-        <v>44</v>
+        <v>89</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>140</v>
+        <v>99</v>
       </c>
       <c r="L31" s="1">
         <v>17.77</v>
       </c>
-      <c r="M31" s="45" t="s">
-        <v>112</v>
-      </c>
-      <c r="N31" s="45" t="s">
-        <v>112</v>
+      <c r="M31" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="N31" s="44" t="s">
+        <v>111</v>
       </c>
       <c r="O31" s="1">
         <v>0.95</v>
@@ -2582,13 +2579,13 @@
         <v>0.86</v>
       </c>
       <c r="Q31" s="6">
-        <v>200</v>
+        <v>120</v>
       </c>
       <c r="R31" s="6">
         <v>0</v>
       </c>
       <c r="S31" s="6">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
@@ -2596,7 +2593,7 @@
         <v>2023</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>18</v>
@@ -2605,7 +2602,7 @@
         <v>7</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>10</v>
@@ -2620,7 +2617,7 @@
         <v>80</v>
       </c>
       <c r="J32" s="10" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>139</v>
@@ -2628,11 +2625,11 @@
       <c r="L32" s="1">
         <v>17.77</v>
       </c>
-      <c r="M32" s="45" t="s">
-        <v>112</v>
-      </c>
-      <c r="N32" s="45" t="s">
-        <v>112</v>
+      <c r="M32" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="N32" s="44" t="s">
+        <v>111</v>
       </c>
       <c r="O32" s="1">
         <v>0.95</v>
@@ -2641,7 +2638,7 @@
         <v>0.86</v>
       </c>
       <c r="Q32" s="6">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="R32" s="6">
         <v>0</v>
@@ -2655,7 +2652,7 @@
         <v>2023</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>18</v>
@@ -2664,7 +2661,7 @@
         <v>7</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>10</v>
@@ -2679,25 +2676,25 @@
         <v>80</v>
       </c>
       <c r="J33" s="10" t="s">
-        <v>133</v>
+        <v>89</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="L33" s="1">
         <v>17.77</v>
       </c>
-      <c r="M33" s="45" t="s">
-        <v>112</v>
-      </c>
-      <c r="N33" s="45" t="s">
-        <v>112</v>
+      <c r="M33" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="N33" s="44" t="s">
+        <v>111</v>
       </c>
       <c r="O33" s="1">
-        <v>0.39</v>
+        <v>0.95</v>
       </c>
       <c r="P33" s="1">
-        <v>0.35</v>
+        <v>0.86</v>
       </c>
       <c r="Q33" s="6">
         <v>300</v>
@@ -2714,7 +2711,7 @@
         <v>2023</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>18</v>
@@ -2723,7 +2720,7 @@
         <v>7</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>10</v>
@@ -2738,183 +2735,183 @@
         <v>80</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>44</v>
+        <v>132</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="L34" s="1">
         <v>17.77</v>
       </c>
-      <c r="M34" s="45" t="s">
-        <v>112</v>
-      </c>
-      <c r="N34" s="45" t="s">
-        <v>112</v>
+      <c r="M34" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="N34" s="44" t="s">
+        <v>111</v>
       </c>
       <c r="O34" s="1">
+        <v>0.39</v>
+      </c>
+      <c r="P34" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="Q34" s="6">
+        <v>300</v>
+      </c>
+      <c r="R34" s="6">
+        <v>0</v>
+      </c>
+      <c r="S34" s="6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J35" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="L35" s="1">
+        <v>17.77</v>
+      </c>
+      <c r="M35" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="N35" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="O35" s="1">
         <v>0.77</v>
       </c>
-      <c r="P34" s="1">
+      <c r="P35" s="1">
         <v>0.69</v>
       </c>
-      <c r="Q34" s="6">
+      <c r="Q35" s="6">
         <v>400</v>
       </c>
-      <c r="R34" s="6">
-        <v>0</v>
-      </c>
-      <c r="S34" s="6">
+      <c r="R35" s="6">
+        <v>0</v>
+      </c>
+      <c r="S35" s="6">
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="28">
+    <row r="36" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="28">
         <v>2025</v>
       </c>
-      <c r="B35" s="28" t="s">
+      <c r="B36" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="C36" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="D36" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="E36" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="C35" s="28" t="s">
+      <c r="H36" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="I36" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="J36" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="M36" s="45"/>
+      <c r="N36" s="45"/>
+      <c r="Q36" s="30"/>
+      <c r="R36" s="30"/>
+      <c r="S36" s="30"/>
+    </row>
+    <row r="37" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="15">
+        <v>2035</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="D37" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="D35" s="28" t="s">
-        <v>104</v>
-      </c>
-      <c r="E35" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="H35" s="28" t="s">
+      <c r="E37" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="F37" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="G37" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="H37" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I35" s="28" t="s">
-        <v>136</v>
-      </c>
-      <c r="J35" s="29" t="s">
+      <c r="I37" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="J37" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="M35" s="46"/>
-      <c r="N35" s="46"/>
-      <c r="Q35" s="30"/>
-      <c r="R35" s="30"/>
-      <c r="S35" s="30"/>
-    </row>
-    <row r="36" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="15">
-        <v>2035</v>
-      </c>
-      <c r="B36" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="C36" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="D36" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="E36" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="F36" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="G36" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="H36" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="I36" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="J36" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="K36" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="L36" s="15">
+      <c r="K37" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="L37" s="15">
         <v>15.85</v>
       </c>
-      <c r="M36" s="47">
+      <c r="M37" s="46">
         <v>-0.27</v>
       </c>
-      <c r="N36" s="47">
-        <v>0</v>
-      </c>
-      <c r="O36" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="P36" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q36" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="R36" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="S36" s="17" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="12">
-        <v>2035</v>
-      </c>
-      <c r="B37" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D37" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="E37" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="F37" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G37" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H37" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I37" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="J37" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="K37" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="L37" s="12">
-        <v>15.85</v>
-      </c>
-      <c r="M37" s="48" t="s">
-        <v>112</v>
-      </c>
-      <c r="N37" s="48" t="s">
-        <v>112</v>
-      </c>
-      <c r="O37" s="14">
-        <v>1.27</v>
-      </c>
-      <c r="P37" s="14">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="Q37" s="14">
-        <v>120</v>
-      </c>
-      <c r="R37" s="14">
-        <v>0</v>
-      </c>
-      <c r="S37" s="14">
-        <v>45</v>
+      <c r="N37" s="46">
+        <v>0</v>
+      </c>
+      <c r="O37" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="P37" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q37" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="R37" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="S37" s="17" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="38" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -2922,16 +2919,16 @@
         <v>2035</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C38" s="12" t="s">
         <v>18</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F38" s="12" t="s">
         <v>10</v>
@@ -2943,22 +2940,22 @@
         <v>12</v>
       </c>
       <c r="I38" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J38" s="13" t="s">
-        <v>111</v>
+        <v>44</v>
       </c>
       <c r="K38" s="12" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="L38" s="12">
-        <v>18.64</v>
-      </c>
-      <c r="M38" s="48" t="s">
-        <v>112</v>
-      </c>
-      <c r="N38" s="48" t="s">
-        <v>112</v>
+        <v>15.85</v>
+      </c>
+      <c r="M38" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="N38" s="47" t="s">
+        <v>111</v>
       </c>
       <c r="O38" s="14">
         <v>1.27</v>
@@ -2981,16 +2978,16 @@
         <v>2035</v>
       </c>
       <c r="B39" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="C39" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D39" s="12" t="s">
-        <v>104</v>
-      </c>
       <c r="E39" s="12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F39" s="12" t="s">
         <v>10</v>
@@ -3002,22 +2999,22 @@
         <v>12</v>
       </c>
       <c r="I39" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J39" s="13" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="K39" s="12" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="L39" s="12">
         <v>18.64</v>
       </c>
-      <c r="M39" s="48" t="s">
-        <v>112</v>
-      </c>
-      <c r="N39" s="48" t="s">
-        <v>112</v>
+      <c r="M39" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="N39" s="47" t="s">
+        <v>111</v>
       </c>
       <c r="O39" s="14">
         <v>1.27</v>
@@ -3026,13 +3023,13 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="Q39" s="14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="R39" s="14">
         <v>0</v>
       </c>
       <c r="S39" s="14">
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="40" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -3040,16 +3037,16 @@
         <v>2035</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="C40" s="12" t="s">
         <v>18</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="F40" s="12" t="s">
         <v>10</v>
@@ -3061,37 +3058,37 @@
         <v>12</v>
       </c>
       <c r="I40" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J40" s="13" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="K40" s="12" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="L40" s="12">
         <v>18.64</v>
       </c>
-      <c r="M40" s="48" t="s">
-        <v>112</v>
-      </c>
-      <c r="N40" s="48" t="s">
-        <v>112</v>
-      </c>
-      <c r="O40" s="12">
-        <v>0.95</v>
-      </c>
-      <c r="P40" s="12">
-        <v>0.86</v>
+      <c r="M40" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="N40" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="O40" s="14">
+        <v>1.27</v>
+      </c>
+      <c r="P40" s="14">
+        <v>1.1499999999999999</v>
       </c>
       <c r="Q40" s="14">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="R40" s="14">
         <v>0</v>
       </c>
       <c r="S40" s="14">
-        <v>45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -3099,16 +3096,16 @@
         <v>2035</v>
       </c>
       <c r="B41" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E41" s="12" t="s">
         <v>124</v>
-      </c>
-      <c r="C41" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D41" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="E41" s="12" t="s">
-        <v>126</v>
       </c>
       <c r="F41" s="12" t="s">
         <v>10</v>
@@ -3120,10 +3117,10 @@
         <v>12</v>
       </c>
       <c r="I41" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J41" s="13" t="s">
-        <v>43</v>
+        <v>110</v>
       </c>
       <c r="K41" s="12" t="s">
         <v>127</v>
@@ -3131,11 +3128,11 @@
       <c r="L41" s="12">
         <v>18.64</v>
       </c>
-      <c r="M41" s="48" t="s">
-        <v>112</v>
-      </c>
-      <c r="N41" s="48" t="s">
-        <v>112</v>
+      <c r="M41" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="N41" s="47" t="s">
+        <v>111</v>
       </c>
       <c r="O41" s="12">
         <v>0.95</v>
@@ -3144,77 +3141,137 @@
         <v>0.86</v>
       </c>
       <c r="Q41" s="14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="R41" s="14">
         <v>0</v>
       </c>
       <c r="S41" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="24">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="F42" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G42" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H42" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I42" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="J42" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K42" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="L42" s="12">
+        <v>18.64</v>
+      </c>
+      <c r="M42" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="N42" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="O42" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="P42" s="12">
+        <v>0.86</v>
+      </c>
+      <c r="Q42" s="14">
+        <v>0</v>
+      </c>
+      <c r="R42" s="14">
+        <v>0</v>
+      </c>
+      <c r="S42" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="24">
         <v>2050</v>
       </c>
-      <c r="B42" s="24" t="s">
+      <c r="B43" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="C43" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="D43" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="E43" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="F43" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="G43" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="I43" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="C42" s="24" t="s">
-        <v>116</v>
-      </c>
-      <c r="D42" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="E42" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="F42" s="24" t="s">
-        <v>121</v>
-      </c>
-      <c r="G42" s="25" t="s">
-        <v>120</v>
-      </c>
-      <c r="I42" s="24" t="s">
+      <c r="J43" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="J42" s="26" t="s">
-        <v>133</v>
-      </c>
-      <c r="K42" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="L42" s="24">
+      <c r="K43" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="L43" s="24">
         <v>17.440000000000001</v>
       </c>
-      <c r="M42" s="49">
+      <c r="M43" s="48">
         <v>-0.33</v>
       </c>
-      <c r="N42" s="49">
-        <v>0</v>
-      </c>
-      <c r="O42" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="P42" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q42" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="R42" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="S42" s="27" t="s">
-        <v>112</v>
+      <c r="N43" s="48">
+        <v>0</v>
+      </c>
+      <c r="O43" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="P43" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q43" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="R43" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="S43" s="27" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="K5" r:id="rId1" xr:uid="{1BE7DD4C-B567-4320-9B69-E8B55CE41797}"/>
+    <hyperlink ref="K6" r:id="rId2" xr:uid="{A52BF015-28DA-4569-A638-6E56CCBD2F4D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding 2015 calib12 to run log, so it will be picked up by across_RTP2025_IP_JourneyToWorkModes_TM160.twb
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-v1.6_develop\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7583F77C-FB54-424E-A7C1-F955923A77EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A39BEC-05F6-4F17-9023-46103C75F65B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="161">
   <si>
     <t>year</t>
   </si>
@@ -513,6 +513,12 @@
   </si>
   <si>
     <t>2015_TM160_IPA_02</t>
+  </si>
+  <si>
+    <t>2015_TM160_IPA_02_calib9</t>
+  </si>
+  <si>
+    <t>2015_TM160_IPA_02_calib12</t>
   </si>
 </sst>
 </file>
@@ -561,7 +567,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -616,6 +622,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -647,7 +659,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -755,6 +767,17 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1069,11 +1092,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9564CC59-3725-4FDA-8BF2-0F68CB1B6F5A}">
-  <dimension ref="A1:S43"/>
+  <dimension ref="A1:S45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1396,95 +1419,115 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>2023</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M7" s="43">
-        <v>-0.44</v>
-      </c>
-      <c r="N7" s="43">
-        <v>-0.23</v>
-      </c>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="6">
-        <v>0</v>
-      </c>
-      <c r="R7" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>2023</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J8" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="M8" s="43">
-        <v>-1.25</v>
-      </c>
-      <c r="N8" s="43">
-        <v>-0.75</v>
-      </c>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6">
-        <v>30</v>
-      </c>
-      <c r="R8" s="6">
+    <row r="7" spans="1:19" s="50" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="49">
+        <v>2015</v>
+      </c>
+      <c r="B7" s="50" t="s">
+        <v>159</v>
+      </c>
+      <c r="C7" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="50" t="s">
+        <v>157</v>
+      </c>
+      <c r="F7" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="50" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="50" t="s">
+        <v>149</v>
+      </c>
+      <c r="J7" s="51" t="s">
+        <v>44</v>
+      </c>
+      <c r="K7" s="50" t="s">
+        <v>150</v>
+      </c>
+      <c r="M7" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="N7" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="O7" s="53">
+        <v>0.32</v>
+      </c>
+      <c r="P7" s="53">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="Q7" s="53">
+        <v>0</v>
+      </c>
+      <c r="R7" s="53">
+        <v>0</v>
+      </c>
+      <c r="S7" s="53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" s="50" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="49">
+        <v>2015</v>
+      </c>
+      <c r="B8" s="50" t="s">
+        <v>160</v>
+      </c>
+      <c r="C8" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="50" t="s">
+        <v>157</v>
+      </c>
+      <c r="F8" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="50" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="50" t="s">
+        <v>149</v>
+      </c>
+      <c r="J8" s="51" t="s">
+        <v>44</v>
+      </c>
+      <c r="K8" s="50" t="s">
+        <v>150</v>
+      </c>
+      <c r="M8" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="N8" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="O8" s="53">
+        <v>0.32</v>
+      </c>
+      <c r="P8" s="53">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="Q8" s="53">
+        <v>0</v>
+      </c>
+      <c r="R8" s="53">
+        <v>0</v>
+      </c>
+      <c r="S8" s="53">
         <v>0</v>
       </c>
     </row>
@@ -1493,7 +1536,7 @@
         <v>2023</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>18</v>
@@ -1502,7 +1545,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>10</v>
@@ -1511,27 +1554,27 @@
         <v>11</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="J9" s="9" t="s">
         <v>17</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="M9" s="43">
-        <v>-1.25</v>
+        <v>-0.44</v>
       </c>
       <c r="N9" s="43">
-        <v>-0.75</v>
+        <v>-0.23</v>
       </c>
       <c r="O9" s="6"/>
       <c r="P9" s="6"/>
       <c r="Q9" s="6">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="R9" s="6">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
@@ -1539,7 +1582,7 @@
         <v>2023</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>18</v>
@@ -1548,7 +1591,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>10</v>
@@ -1557,13 +1600,13 @@
         <v>11</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="J10" s="9" t="s">
         <v>17</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="M10" s="43">
         <v>-1.25</v>
@@ -1574,10 +1617,10 @@
       <c r="O10" s="6"/>
       <c r="P10" s="6"/>
       <c r="Q10" s="6">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="R10" s="6">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
@@ -1585,7 +1628,7 @@
         <v>2023</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>18</v>
@@ -1594,7 +1637,7 @@
         <v>7</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>10</v>
@@ -1603,13 +1646,13 @@
         <v>11</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J11" s="9" t="s">
         <v>17</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="M11" s="43">
         <v>-1.25</v>
@@ -1619,10 +1662,10 @@
       </c>
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
-      <c r="Q11" s="11">
-        <v>75</v>
-      </c>
-      <c r="R11" s="11">
+      <c r="Q11" s="6">
+        <v>45</v>
+      </c>
+      <c r="R11" s="6">
         <v>15</v>
       </c>
     </row>
@@ -1631,7 +1674,7 @@
         <v>2023</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>18</v>
@@ -1640,7 +1683,7 @@
         <v>7</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>10</v>
@@ -1652,10 +1695,10 @@
         <v>33</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="M12" s="43">
         <v>-1.25</v>
@@ -1665,10 +1708,10 @@
       </c>
       <c r="O12" s="6"/>
       <c r="P12" s="6"/>
-      <c r="Q12" s="7">
-        <v>85</v>
-      </c>
-      <c r="R12" s="7">
+      <c r="Q12" s="6">
+        <v>75</v>
+      </c>
+      <c r="R12" s="6">
         <v>15</v>
       </c>
     </row>
@@ -1677,7 +1720,7 @@
         <v>2023</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>18</v>
@@ -1686,7 +1729,7 @@
         <v>7</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>10</v>
@@ -1698,10 +1741,10 @@
         <v>33</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="M13" s="43">
         <v>-1.25</v>
@@ -1711,10 +1754,10 @@
       </c>
       <c r="O13" s="6"/>
       <c r="P13" s="6"/>
-      <c r="Q13" s="7">
-        <v>95</v>
-      </c>
-      <c r="R13" s="7">
+      <c r="Q13" s="11">
+        <v>75</v>
+      </c>
+      <c r="R13" s="11">
         <v>15</v>
       </c>
     </row>
@@ -1723,7 +1766,7 @@
         <v>2023</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>18</v>
@@ -1744,7 +1787,7 @@
         <v>33</v>
       </c>
       <c r="J14" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>46</v>
@@ -1761,7 +1804,7 @@
         <v>85</v>
       </c>
       <c r="R14" s="7">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
@@ -1769,7 +1812,7 @@
         <v>2023</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>18</v>
@@ -1778,7 +1821,7 @@
         <v>7</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>10</v>
@@ -1787,13 +1830,13 @@
         <v>11</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J15" s="10" t="s">
-        <v>43</v>
+        <v>33</v>
+      </c>
+      <c r="J15" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="M15" s="43">
         <v>-1.25</v>
@@ -1804,10 +1847,10 @@
       <c r="O15" s="6"/>
       <c r="P15" s="6"/>
       <c r="Q15" s="7">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="R15" s="7">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
@@ -1815,7 +1858,7 @@
         <v>2023</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>18</v>
@@ -1824,7 +1867,7 @@
         <v>7</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>10</v>
@@ -1833,13 +1876,13 @@
         <v>11</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J16" s="10" t="s">
-        <v>43</v>
+        <v>33</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>45</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="M16" s="43">
         <v>-1.25</v>
@@ -1850,7 +1893,7 @@
       <c r="O16" s="6"/>
       <c r="P16" s="6"/>
       <c r="Q16" s="7">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="R16" s="7">
         <v>30</v>
@@ -1861,7 +1904,7 @@
         <v>2023</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>18</v>
@@ -1870,7 +1913,7 @@
         <v>7</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>10</v>
@@ -1879,13 +1922,13 @@
         <v>11</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="M17" s="43">
         <v>-1.25</v>
@@ -1896,7 +1939,7 @@
       <c r="O17" s="6"/>
       <c r="P17" s="6"/>
       <c r="Q17" s="7">
-        <v>120</v>
+        <v>85</v>
       </c>
       <c r="R17" s="7">
         <v>30</v>
@@ -1907,7 +1950,7 @@
         <v>2023</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>18</v>
@@ -1916,7 +1959,7 @@
         <v>7</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>10</v>
@@ -1925,13 +1968,13 @@
         <v>11</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="J18" s="10" t="s">
         <v>43</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="M18" s="43">
         <v>-1.25</v>
@@ -1942,10 +1985,10 @@
       <c r="O18" s="6"/>
       <c r="P18" s="6"/>
       <c r="Q18" s="7">
-        <v>180</v>
+        <v>95</v>
       </c>
       <c r="R18" s="7">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
@@ -1953,7 +1996,7 @@
         <v>2023</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>18</v>
@@ -1962,7 +2005,7 @@
         <v>7</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>10</v>
@@ -1971,13 +2014,13 @@
         <v>11</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="M19" s="43">
         <v>-1.25</v>
@@ -1988,10 +2031,10 @@
       <c r="O19" s="6"/>
       <c r="P19" s="6"/>
       <c r="Q19" s="7">
-        <v>300</v>
+        <v>120</v>
       </c>
       <c r="R19" s="7">
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
@@ -1999,7 +2042,7 @@
         <v>2023</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>18</v>
@@ -2008,7 +2051,7 @@
         <v>7</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>10</v>
@@ -2023,7 +2066,7 @@
         <v>43</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="M20" s="43">
         <v>-1.25</v>
@@ -2034,10 +2077,10 @@
       <c r="O20" s="6"/>
       <c r="P20" s="6"/>
       <c r="Q20" s="7">
-        <v>250</v>
+        <v>180</v>
       </c>
       <c r="R20" s="7">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
@@ -2045,7 +2088,7 @@
         <v>2023</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>18</v>
@@ -2080,7 +2123,7 @@
       <c r="O21" s="6"/>
       <c r="P21" s="6"/>
       <c r="Q21" s="7">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="R21" s="7">
         <v>5</v>
@@ -2091,7 +2134,7 @@
         <v>2023</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>18</v>
@@ -2100,7 +2143,7 @@
         <v>7</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>10</v>
@@ -2109,13 +2152,13 @@
         <v>11</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="J22" s="10" t="s">
         <v>43</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M22" s="43">
         <v>-1.25</v>
@@ -2126,10 +2169,10 @@
       <c r="O22" s="6"/>
       <c r="P22" s="6"/>
       <c r="Q22" s="7">
-        <v>120</v>
+        <v>250</v>
       </c>
       <c r="R22" s="7">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
@@ -2137,7 +2180,7 @@
         <v>2023</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>18</v>
@@ -2146,7 +2189,7 @@
         <v>7</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>10</v>
@@ -2155,13 +2198,13 @@
         <v>11</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="J23" s="10" t="s">
         <v>43</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="M23" s="43">
         <v>-1.25</v>
@@ -2172,10 +2215,10 @@
       <c r="O23" s="6"/>
       <c r="P23" s="6"/>
       <c r="Q23" s="7">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="R23" s="7">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
@@ -2183,7 +2226,7 @@
         <v>2023</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>18</v>
@@ -2192,7 +2235,7 @@
         <v>7</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>10</v>
@@ -2201,13 +2244,13 @@
         <v>11</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="J24" s="10" t="s">
         <v>43</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="M24" s="43">
         <v>-1.25</v>
@@ -2229,7 +2272,7 @@
         <v>2023</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>18</v>
@@ -2238,7 +2281,7 @@
         <v>7</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>10</v>
@@ -2247,20 +2290,22 @@
         <v>11</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>89</v>
+        <v>43</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="O25" s="6">
-        <v>1.27</v>
-      </c>
-      <c r="P25" s="6">
-        <v>1.1499999999999999</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="M25" s="43">
+        <v>-1.25</v>
+      </c>
+      <c r="N25" s="43">
+        <v>-0.75</v>
+      </c>
+      <c r="O25" s="6"/>
+      <c r="P25" s="6"/>
       <c r="Q25" s="7">
         <v>120</v>
       </c>
@@ -2273,7 +2318,7 @@
         <v>2023</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>18</v>
@@ -2282,7 +2327,7 @@
         <v>7</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>10</v>
@@ -2297,7 +2342,7 @@
         <v>43</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="M26" s="43">
         <v>-1.25</v>
@@ -2313,16 +2358,13 @@
       <c r="R26" s="7">
         <v>0</v>
       </c>
-      <c r="S26" s="7">
-        <v>30</v>
-      </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>2023</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>18</v>
@@ -2331,7 +2373,7 @@
         <v>7</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>10</v>
@@ -2346,7 +2388,7 @@
         <v>89</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="O27" s="6">
         <v>1.27</v>
@@ -2359,9 +2401,6 @@
       </c>
       <c r="R27" s="7">
         <v>0</v>
-      </c>
-      <c r="S27" s="7">
-        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
@@ -2369,7 +2408,7 @@
         <v>2023</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>18</v>
@@ -2378,16 +2417,13 @@
         <v>7</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>80</v>
@@ -2396,7 +2432,7 @@
         <v>43</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="M28" s="43">
         <v>-1.25</v>
@@ -2404,6 +2440,8 @@
       <c r="N28" s="43">
         <v>-0.75</v>
       </c>
+      <c r="O28" s="6"/>
+      <c r="P28" s="6"/>
       <c r="Q28" s="7">
         <v>120</v>
       </c>
@@ -2411,7 +2449,7 @@
         <v>0</v>
       </c>
       <c r="S28" s="7">
-        <v>45</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
@@ -2419,7 +2457,7 @@
         <v>2023</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>18</v>
@@ -2428,16 +2466,13 @@
         <v>7</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>80</v>
@@ -2446,16 +2481,7 @@
         <v>89</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="L29" s="1">
-        <v>17.77</v>
-      </c>
-      <c r="M29" s="44" t="s">
-        <v>111</v>
-      </c>
-      <c r="N29" s="44" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="O29" s="6">
         <v>1.27</v>
@@ -2470,7 +2496,7 @@
         <v>0</v>
       </c>
       <c r="S29" s="7">
-        <v>45</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
@@ -2478,7 +2504,7 @@
         <v>2023</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>18</v>
@@ -2487,7 +2513,7 @@
         <v>7</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>10</v>
@@ -2505,22 +2531,13 @@
         <v>43</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="L30" s="1">
-        <v>17.77</v>
-      </c>
-      <c r="M30" s="44" t="s">
-        <v>111</v>
-      </c>
-      <c r="N30" s="44" t="s">
-        <v>111</v>
-      </c>
-      <c r="O30" s="1">
-        <v>0.64</v>
-      </c>
-      <c r="P30" s="1">
-        <v>0.57999999999999996</v>
+        <v>94</v>
+      </c>
+      <c r="M30" s="43">
+        <v>-1.25</v>
+      </c>
+      <c r="N30" s="43">
+        <v>-0.75</v>
       </c>
       <c r="Q30" s="7">
         <v>120</v>
@@ -2537,7 +2554,7 @@
         <v>2023</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>18</v>
@@ -2546,7 +2563,7 @@
         <v>7</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>156</v>
+        <v>93</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>10</v>
@@ -2564,7 +2581,7 @@
         <v>89</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="L31" s="1">
         <v>17.77</v>
@@ -2575,19 +2592,19 @@
       <c r="N31" s="44" t="s">
         <v>111</v>
       </c>
-      <c r="O31" s="1">
-        <v>0.95</v>
-      </c>
-      <c r="P31" s="1">
-        <v>0.86</v>
-      </c>
-      <c r="Q31" s="6">
+      <c r="O31" s="6">
+        <v>1.27</v>
+      </c>
+      <c r="P31" s="6">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="Q31" s="7">
         <v>120</v>
       </c>
-      <c r="R31" s="6">
-        <v>0</v>
-      </c>
-      <c r="S31" s="6">
+      <c r="R31" s="7">
+        <v>0</v>
+      </c>
+      <c r="S31" s="7">
         <v>45</v>
       </c>
     </row>
@@ -2596,7 +2613,7 @@
         <v>2023</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>141</v>
+        <v>95</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>18</v>
@@ -2605,7 +2622,7 @@
         <v>7</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>136</v>
+        <v>97</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>10</v>
@@ -2620,10 +2637,10 @@
         <v>80</v>
       </c>
       <c r="J32" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>139</v>
+        <v>98</v>
       </c>
       <c r="L32" s="1">
         <v>17.77</v>
@@ -2635,19 +2652,19 @@
         <v>111</v>
       </c>
       <c r="O32" s="1">
-        <v>0.95</v>
+        <v>0.64</v>
       </c>
       <c r="P32" s="1">
-        <v>0.86</v>
-      </c>
-      <c r="Q32" s="6">
-        <v>200</v>
-      </c>
-      <c r="R32" s="6">
-        <v>0</v>
-      </c>
-      <c r="S32" s="6">
-        <v>50</v>
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="Q32" s="7">
+        <v>120</v>
+      </c>
+      <c r="R32" s="7">
+        <v>0</v>
+      </c>
+      <c r="S32" s="7">
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.3">
@@ -2655,7 +2672,7 @@
         <v>2023</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>142</v>
+        <v>96</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>18</v>
@@ -2664,7 +2681,7 @@
         <v>7</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>137</v>
+        <v>156</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>10</v>
@@ -2682,7 +2699,7 @@
         <v>89</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>138</v>
+        <v>99</v>
       </c>
       <c r="L33" s="1">
         <v>17.77</v>
@@ -2700,13 +2717,13 @@
         <v>0.86</v>
       </c>
       <c r="Q33" s="6">
-        <v>300</v>
+        <v>120</v>
       </c>
       <c r="R33" s="6">
         <v>0</v>
       </c>
       <c r="S33" s="6">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.3">
@@ -2714,7 +2731,7 @@
         <v>2023</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>18</v>
@@ -2723,7 +2740,7 @@
         <v>7</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>10</v>
@@ -2738,10 +2755,10 @@
         <v>80</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>132</v>
+        <v>44</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L34" s="1">
         <v>17.77</v>
@@ -2753,13 +2770,13 @@
         <v>111</v>
       </c>
       <c r="O34" s="1">
-        <v>0.39</v>
+        <v>0.95</v>
       </c>
       <c r="P34" s="1">
-        <v>0.35</v>
+        <v>0.86</v>
       </c>
       <c r="Q34" s="6">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="R34" s="6">
         <v>0</v>
@@ -2773,7 +2790,7 @@
         <v>2023</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>18</v>
@@ -2782,7 +2799,7 @@
         <v>7</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>10</v>
@@ -2797,10 +2814,10 @@
         <v>80</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>44</v>
+        <v>89</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="L35" s="1">
         <v>17.77</v>
@@ -2812,227 +2829,227 @@
         <v>111</v>
       </c>
       <c r="O35" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="P35" s="1">
+        <v>0.86</v>
+      </c>
+      <c r="Q35" s="6">
+        <v>300</v>
+      </c>
+      <c r="R35" s="6">
+        <v>0</v>
+      </c>
+      <c r="S35" s="6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J36" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="L36" s="1">
+        <v>17.77</v>
+      </c>
+      <c r="M36" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="N36" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="O36" s="1">
+        <v>0.39</v>
+      </c>
+      <c r="P36" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="Q36" s="6">
+        <v>300</v>
+      </c>
+      <c r="R36" s="6">
+        <v>0</v>
+      </c>
+      <c r="S36" s="6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J37" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="L37" s="1">
+        <v>17.77</v>
+      </c>
+      <c r="M37" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="N37" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="O37" s="1">
         <v>0.77</v>
       </c>
-      <c r="P35" s="1">
+      <c r="P37" s="1">
         <v>0.69</v>
       </c>
-      <c r="Q35" s="6">
+      <c r="Q37" s="6">
         <v>400</v>
       </c>
-      <c r="R35" s="6">
-        <v>0</v>
-      </c>
-      <c r="S35" s="6">
+      <c r="R37" s="6">
+        <v>0</v>
+      </c>
+      <c r="S37" s="6">
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="28">
+    <row r="38" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="28">
         <v>2025</v>
       </c>
-      <c r="B36" s="28" t="s">
+      <c r="B38" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="C36" s="28" t="s">
+      <c r="C38" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="D36" s="28" t="s">
+      <c r="D38" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="E36" s="28" t="s">
+      <c r="E38" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="H36" s="28" t="s">
+      <c r="H38" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="I36" s="28" t="s">
+      <c r="I38" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="J36" s="29" t="s">
+      <c r="J38" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="M36" s="45"/>
-      <c r="N36" s="45"/>
-      <c r="Q36" s="30"/>
-      <c r="R36" s="30"/>
-      <c r="S36" s="30"/>
-    </row>
-    <row r="37" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="15">
+      <c r="M38" s="45"/>
+      <c r="N38" s="45"/>
+      <c r="Q38" s="30"/>
+      <c r="R38" s="30"/>
+      <c r="S38" s="30"/>
+    </row>
+    <row r="39" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="15">
         <v>2035</v>
       </c>
-      <c r="B37" s="15" t="s">
+      <c r="B39" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="C37" s="15" t="s">
+      <c r="C39" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="D37" s="15" t="s">
+      <c r="D39" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="E37" s="15" t="s">
+      <c r="E39" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="F37" s="15" t="s">
+      <c r="F39" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="G37" s="18" t="s">
+      <c r="G39" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="H37" s="15" t="s">
+      <c r="H39" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I37" s="15" t="s">
+      <c r="I39" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="J37" s="16" t="s">
+      <c r="J39" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="K37" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="L37" s="15">
+      <c r="K39" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="L39" s="15">
         <v>15.85</v>
       </c>
-      <c r="M37" s="46">
+      <c r="M39" s="46">
         <v>-0.27</v>
       </c>
-      <c r="N37" s="46">
-        <v>0</v>
-      </c>
-      <c r="O37" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="P37" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q37" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="R37" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="S37" s="17" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="12">
-        <v>2035</v>
-      </c>
-      <c r="B38" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="C38" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D38" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="E38" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="F38" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G38" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H38" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I38" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="J38" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="K38" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="L38" s="12">
-        <v>15.85</v>
-      </c>
-      <c r="M38" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="N38" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="O38" s="14">
-        <v>1.27</v>
-      </c>
-      <c r="P38" s="14">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="Q38" s="14">
-        <v>120</v>
-      </c>
-      <c r="R38" s="14">
-        <v>0</v>
-      </c>
-      <c r="S38" s="14">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="12">
-        <v>2035</v>
-      </c>
-      <c r="B39" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="C39" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D39" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="E39" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="F39" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G39" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H39" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I39" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="J39" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="K39" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="L39" s="12">
-        <v>18.64</v>
-      </c>
-      <c r="M39" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="N39" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="O39" s="14">
-        <v>1.27</v>
-      </c>
-      <c r="P39" s="14">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="Q39" s="14">
-        <v>120</v>
-      </c>
-      <c r="R39" s="14">
-        <v>0</v>
-      </c>
-      <c r="S39" s="14">
-        <v>45</v>
+      <c r="N39" s="46">
+        <v>0</v>
+      </c>
+      <c r="O39" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="P39" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q39" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="R39" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="S39" s="17" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="40" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -3040,7 +3057,7 @@
         <v>2035</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C40" s="12" t="s">
         <v>18</v>
@@ -3049,7 +3066,7 @@
         <v>103</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F40" s="12" t="s">
         <v>10</v>
@@ -3064,13 +3081,13 @@
         <v>105</v>
       </c>
       <c r="J40" s="13" t="s">
-        <v>112</v>
+        <v>44</v>
       </c>
       <c r="K40" s="12" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="L40" s="12">
-        <v>18.64</v>
+        <v>15.85</v>
       </c>
       <c r="M40" s="47" t="s">
         <v>111</v>
@@ -3085,13 +3102,13 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="Q40" s="14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="R40" s="14">
         <v>0</v>
       </c>
       <c r="S40" s="14">
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -3099,7 +3116,7 @@
         <v>2035</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="C41" s="12" t="s">
         <v>18</v>
@@ -3108,7 +3125,7 @@
         <v>103</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="F41" s="12" t="s">
         <v>10</v>
@@ -3126,7 +3143,7 @@
         <v>110</v>
       </c>
       <c r="K41" s="12" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L41" s="12">
         <v>18.64</v>
@@ -3137,11 +3154,11 @@
       <c r="N41" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="O41" s="12">
-        <v>0.95</v>
-      </c>
-      <c r="P41" s="12">
-        <v>0.86</v>
+      <c r="O41" s="14">
+        <v>1.27</v>
+      </c>
+      <c r="P41" s="14">
+        <v>1.1499999999999999</v>
       </c>
       <c r="Q41" s="14">
         <v>120</v>
@@ -3158,7 +3175,7 @@
         <v>2035</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="C42" s="12" t="s">
         <v>18</v>
@@ -3167,7 +3184,7 @@
         <v>103</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="F42" s="12" t="s">
         <v>10</v>
@@ -3182,10 +3199,10 @@
         <v>105</v>
       </c>
       <c r="J42" s="13" t="s">
-        <v>43</v>
+        <v>112</v>
       </c>
       <c r="K42" s="12" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="L42" s="12">
         <v>18.64</v>
@@ -3196,75 +3213,193 @@
       <c r="N42" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="O42" s="12">
+      <c r="O42" s="14">
+        <v>1.27</v>
+      </c>
+      <c r="P42" s="14">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="Q42" s="14">
+        <v>0</v>
+      </c>
+      <c r="R42" s="14">
+        <v>0</v>
+      </c>
+      <c r="S42" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E43" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="F43" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G43" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H43" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I43" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="J43" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="K43" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="L43" s="12">
+        <v>18.64</v>
+      </c>
+      <c r="M43" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="N43" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="O43" s="12">
         <v>0.95</v>
       </c>
-      <c r="P42" s="12">
+      <c r="P43" s="12">
         <v>0.86</v>
       </c>
-      <c r="Q42" s="14">
-        <v>0</v>
-      </c>
-      <c r="R42" s="14">
-        <v>0</v>
-      </c>
-      <c r="S42" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="24">
+      <c r="Q43" s="14">
+        <v>120</v>
+      </c>
+      <c r="R43" s="14">
+        <v>0</v>
+      </c>
+      <c r="S43" s="14">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E44" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="F44" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G44" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H44" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I44" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="J44" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K44" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="L44" s="12">
+        <v>18.64</v>
+      </c>
+      <c r="M44" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="N44" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="O44" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="P44" s="12">
+        <v>0.86</v>
+      </c>
+      <c r="Q44" s="14">
+        <v>0</v>
+      </c>
+      <c r="R44" s="14">
+        <v>0</v>
+      </c>
+      <c r="S44" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="24">
         <v>2050</v>
       </c>
-      <c r="B43" s="24" t="s">
+      <c r="B45" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="C43" s="24" t="s">
+      <c r="C45" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="D43" s="24" t="s">
+      <c r="D45" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="E43" s="24" t="s">
+      <c r="E45" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="F43" s="24" t="s">
+      <c r="F45" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="G43" s="25" t="s">
+      <c r="G45" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="I43" s="24" t="s">
+      <c r="I45" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="J43" s="26" t="s">
+      <c r="J45" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="K43" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="L43" s="24">
+      <c r="K45" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="L45" s="24">
         <v>17.440000000000001</v>
       </c>
-      <c r="M43" s="48">
+      <c r="M45" s="48">
         <v>-0.33</v>
       </c>
-      <c r="N43" s="48">
-        <v>0</v>
-      </c>
-      <c r="O43" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="P43" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q43" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="R43" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="S43" s="27" t="s">
+      <c r="N45" s="48">
+        <v>0</v>
+      </c>
+      <c r="O45" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="P45" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q45" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="R45" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="S45" s="27" t="s">
         <v>111</v>
       </c>
     </row>
@@ -3273,8 +3408,10 @@
   <hyperlinks>
     <hyperlink ref="K5" r:id="rId1" xr:uid="{1BE7DD4C-B567-4320-9B69-E8B55CE41797}"/>
     <hyperlink ref="K6" r:id="rId2" xr:uid="{A52BF015-28DA-4569-A638-6E56CCBD2F4D}"/>
+    <hyperlink ref="K8" r:id="rId3" xr:uid="{70B88B93-E906-4801-9012-B01BCDB48CBF}"/>
+    <hyperlink ref="K7" r:id="rId4" xr:uid="{57A3A870-1138-4A46-9914-6E556D2F44BC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding 2015_TM160_IPA_03 to the model run log
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-v1.6_develop\utilities\RTP\config_RTP2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A39BEC-05F6-4F17-9023-46103C75F65B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{970D7454-D332-4B70-A502-F37C2E84A8F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="163">
   <si>
     <t>year</t>
   </si>
@@ -515,16 +515,25 @@
     <t>2015_TM160_IPA_02</t>
   </si>
   <si>
-    <t>2015_TM160_IPA_02_calib9</t>
-  </si>
-  <si>
     <t>2015_TM160_IPA_02_calib12</t>
+  </si>
+  <si>
+    <t>2015_TM160_IPA_03</t>
+  </si>
+  <si>
+    <t>New CDAP, WFH rate at ~12%</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1205741891321014/f</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -567,7 +576,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -622,12 +631,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -659,7 +662,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -767,17 +770,7 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1094,9 +1087,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9564CC59-3725-4FDA-8BF2-0F68CB1B6F5A}">
   <dimension ref="A1:S45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomLeft" activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1385,9 +1378,6 @@
       <c r="G6" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="36" t="s">
-        <v>12</v>
-      </c>
       <c r="I6" s="36" t="s">
         <v>149</v>
       </c>
@@ -1419,115 +1409,112 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:19" s="50" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="49">
+    <row r="7" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="35">
         <v>2015</v>
       </c>
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="36" t="s">
         <v>159</v>
       </c>
-      <c r="C7" s="50" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="50" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="50" t="s">
+      <c r="C7" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="36" t="s">
         <v>157</v>
       </c>
-      <c r="F7" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="50" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="50" t="s">
+      <c r="F7" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="J7" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="K7" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="M7" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="N7" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="O7" s="38">
+        <v>0.32</v>
+      </c>
+      <c r="P7" s="38">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="Q7" s="38">
+        <v>0</v>
+      </c>
+      <c r="R7" s="38">
+        <v>0</v>
+      </c>
+      <c r="S7" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="35">
+        <v>2015</v>
+      </c>
+      <c r="B8" s="36" t="s">
+        <v>160</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="36" t="s">
+        <v>161</v>
+      </c>
+      <c r="F8" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="50" t="s">
+      <c r="I8" s="36" t="s">
         <v>149</v>
       </c>
-      <c r="J7" s="51" t="s">
-        <v>44</v>
-      </c>
-      <c r="K7" s="50" t="s">
-        <v>150</v>
-      </c>
-      <c r="M7" s="52" t="s">
-        <v>111</v>
-      </c>
-      <c r="N7" s="52" t="s">
-        <v>111</v>
-      </c>
-      <c r="O7" s="53">
-        <v>0.32</v>
-      </c>
-      <c r="P7" s="53">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="Q7" s="53">
-        <v>0</v>
-      </c>
-      <c r="R7" s="53">
-        <v>0</v>
-      </c>
-      <c r="S7" s="53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" s="50" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="49">
-        <v>2015</v>
-      </c>
-      <c r="B8" s="50" t="s">
-        <v>160</v>
-      </c>
-      <c r="C8" s="50" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="50" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="50" t="s">
-        <v>157</v>
-      </c>
-      <c r="F8" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="50" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="50" t="s">
-        <v>12</v>
-      </c>
-      <c r="I8" s="50" t="s">
-        <v>149</v>
-      </c>
-      <c r="J8" s="51" t="s">
-        <v>44</v>
-      </c>
-      <c r="K8" s="50" t="s">
-        <v>150</v>
-      </c>
-      <c r="M8" s="52" t="s">
-        <v>111</v>
-      </c>
-      <c r="N8" s="52" t="s">
-        <v>111</v>
-      </c>
-      <c r="O8" s="53">
-        <v>0.32</v>
-      </c>
-      <c r="P8" s="53">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="Q8" s="53">
-        <v>0</v>
-      </c>
-      <c r="R8" s="53">
-        <v>0</v>
-      </c>
-      <c r="S8" s="53">
+      <c r="J8" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="M8" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="N8" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="O8" s="49">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="P8" s="49">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="Q8" s="38">
+        <v>0</v>
+      </c>
+      <c r="R8" s="38">
+        <v>0</v>
+      </c>
+      <c r="S8" s="38">
         <v>0</v>
       </c>
     </row>
@@ -3408,10 +3395,9 @@
   <hyperlinks>
     <hyperlink ref="K5" r:id="rId1" xr:uid="{1BE7DD4C-B567-4320-9B69-E8B55CE41797}"/>
     <hyperlink ref="K6" r:id="rId2" xr:uid="{A52BF015-28DA-4569-A638-6E56CCBD2F4D}"/>
-    <hyperlink ref="K8" r:id="rId3" xr:uid="{70B88B93-E906-4801-9012-B01BCDB48CBF}"/>
-    <hyperlink ref="K7" r:id="rId4" xr:uid="{57A3A870-1138-4A46-9914-6E556D2F44BC}"/>
+    <hyperlink ref="K7" r:id="rId3" xr:uid="{70B88B93-E906-4801-9012-B01BCDB48CBF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added two 2023 runs with the new CDAP (these two runs are the same except for the network version)
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{970D7454-D332-4B70-A502-F37C2E84A8F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F223FD7-9BA5-406C-9005-9CB00A5ACC78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="169">
   <si>
     <t>year</t>
   </si>
@@ -525,6 +525,24 @@
   </si>
   <si>
     <t>https://app.asana.com/0/1204085012544660/1205741891321014/f</t>
+  </si>
+  <si>
+    <t>2023_TM160_IPA_26</t>
+  </si>
+  <si>
+    <t>New CDAP, WFH at ~25%, , trn hes=120, 0, 45</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1205764227468992/f</t>
+  </si>
+  <si>
+    <t>2023_TM160_IPA_27</t>
+  </si>
+  <si>
+    <t>BlueprintNetworks_v10\net_2023_Blueprint</t>
+  </si>
+  <si>
+    <t>New CDAP, WFH at ~25%, trn hes=120, 0, 45, network v10</t>
   </si>
 </sst>
 </file>
@@ -1085,11 +1103,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9564CC59-3725-4FDA-8BF2-0F68CB1B6F5A}">
-  <dimension ref="A1:S45"/>
+  <dimension ref="A1:S47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P8" sqref="P8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -2949,212 +2967,212 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="28">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J38" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="L38" s="1">
+        <v>17.77</v>
+      </c>
+      <c r="M38" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="N38" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="O38" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="P38" s="1">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="Q38" s="6">
+        <v>120</v>
+      </c>
+      <c r="R38" s="6">
+        <v>0</v>
+      </c>
+      <c r="S38" s="6">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="J39" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="L39" s="1">
+        <v>17.77</v>
+      </c>
+      <c r="M39" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="N39" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="O39" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="P39" s="1">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="Q39" s="6">
+        <v>120</v>
+      </c>
+      <c r="R39" s="6">
+        <v>0</v>
+      </c>
+      <c r="S39" s="6">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="28">
         <v>2025</v>
       </c>
-      <c r="B38" s="28" t="s">
+      <c r="B40" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="C38" s="28" t="s">
+      <c r="C40" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="D38" s="28" t="s">
+      <c r="D40" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="E38" s="28" t="s">
+      <c r="E40" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="H38" s="28" t="s">
+      <c r="H40" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="I38" s="28" t="s">
+      <c r="I40" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="J38" s="29" t="s">
+      <c r="J40" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="M38" s="45"/>
-      <c r="N38" s="45"/>
-      <c r="Q38" s="30"/>
-      <c r="R38" s="30"/>
-      <c r="S38" s="30"/>
-    </row>
-    <row r="39" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="15">
+      <c r="M40" s="45"/>
+      <c r="N40" s="45"/>
+      <c r="Q40" s="30"/>
+      <c r="R40" s="30"/>
+      <c r="S40" s="30"/>
+    </row>
+    <row r="41" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="15">
         <v>2035</v>
       </c>
-      <c r="B39" s="15" t="s">
+      <c r="B41" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="C39" s="15" t="s">
+      <c r="C41" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="D39" s="15" t="s">
+      <c r="D41" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="E39" s="15" t="s">
+      <c r="E41" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="F39" s="15" t="s">
+      <c r="F41" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="G39" s="18" t="s">
+      <c r="G41" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="H39" s="15" t="s">
+      <c r="H41" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="15" t="s">
+      <c r="I41" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="J39" s="16" t="s">
+      <c r="J41" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="K39" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="L39" s="15">
+      <c r="K41" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="L41" s="15">
         <v>15.85</v>
       </c>
-      <c r="M39" s="46">
+      <c r="M41" s="46">
         <v>-0.27</v>
       </c>
-      <c r="N39" s="46">
-        <v>0</v>
-      </c>
-      <c r="O39" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="P39" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q39" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="R39" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="S39" s="17" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="12">
-        <v>2035</v>
-      </c>
-      <c r="B40" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="C40" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D40" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="E40" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="F40" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G40" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H40" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I40" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="J40" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="K40" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="L40" s="12">
-        <v>15.85</v>
-      </c>
-      <c r="M40" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="N40" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="O40" s="14">
-        <v>1.27</v>
-      </c>
-      <c r="P40" s="14">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="Q40" s="14">
-        <v>120</v>
-      </c>
-      <c r="R40" s="14">
-        <v>0</v>
-      </c>
-      <c r="S40" s="14">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="41" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="12">
-        <v>2035</v>
-      </c>
-      <c r="B41" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="C41" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D41" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="E41" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="F41" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G41" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H41" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I41" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="J41" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="K41" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="L41" s="12">
-        <v>18.64</v>
-      </c>
-      <c r="M41" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="N41" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="O41" s="14">
-        <v>1.27</v>
-      </c>
-      <c r="P41" s="14">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="Q41" s="14">
-        <v>120</v>
-      </c>
-      <c r="R41" s="14">
-        <v>0</v>
-      </c>
-      <c r="S41" s="14">
-        <v>45</v>
+      <c r="N41" s="46">
+        <v>0</v>
+      </c>
+      <c r="O41" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="P41" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q41" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="R41" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="S41" s="17" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -3162,7 +3180,7 @@
         <v>2035</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C42" s="12" t="s">
         <v>18</v>
@@ -3171,7 +3189,7 @@
         <v>103</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F42" s="12" t="s">
         <v>10</v>
@@ -3186,13 +3204,13 @@
         <v>105</v>
       </c>
       <c r="J42" s="13" t="s">
-        <v>112</v>
+        <v>44</v>
       </c>
       <c r="K42" s="12" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="L42" s="12">
-        <v>18.64</v>
+        <v>15.85</v>
       </c>
       <c r="M42" s="47" t="s">
         <v>111</v>
@@ -3207,13 +3225,13 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="Q42" s="14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="R42" s="14">
         <v>0</v>
       </c>
       <c r="S42" s="14">
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -3221,7 +3239,7 @@
         <v>2035</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="C43" s="12" t="s">
         <v>18</v>
@@ -3230,7 +3248,7 @@
         <v>103</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="F43" s="12" t="s">
         <v>10</v>
@@ -3248,7 +3266,7 @@
         <v>110</v>
       </c>
       <c r="K43" s="12" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L43" s="12">
         <v>18.64</v>
@@ -3259,11 +3277,11 @@
       <c r="N43" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="O43" s="12">
-        <v>0.95</v>
-      </c>
-      <c r="P43" s="12">
-        <v>0.86</v>
+      <c r="O43" s="14">
+        <v>1.27</v>
+      </c>
+      <c r="P43" s="14">
+        <v>1.1499999999999999</v>
       </c>
       <c r="Q43" s="14">
         <v>120</v>
@@ -3280,7 +3298,7 @@
         <v>2035</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="C44" s="12" t="s">
         <v>18</v>
@@ -3289,7 +3307,7 @@
         <v>103</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="F44" s="12" t="s">
         <v>10</v>
@@ -3304,10 +3322,10 @@
         <v>105</v>
       </c>
       <c r="J44" s="13" t="s">
-        <v>43</v>
+        <v>112</v>
       </c>
       <c r="K44" s="12" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="L44" s="12">
         <v>18.64</v>
@@ -3318,75 +3336,193 @@
       <c r="N44" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="O44" s="12">
+      <c r="O44" s="14">
+        <v>1.27</v>
+      </c>
+      <c r="P44" s="14">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="Q44" s="14">
+        <v>0</v>
+      </c>
+      <c r="R44" s="14">
+        <v>0</v>
+      </c>
+      <c r="S44" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E45" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="F45" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G45" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H45" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I45" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="J45" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="K45" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="L45" s="12">
+        <v>18.64</v>
+      </c>
+      <c r="M45" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="N45" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="O45" s="12">
         <v>0.95</v>
       </c>
-      <c r="P44" s="12">
+      <c r="P45" s="12">
         <v>0.86</v>
       </c>
-      <c r="Q44" s="14">
-        <v>0</v>
-      </c>
-      <c r="R44" s="14">
-        <v>0</v>
-      </c>
-      <c r="S44" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="24">
+      <c r="Q45" s="14">
+        <v>120</v>
+      </c>
+      <c r="R45" s="14">
+        <v>0</v>
+      </c>
+      <c r="S45" s="14">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E46" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="F46" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G46" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H46" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I46" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="J46" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K46" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="L46" s="12">
+        <v>18.64</v>
+      </c>
+      <c r="M46" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="N46" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="O46" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="P46" s="12">
+        <v>0.86</v>
+      </c>
+      <c r="Q46" s="14">
+        <v>0</v>
+      </c>
+      <c r="R46" s="14">
+        <v>0</v>
+      </c>
+      <c r="S46" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="24">
         <v>2050</v>
       </c>
-      <c r="B45" s="24" t="s">
+      <c r="B47" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="C45" s="24" t="s">
+      <c r="C47" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="D45" s="24" t="s">
+      <c r="D47" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="E45" s="24" t="s">
+      <c r="E47" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="F45" s="24" t="s">
+      <c r="F47" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="G45" s="25" t="s">
+      <c r="G47" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="I45" s="24" t="s">
+      <c r="I47" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="J45" s="26" t="s">
+      <c r="J47" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="K45" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="L45" s="24">
+      <c r="K47" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="L47" s="24">
         <v>17.440000000000001</v>
       </c>
-      <c r="M45" s="48">
+      <c r="M47" s="48">
         <v>-0.33</v>
       </c>
-      <c r="N45" s="48">
-        <v>0</v>
-      </c>
-      <c r="O45" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="P45" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q45" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="R45" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="S45" s="27" t="s">
+      <c r="N47" s="48">
+        <v>0</v>
+      </c>
+      <c r="O47" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="P47" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q47" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="R47" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="S47" s="27" t="s">
         <v>111</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added 2023_TM160_IPA_28 to the model run log
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F223FD7-9BA5-406C-9005-9CB00A5ACC78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9B4B422-C6D2-4643-B3ED-438D8F3BDB34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="171">
   <si>
     <t>year</t>
   </si>
@@ -543,6 +543,12 @@
   </si>
   <si>
     <t>New CDAP, WFH at ~25%, trn hes=120, 0, 45, network v10</t>
+  </si>
+  <si>
+    <t>2023_TM160_IPA_28</t>
+  </si>
+  <si>
+    <t>Added BART hesistancy to Caltrain and ferry, WFH remains at ~25%</t>
   </si>
 </sst>
 </file>
@@ -1103,11 +1109,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9564CC59-3725-4FDA-8BF2-0F68CB1B6F5A}">
-  <dimension ref="A1:S47"/>
+  <dimension ref="A1:S48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -3085,153 +3091,153 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="28">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="J40" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="L40" s="1">
+        <v>17.77</v>
+      </c>
+      <c r="M40" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="N40" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="O40" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="P40" s="1">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="Q40" s="6">
+        <v>120</v>
+      </c>
+      <c r="R40" s="6">
+        <v>0</v>
+      </c>
+      <c r="S40" s="6">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="28">
         <v>2025</v>
       </c>
-      <c r="B40" s="28" t="s">
+      <c r="B41" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="C40" s="28" t="s">
+      <c r="C41" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="D40" s="28" t="s">
+      <c r="D41" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="E40" s="28" t="s">
+      <c r="E41" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="H40" s="28" t="s">
+      <c r="H41" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="I40" s="28" t="s">
+      <c r="I41" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="J40" s="29" t="s">
+      <c r="J41" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="M40" s="45"/>
-      <c r="N40" s="45"/>
-      <c r="Q40" s="30"/>
-      <c r="R40" s="30"/>
-      <c r="S40" s="30"/>
-    </row>
-    <row r="41" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="15">
+      <c r="M41" s="45"/>
+      <c r="N41" s="45"/>
+      <c r="Q41" s="30"/>
+      <c r="R41" s="30"/>
+      <c r="S41" s="30"/>
+    </row>
+    <row r="42" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="15">
         <v>2035</v>
       </c>
-      <c r="B41" s="15" t="s">
+      <c r="B42" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="C41" s="15" t="s">
+      <c r="C42" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="D41" s="15" t="s">
+      <c r="D42" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="E41" s="15" t="s">
+      <c r="E42" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="F41" s="15" t="s">
+      <c r="F42" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="G41" s="18" t="s">
+      <c r="G42" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="H41" s="15" t="s">
+      <c r="H42" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I41" s="15" t="s">
+      <c r="I42" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="J41" s="16" t="s">
+      <c r="J42" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="K41" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="L41" s="15">
+      <c r="K42" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="L42" s="15">
         <v>15.85</v>
       </c>
-      <c r="M41" s="46">
+      <c r="M42" s="46">
         <v>-0.27</v>
       </c>
-      <c r="N41" s="46">
-        <v>0</v>
-      </c>
-      <c r="O41" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="P41" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q41" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="R41" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="S41" s="17" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="42" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="12">
-        <v>2035</v>
-      </c>
-      <c r="B42" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="C42" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D42" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="E42" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="F42" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G42" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H42" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I42" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="J42" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="K42" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="L42" s="12">
-        <v>15.85</v>
-      </c>
-      <c r="M42" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="N42" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="O42" s="14">
-        <v>1.27</v>
-      </c>
-      <c r="P42" s="14">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="Q42" s="14">
-        <v>120</v>
-      </c>
-      <c r="R42" s="14">
-        <v>0</v>
-      </c>
-      <c r="S42" s="14">
-        <v>45</v>
+      <c r="N42" s="46">
+        <v>0</v>
+      </c>
+      <c r="O42" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="P42" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q42" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="R42" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="S42" s="17" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -3239,7 +3245,7 @@
         <v>2035</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C43" s="12" t="s">
         <v>18</v>
@@ -3248,7 +3254,7 @@
         <v>103</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F43" s="12" t="s">
         <v>10</v>
@@ -3263,13 +3269,13 @@
         <v>105</v>
       </c>
       <c r="J43" s="13" t="s">
-        <v>110</v>
+        <v>44</v>
       </c>
       <c r="K43" s="12" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="L43" s="12">
-        <v>18.64</v>
+        <v>15.85</v>
       </c>
       <c r="M43" s="47" t="s">
         <v>111</v>
@@ -3298,7 +3304,7 @@
         <v>2035</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C44" s="12" t="s">
         <v>18</v>
@@ -3307,7 +3313,7 @@
         <v>103</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F44" s="12" t="s">
         <v>10</v>
@@ -3322,10 +3328,10 @@
         <v>105</v>
       </c>
       <c r="J44" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K44" s="12" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="L44" s="12">
         <v>18.64</v>
@@ -3343,13 +3349,13 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="Q44" s="14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="R44" s="14">
         <v>0</v>
       </c>
       <c r="S44" s="14">
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="45" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -3357,7 +3363,7 @@
         <v>2035</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="C45" s="12" t="s">
         <v>18</v>
@@ -3366,7 +3372,7 @@
         <v>103</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="F45" s="12" t="s">
         <v>10</v>
@@ -3381,10 +3387,10 @@
         <v>105</v>
       </c>
       <c r="J45" s="13" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="K45" s="12" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="L45" s="12">
         <v>18.64</v>
@@ -3395,20 +3401,20 @@
       <c r="N45" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="O45" s="12">
-        <v>0.95</v>
-      </c>
-      <c r="P45" s="12">
-        <v>0.86</v>
+      <c r="O45" s="14">
+        <v>1.27</v>
+      </c>
+      <c r="P45" s="14">
+        <v>1.1499999999999999</v>
       </c>
       <c r="Q45" s="14">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="R45" s="14">
         <v>0</v>
       </c>
       <c r="S45" s="14">
-        <v>45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -3416,7 +3422,7 @@
         <v>2035</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C46" s="12" t="s">
         <v>18</v>
@@ -3425,7 +3431,7 @@
         <v>103</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F46" s="12" t="s">
         <v>10</v>
@@ -3440,10 +3446,10 @@
         <v>105</v>
       </c>
       <c r="J46" s="13" t="s">
-        <v>43</v>
+        <v>110</v>
       </c>
       <c r="K46" s="12" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="L46" s="12">
         <v>18.64</v>
@@ -3461,68 +3467,127 @@
         <v>0.86</v>
       </c>
       <c r="Q46" s="14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="R46" s="14">
         <v>0</v>
       </c>
       <c r="S46" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="24">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E47" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="F47" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G47" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H47" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I47" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="J47" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K47" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="L47" s="12">
+        <v>18.64</v>
+      </c>
+      <c r="M47" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="N47" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="O47" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="P47" s="12">
+        <v>0.86</v>
+      </c>
+      <c r="Q47" s="14">
+        <v>0</v>
+      </c>
+      <c r="R47" s="14">
+        <v>0</v>
+      </c>
+      <c r="S47" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="24">
         <v>2050</v>
       </c>
-      <c r="B47" s="24" t="s">
+      <c r="B48" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="C47" s="24" t="s">
+      <c r="C48" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="D47" s="24" t="s">
+      <c r="D48" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="E47" s="24" t="s">
+      <c r="E48" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="F47" s="24" t="s">
+      <c r="F48" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="G47" s="25" t="s">
+      <c r="G48" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="I47" s="24" t="s">
+      <c r="I48" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="J47" s="26" t="s">
+      <c r="J48" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="K47" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="L47" s="24">
+      <c r="K48" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="L48" s="24">
         <v>17.440000000000001</v>
       </c>
-      <c r="M47" s="48">
+      <c r="M48" s="48">
         <v>-0.33</v>
       </c>
-      <c r="N47" s="48">
-        <v>0</v>
-      </c>
-      <c r="O47" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="P47" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q47" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="R47" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="S47" s="27" t="s">
+      <c r="N48" s="48">
+        <v>0</v>
+      </c>
+      <c r="O48" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="P48" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q48" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="R48" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="S48" s="27" t="s">
         <v>111</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding 2023 model run v29 (with refined employed residents estimates) to the run log
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9B4B422-C6D2-4643-B3ED-438D8F3BDB34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B663026C-FC1F-4A5E-BA1B-D9EBD3CE19E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="174">
   <si>
     <t>year</t>
   </si>
@@ -549,6 +549,15 @@
   </si>
   <si>
     <t>Added BART hesistancy to Caltrain and ferry, WFH remains at ~25%</t>
+  </si>
+  <si>
+    <t>2023_TM160_IPA_29</t>
+  </si>
+  <si>
+    <t>Refined empres estimates, WFH remains at ~25%</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1205838169476835/f</t>
   </si>
 </sst>
 </file>
@@ -1109,11 +1118,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9564CC59-3725-4FDA-8BF2-0F68CB1B6F5A}">
-  <dimension ref="A1:S48"/>
+  <dimension ref="A1:S49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B40" sqref="B40"/>
+      <selection pane="bottomLeft" activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -2641,9 +2650,6 @@
       <c r="G32" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H32" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="I32" s="1" t="s">
         <v>80</v>
       </c>
@@ -2759,9 +2765,6 @@
       <c r="G34" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H34" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="I34" s="1" t="s">
         <v>80</v>
       </c>
@@ -2818,9 +2821,6 @@
       <c r="G35" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H35" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="I35" s="1" t="s">
         <v>80</v>
       </c>
@@ -2877,9 +2877,6 @@
       <c r="G36" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H36" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="I36" s="1" t="s">
         <v>80</v>
       </c>
@@ -2936,9 +2933,6 @@
       <c r="G37" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H37" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="I37" s="1" t="s">
         <v>80</v>
       </c>
@@ -3150,153 +3144,153 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="28">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="J41" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="L41" s="1">
+        <v>17.77</v>
+      </c>
+      <c r="M41" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="N41" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="O41" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="P41" s="1">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="Q41" s="6">
+        <v>120</v>
+      </c>
+      <c r="R41" s="6">
+        <v>0</v>
+      </c>
+      <c r="S41" s="6">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="28">
         <v>2025</v>
       </c>
-      <c r="B41" s="28" t="s">
+      <c r="B42" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="C41" s="28" t="s">
+      <c r="C42" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="D41" s="28" t="s">
+      <c r="D42" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="E41" s="28" t="s">
+      <c r="E42" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="H41" s="28" t="s">
+      <c r="H42" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="I41" s="28" t="s">
+      <c r="I42" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="J41" s="29" t="s">
+      <c r="J42" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="M41" s="45"/>
-      <c r="N41" s="45"/>
-      <c r="Q41" s="30"/>
-      <c r="R41" s="30"/>
-      <c r="S41" s="30"/>
-    </row>
-    <row r="42" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="15">
+      <c r="M42" s="45"/>
+      <c r="N42" s="45"/>
+      <c r="Q42" s="30"/>
+      <c r="R42" s="30"/>
+      <c r="S42" s="30"/>
+    </row>
+    <row r="43" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="15">
         <v>2035</v>
       </c>
-      <c r="B42" s="15" t="s">
+      <c r="B43" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="C42" s="15" t="s">
+      <c r="C43" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="D42" s="15" t="s">
+      <c r="D43" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="E42" s="15" t="s">
+      <c r="E43" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="F42" s="15" t="s">
+      <c r="F43" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="G42" s="18" t="s">
+      <c r="G43" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="H42" s="15" t="s">
+      <c r="H43" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I42" s="15" t="s">
+      <c r="I43" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="J42" s="16" t="s">
+      <c r="J43" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="K42" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="L42" s="15">
+      <c r="K43" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="L43" s="15">
         <v>15.85</v>
       </c>
-      <c r="M42" s="46">
+      <c r="M43" s="46">
         <v>-0.27</v>
       </c>
-      <c r="N42" s="46">
-        <v>0</v>
-      </c>
-      <c r="O42" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="P42" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q42" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="R42" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="S42" s="17" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="43" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="12">
-        <v>2035</v>
-      </c>
-      <c r="B43" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="C43" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D43" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="E43" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="F43" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G43" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H43" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I43" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="J43" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="K43" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="L43" s="12">
-        <v>15.85</v>
-      </c>
-      <c r="M43" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="N43" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="O43" s="14">
-        <v>1.27</v>
-      </c>
-      <c r="P43" s="14">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="Q43" s="14">
-        <v>120</v>
-      </c>
-      <c r="R43" s="14">
-        <v>0</v>
-      </c>
-      <c r="S43" s="14">
-        <v>45</v>
+      <c r="N43" s="46">
+        <v>0</v>
+      </c>
+      <c r="O43" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="P43" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q43" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="R43" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="S43" s="17" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="44" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -3304,7 +3298,7 @@
         <v>2035</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C44" s="12" t="s">
         <v>18</v>
@@ -3313,7 +3307,7 @@
         <v>103</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F44" s="12" t="s">
         <v>10</v>
@@ -3328,13 +3322,13 @@
         <v>105</v>
       </c>
       <c r="J44" s="13" t="s">
-        <v>110</v>
+        <v>44</v>
       </c>
       <c r="K44" s="12" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="L44" s="12">
-        <v>18.64</v>
+        <v>15.85</v>
       </c>
       <c r="M44" s="47" t="s">
         <v>111</v>
@@ -3363,7 +3357,7 @@
         <v>2035</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C45" s="12" t="s">
         <v>18</v>
@@ -3372,7 +3366,7 @@
         <v>103</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F45" s="12" t="s">
         <v>10</v>
@@ -3387,10 +3381,10 @@
         <v>105</v>
       </c>
       <c r="J45" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K45" s="12" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="L45" s="12">
         <v>18.64</v>
@@ -3408,13 +3402,13 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="Q45" s="14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="R45" s="14">
         <v>0</v>
       </c>
       <c r="S45" s="14">
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -3422,7 +3416,7 @@
         <v>2035</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="C46" s="12" t="s">
         <v>18</v>
@@ -3431,7 +3425,7 @@
         <v>103</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="F46" s="12" t="s">
         <v>10</v>
@@ -3446,10 +3440,10 @@
         <v>105</v>
       </c>
       <c r="J46" s="13" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="K46" s="12" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="L46" s="12">
         <v>18.64</v>
@@ -3460,20 +3454,20 @@
       <c r="N46" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="O46" s="12">
-        <v>0.95</v>
-      </c>
-      <c r="P46" s="12">
-        <v>0.86</v>
+      <c r="O46" s="14">
+        <v>1.27</v>
+      </c>
+      <c r="P46" s="14">
+        <v>1.1499999999999999</v>
       </c>
       <c r="Q46" s="14">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="R46" s="14">
         <v>0</v>
       </c>
       <c r="S46" s="14">
-        <v>45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -3481,7 +3475,7 @@
         <v>2035</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C47" s="12" t="s">
         <v>18</v>
@@ -3490,7 +3484,7 @@
         <v>103</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F47" s="12" t="s">
         <v>10</v>
@@ -3505,10 +3499,10 @@
         <v>105</v>
       </c>
       <c r="J47" s="13" t="s">
-        <v>43</v>
+        <v>110</v>
       </c>
       <c r="K47" s="12" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="L47" s="12">
         <v>18.64</v>
@@ -3526,68 +3520,127 @@
         <v>0.86</v>
       </c>
       <c r="Q47" s="14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="R47" s="14">
         <v>0</v>
       </c>
       <c r="S47" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="24">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="F48" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G48" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H48" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I48" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="J48" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K48" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="L48" s="12">
+        <v>18.64</v>
+      </c>
+      <c r="M48" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="N48" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="O48" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="P48" s="12">
+        <v>0.86</v>
+      </c>
+      <c r="Q48" s="14">
+        <v>0</v>
+      </c>
+      <c r="R48" s="14">
+        <v>0</v>
+      </c>
+      <c r="S48" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="24">
         <v>2050</v>
       </c>
-      <c r="B48" s="24" t="s">
+      <c r="B49" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="C48" s="24" t="s">
+      <c r="C49" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="D48" s="24" t="s">
+      <c r="D49" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="E48" s="24" t="s">
+      <c r="E49" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="F48" s="24" t="s">
+      <c r="F49" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="G48" s="25" t="s">
+      <c r="G49" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="I48" s="24" t="s">
+      <c r="I49" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="J48" s="26" t="s">
+      <c r="J49" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="K48" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="L48" s="24">
+      <c r="K49" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="L49" s="24">
         <v>17.440000000000001</v>
       </c>
-      <c r="M48" s="48">
+      <c r="M49" s="48">
         <v>-0.33</v>
       </c>
-      <c r="N48" s="48">
-        <v>0</v>
-      </c>
-      <c r="O48" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="P48" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q48" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="R48" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="S48" s="27" t="s">
+      <c r="N49" s="48">
+        <v>0</v>
+      </c>
+      <c r="O49" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="P49" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q49" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="R49" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="S49" s="27" t="s">
         <v>111</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added 2023 v30 (higher tolls) to the model run log
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B663026C-FC1F-4A5E-BA1B-D9EBD3CE19E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE6B2728-B2C3-4088-9C76-A66D65A069C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="178">
   <si>
     <t>year</t>
   </si>
@@ -558,6 +558,18 @@
   </si>
   <si>
     <t>https://app.asana.com/0/1204085012544660/1205838169476835/f</t>
+  </si>
+  <si>
+    <t>2023_TM160_IPA_30</t>
+  </si>
+  <si>
+    <t>Higher tolls, WFH remains at ~25%</t>
+  </si>
+  <si>
+    <t>BlueprintNetworks_v11\net_2023_Blueprint</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1205866185692454/f</t>
   </si>
 </sst>
 </file>
@@ -1118,11 +1130,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9564CC59-3725-4FDA-8BF2-0F68CB1B6F5A}">
-  <dimension ref="A1:S49"/>
+  <dimension ref="A1:S50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A41" sqref="A41"/>
+      <selection pane="bottomLeft" activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -3203,153 +3215,153 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="28">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A42" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="J42" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="L42" s="1">
+        <v>17.77</v>
+      </c>
+      <c r="M42" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="N42" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="O42" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="P42" s="1">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="Q42" s="6">
+        <v>120</v>
+      </c>
+      <c r="R42" s="6">
+        <v>0</v>
+      </c>
+      <c r="S42" s="6">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="28">
         <v>2025</v>
       </c>
-      <c r="B42" s="28" t="s">
+      <c r="B43" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="C42" s="28" t="s">
+      <c r="C43" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="D42" s="28" t="s">
+      <c r="D43" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="E42" s="28" t="s">
+      <c r="E43" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="H42" s="28" t="s">
+      <c r="H43" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="I42" s="28" t="s">
+      <c r="I43" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="J42" s="29" t="s">
+      <c r="J43" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="M42" s="45"/>
-      <c r="N42" s="45"/>
-      <c r="Q42" s="30"/>
-      <c r="R42" s="30"/>
-      <c r="S42" s="30"/>
-    </row>
-    <row r="43" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="15">
+      <c r="M43" s="45"/>
+      <c r="N43" s="45"/>
+      <c r="Q43" s="30"/>
+      <c r="R43" s="30"/>
+      <c r="S43" s="30"/>
+    </row>
+    <row r="44" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="15">
         <v>2035</v>
       </c>
-      <c r="B43" s="15" t="s">
+      <c r="B44" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="C43" s="15" t="s">
+      <c r="C44" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="D43" s="15" t="s">
+      <c r="D44" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="E43" s="15" t="s">
+      <c r="E44" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="F43" s="15" t="s">
+      <c r="F44" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="G43" s="18" t="s">
+      <c r="G44" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="H43" s="15" t="s">
+      <c r="H44" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I43" s="15" t="s">
+      <c r="I44" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="J43" s="16" t="s">
+      <c r="J44" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="K43" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="L43" s="15">
+      <c r="K44" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="L44" s="15">
         <v>15.85</v>
       </c>
-      <c r="M43" s="46">
+      <c r="M44" s="46">
         <v>-0.27</v>
       </c>
-      <c r="N43" s="46">
-        <v>0</v>
-      </c>
-      <c r="O43" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="P43" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q43" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="R43" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="S43" s="17" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="44" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="12">
-        <v>2035</v>
-      </c>
-      <c r="B44" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="C44" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D44" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="E44" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="F44" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G44" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H44" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I44" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="J44" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="K44" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="L44" s="12">
-        <v>15.85</v>
-      </c>
-      <c r="M44" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="N44" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="O44" s="14">
-        <v>1.27</v>
-      </c>
-      <c r="P44" s="14">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="Q44" s="14">
-        <v>120</v>
-      </c>
-      <c r="R44" s="14">
-        <v>0</v>
-      </c>
-      <c r="S44" s="14">
-        <v>45</v>
+      <c r="N44" s="46">
+        <v>0</v>
+      </c>
+      <c r="O44" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="P44" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q44" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="R44" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="S44" s="17" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="45" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -3357,7 +3369,7 @@
         <v>2035</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C45" s="12" t="s">
         <v>18</v>
@@ -3366,7 +3378,7 @@
         <v>103</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F45" s="12" t="s">
         <v>10</v>
@@ -3381,13 +3393,13 @@
         <v>105</v>
       </c>
       <c r="J45" s="13" t="s">
-        <v>110</v>
+        <v>44</v>
       </c>
       <c r="K45" s="12" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="L45" s="12">
-        <v>18.64</v>
+        <v>15.85</v>
       </c>
       <c r="M45" s="47" t="s">
         <v>111</v>
@@ -3416,7 +3428,7 @@
         <v>2035</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C46" s="12" t="s">
         <v>18</v>
@@ -3425,7 +3437,7 @@
         <v>103</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F46" s="12" t="s">
         <v>10</v>
@@ -3440,10 +3452,10 @@
         <v>105</v>
       </c>
       <c r="J46" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K46" s="12" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="L46" s="12">
         <v>18.64</v>
@@ -3461,13 +3473,13 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="Q46" s="14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="R46" s="14">
         <v>0</v>
       </c>
       <c r="S46" s="14">
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -3475,7 +3487,7 @@
         <v>2035</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="C47" s="12" t="s">
         <v>18</v>
@@ -3484,7 +3496,7 @@
         <v>103</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="F47" s="12" t="s">
         <v>10</v>
@@ -3499,10 +3511,10 @@
         <v>105</v>
       </c>
       <c r="J47" s="13" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="K47" s="12" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="L47" s="12">
         <v>18.64</v>
@@ -3513,20 +3525,20 @@
       <c r="N47" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="O47" s="12">
-        <v>0.95</v>
-      </c>
-      <c r="P47" s="12">
-        <v>0.86</v>
+      <c r="O47" s="14">
+        <v>1.27</v>
+      </c>
+      <c r="P47" s="14">
+        <v>1.1499999999999999</v>
       </c>
       <c r="Q47" s="14">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="R47" s="14">
         <v>0</v>
       </c>
       <c r="S47" s="14">
-        <v>45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -3534,7 +3546,7 @@
         <v>2035</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C48" s="12" t="s">
         <v>18</v>
@@ -3543,7 +3555,7 @@
         <v>103</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F48" s="12" t="s">
         <v>10</v>
@@ -3558,10 +3570,10 @@
         <v>105</v>
       </c>
       <c r="J48" s="13" t="s">
-        <v>43</v>
+        <v>110</v>
       </c>
       <c r="K48" s="12" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="L48" s="12">
         <v>18.64</v>
@@ -3579,68 +3591,127 @@
         <v>0.86</v>
       </c>
       <c r="Q48" s="14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="R48" s="14">
         <v>0</v>
       </c>
       <c r="S48" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="24">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="C49" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E49" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="F49" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G49" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H49" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I49" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="J49" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K49" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="L49" s="12">
+        <v>18.64</v>
+      </c>
+      <c r="M49" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="N49" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="O49" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="P49" s="12">
+        <v>0.86</v>
+      </c>
+      <c r="Q49" s="14">
+        <v>0</v>
+      </c>
+      <c r="R49" s="14">
+        <v>0</v>
+      </c>
+      <c r="S49" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="24">
         <v>2050</v>
       </c>
-      <c r="B49" s="24" t="s">
+      <c r="B50" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="C49" s="24" t="s">
+      <c r="C50" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="D49" s="24" t="s">
+      <c r="D50" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="E49" s="24" t="s">
+      <c r="E50" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="F49" s="24" t="s">
+      <c r="F50" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="G49" s="25" t="s">
+      <c r="G50" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="I49" s="24" t="s">
+      <c r="I50" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="J49" s="26" t="s">
+      <c r="J50" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="K49" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="L49" s="24">
+      <c r="K50" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="L50" s="24">
         <v>17.440000000000001</v>
       </c>
-      <c r="M49" s="48">
+      <c r="M50" s="48">
         <v>-0.33</v>
       </c>
-      <c r="N49" s="48">
-        <v>0</v>
-      </c>
-      <c r="O49" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="P49" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q49" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="R49" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="S49" s="27" t="s">
+      <c r="N50" s="48">
+        <v>0</v>
+      </c>
+      <c r="O50" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="P50" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q50" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="R50" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="S50" s="27" t="s">
         <v>111</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add v31 (WFH at ~27%) in the model run log
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE6B2728-B2C3-4088-9C76-A66D65A069C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876748D9-CE8F-42CA-A7F7-88A52AE67549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="181">
   <si>
     <t>year</t>
   </si>
@@ -570,6 +570,15 @@
   </si>
   <si>
     <t>https://app.asana.com/0/1204085012544660/1205866185692454/f</t>
+  </si>
+  <si>
+    <t>2023_TM160_IPA_31</t>
+  </si>
+  <si>
+    <t>Higher tolls, WFH remains at ~27%</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1205893933741809/f</t>
   </si>
 </sst>
 </file>
@@ -1130,11 +1139,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9564CC59-3725-4FDA-8BF2-0F68CB1B6F5A}">
-  <dimension ref="A1:S50"/>
+  <dimension ref="A1:S51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A42" sqref="A42"/>
+      <selection pane="bottomLeft" activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -3274,153 +3283,153 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="28">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A43" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="J43" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="L43" s="1">
+        <v>17.77</v>
+      </c>
+      <c r="M43" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="N43" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="O43" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="P43" s="1">
+        <v>0.89</v>
+      </c>
+      <c r="Q43" s="6">
+        <v>120</v>
+      </c>
+      <c r="R43" s="6">
+        <v>0</v>
+      </c>
+      <c r="S43" s="6">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="28">
         <v>2025</v>
       </c>
-      <c r="B43" s="28" t="s">
+      <c r="B44" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="C43" s="28" t="s">
+      <c r="C44" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="D43" s="28" t="s">
+      <c r="D44" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="E43" s="28" t="s">
+      <c r="E44" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="H43" s="28" t="s">
+      <c r="H44" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="I43" s="28" t="s">
+      <c r="I44" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="J43" s="29" t="s">
+      <c r="J44" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="M43" s="45"/>
-      <c r="N43" s="45"/>
-      <c r="Q43" s="30"/>
-      <c r="R43" s="30"/>
-      <c r="S43" s="30"/>
-    </row>
-    <row r="44" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="15">
+      <c r="M44" s="45"/>
+      <c r="N44" s="45"/>
+      <c r="Q44" s="30"/>
+      <c r="R44" s="30"/>
+      <c r="S44" s="30"/>
+    </row>
+    <row r="45" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="15">
         <v>2035</v>
       </c>
-      <c r="B44" s="15" t="s">
+      <c r="B45" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="C44" s="15" t="s">
+      <c r="C45" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="D44" s="15" t="s">
+      <c r="D45" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="E44" s="15" t="s">
+      <c r="E45" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="F44" s="15" t="s">
+      <c r="F45" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="G44" s="18" t="s">
+      <c r="G45" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="H44" s="15" t="s">
+      <c r="H45" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I44" s="15" t="s">
+      <c r="I45" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="J44" s="16" t="s">
+      <c r="J45" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="K44" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="L44" s="15">
+      <c r="K45" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="L45" s="15">
         <v>15.85</v>
       </c>
-      <c r="M44" s="46">
+      <c r="M45" s="46">
         <v>-0.27</v>
       </c>
-      <c r="N44" s="46">
-        <v>0</v>
-      </c>
-      <c r="O44" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="P44" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q44" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="R44" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="S44" s="17" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="45" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="12">
-        <v>2035</v>
-      </c>
-      <c r="B45" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="C45" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D45" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="E45" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="F45" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G45" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H45" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I45" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="J45" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="K45" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="L45" s="12">
-        <v>15.85</v>
-      </c>
-      <c r="M45" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="N45" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="O45" s="14">
-        <v>1.27</v>
-      </c>
-      <c r="P45" s="14">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="Q45" s="14">
-        <v>120</v>
-      </c>
-      <c r="R45" s="14">
-        <v>0</v>
-      </c>
-      <c r="S45" s="14">
-        <v>45</v>
+      <c r="N45" s="46">
+        <v>0</v>
+      </c>
+      <c r="O45" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="P45" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q45" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="R45" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="S45" s="17" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="46" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -3428,7 +3437,7 @@
         <v>2035</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C46" s="12" t="s">
         <v>18</v>
@@ -3437,7 +3446,7 @@
         <v>103</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F46" s="12" t="s">
         <v>10</v>
@@ -3452,13 +3461,13 @@
         <v>105</v>
       </c>
       <c r="J46" s="13" t="s">
-        <v>110</v>
+        <v>44</v>
       </c>
       <c r="K46" s="12" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="L46" s="12">
-        <v>18.64</v>
+        <v>15.85</v>
       </c>
       <c r="M46" s="47" t="s">
         <v>111</v>
@@ -3487,7 +3496,7 @@
         <v>2035</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C47" s="12" t="s">
         <v>18</v>
@@ -3496,7 +3505,7 @@
         <v>103</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F47" s="12" t="s">
         <v>10</v>
@@ -3511,10 +3520,10 @@
         <v>105</v>
       </c>
       <c r="J47" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K47" s="12" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="L47" s="12">
         <v>18.64</v>
@@ -3532,13 +3541,13 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="Q47" s="14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="R47" s="14">
         <v>0</v>
       </c>
       <c r="S47" s="14">
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -3546,7 +3555,7 @@
         <v>2035</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="C48" s="12" t="s">
         <v>18</v>
@@ -3555,7 +3564,7 @@
         <v>103</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="F48" s="12" t="s">
         <v>10</v>
@@ -3570,10 +3579,10 @@
         <v>105</v>
       </c>
       <c r="J48" s="13" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="K48" s="12" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="L48" s="12">
         <v>18.64</v>
@@ -3584,20 +3593,20 @@
       <c r="N48" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="O48" s="12">
-        <v>0.95</v>
-      </c>
-      <c r="P48" s="12">
-        <v>0.86</v>
+      <c r="O48" s="14">
+        <v>1.27</v>
+      </c>
+      <c r="P48" s="14">
+        <v>1.1499999999999999</v>
       </c>
       <c r="Q48" s="14">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="R48" s="14">
         <v>0</v>
       </c>
       <c r="S48" s="14">
-        <v>45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -3605,7 +3614,7 @@
         <v>2035</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C49" s="12" t="s">
         <v>18</v>
@@ -3614,7 +3623,7 @@
         <v>103</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F49" s="12" t="s">
         <v>10</v>
@@ -3629,10 +3638,10 @@
         <v>105</v>
       </c>
       <c r="J49" s="13" t="s">
-        <v>43</v>
+        <v>110</v>
       </c>
       <c r="K49" s="12" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="L49" s="12">
         <v>18.64</v>
@@ -3650,68 +3659,127 @@
         <v>0.86</v>
       </c>
       <c r="Q49" s="14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="R49" s="14">
         <v>0</v>
       </c>
       <c r="S49" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="24">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="F50" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G50" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H50" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I50" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="J50" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K50" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="L50" s="12">
+        <v>18.64</v>
+      </c>
+      <c r="M50" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="N50" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="O50" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="P50" s="12">
+        <v>0.86</v>
+      </c>
+      <c r="Q50" s="14">
+        <v>0</v>
+      </c>
+      <c r="R50" s="14">
+        <v>0</v>
+      </c>
+      <c r="S50" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="24">
         <v>2050</v>
       </c>
-      <c r="B50" s="24" t="s">
+      <c r="B51" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="C50" s="24" t="s">
+      <c r="C51" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="D50" s="24" t="s">
+      <c r="D51" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="E50" s="24" t="s">
+      <c r="E51" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="F50" s="24" t="s">
+      <c r="F51" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="G50" s="25" t="s">
+      <c r="G51" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="I50" s="24" t="s">
+      <c r="I51" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="J50" s="26" t="s">
+      <c r="J51" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="K50" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="L50" s="24">
+      <c r="K51" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="L51" s="24">
         <v>17.440000000000001</v>
       </c>
-      <c r="M50" s="48">
+      <c r="M51" s="48">
         <v>-0.33</v>
       </c>
-      <c r="N50" s="48">
-        <v>0</v>
-      </c>
-      <c r="O50" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="P50" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q50" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="R50" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="S50" s="27" t="s">
+      <c r="N51" s="48">
+        <v>0</v>
+      </c>
+      <c r="O51" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="P51" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q51" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="R51" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="S51" s="27" t="s">
         <v>111</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added 2023 runs with different WFH and transit hesitancy levels (v32 to v37) to the run log
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876748D9-CE8F-42CA-A7F7-88A52AE67549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FFBECA8-9E07-41F1-BEE8-804620E1DAF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="203">
   <si>
     <t>year</t>
   </si>
@@ -575,10 +575,76 @@
     <t>2023_TM160_IPA_31</t>
   </si>
   <si>
-    <t>Higher tolls, WFH remains at ~27%</t>
-  </si>
-  <si>
     <t>https://app.asana.com/0/1204085012544660/1205893933741809/f</t>
+  </si>
+  <si>
+    <t>2023_TM160_IPA_32</t>
+  </si>
+  <si>
+    <t>Higher tolls, WFH at ~27%</t>
+  </si>
+  <si>
+    <t>BlueprintNetworks_v12\net_2023_Blueprint</t>
+  </si>
+  <si>
+    <t>Toll rate fixes, WFH at ~27%</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1205909635346843/f</t>
+  </si>
+  <si>
+    <t>Toll rate fixes, WFH at ~29%</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1205910032623946/f</t>
+  </si>
+  <si>
+    <t>2023_TM160_IPA_33</t>
+  </si>
+  <si>
+    <t>2023_TM160_IPA_34</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1205800562404712/f</t>
+  </si>
+  <si>
+    <t>work trn hes=100, rail/ferry hes=60, WFH at ~27%</t>
+  </si>
+  <si>
+    <t>2023_TM160_IPA_35</t>
+  </si>
+  <si>
+    <t>work trn hes=100, rail/ferry hes=60, WFH at ~29%</t>
+  </si>
+  <si>
+    <t>2035_TM160_IPA_06</t>
+  </si>
+  <si>
+    <t>same as v05 except for nonres</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1205911053939954/f</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1205909635346849/f</t>
+  </si>
+  <si>
+    <t>2023_TM160_IPA_36</t>
+  </si>
+  <si>
+    <t>2023_TM160_IPA_37</t>
+  </si>
+  <si>
+    <t>work trn hes=90, rail/ferry hes=70, WFH at ~27%</t>
+  </si>
+  <si>
+    <t>work trn hes=90, rail/ferry hes=70, WFH at ~29%</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1205912003541563/f</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1205912003541566/f</t>
   </si>
 </sst>
 </file>
@@ -588,7 +654,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -628,6 +694,14 @@
       <color rgb="FFFF0000"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -713,10 +787,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -825,8 +900,18 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1139,11 +1224,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9564CC59-3725-4FDA-8BF2-0F68CB1B6F5A}">
-  <dimension ref="A1:S51"/>
+  <dimension ref="A1:S58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E43" sqref="E43"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E20" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A44" sqref="A44:XFD49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1152,7 +1239,7 @@
     <col min="2" max="2" width="27.6328125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.81640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.81640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="28.6328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="42.26953125" style="1" customWidth="1"/>
     <col min="6" max="6" width="11.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.1796875" style="1" customWidth="1"/>
     <col min="8" max="8" width="6.7265625" style="1" bestFit="1" customWidth="1"/>
@@ -3010,9 +3097,6 @@
       <c r="G38" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H38" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="I38" s="1" t="s">
         <v>80</v>
       </c>
@@ -3069,9 +3153,6 @@
       <c r="G39" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H39" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="I39" s="1" t="s">
         <v>167</v>
       </c>
@@ -3128,9 +3209,6 @@
       <c r="G40" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H40" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="I40" s="1" t="s">
         <v>167</v>
       </c>
@@ -3187,9 +3265,6 @@
       <c r="G41" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H41" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="I41" s="1" t="s">
         <v>167</v>
       </c>
@@ -3297,7 +3372,7 @@
         <v>7</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>10</v>
@@ -3315,7 +3390,7 @@
         <v>17</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="L43" s="1">
         <v>17.77</v>
@@ -3342,444 +3417,857 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="28">
+    <row r="44" spans="1:19" s="50" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="50">
+        <v>2023</v>
+      </c>
+      <c r="B44" s="50" t="s">
+        <v>180</v>
+      </c>
+      <c r="C44" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" s="50" t="s">
+        <v>183</v>
+      </c>
+      <c r="F44" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="G44" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="H44" s="50" t="s">
+        <v>12</v>
+      </c>
+      <c r="I44" s="50" t="s">
+        <v>182</v>
+      </c>
+      <c r="J44" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="K44" s="50" t="s">
+        <v>184</v>
+      </c>
+      <c r="L44" s="50">
+        <v>17.77</v>
+      </c>
+      <c r="M44" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="N44" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="O44" s="50">
+        <v>0.99</v>
+      </c>
+      <c r="P44" s="50">
+        <v>0.89</v>
+      </c>
+      <c r="Q44" s="53">
+        <v>120</v>
+      </c>
+      <c r="R44" s="53">
+        <v>0</v>
+      </c>
+      <c r="S44" s="53">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" s="50" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="50">
+        <v>2023</v>
+      </c>
+      <c r="B45" s="50" t="s">
+        <v>187</v>
+      </c>
+      <c r="C45" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" s="50" t="s">
+        <v>185</v>
+      </c>
+      <c r="F45" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="G45" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="H45" s="50" t="s">
+        <v>12</v>
+      </c>
+      <c r="I45" s="50" t="s">
+        <v>182</v>
+      </c>
+      <c r="J45" s="51" t="s">
+        <v>112</v>
+      </c>
+      <c r="K45" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="L45" s="50">
+        <v>17.77</v>
+      </c>
+      <c r="M45" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="N45" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="O45" s="50">
+        <v>1.04</v>
+      </c>
+      <c r="P45" s="50">
+        <v>0.94</v>
+      </c>
+      <c r="Q45" s="53">
+        <v>120</v>
+      </c>
+      <c r="R45" s="53">
+        <v>0</v>
+      </c>
+      <c r="S45" s="53">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" s="50" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="50">
+        <v>2023</v>
+      </c>
+      <c r="B46" s="50" t="s">
+        <v>188</v>
+      </c>
+      <c r="C46" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="D46" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E46" s="50" t="s">
+        <v>190</v>
+      </c>
+      <c r="F46" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="G46" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="H46" s="50" t="s">
+        <v>12</v>
+      </c>
+      <c r="I46" s="50" t="s">
+        <v>182</v>
+      </c>
+      <c r="J46" s="51" t="s">
+        <v>45</v>
+      </c>
+      <c r="K46" s="50" t="s">
+        <v>189</v>
+      </c>
+      <c r="L46" s="50">
+        <v>17.77</v>
+      </c>
+      <c r="M46" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="N46" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="O46" s="50">
+        <v>0.99</v>
+      </c>
+      <c r="P46" s="50">
+        <v>0.89</v>
+      </c>
+      <c r="Q46" s="53">
+        <v>100</v>
+      </c>
+      <c r="R46" s="53">
+        <v>0</v>
+      </c>
+      <c r="S46" s="53">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" s="50" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="50">
+        <v>2023</v>
+      </c>
+      <c r="B47" s="50" t="s">
+        <v>191</v>
+      </c>
+      <c r="C47" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="D47" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" s="50" t="s">
+        <v>192</v>
+      </c>
+      <c r="F47" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="G47" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="H47" s="50" t="s">
+        <v>12</v>
+      </c>
+      <c r="I47" s="50" t="s">
+        <v>182</v>
+      </c>
+      <c r="J47" s="51" t="s">
+        <v>132</v>
+      </c>
+      <c r="K47" s="50" t="s">
+        <v>195</v>
+      </c>
+      <c r="L47" s="50">
+        <v>17.77</v>
+      </c>
+      <c r="M47" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="N47" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="O47" s="50">
+        <v>1.04</v>
+      </c>
+      <c r="P47" s="50">
+        <v>0.94</v>
+      </c>
+      <c r="Q47" s="53">
+        <v>100</v>
+      </c>
+      <c r="R47" s="53">
+        <v>0</v>
+      </c>
+      <c r="S47" s="53">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" s="50" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A48" s="50">
+        <v>2023</v>
+      </c>
+      <c r="B48" s="50" t="s">
+        <v>197</v>
+      </c>
+      <c r="C48" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="D48" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E48" s="50" t="s">
+        <v>199</v>
+      </c>
+      <c r="F48" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="G48" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="H48" s="50" t="s">
+        <v>12</v>
+      </c>
+      <c r="I48" s="50" t="s">
+        <v>182</v>
+      </c>
+      <c r="J48" s="51" t="s">
+        <v>44</v>
+      </c>
+      <c r="K48" s="54" t="s">
+        <v>201</v>
+      </c>
+      <c r="L48" s="50">
+        <v>17.77</v>
+      </c>
+      <c r="M48" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="N48" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="O48" s="50">
+        <v>0.99</v>
+      </c>
+      <c r="P48" s="50">
+        <v>0.89</v>
+      </c>
+      <c r="Q48" s="53">
+        <v>90</v>
+      </c>
+      <c r="R48" s="53">
+        <v>0</v>
+      </c>
+      <c r="S48" s="53">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" s="50" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="50">
+        <v>2023</v>
+      </c>
+      <c r="B49" s="50" t="s">
+        <v>198</v>
+      </c>
+      <c r="C49" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="D49" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49" s="50" t="s">
+        <v>200</v>
+      </c>
+      <c r="F49" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="G49" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="H49" s="50" t="s">
+        <v>12</v>
+      </c>
+      <c r="I49" s="50" t="s">
+        <v>182</v>
+      </c>
+      <c r="J49" s="51" t="s">
+        <v>89</v>
+      </c>
+      <c r="K49" s="50" t="s">
+        <v>202</v>
+      </c>
+      <c r="L49" s="50">
+        <v>17.77</v>
+      </c>
+      <c r="M49" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="N49" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="O49" s="50">
+        <v>1.04</v>
+      </c>
+      <c r="P49" s="50">
+        <v>0.94</v>
+      </c>
+      <c r="Q49" s="53">
+        <v>90</v>
+      </c>
+      <c r="R49" s="53">
+        <v>0</v>
+      </c>
+      <c r="S49" s="53">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="28">
         <v>2025</v>
       </c>
-      <c r="B44" s="28" t="s">
+      <c r="B50" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="C44" s="28" t="s">
+      <c r="C50" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="D44" s="28" t="s">
+      <c r="D50" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="E44" s="28" t="s">
+      <c r="E50" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="H44" s="28" t="s">
+      <c r="H50" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="I44" s="28" t="s">
+      <c r="I50" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="J44" s="29" t="s">
+      <c r="J50" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="M44" s="45"/>
-      <c r="N44" s="45"/>
-      <c r="Q44" s="30"/>
-      <c r="R44" s="30"/>
-      <c r="S44" s="30"/>
-    </row>
-    <row r="45" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="15">
+      <c r="M50" s="45"/>
+      <c r="N50" s="45"/>
+      <c r="Q50" s="30"/>
+      <c r="R50" s="30"/>
+      <c r="S50" s="30"/>
+    </row>
+    <row r="51" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="15">
         <v>2035</v>
       </c>
-      <c r="B45" s="15" t="s">
+      <c r="B51" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="C45" s="15" t="s">
+      <c r="C51" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="D45" s="15" t="s">
+      <c r="D51" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="E45" s="15" t="s">
+      <c r="E51" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="F45" s="15" t="s">
+      <c r="F51" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="G45" s="18" t="s">
+      <c r="G51" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="H45" s="15" t="s">
+      <c r="H51" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="15" t="s">
+      <c r="I51" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="J45" s="16" t="s">
+      <c r="J51" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="K45" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="L45" s="15">
+      <c r="K51" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="L51" s="15">
         <v>15.85</v>
       </c>
-      <c r="M45" s="46">
+      <c r="M51" s="46">
         <v>-0.27</v>
       </c>
-      <c r="N45" s="46">
-        <v>0</v>
-      </c>
-      <c r="O45" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="P45" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q45" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="R45" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="S45" s="17" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="46" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="12">
+      <c r="N51" s="46">
+        <v>0</v>
+      </c>
+      <c r="O51" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="P51" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q51" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="R51" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="S51" s="17" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="12">
         <v>2035</v>
       </c>
-      <c r="B46" s="12" t="s">
+      <c r="B52" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="C46" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D46" s="12" t="s">
+      <c r="C52" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D52" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="E46" s="12" t="s">
+      <c r="E52" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="F46" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G46" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H46" s="12" t="s">
+      <c r="F52" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G52" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H52" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="12" t="s">
+      <c r="I52" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="J46" s="13" t="s">
+      <c r="J52" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="K46" s="12" t="s">
+      <c r="K52" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="L46" s="12">
+      <c r="L52" s="12">
         <v>15.85</v>
       </c>
-      <c r="M46" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="N46" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="O46" s="14">
+      <c r="M52" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="N52" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="O52" s="14">
         <v>1.27</v>
       </c>
-      <c r="P46" s="14">
+      <c r="P52" s="14">
         <v>1.1499999999999999</v>
       </c>
-      <c r="Q46" s="14">
+      <c r="Q52" s="14">
         <v>120</v>
       </c>
-      <c r="R46" s="14">
-        <v>0</v>
-      </c>
-      <c r="S46" s="14">
+      <c r="R52" s="14">
+        <v>0</v>
+      </c>
+      <c r="S52" s="14">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="12">
+    <row r="53" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="12">
         <v>2035</v>
       </c>
-      <c r="B47" s="12" t="s">
+      <c r="B53" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="C47" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D47" s="12" t="s">
+      <c r="C53" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D53" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="E47" s="12" t="s">
+      <c r="E53" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="F47" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G47" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H47" s="12" t="s">
+      <c r="F53" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G53" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H53" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="I47" s="12" t="s">
+      <c r="I53" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="J47" s="13" t="s">
+      <c r="J53" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="K47" s="12" t="s">
+      <c r="K53" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="L47" s="12">
+      <c r="L53" s="12">
         <v>18.64</v>
       </c>
-      <c r="M47" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="N47" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="O47" s="14">
+      <c r="M53" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="N53" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="O53" s="14">
         <v>1.27</v>
       </c>
-      <c r="P47" s="14">
+      <c r="P53" s="14">
         <v>1.1499999999999999</v>
       </c>
-      <c r="Q47" s="14">
+      <c r="Q53" s="14">
         <v>120</v>
       </c>
-      <c r="R47" s="14">
-        <v>0</v>
-      </c>
-      <c r="S47" s="14">
+      <c r="R53" s="14">
+        <v>0</v>
+      </c>
+      <c r="S53" s="14">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="12">
+    <row r="54" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="12">
         <v>2035</v>
       </c>
-      <c r="B48" s="12" t="s">
+      <c r="B54" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="C48" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D48" s="12" t="s">
+      <c r="C54" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D54" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="E48" s="12" t="s">
+      <c r="E54" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="F48" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G48" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H48" s="12" t="s">
+      <c r="F54" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G54" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H54" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="I48" s="12" t="s">
+      <c r="I54" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="J48" s="13" t="s">
+      <c r="J54" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="K48" s="12" t="s">
+      <c r="K54" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="L48" s="12">
+      <c r="L54" s="12">
         <v>18.64</v>
       </c>
-      <c r="M48" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="N48" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="O48" s="14">
+      <c r="M54" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="N54" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="O54" s="14">
         <v>1.27</v>
       </c>
-      <c r="P48" s="14">
+      <c r="P54" s="14">
         <v>1.1499999999999999</v>
       </c>
-      <c r="Q48" s="14">
-        <v>0</v>
-      </c>
-      <c r="R48" s="14">
-        <v>0</v>
-      </c>
-      <c r="S48" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="12">
+      <c r="Q54" s="14">
+        <v>0</v>
+      </c>
+      <c r="R54" s="14">
+        <v>0</v>
+      </c>
+      <c r="S54" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="12">
         <v>2035</v>
       </c>
-      <c r="B49" s="12" t="s">
+      <c r="B55" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="C49" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D49" s="12" t="s">
+      <c r="C55" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D55" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="E49" s="12" t="s">
+      <c r="E55" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="F49" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G49" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H49" s="12" t="s">
+      <c r="F55" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G55" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H55" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="I49" s="12" t="s">
+      <c r="I55" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="J49" s="13" t="s">
+      <c r="J55" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="K49" s="12" t="s">
+      <c r="K55" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="L49" s="12">
+      <c r="L55" s="12">
         <v>18.64</v>
       </c>
-      <c r="M49" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="N49" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="O49" s="12">
+      <c r="M55" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="N55" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="O55" s="12">
         <v>0.95</v>
       </c>
-      <c r="P49" s="12">
+      <c r="P55" s="12">
         <v>0.86</v>
       </c>
-      <c r="Q49" s="14">
+      <c r="Q55" s="14">
         <v>120</v>
       </c>
-      <c r="R49" s="14">
-        <v>0</v>
-      </c>
-      <c r="S49" s="14">
+      <c r="R55" s="14">
+        <v>0</v>
+      </c>
+      <c r="S55" s="14">
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="12">
+    <row r="56" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="12">
         <v>2035</v>
       </c>
-      <c r="B50" s="12" t="s">
+      <c r="B56" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="C50" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D50" s="12" t="s">
+      <c r="C56" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D56" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="E50" s="12" t="s">
+      <c r="E56" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="F50" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G50" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H50" s="12" t="s">
+      <c r="F56" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G56" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H56" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="I50" s="12" t="s">
+      <c r="I56" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="J50" s="13" t="s">
+      <c r="J56" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="K50" s="12" t="s">
+      <c r="K56" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="L50" s="12">
+      <c r="L56" s="12">
         <v>18.64</v>
       </c>
-      <c r="M50" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="N50" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="O50" s="12">
+      <c r="M56" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="N56" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="O56" s="12">
         <v>0.95</v>
       </c>
-      <c r="P50" s="12">
+      <c r="P56" s="12">
         <v>0.86</v>
       </c>
-      <c r="Q50" s="14">
-        <v>0</v>
-      </c>
-      <c r="R50" s="14">
-        <v>0</v>
-      </c>
-      <c r="S50" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="24">
+      <c r="Q56" s="14">
+        <v>0</v>
+      </c>
+      <c r="R56" s="14">
+        <v>0</v>
+      </c>
+      <c r="S56" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B57" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D57" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E57" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="F57" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G57" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H57" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I57" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="J57" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="K57" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="L57" s="12">
+        <v>18.64</v>
+      </c>
+      <c r="M57" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="N57" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="O57" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="P57" s="12">
+        <v>0.86</v>
+      </c>
+      <c r="Q57" s="14">
+        <v>0</v>
+      </c>
+      <c r="R57" s="14">
+        <v>0</v>
+      </c>
+      <c r="S57" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="24">
         <v>2050</v>
       </c>
-      <c r="B51" s="24" t="s">
+      <c r="B58" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="C51" s="24" t="s">
+      <c r="C58" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="D51" s="24" t="s">
+      <c r="D58" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="E51" s="24" t="s">
+      <c r="E58" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="F51" s="24" t="s">
+      <c r="F58" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="G51" s="25" t="s">
+      <c r="G58" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="I51" s="24" t="s">
+      <c r="I58" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="J51" s="26" t="s">
+      <c r="J58" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="K51" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="L51" s="24">
+      <c r="K58" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="L58" s="24">
         <v>17.440000000000001</v>
       </c>
-      <c r="M51" s="48">
+      <c r="M58" s="48">
         <v>-0.33</v>
       </c>
-      <c r="N51" s="48">
-        <v>0</v>
-      </c>
-      <c r="O51" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="P51" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q51" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="R51" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="S51" s="27" t="s">
+      <c r="N58" s="48">
+        <v>0</v>
+      </c>
+      <c r="O58" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="P58" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q58" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="R58" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="S58" s="27" t="s">
         <v>111</v>
       </c>
     </row>
@@ -3789,8 +4277,9 @@
     <hyperlink ref="K5" r:id="rId1" xr:uid="{1BE7DD4C-B567-4320-9B69-E8B55CE41797}"/>
     <hyperlink ref="K6" r:id="rId2" xr:uid="{A52BF015-28DA-4569-A638-6E56CCBD2F4D}"/>
     <hyperlink ref="K7" r:id="rId3" xr:uid="{70B88B93-E906-4801-9012-B01BCDB48CBF}"/>
+    <hyperlink ref="K48" r:id="rId4" xr:uid="{AE2270FD-647C-4E5C-90C3-53AF1778C16F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added v38 to the run log (transit hesitancy was increased to 80)
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FFBECA8-9E07-41F1-BEE8-804620E1DAF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63848503-B520-4834-A9EC-CC1363653561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="205">
   <si>
     <t>year</t>
   </si>
@@ -581,21 +581,12 @@
     <t>2023_TM160_IPA_32</t>
   </si>
   <si>
-    <t>Higher tolls, WFH at ~27%</t>
-  </si>
-  <si>
     <t>BlueprintNetworks_v12\net_2023_Blueprint</t>
   </si>
   <si>
-    <t>Toll rate fixes, WFH at ~27%</t>
-  </si>
-  <si>
     <t>https://app.asana.com/0/1204085012544660/1205909635346843/f</t>
   </si>
   <si>
-    <t>Toll rate fixes, WFH at ~29%</t>
-  </si>
-  <si>
     <t>https://app.asana.com/0/1204085012544660/1205910032623946/f</t>
   </si>
   <si>
@@ -608,15 +599,9 @@
     <t>https://app.asana.com/0/1204085012544660/1205800562404712/f</t>
   </si>
   <si>
-    <t>work trn hes=100, rail/ferry hes=60, WFH at ~27%</t>
-  </si>
-  <si>
     <t>2023_TM160_IPA_35</t>
   </si>
   <si>
-    <t>work trn hes=100, rail/ferry hes=60, WFH at ~29%</t>
-  </si>
-  <si>
     <t>2035_TM160_IPA_06</t>
   </si>
   <si>
@@ -635,16 +620,37 @@
     <t>2023_TM160_IPA_37</t>
   </si>
   <si>
-    <t>work trn hes=90, rail/ferry hes=70, WFH at ~27%</t>
-  </si>
-  <si>
-    <t>work trn hes=90, rail/ferry hes=70, WFH at ~29%</t>
-  </si>
-  <si>
     <t>https://app.asana.com/0/1204085012544660/1205912003541563/f</t>
   </si>
   <si>
     <t>https://app.asana.com/0/1204085012544660/1205912003541566/f</t>
+  </si>
+  <si>
+    <t>2023_TM160_IPA_38</t>
+  </si>
+  <si>
+    <t>work trn hes=100, rail/ferry hes=80, WFH at ~30%</t>
+  </si>
+  <si>
+    <t>work trn hes=90, rail/ferry hes=70, WFH at ~31%</t>
+  </si>
+  <si>
+    <t>work trn hes=90, rail/ferry hes=70, WFH at ~30%</t>
+  </si>
+  <si>
+    <t>work trn hes=100, rail/ferry hes=60, WFH at ~31%</t>
+  </si>
+  <si>
+    <t>work trn hes=100, rail/ferry hes=60, WFH at ~30%</t>
+  </si>
+  <si>
+    <t>Toll rate fixes, WFH at ~31%</t>
+  </si>
+  <si>
+    <t>Toll rate fixes, WFH at ~30%</t>
+  </si>
+  <si>
+    <t>Higher tolls, WFH at ~30%</t>
   </si>
 </sst>
 </file>
@@ -791,7 +797,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -900,14 +906,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -1224,13 +1222,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9564CC59-3725-4FDA-8BF2-0F68CB1B6F5A}">
-  <dimension ref="A1:S58"/>
+  <dimension ref="A1:S59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A44" sqref="A44:XFD49"/>
+      <selection pane="bottomRight" activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -3372,7 +3370,7 @@
         <v>7</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>181</v>
+        <v>204</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>10</v>
@@ -3417,507 +3415,504 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:19" s="50" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="50">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A44" s="1">
         <v>2023</v>
       </c>
-      <c r="B44" s="50" t="s">
+      <c r="B44" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="C44" s="50" t="s">
-        <v>18</v>
-      </c>
-      <c r="D44" s="50" t="s">
-        <v>7</v>
-      </c>
-      <c r="E44" s="50" t="s">
+      <c r="C44" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="J44" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="L44" s="1">
+        <v>17.77</v>
+      </c>
+      <c r="M44" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="N44" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="O44" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="P44" s="1">
+        <v>0.89</v>
+      </c>
+      <c r="Q44" s="6">
+        <v>120</v>
+      </c>
+      <c r="R44" s="6">
+        <v>0</v>
+      </c>
+      <c r="S44" s="6">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A45" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="J45" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="K45" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="F44" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="G44" s="50" t="s">
-        <v>11</v>
-      </c>
-      <c r="H44" s="50" t="s">
+      <c r="L45" s="1">
+        <v>17.77</v>
+      </c>
+      <c r="M45" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="N45" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="O45" s="1">
+        <v>1.04</v>
+      </c>
+      <c r="P45" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="Q45" s="6">
+        <v>120</v>
+      </c>
+      <c r="R45" s="6">
+        <v>0</v>
+      </c>
+      <c r="S45" s="6">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A46" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H46" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I44" s="50" t="s">
-        <v>182</v>
-      </c>
-      <c r="J44" s="51" t="s">
+      <c r="I46" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="J46" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="L46" s="1">
+        <v>17.77</v>
+      </c>
+      <c r="M46" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="N46" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="O46" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="P46" s="1">
+        <v>0.89</v>
+      </c>
+      <c r="Q46" s="6">
+        <v>100</v>
+      </c>
+      <c r="R46" s="6">
+        <v>0</v>
+      </c>
+      <c r="S46" s="6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A47" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="J47" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="L47" s="1">
+        <v>17.77</v>
+      </c>
+      <c r="M47" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="N47" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="O47" s="1">
+        <v>1.04</v>
+      </c>
+      <c r="P47" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="Q47" s="6">
+        <v>100</v>
+      </c>
+      <c r="R47" s="6">
+        <v>0</v>
+      </c>
+      <c r="S47" s="6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A48" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="J48" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="K48" s="50" t="s">
+        <v>194</v>
+      </c>
+      <c r="L48" s="1">
+        <v>17.77</v>
+      </c>
+      <c r="M48" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="N48" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="O48" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="P48" s="1">
+        <v>0.89</v>
+      </c>
+      <c r="Q48" s="6">
+        <v>90</v>
+      </c>
+      <c r="R48" s="6">
+        <v>0</v>
+      </c>
+      <c r="S48" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A49" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="J49" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="L49" s="1">
+        <v>17.77</v>
+      </c>
+      <c r="M49" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="N49" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="O49" s="1">
+        <v>1.04</v>
+      </c>
+      <c r="P49" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="Q49" s="6">
+        <v>90</v>
+      </c>
+      <c r="R49" s="6">
+        <v>0</v>
+      </c>
+      <c r="S49" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A50" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="J50" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="L50" s="1">
+        <v>17.77</v>
+      </c>
+      <c r="M50" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="N50" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="O50" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="P50" s="1">
+        <v>0.89</v>
+      </c>
+      <c r="Q50" s="6">
+        <v>100</v>
+      </c>
+      <c r="R50" s="6">
+        <v>0</v>
+      </c>
+      <c r="S50" s="6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="28">
+        <v>2025</v>
+      </c>
+      <c r="B51" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="C51" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="D51" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="E51" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="H51" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="I51" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="J51" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="K44" s="50" t="s">
-        <v>184</v>
-      </c>
-      <c r="L44" s="50">
-        <v>17.77</v>
-      </c>
-      <c r="M44" s="52" t="s">
-        <v>111</v>
-      </c>
-      <c r="N44" s="52" t="s">
-        <v>111</v>
-      </c>
-      <c r="O44" s="50">
-        <v>0.99</v>
-      </c>
-      <c r="P44" s="50">
-        <v>0.89</v>
-      </c>
-      <c r="Q44" s="53">
+      <c r="M51" s="45"/>
+      <c r="N51" s="45"/>
+      <c r="Q51" s="30"/>
+      <c r="R51" s="30"/>
+      <c r="S51" s="30"/>
+    </row>
+    <row r="52" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="15">
+        <v>2035</v>
+      </c>
+      <c r="B52" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C52" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="D52" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="E52" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="F52" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="R44" s="53">
-        <v>0</v>
-      </c>
-      <c r="S44" s="53">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="45" spans="1:19" s="50" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="50">
-        <v>2023</v>
-      </c>
-      <c r="B45" s="50" t="s">
-        <v>187</v>
-      </c>
-      <c r="C45" s="50" t="s">
-        <v>18</v>
-      </c>
-      <c r="D45" s="50" t="s">
-        <v>7</v>
-      </c>
-      <c r="E45" s="50" t="s">
-        <v>185</v>
-      </c>
-      <c r="F45" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="G45" s="50" t="s">
-        <v>11</v>
-      </c>
-      <c r="H45" s="50" t="s">
+      <c r="G52" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="H52" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="50" t="s">
-        <v>182</v>
-      </c>
-      <c r="J45" s="51" t="s">
-        <v>112</v>
-      </c>
-      <c r="K45" s="50" t="s">
-        <v>186</v>
-      </c>
-      <c r="L45" s="50">
-        <v>17.77</v>
-      </c>
-      <c r="M45" s="52" t="s">
-        <v>111</v>
-      </c>
-      <c r="N45" s="52" t="s">
-        <v>111</v>
-      </c>
-      <c r="O45" s="50">
-        <v>1.04</v>
-      </c>
-      <c r="P45" s="50">
-        <v>0.94</v>
-      </c>
-      <c r="Q45" s="53">
-        <v>120</v>
-      </c>
-      <c r="R45" s="53">
-        <v>0</v>
-      </c>
-      <c r="S45" s="53">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="46" spans="1:19" s="50" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="50">
-        <v>2023</v>
-      </c>
-      <c r="B46" s="50" t="s">
-        <v>188</v>
-      </c>
-      <c r="C46" s="50" t="s">
-        <v>18</v>
-      </c>
-      <c r="D46" s="50" t="s">
-        <v>7</v>
-      </c>
-      <c r="E46" s="50" t="s">
-        <v>190</v>
-      </c>
-      <c r="F46" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="G46" s="50" t="s">
-        <v>11</v>
-      </c>
-      <c r="H46" s="50" t="s">
-        <v>12</v>
-      </c>
-      <c r="I46" s="50" t="s">
-        <v>182</v>
-      </c>
-      <c r="J46" s="51" t="s">
-        <v>45</v>
-      </c>
-      <c r="K46" s="50" t="s">
-        <v>189</v>
-      </c>
-      <c r="L46" s="50">
-        <v>17.77</v>
-      </c>
-      <c r="M46" s="52" t="s">
-        <v>111</v>
-      </c>
-      <c r="N46" s="52" t="s">
-        <v>111</v>
-      </c>
-      <c r="O46" s="50">
-        <v>0.99</v>
-      </c>
-      <c r="P46" s="50">
-        <v>0.89</v>
-      </c>
-      <c r="Q46" s="53">
-        <v>100</v>
-      </c>
-      <c r="R46" s="53">
-        <v>0</v>
-      </c>
-      <c r="S46" s="53">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="47" spans="1:19" s="50" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="50">
-        <v>2023</v>
-      </c>
-      <c r="B47" s="50" t="s">
-        <v>191</v>
-      </c>
-      <c r="C47" s="50" t="s">
-        <v>18</v>
-      </c>
-      <c r="D47" s="50" t="s">
-        <v>7</v>
-      </c>
-      <c r="E47" s="50" t="s">
-        <v>192</v>
-      </c>
-      <c r="F47" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="G47" s="50" t="s">
-        <v>11</v>
-      </c>
-      <c r="H47" s="50" t="s">
-        <v>12</v>
-      </c>
-      <c r="I47" s="50" t="s">
-        <v>182</v>
-      </c>
-      <c r="J47" s="51" t="s">
-        <v>132</v>
-      </c>
-      <c r="K47" s="50" t="s">
-        <v>195</v>
-      </c>
-      <c r="L47" s="50">
-        <v>17.77</v>
-      </c>
-      <c r="M47" s="52" t="s">
-        <v>111</v>
-      </c>
-      <c r="N47" s="52" t="s">
-        <v>111</v>
-      </c>
-      <c r="O47" s="50">
-        <v>1.04</v>
-      </c>
-      <c r="P47" s="50">
-        <v>0.94</v>
-      </c>
-      <c r="Q47" s="53">
-        <v>100</v>
-      </c>
-      <c r="R47" s="53">
-        <v>0</v>
-      </c>
-      <c r="S47" s="53">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="48" spans="1:19" s="50" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A48" s="50">
-        <v>2023</v>
-      </c>
-      <c r="B48" s="50" t="s">
-        <v>197</v>
-      </c>
-      <c r="C48" s="50" t="s">
-        <v>18</v>
-      </c>
-      <c r="D48" s="50" t="s">
-        <v>7</v>
-      </c>
-      <c r="E48" s="50" t="s">
-        <v>199</v>
-      </c>
-      <c r="F48" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="G48" s="50" t="s">
-        <v>11</v>
-      </c>
-      <c r="H48" s="50" t="s">
-        <v>12</v>
-      </c>
-      <c r="I48" s="50" t="s">
-        <v>182</v>
-      </c>
-      <c r="J48" s="51" t="s">
-        <v>44</v>
-      </c>
-      <c r="K48" s="54" t="s">
-        <v>201</v>
-      </c>
-      <c r="L48" s="50">
-        <v>17.77</v>
-      </c>
-      <c r="M48" s="52" t="s">
-        <v>111</v>
-      </c>
-      <c r="N48" s="52" t="s">
-        <v>111</v>
-      </c>
-      <c r="O48" s="50">
-        <v>0.99</v>
-      </c>
-      <c r="P48" s="50">
-        <v>0.89</v>
-      </c>
-      <c r="Q48" s="53">
-        <v>90</v>
-      </c>
-      <c r="R48" s="53">
-        <v>0</v>
-      </c>
-      <c r="S48" s="53">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="49" spans="1:19" s="50" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="50">
-        <v>2023</v>
-      </c>
-      <c r="B49" s="50" t="s">
-        <v>198</v>
-      </c>
-      <c r="C49" s="50" t="s">
-        <v>18</v>
-      </c>
-      <c r="D49" s="50" t="s">
-        <v>7</v>
-      </c>
-      <c r="E49" s="50" t="s">
-        <v>200</v>
-      </c>
-      <c r="F49" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="G49" s="50" t="s">
-        <v>11</v>
-      </c>
-      <c r="H49" s="50" t="s">
-        <v>12</v>
-      </c>
-      <c r="I49" s="50" t="s">
-        <v>182</v>
-      </c>
-      <c r="J49" s="51" t="s">
-        <v>89</v>
-      </c>
-      <c r="K49" s="50" t="s">
-        <v>202</v>
-      </c>
-      <c r="L49" s="50">
-        <v>17.77</v>
-      </c>
-      <c r="M49" s="52" t="s">
-        <v>111</v>
-      </c>
-      <c r="N49" s="52" t="s">
-        <v>111</v>
-      </c>
-      <c r="O49" s="50">
-        <v>1.04</v>
-      </c>
-      <c r="P49" s="50">
-        <v>0.94</v>
-      </c>
-      <c r="Q49" s="53">
-        <v>90</v>
-      </c>
-      <c r="R49" s="53">
-        <v>0</v>
-      </c>
-      <c r="S49" s="53">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="50" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="28">
-        <v>2025</v>
-      </c>
-      <c r="B50" s="28" t="s">
-        <v>133</v>
-      </c>
-      <c r="C50" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="D50" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="E50" s="28" t="s">
-        <v>134</v>
-      </c>
-      <c r="H50" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="I50" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="J50" s="29" t="s">
+      <c r="I52" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="J52" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="M50" s="45"/>
-      <c r="N50" s="45"/>
-      <c r="Q50" s="30"/>
-      <c r="R50" s="30"/>
-      <c r="S50" s="30"/>
-    </row>
-    <row r="51" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="15">
-        <v>2035</v>
-      </c>
-      <c r="B51" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="C51" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="D51" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="E51" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="F51" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="G51" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="H51" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="I51" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="J51" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="K51" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="L51" s="15">
+      <c r="K52" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="L52" s="15">
         <v>15.85</v>
       </c>
-      <c r="M51" s="46">
+      <c r="M52" s="46">
         <v>-0.27</v>
       </c>
-      <c r="N51" s="46">
-        <v>0</v>
-      </c>
-      <c r="O51" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="P51" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q51" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="R51" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="S51" s="17" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="52" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="12">
-        <v>2035</v>
-      </c>
-      <c r="B52" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="C52" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D52" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="E52" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="F52" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G52" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H52" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I52" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="J52" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="K52" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="L52" s="12">
-        <v>15.85</v>
-      </c>
-      <c r="M52" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="N52" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="O52" s="14">
-        <v>1.27</v>
-      </c>
-      <c r="P52" s="14">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="Q52" s="14">
-        <v>120</v>
-      </c>
-      <c r="R52" s="14">
-        <v>0</v>
-      </c>
-      <c r="S52" s="14">
-        <v>45</v>
+      <c r="N52" s="46">
+        <v>0</v>
+      </c>
+      <c r="O52" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="P52" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q52" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="R52" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="S52" s="17" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="53" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -3925,7 +3920,7 @@
         <v>2035</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C53" s="12" t="s">
         <v>18</v>
@@ -3934,7 +3929,7 @@
         <v>103</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F53" s="12" t="s">
         <v>10</v>
@@ -3949,13 +3944,13 @@
         <v>105</v>
       </c>
       <c r="J53" s="13" t="s">
-        <v>110</v>
+        <v>44</v>
       </c>
       <c r="K53" s="12" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="L53" s="12">
-        <v>18.64</v>
+        <v>15.85</v>
       </c>
       <c r="M53" s="47" t="s">
         <v>111</v>
@@ -3984,7 +3979,7 @@
         <v>2035</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C54" s="12" t="s">
         <v>18</v>
@@ -3993,7 +3988,7 @@
         <v>103</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F54" s="12" t="s">
         <v>10</v>
@@ -4008,10 +4003,10 @@
         <v>105</v>
       </c>
       <c r="J54" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K54" s="12" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="L54" s="12">
         <v>18.64</v>
@@ -4029,13 +4024,13 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="Q54" s="14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="R54" s="14">
         <v>0</v>
       </c>
       <c r="S54" s="14">
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="55" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -4043,7 +4038,7 @@
         <v>2035</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="C55" s="12" t="s">
         <v>18</v>
@@ -4052,7 +4047,7 @@
         <v>103</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="F55" s="12" t="s">
         <v>10</v>
@@ -4067,10 +4062,10 @@
         <v>105</v>
       </c>
       <c r="J55" s="13" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="K55" s="12" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="L55" s="12">
         <v>18.64</v>
@@ -4081,20 +4076,20 @@
       <c r="N55" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="O55" s="12">
-        <v>0.95</v>
-      </c>
-      <c r="P55" s="12">
-        <v>0.86</v>
+      <c r="O55" s="14">
+        <v>1.27</v>
+      </c>
+      <c r="P55" s="14">
+        <v>1.1499999999999999</v>
       </c>
       <c r="Q55" s="14">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="R55" s="14">
         <v>0</v>
       </c>
       <c r="S55" s="14">
-        <v>45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -4102,7 +4097,7 @@
         <v>2035</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C56" s="12" t="s">
         <v>18</v>
@@ -4111,7 +4106,7 @@
         <v>103</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F56" s="12" t="s">
         <v>10</v>
@@ -4126,10 +4121,10 @@
         <v>105</v>
       </c>
       <c r="J56" s="13" t="s">
-        <v>43</v>
+        <v>110</v>
       </c>
       <c r="K56" s="12" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="L56" s="12">
         <v>18.64</v>
@@ -4147,13 +4142,13 @@
         <v>0.86</v>
       </c>
       <c r="Q56" s="14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="R56" s="14">
         <v>0</v>
       </c>
       <c r="S56" s="14">
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="57" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -4161,7 +4156,7 @@
         <v>2035</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>193</v>
+        <v>123</v>
       </c>
       <c r="C57" s="12" t="s">
         <v>18</v>
@@ -4170,7 +4165,7 @@
         <v>103</v>
       </c>
       <c r="E57" s="12" t="s">
-        <v>194</v>
+        <v>125</v>
       </c>
       <c r="F57" s="12" t="s">
         <v>10</v>
@@ -4185,10 +4180,10 @@
         <v>105</v>
       </c>
       <c r="J57" s="13" t="s">
-        <v>110</v>
+        <v>43</v>
       </c>
       <c r="K57" s="12" t="s">
-        <v>196</v>
+        <v>126</v>
       </c>
       <c r="L57" s="12">
         <v>18.64</v>
@@ -4215,59 +4210,118 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="24">
+    <row r="58" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B58" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E58" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="F58" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G58" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H58" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I58" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="J58" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="K58" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="L58" s="12">
+        <v>18.64</v>
+      </c>
+      <c r="M58" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="N58" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="O58" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="P58" s="12">
+        <v>0.86</v>
+      </c>
+      <c r="Q58" s="14">
+        <v>0</v>
+      </c>
+      <c r="R58" s="14">
+        <v>0</v>
+      </c>
+      <c r="S58" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="24">
         <v>2050</v>
       </c>
-      <c r="B58" s="24" t="s">
+      <c r="B59" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="C58" s="24" t="s">
+      <c r="C59" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="D58" s="24" t="s">
+      <c r="D59" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="E58" s="24" t="s">
+      <c r="E59" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="F58" s="24" t="s">
+      <c r="F59" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="G58" s="25" t="s">
+      <c r="G59" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="I58" s="24" t="s">
+      <c r="I59" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="J58" s="26" t="s">
+      <c r="J59" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="K58" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="L58" s="24">
+      <c r="K59" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="L59" s="24">
         <v>17.440000000000001</v>
       </c>
-      <c r="M58" s="48">
+      <c r="M59" s="48">
         <v>-0.33</v>
       </c>
-      <c r="N58" s="48">
-        <v>0</v>
-      </c>
-      <c r="O58" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="P58" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q58" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="R58" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="S58" s="27" t="s">
+      <c r="N59" s="48">
+        <v>0</v>
+      </c>
+      <c r="O59" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="P59" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q59" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="R59" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="S59" s="27" t="s">
         <v>111</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add v39 to the run log (lower Rail/ferry Hesitancy than v38)
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63848503-B520-4834-A9EC-CC1363653561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC1FC4E-02B5-46BC-B043-6FF2B970FDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="208">
   <si>
     <t>year</t>
   </si>
@@ -651,6 +651,15 @@
   </si>
   <si>
     <t>Higher tolls, WFH at ~30%</t>
+  </si>
+  <si>
+    <t>2023_TM160_IPA_39</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1205937699715122/f</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1205937699715120/f</t>
   </si>
 </sst>
 </file>
@@ -710,7 +719,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -765,6 +774,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -797,7 +812,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -907,6 +922,7 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1222,13 +1238,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9564CC59-3725-4FDA-8BF2-0F68CB1B6F5A}">
-  <dimension ref="A1:S59"/>
+  <dimension ref="A1:S60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C41" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="J34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A50" sqref="A50"/>
+      <selection pane="bottomRight" activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -3301,7 +3317,7 @@
       <c r="A42" s="1">
         <v>2023</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="51" t="s">
         <v>174</v>
       </c>
       <c r="C42" s="1" t="s">
@@ -3537,7 +3553,7 @@
       <c r="A46" s="1">
         <v>2023</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" s="51" t="s">
         <v>185</v>
       </c>
       <c r="C46" s="1" t="s">
@@ -3800,6 +3816,9 @@
       <c r="J50" s="10" t="s">
         <v>112</v>
       </c>
+      <c r="K50" s="1" t="s">
+        <v>207</v>
+      </c>
       <c r="L50" s="1">
         <v>17.77</v>
       </c>
@@ -3825,153 +3844,153 @@
         <v>80</v>
       </c>
     </row>
-    <row r="51" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="28">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A51" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="J51" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="L51" s="1">
+        <v>17.77</v>
+      </c>
+      <c r="M51" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="N51" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="O51" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="P51" s="1">
+        <v>0.89</v>
+      </c>
+      <c r="Q51" s="6">
+        <v>100</v>
+      </c>
+      <c r="R51" s="6">
+        <v>0</v>
+      </c>
+      <c r="S51" s="6">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="28">
         <v>2025</v>
       </c>
-      <c r="B51" s="28" t="s">
+      <c r="B52" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="C51" s="28" t="s">
+      <c r="C52" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="D51" s="28" t="s">
+      <c r="D52" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="E51" s="28" t="s">
+      <c r="E52" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="H51" s="28" t="s">
+      <c r="H52" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="I51" s="28" t="s">
+      <c r="I52" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="J51" s="29" t="s">
+      <c r="J52" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="M51" s="45"/>
-      <c r="N51" s="45"/>
-      <c r="Q51" s="30"/>
-      <c r="R51" s="30"/>
-      <c r="S51" s="30"/>
-    </row>
-    <row r="52" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="15">
+      <c r="M52" s="45"/>
+      <c r="N52" s="45"/>
+      <c r="Q52" s="30"/>
+      <c r="R52" s="30"/>
+      <c r="S52" s="30"/>
+    </row>
+    <row r="53" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="15">
         <v>2035</v>
       </c>
-      <c r="B52" s="15" t="s">
+      <c r="B53" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="C52" s="15" t="s">
+      <c r="C53" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="D52" s="15" t="s">
+      <c r="D53" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="E52" s="15" t="s">
+      <c r="E53" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="F52" s="15" t="s">
+      <c r="F53" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="G52" s="18" t="s">
+      <c r="G53" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="H52" s="15" t="s">
+      <c r="H53" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I52" s="15" t="s">
+      <c r="I53" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="J52" s="16" t="s">
+      <c r="J53" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="K52" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="L52" s="15">
+      <c r="K53" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="L53" s="15">
         <v>15.85</v>
       </c>
-      <c r="M52" s="46">
+      <c r="M53" s="46">
         <v>-0.27</v>
       </c>
-      <c r="N52" s="46">
-        <v>0</v>
-      </c>
-      <c r="O52" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="P52" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q52" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="R52" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="S52" s="17" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="53" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="12">
-        <v>2035</v>
-      </c>
-      <c r="B53" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="C53" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D53" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="E53" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="F53" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G53" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H53" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I53" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="J53" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="K53" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="L53" s="12">
-        <v>15.85</v>
-      </c>
-      <c r="M53" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="N53" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="O53" s="14">
-        <v>1.27</v>
-      </c>
-      <c r="P53" s="14">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="Q53" s="14">
-        <v>120</v>
-      </c>
-      <c r="R53" s="14">
-        <v>0</v>
-      </c>
-      <c r="S53" s="14">
-        <v>45</v>
+      <c r="N53" s="46">
+        <v>0</v>
+      </c>
+      <c r="O53" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="P53" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q53" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="R53" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="S53" s="17" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="54" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -3979,7 +3998,7 @@
         <v>2035</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C54" s="12" t="s">
         <v>18</v>
@@ -3988,7 +4007,7 @@
         <v>103</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F54" s="12" t="s">
         <v>10</v>
@@ -4003,13 +4022,13 @@
         <v>105</v>
       </c>
       <c r="J54" s="13" t="s">
-        <v>110</v>
+        <v>44</v>
       </c>
       <c r="K54" s="12" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="L54" s="12">
-        <v>18.64</v>
+        <v>15.85</v>
       </c>
       <c r="M54" s="47" t="s">
         <v>111</v>
@@ -4038,7 +4057,7 @@
         <v>2035</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C55" s="12" t="s">
         <v>18</v>
@@ -4047,7 +4066,7 @@
         <v>103</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F55" s="12" t="s">
         <v>10</v>
@@ -4062,10 +4081,10 @@
         <v>105</v>
       </c>
       <c r="J55" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K55" s="12" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="L55" s="12">
         <v>18.64</v>
@@ -4083,13 +4102,13 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="Q55" s="14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="R55" s="14">
         <v>0</v>
       </c>
       <c r="S55" s="14">
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="56" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -4097,7 +4116,7 @@
         <v>2035</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="C56" s="12" t="s">
         <v>18</v>
@@ -4106,7 +4125,7 @@
         <v>103</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="F56" s="12" t="s">
         <v>10</v>
@@ -4121,10 +4140,10 @@
         <v>105</v>
       </c>
       <c r="J56" s="13" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="K56" s="12" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="L56" s="12">
         <v>18.64</v>
@@ -4135,20 +4154,20 @@
       <c r="N56" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="O56" s="12">
-        <v>0.95</v>
-      </c>
-      <c r="P56" s="12">
-        <v>0.86</v>
+      <c r="O56" s="14">
+        <v>1.27</v>
+      </c>
+      <c r="P56" s="14">
+        <v>1.1499999999999999</v>
       </c>
       <c r="Q56" s="14">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="R56" s="14">
         <v>0</v>
       </c>
       <c r="S56" s="14">
-        <v>45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -4156,7 +4175,7 @@
         <v>2035</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C57" s="12" t="s">
         <v>18</v>
@@ -4165,7 +4184,7 @@
         <v>103</v>
       </c>
       <c r="E57" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F57" s="12" t="s">
         <v>10</v>
@@ -4180,10 +4199,10 @@
         <v>105</v>
       </c>
       <c r="J57" s="13" t="s">
-        <v>43</v>
+        <v>110</v>
       </c>
       <c r="K57" s="12" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="L57" s="12">
         <v>18.64</v>
@@ -4201,13 +4220,13 @@
         <v>0.86</v>
       </c>
       <c r="Q57" s="14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="R57" s="14">
         <v>0</v>
       </c>
       <c r="S57" s="14">
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="58" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -4215,7 +4234,7 @@
         <v>2035</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>188</v>
+        <v>123</v>
       </c>
       <c r="C58" s="12" t="s">
         <v>18</v>
@@ -4224,7 +4243,7 @@
         <v>103</v>
       </c>
       <c r="E58" s="12" t="s">
-        <v>189</v>
+        <v>125</v>
       </c>
       <c r="F58" s="12" t="s">
         <v>10</v>
@@ -4239,10 +4258,10 @@
         <v>105</v>
       </c>
       <c r="J58" s="13" t="s">
-        <v>110</v>
+        <v>43</v>
       </c>
       <c r="K58" s="12" t="s">
-        <v>191</v>
+        <v>126</v>
       </c>
       <c r="L58" s="12">
         <v>18.64</v>
@@ -4269,59 +4288,118 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="24">
+    <row r="59" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B59" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D59" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E59" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="F59" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G59" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H59" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I59" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="J59" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="K59" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="L59" s="12">
+        <v>18.64</v>
+      </c>
+      <c r="M59" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="N59" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="O59" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="P59" s="12">
+        <v>0.86</v>
+      </c>
+      <c r="Q59" s="14">
+        <v>0</v>
+      </c>
+      <c r="R59" s="14">
+        <v>0</v>
+      </c>
+      <c r="S59" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="24">
         <v>2050</v>
       </c>
-      <c r="B59" s="24" t="s">
+      <c r="B60" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="C59" s="24" t="s">
+      <c r="C60" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="D59" s="24" t="s">
+      <c r="D60" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="E59" s="24" t="s">
+      <c r="E60" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="F59" s="24" t="s">
+      <c r="F60" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="G59" s="25" t="s">
+      <c r="G60" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="I59" s="24" t="s">
+      <c r="I60" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="J59" s="26" t="s">
+      <c r="J60" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="K59" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="L59" s="24">
+      <c r="K60" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="L60" s="24">
         <v>17.440000000000001</v>
       </c>
-      <c r="M59" s="48">
+      <c r="M60" s="48">
         <v>-0.33</v>
       </c>
-      <c r="N59" s="48">
-        <v>0</v>
-      </c>
-      <c r="O59" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="P59" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q59" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="R59" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="S59" s="27" t="s">
+      <c r="N60" s="48">
+        <v>0</v>
+      </c>
+      <c r="O60" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="P60" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q60" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="R60" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="S60" s="27" t="s">
         <v>111</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added to the model run log 2023 v40, with AOC=16.46 cents
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC1FC4E-02B5-46BC-B043-6FF2B970FDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE7032E-FFC1-41A8-A837-8E27C0641118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="211">
   <si>
     <t>year</t>
   </si>
@@ -660,6 +660,15 @@
   </si>
   <si>
     <t>https://app.asana.com/0/1204085012544660/1205937699715120/f</t>
+  </si>
+  <si>
+    <t>2023_TM160_IPA_40</t>
+  </si>
+  <si>
+    <t>new AOC (16.46 cents)</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1205973396667333/f</t>
   </si>
 </sst>
 </file>
@@ -1238,13 +1247,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9564CC59-3725-4FDA-8BF2-0F68CB1B6F5A}">
-  <dimension ref="A1:S60"/>
+  <dimension ref="A1:S61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B46" sqref="B46"/>
+      <selection pane="bottomRight" activeCell="T52" sqref="T52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -3903,153 +3912,153 @@
         <v>75</v>
       </c>
     </row>
-    <row r="52" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="28">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A52" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="J52" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="L52" s="1">
+        <v>16.45</v>
+      </c>
+      <c r="M52" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="N52" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="O52" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="P52" s="1">
+        <v>0.89</v>
+      </c>
+      <c r="Q52" s="6">
+        <v>100</v>
+      </c>
+      <c r="R52" s="6">
+        <v>0</v>
+      </c>
+      <c r="S52" s="6">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="28">
         <v>2025</v>
       </c>
-      <c r="B52" s="28" t="s">
+      <c r="B53" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="C52" s="28" t="s">
+      <c r="C53" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="D52" s="28" t="s">
+      <c r="D53" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="E52" s="28" t="s">
+      <c r="E53" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="H52" s="28" t="s">
+      <c r="H53" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="I52" s="28" t="s">
+      <c r="I53" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="J52" s="29" t="s">
+      <c r="J53" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="M52" s="45"/>
-      <c r="N52" s="45"/>
-      <c r="Q52" s="30"/>
-      <c r="R52" s="30"/>
-      <c r="S52" s="30"/>
-    </row>
-    <row r="53" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="15">
+      <c r="M53" s="45"/>
+      <c r="N53" s="45"/>
+      <c r="Q53" s="30"/>
+      <c r="R53" s="30"/>
+      <c r="S53" s="30"/>
+    </row>
+    <row r="54" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="15">
         <v>2035</v>
       </c>
-      <c r="B53" s="15" t="s">
+      <c r="B54" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="C53" s="15" t="s">
+      <c r="C54" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="D53" s="15" t="s">
+      <c r="D54" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="E53" s="15" t="s">
+      <c r="E54" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="F53" s="15" t="s">
+      <c r="F54" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="G53" s="18" t="s">
+      <c r="G54" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="H53" s="15" t="s">
+      <c r="H54" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="15" t="s">
+      <c r="I54" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="J53" s="16" t="s">
+      <c r="J54" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="K53" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="L53" s="15">
+      <c r="K54" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="L54" s="15">
         <v>15.85</v>
       </c>
-      <c r="M53" s="46">
+      <c r="M54" s="46">
         <v>-0.27</v>
       </c>
-      <c r="N53" s="46">
-        <v>0</v>
-      </c>
-      <c r="O53" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="P53" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q53" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="R53" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="S53" s="17" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="54" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="12">
-        <v>2035</v>
-      </c>
-      <c r="B54" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="C54" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D54" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="E54" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="F54" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G54" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H54" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I54" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="J54" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="K54" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="L54" s="12">
-        <v>15.85</v>
-      </c>
-      <c r="M54" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="N54" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="O54" s="14">
-        <v>1.27</v>
-      </c>
-      <c r="P54" s="14">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="Q54" s="14">
-        <v>120</v>
-      </c>
-      <c r="R54" s="14">
-        <v>0</v>
-      </c>
-      <c r="S54" s="14">
-        <v>45</v>
+      <c r="N54" s="46">
+        <v>0</v>
+      </c>
+      <c r="O54" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="P54" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q54" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="R54" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="S54" s="17" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="55" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -4057,7 +4066,7 @@
         <v>2035</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C55" s="12" t="s">
         <v>18</v>
@@ -4066,7 +4075,7 @@
         <v>103</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F55" s="12" t="s">
         <v>10</v>
@@ -4081,13 +4090,13 @@
         <v>105</v>
       </c>
       <c r="J55" s="13" t="s">
-        <v>110</v>
+        <v>44</v>
       </c>
       <c r="K55" s="12" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="L55" s="12">
-        <v>18.64</v>
+        <v>15.85</v>
       </c>
       <c r="M55" s="47" t="s">
         <v>111</v>
@@ -4116,7 +4125,7 @@
         <v>2035</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C56" s="12" t="s">
         <v>18</v>
@@ -4125,7 +4134,7 @@
         <v>103</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F56" s="12" t="s">
         <v>10</v>
@@ -4140,10 +4149,10 @@
         <v>105</v>
       </c>
       <c r="J56" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K56" s="12" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="L56" s="12">
         <v>18.64</v>
@@ -4161,13 +4170,13 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="Q56" s="14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="R56" s="14">
         <v>0</v>
       </c>
       <c r="S56" s="14">
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="57" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -4175,7 +4184,7 @@
         <v>2035</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="C57" s="12" t="s">
         <v>18</v>
@@ -4184,7 +4193,7 @@
         <v>103</v>
       </c>
       <c r="E57" s="12" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="F57" s="12" t="s">
         <v>10</v>
@@ -4199,10 +4208,10 @@
         <v>105</v>
       </c>
       <c r="J57" s="13" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="K57" s="12" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="L57" s="12">
         <v>18.64</v>
@@ -4213,20 +4222,20 @@
       <c r="N57" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="O57" s="12">
-        <v>0.95</v>
-      </c>
-      <c r="P57" s="12">
-        <v>0.86</v>
+      <c r="O57" s="14">
+        <v>1.27</v>
+      </c>
+      <c r="P57" s="14">
+        <v>1.1499999999999999</v>
       </c>
       <c r="Q57" s="14">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="R57" s="14">
         <v>0</v>
       </c>
       <c r="S57" s="14">
-        <v>45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -4234,7 +4243,7 @@
         <v>2035</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C58" s="12" t="s">
         <v>18</v>
@@ -4243,7 +4252,7 @@
         <v>103</v>
       </c>
       <c r="E58" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F58" s="12" t="s">
         <v>10</v>
@@ -4258,10 +4267,10 @@
         <v>105</v>
       </c>
       <c r="J58" s="13" t="s">
-        <v>43</v>
+        <v>110</v>
       </c>
       <c r="K58" s="12" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="L58" s="12">
         <v>18.64</v>
@@ -4279,13 +4288,13 @@
         <v>0.86</v>
       </c>
       <c r="Q58" s="14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="R58" s="14">
         <v>0</v>
       </c>
       <c r="S58" s="14">
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="59" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -4293,7 +4302,7 @@
         <v>2035</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>188</v>
+        <v>123</v>
       </c>
       <c r="C59" s="12" t="s">
         <v>18</v>
@@ -4302,7 +4311,7 @@
         <v>103</v>
       </c>
       <c r="E59" s="12" t="s">
-        <v>189</v>
+        <v>125</v>
       </c>
       <c r="F59" s="12" t="s">
         <v>10</v>
@@ -4317,10 +4326,10 @@
         <v>105</v>
       </c>
       <c r="J59" s="13" t="s">
-        <v>110</v>
+        <v>43</v>
       </c>
       <c r="K59" s="12" t="s">
-        <v>191</v>
+        <v>126</v>
       </c>
       <c r="L59" s="12">
         <v>18.64</v>
@@ -4347,59 +4356,118 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="24">
+    <row r="60" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B60" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="C60" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D60" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E60" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="F60" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G60" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H60" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I60" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="J60" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="K60" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="L60" s="12">
+        <v>18.64</v>
+      </c>
+      <c r="M60" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="N60" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="O60" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="P60" s="12">
+        <v>0.86</v>
+      </c>
+      <c r="Q60" s="14">
+        <v>0</v>
+      </c>
+      <c r="R60" s="14">
+        <v>0</v>
+      </c>
+      <c r="S60" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="24">
         <v>2050</v>
       </c>
-      <c r="B60" s="24" t="s">
+      <c r="B61" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="C60" s="24" t="s">
+      <c r="C61" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="D60" s="24" t="s">
+      <c r="D61" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="E60" s="24" t="s">
+      <c r="E61" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="F60" s="24" t="s">
+      <c r="F61" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="G60" s="25" t="s">
+      <c r="G61" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="I60" s="24" t="s">
+      <c r="I61" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="J60" s="26" t="s">
+      <c r="J61" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="K60" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="L60" s="24">
+      <c r="K61" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="L61" s="24">
         <v>17.440000000000001</v>
       </c>
-      <c r="M60" s="48">
+      <c r="M61" s="48">
         <v>-0.33</v>
       </c>
-      <c r="N60" s="48">
-        <v>0</v>
-      </c>
-      <c r="O60" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="P60" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q60" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="R60" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="S60" s="27" t="s">
+      <c r="N61" s="48">
+        <v>0</v>
+      </c>
+      <c r="O61" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="P61" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q61" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="R61" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="S61" s="27" t="s">
         <v>111</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added 2015_TM160_IPA_03_AOCplus10pct, 2035_TM160_IPA_06_EN7test, 2035_TM160_IPA_07
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE7032E-FFC1-41A8-A837-8E27C0641118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F143BB5-3C87-4DEF-B653-7A920D098DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
+    <workbookView xWindow="9900" yWindow="2340" windowWidth="24465" windowHeight="11640" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelRuns" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="220">
   <si>
     <t>year</t>
   </si>
@@ -605,9 +605,6 @@
     <t>2035_TM160_IPA_06</t>
   </si>
   <si>
-    <t>same as v05 except for nonres</t>
-  </si>
-  <si>
     <t>https://app.asana.com/0/1204085012544660/1205911053939954/f</t>
   </si>
   <si>
@@ -669,6 +666,36 @@
   </si>
   <si>
     <t>https://app.asana.com/0/1204085012544660/1205973396667333/f</t>
+  </si>
+  <si>
+    <t>2035_TM160_IPA_07</t>
+  </si>
+  <si>
+    <t>2035_TM160_IPA_06_EN7test</t>
+  </si>
+  <si>
+    <t>Best guess at IPA assumptions</t>
+  </si>
+  <si>
+    <t>Same as v05 except for nonres</t>
+  </si>
+  <si>
+    <t>Same as v06 but with EN7</t>
+  </si>
+  <si>
+    <t>FBP scaled to RGF</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1205943552385938/f</t>
+  </si>
+  <si>
+    <t>2015_TM160_IPA_03_AOCplus10pct</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1205973396667340/f</t>
+  </si>
+  <si>
+    <t>Same as 2015_TM160_IPA_03</t>
   </si>
 </sst>
 </file>
@@ -678,7 +705,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -718,14 +745,6 @@
       <color rgb="FFFF0000"/>
       <name val="Consolas"/>
       <family val="3"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="11">
@@ -817,11 +836,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -930,11 +948,11 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1247,34 +1265,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9564CC59-3725-4FDA-8BF2-0F68CB1B6F5A}">
-  <dimension ref="A1:S61"/>
+  <dimension ref="A1:S64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T52" sqref="T52"/>
+      <selection pane="bottomRight" activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.81640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.81640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="42.26953125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.1796875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="6.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.1796875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.26953125" style="10" customWidth="1"/>
-    <col min="11" max="11" width="17.54296875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="5.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="9.1796875" style="44"/>
-    <col min="15" max="16384" width="9.1796875" style="1"/>
+    <col min="2" max="2" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="42.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" style="10" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="6.28515625" style="1" customWidth="1"/>
+    <col min="13" max="14" width="9.140625" style="44"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="5" customFormat="1" ht="52" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1333,7 +1351,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="19">
         <v>2005</v>
       </c>
@@ -1362,7 +1380,7 @@
       <c r="Q2" s="23"/>
       <c r="R2" s="23"/>
     </row>
-    <row r="3" spans="1:19" s="32" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="31">
         <v>2005</v>
       </c>
@@ -1415,7 +1433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="35">
         <v>2015</v>
       </c>
@@ -1464,7 +1482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="35">
         <v>2015</v>
       </c>
@@ -1520,7 +1538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="35">
         <v>2015</v>
       </c>
@@ -1573,7 +1591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="35">
         <v>2015</v>
       </c>
@@ -1626,7 +1644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="35">
         <v>2015</v>
       </c>
@@ -1660,13 +1678,16 @@
       <c r="K8" s="36" t="s">
         <v>162</v>
       </c>
+      <c r="L8" s="52">
+        <v>15.1</v>
+      </c>
       <c r="M8" s="42" t="s">
         <v>111</v>
       </c>
       <c r="N8" s="42" t="s">
         <v>111</v>
       </c>
-      <c r="O8" s="49">
+      <c r="O8" s="38">
         <v>0.32300000000000001</v>
       </c>
       <c r="P8" s="49">
@@ -1682,58 +1703,71 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>2023</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J9" s="9" t="s">
+    <row r="9" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="35">
+        <v>2015</v>
+      </c>
+      <c r="B9" s="36" t="s">
+        <v>217</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="36" t="s">
+        <v>219</v>
+      </c>
+      <c r="F9" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="J9" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="K9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M9" s="43">
-        <v>-0.44</v>
-      </c>
-      <c r="N9" s="43">
-        <v>-0.23</v>
-      </c>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6">
-        <v>0</v>
-      </c>
-      <c r="R9" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="K9" s="36" t="s">
+        <v>218</v>
+      </c>
+      <c r="L9" s="36">
+        <v>13.73</v>
+      </c>
+      <c r="M9" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="N9" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="O9" s="38">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="P9" s="49">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="Q9" s="38">
+        <v>0</v>
+      </c>
+      <c r="R9" s="38">
+        <v>0</v>
+      </c>
+      <c r="S9" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>2023</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>18</v>
@@ -1742,7 +1776,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>10</v>
@@ -1757,29 +1791,29 @@
         <v>17</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M10" s="43">
-        <v>-1.25</v>
+        <v>-0.44</v>
       </c>
       <c r="N10" s="43">
-        <v>-0.75</v>
+        <v>-0.23</v>
       </c>
       <c r="O10" s="6"/>
       <c r="P10" s="6"/>
       <c r="Q10" s="6">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="R10" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>2023</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>18</v>
@@ -1788,7 +1822,7 @@
         <v>7</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>10</v>
@@ -1797,13 +1831,13 @@
         <v>11</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="J11" s="9" t="s">
         <v>17</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="M11" s="43">
         <v>-1.25</v>
@@ -1814,18 +1848,18 @@
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
       <c r="Q11" s="6">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="R11" s="6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>2023</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>18</v>
@@ -1834,7 +1868,7 @@
         <v>7</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>10</v>
@@ -1843,13 +1877,13 @@
         <v>11</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J12" s="9" t="s">
         <v>17</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M12" s="43">
         <v>-1.25</v>
@@ -1860,18 +1894,18 @@
       <c r="O12" s="6"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="6">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="R12" s="6">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>2023</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>18</v>
@@ -1880,7 +1914,7 @@
         <v>7</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>10</v>
@@ -1895,7 +1929,7 @@
         <v>17</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="M13" s="43">
         <v>-1.25</v>
@@ -1905,19 +1939,19 @@
       </c>
       <c r="O13" s="6"/>
       <c r="P13" s="6"/>
-      <c r="Q13" s="11">
+      <c r="Q13" s="6">
         <v>75</v>
       </c>
-      <c r="R13" s="11">
+      <c r="R13" s="6">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>2023</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>18</v>
@@ -1926,7 +1960,7 @@
         <v>7</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>10</v>
@@ -1938,10 +1972,10 @@
         <v>33</v>
       </c>
       <c r="J14" s="9" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="M14" s="43">
         <v>-1.25</v>
@@ -1951,19 +1985,19 @@
       </c>
       <c r="O14" s="6"/>
       <c r="P14" s="6"/>
-      <c r="Q14" s="7">
-        <v>85</v>
-      </c>
-      <c r="R14" s="7">
+      <c r="Q14" s="11">
+        <v>75</v>
+      </c>
+      <c r="R14" s="11">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>2023</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>18</v>
@@ -1984,7 +2018,7 @@
         <v>33</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>46</v>
@@ -1998,18 +2032,18 @@
       <c r="O15" s="6"/>
       <c r="P15" s="6"/>
       <c r="Q15" s="7">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="R15" s="7">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>2023</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>18</v>
@@ -2030,7 +2064,7 @@
         <v>33</v>
       </c>
       <c r="J16" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>46</v>
@@ -2044,18 +2078,18 @@
       <c r="O16" s="6"/>
       <c r="P16" s="6"/>
       <c r="Q16" s="7">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="R16" s="7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>2023</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>18</v>
@@ -2064,7 +2098,7 @@
         <v>7</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>10</v>
@@ -2073,13 +2107,13 @@
         <v>11</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J17" s="10" t="s">
-        <v>43</v>
+        <v>33</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>45</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="M17" s="43">
         <v>-1.25</v>
@@ -2096,12 +2130,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>2023</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>18</v>
@@ -2110,7 +2144,7 @@
         <v>7</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>10</v>
@@ -2119,13 +2153,13 @@
         <v>11</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="J18" s="10" t="s">
         <v>43</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="M18" s="43">
         <v>-1.25</v>
@@ -2136,18 +2170,18 @@
       <c r="O18" s="6"/>
       <c r="P18" s="6"/>
       <c r="Q18" s="7">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="R18" s="7">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>2023</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>18</v>
@@ -2156,7 +2190,7 @@
         <v>7</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>10</v>
@@ -2168,7 +2202,7 @@
         <v>54</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>57</v>
@@ -2182,18 +2216,18 @@
       <c r="O19" s="6"/>
       <c r="P19" s="6"/>
       <c r="Q19" s="7">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="R19" s="7">
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>2023</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>18</v>
@@ -2202,7 +2236,7 @@
         <v>7</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>10</v>
@@ -2211,13 +2245,13 @@
         <v>11</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="M20" s="43">
         <v>-1.25</v>
@@ -2228,18 +2262,18 @@
       <c r="O20" s="6"/>
       <c r="P20" s="6"/>
       <c r="Q20" s="7">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="R20" s="7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>2023</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>18</v>
@@ -2248,7 +2282,7 @@
         <v>7</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>10</v>
@@ -2263,7 +2297,7 @@
         <v>43</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="M21" s="43">
         <v>-1.25</v>
@@ -2274,18 +2308,18 @@
       <c r="O21" s="6"/>
       <c r="P21" s="6"/>
       <c r="Q21" s="7">
-        <v>300</v>
+        <v>180</v>
       </c>
       <c r="R21" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>2023</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>18</v>
@@ -2320,18 +2354,18 @@
       <c r="O22" s="6"/>
       <c r="P22" s="6"/>
       <c r="Q22" s="7">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="R22" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>2023</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>18</v>
@@ -2366,18 +2400,18 @@
       <c r="O23" s="6"/>
       <c r="P23" s="6"/>
       <c r="Q23" s="7">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="R23" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>2023</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>18</v>
@@ -2386,7 +2420,7 @@
         <v>7</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>10</v>
@@ -2395,13 +2429,13 @@
         <v>11</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="J24" s="10" t="s">
         <v>43</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M24" s="43">
         <v>-1.25</v>
@@ -2412,18 +2446,18 @@
       <c r="O24" s="6"/>
       <c r="P24" s="6"/>
       <c r="Q24" s="7">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="R24" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>2023</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>18</v>
@@ -2432,7 +2466,7 @@
         <v>7</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>10</v>
@@ -2441,13 +2475,13 @@
         <v>11</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="J25" s="10" t="s">
         <v>43</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="M25" s="43">
         <v>-1.25</v>
@@ -2464,12 +2498,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>2023</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>18</v>
@@ -2478,7 +2512,7 @@
         <v>7</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>10</v>
@@ -2487,13 +2521,13 @@
         <v>11</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="J26" s="10" t="s">
         <v>43</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="M26" s="43">
         <v>-1.25</v>
@@ -2510,12 +2544,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>2023</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>18</v>
@@ -2524,7 +2558,7 @@
         <v>7</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>10</v>
@@ -2536,17 +2570,19 @@
         <v>80</v>
       </c>
       <c r="J27" s="10" t="s">
-        <v>89</v>
+        <v>43</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="O27" s="6">
-        <v>1.27</v>
-      </c>
-      <c r="P27" s="6">
-        <v>1.1499999999999999</v>
-      </c>
+      <c r="M27" s="43">
+        <v>-1.25</v>
+      </c>
+      <c r="N27" s="43">
+        <v>-0.75</v>
+      </c>
+      <c r="O27" s="6"/>
+      <c r="P27" s="6"/>
       <c r="Q27" s="7">
         <v>120</v>
       </c>
@@ -2554,12 +2590,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>2023</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>18</v>
@@ -2568,7 +2604,7 @@
         <v>7</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>10</v>
@@ -2580,35 +2616,30 @@
         <v>80</v>
       </c>
       <c r="J28" s="10" t="s">
-        <v>43</v>
+        <v>89</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="M28" s="43">
-        <v>-1.25</v>
-      </c>
-      <c r="N28" s="43">
-        <v>-0.75</v>
-      </c>
-      <c r="O28" s="6"/>
-      <c r="P28" s="6"/>
+        <v>82</v>
+      </c>
+      <c r="O28" s="6">
+        <v>1.27</v>
+      </c>
+      <c r="P28" s="6">
+        <v>1.1499999999999999</v>
+      </c>
       <c r="Q28" s="7">
         <v>120</v>
       </c>
       <c r="R28" s="7">
         <v>0</v>
       </c>
-      <c r="S28" s="7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>2023</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>18</v>
@@ -2629,17 +2660,19 @@
         <v>80</v>
       </c>
       <c r="J29" s="10" t="s">
-        <v>89</v>
+        <v>43</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="O29" s="6">
-        <v>1.27</v>
-      </c>
-      <c r="P29" s="6">
-        <v>1.1499999999999999</v>
-      </c>
+      <c r="M29" s="43">
+        <v>-1.25</v>
+      </c>
+      <c r="N29" s="43">
+        <v>-0.75</v>
+      </c>
+      <c r="O29" s="6"/>
+      <c r="P29" s="6"/>
       <c r="Q29" s="7">
         <v>120</v>
       </c>
@@ -2650,12 +2683,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>2023</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>18</v>
@@ -2664,31 +2697,28 @@
         <v>7</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>80</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>43</v>
+        <v>89</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="M30" s="43">
-        <v>-1.25</v>
-      </c>
-      <c r="N30" s="43">
-        <v>-0.75</v>
+        <v>90</v>
+      </c>
+      <c r="O30" s="6">
+        <v>1.27</v>
+      </c>
+      <c r="P30" s="6">
+        <v>1.1499999999999999</v>
       </c>
       <c r="Q30" s="7">
         <v>120</v>
@@ -2697,15 +2727,15 @@
         <v>0</v>
       </c>
       <c r="S30" s="7">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>2023</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>18</v>
@@ -2729,25 +2759,16 @@
         <v>80</v>
       </c>
       <c r="J31" s="10" t="s">
-        <v>89</v>
+        <v>43</v>
       </c>
       <c r="K31" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="L31" s="1">
-        <v>17.77</v>
-      </c>
-      <c r="M31" s="44" t="s">
-        <v>111</v>
-      </c>
-      <c r="N31" s="44" t="s">
-        <v>111</v>
-      </c>
-      <c r="O31" s="6">
-        <v>1.27</v>
-      </c>
-      <c r="P31" s="6">
-        <v>1.1499999999999999</v>
+      <c r="M31" s="43">
+        <v>-1.25</v>
+      </c>
+      <c r="N31" s="43">
+        <v>-0.75</v>
       </c>
       <c r="Q31" s="7">
         <v>120</v>
@@ -2759,12 +2780,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>2023</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>18</v>
@@ -2773,22 +2794,25 @@
         <v>7</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>80</v>
       </c>
       <c r="J32" s="10" t="s">
-        <v>43</v>
+        <v>89</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="L32" s="1">
         <v>17.77</v>
@@ -2799,11 +2823,11 @@
       <c r="N32" s="44" t="s">
         <v>111</v>
       </c>
-      <c r="O32" s="1">
-        <v>0.64</v>
-      </c>
-      <c r="P32" s="1">
-        <v>0.57999999999999996</v>
+      <c r="O32" s="6">
+        <v>1.27</v>
+      </c>
+      <c r="P32" s="6">
+        <v>1.1499999999999999</v>
       </c>
       <c r="Q32" s="7">
         <v>120</v>
@@ -2815,12 +2839,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>2023</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>18</v>
@@ -2829,25 +2853,22 @@
         <v>7</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>156</v>
+        <v>97</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>80</v>
       </c>
       <c r="J33" s="10" t="s">
-        <v>89</v>
+        <v>43</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L33" s="1">
         <v>17.77</v>
@@ -2859,27 +2880,27 @@
         <v>111</v>
       </c>
       <c r="O33" s="1">
-        <v>0.95</v>
+        <v>0.64</v>
       </c>
       <c r="P33" s="1">
-        <v>0.86</v>
-      </c>
-      <c r="Q33" s="6">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="Q33" s="7">
         <v>120</v>
       </c>
-      <c r="R33" s="6">
-        <v>0</v>
-      </c>
-      <c r="S33" s="6">
+      <c r="R33" s="7">
+        <v>0</v>
+      </c>
+      <c r="S33" s="7">
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>2023</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>141</v>
+        <v>96</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>18</v>
@@ -2888,22 +2909,25 @@
         <v>7</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>80</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>44</v>
+        <v>89</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>139</v>
+        <v>99</v>
       </c>
       <c r="L34" s="1">
         <v>17.77</v>
@@ -2921,21 +2945,21 @@
         <v>0.86</v>
       </c>
       <c r="Q34" s="6">
-        <v>200</v>
+        <v>120</v>
       </c>
       <c r="R34" s="6">
         <v>0</v>
       </c>
       <c r="S34" s="6">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>2023</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>18</v>
@@ -2944,7 +2968,7 @@
         <v>7</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>10</v>
@@ -2956,10 +2980,10 @@
         <v>80</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="L35" s="1">
         <v>17.77</v>
@@ -2977,7 +3001,7 @@
         <v>0.86</v>
       </c>
       <c r="Q35" s="6">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="R35" s="6">
         <v>0</v>
@@ -2986,12 +3010,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>2023</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>18</v>
@@ -3000,7 +3024,7 @@
         <v>7</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>10</v>
@@ -3012,10 +3036,10 @@
         <v>80</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>132</v>
+        <v>89</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="L36" s="1">
         <v>17.77</v>
@@ -3027,10 +3051,10 @@
         <v>111</v>
       </c>
       <c r="O36" s="1">
-        <v>0.39</v>
+        <v>0.95</v>
       </c>
       <c r="P36" s="1">
-        <v>0.35</v>
+        <v>0.86</v>
       </c>
       <c r="Q36" s="6">
         <v>300</v>
@@ -3042,12 +3066,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>2023</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>18</v>
@@ -3056,7 +3080,7 @@
         <v>7</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>10</v>
@@ -3068,10 +3092,10 @@
         <v>80</v>
       </c>
       <c r="J37" s="10" t="s">
-        <v>44</v>
+        <v>132</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="L37" s="1">
         <v>17.77</v>
@@ -3083,27 +3107,27 @@
         <v>111</v>
       </c>
       <c r="O37" s="1">
-        <v>0.77</v>
+        <v>0.39</v>
       </c>
       <c r="P37" s="1">
-        <v>0.69</v>
+        <v>0.35</v>
       </c>
       <c r="Q37" s="6">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="R37" s="6">
         <v>0</v>
       </c>
       <c r="S37" s="6">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>2023</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>18</v>
@@ -3112,7 +3136,7 @@
         <v>7</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>10</v>
@@ -3124,10 +3148,10 @@
         <v>80</v>
       </c>
       <c r="J38" s="10" t="s">
-        <v>132</v>
+        <v>44</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="L38" s="1">
         <v>17.77</v>
@@ -3139,27 +3163,27 @@
         <v>111</v>
       </c>
       <c r="O38" s="1">
-        <v>0.94</v>
+        <v>0.77</v>
       </c>
       <c r="P38" s="1">
-        <v>0.85499999999999998</v>
+        <v>0.69</v>
       </c>
       <c r="Q38" s="6">
-        <v>120</v>
+        <v>400</v>
       </c>
       <c r="R38" s="6">
         <v>0</v>
       </c>
       <c r="S38" s="6">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>2023</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>18</v>
@@ -3168,7 +3192,7 @@
         <v>7</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>10</v>
@@ -3177,7 +3201,7 @@
         <v>11</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>167</v>
+        <v>80</v>
       </c>
       <c r="J39" s="10" t="s">
         <v>132</v>
@@ -3210,12 +3234,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>2023</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>18</v>
@@ -3224,7 +3248,7 @@
         <v>7</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>10</v>
@@ -3266,12 +3290,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>2023</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>18</v>
@@ -3280,7 +3304,7 @@
         <v>7</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>10</v>
@@ -3292,10 +3316,10 @@
         <v>167</v>
       </c>
       <c r="J41" s="10" t="s">
-        <v>17</v>
+        <v>132</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="L41" s="1">
         <v>17.77</v>
@@ -3322,12 +3346,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>2023</v>
       </c>
-      <c r="B42" s="51" t="s">
-        <v>174</v>
+      <c r="B42" s="1" t="s">
+        <v>171</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>18</v>
@@ -3336,7 +3360,7 @@
         <v>7</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>10</v>
@@ -3344,17 +3368,14 @@
       <c r="G42" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H42" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="I42" s="1" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="J42" s="10" t="s">
         <v>17</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="L42" s="1">
         <v>17.77</v>
@@ -3381,12 +3402,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>2023</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>178</v>
+      <c r="B43" s="50" t="s">
+        <v>174</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>18</v>
@@ -3395,7 +3416,7 @@
         <v>7</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>204</v>
+        <v>175</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>10</v>
@@ -3413,7 +3434,7 @@
         <v>17</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="L43" s="1">
         <v>17.77</v>
@@ -3425,10 +3446,10 @@
         <v>111</v>
       </c>
       <c r="O43" s="1">
-        <v>0.99</v>
+        <v>0.94</v>
       </c>
       <c r="P43" s="1">
-        <v>0.89</v>
+        <v>0.85499999999999998</v>
       </c>
       <c r="Q43" s="6">
         <v>120</v>
@@ -3440,12 +3461,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>2023</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>18</v>
@@ -3466,13 +3487,13 @@
         <v>12</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="J44" s="10" t="s">
         <v>17</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="L44" s="1">
         <v>17.77</v>
@@ -3499,12 +3520,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>2023</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>18</v>
@@ -3528,10 +3549,10 @@
         <v>181</v>
       </c>
       <c r="J45" s="10" t="s">
-        <v>112</v>
+        <v>17</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L45" s="1">
         <v>17.77</v>
@@ -3543,10 +3564,10 @@
         <v>111</v>
       </c>
       <c r="O45" s="1">
-        <v>1.04</v>
+        <v>0.99</v>
       </c>
       <c r="P45" s="1">
-        <v>0.94</v>
+        <v>0.89</v>
       </c>
       <c r="Q45" s="6">
         <v>120</v>
@@ -3558,12 +3579,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>2023</v>
       </c>
-      <c r="B46" s="51" t="s">
-        <v>185</v>
+      <c r="B46" s="1" t="s">
+        <v>184</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>18</v>
@@ -3587,10 +3608,10 @@
         <v>181</v>
       </c>
       <c r="J46" s="10" t="s">
-        <v>45</v>
+        <v>112</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="L46" s="1">
         <v>17.77</v>
@@ -3602,27 +3623,27 @@
         <v>111</v>
       </c>
       <c r="O46" s="1">
-        <v>0.99</v>
+        <v>1.04</v>
       </c>
       <c r="P46" s="1">
-        <v>0.89</v>
+        <v>0.94</v>
       </c>
       <c r="Q46" s="6">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="R46" s="6">
         <v>0</v>
       </c>
       <c r="S46" s="6">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>2023</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>187</v>
+      <c r="B47" s="50" t="s">
+        <v>185</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>18</v>
@@ -3646,10 +3667,10 @@
         <v>181</v>
       </c>
       <c r="J47" s="10" t="s">
-        <v>132</v>
+        <v>45</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="L47" s="1">
         <v>17.77</v>
@@ -3661,10 +3682,10 @@
         <v>111</v>
       </c>
       <c r="O47" s="1">
-        <v>1.04</v>
+        <v>0.99</v>
       </c>
       <c r="P47" s="1">
-        <v>0.94</v>
+        <v>0.89</v>
       </c>
       <c r="Q47" s="6">
         <v>100</v>
@@ -3676,12 +3697,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>2023</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>18</v>
@@ -3705,10 +3726,10 @@
         <v>181</v>
       </c>
       <c r="J48" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="K48" s="50" t="s">
-        <v>194</v>
+        <v>132</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>189</v>
       </c>
       <c r="L48" s="1">
         <v>17.77</v>
@@ -3720,27 +3741,27 @@
         <v>111</v>
       </c>
       <c r="O48" s="1">
-        <v>0.99</v>
+        <v>1.04</v>
       </c>
       <c r="P48" s="1">
-        <v>0.89</v>
+        <v>0.94</v>
       </c>
       <c r="Q48" s="6">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="R48" s="6">
         <v>0</v>
       </c>
       <c r="S48" s="6">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>2023</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>18</v>
@@ -3764,10 +3785,10 @@
         <v>181</v>
       </c>
       <c r="J49" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="K49" s="1" t="s">
-        <v>195</v>
+        <v>44</v>
+      </c>
+      <c r="K49" s="51" t="s">
+        <v>193</v>
       </c>
       <c r="L49" s="1">
         <v>17.77</v>
@@ -3779,10 +3800,10 @@
         <v>111</v>
       </c>
       <c r="O49" s="1">
-        <v>1.04</v>
+        <v>0.99</v>
       </c>
       <c r="P49" s="1">
-        <v>0.94</v>
+        <v>0.89</v>
       </c>
       <c r="Q49" s="6">
         <v>90</v>
@@ -3794,12 +3815,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>2023</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>18</v>
@@ -3823,10 +3844,10 @@
         <v>181</v>
       </c>
       <c r="J50" s="10" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="L50" s="1">
         <v>17.77</v>
@@ -3838,27 +3859,27 @@
         <v>111</v>
       </c>
       <c r="O50" s="1">
-        <v>0.99</v>
+        <v>1.04</v>
       </c>
       <c r="P50" s="1">
-        <v>0.89</v>
+        <v>0.94</v>
       </c>
       <c r="Q50" s="6">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="R50" s="6">
         <v>0</v>
       </c>
       <c r="S50" s="6">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>2023</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>18</v>
@@ -3867,7 +3888,7 @@
         <v>7</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>10</v>
@@ -3909,15 +3930,15 @@
         <v>0</v>
       </c>
       <c r="S51" s="6">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>2023</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>18</v>
@@ -3926,7 +3947,7 @@
         <v>7</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>10</v>
@@ -3941,13 +3962,13 @@
         <v>181</v>
       </c>
       <c r="J52" s="10" t="s">
-        <v>44</v>
+        <v>112</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="L52" s="1">
-        <v>16.45</v>
+        <v>17.77</v>
       </c>
       <c r="M52" s="44" t="s">
         <v>111</v>
@@ -3971,161 +3992,161 @@
         <v>75</v>
       </c>
     </row>
-    <row r="53" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="28">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="J53" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="L53" s="1">
+        <v>16.45</v>
+      </c>
+      <c r="M53" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="N53" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="O53" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="P53" s="1">
+        <v>0.89</v>
+      </c>
+      <c r="Q53" s="6">
+        <v>100</v>
+      </c>
+      <c r="R53" s="6">
+        <v>0</v>
+      </c>
+      <c r="S53" s="6">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="28">
         <v>2025</v>
       </c>
-      <c r="B53" s="28" t="s">
+      <c r="B54" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="C53" s="28" t="s">
+      <c r="C54" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="D53" s="28" t="s">
+      <c r="D54" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="E53" s="28" t="s">
+      <c r="E54" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="H53" s="28" t="s">
+      <c r="H54" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="28" t="s">
+      <c r="I54" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="J53" s="29" t="s">
+      <c r="J54" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="M53" s="45"/>
-      <c r="N53" s="45"/>
-      <c r="Q53" s="30"/>
-      <c r="R53" s="30"/>
-      <c r="S53" s="30"/>
-    </row>
-    <row r="54" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="15">
+      <c r="M54" s="45"/>
+      <c r="N54" s="45"/>
+      <c r="Q54" s="30"/>
+      <c r="R54" s="30"/>
+      <c r="S54" s="30"/>
+    </row>
+    <row r="55" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="15">
         <v>2035</v>
       </c>
-      <c r="B54" s="15" t="s">
+      <c r="B55" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="C54" s="15" t="s">
+      <c r="C55" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="D54" s="15" t="s">
+      <c r="D55" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="E54" s="15" t="s">
+      <c r="E55" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="F54" s="15" t="s">
+      <c r="F55" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="G54" s="18" t="s">
+      <c r="G55" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="H54" s="15" t="s">
+      <c r="H55" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I54" s="15" t="s">
+      <c r="I55" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="J54" s="16" t="s">
+      <c r="J55" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="K54" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="L54" s="15">
+      <c r="K55" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="L55" s="15">
         <v>15.85</v>
       </c>
-      <c r="M54" s="46">
+      <c r="M55" s="46">
         <v>-0.27</v>
       </c>
-      <c r="N54" s="46">
-        <v>0</v>
-      </c>
-      <c r="O54" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="P54" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q54" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="R54" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="S54" s="17" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="55" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="12">
-        <v>2035</v>
-      </c>
-      <c r="B55" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="C55" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D55" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="E55" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="F55" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G55" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H55" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I55" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="J55" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="K55" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="L55" s="12">
-        <v>15.85</v>
-      </c>
-      <c r="M55" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="N55" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="O55" s="14">
-        <v>1.27</v>
-      </c>
-      <c r="P55" s="14">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="Q55" s="14">
-        <v>120</v>
-      </c>
-      <c r="R55" s="14">
-        <v>0</v>
-      </c>
-      <c r="S55" s="14">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="56" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N55" s="46">
+        <v>0</v>
+      </c>
+      <c r="O55" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="P55" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q55" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="R55" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="S55" s="17" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="12">
         <v>2035</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C56" s="12" t="s">
         <v>18</v>
@@ -4134,7 +4155,7 @@
         <v>103</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F56" s="12" t="s">
         <v>10</v>
@@ -4149,13 +4170,13 @@
         <v>105</v>
       </c>
       <c r="J56" s="13" t="s">
-        <v>110</v>
+        <v>44</v>
       </c>
       <c r="K56" s="12" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="L56" s="12">
-        <v>18.64</v>
+        <v>15.85</v>
       </c>
       <c r="M56" s="47" t="s">
         <v>111</v>
@@ -4179,12 +4200,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="57" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="12">
         <v>2035</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C57" s="12" t="s">
         <v>18</v>
@@ -4193,7 +4214,7 @@
         <v>103</v>
       </c>
       <c r="E57" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F57" s="12" t="s">
         <v>10</v>
@@ -4208,10 +4229,10 @@
         <v>105</v>
       </c>
       <c r="J57" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K57" s="12" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="L57" s="12">
         <v>18.64</v>
@@ -4229,21 +4250,21 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="Q57" s="14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="R57" s="14">
         <v>0</v>
       </c>
       <c r="S57" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="12">
         <v>2035</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="C58" s="12" t="s">
         <v>18</v>
@@ -4252,7 +4273,7 @@
         <v>103</v>
       </c>
       <c r="E58" s="12" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="F58" s="12" t="s">
         <v>10</v>
@@ -4267,10 +4288,10 @@
         <v>105</v>
       </c>
       <c r="J58" s="13" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="K58" s="12" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="L58" s="12">
         <v>18.64</v>
@@ -4281,28 +4302,28 @@
       <c r="N58" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="O58" s="12">
-        <v>0.95</v>
-      </c>
-      <c r="P58" s="12">
-        <v>0.86</v>
+      <c r="O58" s="14">
+        <v>1.27</v>
+      </c>
+      <c r="P58" s="14">
+        <v>1.1499999999999999</v>
       </c>
       <c r="Q58" s="14">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="R58" s="14">
         <v>0</v>
       </c>
       <c r="S58" s="14">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="59" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="12">
         <v>2035</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C59" s="12" t="s">
         <v>18</v>
@@ -4311,7 +4332,7 @@
         <v>103</v>
       </c>
       <c r="E59" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F59" s="12" t="s">
         <v>10</v>
@@ -4326,10 +4347,10 @@
         <v>105</v>
       </c>
       <c r="J59" s="13" t="s">
-        <v>43</v>
+        <v>110</v>
       </c>
       <c r="K59" s="12" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="L59" s="12">
         <v>18.64</v>
@@ -4347,21 +4368,21 @@
         <v>0.86</v>
       </c>
       <c r="Q59" s="14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="R59" s="14">
         <v>0</v>
       </c>
       <c r="S59" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="12">
         <v>2035</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>188</v>
+        <v>123</v>
       </c>
       <c r="C60" s="12" t="s">
         <v>18</v>
@@ -4370,7 +4391,7 @@
         <v>103</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>189</v>
+        <v>125</v>
       </c>
       <c r="F60" s="12" t="s">
         <v>10</v>
@@ -4385,10 +4406,10 @@
         <v>105</v>
       </c>
       <c r="J60" s="13" t="s">
-        <v>110</v>
+        <v>43</v>
       </c>
       <c r="K60" s="12" t="s">
-        <v>191</v>
+        <v>126</v>
       </c>
       <c r="L60" s="12">
         <v>18.64</v>
@@ -4415,59 +4436,236 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="24">
+    <row r="61" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B61" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="C61" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D61" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E61" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="F61" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G61" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H61" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I61" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="J61" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="K61" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="L61" s="12">
+        <v>18.64</v>
+      </c>
+      <c r="M61" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="N61" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="O61" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="P61" s="12">
+        <v>0.86</v>
+      </c>
+      <c r="Q61" s="14">
+        <v>0</v>
+      </c>
+      <c r="R61" s="14">
+        <v>0</v>
+      </c>
+      <c r="S61" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B62" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="C62" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D62" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E62" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="F62" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G62" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H62" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I62" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="J62" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="K62" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="L62" s="12">
+        <v>18.64</v>
+      </c>
+      <c r="M62" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="N62" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="O62" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="P62" s="12">
+        <v>0.86</v>
+      </c>
+      <c r="Q62" s="14">
+        <v>0</v>
+      </c>
+      <c r="R62" s="14">
+        <v>0</v>
+      </c>
+      <c r="S62" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B63" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="C63" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D63" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E63" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="F63" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="G63" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="H63" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I63" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="J63" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="K63" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="L63" s="12">
+        <v>18.64</v>
+      </c>
+      <c r="M63" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="N63" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="O63" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="P63" s="12">
+        <v>0.86</v>
+      </c>
+      <c r="Q63" s="14">
+        <v>100</v>
+      </c>
+      <c r="R63" s="14">
+        <v>0</v>
+      </c>
+      <c r="S63" s="14">
+        <v>41.25</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="24">
         <v>2050</v>
       </c>
-      <c r="B61" s="24" t="s">
+      <c r="B64" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="C61" s="24" t="s">
+      <c r="C64" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="D61" s="24" t="s">
+      <c r="D64" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="E61" s="24" t="s">
+      <c r="E64" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="F61" s="24" t="s">
+      <c r="F64" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="G61" s="25" t="s">
+      <c r="G64" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="I61" s="24" t="s">
+      <c r="I64" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="J61" s="26" t="s">
+      <c r="J64" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="K61" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="L61" s="24">
+      <c r="K64" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="L64" s="24">
         <v>17.440000000000001</v>
       </c>
-      <c r="M61" s="48">
+      <c r="M64" s="48">
         <v>-0.33</v>
       </c>
-      <c r="N61" s="48">
-        <v>0</v>
-      </c>
-      <c r="O61" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="P61" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q61" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="R61" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="S61" s="27" t="s">
+      <c r="N64" s="48">
+        <v>0</v>
+      </c>
+      <c r="O64" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="P64" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q64" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="R64" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="S64" s="27" t="s">
         <v>111</v>
       </c>
     </row>
@@ -4477,9 +4675,8 @@
     <hyperlink ref="K5" r:id="rId1" xr:uid="{1BE7DD4C-B567-4320-9B69-E8B55CE41797}"/>
     <hyperlink ref="K6" r:id="rId2" xr:uid="{A52BF015-28DA-4569-A638-6E56CCBD2F4D}"/>
     <hyperlink ref="K7" r:id="rId3" xr:uid="{70B88B93-E906-4801-9012-B01BCDB48CBF}"/>
-    <hyperlink ref="K48" r:id="rId4" xr:uid="{AE2270FD-647C-4E5C-90C3-53AF1778C16F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add 2023 v41 and v42 to run log
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\config_RTP2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F143BB5-3C87-4DEF-B653-7A920D098DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14CEF60C-47E2-4C15-96FD-70189C7203F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9900" yWindow="2340" windowWidth="24465" windowHeight="11640" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelRuns" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="226">
   <si>
     <t>year</t>
   </si>
@@ -696,6 +696,24 @@
   </si>
   <si>
     <t>Same as 2015_TM160_IPA_03</t>
+  </si>
+  <si>
+    <t>2023_TM160_IPA_41</t>
+  </si>
+  <si>
+    <t>AOC=16.61, WFH at ~30%</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1205980528918816/f</t>
+  </si>
+  <si>
+    <t>2023_TM160_IPA_42</t>
+  </si>
+  <si>
+    <t>AOC=16.61, WFH at ~31%</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1205983427401938/f</t>
   </si>
 </sst>
 </file>
@@ -839,7 +857,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -949,7 +967,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="2" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1265,34 +1282,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9564CC59-3725-4FDA-8BF2-0F68CB1B6F5A}">
-  <dimension ref="A1:S64"/>
+  <dimension ref="A1:S66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D57" sqref="D57"/>
+      <selection pane="bottomRight" activeCell="J56" sqref="J56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="42.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="42.26953125" style="1" customWidth="1"/>
     <col min="6" max="6" width="23" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" style="10" customWidth="1"/>
-    <col min="11" max="11" width="17.5703125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="6.28515625" style="1" customWidth="1"/>
-    <col min="13" max="14" width="9.140625" style="44"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="8.1796875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="6.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.1796875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.26953125" style="10" customWidth="1"/>
+    <col min="11" max="11" width="17.54296875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="6.26953125" style="1" customWidth="1"/>
+    <col min="13" max="14" width="9.1796875" style="44"/>
+    <col min="15" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="5" customFormat="1" ht="39" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1351,7 +1368,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19">
         <v>2005</v>
       </c>
@@ -1380,7 +1397,7 @@
       <c r="Q2" s="23"/>
       <c r="R2" s="23"/>
     </row>
-    <row r="3" spans="1:19" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="31">
         <v>2005</v>
       </c>
@@ -1433,7 +1450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="35">
         <v>2015</v>
       </c>
@@ -1482,7 +1499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="35">
         <v>2015</v>
       </c>
@@ -1538,7 +1555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="35">
         <v>2015</v>
       </c>
@@ -1591,7 +1608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="35">
         <v>2015</v>
       </c>
@@ -1644,7 +1661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="35">
         <v>2015</v>
       </c>
@@ -1678,7 +1695,7 @@
       <c r="K8" s="36" t="s">
         <v>162</v>
       </c>
-      <c r="L8" s="52">
+      <c r="L8" s="51">
         <v>15.1</v>
       </c>
       <c r="M8" s="42" t="s">
@@ -1703,7 +1720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="35">
         <v>2015</v>
       </c>
@@ -1762,7 +1779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>2023</v>
       </c>
@@ -1808,7 +1825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>2023</v>
       </c>
@@ -1854,7 +1871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>2023</v>
       </c>
@@ -1900,7 +1917,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>2023</v>
       </c>
@@ -1946,7 +1963,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>2023</v>
       </c>
@@ -1992,7 +2009,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>2023</v>
       </c>
@@ -2038,7 +2055,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>2023</v>
       </c>
@@ -2084,7 +2101,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>2023</v>
       </c>
@@ -2130,7 +2147,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>2023</v>
       </c>
@@ -2176,7 +2193,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>2023</v>
       </c>
@@ -2222,7 +2239,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>2023</v>
       </c>
@@ -2268,7 +2285,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>2023</v>
       </c>
@@ -2314,7 +2331,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>2023</v>
       </c>
@@ -2360,7 +2377,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>2023</v>
       </c>
@@ -2406,7 +2423,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>2023</v>
       </c>
@@ -2452,7 +2469,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>2023</v>
       </c>
@@ -2498,7 +2515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>2023</v>
       </c>
@@ -2544,7 +2561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>2023</v>
       </c>
@@ -2590,7 +2607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>2023</v>
       </c>
@@ -2634,7 +2651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>2023</v>
       </c>
@@ -2683,7 +2700,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>2023</v>
       </c>
@@ -2730,7 +2747,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>2023</v>
       </c>
@@ -2780,7 +2797,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>2023</v>
       </c>
@@ -2839,7 +2856,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>2023</v>
       </c>
@@ -2895,7 +2912,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>2023</v>
       </c>
@@ -2954,7 +2971,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>2023</v>
       </c>
@@ -3010,7 +3027,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>2023</v>
       </c>
@@ -3066,7 +3083,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>2023</v>
       </c>
@@ -3122,7 +3139,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>2023</v>
       </c>
@@ -3178,7 +3195,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>2023</v>
       </c>
@@ -3234,7 +3251,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>2023</v>
       </c>
@@ -3290,7 +3307,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>2023</v>
       </c>
@@ -3346,7 +3363,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>2023</v>
       </c>
@@ -3402,7 +3419,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>2023</v>
       </c>
@@ -3461,7 +3478,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>2023</v>
       </c>
@@ -3520,7 +3537,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>2023</v>
       </c>
@@ -3579,7 +3596,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>2023</v>
       </c>
@@ -3638,7 +3655,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>2023</v>
       </c>
@@ -3697,7 +3714,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>2023</v>
       </c>
@@ -3756,7 +3773,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>2023</v>
       </c>
@@ -3787,7 +3804,7 @@
       <c r="J49" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="K49" s="51" t="s">
+      <c r="K49" s="1" t="s">
         <v>193</v>
       </c>
       <c r="L49" s="1">
@@ -3815,7 +3832,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>2023</v>
       </c>
@@ -3874,7 +3891,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>2023</v>
       </c>
@@ -3933,7 +3950,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>2023</v>
       </c>
@@ -3992,7 +4009,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>2023</v>
       </c>
@@ -4051,220 +4068,220 @@
         <v>75</v>
       </c>
     </row>
-    <row r="54" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="28">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A54" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="J54" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="L54" s="1">
+        <v>16.61</v>
+      </c>
+      <c r="M54" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="N54" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="O54" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="P54" s="1">
+        <v>0.89</v>
+      </c>
+      <c r="Q54" s="6">
+        <v>100</v>
+      </c>
+      <c r="R54" s="6">
+        <v>0</v>
+      </c>
+      <c r="S54" s="6">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A55" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="J55" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="L55" s="1">
+        <v>16.61</v>
+      </c>
+      <c r="M55" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="N55" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="O55" s="1">
+        <v>1.04</v>
+      </c>
+      <c r="P55" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="Q55" s="6">
+        <v>100</v>
+      </c>
+      <c r="R55" s="6">
+        <v>0</v>
+      </c>
+      <c r="S55" s="6">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="28">
         <v>2025</v>
       </c>
-      <c r="B54" s="28" t="s">
+      <c r="B56" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="C54" s="28" t="s">
+      <c r="C56" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="D54" s="28" t="s">
+      <c r="D56" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="E54" s="28" t="s">
+      <c r="E56" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="H54" s="28" t="s">
+      <c r="H56" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="I54" s="28" t="s">
+      <c r="I56" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="J54" s="29" t="s">
+      <c r="J56" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="M54" s="45"/>
-      <c r="N54" s="45"/>
-      <c r="Q54" s="30"/>
-      <c r="R54" s="30"/>
-      <c r="S54" s="30"/>
-    </row>
-    <row r="55" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="15">
+      <c r="M56" s="45"/>
+      <c r="N56" s="45"/>
+      <c r="Q56" s="30"/>
+      <c r="R56" s="30"/>
+      <c r="S56" s="30"/>
+    </row>
+    <row r="57" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="15">
         <v>2035</v>
       </c>
-      <c r="B55" s="15" t="s">
+      <c r="B57" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="C55" s="15" t="s">
+      <c r="C57" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="D55" s="15" t="s">
+      <c r="D57" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="E55" s="15" t="s">
+      <c r="E57" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="F55" s="15" t="s">
+      <c r="F57" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="G55" s="18" t="s">
+      <c r="G57" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="H55" s="15" t="s">
+      <c r="H57" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I55" s="15" t="s">
+      <c r="I57" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="J55" s="16" t="s">
+      <c r="J57" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="K55" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="L55" s="15">
+      <c r="K57" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="L57" s="15">
         <v>15.85</v>
       </c>
-      <c r="M55" s="46">
+      <c r="M57" s="46">
         <v>-0.27</v>
       </c>
-      <c r="N55" s="46">
-        <v>0</v>
-      </c>
-      <c r="O55" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="P55" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q55" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="R55" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="S55" s="17" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="56" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="12">
-        <v>2035</v>
-      </c>
-      <c r="B56" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="C56" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D56" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="E56" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="F56" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G56" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H56" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I56" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="J56" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="K56" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="L56" s="12">
-        <v>15.85</v>
-      </c>
-      <c r="M56" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="N56" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="O56" s="14">
-        <v>1.27</v>
-      </c>
-      <c r="P56" s="14">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="Q56" s="14">
-        <v>120</v>
-      </c>
-      <c r="R56" s="14">
-        <v>0</v>
-      </c>
-      <c r="S56" s="14">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="57" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="12">
-        <v>2035</v>
-      </c>
-      <c r="B57" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="C57" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D57" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="E57" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="F57" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G57" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H57" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I57" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="J57" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="K57" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="L57" s="12">
-        <v>18.64</v>
-      </c>
-      <c r="M57" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="N57" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="O57" s="14">
-        <v>1.27</v>
-      </c>
-      <c r="P57" s="14">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="Q57" s="14">
-        <v>120</v>
-      </c>
-      <c r="R57" s="14">
-        <v>0</v>
-      </c>
-      <c r="S57" s="14">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="58" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="N57" s="46">
+        <v>0</v>
+      </c>
+      <c r="O57" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="P57" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q57" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="R57" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="S57" s="17" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="12">
         <v>2035</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C58" s="12" t="s">
         <v>18</v>
@@ -4273,7 +4290,7 @@
         <v>103</v>
       </c>
       <c r="E58" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F58" s="12" t="s">
         <v>10</v>
@@ -4288,13 +4305,13 @@
         <v>105</v>
       </c>
       <c r="J58" s="13" t="s">
-        <v>112</v>
+        <v>44</v>
       </c>
       <c r="K58" s="12" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="L58" s="12">
-        <v>18.64</v>
+        <v>15.85</v>
       </c>
       <c r="M58" s="47" t="s">
         <v>111</v>
@@ -4309,21 +4326,21 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="Q58" s="14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="R58" s="14">
         <v>0</v>
       </c>
       <c r="S58" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="12">
         <v>2035</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="C59" s="12" t="s">
         <v>18</v>
@@ -4332,7 +4349,7 @@
         <v>103</v>
       </c>
       <c r="E59" s="12" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="F59" s="12" t="s">
         <v>10</v>
@@ -4350,7 +4367,7 @@
         <v>110</v>
       </c>
       <c r="K59" s="12" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="L59" s="12">
         <v>18.64</v>
@@ -4361,11 +4378,11 @@
       <c r="N59" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="O59" s="12">
-        <v>0.95</v>
-      </c>
-      <c r="P59" s="12">
-        <v>0.86</v>
+      <c r="O59" s="14">
+        <v>1.27</v>
+      </c>
+      <c r="P59" s="14">
+        <v>1.1499999999999999</v>
       </c>
       <c r="Q59" s="14">
         <v>120</v>
@@ -4377,12 +4394,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="60" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="12">
         <v>2035</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="C60" s="12" t="s">
         <v>18</v>
@@ -4391,7 +4408,7 @@
         <v>103</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="F60" s="12" t="s">
         <v>10</v>
@@ -4406,10 +4423,10 @@
         <v>105</v>
       </c>
       <c r="J60" s="13" t="s">
-        <v>43</v>
+        <v>112</v>
       </c>
       <c r="K60" s="12" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="L60" s="12">
         <v>18.64</v>
@@ -4420,11 +4437,11 @@
       <c r="N60" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="O60" s="12">
-        <v>0.95</v>
-      </c>
-      <c r="P60" s="12">
-        <v>0.86</v>
+      <c r="O60" s="14">
+        <v>1.27</v>
+      </c>
+      <c r="P60" s="14">
+        <v>1.1499999999999999</v>
       </c>
       <c r="Q60" s="14">
         <v>0</v>
@@ -4436,12 +4453,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="12">
         <v>2035</v>
       </c>
       <c r="B61" s="12" t="s">
-        <v>188</v>
+        <v>122</v>
       </c>
       <c r="C61" s="12" t="s">
         <v>18</v>
@@ -4450,7 +4467,7 @@
         <v>103</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>213</v>
+        <v>124</v>
       </c>
       <c r="F61" s="12" t="s">
         <v>10</v>
@@ -4468,7 +4485,7 @@
         <v>110</v>
       </c>
       <c r="K61" s="12" t="s">
-        <v>190</v>
+        <v>127</v>
       </c>
       <c r="L61" s="12">
         <v>18.64</v>
@@ -4486,21 +4503,21 @@
         <v>0.86</v>
       </c>
       <c r="Q61" s="14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="R61" s="14">
         <v>0</v>
       </c>
       <c r="S61" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="12">
         <v>2035</v>
       </c>
       <c r="B62" s="12" t="s">
-        <v>211</v>
+        <v>123</v>
       </c>
       <c r="C62" s="12" t="s">
         <v>18</v>
@@ -4509,7 +4526,7 @@
         <v>103</v>
       </c>
       <c r="E62" s="12" t="s">
-        <v>214</v>
+        <v>125</v>
       </c>
       <c r="F62" s="12" t="s">
         <v>10</v>
@@ -4524,10 +4541,10 @@
         <v>105</v>
       </c>
       <c r="J62" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K62" s="12" t="s">
-        <v>190</v>
+        <v>126</v>
       </c>
       <c r="L62" s="12">
         <v>18.64</v>
@@ -4554,12 +4571,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="12">
         <v>2035</v>
       </c>
       <c r="B63" s="12" t="s">
-        <v>210</v>
+        <v>188</v>
       </c>
       <c r="C63" s="12" t="s">
         <v>18</v>
@@ -4568,13 +4585,13 @@
         <v>103</v>
       </c>
       <c r="E63" s="12" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="F63" s="12" t="s">
-        <v>215</v>
+        <v>10</v>
       </c>
       <c r="G63" s="12" t="s">
-        <v>119</v>
+        <v>11</v>
       </c>
       <c r="H63" s="12" t="s">
         <v>12</v>
@@ -4583,10 +4600,10 @@
         <v>105</v>
       </c>
       <c r="J63" s="13" t="s">
-        <v>45</v>
+        <v>110</v>
       </c>
       <c r="K63" s="12" t="s">
-        <v>216</v>
+        <v>190</v>
       </c>
       <c r="L63" s="12">
         <v>18.64</v>
@@ -4604,68 +4621,186 @@
         <v>0.86</v>
       </c>
       <c r="Q63" s="14">
+        <v>0</v>
+      </c>
+      <c r="R63" s="14">
+        <v>0</v>
+      </c>
+      <c r="S63" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B64" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="C64" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D64" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E64" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="F64" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G64" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H64" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I64" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="J64" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="K64" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="L64" s="12">
+        <v>18.64</v>
+      </c>
+      <c r="M64" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="N64" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="O64" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="P64" s="12">
+        <v>0.86</v>
+      </c>
+      <c r="Q64" s="14">
+        <v>0</v>
+      </c>
+      <c r="R64" s="14">
+        <v>0</v>
+      </c>
+      <c r="S64" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B65" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="C65" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D65" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E65" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="F65" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="G65" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="H65" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I65" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="J65" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="K65" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="L65" s="12">
+        <v>18.64</v>
+      </c>
+      <c r="M65" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="N65" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="O65" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="P65" s="12">
+        <v>0.86</v>
+      </c>
+      <c r="Q65" s="14">
         <v>100</v>
       </c>
-      <c r="R63" s="14">
-        <v>0</v>
-      </c>
-      <c r="S63" s="14">
+      <c r="R65" s="14">
+        <v>0</v>
+      </c>
+      <c r="S65" s="14">
         <v>41.25</v>
       </c>
     </row>
-    <row r="64" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="24">
+    <row r="66" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="24">
         <v>2050</v>
       </c>
-      <c r="B64" s="24" t="s">
+      <c r="B66" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="C64" s="24" t="s">
+      <c r="C66" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="D64" s="24" t="s">
+      <c r="D66" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="E64" s="24" t="s">
+      <c r="E66" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="F64" s="24" t="s">
+      <c r="F66" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="G64" s="25" t="s">
+      <c r="G66" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="I64" s="24" t="s">
+      <c r="I66" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="J64" s="26" t="s">
+      <c r="J66" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="K64" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="L64" s="24">
+      <c r="K66" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="L66" s="24">
         <v>17.440000000000001</v>
       </c>
-      <c r="M64" s="48">
+      <c r="M66" s="48">
         <v>-0.33</v>
       </c>
-      <c r="N64" s="48">
-        <v>0</v>
-      </c>
-      <c r="O64" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="P64" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q64" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="R64" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="S64" s="27" t="s">
+      <c r="N66" s="48">
+        <v>0</v>
+      </c>
+      <c r="O66" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="P66" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q66" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="R66" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="S66" s="27" t="s">
         <v>111</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add IPA round of model runs
2005_TM160_IPA_02
2035_TM160_IPA_08
2035_TM160_IPA_09
2035_TM160_IPA_09_PBA50landuse
2035_TM160_IPA_09_PBA50aoc
2035_TM160_IPA_09_minusModePref
2035_TM160_IPA_09_PBA50ixex
2035_TM160_IPA_09_PBA50wfh
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14CEF60C-47E2-4C15-96FD-70189C7203F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2377509-8066-4945-98BE-C57920FF8E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
+    <workbookView xWindow="9405" yWindow="1095" windowWidth="26580" windowHeight="13170" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelRuns" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="251">
   <si>
     <t>year</t>
   </si>
@@ -503,9 +503,6 @@
     <t>https://app.asana.com/0/1204085012544660/1205634764978035/f</t>
   </si>
   <si>
-    <t>\RTP2021\IncrementalProgress\2005_TM152_IPA_03\INPUT</t>
-  </si>
-  <si>
     <t>WFH at 25%, trn hes=120, 0, 45</t>
   </si>
   <si>
@@ -714,6 +711,84 @@
   </si>
   <si>
     <t>https://app.asana.com/0/1204085012544660/1205983427401938/f</t>
+  </si>
+  <si>
+    <t>2005_TM160_IPA_02</t>
+  </si>
+  <si>
+    <t>TM160 2005 run with WFH equivalent to PBA50 2005</t>
+  </si>
+  <si>
+    <t>RTP2021\IncrementalProgress\2005_TM152_IPA_03\INPUT</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1205996578467417/f</t>
+  </si>
+  <si>
+    <t>IPA minus EN7</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1205987181125876/f</t>
+  </si>
+  <si>
+    <t>2035_TM160_IPA_08</t>
+  </si>
+  <si>
+    <t>2035_TM160_IPA_09</t>
+  </si>
+  <si>
+    <t>IPA with all in</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1205996812896085/f</t>
+  </si>
+  <si>
+    <t>2035_TM160_IPA_09_PBA50landuse</t>
+  </si>
+  <si>
+    <t>IPA with PBA50 landuse/pop</t>
+  </si>
+  <si>
+    <t>POPLU_v225_UBI</t>
+  </si>
+  <si>
+    <t>run183</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1205995415086649/f</t>
+  </si>
+  <si>
+    <t>2035_TM160_IPA_09_PBA50aoc</t>
+  </si>
+  <si>
+    <t>IPA with PBA50 aoc</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1205995415086641/f</t>
+  </si>
+  <si>
+    <t>2035_TM160_IPA_09_PBA50ixex</t>
+  </si>
+  <si>
+    <t>IPA with PBA50 ixex</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1205995415086647/f</t>
+  </si>
+  <si>
+    <t>2035_TM160_IPA_09_PBA50wfh</t>
+  </si>
+  <si>
+    <t>IPA with PBA50 wfh</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1205995415086637/f</t>
+  </si>
+  <si>
+    <t>2035_TM160_IPA_09_minusModePref</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1205995415086639/f</t>
   </si>
 </sst>
 </file>
@@ -765,7 +840,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -826,6 +901,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -857,7 +938,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -968,6 +1049,8 @@
     <xf numFmtId="164" fontId="4" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="2" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="4" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1282,34 +1365,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9564CC59-3725-4FDA-8BF2-0F68CB1B6F5A}">
-  <dimension ref="A1:S66"/>
+  <dimension ref="A1:S74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C39" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J56" sqref="J56"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.81640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.81640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="42.26953125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="42.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="23" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.1796875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="6.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.1796875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.26953125" style="10" customWidth="1"/>
-    <col min="11" max="11" width="17.54296875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="6.26953125" style="1" customWidth="1"/>
-    <col min="13" max="14" width="9.1796875" style="44"/>
-    <col min="15" max="16384" width="9.1796875" style="1"/>
+    <col min="7" max="7" width="8.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" style="10" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="6.28515625" style="1" customWidth="1"/>
+    <col min="13" max="14" width="9.140625" style="44"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="5" customFormat="1" ht="39" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1368,7 +1451,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="19">
         <v>2005</v>
       </c>
@@ -1397,7 +1480,7 @@
       <c r="Q2" s="23"/>
       <c r="R2" s="23"/>
     </row>
-    <row r="3" spans="1:19" s="32" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="31">
         <v>2005</v>
       </c>
@@ -1413,11 +1496,11 @@
       <c r="E3" s="32" t="s">
         <v>153</v>
       </c>
-      <c r="H3" s="32" t="s">
-        <v>12</v>
+      <c r="G3" s="32" t="s">
+        <v>11</v>
       </c>
       <c r="I3" s="32" t="s">
-        <v>155</v>
+        <v>227</v>
       </c>
       <c r="J3" s="33" t="s">
         <v>89</v>
@@ -1450,61 +1533,64 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="35">
-        <v>2015</v>
-      </c>
-      <c r="B4" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="36" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="36" t="s">
+    <row r="4" spans="1:19" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="31">
+        <v>2005</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>225</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="32" t="s">
+        <v>226</v>
+      </c>
+      <c r="G4" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" s="36" t="s">
-        <v>24</v>
-      </c>
-      <c r="M4" s="42">
-        <v>-0.09</v>
-      </c>
-      <c r="N4" s="42">
-        <v>0.9</v>
-      </c>
-      <c r="O4" s="38"/>
-      <c r="P4" s="38"/>
-      <c r="Q4" s="38">
-        <v>0</v>
-      </c>
-      <c r="R4" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="I4" s="32" t="s">
+        <v>227</v>
+      </c>
+      <c r="J4" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="K4" s="32" t="s">
+        <v>228</v>
+      </c>
+      <c r="L4" s="32">
+        <v>14.87</v>
+      </c>
+      <c r="M4" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="N4" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="O4" s="34"/>
+      <c r="P4" s="34"/>
+      <c r="Q4" s="34">
+        <v>0</v>
+      </c>
+      <c r="R4" s="34">
+        <v>0</v>
+      </c>
+      <c r="S4" s="34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="35">
         <v>2015</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>148</v>
+        <v>9</v>
       </c>
       <c r="C5" s="36" t="s">
         <v>18</v>
@@ -1513,7 +1599,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="36" t="s">
-        <v>152</v>
+        <v>20</v>
       </c>
       <c r="F5" s="36" t="s">
         <v>10</v>
@@ -1525,42 +1611,35 @@
         <v>12</v>
       </c>
       <c r="I5" s="36" t="s">
-        <v>149</v>
+        <v>14</v>
       </c>
       <c r="J5" s="37" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="K5" s="36" t="s">
-        <v>150</v>
-      </c>
-      <c r="M5" s="42" t="s">
-        <v>111</v>
-      </c>
-      <c r="N5" s="42" t="s">
-        <v>111</v>
-      </c>
-      <c r="O5" s="38">
-        <v>0</v>
-      </c>
-      <c r="P5" s="38">
-        <v>0</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="M5" s="42">
+        <v>-0.09</v>
+      </c>
+      <c r="N5" s="42">
+        <v>0.9</v>
+      </c>
+      <c r="O5" s="38"/>
+      <c r="P5" s="38"/>
       <c r="Q5" s="38">
         <v>0</v>
       </c>
       <c r="R5" s="38">
         <v>0</v>
       </c>
-      <c r="S5" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="35">
         <v>2015</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C6" s="36" t="s">
         <v>18</v>
@@ -1569,13 +1648,16 @@
         <v>7</v>
       </c>
       <c r="E6" s="36" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="F6" s="36" t="s">
         <v>10</v>
       </c>
       <c r="G6" s="36" t="s">
         <v>11</v>
+      </c>
+      <c r="H6" s="36" t="s">
+        <v>12</v>
       </c>
       <c r="I6" s="36" t="s">
         <v>149</v>
@@ -1593,10 +1675,10 @@
         <v>111</v>
       </c>
       <c r="O6" s="38">
-        <v>0.32</v>
+        <v>0</v>
       </c>
       <c r="P6" s="38">
-        <v>0.28000000000000003</v>
+        <v>0</v>
       </c>
       <c r="Q6" s="38">
         <v>0</v>
@@ -1608,12 +1690,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="35">
         <v>2015</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C7" s="36" t="s">
         <v>18</v>
@@ -1622,7 +1704,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="36" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F7" s="36" t="s">
         <v>10</v>
@@ -1661,12 +1743,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="35">
         <v>2015</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C8" s="36" t="s">
         <v>18</v>
@@ -1675,28 +1757,22 @@
         <v>7</v>
       </c>
       <c r="E8" s="36" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="F8" s="36" t="s">
         <v>10</v>
       </c>
       <c r="G8" s="36" t="s">
         <v>11</v>
-      </c>
-      <c r="H8" s="36" t="s">
-        <v>12</v>
       </c>
       <c r="I8" s="36" t="s">
         <v>149</v>
       </c>
       <c r="J8" s="37" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="K8" s="36" t="s">
-        <v>162</v>
-      </c>
-      <c r="L8" s="51">
-        <v>15.1</v>
+        <v>150</v>
       </c>
       <c r="M8" s="42" t="s">
         <v>111</v>
@@ -1705,10 +1781,10 @@
         <v>111</v>
       </c>
       <c r="O8" s="38">
-        <v>0.32300000000000001</v>
-      </c>
-      <c r="P8" s="49">
-        <v>0.83099999999999996</v>
+        <v>0.32</v>
+      </c>
+      <c r="P8" s="38">
+        <v>0.28000000000000003</v>
       </c>
       <c r="Q8" s="38">
         <v>0</v>
@@ -1720,12 +1796,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="35">
         <v>2015</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>217</v>
+        <v>159</v>
       </c>
       <c r="C9" s="36" t="s">
         <v>18</v>
@@ -1734,7 +1810,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="36" t="s">
-        <v>219</v>
+        <v>160</v>
       </c>
       <c r="F9" s="36" t="s">
         <v>10</v>
@@ -1752,10 +1828,10 @@
         <v>17</v>
       </c>
       <c r="K9" s="36" t="s">
-        <v>218</v>
-      </c>
-      <c r="L9" s="36">
-        <v>13.73</v>
+        <v>161</v>
+      </c>
+      <c r="L9" s="51">
+        <v>15.1</v>
       </c>
       <c r="M9" s="42" t="s">
         <v>111</v>
@@ -1779,58 +1855,71 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <v>2023</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J10" s="9" t="s">
+    <row r="10" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="35">
+        <v>2015</v>
+      </c>
+      <c r="B10" s="36" t="s">
+        <v>216</v>
+      </c>
+      <c r="C10" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="36" t="s">
+        <v>218</v>
+      </c>
+      <c r="F10" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="J10" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M10" s="43">
-        <v>-0.44</v>
-      </c>
-      <c r="N10" s="43">
-        <v>-0.23</v>
-      </c>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6">
-        <v>0</v>
-      </c>
-      <c r="R10" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="K10" s="36" t="s">
+        <v>217</v>
+      </c>
+      <c r="L10" s="36">
+        <v>13.73</v>
+      </c>
+      <c r="M10" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="N10" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="O10" s="38">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="P10" s="49">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="Q10" s="38">
+        <v>0</v>
+      </c>
+      <c r="R10" s="38">
+        <v>0</v>
+      </c>
+      <c r="S10" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>2023</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>18</v>
@@ -1839,7 +1928,7 @@
         <v>7</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>10</v>
@@ -1854,29 +1943,29 @@
         <v>17</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M11" s="43">
-        <v>-1.25</v>
+        <v>-0.44</v>
       </c>
       <c r="N11" s="43">
-        <v>-0.75</v>
+        <v>-0.23</v>
       </c>
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
       <c r="Q11" s="6">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="R11" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>2023</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>18</v>
@@ -1885,7 +1974,7 @@
         <v>7</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>10</v>
@@ -1894,13 +1983,13 @@
         <v>11</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="J12" s="9" t="s">
         <v>17</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="M12" s="43">
         <v>-1.25</v>
@@ -1911,18 +2000,18 @@
       <c r="O12" s="6"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="6">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="R12" s="6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>2023</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>18</v>
@@ -1931,7 +2020,7 @@
         <v>7</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>10</v>
@@ -1940,13 +2029,13 @@
         <v>11</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J13" s="9" t="s">
         <v>17</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M13" s="43">
         <v>-1.25</v>
@@ -1957,18 +2046,18 @@
       <c r="O13" s="6"/>
       <c r="P13" s="6"/>
       <c r="Q13" s="6">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="R13" s="6">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>2023</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>18</v>
@@ -1977,7 +2066,7 @@
         <v>7</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>10</v>
@@ -1992,7 +2081,7 @@
         <v>17</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="M14" s="43">
         <v>-1.25</v>
@@ -2002,19 +2091,19 @@
       </c>
       <c r="O14" s="6"/>
       <c r="P14" s="6"/>
-      <c r="Q14" s="11">
+      <c r="Q14" s="6">
         <v>75</v>
       </c>
-      <c r="R14" s="11">
+      <c r="R14" s="6">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>2023</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>18</v>
@@ -2023,7 +2112,7 @@
         <v>7</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>10</v>
@@ -2035,10 +2124,10 @@
         <v>33</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="M15" s="43">
         <v>-1.25</v>
@@ -2048,19 +2137,19 @@
       </c>
       <c r="O15" s="6"/>
       <c r="P15" s="6"/>
-      <c r="Q15" s="7">
-        <v>85</v>
-      </c>
-      <c r="R15" s="7">
+      <c r="Q15" s="11">
+        <v>75</v>
+      </c>
+      <c r="R15" s="11">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>2023</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>18</v>
@@ -2081,7 +2170,7 @@
         <v>33</v>
       </c>
       <c r="J16" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>46</v>
@@ -2095,18 +2184,18 @@
       <c r="O16" s="6"/>
       <c r="P16" s="6"/>
       <c r="Q16" s="7">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="R16" s="7">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>2023</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>18</v>
@@ -2127,7 +2216,7 @@
         <v>33</v>
       </c>
       <c r="J17" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>46</v>
@@ -2141,18 +2230,18 @@
       <c r="O17" s="6"/>
       <c r="P17" s="6"/>
       <c r="Q17" s="7">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="R17" s="7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>2023</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>18</v>
@@ -2161,7 +2250,7 @@
         <v>7</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>10</v>
@@ -2170,13 +2259,13 @@
         <v>11</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J18" s="10" t="s">
-        <v>43</v>
+        <v>33</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>45</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="M18" s="43">
         <v>-1.25</v>
@@ -2193,12 +2282,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>2023</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>18</v>
@@ -2207,7 +2296,7 @@
         <v>7</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>10</v>
@@ -2216,13 +2305,13 @@
         <v>11</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="J19" s="10" t="s">
         <v>43</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="M19" s="43">
         <v>-1.25</v>
@@ -2233,18 +2322,18 @@
       <c r="O19" s="6"/>
       <c r="P19" s="6"/>
       <c r="Q19" s="7">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="R19" s="7">
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>2023</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>18</v>
@@ -2253,7 +2342,7 @@
         <v>7</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>10</v>
@@ -2265,7 +2354,7 @@
         <v>54</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>57</v>
@@ -2279,18 +2368,18 @@
       <c r="O20" s="6"/>
       <c r="P20" s="6"/>
       <c r="Q20" s="7">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="R20" s="7">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>2023</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>18</v>
@@ -2299,7 +2388,7 @@
         <v>7</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>10</v>
@@ -2308,13 +2397,13 @@
         <v>11</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="M21" s="43">
         <v>-1.25</v>
@@ -2325,18 +2414,18 @@
       <c r="O21" s="6"/>
       <c r="P21" s="6"/>
       <c r="Q21" s="7">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="R21" s="7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>2023</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>18</v>
@@ -2345,7 +2434,7 @@
         <v>7</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>10</v>
@@ -2360,7 +2449,7 @@
         <v>43</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="M22" s="43">
         <v>-1.25</v>
@@ -2371,18 +2460,18 @@
       <c r="O22" s="6"/>
       <c r="P22" s="6"/>
       <c r="Q22" s="7">
-        <v>300</v>
+        <v>180</v>
       </c>
       <c r="R22" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>2023</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>18</v>
@@ -2417,18 +2506,18 @@
       <c r="O23" s="6"/>
       <c r="P23" s="6"/>
       <c r="Q23" s="7">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="R23" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>2023</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>18</v>
@@ -2463,18 +2552,18 @@
       <c r="O24" s="6"/>
       <c r="P24" s="6"/>
       <c r="Q24" s="7">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="R24" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>2023</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>18</v>
@@ -2483,7 +2572,7 @@
         <v>7</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>10</v>
@@ -2492,13 +2581,13 @@
         <v>11</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="J25" s="10" t="s">
         <v>43</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M25" s="43">
         <v>-1.25</v>
@@ -2509,18 +2598,18 @@
       <c r="O25" s="6"/>
       <c r="P25" s="6"/>
       <c r="Q25" s="7">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="R25" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>2023</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>18</v>
@@ -2529,7 +2618,7 @@
         <v>7</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>10</v>
@@ -2538,13 +2627,13 @@
         <v>11</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="J26" s="10" t="s">
         <v>43</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="M26" s="43">
         <v>-1.25</v>
@@ -2561,12 +2650,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>2023</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>18</v>
@@ -2575,7 +2664,7 @@
         <v>7</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>10</v>
@@ -2584,13 +2673,13 @@
         <v>11</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="J27" s="10" t="s">
         <v>43</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="M27" s="43">
         <v>-1.25</v>
@@ -2607,12 +2696,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>2023</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>18</v>
@@ -2621,7 +2710,7 @@
         <v>7</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>10</v>
@@ -2633,17 +2722,19 @@
         <v>80</v>
       </c>
       <c r="J28" s="10" t="s">
-        <v>89</v>
+        <v>43</v>
       </c>
       <c r="K28" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="O28" s="6">
-        <v>1.27</v>
-      </c>
-      <c r="P28" s="6">
-        <v>1.1499999999999999</v>
-      </c>
+      <c r="M28" s="43">
+        <v>-1.25</v>
+      </c>
+      <c r="N28" s="43">
+        <v>-0.75</v>
+      </c>
+      <c r="O28" s="6"/>
+      <c r="P28" s="6"/>
       <c r="Q28" s="7">
         <v>120</v>
       </c>
@@ -2651,12 +2742,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>2023</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>18</v>
@@ -2665,7 +2756,7 @@
         <v>7</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>10</v>
@@ -2677,35 +2768,30 @@
         <v>80</v>
       </c>
       <c r="J29" s="10" t="s">
-        <v>43</v>
+        <v>89</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="M29" s="43">
-        <v>-1.25</v>
-      </c>
-      <c r="N29" s="43">
-        <v>-0.75</v>
-      </c>
-      <c r="O29" s="6"/>
-      <c r="P29" s="6"/>
+        <v>82</v>
+      </c>
+      <c r="O29" s="6">
+        <v>1.27</v>
+      </c>
+      <c r="P29" s="6">
+        <v>1.1499999999999999</v>
+      </c>
       <c r="Q29" s="7">
         <v>120</v>
       </c>
       <c r="R29" s="7">
         <v>0</v>
       </c>
-      <c r="S29" s="7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>2023</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>18</v>
@@ -2726,17 +2812,19 @@
         <v>80</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>89</v>
+        <v>43</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="O30" s="6">
-        <v>1.27</v>
-      </c>
-      <c r="P30" s="6">
-        <v>1.1499999999999999</v>
-      </c>
+      <c r="M30" s="43">
+        <v>-1.25</v>
+      </c>
+      <c r="N30" s="43">
+        <v>-0.75</v>
+      </c>
+      <c r="O30" s="6"/>
+      <c r="P30" s="6"/>
       <c r="Q30" s="7">
         <v>120</v>
       </c>
@@ -2747,12 +2835,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>2023</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>18</v>
@@ -2761,31 +2849,28 @@
         <v>7</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>80</v>
       </c>
       <c r="J31" s="10" t="s">
-        <v>43</v>
+        <v>89</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="M31" s="43">
-        <v>-1.25</v>
-      </c>
-      <c r="N31" s="43">
-        <v>-0.75</v>
+        <v>90</v>
+      </c>
+      <c r="O31" s="6">
+        <v>1.27</v>
+      </c>
+      <c r="P31" s="6">
+        <v>1.1499999999999999</v>
       </c>
       <c r="Q31" s="7">
         <v>120</v>
@@ -2794,15 +2879,15 @@
         <v>0</v>
       </c>
       <c r="S31" s="7">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>2023</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>18</v>
@@ -2826,25 +2911,16 @@
         <v>80</v>
       </c>
       <c r="J32" s="10" t="s">
-        <v>89</v>
+        <v>43</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="L32" s="1">
-        <v>17.77</v>
-      </c>
-      <c r="M32" s="44" t="s">
-        <v>111</v>
-      </c>
-      <c r="N32" s="44" t="s">
-        <v>111</v>
-      </c>
-      <c r="O32" s="6">
-        <v>1.27</v>
-      </c>
-      <c r="P32" s="6">
-        <v>1.1499999999999999</v>
+      <c r="M32" s="43">
+        <v>-1.25</v>
+      </c>
+      <c r="N32" s="43">
+        <v>-0.75</v>
       </c>
       <c r="Q32" s="7">
         <v>120</v>
@@ -2856,12 +2932,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>2023</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>18</v>
@@ -2870,22 +2946,25 @@
         <v>7</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>80</v>
       </c>
       <c r="J33" s="10" t="s">
-        <v>43</v>
+        <v>89</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="L33" s="1">
         <v>17.77</v>
@@ -2896,11 +2975,11 @@
       <c r="N33" s="44" t="s">
         <v>111</v>
       </c>
-      <c r="O33" s="1">
-        <v>0.64</v>
-      </c>
-      <c r="P33" s="1">
-        <v>0.57999999999999996</v>
+      <c r="O33" s="6">
+        <v>1.27</v>
+      </c>
+      <c r="P33" s="6">
+        <v>1.1499999999999999</v>
       </c>
       <c r="Q33" s="7">
         <v>120</v>
@@ -2912,12 +2991,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>2023</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>18</v>
@@ -2926,25 +3005,22 @@
         <v>7</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>156</v>
+        <v>97</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>80</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>89</v>
+        <v>43</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L34" s="1">
         <v>17.77</v>
@@ -2956,27 +3032,27 @@
         <v>111</v>
       </c>
       <c r="O34" s="1">
-        <v>0.95</v>
+        <v>0.64</v>
       </c>
       <c r="P34" s="1">
-        <v>0.86</v>
-      </c>
-      <c r="Q34" s="6">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="Q34" s="7">
         <v>120</v>
       </c>
-      <c r="R34" s="6">
-        <v>0</v>
-      </c>
-      <c r="S34" s="6">
+      <c r="R34" s="7">
+        <v>0</v>
+      </c>
+      <c r="S34" s="7">
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>2023</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>141</v>
+        <v>96</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>18</v>
@@ -2985,22 +3061,25 @@
         <v>7</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>136</v>
+        <v>155</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>80</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>44</v>
+        <v>89</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>139</v>
+        <v>99</v>
       </c>
       <c r="L35" s="1">
         <v>17.77</v>
@@ -3018,21 +3097,21 @@
         <v>0.86</v>
       </c>
       <c r="Q35" s="6">
-        <v>200</v>
+        <v>120</v>
       </c>
       <c r="R35" s="6">
         <v>0</v>
       </c>
       <c r="S35" s="6">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>2023</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>18</v>
@@ -3041,7 +3120,7 @@
         <v>7</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>10</v>
@@ -3053,10 +3132,10 @@
         <v>80</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="L36" s="1">
         <v>17.77</v>
@@ -3074,7 +3153,7 @@
         <v>0.86</v>
       </c>
       <c r="Q36" s="6">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="R36" s="6">
         <v>0</v>
@@ -3083,12 +3162,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>2023</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>18</v>
@@ -3097,7 +3176,7 @@
         <v>7</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>10</v>
@@ -3109,10 +3188,10 @@
         <v>80</v>
       </c>
       <c r="J37" s="10" t="s">
-        <v>132</v>
+        <v>89</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="L37" s="1">
         <v>17.77</v>
@@ -3124,10 +3203,10 @@
         <v>111</v>
       </c>
       <c r="O37" s="1">
-        <v>0.39</v>
+        <v>0.95</v>
       </c>
       <c r="P37" s="1">
-        <v>0.35</v>
+        <v>0.86</v>
       </c>
       <c r="Q37" s="6">
         <v>300</v>
@@ -3139,12 +3218,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>2023</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>18</v>
@@ -3153,7 +3232,7 @@
         <v>7</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>10</v>
@@ -3165,10 +3244,10 @@
         <v>80</v>
       </c>
       <c r="J38" s="10" t="s">
-        <v>44</v>
+        <v>132</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="L38" s="1">
         <v>17.77</v>
@@ -3180,27 +3259,27 @@
         <v>111</v>
       </c>
       <c r="O38" s="1">
-        <v>0.77</v>
+        <v>0.39</v>
       </c>
       <c r="P38" s="1">
-        <v>0.69</v>
+        <v>0.35</v>
       </c>
       <c r="Q38" s="6">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="R38" s="6">
         <v>0</v>
       </c>
       <c r="S38" s="6">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>2023</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>18</v>
@@ -3209,7 +3288,7 @@
         <v>7</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>10</v>
@@ -3221,10 +3300,10 @@
         <v>80</v>
       </c>
       <c r="J39" s="10" t="s">
-        <v>132</v>
+        <v>44</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="L39" s="1">
         <v>17.77</v>
@@ -3236,27 +3315,27 @@
         <v>111</v>
       </c>
       <c r="O39" s="1">
-        <v>0.94</v>
+        <v>0.77</v>
       </c>
       <c r="P39" s="1">
-        <v>0.85499999999999998</v>
+        <v>0.69</v>
       </c>
       <c r="Q39" s="6">
-        <v>120</v>
+        <v>400</v>
       </c>
       <c r="R39" s="6">
         <v>0</v>
       </c>
       <c r="S39" s="6">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>2023</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>18</v>
@@ -3265,7 +3344,7 @@
         <v>7</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>10</v>
@@ -3274,13 +3353,13 @@
         <v>11</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>167</v>
+        <v>80</v>
       </c>
       <c r="J40" s="10" t="s">
         <v>132</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L40" s="1">
         <v>17.77</v>
@@ -3307,12 +3386,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>2023</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>18</v>
@@ -3321,7 +3400,7 @@
         <v>7</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>10</v>
@@ -3330,13 +3409,13 @@
         <v>11</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J41" s="10" t="s">
         <v>132</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L41" s="1">
         <v>17.77</v>
@@ -3363,12 +3442,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>2023</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>18</v>
@@ -3377,7 +3456,7 @@
         <v>7</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>10</v>
@@ -3386,13 +3465,13 @@
         <v>11</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J42" s="10" t="s">
-        <v>17</v>
+        <v>132</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="L42" s="1">
         <v>17.77</v>
@@ -3419,12 +3498,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>2023</v>
       </c>
-      <c r="B43" s="50" t="s">
-        <v>174</v>
+      <c r="B43" s="1" t="s">
+        <v>170</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>18</v>
@@ -3433,7 +3512,7 @@
         <v>7</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>10</v>
@@ -3441,17 +3520,14 @@
       <c r="G43" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H43" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="I43" s="1" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="J43" s="10" t="s">
         <v>17</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="L43" s="1">
         <v>17.77</v>
@@ -3478,12 +3554,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>2023</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>178</v>
+      <c r="B44" s="50" t="s">
+        <v>173</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>18</v>
@@ -3492,7 +3568,7 @@
         <v>7</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>203</v>
+        <v>174</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>10</v>
@@ -3500,17 +3576,14 @@
       <c r="G44" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H44" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="I44" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J44" s="10" t="s">
         <v>17</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="L44" s="1">
         <v>17.77</v>
@@ -3522,10 +3595,10 @@
         <v>111</v>
       </c>
       <c r="O44" s="1">
-        <v>0.99</v>
+        <v>0.94</v>
       </c>
       <c r="P44" s="1">
-        <v>0.89</v>
+        <v>0.85499999999999998</v>
       </c>
       <c r="Q44" s="6">
         <v>120</v>
@@ -3537,12 +3610,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>2023</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>18</v>
@@ -3559,17 +3632,14 @@
       <c r="G45" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H45" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="I45" s="1" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="J45" s="10" t="s">
         <v>17</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="L45" s="1">
         <v>17.77</v>
@@ -3596,12 +3666,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>2023</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>18</v>
@@ -3618,17 +3688,14 @@
       <c r="G46" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H46" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="I46" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="J46" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="K46" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="J46" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="K46" s="1" t="s">
-        <v>183</v>
       </c>
       <c r="L46" s="1">
         <v>17.77</v>
@@ -3640,10 +3707,10 @@
         <v>111</v>
       </c>
       <c r="O46" s="1">
-        <v>1.04</v>
+        <v>0.99</v>
       </c>
       <c r="P46" s="1">
-        <v>0.94</v>
+        <v>0.89</v>
       </c>
       <c r="Q46" s="6">
         <v>120</v>
@@ -3655,12 +3722,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>2023</v>
       </c>
-      <c r="B47" s="50" t="s">
-        <v>185</v>
+      <c r="B47" s="1" t="s">
+        <v>183</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>18</v>
@@ -3677,17 +3744,14 @@
       <c r="G47" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H47" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="I47" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J47" s="10" t="s">
-        <v>45</v>
+        <v>112</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="L47" s="1">
         <v>17.77</v>
@@ -3699,27 +3763,27 @@
         <v>111</v>
       </c>
       <c r="O47" s="1">
-        <v>0.99</v>
+        <v>1.04</v>
       </c>
       <c r="P47" s="1">
-        <v>0.89</v>
+        <v>0.94</v>
       </c>
       <c r="Q47" s="6">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="R47" s="6">
         <v>0</v>
       </c>
       <c r="S47" s="6">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>2023</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>187</v>
+      <c r="B48" s="50" t="s">
+        <v>184</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>18</v>
@@ -3736,17 +3800,14 @@
       <c r="G48" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H48" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="I48" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J48" s="10" t="s">
-        <v>132</v>
+        <v>45</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="L48" s="1">
         <v>17.77</v>
@@ -3758,10 +3819,10 @@
         <v>111</v>
       </c>
       <c r="O48" s="1">
-        <v>1.04</v>
+        <v>0.99</v>
       </c>
       <c r="P48" s="1">
-        <v>0.94</v>
+        <v>0.89</v>
       </c>
       <c r="Q48" s="6">
         <v>100</v>
@@ -3773,12 +3834,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>2023</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>18</v>
@@ -3795,17 +3856,14 @@
       <c r="G49" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H49" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="I49" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J49" s="10" t="s">
-        <v>44</v>
+        <v>132</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="L49" s="1">
         <v>17.77</v>
@@ -3817,27 +3875,27 @@
         <v>111</v>
       </c>
       <c r="O49" s="1">
-        <v>0.99</v>
+        <v>1.04</v>
       </c>
       <c r="P49" s="1">
-        <v>0.89</v>
+        <v>0.94</v>
       </c>
       <c r="Q49" s="6">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="R49" s="6">
         <v>0</v>
       </c>
       <c r="S49" s="6">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>2023</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>18</v>
@@ -3854,17 +3912,14 @@
       <c r="G50" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H50" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="I50" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J50" s="10" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="L50" s="1">
         <v>17.77</v>
@@ -3876,10 +3931,10 @@
         <v>111</v>
       </c>
       <c r="O50" s="1">
-        <v>1.04</v>
+        <v>0.99</v>
       </c>
       <c r="P50" s="1">
-        <v>0.94</v>
+        <v>0.89</v>
       </c>
       <c r="Q50" s="6">
         <v>90</v>
@@ -3891,12 +3946,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>2023</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>18</v>
@@ -3913,17 +3968,14 @@
       <c r="G51" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H51" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="I51" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J51" s="10" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="L51" s="1">
         <v>17.77</v>
@@ -3935,27 +3987,27 @@
         <v>111</v>
       </c>
       <c r="O51" s="1">
-        <v>0.99</v>
+        <v>1.04</v>
       </c>
       <c r="P51" s="1">
-        <v>0.89</v>
+        <v>0.94</v>
       </c>
       <c r="Q51" s="6">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="R51" s="6">
         <v>0</v>
       </c>
       <c r="S51" s="6">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>2023</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>18</v>
@@ -3964,7 +4016,7 @@
         <v>7</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>10</v>
@@ -3972,11 +4024,8 @@
       <c r="G52" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H52" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="I52" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J52" s="10" t="s">
         <v>112</v>
@@ -4006,15 +4055,15 @@
         <v>0</v>
       </c>
       <c r="S52" s="6">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>2023</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>18</v>
@@ -4023,7 +4072,7 @@
         <v>7</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>10</v>
@@ -4031,20 +4080,17 @@
       <c r="G53" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H53" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="I53" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J53" s="10" t="s">
-        <v>44</v>
+        <v>112</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="L53" s="1">
-        <v>16.45</v>
+        <v>17.77</v>
       </c>
       <c r="M53" s="44" t="s">
         <v>111</v>
@@ -4068,12 +4114,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>2023</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>18</v>
@@ -4082,7 +4128,7 @@
         <v>7</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>10</v>
@@ -4094,16 +4140,16 @@
         <v>12</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J54" s="10" t="s">
         <v>44</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="L54" s="1">
-        <v>16.61</v>
+        <v>16.45</v>
       </c>
       <c r="M54" s="44" t="s">
         <v>111</v>
@@ -4127,12 +4173,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>2023</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>18</v>
@@ -4141,7 +4187,7 @@
         <v>7</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>10</v>
@@ -4153,13 +4199,13 @@
         <v>12</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J55" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="L55" s="1">
         <v>16.61</v>
@@ -4171,10 +4217,10 @@
         <v>111</v>
       </c>
       <c r="O55" s="1">
-        <v>1.04</v>
+        <v>0.99</v>
       </c>
       <c r="P55" s="1">
-        <v>0.94</v>
+        <v>0.89</v>
       </c>
       <c r="Q55" s="6">
         <v>100</v>
@@ -4186,161 +4232,161 @@
         <v>75</v>
       </c>
     </row>
-    <row r="56" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="28">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="J56" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="L56" s="1">
+        <v>16.61</v>
+      </c>
+      <c r="M56" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="N56" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="O56" s="1">
+        <v>1.04</v>
+      </c>
+      <c r="P56" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="Q56" s="6">
+        <v>100</v>
+      </c>
+      <c r="R56" s="6">
+        <v>0</v>
+      </c>
+      <c r="S56" s="6">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="28">
         <v>2025</v>
       </c>
-      <c r="B56" s="28" t="s">
+      <c r="B57" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="C56" s="28" t="s">
+      <c r="C57" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="D56" s="28" t="s">
+      <c r="D57" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="E56" s="28" t="s">
+      <c r="E57" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="H56" s="28" t="s">
+      <c r="H57" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="I56" s="28" t="s">
+      <c r="I57" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="J56" s="29" t="s">
+      <c r="J57" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="M56" s="45"/>
-      <c r="N56" s="45"/>
-      <c r="Q56" s="30"/>
-      <c r="R56" s="30"/>
-      <c r="S56" s="30"/>
-    </row>
-    <row r="57" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="15">
+      <c r="M57" s="45"/>
+      <c r="N57" s="45"/>
+      <c r="Q57" s="30"/>
+      <c r="R57" s="30"/>
+      <c r="S57" s="30"/>
+    </row>
+    <row r="58" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="15">
         <v>2035</v>
       </c>
-      <c r="B57" s="15" t="s">
+      <c r="B58" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="C57" s="15" t="s">
+      <c r="C58" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="D57" s="15" t="s">
+      <c r="D58" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="E57" s="15" t="s">
+      <c r="E58" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="F57" s="15" t="s">
+      <c r="F58" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="G57" s="18" t="s">
+      <c r="G58" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="H57" s="15" t="s">
+      <c r="H58" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I57" s="15" t="s">
+      <c r="I58" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="J57" s="16" t="s">
+      <c r="J58" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="K57" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="L57" s="15">
+      <c r="K58" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="L58" s="15">
         <v>15.85</v>
       </c>
-      <c r="M57" s="46">
+      <c r="M58" s="46">
         <v>-0.27</v>
       </c>
-      <c r="N57" s="46">
-        <v>0</v>
-      </c>
-      <c r="O57" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="P57" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q57" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="R57" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="S57" s="17" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="58" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="12">
-        <v>2035</v>
-      </c>
-      <c r="B58" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="C58" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D58" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="E58" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="F58" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G58" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H58" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I58" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="J58" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="K58" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="L58" s="12">
-        <v>15.85</v>
-      </c>
-      <c r="M58" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="N58" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="O58" s="14">
-        <v>1.27</v>
-      </c>
-      <c r="P58" s="14">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="Q58" s="14">
-        <v>120</v>
-      </c>
-      <c r="R58" s="14">
-        <v>0</v>
-      </c>
-      <c r="S58" s="14">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="59" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N58" s="46">
+        <v>0</v>
+      </c>
+      <c r="O58" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="P58" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q58" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="R58" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="S58" s="17" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="12">
         <v>2035</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C59" s="12" t="s">
         <v>18</v>
@@ -4349,28 +4395,25 @@
         <v>103</v>
       </c>
       <c r="E59" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F59" s="12" t="s">
         <v>10</v>
       </c>
       <c r="G59" s="12" t="s">
         <v>11</v>
-      </c>
-      <c r="H59" s="12" t="s">
-        <v>12</v>
       </c>
       <c r="I59" s="12" t="s">
         <v>105</v>
       </c>
       <c r="J59" s="13" t="s">
-        <v>110</v>
+        <v>44</v>
       </c>
       <c r="K59" s="12" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="L59" s="12">
-        <v>18.64</v>
+        <v>15.85</v>
       </c>
       <c r="M59" s="47" t="s">
         <v>111</v>
@@ -4394,12 +4437,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="60" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="12">
         <v>2035</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C60" s="12" t="s">
         <v>18</v>
@@ -4408,25 +4451,22 @@
         <v>103</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F60" s="12" t="s">
         <v>10</v>
       </c>
       <c r="G60" s="12" t="s">
         <v>11</v>
-      </c>
-      <c r="H60" s="12" t="s">
-        <v>12</v>
       </c>
       <c r="I60" s="12" t="s">
         <v>105</v>
       </c>
       <c r="J60" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K60" s="12" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="L60" s="12">
         <v>18.64</v>
@@ -4444,21 +4484,21 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="Q60" s="14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="R60" s="14">
         <v>0</v>
       </c>
       <c r="S60" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="12">
         <v>2035</v>
       </c>
       <c r="B61" s="12" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="C61" s="12" t="s">
         <v>18</v>
@@ -4467,25 +4507,22 @@
         <v>103</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="F61" s="12" t="s">
         <v>10</v>
       </c>
       <c r="G61" s="12" t="s">
         <v>11</v>
-      </c>
-      <c r="H61" s="12" t="s">
-        <v>12</v>
       </c>
       <c r="I61" s="12" t="s">
         <v>105</v>
       </c>
       <c r="J61" s="13" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="K61" s="12" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="L61" s="12">
         <v>18.64</v>
@@ -4496,28 +4533,28 @@
       <c r="N61" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="O61" s="12">
-        <v>0.95</v>
-      </c>
-      <c r="P61" s="12">
-        <v>0.86</v>
+      <c r="O61" s="14">
+        <v>1.27</v>
+      </c>
+      <c r="P61" s="14">
+        <v>1.1499999999999999</v>
       </c>
       <c r="Q61" s="14">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="R61" s="14">
         <v>0</v>
       </c>
       <c r="S61" s="14">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="62" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="12">
         <v>2035</v>
       </c>
       <c r="B62" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C62" s="12" t="s">
         <v>18</v>
@@ -4526,25 +4563,22 @@
         <v>103</v>
       </c>
       <c r="E62" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F62" s="12" t="s">
         <v>10</v>
       </c>
       <c r="G62" s="12" t="s">
         <v>11</v>
-      </c>
-      <c r="H62" s="12" t="s">
-        <v>12</v>
       </c>
       <c r="I62" s="12" t="s">
         <v>105</v>
       </c>
       <c r="J62" s="13" t="s">
-        <v>43</v>
+        <v>110</v>
       </c>
       <c r="K62" s="12" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="L62" s="12">
         <v>18.64</v>
@@ -4562,21 +4596,21 @@
         <v>0.86</v>
       </c>
       <c r="Q62" s="14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="R62" s="14">
         <v>0</v>
       </c>
       <c r="S62" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="12">
         <v>2035</v>
       </c>
       <c r="B63" s="12" t="s">
-        <v>188</v>
+        <v>123</v>
       </c>
       <c r="C63" s="12" t="s">
         <v>18</v>
@@ -4585,25 +4619,22 @@
         <v>103</v>
       </c>
       <c r="E63" s="12" t="s">
-        <v>213</v>
+        <v>125</v>
       </c>
       <c r="F63" s="12" t="s">
         <v>10</v>
       </c>
       <c r="G63" s="12" t="s">
         <v>11</v>
-      </c>
-      <c r="H63" s="12" t="s">
-        <v>12</v>
       </c>
       <c r="I63" s="12" t="s">
         <v>105</v>
       </c>
       <c r="J63" s="13" t="s">
-        <v>110</v>
+        <v>43</v>
       </c>
       <c r="K63" s="12" t="s">
-        <v>190</v>
+        <v>126</v>
       </c>
       <c r="L63" s="12">
         <v>18.64</v>
@@ -4630,12 +4661,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="12">
         <v>2035</v>
       </c>
       <c r="B64" s="12" t="s">
-        <v>211</v>
+        <v>187</v>
       </c>
       <c r="C64" s="12" t="s">
         <v>18</v>
@@ -4644,25 +4675,22 @@
         <v>103</v>
       </c>
       <c r="E64" s="12" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F64" s="12" t="s">
         <v>10</v>
       </c>
       <c r="G64" s="12" t="s">
         <v>11</v>
-      </c>
-      <c r="H64" s="12" t="s">
-        <v>12</v>
       </c>
       <c r="I64" s="12" t="s">
         <v>105</v>
       </c>
       <c r="J64" s="13" t="s">
-        <v>45</v>
+        <v>110</v>
       </c>
       <c r="K64" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="L64" s="12">
         <v>18.64</v>
@@ -4689,7 +4717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="12">
         <v>2035</v>
       </c>
@@ -4703,16 +4731,13 @@
         <v>103</v>
       </c>
       <c r="E65" s="12" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="F65" s="12" t="s">
-        <v>215</v>
+        <v>10</v>
       </c>
       <c r="G65" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="H65" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I65" s="12" t="s">
         <v>105</v>
@@ -4721,7 +4746,7 @@
         <v>45</v>
       </c>
       <c r="K65" s="12" t="s">
-        <v>216</v>
+        <v>189</v>
       </c>
       <c r="L65" s="12">
         <v>18.64</v>
@@ -4739,77 +4764,542 @@
         <v>0.86</v>
       </c>
       <c r="Q65" s="14">
+        <v>0</v>
+      </c>
+      <c r="R65" s="14">
+        <v>0</v>
+      </c>
+      <c r="S65" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B66" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="C66" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D66" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E66" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="F66" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="G66" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="I66" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="J66" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="K66" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="L66" s="12">
+        <v>18.64</v>
+      </c>
+      <c r="M66" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="N66" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="O66" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="P66" s="12">
+        <v>0.86</v>
+      </c>
+      <c r="Q66" s="14">
         <v>100</v>
       </c>
-      <c r="R65" s="14">
-        <v>0</v>
-      </c>
-      <c r="S65" s="14">
+      <c r="R66" s="14">
+        <v>0</v>
+      </c>
+      <c r="S66" s="14">
         <v>41.25</v>
       </c>
     </row>
-    <row r="66" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="24">
+    <row r="67" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B67" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="C67" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D67" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E67" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="F67" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="G67" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="H67" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I67" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="J67" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K67" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="L67" s="12">
+        <v>20.55</v>
+      </c>
+      <c r="M67" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="N67" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="O67" s="12">
+        <v>0.99</v>
+      </c>
+      <c r="P67" s="12">
+        <v>0.89</v>
+      </c>
+      <c r="Q67" s="14">
+        <v>100</v>
+      </c>
+      <c r="R67" s="14">
+        <v>0</v>
+      </c>
+      <c r="S67" s="14">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B68" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="C68" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D68" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E68" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="F68" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="G68" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="H68" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I68" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="J68" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="K68" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="L68" s="12">
+        <v>20.55</v>
+      </c>
+      <c r="M68" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="N68" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="O68" s="12">
+        <v>0.99</v>
+      </c>
+      <c r="P68" s="12">
+        <v>0.89</v>
+      </c>
+      <c r="Q68" s="14">
+        <v>100</v>
+      </c>
+      <c r="R68" s="14">
+        <v>0</v>
+      </c>
+      <c r="S68" s="14">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B69" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="C69" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D69" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E69" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="F69" s="53" t="s">
+        <v>237</v>
+      </c>
+      <c r="G69" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="H69" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I69" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="J69" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="K69" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="L69" s="12">
+        <v>20.55</v>
+      </c>
+      <c r="M69" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="N69" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="O69" s="12">
+        <v>0.99</v>
+      </c>
+      <c r="P69" s="12">
+        <v>0.89</v>
+      </c>
+      <c r="Q69" s="14">
+        <v>100</v>
+      </c>
+      <c r="R69" s="14">
+        <v>0</v>
+      </c>
+      <c r="S69" s="14">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B70" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="C70" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D70" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E70" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="F70" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="G70" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="H70" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I70" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="J70" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="K70" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="L70" s="53">
+        <v>15.85</v>
+      </c>
+      <c r="M70" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="N70" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="O70" s="12">
+        <v>0.99</v>
+      </c>
+      <c r="P70" s="12">
+        <v>0.89</v>
+      </c>
+      <c r="Q70" s="14">
+        <v>100</v>
+      </c>
+      <c r="R70" s="14">
+        <v>0</v>
+      </c>
+      <c r="S70" s="14">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B71" s="12" t="s">
+        <v>249</v>
+      </c>
+      <c r="C71" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D71" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E71" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="F71" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="G71" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="H71" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I71" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="J71" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="K71" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="L71" s="12">
+        <v>20.55</v>
+      </c>
+      <c r="M71" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="N71" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="O71" s="12">
+        <v>0.99</v>
+      </c>
+      <c r="P71" s="12">
+        <v>0.89</v>
+      </c>
+      <c r="Q71" s="52">
+        <v>0</v>
+      </c>
+      <c r="R71" s="52">
+        <v>0</v>
+      </c>
+      <c r="S71" s="52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B72" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="C72" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D72" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E72" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="F72" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="G72" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="H72" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I72" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="J72" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="K72" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="L72" s="12">
+        <v>20.55</v>
+      </c>
+      <c r="M72" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="N72" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="O72" s="12">
+        <v>0.99</v>
+      </c>
+      <c r="P72" s="12">
+        <v>0.89</v>
+      </c>
+      <c r="Q72" s="14">
+        <v>100</v>
+      </c>
+      <c r="R72" s="14">
+        <v>0</v>
+      </c>
+      <c r="S72" s="14">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="73" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B73" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="C73" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D73" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E73" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="F73" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="G73" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="H73" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I73" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="J73" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="K73" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="L73" s="12">
+        <v>20.55</v>
+      </c>
+      <c r="M73" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="N73" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="O73" s="53"/>
+      <c r="P73" s="53"/>
+      <c r="Q73" s="14">
+        <v>100</v>
+      </c>
+      <c r="R73" s="14">
+        <v>0</v>
+      </c>
+      <c r="S73" s="14">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="24">
         <v>2050</v>
       </c>
-      <c r="B66" s="24" t="s">
+      <c r="B74" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="C66" s="24" t="s">
+      <c r="C74" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="D66" s="24" t="s">
+      <c r="D74" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="E66" s="24" t="s">
+      <c r="E74" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="F66" s="24" t="s">
+      <c r="F74" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="G66" s="25" t="s">
+      <c r="G74" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="I66" s="24" t="s">
+      <c r="I74" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="J66" s="26" t="s">
+      <c r="J74" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="K66" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="L66" s="24">
+      <c r="K74" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="L74" s="24">
         <v>17.440000000000001</v>
       </c>
-      <c r="M66" s="48">
+      <c r="M74" s="48">
         <v>-0.33</v>
       </c>
-      <c r="N66" s="48">
-        <v>0</v>
-      </c>
-      <c r="O66" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="P66" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q66" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="R66" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="S66" s="27" t="s">
+      <c r="N74" s="48">
+        <v>0</v>
+      </c>
+      <c r="O74" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="P74" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q74" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="R74" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="S74" s="27" t="s">
         <v>111</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="K5" r:id="rId1" xr:uid="{1BE7DD4C-B567-4320-9B69-E8B55CE41797}"/>
-    <hyperlink ref="K6" r:id="rId2" xr:uid="{A52BF015-28DA-4569-A638-6E56CCBD2F4D}"/>
-    <hyperlink ref="K7" r:id="rId3" xr:uid="{70B88B93-E906-4801-9012-B01BCDB48CBF}"/>
+    <hyperlink ref="K6" r:id="rId1" xr:uid="{1BE7DD4C-B567-4320-9B69-E8B55CE41797}"/>
+    <hyperlink ref="K7" r:id="rId2" xr:uid="{A52BF015-28DA-4569-A638-6E56CCBD2F4D}"/>
+    <hyperlink ref="K8" r:id="rId3" xr:uid="{70B88B93-E906-4801-9012-B01BCDB48CBF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>

<commit_message>
Annotate 2005_TM160_IPA_01 as having wrong land use
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2377509-8066-4945-98BE-C57920FF8E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79BD7FDA-2621-4B18-9FF5-BAB5F61DEE72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9405" yWindow="1095" windowWidth="26580" windowHeight="13170" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
+    <workbookView xWindow="2955" yWindow="1455" windowWidth="26580" windowHeight="13170" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelRuns" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="252">
   <si>
     <t>year</t>
   </si>
@@ -789,6 +789,9 @@
   </si>
   <si>
     <t>https://app.asana.com/0/1204085012544660/1205995415086639/f</t>
+  </si>
+  <si>
+    <t>2015 land use</t>
   </si>
 </sst>
 </file>
@@ -1371,7 +1374,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1496,6 +1499,9 @@
       <c r="E3" s="32" t="s">
         <v>153</v>
       </c>
+      <c r="F3" s="32" t="s">
+        <v>251</v>
+      </c>
       <c r="G3" s="32" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Fix description for 2035_TM160_IPA_09_minusModePref
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79BD7FDA-2621-4B18-9FF5-BAB5F61DEE72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{831BC428-66C8-4FA2-9F46-A3B20D7113D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2955" yWindow="1455" windowWidth="26580" windowHeight="13170" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="253">
   <si>
     <t>year</t>
   </si>
@@ -792,6 +792,9 @@
   </si>
   <si>
     <t>2015 land use</t>
+  </si>
+  <si>
+    <t>IPA with PBA50 ModePrefs</t>
   </si>
 </sst>
 </file>
@@ -1371,10 +1374,10 @@
   <dimension ref="A1:S74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D56" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight" activeCell="E80" sqref="E80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5085,7 +5088,7 @@
         <v>103</v>
       </c>
       <c r="E71" s="12" t="s">
-        <v>233</v>
+        <v>252</v>
       </c>
       <c r="F71" s="12" t="s">
         <v>214</v>

</xml_diff>

<commit_message>
set run_set for 2005_TM152_IPA_03 to RTP2021
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\config_RTP2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{831BC428-66C8-4FA2-9F46-A3B20D7113D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665A7AB3-4B6A-47F1-9B56-432BB8E01AD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2955" yWindow="1455" windowWidth="26580" windowHeight="13170" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
+    <workbookView xWindow="600" yWindow="840" windowWidth="26580" windowHeight="13170" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelRuns" sheetId="1" r:id="rId1"/>
@@ -1374,10 +1374,10 @@
   <dimension ref="A1:S74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D56" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E80" sqref="E80"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1465,7 +1465,7 @@
         <v>128</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>18</v>
+        <v>115</v>
       </c>
       <c r="D2" s="20" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Update run_set again for 2005 RTP2021 run and demote 2005_TM160_IPA_02 from current since it's in progress
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665A7AB3-4B6A-47F1-9B56-432BB8E01AD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E05D57-0B79-469C-A854-ED291E0F8C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="840" windowWidth="26580" windowHeight="13170" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="254">
   <si>
     <t>year</t>
   </si>
@@ -795,6 +795,9 @@
   </si>
   <si>
     <t>IPA with PBA50 ModePrefs</t>
+  </si>
+  <si>
+    <t>RTP2021_IP</t>
   </si>
 </sst>
 </file>
@@ -1374,10 +1377,10 @@
   <dimension ref="A1:S74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1465,7 +1468,7 @@
         <v>128</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>115</v>
+        <v>253</v>
       </c>
       <c r="D2" s="20" t="s">
         <v>7</v>
@@ -1560,9 +1563,6 @@
       </c>
       <c r="G4" s="32" t="s">
         <v>11</v>
-      </c>
-      <c r="H4" s="32" t="s">
-        <v>12</v>
       </c>
       <c r="I4" s="32" t="s">
         <v>227</v>

</xml_diff>

<commit_message>
Demote more runs from current
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E05D57-0B79-469C-A854-ED291E0F8C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA0032FA-A144-4635-9CBE-8D278FD022CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="840" windowWidth="26580" windowHeight="13170" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="254">
   <si>
     <t>year</t>
   </si>
@@ -1377,10 +1377,10 @@
   <dimension ref="A1:S74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C52" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="H74" sqref="H74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1616,9 +1616,6 @@
       <c r="G5" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="36" t="s">
-        <v>12</v>
-      </c>
       <c r="I5" s="36" t="s">
         <v>14</v>
       </c>
@@ -1665,9 +1662,6 @@
       <c r="G6" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="36" t="s">
-        <v>12</v>
-      </c>
       <c r="I6" s="36" t="s">
         <v>149</v>
       </c>
@@ -1885,9 +1879,6 @@
       </c>
       <c r="G10" s="36" t="s">
         <v>11</v>
-      </c>
-      <c r="H10" s="36" t="s">
-        <v>12</v>
       </c>
       <c r="I10" s="36" t="s">
         <v>149</v>
@@ -2913,9 +2904,6 @@
       <c r="G32" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H32" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="I32" s="1" t="s">
         <v>80</v>
       </c>
@@ -2963,9 +2951,6 @@
       <c r="G33" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H33" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="I33" s="1" t="s">
         <v>80</v>
       </c>
@@ -3078,9 +3063,6 @@
       <c r="G35" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H35" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="I35" s="1" t="s">
         <v>80</v>
       </c>
@@ -4145,9 +4127,6 @@
       <c r="G54" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H54" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="I54" s="1" t="s">
         <v>180</v>
       </c>
@@ -4203,9 +4182,6 @@
       </c>
       <c r="G55" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="H55" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="I55" s="1" t="s">
         <v>180</v>
@@ -5213,9 +5189,6 @@
       </c>
       <c r="G73" s="12" t="s">
         <v>119</v>
-      </c>
-      <c r="H73" s="12" t="s">
-        <v>12</v>
       </c>
       <c r="I73" s="12" t="s">
         <v>105</v>

</xml_diff>

<commit_message>
Update categories for clarity
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA0032FA-A144-4635-9CBE-8D278FD022CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85BB413C-4B24-436D-A38C-8EB83CEB74E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="840" windowWidth="26580" windowHeight="13170" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
+    <workbookView xWindow="600" yWindow="840" windowWidth="31110" windowHeight="18795" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelRuns" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="256">
   <si>
     <t>year</t>
   </si>
@@ -59,9 +59,6 @@
     <t>network</t>
   </si>
   <si>
-    <t>Past year</t>
-  </si>
-  <si>
     <t>landuse_path</t>
   </si>
   <si>
@@ -347,9 +344,6 @@
     <t>2035_TM160_IPA_03</t>
   </si>
   <si>
-    <t>Future year</t>
-  </si>
-  <si>
     <t>https://app.asana.com/0/1204085012544660/1205533462992294/f</t>
   </si>
   <si>
@@ -386,9 +380,6 @@
     <t>RTP2021</t>
   </si>
   <si>
-    <t>Plan</t>
-  </si>
-  <si>
     <t>RTP21 adopted run</t>
   </si>
   <si>
@@ -798,6 +789,21 @@
   </si>
   <si>
     <t>RTP2021_IP</t>
+  </si>
+  <si>
+    <t>IPA</t>
+  </si>
+  <si>
+    <t>Previous Plan</t>
+  </si>
+  <si>
+    <t>Base year</t>
+  </si>
+  <si>
+    <t>Previous base year</t>
+  </si>
+  <si>
+    <t>SB375 Base year</t>
   </si>
 </sst>
 </file>
@@ -1377,10 +1383,10 @@
   <dimension ref="A1:S74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C52" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H74" sqref="H74"/>
+      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1388,7 +1394,7 @@
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17" style="1" customWidth="1"/>
     <col min="5" max="5" width="42.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="23" style="1" customWidth="1"/>
     <col min="7" max="7" width="8.140625" style="1" customWidth="1"/>
@@ -1415,10 +1421,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>4</v>
@@ -1430,34 +1436,34 @@
         <v>6</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="M1" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="39" t="s">
-        <v>39</v>
-      </c>
       <c r="O1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="P1" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="S1" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.2">
@@ -1465,21 +1471,21 @@
         <v>2005</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>7</v>
+        <v>255</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F2" s="20"/>
       <c r="G2" s="20"/>
       <c r="H2" s="20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J2" s="22"/>
       <c r="M2" s="40"/>
@@ -1494,40 +1500,40 @@
         <v>2005</v>
       </c>
       <c r="B3" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>255</v>
+      </c>
+      <c r="E3" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>248</v>
+      </c>
+      <c r="G3" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="32" t="s">
+        <v>224</v>
+      </c>
+      <c r="J3" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="K3" s="32" t="s">
         <v>151</v>
-      </c>
-      <c r="C3" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="32" t="s">
-        <v>153</v>
-      </c>
-      <c r="F3" s="32" t="s">
-        <v>251</v>
-      </c>
-      <c r="G3" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="32" t="s">
-        <v>227</v>
-      </c>
-      <c r="J3" s="33" t="s">
-        <v>89</v>
-      </c>
-      <c r="K3" s="32" t="s">
-        <v>154</v>
       </c>
       <c r="L3" s="32">
         <v>14.87</v>
       </c>
       <c r="M3" s="41" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N3" s="41" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O3" s="34">
         <v>0</v>
@@ -1550,37 +1556,37 @@
         <v>2005</v>
       </c>
       <c r="B4" s="32" t="s">
+        <v>222</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>255</v>
+      </c>
+      <c r="E4" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="G4" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="32" t="s">
+        <v>224</v>
+      </c>
+      <c r="J4" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="K4" s="32" t="s">
         <v>225</v>
-      </c>
-      <c r="C4" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="32" t="s">
-        <v>226</v>
-      </c>
-      <c r="G4" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="32" t="s">
-        <v>227</v>
-      </c>
-      <c r="J4" s="33" t="s">
-        <v>89</v>
-      </c>
-      <c r="K4" s="32" t="s">
-        <v>228</v>
       </c>
       <c r="L4" s="32">
         <v>14.87</v>
       </c>
       <c r="M4" s="41" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N4" s="41" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O4" s="34"/>
       <c r="P4" s="34"/>
@@ -1599,31 +1605,31 @@
         <v>2015</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" s="36" t="s">
-        <v>7</v>
+        <v>254</v>
       </c>
       <c r="E5" s="36" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5" s="36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G5" s="36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I5" s="36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J5" s="37" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K5" s="36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M5" s="42">
         <v>-0.09</v>
@@ -1645,37 +1651,37 @@
         <v>2015</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>7</v>
+        <v>254</v>
       </c>
       <c r="E6" s="36" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F6" s="36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G6" s="36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I6" s="36" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J6" s="37" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K6" s="36" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="M6" s="42" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N6" s="42" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O6" s="38">
         <v>0</v>
@@ -1698,37 +1704,37 @@
         <v>2015</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="36" t="s">
-        <v>7</v>
+        <v>254</v>
       </c>
       <c r="E7" s="36" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F7" s="36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G7" s="36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I7" s="36" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J7" s="37" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K7" s="36" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="M7" s="42" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N7" s="42" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O7" s="38">
         <v>0.32</v>
@@ -1751,37 +1757,37 @@
         <v>2015</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" s="36" t="s">
-        <v>7</v>
+        <v>254</v>
       </c>
       <c r="E8" s="36" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F8" s="36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G8" s="36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I8" s="36" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J8" s="37" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K8" s="36" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="M8" s="42" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N8" s="42" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O8" s="38">
         <v>0.32</v>
@@ -1804,43 +1810,43 @@
         <v>2015</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" s="36" t="s">
-        <v>7</v>
+        <v>254</v>
       </c>
       <c r="E9" s="36" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F9" s="36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G9" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="36" t="s">
-        <v>12</v>
-      </c>
       <c r="I9" s="36" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J9" s="37" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K9" s="36" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="L9" s="51">
         <v>15.1</v>
       </c>
       <c r="M9" s="42" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N9" s="42" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O9" s="38">
         <v>0.32300000000000001</v>
@@ -1863,40 +1869,40 @@
         <v>2015</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" s="36" t="s">
-        <v>7</v>
+        <v>254</v>
       </c>
       <c r="E10" s="36" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F10" s="36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G10" s="36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I10" s="36" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J10" s="37" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K10" s="36" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="L10" s="36">
         <v>13.73</v>
       </c>
       <c r="M10" s="42" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N10" s="42" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O10" s="38">
         <v>0.32300000000000001</v>
@@ -1919,31 +1925,31 @@
         <v>2023</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>7</v>
+        <v>253</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J11" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M11" s="43">
         <v>-0.44</v>
@@ -1965,31 +1971,31 @@
         <v>2023</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="F12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M12" s="43">
         <v>-1.25</v>
@@ -2011,31 +2017,31 @@
         <v>2023</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I13" s="1" t="s">
+      <c r="J13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K13" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="J13" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="M13" s="43">
         <v>-1.25</v>
@@ -2057,31 +2063,31 @@
         <v>2023</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K14" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J14" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="M14" s="43">
         <v>-1.25</v>
@@ -2103,31 +2109,31 @@
         <v>2023</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>7</v>
+        <v>253</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M15" s="43">
         <v>-1.25</v>
@@ -2149,31 +2155,31 @@
         <v>2023</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>7</v>
+        <v>253</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J16" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M16" s="43">
         <v>-1.25</v>
@@ -2195,31 +2201,31 @@
         <v>2023</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>7</v>
+        <v>253</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J17" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M17" s="43">
         <v>-1.25</v>
@@ -2241,31 +2247,31 @@
         <v>2023</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>7</v>
+        <v>253</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J18" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="K18" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="M18" s="43">
         <v>-1.25</v>
@@ -2287,31 +2293,31 @@
         <v>2023</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I19" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I19" s="1" t="s">
+      <c r="J19" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="K19" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="J19" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="M19" s="43">
         <v>-1.25</v>
@@ -2333,31 +2339,31 @@
         <v>2023</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="J20" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M20" s="43">
         <v>-1.25</v>
@@ -2379,31 +2385,31 @@
         <v>2023</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J21" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="K21" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J21" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="M21" s="43">
         <v>-1.25</v>
@@ -2425,31 +2431,31 @@
         <v>2023</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I22" s="1" t="s">
+      <c r="J22" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="K22" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="J22" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="M22" s="43">
         <v>-1.25</v>
@@ -2471,31 +2477,31 @@
         <v>2023</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="F23" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J23" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M23" s="43">
         <v>-1.25</v>
@@ -2517,31 +2523,31 @@
         <v>2023</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J24" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="K24" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="J24" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="M24" s="43">
         <v>-1.25</v>
@@ -2563,31 +2569,31 @@
         <v>2023</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>7</v>
+        <v>253</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M25" s="43">
         <v>-1.25</v>
@@ -2609,31 +2615,31 @@
         <v>2023</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>7</v>
+        <v>253</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M26" s="43">
         <v>-1.25</v>
@@ -2655,31 +2661,31 @@
         <v>2023</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="1" t="s">
+      <c r="F27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I27" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I27" s="1" t="s">
+      <c r="J27" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="K27" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="J27" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="M27" s="43">
         <v>-1.25</v>
@@ -2701,31 +2707,31 @@
         <v>2023</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E28" s="1" t="s">
+      <c r="F28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I28" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="J28" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M28" s="43">
         <v>-1.25</v>
@@ -2747,31 +2753,31 @@
         <v>2023</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>7</v>
+        <v>253</v>
       </c>
       <c r="E29" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J29" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="K29" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="J29" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="O29" s="6">
         <v>1.27</v>
@@ -2791,31 +2797,31 @@
         <v>2023</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>7</v>
+        <v>253</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M30" s="43">
         <v>-1.25</v>
@@ -2840,31 +2846,31 @@
         <v>2023</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E31" s="1" t="s">
+      <c r="F31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J31" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="F31" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="J31" s="10" t="s">
+      <c r="K31" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="K31" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="O31" s="6">
         <v>1.27</v>
@@ -2887,31 +2893,31 @@
         <v>2023</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>7</v>
+        <v>253</v>
       </c>
       <c r="E32" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J32" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="K32" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="J32" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="K32" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="M32" s="43">
         <v>-1.25</v>
@@ -2934,40 +2940,40 @@
         <v>2023</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E33" s="1" t="s">
+      <c r="F33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J33" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="K33" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="J33" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="K33" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="L33" s="1">
         <v>17.77</v>
       </c>
       <c r="M33" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N33" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O33" s="6">
         <v>1.27</v>
@@ -2990,40 +2996,40 @@
         <v>2023</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>7</v>
+        <v>253</v>
       </c>
       <c r="E34" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J34" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="K34" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="J34" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="K34" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="L34" s="1">
         <v>17.77</v>
       </c>
       <c r="M34" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N34" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O34" s="1">
         <v>0.64</v>
@@ -3046,40 +3052,40 @@
         <v>2023</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>7</v>
+        <v>253</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L35" s="1">
         <v>17.77</v>
       </c>
       <c r="M35" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N35" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O35" s="1">
         <v>0.95</v>
@@ -3102,40 +3108,40 @@
         <v>2023</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>7</v>
+        <v>253</v>
       </c>
       <c r="E36" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J36" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="K36" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="J36" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="K36" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="L36" s="1">
         <v>17.77</v>
       </c>
       <c r="M36" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N36" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O36" s="1">
         <v>0.95</v>
@@ -3158,40 +3164,40 @@
         <v>2023</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>7</v>
+        <v>253</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J37" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="L37" s="1">
         <v>17.77</v>
       </c>
       <c r="M37" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N37" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O37" s="1">
         <v>0.95</v>
@@ -3214,40 +3220,40 @@
         <v>2023</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>7</v>
+        <v>253</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J38" s="10" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="L38" s="1">
         <v>17.77</v>
       </c>
       <c r="M38" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N38" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O38" s="1">
         <v>0.39</v>
@@ -3270,40 +3276,40 @@
         <v>2023</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>7</v>
+        <v>253</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J39" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="L39" s="1">
         <v>17.77</v>
       </c>
       <c r="M39" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N39" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O39" s="1">
         <v>0.77</v>
@@ -3326,40 +3332,40 @@
         <v>2023</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>7</v>
+        <v>253</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="L40" s="1">
         <v>17.77</v>
       </c>
       <c r="M40" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N40" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O40" s="1">
         <v>0.94</v>
@@ -3382,40 +3388,40 @@
         <v>2023</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>7</v>
+        <v>253</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="J41" s="10" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="L41" s="1">
         <v>17.77</v>
       </c>
       <c r="M41" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N41" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O41" s="1">
         <v>0.94</v>
@@ -3438,40 +3444,40 @@
         <v>2023</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>7</v>
+        <v>253</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="J42" s="10" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="L42" s="1">
         <v>17.77</v>
       </c>
       <c r="M42" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N42" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O42" s="1">
         <v>0.94</v>
@@ -3494,40 +3500,40 @@
         <v>2023</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>7</v>
+        <v>253</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="J43" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="L43" s="1">
         <v>17.77</v>
       </c>
       <c r="M43" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N43" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O43" s="1">
         <v>0.94</v>
@@ -3550,40 +3556,40 @@
         <v>2023</v>
       </c>
       <c r="B44" s="50" t="s">
+        <v>170</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J44" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K44" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I44" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="J44" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="K44" s="1" t="s">
-        <v>176</v>
       </c>
       <c r="L44" s="1">
         <v>17.77</v>
       </c>
       <c r="M44" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N44" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O44" s="1">
         <v>0.94</v>
@@ -3606,40 +3612,40 @@
         <v>2023</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>7</v>
+        <v>253</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I45" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J45" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K45" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="J45" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="K45" s="1" t="s">
-        <v>178</v>
       </c>
       <c r="L45" s="1">
         <v>17.77</v>
       </c>
       <c r="M45" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N45" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O45" s="1">
         <v>0.99</v>
@@ -3662,40 +3668,40 @@
         <v>2023</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>7</v>
+        <v>253</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="J46" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="L46" s="1">
         <v>17.77</v>
       </c>
       <c r="M46" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N46" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O46" s="1">
         <v>0.99</v>
@@ -3718,40 +3724,40 @@
         <v>2023</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>7</v>
+        <v>253</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="J47" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="L47" s="1">
         <v>17.77</v>
       </c>
       <c r="M47" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N47" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O47" s="1">
         <v>1.04</v>
@@ -3774,40 +3780,40 @@
         <v>2023</v>
       </c>
       <c r="B48" s="50" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>7</v>
+        <v>253</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="J48" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="L48" s="1">
         <v>17.77</v>
       </c>
       <c r="M48" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N48" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O48" s="1">
         <v>0.99</v>
@@ -3830,40 +3836,40 @@
         <v>2023</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>7</v>
+        <v>253</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="J49" s="10" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="L49" s="1">
         <v>17.77</v>
       </c>
       <c r="M49" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N49" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O49" s="1">
         <v>1.04</v>
@@ -3886,40 +3892,40 @@
         <v>2023</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>7</v>
+        <v>253</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="J50" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="L50" s="1">
         <v>17.77</v>
       </c>
       <c r="M50" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N50" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O50" s="1">
         <v>0.99</v>
@@ -3942,40 +3948,40 @@
         <v>2023</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>7</v>
+        <v>253</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="J51" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="L51" s="1">
         <v>17.77</v>
       </c>
       <c r="M51" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N51" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O51" s="1">
         <v>1.04</v>
@@ -3998,40 +4004,40 @@
         <v>2023</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>7</v>
+        <v>253</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="J52" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="L52" s="1">
         <v>17.77</v>
       </c>
       <c r="M52" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N52" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O52" s="1">
         <v>0.99</v>
@@ -4054,40 +4060,40 @@
         <v>2023</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>7</v>
+        <v>253</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="J53" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="L53" s="1">
         <v>17.77</v>
       </c>
       <c r="M53" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N53" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O53" s="1">
         <v>0.99</v>
@@ -4110,40 +4116,40 @@
         <v>2023</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>7</v>
+        <v>253</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="J54" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="L54" s="1">
         <v>16.45</v>
       </c>
       <c r="M54" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N54" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O54" s="1">
         <v>0.99</v>
@@ -4166,40 +4172,40 @@
         <v>2023</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>7</v>
+        <v>253</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="J55" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="L55" s="1">
         <v>16.61</v>
       </c>
       <c r="M55" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N55" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O55" s="1">
         <v>0.99</v>
@@ -4222,43 +4228,43 @@
         <v>2023</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>7</v>
+        <v>253</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G56" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H56" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H56" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="I56" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="J56" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="L56" s="1">
         <v>16.61</v>
       </c>
       <c r="M56" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N56" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O56" s="1">
         <v>1.04</v>
@@ -4281,25 +4287,25 @@
         <v>2025</v>
       </c>
       <c r="B57" s="28" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C57" s="28" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D57" s="28" t="s">
-        <v>103</v>
+        <v>252</v>
       </c>
       <c r="E57" s="28" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H57" s="28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I57" s="28" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J57" s="29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M57" s="45"/>
       <c r="N57" s="45"/>
@@ -4312,34 +4318,34 @@
         <v>2035</v>
       </c>
       <c r="B58" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="C58" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="D58" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="E58" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="C58" s="15" t="s">
+      <c r="F58" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="G58" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="H58" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="I58" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="D58" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="E58" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="F58" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="G58" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="H58" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="I58" s="15" t="s">
-        <v>118</v>
-      </c>
       <c r="J58" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K58" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="L58" s="15">
         <v>15.85</v>
@@ -4351,19 +4357,19 @@
         <v>0</v>
       </c>
       <c r="O58" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="P58" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="Q58" s="17" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="R58" s="17" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="S58" s="17" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="59" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
@@ -4371,40 +4377,40 @@
         <v>2035</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D59" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="E59" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="F59" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G59" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I59" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="E59" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="F59" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G59" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I59" s="12" t="s">
-        <v>105</v>
-      </c>
       <c r="J59" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K59" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="L59" s="12">
         <v>15.85</v>
       </c>
       <c r="M59" s="47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N59" s="47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O59" s="14">
         <v>1.27</v>
@@ -4427,40 +4433,40 @@
         <v>2035</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D60" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="E60" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="F60" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G60" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I60" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="E60" s="12" t="s">
+      <c r="J60" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="K60" s="12" t="s">
         <v>107</v>
-      </c>
-      <c r="F60" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G60" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I60" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="J60" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="K60" s="12" t="s">
-        <v>109</v>
       </c>
       <c r="L60" s="12">
         <v>18.64</v>
       </c>
       <c r="M60" s="47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N60" s="47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O60" s="14">
         <v>1.27</v>
@@ -4483,40 +4489,40 @@
         <v>2035</v>
       </c>
       <c r="B61" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D61" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="E61" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="F61" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G61" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I61" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="E61" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="F61" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G61" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I61" s="12" t="s">
-        <v>105</v>
-      </c>
       <c r="J61" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K61" s="12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="L61" s="12">
         <v>18.64</v>
       </c>
       <c r="M61" s="47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N61" s="47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O61" s="14">
         <v>1.27</v>
@@ -4539,40 +4545,40 @@
         <v>2035</v>
       </c>
       <c r="B62" s="12" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D62" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="E62" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="F62" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G62" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I62" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="E62" s="12" t="s">
+      <c r="J62" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="K62" s="12" t="s">
         <v>124</v>
-      </c>
-      <c r="F62" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G62" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I62" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="J62" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="K62" s="12" t="s">
-        <v>127</v>
       </c>
       <c r="L62" s="12">
         <v>18.64</v>
       </c>
       <c r="M62" s="47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N62" s="47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O62" s="12">
         <v>0.95</v>
@@ -4595,40 +4601,40 @@
         <v>2035</v>
       </c>
       <c r="B63" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C63" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D63" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="E63" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="F63" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G63" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I63" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="J63" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="K63" s="12" t="s">
         <v>123</v>
-      </c>
-      <c r="C63" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D63" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="E63" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="F63" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G63" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I63" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="J63" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="K63" s="12" t="s">
-        <v>126</v>
       </c>
       <c r="L63" s="12">
         <v>18.64</v>
       </c>
       <c r="M63" s="47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N63" s="47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O63" s="12">
         <v>0.95</v>
@@ -4651,40 +4657,40 @@
         <v>2035</v>
       </c>
       <c r="B64" s="12" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D64" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="E64" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="F64" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G64" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I64" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="E64" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="F64" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G64" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I64" s="12" t="s">
-        <v>105</v>
-      </c>
       <c r="J64" s="13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K64" s="12" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L64" s="12">
         <v>18.64</v>
       </c>
       <c r="M64" s="47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N64" s="47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O64" s="12">
         <v>0.95</v>
@@ -4707,40 +4713,40 @@
         <v>2035</v>
       </c>
       <c r="B65" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="C65" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D65" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="E65" s="12" t="s">
         <v>210</v>
       </c>
-      <c r="C65" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D65" s="12" t="s">
+      <c r="F65" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G65" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I65" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="E65" s="12" t="s">
-        <v>213</v>
-      </c>
-      <c r="F65" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G65" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I65" s="12" t="s">
-        <v>105</v>
-      </c>
       <c r="J65" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K65" s="12" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L65" s="12">
         <v>18.64</v>
       </c>
       <c r="M65" s="47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N65" s="47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O65" s="12">
         <v>0.95</v>
@@ -4763,40 +4769,40 @@
         <v>2035</v>
       </c>
       <c r="B66" s="12" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C66" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D66" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="E66" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="F66" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="G66" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="I66" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="E66" s="12" t="s">
-        <v>211</v>
-      </c>
-      <c r="F66" s="12" t="s">
-        <v>214</v>
-      </c>
-      <c r="G66" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="I66" s="12" t="s">
-        <v>105</v>
-      </c>
       <c r="J66" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K66" s="12" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="L66" s="12">
         <v>18.64</v>
       </c>
       <c r="M66" s="47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N66" s="47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O66" s="12">
         <v>0.95</v>
@@ -4819,43 +4825,43 @@
         <v>2035</v>
       </c>
       <c r="B67" s="12" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C67" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D67" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="E67" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="F67" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="G67" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="H67" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I67" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="E67" s="12" t="s">
-        <v>229</v>
-      </c>
-      <c r="F67" s="12" t="s">
-        <v>214</v>
-      </c>
-      <c r="G67" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="H67" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I67" s="12" t="s">
-        <v>105</v>
-      </c>
       <c r="J67" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K67" s="12" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="L67" s="12">
         <v>20.55</v>
       </c>
       <c r="M67" s="47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N67" s="47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O67" s="12">
         <v>0.99</v>
@@ -4878,43 +4884,43 @@
         <v>2035</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D68" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="E68" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="F68" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="G68" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="H68" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I68" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="E68" s="12" t="s">
-        <v>233</v>
-      </c>
-      <c r="F68" s="12" t="s">
-        <v>214</v>
-      </c>
-      <c r="G68" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="H68" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I68" s="12" t="s">
-        <v>105</v>
-      </c>
       <c r="J68" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K68" s="12" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="L68" s="12">
         <v>20.55</v>
       </c>
       <c r="M68" s="47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N68" s="47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O68" s="12">
         <v>0.99</v>
@@ -4937,43 +4943,43 @@
         <v>2035</v>
       </c>
       <c r="B69" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="C69" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D69" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="E69" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="F69" s="53" t="s">
+        <v>234</v>
+      </c>
+      <c r="G69" s="12" t="s">
         <v>235</v>
       </c>
-      <c r="C69" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D69" s="12" t="s">
+      <c r="H69" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I69" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="E69" s="12" t="s">
+      <c r="J69" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="K69" s="12" t="s">
         <v>236</v>
-      </c>
-      <c r="F69" s="53" t="s">
-        <v>237</v>
-      </c>
-      <c r="G69" s="12" t="s">
-        <v>238</v>
-      </c>
-      <c r="H69" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I69" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="J69" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="K69" s="12" t="s">
-        <v>239</v>
       </c>
       <c r="L69" s="12">
         <v>20.55</v>
       </c>
       <c r="M69" s="47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N69" s="47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O69" s="12">
         <v>0.99</v>
@@ -4996,43 +5002,43 @@
         <v>2035</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D70" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="E70" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="F70" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="G70" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="H70" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I70" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="E70" s="12" t="s">
-        <v>241</v>
-      </c>
-      <c r="F70" s="12" t="s">
-        <v>214</v>
-      </c>
-      <c r="G70" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="H70" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I70" s="12" t="s">
-        <v>105</v>
-      </c>
       <c r="J70" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K70" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="L70" s="53">
         <v>15.85</v>
       </c>
       <c r="M70" s="47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N70" s="47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O70" s="12">
         <v>0.99</v>
@@ -5055,43 +5061,43 @@
         <v>2035</v>
       </c>
       <c r="B71" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="C71" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D71" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="E71" s="12" t="s">
         <v>249</v>
       </c>
-      <c r="C71" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D71" s="12" t="s">
+      <c r="F71" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="G71" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="H71" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I71" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="E71" s="12" t="s">
-        <v>252</v>
-      </c>
-      <c r="F71" s="12" t="s">
-        <v>214</v>
-      </c>
-      <c r="G71" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="H71" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I71" s="12" t="s">
-        <v>105</v>
-      </c>
       <c r="J71" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K71" s="12" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="L71" s="12">
         <v>20.55</v>
       </c>
       <c r="M71" s="47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N71" s="47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O71" s="12">
         <v>0.99</v>
@@ -5114,43 +5120,43 @@
         <v>2035</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C72" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D72" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="E72" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="F72" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="G72" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="H72" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I72" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="E72" s="12" t="s">
-        <v>244</v>
-      </c>
-      <c r="F72" s="12" t="s">
-        <v>214</v>
-      </c>
-      <c r="G72" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="H72" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I72" s="12" t="s">
-        <v>105</v>
-      </c>
       <c r="J72" s="13" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K72" s="12" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="L72" s="12">
         <v>20.55</v>
       </c>
       <c r="M72" s="47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N72" s="47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O72" s="12">
         <v>0.99</v>
@@ -5173,40 +5179,40 @@
         <v>2035</v>
       </c>
       <c r="B73" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C73" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D73" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="E73" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="F73" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="G73" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="I73" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="E73" s="12" t="s">
-        <v>247</v>
-      </c>
-      <c r="F73" s="12" t="s">
-        <v>214</v>
-      </c>
-      <c r="G73" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="I73" s="12" t="s">
-        <v>105</v>
-      </c>
       <c r="J73" s="13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K73" s="12" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="L73" s="12">
         <v>20.55</v>
       </c>
       <c r="M73" s="47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N73" s="47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O73" s="53"/>
       <c r="P73" s="53"/>
@@ -5225,31 +5231,31 @@
         <v>2050</v>
       </c>
       <c r="B74" s="24" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C74" s="24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D74" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="E74" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="F74" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="G74" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="E74" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="F74" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="G74" s="25" t="s">
-        <v>119</v>
-      </c>
       <c r="I74" s="24" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="J74" s="26" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K74" s="24" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="L74" s="24">
         <v>17.440000000000001</v>
@@ -5261,19 +5267,19 @@
         <v>0</v>
       </c>
       <c r="O74" s="24" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="P74" s="24" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="Q74" s="27" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="R74" s="27" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="S74" s="27" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add 2035 IPA 11 and promote 2005 v2 to current
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ECF58FB-9221-4F51-A921-98F7E7B38FEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAAE4C42-491B-40A2-9FEE-150717BA8210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1695" yWindow="825" windowWidth="20220" windowHeight="11250" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
+    <workbookView xWindow="765" yWindow="1485" windowWidth="14700" windowHeight="11790" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelRuns" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="265">
   <si>
     <t>year</t>
   </si>
@@ -822,6 +822,15 @@
   </si>
   <si>
     <t>https://app.asana.com/0/1204085012544660/1205973396668369/f</t>
+  </si>
+  <si>
+    <t>2035_TM160_IPA_11</t>
+  </si>
+  <si>
+    <t>IPA with EN7 fixed and bike mode share adjusted</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1206021318810361/f</t>
   </si>
 </sst>
 </file>
@@ -1398,13 +1407,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9564CC59-3725-4FDA-8BF2-0F68CB1B6F5A}">
-  <dimension ref="A1:S76"/>
+  <dimension ref="A1:S77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F52" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B74" sqref="B74"/>
+      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1588,6 +1597,9 @@
       <c r="G4" s="32" t="s">
         <v>10</v>
       </c>
+      <c r="H4" s="32" t="s">
+        <v>11</v>
+      </c>
       <c r="I4" s="32" t="s">
         <v>224</v>
       </c>
@@ -5356,59 +5368,118 @@
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="24">
+    <row r="76" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B76" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="C76" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D76" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="E76" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="F76" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="G76" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="H76" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I76" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="J76" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K76" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="L76" s="12">
+        <v>20.55</v>
+      </c>
+      <c r="M76" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="N76" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="O76" s="12">
+        <v>0.87</v>
+      </c>
+      <c r="P76" s="12">
+        <v>0.78</v>
+      </c>
+      <c r="Q76" s="14">
+        <v>100</v>
+      </c>
+      <c r="R76" s="14">
+        <v>0</v>
+      </c>
+      <c r="S76" s="14">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="24">
         <v>2050</v>
       </c>
-      <c r="B76" s="24" t="s">
+      <c r="B77" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="C76" s="24" t="s">
+      <c r="C77" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="D76" s="24" t="s">
+      <c r="D77" s="24" t="s">
         <v>251</v>
       </c>
-      <c r="E76" s="24" t="s">
+      <c r="E77" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="F76" s="24" t="s">
+      <c r="F77" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="G76" s="25" t="s">
+      <c r="G77" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="I76" s="24" t="s">
+      <c r="I77" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="J76" s="26" t="s">
+      <c r="J77" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="K76" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="L76" s="24">
+      <c r="K77" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="L77" s="24">
         <v>17.440000000000001</v>
       </c>
-      <c r="M76" s="48">
+      <c r="M77" s="48">
         <v>-0.33</v>
       </c>
-      <c r="N76" s="48">
-        <v>0</v>
-      </c>
-      <c r="O76" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="P76" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q76" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="R76" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="S76" s="27" t="s">
+      <c r="N77" s="48">
+        <v>0</v>
+      </c>
+      <c r="O77" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="P77" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q77" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="R77" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="S77" s="27" t="s">
         <v>109</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove current from RTP2021 2005 run
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAAE4C42-491B-40A2-9FEE-150717BA8210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B228A462-C4AD-4FEE-8CF9-A4BB3652A81A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="765" yWindow="1485" windowWidth="14700" windowHeight="11790" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
+    <workbookView xWindow="780" yWindow="1500" windowWidth="14700" windowHeight="11790" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelRuns" sheetId="1" r:id="rId1"/>
@@ -1410,10 +1410,10 @@
   <dimension ref="A1:S77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F55" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomRight" activeCell="H75" sqref="H75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1511,9 +1511,7 @@
       </c>
       <c r="F2" s="20"/>
       <c r="G2" s="20"/>
-      <c r="H2" s="20" t="s">
-        <v>11</v>
-      </c>
+      <c r="H2" s="20"/>
       <c r="J2" s="22"/>
       <c r="M2" s="40"/>
       <c r="N2" s="40"/>
@@ -4927,6 +4925,9 @@
       </c>
       <c r="G68" s="12" t="s">
         <v>116</v>
+      </c>
+      <c r="H68" s="12" t="s">
+        <v>11</v>
       </c>
       <c r="I68" s="12" t="s">
         <v>103</v>

</xml_diff>

<commit_message>
Fix run name typo
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B8A945-1263-470B-9A31-2E8DAC880C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770CA3DD-A7A6-49EA-BDC6-41D0287EA1F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="28800" windowHeight="11385" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
@@ -812,9 +812,6 @@
     <t>https://app.asana.com/0/1204085012544660/1206015047138571/f</t>
   </si>
   <si>
-    <t>2035_TM160_IPA_10_PBA50wfh</t>
-  </si>
-  <si>
     <t>2035_TM160_IPA_10_plusEN7</t>
   </si>
   <si>
@@ -831,6 +828,9 @@
   </si>
   <si>
     <t>https://app.asana.com/0/1204085012544660/1206021318810361/f</t>
+  </si>
+  <si>
+    <t>2035_TM160_IPA_11_PBA50wfh</t>
   </si>
 </sst>
 </file>
@@ -1413,7 +1413,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="F55" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B75" sqref="B75"/>
+      <selection pane="bottomRight" activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5263,7 +5263,7 @@
         <v>2035</v>
       </c>
       <c r="B74" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C74" s="12" t="s">
         <v>17</v>
@@ -5272,7 +5272,7 @@
         <v>250</v>
       </c>
       <c r="E74" s="12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F74" s="12" t="s">
         <v>211</v>
@@ -5290,7 +5290,7 @@
         <v>43</v>
       </c>
       <c r="K74" s="12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="L74" s="12">
         <v>20.55</v>
@@ -5322,7 +5322,7 @@
         <v>2035</v>
       </c>
       <c r="B75" s="12" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="C75" s="12" t="s">
         <v>17</v>
@@ -5381,7 +5381,7 @@
         <v>2035</v>
       </c>
       <c r="B76" s="12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C76" s="12" t="s">
         <v>17</v>
@@ -5390,7 +5390,7 @@
         <v>250</v>
       </c>
       <c r="E76" s="12" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F76" s="12" t="s">
         <v>211</v>
@@ -5408,7 +5408,7 @@
         <v>43</v>
       </c>
       <c r="K76" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="L76" s="12">
         <v>20.55</v>

</xml_diff>

<commit_message>
Add 2005_TM160_IPA_03, 2035_TM160_IPA_11_network2023 and 2035_TM160_IPA_12
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770CA3DD-A7A6-49EA-BDC6-41D0287EA1F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87C0D65-8C37-46A9-B71D-A6F13079136C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="28800" windowHeight="11385" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
+    <workbookView xWindow="2295" yWindow="885" windowWidth="28800" windowHeight="14085" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelRuns" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="276">
   <si>
     <t>year</t>
   </si>
@@ -831,6 +831,39 @@
   </si>
   <si>
     <t>2035_TM160_IPA_11_PBA50wfh</t>
+  </si>
+  <si>
+    <t>2035_TM160_IPA_12</t>
+  </si>
+  <si>
+    <t>IPA with air passenger fix</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1206074168414015/f</t>
+  </si>
+  <si>
+    <t>2035_TM160_IPA_11_network2023</t>
+  </si>
+  <si>
+    <t>IPA v11 with 2023 networks</t>
+  </si>
+  <si>
+    <t>M:\Application\Model One\RTP2025\INPUT_DEVELOPMENT\Networks\BlueprintNetworks_v12\net_2023_Blueprint</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1206031684822718/f</t>
+  </si>
+  <si>
+    <t>2005_TM160_IPA_03</t>
+  </si>
+  <si>
+    <t>TM160 2005 run with air passenger trips fixed</t>
+  </si>
+  <si>
+    <t>2005_v01</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1206071846636750/f</t>
   </si>
 </sst>
 </file>
@@ -1407,13 +1440,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9564CC59-3725-4FDA-8BF2-0F68CB1B6F5A}">
-  <dimension ref="A1:S77"/>
+  <dimension ref="A1:S80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F55" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C59" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B76" sqref="B76"/>
+      <selection pane="bottomRight" activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1592,6 +1625,9 @@
       <c r="E4" s="32" t="s">
         <v>223</v>
       </c>
+      <c r="F4" s="32" t="s">
+        <v>274</v>
+      </c>
       <c r="G4" s="32" t="s">
         <v>10</v>
       </c>
@@ -1628,49 +1664,55 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="35">
-        <v>2015</v>
-      </c>
-      <c r="B5" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="36" t="s">
-        <v>253</v>
-      </c>
-      <c r="E5" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="K5" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="M5" s="42">
-        <v>-0.09</v>
-      </c>
-      <c r="N5" s="42">
-        <v>0.9</v>
-      </c>
-      <c r="O5" s="38"/>
-      <c r="P5" s="38"/>
-      <c r="Q5" s="38">
-        <v>0</v>
-      </c>
-      <c r="R5" s="38">
+    <row r="5" spans="1:19" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="31">
+        <v>2005</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>272</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>254</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>273</v>
+      </c>
+      <c r="F5" s="32" t="s">
+        <v>274</v>
+      </c>
+      <c r="G5" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="32" t="s">
+        <v>224</v>
+      </c>
+      <c r="J5" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="K5" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="L5" s="32">
+        <v>14.87</v>
+      </c>
+      <c r="M5" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="N5" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="O5" s="34"/>
+      <c r="P5" s="34"/>
+      <c r="Q5" s="34">
+        <v>0</v>
+      </c>
+      <c r="R5" s="34">
+        <v>0</v>
+      </c>
+      <c r="S5" s="34">
         <v>0</v>
       </c>
     </row>
@@ -1679,7 +1721,7 @@
         <v>2015</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>145</v>
+        <v>8</v>
       </c>
       <c r="C6" s="36" t="s">
         <v>17</v>
@@ -1688,7 +1730,7 @@
         <v>253</v>
       </c>
       <c r="E6" s="36" t="s">
-        <v>149</v>
+        <v>19</v>
       </c>
       <c r="F6" s="36" t="s">
         <v>9</v>
@@ -1697,33 +1739,26 @@
         <v>10</v>
       </c>
       <c r="I6" s="36" t="s">
-        <v>146</v>
+        <v>13</v>
       </c>
       <c r="J6" s="37" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="K6" s="36" t="s">
-        <v>147</v>
-      </c>
-      <c r="M6" s="42" t="s">
-        <v>109</v>
-      </c>
-      <c r="N6" s="42" t="s">
-        <v>109</v>
-      </c>
-      <c r="O6" s="38">
-        <v>0</v>
-      </c>
-      <c r="P6" s="38">
-        <v>0</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="M6" s="42">
+        <v>-0.09</v>
+      </c>
+      <c r="N6" s="42">
+        <v>0.9</v>
+      </c>
+      <c r="O6" s="38"/>
+      <c r="P6" s="38"/>
       <c r="Q6" s="38">
         <v>0</v>
       </c>
       <c r="R6" s="38">
-        <v>0</v>
-      </c>
-      <c r="S6" s="38">
         <v>0</v>
       </c>
     </row>
@@ -1732,7 +1767,7 @@
         <v>2015</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C7" s="36" t="s">
         <v>17</v>
@@ -1741,7 +1776,7 @@
         <v>253</v>
       </c>
       <c r="E7" s="36" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="F7" s="36" t="s">
         <v>9</v>
@@ -1765,10 +1800,10 @@
         <v>109</v>
       </c>
       <c r="O7" s="38">
-        <v>0.32</v>
+        <v>0</v>
       </c>
       <c r="P7" s="38">
-        <v>0.28000000000000003</v>
+        <v>0</v>
       </c>
       <c r="Q7" s="38">
         <v>0</v>
@@ -1785,7 +1820,7 @@
         <v>2015</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C8" s="36" t="s">
         <v>17</v>
@@ -1838,7 +1873,7 @@
         <v>2015</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C9" s="36" t="s">
         <v>17</v>
@@ -1847,28 +1882,22 @@
         <v>253</v>
       </c>
       <c r="E9" s="36" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F9" s="36" t="s">
         <v>9</v>
       </c>
       <c r="G9" s="36" t="s">
         <v>10</v>
-      </c>
-      <c r="H9" s="36" t="s">
-        <v>11</v>
       </c>
       <c r="I9" s="36" t="s">
         <v>146</v>
       </c>
       <c r="J9" s="37" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="K9" s="36" t="s">
-        <v>158</v>
-      </c>
-      <c r="L9" s="51">
-        <v>15.1</v>
+        <v>147</v>
       </c>
       <c r="M9" s="42" t="s">
         <v>109</v>
@@ -1877,10 +1906,10 @@
         <v>109</v>
       </c>
       <c r="O9" s="38">
-        <v>0.32300000000000001</v>
-      </c>
-      <c r="P9" s="49">
-        <v>0.83099999999999996</v>
+        <v>0.32</v>
+      </c>
+      <c r="P9" s="38">
+        <v>0.28000000000000003</v>
       </c>
       <c r="Q9" s="38">
         <v>0</v>
@@ -1897,7 +1926,7 @@
         <v>2015</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>213</v>
+        <v>156</v>
       </c>
       <c r="C10" s="36" t="s">
         <v>17</v>
@@ -1906,13 +1935,16 @@
         <v>253</v>
       </c>
       <c r="E10" s="36" t="s">
-        <v>215</v>
+        <v>157</v>
       </c>
       <c r="F10" s="36" t="s">
         <v>9</v>
       </c>
       <c r="G10" s="36" t="s">
         <v>10</v>
+      </c>
+      <c r="H10" s="36" t="s">
+        <v>11</v>
       </c>
       <c r="I10" s="36" t="s">
         <v>146</v>
@@ -1921,10 +1953,10 @@
         <v>16</v>
       </c>
       <c r="K10" s="36" t="s">
-        <v>214</v>
-      </c>
-      <c r="L10" s="36">
-        <v>13.73</v>
+        <v>158</v>
+      </c>
+      <c r="L10" s="51">
+        <v>15.1</v>
       </c>
       <c r="M10" s="42" t="s">
         <v>109</v>
@@ -1948,49 +1980,59 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>2023</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J11" s="9" t="s">
+    <row r="11" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="35">
+        <v>2015</v>
+      </c>
+      <c r="B11" s="36" t="s">
+        <v>213</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="36" t="s">
+        <v>253</v>
+      </c>
+      <c r="E11" s="36" t="s">
+        <v>215</v>
+      </c>
+      <c r="F11" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="36" t="s">
+        <v>146</v>
+      </c>
+      <c r="J11" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M11" s="43">
-        <v>-0.44</v>
-      </c>
-      <c r="N11" s="43">
-        <v>-0.23</v>
-      </c>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6">
-        <v>0</v>
-      </c>
-      <c r="R11" s="6">
+      <c r="K11" s="36" t="s">
+        <v>214</v>
+      </c>
+      <c r="L11" s="36">
+        <v>13.73</v>
+      </c>
+      <c r="M11" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="N11" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="O11" s="38">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="P11" s="49">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="Q11" s="38">
+        <v>0</v>
+      </c>
+      <c r="R11" s="38">
+        <v>0</v>
+      </c>
+      <c r="S11" s="38">
         <v>0</v>
       </c>
     </row>
@@ -1999,7 +2041,7 @@
         <v>2023</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>17</v>
@@ -2008,7 +2050,7 @@
         <v>252</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>9</v>
@@ -2023,18 +2065,18 @@
         <v>16</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M12" s="43">
-        <v>-1.25</v>
+        <v>-0.44</v>
       </c>
       <c r="N12" s="43">
-        <v>-0.75</v>
+        <v>-0.23</v>
       </c>
       <c r="O12" s="6"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="6">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="R12" s="6">
         <v>0</v>
@@ -2045,7 +2087,7 @@
         <v>2023</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>17</v>
@@ -2054,7 +2096,7 @@
         <v>252</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>9</v>
@@ -2063,13 +2105,13 @@
         <v>10</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="J13" s="9" t="s">
         <v>16</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="M13" s="43">
         <v>-1.25</v>
@@ -2080,10 +2122,10 @@
       <c r="O13" s="6"/>
       <c r="P13" s="6"/>
       <c r="Q13" s="6">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="R13" s="6">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
@@ -2091,7 +2133,7 @@
         <v>2023</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>17</v>
@@ -2100,7 +2142,7 @@
         <v>252</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>9</v>
@@ -2109,13 +2151,13 @@
         <v>10</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="J14" s="9" t="s">
         <v>16</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="M14" s="43">
         <v>-1.25</v>
@@ -2126,7 +2168,7 @@
       <c r="O14" s="6"/>
       <c r="P14" s="6"/>
       <c r="Q14" s="6">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="R14" s="6">
         <v>15</v>
@@ -2137,7 +2179,7 @@
         <v>2023</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>17</v>
@@ -2146,7 +2188,7 @@
         <v>252</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>9</v>
@@ -2161,7 +2203,7 @@
         <v>16</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="M15" s="43">
         <v>-1.25</v>
@@ -2171,10 +2213,10 @@
       </c>
       <c r="O15" s="6"/>
       <c r="P15" s="6"/>
-      <c r="Q15" s="11">
+      <c r="Q15" s="6">
         <v>75</v>
       </c>
-      <c r="R15" s="11">
+      <c r="R15" s="6">
         <v>15</v>
       </c>
     </row>
@@ -2183,7 +2225,7 @@
         <v>2023</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>17</v>
@@ -2192,7 +2234,7 @@
         <v>252</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>9</v>
@@ -2204,10 +2246,10 @@
         <v>32</v>
       </c>
       <c r="J16" s="9" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="M16" s="43">
         <v>-1.25</v>
@@ -2217,10 +2259,10 @@
       </c>
       <c r="O16" s="6"/>
       <c r="P16" s="6"/>
-      <c r="Q16" s="7">
-        <v>85</v>
-      </c>
-      <c r="R16" s="7">
+      <c r="Q16" s="11">
+        <v>75</v>
+      </c>
+      <c r="R16" s="11">
         <v>15</v>
       </c>
     </row>
@@ -2229,7 +2271,7 @@
         <v>2023</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>17</v>
@@ -2250,7 +2292,7 @@
         <v>32</v>
       </c>
       <c r="J17" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>45</v>
@@ -2264,7 +2306,7 @@
       <c r="O17" s="6"/>
       <c r="P17" s="6"/>
       <c r="Q17" s="7">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="R17" s="7">
         <v>15</v>
@@ -2275,7 +2317,7 @@
         <v>2023</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>17</v>
@@ -2296,7 +2338,7 @@
         <v>32</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>45</v>
@@ -2310,10 +2352,10 @@
       <c r="O18" s="6"/>
       <c r="P18" s="6"/>
       <c r="Q18" s="7">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="R18" s="7">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.2">
@@ -2321,7 +2363,7 @@
         <v>2023</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>17</v>
@@ -2330,7 +2372,7 @@
         <v>252</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>9</v>
@@ -2339,13 +2381,13 @@
         <v>10</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="J19" s="10" t="s">
-        <v>42</v>
+        <v>32</v>
+      </c>
+      <c r="J19" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="M19" s="43">
         <v>-1.25</v>
@@ -2367,7 +2409,7 @@
         <v>2023</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>17</v>
@@ -2376,7 +2418,7 @@
         <v>252</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>9</v>
@@ -2385,13 +2427,13 @@
         <v>10</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="J20" s="10" t="s">
         <v>42</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="M20" s="43">
         <v>-1.25</v>
@@ -2402,7 +2444,7 @@
       <c r="O20" s="6"/>
       <c r="P20" s="6"/>
       <c r="Q20" s="7">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="R20" s="7">
         <v>30</v>
@@ -2413,7 +2455,7 @@
         <v>2023</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>17</v>
@@ -2422,7 +2464,7 @@
         <v>252</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>9</v>
@@ -2434,7 +2476,7 @@
         <v>53</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>56</v>
@@ -2448,7 +2490,7 @@
       <c r="O21" s="6"/>
       <c r="P21" s="6"/>
       <c r="Q21" s="7">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="R21" s="7">
         <v>30</v>
@@ -2459,7 +2501,7 @@
         <v>2023</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>17</v>
@@ -2468,7 +2510,7 @@
         <v>252</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>9</v>
@@ -2477,13 +2519,13 @@
         <v>10</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="M22" s="43">
         <v>-1.25</v>
@@ -2494,10 +2536,10 @@
       <c r="O22" s="6"/>
       <c r="P22" s="6"/>
       <c r="Q22" s="7">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="R22" s="7">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.2">
@@ -2505,7 +2547,7 @@
         <v>2023</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>17</v>
@@ -2514,7 +2556,7 @@
         <v>252</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>9</v>
@@ -2529,7 +2571,7 @@
         <v>42</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="M23" s="43">
         <v>-1.25</v>
@@ -2540,10 +2582,10 @@
       <c r="O23" s="6"/>
       <c r="P23" s="6"/>
       <c r="Q23" s="7">
-        <v>300</v>
+        <v>180</v>
       </c>
       <c r="R23" s="7">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.2">
@@ -2551,7 +2593,7 @@
         <v>2023</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>17</v>
@@ -2586,7 +2628,7 @@
       <c r="O24" s="6"/>
       <c r="P24" s="6"/>
       <c r="Q24" s="7">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="R24" s="7">
         <v>5</v>
@@ -2597,7 +2639,7 @@
         <v>2023</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>17</v>
@@ -2632,7 +2674,7 @@
       <c r="O25" s="6"/>
       <c r="P25" s="6"/>
       <c r="Q25" s="7">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="R25" s="7">
         <v>5</v>
@@ -2643,7 +2685,7 @@
         <v>2023</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>17</v>
@@ -2652,7 +2694,7 @@
         <v>252</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>9</v>
@@ -2661,13 +2703,13 @@
         <v>10</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="J26" s="10" t="s">
         <v>42</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M26" s="43">
         <v>-1.25</v>
@@ -2678,10 +2720,10 @@
       <c r="O26" s="6"/>
       <c r="P26" s="6"/>
       <c r="Q26" s="7">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="R26" s="7">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.2">
@@ -2689,7 +2731,7 @@
         <v>2023</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>17</v>
@@ -2698,7 +2740,7 @@
         <v>252</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>9</v>
@@ -2707,13 +2749,13 @@
         <v>10</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="J27" s="10" t="s">
         <v>42</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="M27" s="43">
         <v>-1.25</v>
@@ -2735,7 +2777,7 @@
         <v>2023</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>17</v>
@@ -2744,7 +2786,7 @@
         <v>252</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>9</v>
@@ -2753,13 +2795,13 @@
         <v>10</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="J28" s="10" t="s">
         <v>42</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="M28" s="43">
         <v>-1.25</v>
@@ -2781,7 +2823,7 @@
         <v>2023</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>17</v>
@@ -2790,7 +2832,7 @@
         <v>252</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>9</v>
@@ -2802,17 +2844,19 @@
         <v>79</v>
       </c>
       <c r="J29" s="10" t="s">
-        <v>88</v>
+        <v>42</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="O29" s="6">
-        <v>1.27</v>
-      </c>
-      <c r="P29" s="6">
-        <v>1.1499999999999999</v>
-      </c>
+      <c r="M29" s="43">
+        <v>-1.25</v>
+      </c>
+      <c r="N29" s="43">
+        <v>-0.75</v>
+      </c>
+      <c r="O29" s="6"/>
+      <c r="P29" s="6"/>
       <c r="Q29" s="7">
         <v>120</v>
       </c>
@@ -2825,7 +2869,7 @@
         <v>2023</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>17</v>
@@ -2834,7 +2878,7 @@
         <v>252</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>9</v>
@@ -2846,27 +2890,22 @@
         <v>79</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>42</v>
+        <v>88</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="M30" s="43">
-        <v>-1.25</v>
-      </c>
-      <c r="N30" s="43">
-        <v>-0.75</v>
-      </c>
-      <c r="O30" s="6"/>
-      <c r="P30" s="6"/>
+        <v>81</v>
+      </c>
+      <c r="O30" s="6">
+        <v>1.27</v>
+      </c>
+      <c r="P30" s="6">
+        <v>1.1499999999999999</v>
+      </c>
       <c r="Q30" s="7">
         <v>120</v>
       </c>
       <c r="R30" s="7">
         <v>0</v>
-      </c>
-      <c r="S30" s="7">
-        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.2">
@@ -2874,7 +2913,7 @@
         <v>2023</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>17</v>
@@ -2895,17 +2934,19 @@
         <v>79</v>
       </c>
       <c r="J31" s="10" t="s">
-        <v>88</v>
+        <v>42</v>
       </c>
       <c r="K31" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="O31" s="6">
-        <v>1.27</v>
-      </c>
-      <c r="P31" s="6">
-        <v>1.1499999999999999</v>
-      </c>
+      <c r="M31" s="43">
+        <v>-1.25</v>
+      </c>
+      <c r="N31" s="43">
+        <v>-0.75</v>
+      </c>
+      <c r="O31" s="6"/>
+      <c r="P31" s="6"/>
       <c r="Q31" s="7">
         <v>120</v>
       </c>
@@ -2921,7 +2962,7 @@
         <v>2023</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>17</v>
@@ -2930,7 +2971,7 @@
         <v>252</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>9</v>
@@ -2942,16 +2983,16 @@
         <v>79</v>
       </c>
       <c r="J32" s="10" t="s">
-        <v>42</v>
+        <v>88</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="M32" s="43">
-        <v>-1.25</v>
-      </c>
-      <c r="N32" s="43">
-        <v>-0.75</v>
+        <v>89</v>
+      </c>
+      <c r="O32" s="6">
+        <v>1.27</v>
+      </c>
+      <c r="P32" s="6">
+        <v>1.1499999999999999</v>
       </c>
       <c r="Q32" s="7">
         <v>120</v>
@@ -2960,7 +3001,7 @@
         <v>0</v>
       </c>
       <c r="S32" s="7">
-        <v>45</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.2">
@@ -2968,7 +3009,7 @@
         <v>2023</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>17</v>
@@ -2989,25 +3030,16 @@
         <v>79</v>
       </c>
       <c r="J33" s="10" t="s">
-        <v>88</v>
+        <v>42</v>
       </c>
       <c r="K33" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="L33" s="1">
-        <v>17.77</v>
-      </c>
-      <c r="M33" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="N33" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O33" s="6">
-        <v>1.27</v>
-      </c>
-      <c r="P33" s="6">
-        <v>1.1499999999999999</v>
+      <c r="M33" s="43">
+        <v>-1.25</v>
+      </c>
+      <c r="N33" s="43">
+        <v>-0.75</v>
       </c>
       <c r="Q33" s="7">
         <v>120</v>
@@ -3024,7 +3056,7 @@
         <v>2023</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>17</v>
@@ -3033,7 +3065,7 @@
         <v>252</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>9</v>
@@ -3045,10 +3077,10 @@
         <v>79</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>42</v>
+        <v>88</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="L34" s="1">
         <v>17.77</v>
@@ -3059,11 +3091,11 @@
       <c r="N34" s="44" t="s">
         <v>109</v>
       </c>
-      <c r="O34" s="1">
-        <v>0.64</v>
-      </c>
-      <c r="P34" s="1">
-        <v>0.57999999999999996</v>
+      <c r="O34" s="6">
+        <v>1.27</v>
+      </c>
+      <c r="P34" s="6">
+        <v>1.1499999999999999</v>
       </c>
       <c r="Q34" s="7">
         <v>120</v>
@@ -3080,7 +3112,7 @@
         <v>2023</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>17</v>
@@ -3089,7 +3121,7 @@
         <v>252</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>152</v>
+        <v>96</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>9</v>
@@ -3101,10 +3133,10 @@
         <v>79</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>88</v>
+        <v>42</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L35" s="1">
         <v>17.77</v>
@@ -3116,18 +3148,18 @@
         <v>109</v>
       </c>
       <c r="O35" s="1">
-        <v>0.95</v>
+        <v>0.64</v>
       </c>
       <c r="P35" s="1">
-        <v>0.86</v>
-      </c>
-      <c r="Q35" s="6">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="Q35" s="7">
         <v>120</v>
       </c>
-      <c r="R35" s="6">
-        <v>0</v>
-      </c>
-      <c r="S35" s="6">
+      <c r="R35" s="7">
+        <v>0</v>
+      </c>
+      <c r="S35" s="7">
         <v>45</v>
       </c>
     </row>
@@ -3136,7 +3168,7 @@
         <v>2023</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>138</v>
+        <v>95</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>17</v>
@@ -3145,7 +3177,7 @@
         <v>252</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>133</v>
+        <v>152</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>9</v>
@@ -3157,10 +3189,10 @@
         <v>79</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="L36" s="1">
         <v>17.77</v>
@@ -3178,13 +3210,13 @@
         <v>0.86</v>
       </c>
       <c r="Q36" s="6">
-        <v>200</v>
+        <v>120</v>
       </c>
       <c r="R36" s="6">
         <v>0</v>
       </c>
       <c r="S36" s="6">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.2">
@@ -3192,7 +3224,7 @@
         <v>2023</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>17</v>
@@ -3201,7 +3233,7 @@
         <v>252</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>9</v>
@@ -3213,10 +3245,10 @@
         <v>79</v>
       </c>
       <c r="J37" s="10" t="s">
-        <v>88</v>
+        <v>43</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="L37" s="1">
         <v>17.77</v>
@@ -3234,7 +3266,7 @@
         <v>0.86</v>
       </c>
       <c r="Q37" s="6">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="R37" s="6">
         <v>0</v>
@@ -3248,7 +3280,7 @@
         <v>2023</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>17</v>
@@ -3257,7 +3289,7 @@
         <v>252</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>9</v>
@@ -3269,10 +3301,10 @@
         <v>79</v>
       </c>
       <c r="J38" s="10" t="s">
-        <v>129</v>
+        <v>88</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L38" s="1">
         <v>17.77</v>
@@ -3284,10 +3316,10 @@
         <v>109</v>
       </c>
       <c r="O38" s="1">
-        <v>0.39</v>
+        <v>0.95</v>
       </c>
       <c r="P38" s="1">
-        <v>0.35</v>
+        <v>0.86</v>
       </c>
       <c r="Q38" s="6">
         <v>300</v>
@@ -3304,7 +3336,7 @@
         <v>2023</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>17</v>
@@ -3313,7 +3345,7 @@
         <v>252</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>9</v>
@@ -3325,10 +3357,10 @@
         <v>79</v>
       </c>
       <c r="J39" s="10" t="s">
-        <v>43</v>
+        <v>129</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="L39" s="1">
         <v>17.77</v>
@@ -3340,19 +3372,19 @@
         <v>109</v>
       </c>
       <c r="O39" s="1">
-        <v>0.77</v>
+        <v>0.39</v>
       </c>
       <c r="P39" s="1">
-        <v>0.69</v>
+        <v>0.35</v>
       </c>
       <c r="Q39" s="6">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="R39" s="6">
         <v>0</v>
       </c>
       <c r="S39" s="6">
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.2">
@@ -3360,7 +3392,7 @@
         <v>2023</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>17</v>
@@ -3369,7 +3401,7 @@
         <v>252</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>9</v>
@@ -3381,10 +3413,10 @@
         <v>79</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>129</v>
+        <v>43</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
       <c r="L40" s="1">
         <v>17.77</v>
@@ -3396,19 +3428,19 @@
         <v>109</v>
       </c>
       <c r="O40" s="1">
-        <v>0.94</v>
+        <v>0.77</v>
       </c>
       <c r="P40" s="1">
-        <v>0.85499999999999998</v>
+        <v>0.69</v>
       </c>
       <c r="Q40" s="6">
-        <v>120</v>
+        <v>400</v>
       </c>
       <c r="R40" s="6">
         <v>0</v>
       </c>
       <c r="S40" s="6">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.2">
@@ -3416,7 +3448,7 @@
         <v>2023</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>17</v>
@@ -3425,7 +3457,7 @@
         <v>252</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>9</v>
@@ -3434,7 +3466,7 @@
         <v>10</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>163</v>
+        <v>79</v>
       </c>
       <c r="J41" s="10" t="s">
         <v>129</v>
@@ -3472,7 +3504,7 @@
         <v>2023</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>17</v>
@@ -3481,7 +3513,7 @@
         <v>252</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>9</v>
@@ -3528,7 +3560,7 @@
         <v>2023</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>17</v>
@@ -3537,7 +3569,7 @@
         <v>252</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>9</v>
@@ -3549,10 +3581,10 @@
         <v>163</v>
       </c>
       <c r="J43" s="10" t="s">
-        <v>16</v>
+        <v>129</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="L43" s="1">
         <v>17.77</v>
@@ -3583,8 +3615,8 @@
       <c r="A44" s="1">
         <v>2023</v>
       </c>
-      <c r="B44" s="50" t="s">
-        <v>170</v>
+      <c r="B44" s="1" t="s">
+        <v>167</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>17</v>
@@ -3593,7 +3625,7 @@
         <v>252</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>9</v>
@@ -3602,13 +3634,13 @@
         <v>10</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="J44" s="10" t="s">
         <v>16</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="L44" s="1">
         <v>17.77</v>
@@ -3639,8 +3671,8 @@
       <c r="A45" s="1">
         <v>2023</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>174</v>
+      <c r="B45" s="50" t="s">
+        <v>170</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>17</v>
@@ -3649,7 +3681,7 @@
         <v>252</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>199</v>
+        <v>171</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>9</v>
@@ -3664,7 +3696,7 @@
         <v>16</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="L45" s="1">
         <v>17.77</v>
@@ -3676,10 +3708,10 @@
         <v>109</v>
       </c>
       <c r="O45" s="1">
-        <v>0.99</v>
+        <v>0.94</v>
       </c>
       <c r="P45" s="1">
-        <v>0.89</v>
+        <v>0.85499999999999998</v>
       </c>
       <c r="Q45" s="6">
         <v>120</v>
@@ -3696,7 +3728,7 @@
         <v>2023</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>17</v>
@@ -3705,7 +3737,7 @@
         <v>252</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>9</v>
@@ -3714,13 +3746,13 @@
         <v>10</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="J46" s="10" t="s">
         <v>16</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="L46" s="1">
         <v>17.77</v>
@@ -3752,7 +3784,7 @@
         <v>2023</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>17</v>
@@ -3761,7 +3793,7 @@
         <v>252</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>9</v>
@@ -3773,10 +3805,10 @@
         <v>177</v>
       </c>
       <c r="J47" s="10" t="s">
-        <v>110</v>
+        <v>16</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L47" s="1">
         <v>17.77</v>
@@ -3788,10 +3820,10 @@
         <v>109</v>
       </c>
       <c r="O47" s="1">
-        <v>1.04</v>
+        <v>0.99</v>
       </c>
       <c r="P47" s="1">
-        <v>0.94</v>
+        <v>0.89</v>
       </c>
       <c r="Q47" s="6">
         <v>120</v>
@@ -3807,8 +3839,8 @@
       <c r="A48" s="1">
         <v>2023</v>
       </c>
-      <c r="B48" s="50" t="s">
-        <v>181</v>
+      <c r="B48" s="1" t="s">
+        <v>180</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>17</v>
@@ -3817,7 +3849,7 @@
         <v>252</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>9</v>
@@ -3829,10 +3861,10 @@
         <v>177</v>
       </c>
       <c r="J48" s="10" t="s">
-        <v>44</v>
+        <v>110</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="L48" s="1">
         <v>17.77</v>
@@ -3844,27 +3876,27 @@
         <v>109</v>
       </c>
       <c r="O48" s="1">
-        <v>0.99</v>
+        <v>1.04</v>
       </c>
       <c r="P48" s="1">
-        <v>0.89</v>
+        <v>0.94</v>
       </c>
       <c r="Q48" s="6">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="R48" s="6">
         <v>0</v>
       </c>
       <c r="S48" s="6">
-        <v>60</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>2023</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>183</v>
+      <c r="B49" s="50" t="s">
+        <v>181</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>17</v>
@@ -3873,7 +3905,7 @@
         <v>252</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>9</v>
@@ -3885,10 +3917,10 @@
         <v>177</v>
       </c>
       <c r="J49" s="10" t="s">
-        <v>129</v>
+        <v>44</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="L49" s="1">
         <v>17.77</v>
@@ -3900,10 +3932,10 @@
         <v>109</v>
       </c>
       <c r="O49" s="1">
-        <v>1.04</v>
+        <v>0.99</v>
       </c>
       <c r="P49" s="1">
-        <v>0.94</v>
+        <v>0.89</v>
       </c>
       <c r="Q49" s="6">
         <v>100</v>
@@ -3920,7 +3952,7 @@
         <v>2023</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>17</v>
@@ -3929,7 +3961,7 @@
         <v>252</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>9</v>
@@ -3941,10 +3973,10 @@
         <v>177</v>
       </c>
       <c r="J50" s="10" t="s">
-        <v>43</v>
+        <v>129</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="L50" s="1">
         <v>17.77</v>
@@ -3956,19 +3988,19 @@
         <v>109</v>
       </c>
       <c r="O50" s="1">
-        <v>0.99</v>
+        <v>1.04</v>
       </c>
       <c r="P50" s="1">
-        <v>0.89</v>
+        <v>0.94</v>
       </c>
       <c r="Q50" s="6">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="R50" s="6">
         <v>0</v>
       </c>
       <c r="S50" s="6">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.2">
@@ -3976,7 +4008,7 @@
         <v>2023</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>17</v>
@@ -3985,7 +4017,7 @@
         <v>252</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>9</v>
@@ -3997,10 +4029,10 @@
         <v>177</v>
       </c>
       <c r="J51" s="10" t="s">
-        <v>88</v>
+        <v>43</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="L51" s="1">
         <v>17.77</v>
@@ -4012,10 +4044,10 @@
         <v>109</v>
       </c>
       <c r="O51" s="1">
-        <v>1.04</v>
+        <v>0.99</v>
       </c>
       <c r="P51" s="1">
-        <v>0.94</v>
+        <v>0.89</v>
       </c>
       <c r="Q51" s="6">
         <v>90</v>
@@ -4032,7 +4064,7 @@
         <v>2023</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>17</v>
@@ -4041,7 +4073,7 @@
         <v>252</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>9</v>
@@ -4053,10 +4085,10 @@
         <v>177</v>
       </c>
       <c r="J52" s="10" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="L52" s="1">
         <v>17.77</v>
@@ -4068,19 +4100,19 @@
         <v>109</v>
       </c>
       <c r="O52" s="1">
-        <v>0.99</v>
+        <v>1.04</v>
       </c>
       <c r="P52" s="1">
-        <v>0.89</v>
+        <v>0.94</v>
       </c>
       <c r="Q52" s="6">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="R52" s="6">
         <v>0</v>
       </c>
       <c r="S52" s="6">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.2">
@@ -4088,7 +4120,7 @@
         <v>2023</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>17</v>
@@ -4112,7 +4144,7 @@
         <v>110</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="L53" s="1">
         <v>17.77</v>
@@ -4136,7 +4168,7 @@
         <v>0</v>
       </c>
       <c r="S53" s="6">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.2">
@@ -4144,7 +4176,7 @@
         <v>2023</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>17</v>
@@ -4153,7 +4185,7 @@
         <v>252</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>9</v>
@@ -4165,13 +4197,13 @@
         <v>177</v>
       </c>
       <c r="J54" s="10" t="s">
-        <v>43</v>
+        <v>110</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="L54" s="1">
-        <v>16.45</v>
+        <v>17.77</v>
       </c>
       <c r="M54" s="44" t="s">
         <v>109</v>
@@ -4200,7 +4232,7 @@
         <v>2023</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>17</v>
@@ -4209,7 +4241,7 @@
         <v>252</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>9</v>
@@ -4224,10 +4256,10 @@
         <v>43</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="L55" s="1">
-        <v>16.61</v>
+        <v>16.45</v>
       </c>
       <c r="M55" s="44" t="s">
         <v>109</v>
@@ -4256,7 +4288,7 @@
         <v>2023</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>17</v>
@@ -4265,25 +4297,22 @@
         <v>252</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G56" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="I56" s="1" t="s">
         <v>177</v>
       </c>
       <c r="J56" s="10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="L56" s="1">
         <v>16.61</v>
@@ -4295,10 +4324,10 @@
         <v>109</v>
       </c>
       <c r="O56" s="1">
-        <v>1.04</v>
+        <v>0.99</v>
       </c>
       <c r="P56" s="1">
-        <v>0.94</v>
+        <v>0.89</v>
       </c>
       <c r="Q56" s="6">
         <v>100</v>
@@ -4310,150 +4339,153 @@
         <v>75</v>
       </c>
     </row>
-    <row r="57" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="28">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="J57" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="L57" s="1">
+        <v>16.61</v>
+      </c>
+      <c r="M57" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="N57" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="O57" s="1">
+        <v>1.04</v>
+      </c>
+      <c r="P57" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="Q57" s="6">
+        <v>100</v>
+      </c>
+      <c r="R57" s="6">
+        <v>0</v>
+      </c>
+      <c r="S57" s="6">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="28">
         <v>2025</v>
       </c>
-      <c r="B57" s="28" t="s">
+      <c r="B58" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="C57" s="28" t="s">
+      <c r="C58" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="D57" s="28" t="s">
+      <c r="D58" s="28" t="s">
         <v>251</v>
       </c>
-      <c r="E57" s="28" t="s">
+      <c r="E58" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="H57" s="28" t="s">
+      <c r="H58" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="I57" s="28" t="s">
+      <c r="I58" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="J57" s="29" t="s">
+      <c r="J58" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="M57" s="45"/>
-      <c r="N57" s="45"/>
-      <c r="Q57" s="30"/>
-      <c r="R57" s="30"/>
-      <c r="S57" s="30"/>
-    </row>
-    <row r="58" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="15">
+      <c r="M58" s="45"/>
+      <c r="N58" s="45"/>
+      <c r="Q58" s="30"/>
+      <c r="R58" s="30"/>
+      <c r="S58" s="30"/>
+    </row>
+    <row r="59" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="15">
         <v>2035</v>
       </c>
-      <c r="B58" s="15" t="s">
+      <c r="B59" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="C58" s="15" t="s">
+      <c r="C59" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="D58" s="15" t="s">
+      <c r="D59" s="15" t="s">
         <v>251</v>
       </c>
-      <c r="E58" s="15" t="s">
+      <c r="E59" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="F58" s="15" t="s">
+      <c r="F59" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="G58" s="18" t="s">
+      <c r="G59" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="H58" s="15" t="s">
+      <c r="H59" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="I58" s="15" t="s">
+      <c r="I59" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="J58" s="16" t="s">
+      <c r="J59" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="K58" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="L58" s="15">
+      <c r="K59" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="L59" s="15">
         <v>15.85</v>
       </c>
-      <c r="M58" s="46">
+      <c r="M59" s="46">
         <v>-0.27</v>
       </c>
-      <c r="N58" s="46">
-        <v>0</v>
-      </c>
-      <c r="O58" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="P58" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q58" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="R58" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="S58" s="17" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="59" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="12">
-        <v>2035</v>
-      </c>
-      <c r="B59" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="C59" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D59" s="12" t="s">
-        <v>250</v>
-      </c>
-      <c r="E59" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="F59" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="G59" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="I59" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="J59" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="K59" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="L59" s="12">
-        <v>15.85</v>
-      </c>
-      <c r="M59" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="N59" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="O59" s="14">
-        <v>1.27</v>
-      </c>
-      <c r="P59" s="14">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="Q59" s="14">
-        <v>120</v>
-      </c>
-      <c r="R59" s="14">
-        <v>0</v>
-      </c>
-      <c r="S59" s="14">
-        <v>45</v>
+      <c r="N59" s="46">
+        <v>0</v>
+      </c>
+      <c r="O59" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="P59" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q59" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="R59" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="S59" s="17" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="60" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
@@ -4461,7 +4493,7 @@
         <v>2035</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C60" s="12" t="s">
         <v>17</v>
@@ -4470,7 +4502,7 @@
         <v>250</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F60" s="12" t="s">
         <v>9</v>
@@ -4482,13 +4514,13 @@
         <v>103</v>
       </c>
       <c r="J60" s="13" t="s">
-        <v>108</v>
+        <v>43</v>
       </c>
       <c r="K60" s="12" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="L60" s="12">
-        <v>18.64</v>
+        <v>15.85</v>
       </c>
       <c r="M60" s="47" t="s">
         <v>109</v>
@@ -4517,7 +4549,7 @@
         <v>2035</v>
       </c>
       <c r="B61" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C61" s="12" t="s">
         <v>17</v>
@@ -4526,7 +4558,7 @@
         <v>250</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F61" s="12" t="s">
         <v>9</v>
@@ -4538,10 +4570,10 @@
         <v>103</v>
       </c>
       <c r="J61" s="13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K61" s="12" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="L61" s="12">
         <v>18.64</v>
@@ -4559,13 +4591,13 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="Q61" s="14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="R61" s="14">
         <v>0</v>
       </c>
       <c r="S61" s="14">
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="62" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
@@ -4573,7 +4605,7 @@
         <v>2035</v>
       </c>
       <c r="B62" s="12" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="C62" s="12" t="s">
         <v>17</v>
@@ -4582,7 +4614,7 @@
         <v>250</v>
       </c>
       <c r="E62" s="12" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="F62" s="12" t="s">
         <v>9</v>
@@ -4594,10 +4626,10 @@
         <v>103</v>
       </c>
       <c r="J62" s="13" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="K62" s="12" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="L62" s="12">
         <v>18.64</v>
@@ -4608,20 +4640,20 @@
       <c r="N62" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="O62" s="12">
-        <v>0.95</v>
-      </c>
-      <c r="P62" s="12">
-        <v>0.86</v>
+      <c r="O62" s="14">
+        <v>1.27</v>
+      </c>
+      <c r="P62" s="14">
+        <v>1.1499999999999999</v>
       </c>
       <c r="Q62" s="14">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="R62" s="14">
         <v>0</v>
       </c>
       <c r="S62" s="14">
-        <v>45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
@@ -4629,7 +4661,7 @@
         <v>2035</v>
       </c>
       <c r="B63" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C63" s="12" t="s">
         <v>17</v>
@@ -4638,7 +4670,7 @@
         <v>250</v>
       </c>
       <c r="E63" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F63" s="12" t="s">
         <v>9</v>
@@ -4650,10 +4682,10 @@
         <v>103</v>
       </c>
       <c r="J63" s="13" t="s">
-        <v>42</v>
+        <v>108</v>
       </c>
       <c r="K63" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="L63" s="12">
         <v>18.64</v>
@@ -4671,13 +4703,13 @@
         <v>0.86</v>
       </c>
       <c r="Q63" s="14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="R63" s="14">
         <v>0</v>
       </c>
       <c r="S63" s="14">
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="64" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
@@ -4685,7 +4717,7 @@
         <v>2035</v>
       </c>
       <c r="B64" s="12" t="s">
-        <v>184</v>
+        <v>120</v>
       </c>
       <c r="C64" s="12" t="s">
         <v>17</v>
@@ -4694,7 +4726,7 @@
         <v>250</v>
       </c>
       <c r="E64" s="12" t="s">
-        <v>209</v>
+        <v>122</v>
       </c>
       <c r="F64" s="12" t="s">
         <v>9</v>
@@ -4706,10 +4738,10 @@
         <v>103</v>
       </c>
       <c r="J64" s="13" t="s">
-        <v>108</v>
+        <v>42</v>
       </c>
       <c r="K64" s="12" t="s">
-        <v>186</v>
+        <v>123</v>
       </c>
       <c r="L64" s="12">
         <v>18.64</v>
@@ -4741,7 +4773,7 @@
         <v>2035</v>
       </c>
       <c r="B65" s="12" t="s">
-        <v>207</v>
+        <v>184</v>
       </c>
       <c r="C65" s="12" t="s">
         <v>17</v>
@@ -4750,7 +4782,7 @@
         <v>250</v>
       </c>
       <c r="E65" s="12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F65" s="12" t="s">
         <v>9</v>
@@ -4762,7 +4794,7 @@
         <v>103</v>
       </c>
       <c r="J65" s="13" t="s">
-        <v>44</v>
+        <v>108</v>
       </c>
       <c r="K65" s="12" t="s">
         <v>186</v>
@@ -4797,7 +4829,7 @@
         <v>2035</v>
       </c>
       <c r="B66" s="12" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C66" s="12" t="s">
         <v>17</v>
@@ -4806,13 +4838,13 @@
         <v>250</v>
       </c>
       <c r="E66" s="12" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="F66" s="12" t="s">
-        <v>211</v>
+        <v>9</v>
       </c>
       <c r="G66" s="12" t="s">
-        <v>116</v>
+        <v>10</v>
       </c>
       <c r="I66" s="12" t="s">
         <v>103</v>
@@ -4821,7 +4853,7 @@
         <v>44</v>
       </c>
       <c r="K66" s="12" t="s">
-        <v>212</v>
+        <v>186</v>
       </c>
       <c r="L66" s="12">
         <v>18.64</v>
@@ -4839,13 +4871,13 @@
         <v>0.86</v>
       </c>
       <c r="Q66" s="14">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="R66" s="14">
         <v>0</v>
       </c>
       <c r="S66" s="14">
-        <v>41.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
@@ -4853,7 +4885,7 @@
         <v>2035</v>
       </c>
       <c r="B67" s="12" t="s">
-        <v>228</v>
+        <v>206</v>
       </c>
       <c r="C67" s="12" t="s">
         <v>17</v>
@@ -4862,7 +4894,7 @@
         <v>250</v>
       </c>
       <c r="E67" s="12" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
       <c r="F67" s="12" t="s">
         <v>211</v>
@@ -4874,13 +4906,13 @@
         <v>103</v>
       </c>
       <c r="J67" s="13" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="K67" s="12" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="L67" s="12">
-        <v>20.55</v>
+        <v>18.64</v>
       </c>
       <c r="M67" s="47" t="s">
         <v>109</v>
@@ -4889,10 +4921,10 @@
         <v>109</v>
       </c>
       <c r="O67" s="12">
-        <v>0.99</v>
+        <v>0.95</v>
       </c>
       <c r="P67" s="12">
-        <v>0.89</v>
+        <v>0.86</v>
       </c>
       <c r="Q67" s="14">
         <v>100</v>
@@ -4901,7 +4933,7 @@
         <v>0</v>
       </c>
       <c r="S67" s="14">
-        <v>75</v>
+        <v>41.25</v>
       </c>
     </row>
     <row r="68" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
@@ -4909,7 +4941,7 @@
         <v>2035</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C68" s="12" t="s">
         <v>17</v>
@@ -4918,7 +4950,7 @@
         <v>250</v>
       </c>
       <c r="E68" s="12" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="F68" s="12" t="s">
         <v>211</v>
@@ -4926,17 +4958,14 @@
       <c r="G68" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="H68" s="12" t="s">
-        <v>11</v>
-      </c>
       <c r="I68" s="12" t="s">
         <v>103</v>
       </c>
       <c r="J68" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K68" s="12" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="L68" s="12">
         <v>20.55</v>
@@ -4968,7 +4997,7 @@
         <v>2035</v>
       </c>
       <c r="B69" s="12" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C69" s="12" t="s">
         <v>17</v>
@@ -4977,13 +5006,13 @@
         <v>250</v>
       </c>
       <c r="E69" s="12" t="s">
-        <v>233</v>
-      </c>
-      <c r="F69" s="53" t="s">
-        <v>234</v>
+        <v>230</v>
+      </c>
+      <c r="F69" s="12" t="s">
+        <v>211</v>
       </c>
       <c r="G69" s="12" t="s">
-        <v>235</v>
+        <v>116</v>
       </c>
       <c r="H69" s="12" t="s">
         <v>11</v>
@@ -4992,10 +5021,10 @@
         <v>103</v>
       </c>
       <c r="J69" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K69" s="12" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="L69" s="12">
         <v>20.55</v>
@@ -5027,7 +5056,7 @@
         <v>2035</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="C70" s="12" t="s">
         <v>17</v>
@@ -5036,13 +5065,13 @@
         <v>250</v>
       </c>
       <c r="E70" s="12" t="s">
-        <v>238</v>
-      </c>
-      <c r="F70" s="12" t="s">
-        <v>211</v>
+        <v>233</v>
+      </c>
+      <c r="F70" s="53" t="s">
+        <v>234</v>
       </c>
       <c r="G70" s="12" t="s">
-        <v>116</v>
+        <v>235</v>
       </c>
       <c r="H70" s="12" t="s">
         <v>11</v>
@@ -5051,13 +5080,13 @@
         <v>103</v>
       </c>
       <c r="J70" s="13" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="K70" s="12" t="s">
-        <v>239</v>
-      </c>
-      <c r="L70" s="53">
-        <v>15.85</v>
+        <v>236</v>
+      </c>
+      <c r="L70" s="12">
+        <v>20.55</v>
       </c>
       <c r="M70" s="47" t="s">
         <v>109</v>
@@ -5086,7 +5115,7 @@
         <v>2035</v>
       </c>
       <c r="B71" s="12" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="C71" s="12" t="s">
         <v>17</v>
@@ -5095,7 +5124,7 @@
         <v>250</v>
       </c>
       <c r="E71" s="12" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="F71" s="12" t="s">
         <v>211</v>
@@ -5110,13 +5139,13 @@
         <v>103</v>
       </c>
       <c r="J71" s="13" t="s">
-        <v>110</v>
+        <v>16</v>
       </c>
       <c r="K71" s="12" t="s">
-        <v>246</v>
-      </c>
-      <c r="L71" s="12">
-        <v>20.55</v>
+        <v>239</v>
+      </c>
+      <c r="L71" s="53">
+        <v>15.85</v>
       </c>
       <c r="M71" s="47" t="s">
         <v>109</v>
@@ -5130,14 +5159,14 @@
       <c r="P71" s="12">
         <v>0.89</v>
       </c>
-      <c r="Q71" s="52">
-        <v>0</v>
-      </c>
-      <c r="R71" s="52">
-        <v>0</v>
-      </c>
-      <c r="S71" s="52">
-        <v>0</v>
+      <c r="Q71" s="14">
+        <v>100</v>
+      </c>
+      <c r="R71" s="14">
+        <v>0</v>
+      </c>
+      <c r="S71" s="14">
+        <v>75</v>
       </c>
     </row>
     <row r="72" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
@@ -5145,7 +5174,7 @@
         <v>2035</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="C72" s="12" t="s">
         <v>17</v>
@@ -5154,7 +5183,7 @@
         <v>250</v>
       </c>
       <c r="E72" s="12" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="F72" s="12" t="s">
         <v>211</v>
@@ -5169,10 +5198,10 @@
         <v>103</v>
       </c>
       <c r="J72" s="13" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="K72" s="12" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="L72" s="12">
         <v>20.55</v>
@@ -5189,14 +5218,14 @@
       <c r="P72" s="12">
         <v>0.89</v>
       </c>
-      <c r="Q72" s="14">
-        <v>100</v>
-      </c>
-      <c r="R72" s="14">
-        <v>0</v>
-      </c>
-      <c r="S72" s="14">
-        <v>75</v>
+      <c r="Q72" s="52">
+        <v>0</v>
+      </c>
+      <c r="R72" s="52">
+        <v>0</v>
+      </c>
+      <c r="S72" s="52">
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
@@ -5204,7 +5233,7 @@
         <v>2035</v>
       </c>
       <c r="B73" s="12" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="C73" s="12" t="s">
         <v>17</v>
@@ -5213,7 +5242,7 @@
         <v>250</v>
       </c>
       <c r="E73" s="12" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="F73" s="12" t="s">
         <v>211</v>
@@ -5228,10 +5257,10 @@
         <v>103</v>
       </c>
       <c r="J73" s="13" t="s">
-        <v>43</v>
+        <v>129</v>
       </c>
       <c r="K73" s="12" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="L73" s="12">
         <v>20.55</v>
@@ -5243,10 +5272,10 @@
         <v>109</v>
       </c>
       <c r="O73" s="12">
-        <v>0.87</v>
+        <v>0.99</v>
       </c>
       <c r="P73" s="12">
-        <v>0.78</v>
+        <v>0.89</v>
       </c>
       <c r="Q73" s="14">
         <v>100</v>
@@ -5263,7 +5292,7 @@
         <v>2035</v>
       </c>
       <c r="B74" s="12" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C74" s="12" t="s">
         <v>17</v>
@@ -5272,7 +5301,7 @@
         <v>250</v>
       </c>
       <c r="E74" s="12" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F74" s="12" t="s">
         <v>211</v>
@@ -5290,7 +5319,7 @@
         <v>43</v>
       </c>
       <c r="K74" s="12" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="L74" s="12">
         <v>20.55</v>
@@ -5322,7 +5351,7 @@
         <v>2035</v>
       </c>
       <c r="B75" s="12" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="C75" s="12" t="s">
         <v>17</v>
@@ -5331,7 +5360,7 @@
         <v>250</v>
       </c>
       <c r="E75" s="12" t="s">
-        <v>243</v>
+        <v>259</v>
       </c>
       <c r="F75" s="12" t="s">
         <v>211</v>
@@ -5346,10 +5375,10 @@
         <v>103</v>
       </c>
       <c r="J75" s="13" t="s">
-        <v>108</v>
+        <v>43</v>
       </c>
       <c r="K75" s="12" t="s">
-        <v>244</v>
+        <v>260</v>
       </c>
       <c r="L75" s="12">
         <v>20.55</v>
@@ -5360,11 +5389,11 @@
       <c r="N75" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="O75" s="53">
-        <v>0.84</v>
-      </c>
-      <c r="P75" s="53">
-        <v>1.59</v>
+      <c r="O75" s="12">
+        <v>0.87</v>
+      </c>
+      <c r="P75" s="12">
+        <v>0.78</v>
       </c>
       <c r="Q75" s="14">
         <v>100</v>
@@ -5381,7 +5410,7 @@
         <v>2035</v>
       </c>
       <c r="B76" s="12" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="C76" s="12" t="s">
         <v>17</v>
@@ -5390,7 +5419,7 @@
         <v>250</v>
       </c>
       <c r="E76" s="12" t="s">
-        <v>262</v>
+        <v>243</v>
       </c>
       <c r="F76" s="12" t="s">
         <v>211</v>
@@ -5405,10 +5434,10 @@
         <v>103</v>
       </c>
       <c r="J76" s="13" t="s">
-        <v>43</v>
+        <v>108</v>
       </c>
       <c r="K76" s="12" t="s">
-        <v>263</v>
+        <v>244</v>
       </c>
       <c r="L76" s="12">
         <v>20.55</v>
@@ -5419,11 +5448,11 @@
       <c r="N76" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="O76" s="12">
-        <v>0.87</v>
-      </c>
-      <c r="P76" s="12">
-        <v>0.78</v>
+      <c r="O76" s="53">
+        <v>0.84</v>
+      </c>
+      <c r="P76" s="53">
+        <v>1.59</v>
       </c>
       <c r="Q76" s="14">
         <v>100</v>
@@ -5435,68 +5464,240 @@
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="24">
+    <row r="77" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B77" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="C77" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D77" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="E77" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="F77" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="G77" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="H77" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I77" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="J77" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K77" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="L77" s="12">
+        <v>20.55</v>
+      </c>
+      <c r="M77" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="N77" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="O77" s="12">
+        <v>0.87</v>
+      </c>
+      <c r="P77" s="12">
+        <v>0.78</v>
+      </c>
+      <c r="Q77" s="14">
+        <v>100</v>
+      </c>
+      <c r="R77" s="14">
+        <v>0</v>
+      </c>
+      <c r="S77" s="14">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B78" s="12" t="s">
+        <v>268</v>
+      </c>
+      <c r="C78" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D78" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="E78" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="F78" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="G78" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="H78" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I78" s="53" t="s">
+        <v>270</v>
+      </c>
+      <c r="J78" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="K78" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="L78" s="12">
+        <v>20.55</v>
+      </c>
+      <c r="M78" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="N78" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="O78" s="12">
+        <v>0.87</v>
+      </c>
+      <c r="P78" s="12">
+        <v>0.78</v>
+      </c>
+      <c r="Q78" s="14">
+        <v>100</v>
+      </c>
+      <c r="R78" s="14">
+        <v>0</v>
+      </c>
+      <c r="S78" s="14">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="79" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B79" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="C79" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D79" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="E79" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="F79" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="G79" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="I79" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="J79" s="13"/>
+      <c r="K79" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="L79" s="12">
+        <v>20.55</v>
+      </c>
+      <c r="M79" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="N79" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="O79" s="12">
+        <v>0.87</v>
+      </c>
+      <c r="P79" s="12">
+        <v>0.78</v>
+      </c>
+      <c r="Q79" s="14">
+        <v>100</v>
+      </c>
+      <c r="R79" s="14">
+        <v>0</v>
+      </c>
+      <c r="S79" s="14">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="80" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="24">
         <v>2050</v>
       </c>
-      <c r="B77" s="24" t="s">
+      <c r="B80" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="C77" s="24" t="s">
+      <c r="C80" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="D77" s="24" t="s">
+      <c r="D80" s="24" t="s">
         <v>251</v>
       </c>
-      <c r="E77" s="24" t="s">
+      <c r="E80" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="F77" s="24" t="s">
+      <c r="F80" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="G77" s="25" t="s">
+      <c r="G80" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="I77" s="24" t="s">
+      <c r="I80" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="J77" s="26" t="s">
+      <c r="J80" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="K77" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="L77" s="24">
+      <c r="K80" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="L80" s="24">
         <v>17.440000000000001</v>
       </c>
-      <c r="M77" s="48">
+      <c r="M80" s="48">
         <v>-0.33</v>
       </c>
-      <c r="N77" s="48">
-        <v>0</v>
-      </c>
-      <c r="O77" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="P77" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q77" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="R77" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="S77" s="27" t="s">
+      <c r="N80" s="48">
+        <v>0</v>
+      </c>
+      <c r="O80" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="P80" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q80" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="R80" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="S80" s="27" t="s">
         <v>109</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="K6" r:id="rId1" xr:uid="{1BE7DD4C-B567-4320-9B69-E8B55CE41797}"/>
-    <hyperlink ref="K7" r:id="rId2" xr:uid="{A52BF015-28DA-4569-A638-6E56CCBD2F4D}"/>
-    <hyperlink ref="K8" r:id="rId3" xr:uid="{70B88B93-E906-4801-9012-B01BCDB48CBF}"/>
+    <hyperlink ref="K7" r:id="rId1" xr:uid="{1BE7DD4C-B567-4320-9B69-E8B55CE41797}"/>
+    <hyperlink ref="K8" r:id="rId2" xr:uid="{A52BF015-28DA-4569-A638-6E56CCBD2F4D}"/>
+    <hyperlink ref="K9" r:id="rId3" xr:uid="{70B88B93-E906-4801-9012-B01BCDB48CBF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>

<commit_message>
update model run log info re. 2035_TM160_IPA_12
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\config_RTP2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87C0D65-8C37-46A9-B71D-A6F13079136C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD8BE10-FFEE-43B4-BE36-76AD73DD4EA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="885" windowWidth="28800" windowHeight="14085" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelRuns" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="276">
   <si>
     <t>year</t>
   </si>
@@ -728,18 +728,12 @@
     <t>2035_TM160_IPA_09</t>
   </si>
   <si>
-    <t>IPA with all in</t>
-  </si>
-  <si>
     <t>https://app.asana.com/0/1204085012544660/1205996812896085/f</t>
   </si>
   <si>
     <t>2035_TM160_IPA_09_PBA50landuse</t>
   </si>
   <si>
-    <t>IPA with PBA50 landuse/pop</t>
-  </si>
-  <si>
     <t>POPLU_v225_UBI</t>
   </si>
   <si>
@@ -752,18 +746,12 @@
     <t>2035_TM160_IPA_09_PBA50aoc</t>
   </si>
   <si>
-    <t>IPA with PBA50 aoc</t>
-  </si>
-  <si>
     <t>https://app.asana.com/0/1204085012544660/1205995415086641/f</t>
   </si>
   <si>
     <t>2035_TM160_IPA_09_PBA50ixex</t>
   </si>
   <si>
-    <t>IPA with PBA50 ixex</t>
-  </si>
-  <si>
     <t>https://app.asana.com/0/1204085012544660/1205995415086647/f</t>
   </si>
   <si>
@@ -782,9 +770,6 @@
     <t>2015 land use</t>
   </si>
   <si>
-    <t>IPA with PBA50 ModePrefs</t>
-  </si>
-  <si>
     <t>RTP2021_IP</t>
   </si>
   <si>
@@ -864,6 +849,21 @@
   </si>
   <si>
     <t>https://app.asana.com/0/1204085012544660/1206071846636750/f</t>
+  </si>
+  <si>
+    <t>IPA (but with EN7 bug and high bike mode share)</t>
+  </si>
+  <si>
+    <t>IPA v9 with PBA50 landuse/pop</t>
+  </si>
+  <si>
+    <t>IPA v9 with PBA50 aoc</t>
+  </si>
+  <si>
+    <t>IPA v9 with PBA50 ModePrefs</t>
+  </si>
+  <si>
+    <t>IPA v9 with PBA50 ixex</t>
   </si>
 </sst>
 </file>
@@ -873,7 +873,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -913,6 +913,14 @@
       <color rgb="FFFF0000"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="12">
@@ -1010,10 +1018,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1126,8 +1135,10 @@
     <xf numFmtId="2" fontId="2" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="4" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1446,28 +1457,28 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C59" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B79" sqref="B79"/>
+      <selection pane="bottomRight" activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="17" style="1" customWidth="1"/>
-    <col min="5" max="5" width="42.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="42.26953125" style="1" customWidth="1"/>
     <col min="6" max="6" width="23" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" style="10" customWidth="1"/>
-    <col min="11" max="11" width="17.5703125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="6.28515625" style="1" customWidth="1"/>
-    <col min="13" max="14" width="9.140625" style="44"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="8.1796875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="6.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.1796875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.26953125" style="10" customWidth="1"/>
+    <col min="11" max="11" width="17.54296875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="6.26953125" style="1" customWidth="1"/>
+    <col min="13" max="14" width="9.1796875" style="44"/>
+    <col min="15" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="5" customFormat="1" ht="39" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1526,7 +1537,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19">
         <v>2005</v>
       </c>
@@ -1534,10 +1545,10 @@
         <v>125</v>
       </c>
       <c r="C2" s="21" t="s">
+        <v>244</v>
+      </c>
+      <c r="D2" s="20" t="s">
         <v>249</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>254</v>
       </c>
       <c r="E2" s="20" t="s">
         <v>126</v>
@@ -1553,7 +1564,7 @@
       <c r="Q2" s="23"/>
       <c r="R2" s="23"/>
     </row>
-    <row r="3" spans="1:19" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="31">
         <v>2005</v>
       </c>
@@ -1564,13 +1575,13 @@
         <v>17</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>150</v>
       </c>
       <c r="F3" s="32" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="G3" s="32" t="s">
         <v>10</v>
@@ -1609,7 +1620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="31">
         <v>2005</v>
       </c>
@@ -1620,13 +1631,13 @@
         <v>17</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="E4" s="32" t="s">
         <v>223</v>
       </c>
       <c r="F4" s="32" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="G4" s="32" t="s">
         <v>10</v>
@@ -1664,24 +1675,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="31">
         <v>2005</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="C5" s="32" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="32" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="F5" s="32" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="G5" s="32" t="s">
         <v>10</v>
@@ -1693,7 +1704,7 @@
         <v>43</v>
       </c>
       <c r="K5" s="32" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="L5" s="32">
         <v>14.87</v>
@@ -1716,7 +1727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="35">
         <v>2015</v>
       </c>
@@ -1727,7 +1738,7 @@
         <v>17</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="E6" s="36" t="s">
         <v>19</v>
@@ -1762,7 +1773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="35">
         <v>2015</v>
       </c>
@@ -1773,7 +1784,7 @@
         <v>17</v>
       </c>
       <c r="D7" s="36" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="E7" s="36" t="s">
         <v>149</v>
@@ -1815,7 +1826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="35">
         <v>2015</v>
       </c>
@@ -1826,7 +1837,7 @@
         <v>17</v>
       </c>
       <c r="D8" s="36" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="E8" s="36" t="s">
         <v>153</v>
@@ -1868,7 +1879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="35">
         <v>2015</v>
       </c>
@@ -1879,7 +1890,7 @@
         <v>17</v>
       </c>
       <c r="D9" s="36" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="E9" s="36" t="s">
         <v>153</v>
@@ -1921,7 +1932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="35">
         <v>2015</v>
       </c>
@@ -1932,7 +1943,7 @@
         <v>17</v>
       </c>
       <c r="D10" s="36" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="E10" s="36" t="s">
         <v>157</v>
@@ -1980,7 +1991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="35">
         <v>2015</v>
       </c>
@@ -1991,7 +2002,7 @@
         <v>17</v>
       </c>
       <c r="D11" s="36" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="E11" s="36" t="s">
         <v>215</v>
@@ -2036,7 +2047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>2023</v>
       </c>
@@ -2047,7 +2058,7 @@
         <v>17</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>19</v>
@@ -2082,7 +2093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>2023</v>
       </c>
@@ -2093,7 +2104,7 @@
         <v>17</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>21</v>
@@ -2128,7 +2139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>2023</v>
       </c>
@@ -2139,7 +2150,7 @@
         <v>17</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>27</v>
@@ -2174,7 +2185,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>2023</v>
       </c>
@@ -2185,7 +2196,7 @@
         <v>17</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>33</v>
@@ -2220,7 +2231,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>2023</v>
       </c>
@@ -2231,7 +2242,7 @@
         <v>17</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>35</v>
@@ -2266,7 +2277,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>2023</v>
       </c>
@@ -2277,7 +2288,7 @@
         <v>17</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>46</v>
@@ -2312,7 +2323,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>2023</v>
       </c>
@@ -2323,7 +2334,7 @@
         <v>17</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>46</v>
@@ -2358,7 +2369,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>2023</v>
       </c>
@@ -2369,7 +2380,7 @@
         <v>17</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>46</v>
@@ -2404,7 +2415,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>2023</v>
       </c>
@@ -2415,7 +2426,7 @@
         <v>17</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>48</v>
@@ -2450,7 +2461,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>2023</v>
       </c>
@@ -2461,7 +2472,7 @@
         <v>17</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>52</v>
@@ -2496,7 +2507,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>2023</v>
       </c>
@@ -2507,7 +2518,7 @@
         <v>17</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>55</v>
@@ -2542,7 +2553,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>2023</v>
       </c>
@@ -2553,7 +2564,7 @@
         <v>17</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>58</v>
@@ -2588,7 +2599,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>2023</v>
       </c>
@@ -2599,7 +2610,7 @@
         <v>17</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>62</v>
@@ -2634,7 +2645,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>2023</v>
       </c>
@@ -2645,7 +2656,7 @@
         <v>17</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>62</v>
@@ -2680,7 +2691,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>2023</v>
       </c>
@@ -2691,7 +2702,7 @@
         <v>17</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>62</v>
@@ -2726,7 +2737,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>2023</v>
       </c>
@@ -2737,7 +2748,7 @@
         <v>17</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>68</v>
@@ -2772,7 +2783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>2023</v>
       </c>
@@ -2783,7 +2794,7 @@
         <v>17</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>73</v>
@@ -2818,7 +2829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>2023</v>
       </c>
@@ -2829,7 +2840,7 @@
         <v>17</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>78</v>
@@ -2864,7 +2875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>2023</v>
       </c>
@@ -2875,7 +2886,7 @@
         <v>17</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>80</v>
@@ -2908,7 +2919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>2023</v>
       </c>
@@ -2919,7 +2930,7 @@
         <v>17</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>87</v>
@@ -2957,7 +2968,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>2023</v>
       </c>
@@ -2968,7 +2979,7 @@
         <v>17</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>87</v>
@@ -3004,7 +3015,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>2023</v>
       </c>
@@ -3015,7 +3026,7 @@
         <v>17</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>92</v>
@@ -3051,7 +3062,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>2023</v>
       </c>
@@ -3062,7 +3073,7 @@
         <v>17</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>92</v>
@@ -3107,7 +3118,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>2023</v>
       </c>
@@ -3118,7 +3129,7 @@
         <v>17</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>96</v>
@@ -3163,7 +3174,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>2023</v>
       </c>
@@ -3174,7 +3185,7 @@
         <v>17</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>152</v>
@@ -3219,7 +3230,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>2023</v>
       </c>
@@ -3230,7 +3241,7 @@
         <v>17</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>133</v>
@@ -3275,7 +3286,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>2023</v>
       </c>
@@ -3286,7 +3297,7 @@
         <v>17</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>134</v>
@@ -3331,7 +3342,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>2023</v>
       </c>
@@ -3342,7 +3353,7 @@
         <v>17</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>141</v>
@@ -3387,7 +3398,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>2023</v>
       </c>
@@ -3398,7 +3409,7 @@
         <v>17</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>142</v>
@@ -3443,7 +3454,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>2023</v>
       </c>
@@ -3454,7 +3465,7 @@
         <v>17</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>160</v>
@@ -3499,7 +3510,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>2023</v>
       </c>
@@ -3510,7 +3521,7 @@
         <v>17</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>164</v>
@@ -3555,7 +3566,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>2023</v>
       </c>
@@ -3566,7 +3577,7 @@
         <v>17</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>166</v>
@@ -3611,7 +3622,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>2023</v>
       </c>
@@ -3622,7 +3633,7 @@
         <v>17</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>168</v>
@@ -3667,7 +3678,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>2023</v>
       </c>
@@ -3678,7 +3689,7 @@
         <v>17</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>171</v>
@@ -3723,7 +3734,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>2023</v>
       </c>
@@ -3734,7 +3745,7 @@
         <v>17</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>199</v>
@@ -3779,7 +3790,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>2023</v>
       </c>
@@ -3790,7 +3801,7 @@
         <v>17</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>198</v>
@@ -3835,7 +3846,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>2023</v>
       </c>
@@ -3846,7 +3857,7 @@
         <v>17</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>197</v>
@@ -3891,7 +3902,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>2023</v>
       </c>
@@ -3902,7 +3913,7 @@
         <v>17</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>196</v>
@@ -3947,7 +3958,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>2023</v>
       </c>
@@ -3958,7 +3969,7 @@
         <v>17</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>195</v>
@@ -4003,7 +4014,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>2023</v>
       </c>
@@ -4014,7 +4025,7 @@
         <v>17</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>194</v>
@@ -4059,7 +4070,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>2023</v>
       </c>
@@ -4070,7 +4081,7 @@
         <v>17</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>193</v>
@@ -4115,7 +4126,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>2023</v>
       </c>
@@ -4126,7 +4137,7 @@
         <v>17</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>192</v>
@@ -4171,7 +4182,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>2023</v>
       </c>
@@ -4182,7 +4193,7 @@
         <v>17</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>192</v>
@@ -4227,7 +4238,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>2023</v>
       </c>
@@ -4238,7 +4249,7 @@
         <v>17</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>204</v>
@@ -4283,7 +4294,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>2023</v>
       </c>
@@ -4294,7 +4305,7 @@
         <v>17</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>217</v>
@@ -4339,7 +4350,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>2023</v>
       </c>
@@ -4350,7 +4361,7 @@
         <v>17</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>220</v>
@@ -4398,7 +4409,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="58" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="28">
         <v>2025</v>
       </c>
@@ -4409,7 +4420,7 @@
         <v>113</v>
       </c>
       <c r="D58" s="28" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="E58" s="28" t="s">
         <v>131</v>
@@ -4429,7 +4440,7 @@
       <c r="R58" s="30"/>
       <c r="S58" s="30"/>
     </row>
-    <row r="59" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="15">
         <v>2035</v>
       </c>
@@ -4440,7 +4451,7 @@
         <v>113</v>
       </c>
       <c r="D59" s="15" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="E59" s="15" t="s">
         <v>114</v>
@@ -4488,7 +4499,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="60" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="12">
         <v>2035</v>
       </c>
@@ -4499,7 +4510,7 @@
         <v>17</v>
       </c>
       <c r="D60" s="12" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="E60" s="12" t="s">
         <v>104</v>
@@ -4544,7 +4555,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="61" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="12">
         <v>2035</v>
       </c>
@@ -4555,7 +4566,7 @@
         <v>17</v>
       </c>
       <c r="D61" s="12" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="E61" s="12" t="s">
         <v>105</v>
@@ -4600,7 +4611,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="62" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="12">
         <v>2035</v>
       </c>
@@ -4611,7 +4622,7 @@
         <v>17</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="E62" s="12" t="s">
         <v>106</v>
@@ -4656,7 +4667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="12">
         <v>2035</v>
       </c>
@@ -4667,7 +4678,7 @@
         <v>17</v>
       </c>
       <c r="D63" s="12" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="E63" s="12" t="s">
         <v>121</v>
@@ -4712,7 +4723,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="64" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="12">
         <v>2035</v>
       </c>
@@ -4723,7 +4734,7 @@
         <v>17</v>
       </c>
       <c r="D64" s="12" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="E64" s="12" t="s">
         <v>122</v>
@@ -4768,7 +4779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="12">
         <v>2035</v>
       </c>
@@ -4779,7 +4790,7 @@
         <v>17</v>
       </c>
       <c r="D65" s="12" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="E65" s="12" t="s">
         <v>209</v>
@@ -4824,7 +4835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="12">
         <v>2035</v>
       </c>
@@ -4835,7 +4846,7 @@
         <v>17</v>
       </c>
       <c r="D66" s="12" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="E66" s="12" t="s">
         <v>210</v>
@@ -4880,7 +4891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="12">
         <v>2035</v>
       </c>
@@ -4891,7 +4902,7 @@
         <v>17</v>
       </c>
       <c r="D67" s="12" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="E67" s="12" t="s">
         <v>208</v>
@@ -4936,7 +4947,7 @@
         <v>41.25</v>
       </c>
     </row>
-    <row r="68" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="12">
         <v>2035</v>
       </c>
@@ -4947,7 +4958,7 @@
         <v>17</v>
       </c>
       <c r="D68" s="12" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="E68" s="12" t="s">
         <v>226</v>
@@ -4992,7 +5003,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="69" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="12">
         <v>2035</v>
       </c>
@@ -5003,10 +5014,10 @@
         <v>17</v>
       </c>
       <c r="D69" s="12" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="E69" s="12" t="s">
-        <v>230</v>
+        <v>271</v>
       </c>
       <c r="F69" s="12" t="s">
         <v>211</v>
@@ -5024,7 +5035,7 @@
         <v>43</v>
       </c>
       <c r="K69" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="L69" s="12">
         <v>20.55</v>
@@ -5051,27 +5062,27 @@
         <v>75</v>
       </c>
     </row>
-    <row r="70" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="12">
         <v>2035</v>
       </c>
       <c r="B70" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="C70" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D70" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="E70" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="F70" s="53" t="s">
         <v>232</v>
       </c>
-      <c r="C70" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D70" s="12" t="s">
-        <v>250</v>
-      </c>
-      <c r="E70" s="12" t="s">
+      <c r="G70" s="12" t="s">
         <v>233</v>
-      </c>
-      <c r="F70" s="53" t="s">
-        <v>234</v>
-      </c>
-      <c r="G70" s="12" t="s">
-        <v>235</v>
       </c>
       <c r="H70" s="12" t="s">
         <v>11</v>
@@ -5083,7 +5094,7 @@
         <v>44</v>
       </c>
       <c r="K70" s="12" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="L70" s="12">
         <v>20.55</v>
@@ -5110,21 +5121,21 @@
         <v>75</v>
       </c>
     </row>
-    <row r="71" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="12">
         <v>2035</v>
       </c>
       <c r="B71" s="12" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C71" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D71" s="12" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="E71" s="12" t="s">
-        <v>238</v>
+        <v>273</v>
       </c>
       <c r="F71" s="12" t="s">
         <v>211</v>
@@ -5142,7 +5153,7 @@
         <v>16</v>
       </c>
       <c r="K71" s="12" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="L71" s="53">
         <v>15.85</v>
@@ -5169,21 +5180,21 @@
         <v>75</v>
       </c>
     </row>
-    <row r="72" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72" s="12">
         <v>2035</v>
       </c>
       <c r="B72" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="C72" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D72" s="12" t="s">
         <v>245</v>
       </c>
-      <c r="C72" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D72" s="12" t="s">
-        <v>250</v>
-      </c>
       <c r="E72" s="12" t="s">
-        <v>248</v>
+        <v>274</v>
       </c>
       <c r="F72" s="12" t="s">
         <v>211</v>
@@ -5201,7 +5212,7 @@
         <v>110</v>
       </c>
       <c r="K72" s="12" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="L72" s="12">
         <v>20.55</v>
@@ -5228,21 +5239,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="12">
         <v>2035</v>
       </c>
       <c r="B73" s="12" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C73" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D73" s="12" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="E73" s="12" t="s">
-        <v>241</v>
+        <v>275</v>
       </c>
       <c r="F73" s="12" t="s">
         <v>211</v>
@@ -5260,7 +5271,7 @@
         <v>129</v>
       </c>
       <c r="K73" s="12" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="L73" s="12">
         <v>20.55</v>
@@ -5287,21 +5298,21 @@
         <v>75</v>
       </c>
     </row>
-    <row r="74" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="12">
         <v>2035</v>
       </c>
       <c r="B74" s="12" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="C74" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D74" s="12" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="E74" s="12" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="F74" s="12" t="s">
         <v>211</v>
@@ -5319,7 +5330,7 @@
         <v>43</v>
       </c>
       <c r="K74" s="12" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="L74" s="12">
         <v>20.55</v>
@@ -5346,21 +5357,21 @@
         <v>75</v>
       </c>
     </row>
-    <row r="75" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="12">
         <v>2035</v>
       </c>
       <c r="B75" s="12" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="C75" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D75" s="12" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="E75" s="12" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="F75" s="12" t="s">
         <v>211</v>
@@ -5378,7 +5389,7 @@
         <v>43</v>
       </c>
       <c r="K75" s="12" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="L75" s="12">
         <v>20.55</v>
@@ -5405,21 +5416,21 @@
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="12">
         <v>2035</v>
       </c>
       <c r="B76" s="12" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="C76" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D76" s="12" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="E76" s="12" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="F76" s="12" t="s">
         <v>211</v>
@@ -5437,7 +5448,7 @@
         <v>108</v>
       </c>
       <c r="K76" s="12" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="L76" s="12">
         <v>20.55</v>
@@ -5464,21 +5475,21 @@
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="12">
         <v>2035</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="C77" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D77" s="12" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="E77" s="12" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="F77" s="12" t="s">
         <v>211</v>
@@ -5496,7 +5507,7 @@
         <v>43</v>
       </c>
       <c r="K77" s="12" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="L77" s="12">
         <v>20.55</v>
@@ -5523,21 +5534,21 @@
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="12">
         <v>2035</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C78" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D78" s="12" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="E78" s="12" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="F78" s="12" t="s">
         <v>211</v>
@@ -5549,13 +5560,13 @@
         <v>11</v>
       </c>
       <c r="I78" s="53" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="J78" s="13" t="s">
         <v>42</v>
       </c>
       <c r="K78" s="12" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="L78" s="12">
         <v>20.55</v>
@@ -5582,21 +5593,21 @@
         <v>75</v>
       </c>
     </row>
-    <row r="79" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:19" s="12" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A79" s="12">
         <v>2035</v>
       </c>
       <c r="B79" s="12" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="C79" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D79" s="12" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="E79" s="12" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="F79" s="12" t="s">
         <v>211</v>
@@ -5604,12 +5615,17 @@
       <c r="G79" s="12" t="s">
         <v>116</v>
       </c>
+      <c r="H79" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="I79" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="J79" s="13"/>
-      <c r="K79" s="12" t="s">
-        <v>267</v>
+      <c r="J79" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="K79" s="54" t="s">
+        <v>262</v>
       </c>
       <c r="L79" s="12">
         <v>20.55</v>
@@ -5636,7 +5652,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="80" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="24">
         <v>2050</v>
       </c>
@@ -5647,7 +5663,7 @@
         <v>113</v>
       </c>
       <c r="D80" s="24" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="E80" s="24" t="s">
         <v>114</v>
@@ -5698,8 +5714,9 @@
     <hyperlink ref="K7" r:id="rId1" xr:uid="{1BE7DD4C-B567-4320-9B69-E8B55CE41797}"/>
     <hyperlink ref="K8" r:id="rId2" xr:uid="{A52BF015-28DA-4569-A638-6E56CCBD2F4D}"/>
     <hyperlink ref="K9" r:id="rId3" xr:uid="{70B88B93-E906-4801-9012-B01BCDB48CBF}"/>
+    <hyperlink ref="K79" r:id="rId4" xr:uid="{66F560CD-5087-4DAA-A852-89E1F29FB2C6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update for 2035_TM160_IPA_13 with lower AOC
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD8BE10-FFEE-43B4-BE36-76AD73DD4EA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37DBB504-B48E-4463-ADD8-C524284CCFB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
+    <workbookView xWindow="1365" yWindow="5610" windowWidth="17010" windowHeight="8025" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelRuns" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="279">
   <si>
     <t>year</t>
   </si>
@@ -864,6 +864,15 @@
   </si>
   <si>
     <t>IPA v9 with PBA50 ixex</t>
+  </si>
+  <si>
+    <t>2035_TM160_IPA_13</t>
+  </si>
+  <si>
+    <t>IPA with lower AOC</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1206153405312420/f</t>
   </si>
 </sst>
 </file>
@@ -873,7 +882,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -913,14 +922,6 @@
       <color rgb="FFFF0000"/>
       <name val="Consolas"/>
       <family val="3"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="12">
@@ -1018,11 +1019,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1135,10 +1135,8 @@
     <xf numFmtId="2" fontId="2" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="4" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1451,34 +1449,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9564CC59-3725-4FDA-8BF2-0F68CB1B6F5A}">
-  <dimension ref="A1:S80"/>
+  <dimension ref="A1:S84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C59" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G69" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A79" sqref="A79"/>
+      <selection pane="bottomRight" activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="17" style="1" customWidth="1"/>
-    <col min="5" max="5" width="42.26953125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="42.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="23" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.1796875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="6.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.1796875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.26953125" style="10" customWidth="1"/>
-    <col min="11" max="11" width="17.54296875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="6.26953125" style="1" customWidth="1"/>
-    <col min="13" max="14" width="9.1796875" style="44"/>
-    <col min="15" max="16384" width="9.1796875" style="1"/>
+    <col min="7" max="7" width="8.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" style="10" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="6.28515625" style="1" customWidth="1"/>
+    <col min="13" max="14" width="9.140625" style="44"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="5" customFormat="1" ht="39" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1537,7 +1535,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="19">
         <v>2005</v>
       </c>
@@ -1564,7 +1562,7 @@
       <c r="Q2" s="23"/>
       <c r="R2" s="23"/>
     </row>
-    <row r="3" spans="1:19" s="32" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="31">
         <v>2005</v>
       </c>
@@ -1620,7 +1618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="32" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="31">
         <v>2005</v>
       </c>
@@ -1675,7 +1673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19" s="32" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="31">
         <v>2005</v>
       </c>
@@ -1727,7 +1725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="35">
         <v>2015</v>
       </c>
@@ -1773,7 +1771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="35">
         <v>2015</v>
       </c>
@@ -1826,7 +1824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="35">
         <v>2015</v>
       </c>
@@ -1879,7 +1877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="35">
         <v>2015</v>
       </c>
@@ -1932,7 +1930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="35">
         <v>2015</v>
       </c>
@@ -1991,7 +1989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="35">
         <v>2015</v>
       </c>
@@ -2047,7 +2045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>2023</v>
       </c>
@@ -2093,7 +2091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>2023</v>
       </c>
@@ -2139,7 +2137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>2023</v>
       </c>
@@ -2185,7 +2183,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>2023</v>
       </c>
@@ -2231,7 +2229,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>2023</v>
       </c>
@@ -2277,7 +2275,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>2023</v>
       </c>
@@ -2323,7 +2321,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>2023</v>
       </c>
@@ -2369,7 +2367,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>2023</v>
       </c>
@@ -2415,7 +2413,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>2023</v>
       </c>
@@ -2461,7 +2459,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>2023</v>
       </c>
@@ -2507,7 +2505,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>2023</v>
       </c>
@@ -2553,7 +2551,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>2023</v>
       </c>
@@ -2599,7 +2597,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>2023</v>
       </c>
@@ -2645,7 +2643,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>2023</v>
       </c>
@@ -2691,7 +2689,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>2023</v>
       </c>
@@ -2737,7 +2735,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>2023</v>
       </c>
@@ -2783,7 +2781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>2023</v>
       </c>
@@ -2829,7 +2827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>2023</v>
       </c>
@@ -2875,7 +2873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>2023</v>
       </c>
@@ -2919,7 +2917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>2023</v>
       </c>
@@ -2968,7 +2966,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>2023</v>
       </c>
@@ -3015,7 +3013,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>2023</v>
       </c>
@@ -3062,7 +3060,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>2023</v>
       </c>
@@ -3118,7 +3116,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>2023</v>
       </c>
@@ -3174,7 +3172,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>2023</v>
       </c>
@@ -3230,7 +3228,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>2023</v>
       </c>
@@ -3286,7 +3284,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>2023</v>
       </c>
@@ -3342,7 +3340,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>2023</v>
       </c>
@@ -3398,7 +3396,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>2023</v>
       </c>
@@ -3454,7 +3452,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>2023</v>
       </c>
@@ -3510,7 +3508,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>2023</v>
       </c>
@@ -3566,7 +3564,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>2023</v>
       </c>
@@ -3622,7 +3620,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>2023</v>
       </c>
@@ -3678,7 +3676,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>2023</v>
       </c>
@@ -3734,7 +3732,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>2023</v>
       </c>
@@ -3790,7 +3788,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>2023</v>
       </c>
@@ -3846,7 +3844,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>2023</v>
       </c>
@@ -3902,7 +3900,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>2023</v>
       </c>
@@ -3958,7 +3956,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>2023</v>
       </c>
@@ -4014,7 +4012,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>2023</v>
       </c>
@@ -4070,7 +4068,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>2023</v>
       </c>
@@ -4126,7 +4124,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>2023</v>
       </c>
@@ -4182,7 +4180,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>2023</v>
       </c>
@@ -4238,7 +4236,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>2023</v>
       </c>
@@ -4294,7 +4292,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>2023</v>
       </c>
@@ -4350,7 +4348,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>2023</v>
       </c>
@@ -4409,7 +4407,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="58" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="28">
         <v>2025</v>
       </c>
@@ -4440,7 +4438,7 @@
       <c r="R58" s="30"/>
       <c r="S58" s="30"/>
     </row>
-    <row r="59" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="15">
         <v>2035</v>
       </c>
@@ -4499,7 +4497,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="60" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="12">
         <v>2035</v>
       </c>
@@ -4555,7 +4553,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="61" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="12">
         <v>2035</v>
       </c>
@@ -4611,7 +4609,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="62" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="12">
         <v>2035</v>
       </c>
@@ -4667,7 +4665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="12">
         <v>2035</v>
       </c>
@@ -4723,7 +4721,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="64" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="12">
         <v>2035</v>
       </c>
@@ -4779,7 +4777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="12">
         <v>2035</v>
       </c>
@@ -4835,7 +4833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="12">
         <v>2035</v>
       </c>
@@ -4891,7 +4889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="12">
         <v>2035</v>
       </c>
@@ -4947,7 +4945,7 @@
         <v>41.25</v>
       </c>
     </row>
-    <row r="68" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="12">
         <v>2035</v>
       </c>
@@ -5003,7 +5001,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="69" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="12">
         <v>2035</v>
       </c>
@@ -5062,7 +5060,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="70" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="12">
         <v>2035</v>
       </c>
@@ -5121,7 +5119,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="71" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="12">
         <v>2035</v>
       </c>
@@ -5180,7 +5178,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="72" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="12">
         <v>2035</v>
       </c>
@@ -5239,7 +5237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="12">
         <v>2035</v>
       </c>
@@ -5298,7 +5296,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="74" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="12">
         <v>2035</v>
       </c>
@@ -5357,7 +5355,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="75" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="12">
         <v>2035</v>
       </c>
@@ -5416,7 +5414,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="12">
         <v>2035</v>
       </c>
@@ -5475,7 +5473,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="12">
         <v>2035</v>
       </c>
@@ -5534,7 +5532,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="12">
         <v>2035</v>
       </c>
@@ -5593,7 +5591,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="79" spans="1:19" s="12" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="12">
         <v>2035</v>
       </c>
@@ -5624,7 +5622,7 @@
       <c r="J79" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="K79" s="54" t="s">
+      <c r="K79" s="12" t="s">
         <v>262</v>
       </c>
       <c r="L79" s="12">
@@ -5652,60 +5650,139 @@
         <v>75</v>
       </c>
     </row>
-    <row r="80" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="24">
+    <row r="80" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B80" s="12" t="s">
+        <v>276</v>
+      </c>
+      <c r="C80" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D80" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="E80" s="12" t="s">
+        <v>277</v>
+      </c>
+      <c r="F80" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="G80" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="H80" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I80" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="J80" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K80" s="12" t="s">
+        <v>278</v>
+      </c>
+      <c r="L80" s="53">
+        <v>13.68</v>
+      </c>
+      <c r="M80" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="N80" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="O80" s="12">
+        <v>0.87</v>
+      </c>
+      <c r="P80" s="12">
+        <v>0.78</v>
+      </c>
+      <c r="Q80" s="14">
+        <v>100</v>
+      </c>
+      <c r="R80" s="14">
+        <v>0</v>
+      </c>
+      <c r="S80" s="14">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="24">
         <v>2050</v>
       </c>
-      <c r="B80" s="24" t="s">
+      <c r="B81" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="C80" s="24" t="s">
+      <c r="C81" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="D80" s="24" t="s">
+      <c r="D81" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="E80" s="24" t="s">
+      <c r="E81" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="F80" s="24" t="s">
+      <c r="F81" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="G80" s="25" t="s">
+      <c r="G81" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="I80" s="24" t="s">
+      <c r="I81" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="J80" s="26" t="s">
+      <c r="J81" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="K80" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="L80" s="24">
+      <c r="K81" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="L81" s="24">
         <v>17.440000000000001</v>
       </c>
-      <c r="M80" s="48">
+      <c r="M81" s="48">
         <v>-0.33</v>
       </c>
-      <c r="N80" s="48">
-        <v>0</v>
-      </c>
-      <c r="O80" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="P80" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q80" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="R80" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="S80" s="27" t="s">
-        <v>109</v>
+      <c r="N81" s="48">
+        <v>0</v>
+      </c>
+      <c r="O81" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="P81" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q81" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="R81" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="S81" s="27" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="83" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="L83" s="1">
+        <f>L80*2</f>
+        <v>27.36</v>
+      </c>
+      <c r="M83" s="44">
+        <f>L79*2</f>
+        <v>41.1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="L84" s="1">
+        <f>L80*3</f>
+        <v>41.04</v>
+      </c>
+      <c r="M84" s="44">
+        <f>L79*3</f>
+        <v>61.650000000000006</v>
       </c>
     </row>
   </sheetData>
@@ -5714,9 +5791,8 @@
     <hyperlink ref="K7" r:id="rId1" xr:uid="{1BE7DD4C-B567-4320-9B69-E8B55CE41797}"/>
     <hyperlink ref="K8" r:id="rId2" xr:uid="{A52BF015-28DA-4569-A638-6E56CCBD2F4D}"/>
     <hyperlink ref="K9" r:id="rId3" xr:uid="{70B88B93-E906-4801-9012-B01BCDB48CBF}"/>
-    <hyperlink ref="K79" r:id="rId4" xr:uid="{66F560CD-5087-4DAA-A852-89E1F29FB2C6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update for 2035_TM160_IPA_14 with non-fuel AOC fix
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37DBB504-B48E-4463-ADD8-C524284CCFB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9832675-6486-4B09-A540-D6113A1FB1A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1365" yWindow="5610" windowWidth="17010" windowHeight="8025" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="17010" windowHeight="9855" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelRuns" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="283">
   <si>
     <t>year</t>
   </si>
@@ -767,12 +767,6 @@
     <t>https://app.asana.com/0/1204085012544660/1205995415086639/f</t>
   </si>
   <si>
-    <t>2015 land use</t>
-  </si>
-  <si>
-    <t>RTP2021_IP</t>
-  </si>
-  <si>
     <t>IPA</t>
   </si>
   <si>
@@ -873,6 +867,24 @@
   </si>
   <si>
     <t>https://app.asana.com/0/1204085012544660/1206153405312420/f</t>
+  </si>
+  <si>
+    <t>2005 land use</t>
+  </si>
+  <si>
+    <t>2015_TM152_IPA_17</t>
+  </si>
+  <si>
+    <t>RTP21 2015 run</t>
+  </si>
+  <si>
+    <t>IPA with lower AOC and non-fuel fix</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1206165621445907/f</t>
+  </si>
+  <si>
+    <t>2035_TM160_IPA_14</t>
   </si>
 </sst>
 </file>
@@ -924,7 +936,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -991,6 +1003,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -1022,7 +1040,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1135,6 +1153,17 @@
     <xf numFmtId="2" fontId="2" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="4" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1449,13 +1478,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9564CC59-3725-4FDA-8BF2-0F68CB1B6F5A}">
-  <dimension ref="A1:S84"/>
+  <dimension ref="A1:S86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="G69" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C71" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A80" sqref="A80"/>
+      <selection pane="bottomRight" activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1543,24 +1572,49 @@
         <v>125</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>244</v>
+        <v>113</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E2" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
+      <c r="F2" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>10</v>
+      </c>
       <c r="H2" s="20"/>
+      <c r="I2" s="21" t="s">
+        <v>224</v>
+      </c>
       <c r="J2" s="22"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
-      <c r="Q2" s="23"/>
-      <c r="R2" s="23"/>
+      <c r="L2" s="21">
+        <v>14.87</v>
+      </c>
+      <c r="M2" s="40" t="s">
+        <v>109</v>
+      </c>
+      <c r="N2" s="40" t="s">
+        <v>109</v>
+      </c>
+      <c r="O2" s="23">
+        <v>0</v>
+      </c>
+      <c r="P2" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="23">
+        <v>0</v>
+      </c>
+      <c r="R2" s="23">
+        <v>0</v>
+      </c>
+      <c r="S2" s="23">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:19" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="31">
@@ -1573,13 +1627,13 @@
         <v>17</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>150</v>
       </c>
       <c r="F3" s="32" t="s">
-        <v>243</v>
+        <v>277</v>
       </c>
       <c r="G3" s="32" t="s">
         <v>10</v>
@@ -1629,13 +1683,13 @@
         <v>17</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E4" s="32" t="s">
         <v>223</v>
       </c>
       <c r="F4" s="32" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G4" s="32" t="s">
         <v>10</v>
@@ -1678,19 +1732,19 @@
         <v>2005</v>
       </c>
       <c r="B5" s="32" t="s">
+        <v>265</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>247</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="F5" s="32" t="s">
         <v>267</v>
-      </c>
-      <c r="C5" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="32" t="s">
-        <v>249</v>
-      </c>
-      <c r="E5" s="32" t="s">
-        <v>268</v>
-      </c>
-      <c r="F5" s="32" t="s">
-        <v>269</v>
       </c>
       <c r="G5" s="32" t="s">
         <v>10</v>
@@ -1702,7 +1756,7 @@
         <v>43</v>
       </c>
       <c r="K5" s="32" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="L5" s="32">
         <v>14.87</v>
@@ -1725,49 +1779,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="35">
+    <row r="6" spans="1:19" s="55" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="54">
         <v>2015</v>
       </c>
-      <c r="B6" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="36" t="s">
-        <v>248</v>
-      </c>
-      <c r="E6" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="36" t="s">
+      <c r="B6" s="55" t="s">
+        <v>278</v>
+      </c>
+      <c r="C6" s="55" t="s">
+        <v>113</v>
+      </c>
+      <c r="D6" s="55" t="s">
+        <v>246</v>
+      </c>
+      <c r="E6" s="55" t="s">
+        <v>279</v>
+      </c>
+      <c r="F6" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="K6" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="M6" s="42">
+      <c r="G6" s="55" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="56"/>
+      <c r="L6" s="55">
+        <v>13.73</v>
+      </c>
+      <c r="M6" s="57">
         <v>-0.09</v>
       </c>
-      <c r="N6" s="42">
+      <c r="N6" s="57">
         <v>0.9</v>
       </c>
-      <c r="O6" s="38"/>
-      <c r="P6" s="38"/>
-      <c r="Q6" s="38">
-        <v>0</v>
-      </c>
-      <c r="R6" s="38">
+      <c r="O6" s="58"/>
+      <c r="P6" s="58"/>
+      <c r="Q6" s="58">
+        <v>0</v>
+      </c>
+      <c r="R6" s="58">
         <v>0</v>
       </c>
     </row>
@@ -1776,16 +1825,16 @@
         <v>2015</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>145</v>
+        <v>8</v>
       </c>
       <c r="C7" s="36" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="36" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E7" s="36" t="s">
-        <v>149</v>
+        <v>19</v>
       </c>
       <c r="F7" s="36" t="s">
         <v>9</v>
@@ -1794,33 +1843,26 @@
         <v>10</v>
       </c>
       <c r="I7" s="36" t="s">
-        <v>146</v>
+        <v>13</v>
       </c>
       <c r="J7" s="37" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="K7" s="36" t="s">
-        <v>147</v>
-      </c>
-      <c r="M7" s="42" t="s">
-        <v>109</v>
-      </c>
-      <c r="N7" s="42" t="s">
-        <v>109</v>
-      </c>
-      <c r="O7" s="38">
-        <v>0</v>
-      </c>
-      <c r="P7" s="38">
-        <v>0</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="M7" s="42">
+        <v>-0.09</v>
+      </c>
+      <c r="N7" s="42">
+        <v>0.9</v>
+      </c>
+      <c r="O7" s="38"/>
+      <c r="P7" s="38"/>
       <c r="Q7" s="38">
         <v>0</v>
       </c>
       <c r="R7" s="38">
-        <v>0</v>
-      </c>
-      <c r="S7" s="38">
         <v>0</v>
       </c>
     </row>
@@ -1829,16 +1871,16 @@
         <v>2015</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C8" s="36" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="36" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E8" s="36" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="F8" s="36" t="s">
         <v>9</v>
@@ -1862,10 +1904,10 @@
         <v>109</v>
       </c>
       <c r="O8" s="38">
-        <v>0.32</v>
+        <v>0</v>
       </c>
       <c r="P8" s="38">
-        <v>0.28000000000000003</v>
+        <v>0</v>
       </c>
       <c r="Q8" s="38">
         <v>0</v>
@@ -1882,13 +1924,13 @@
         <v>2015</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C9" s="36" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="36" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E9" s="36" t="s">
         <v>153</v>
@@ -1935,16 +1977,16 @@
         <v>2015</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C10" s="36" t="s">
         <v>17</v>
       </c>
       <c r="D10" s="36" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E10" s="36" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F10" s="36" t="s">
         <v>9</v>
@@ -1952,20 +1994,14 @@
       <c r="G10" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="36" t="s">
-        <v>11</v>
-      </c>
       <c r="I10" s="36" t="s">
         <v>146</v>
       </c>
       <c r="J10" s="37" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="K10" s="36" t="s">
-        <v>158</v>
-      </c>
-      <c r="L10" s="51">
-        <v>15.1</v>
+        <v>147</v>
       </c>
       <c r="M10" s="42" t="s">
         <v>109</v>
@@ -1974,10 +2010,10 @@
         <v>109</v>
       </c>
       <c r="O10" s="38">
-        <v>0.32300000000000001</v>
-      </c>
-      <c r="P10" s="49">
-        <v>0.83099999999999996</v>
+        <v>0.32</v>
+      </c>
+      <c r="P10" s="38">
+        <v>0.28000000000000003</v>
       </c>
       <c r="Q10" s="38">
         <v>0</v>
@@ -1994,16 +2030,16 @@
         <v>2015</v>
       </c>
       <c r="B11" s="36" t="s">
-        <v>213</v>
+        <v>156</v>
       </c>
       <c r="C11" s="36" t="s">
         <v>17</v>
       </c>
       <c r="D11" s="36" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E11" s="36" t="s">
-        <v>215</v>
+        <v>157</v>
       </c>
       <c r="F11" s="36" t="s">
         <v>9</v>
@@ -2011,6 +2047,9 @@
       <c r="G11" s="36" t="s">
         <v>10</v>
       </c>
+      <c r="H11" s="36" t="s">
+        <v>11</v>
+      </c>
       <c r="I11" s="36" t="s">
         <v>146</v>
       </c>
@@ -2018,10 +2057,10 @@
         <v>16</v>
       </c>
       <c r="K11" s="36" t="s">
-        <v>214</v>
-      </c>
-      <c r="L11" s="36">
-        <v>13.73</v>
+        <v>158</v>
+      </c>
+      <c r="L11" s="51">
+        <v>15.1</v>
       </c>
       <c r="M11" s="42" t="s">
         <v>109</v>
@@ -2045,49 +2084,59 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <v>2023</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="1" t="s">
+    <row r="12" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="35">
+        <v>2015</v>
+      </c>
+      <c r="B12" s="36" t="s">
+        <v>213</v>
+      </c>
+      <c r="C12" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="36" t="s">
+        <v>246</v>
+      </c>
+      <c r="E12" s="36" t="s">
+        <v>215</v>
+      </c>
+      <c r="F12" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J12" s="9" t="s">
+      <c r="G12" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="36" t="s">
+        <v>146</v>
+      </c>
+      <c r="J12" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="K12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M12" s="43">
-        <v>-0.44</v>
-      </c>
-      <c r="N12" s="43">
-        <v>-0.23</v>
-      </c>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6">
-        <v>0</v>
-      </c>
-      <c r="R12" s="6">
+      <c r="K12" s="36" t="s">
+        <v>214</v>
+      </c>
+      <c r="L12" s="36">
+        <v>13.73</v>
+      </c>
+      <c r="M12" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="N12" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="O12" s="38">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="P12" s="49">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="Q12" s="38">
+        <v>0</v>
+      </c>
+      <c r="R12" s="38">
+        <v>0</v>
+      </c>
+      <c r="S12" s="38">
         <v>0</v>
       </c>
     </row>
@@ -2096,16 +2145,16 @@
         <v>2023</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>9</v>
@@ -2120,18 +2169,18 @@
         <v>16</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M13" s="43">
-        <v>-1.25</v>
+        <v>-0.44</v>
       </c>
       <c r="N13" s="43">
-        <v>-0.75</v>
+        <v>-0.23</v>
       </c>
       <c r="O13" s="6"/>
       <c r="P13" s="6"/>
       <c r="Q13" s="6">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="R13" s="6">
         <v>0</v>
@@ -2142,16 +2191,16 @@
         <v>2023</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>9</v>
@@ -2160,13 +2209,13 @@
         <v>10</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="J14" s="9" t="s">
         <v>16</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="M14" s="43">
         <v>-1.25</v>
@@ -2177,10 +2226,10 @@
       <c r="O14" s="6"/>
       <c r="P14" s="6"/>
       <c r="Q14" s="6">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="R14" s="6">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
@@ -2188,16 +2237,16 @@
         <v>2023</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>9</v>
@@ -2206,13 +2255,13 @@
         <v>10</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="J15" s="9" t="s">
         <v>16</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="M15" s="43">
         <v>-1.25</v>
@@ -2223,7 +2272,7 @@
       <c r="O15" s="6"/>
       <c r="P15" s="6"/>
       <c r="Q15" s="6">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="R15" s="6">
         <v>15</v>
@@ -2234,16 +2283,16 @@
         <v>2023</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>9</v>
@@ -2258,7 +2307,7 @@
         <v>16</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="M16" s="43">
         <v>-1.25</v>
@@ -2268,10 +2317,10 @@
       </c>
       <c r="O16" s="6"/>
       <c r="P16" s="6"/>
-      <c r="Q16" s="11">
+      <c r="Q16" s="6">
         <v>75</v>
       </c>
-      <c r="R16" s="11">
+      <c r="R16" s="6">
         <v>15</v>
       </c>
     </row>
@@ -2280,16 +2329,16 @@
         <v>2023</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>9</v>
@@ -2301,10 +2350,10 @@
         <v>32</v>
       </c>
       <c r="J17" s="9" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="M17" s="43">
         <v>-1.25</v>
@@ -2314,10 +2363,10 @@
       </c>
       <c r="O17" s="6"/>
       <c r="P17" s="6"/>
-      <c r="Q17" s="7">
-        <v>85</v>
-      </c>
-      <c r="R17" s="7">
+      <c r="Q17" s="11">
+        <v>75</v>
+      </c>
+      <c r="R17" s="11">
         <v>15</v>
       </c>
     </row>
@@ -2326,13 +2375,13 @@
         <v>2023</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>46</v>
@@ -2347,7 +2396,7 @@
         <v>32</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>45</v>
@@ -2361,7 +2410,7 @@
       <c r="O18" s="6"/>
       <c r="P18" s="6"/>
       <c r="Q18" s="7">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="R18" s="7">
         <v>15</v>
@@ -2372,13 +2421,13 @@
         <v>2023</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>46</v>
@@ -2393,7 +2442,7 @@
         <v>32</v>
       </c>
       <c r="J19" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>45</v>
@@ -2407,10 +2456,10 @@
       <c r="O19" s="6"/>
       <c r="P19" s="6"/>
       <c r="Q19" s="7">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="R19" s="7">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.2">
@@ -2418,16 +2467,16 @@
         <v>2023</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>9</v>
@@ -2436,13 +2485,13 @@
         <v>10</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="J20" s="10" t="s">
-        <v>42</v>
+        <v>32</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="M20" s="43">
         <v>-1.25</v>
@@ -2464,16 +2513,16 @@
         <v>2023</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>9</v>
@@ -2482,13 +2531,13 @@
         <v>10</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="J21" s="10" t="s">
         <v>42</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="M21" s="43">
         <v>-1.25</v>
@@ -2499,7 +2548,7 @@
       <c r="O21" s="6"/>
       <c r="P21" s="6"/>
       <c r="Q21" s="7">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="R21" s="7">
         <v>30</v>
@@ -2510,16 +2559,16 @@
         <v>2023</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>9</v>
@@ -2531,7 +2580,7 @@
         <v>53</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>56</v>
@@ -2545,7 +2594,7 @@
       <c r="O22" s="6"/>
       <c r="P22" s="6"/>
       <c r="Q22" s="7">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="R22" s="7">
         <v>30</v>
@@ -2556,16 +2605,16 @@
         <v>2023</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>9</v>
@@ -2574,13 +2623,13 @@
         <v>10</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="J23" s="10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="M23" s="43">
         <v>-1.25</v>
@@ -2591,10 +2640,10 @@
       <c r="O23" s="6"/>
       <c r="P23" s="6"/>
       <c r="Q23" s="7">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="R23" s="7">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.2">
@@ -2602,16 +2651,16 @@
         <v>2023</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>9</v>
@@ -2626,7 +2675,7 @@
         <v>42</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="M24" s="43">
         <v>-1.25</v>
@@ -2637,10 +2686,10 @@
       <c r="O24" s="6"/>
       <c r="P24" s="6"/>
       <c r="Q24" s="7">
-        <v>300</v>
+        <v>180</v>
       </c>
       <c r="R24" s="7">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.2">
@@ -2648,13 +2697,13 @@
         <v>2023</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>62</v>
@@ -2683,7 +2732,7 @@
       <c r="O25" s="6"/>
       <c r="P25" s="6"/>
       <c r="Q25" s="7">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="R25" s="7">
         <v>5</v>
@@ -2694,13 +2743,13 @@
         <v>2023</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>62</v>
@@ -2729,7 +2778,7 @@
       <c r="O26" s="6"/>
       <c r="P26" s="6"/>
       <c r="Q26" s="7">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="R26" s="7">
         <v>5</v>
@@ -2740,16 +2789,16 @@
         <v>2023</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>9</v>
@@ -2758,13 +2807,13 @@
         <v>10</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="J27" s="10" t="s">
         <v>42</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M27" s="43">
         <v>-1.25</v>
@@ -2775,10 +2824,10 @@
       <c r="O27" s="6"/>
       <c r="P27" s="6"/>
       <c r="Q27" s="7">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="R27" s="7">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.2">
@@ -2786,16 +2835,16 @@
         <v>2023</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>9</v>
@@ -2804,13 +2853,13 @@
         <v>10</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="J28" s="10" t="s">
         <v>42</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="M28" s="43">
         <v>-1.25</v>
@@ -2832,16 +2881,16 @@
         <v>2023</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>9</v>
@@ -2850,13 +2899,13 @@
         <v>10</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="J29" s="10" t="s">
         <v>42</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="M29" s="43">
         <v>-1.25</v>
@@ -2878,16 +2927,16 @@
         <v>2023</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>9</v>
@@ -2899,17 +2948,19 @@
         <v>79</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>88</v>
+        <v>42</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="O30" s="6">
-        <v>1.27</v>
-      </c>
-      <c r="P30" s="6">
-        <v>1.1499999999999999</v>
-      </c>
+      <c r="M30" s="43">
+        <v>-1.25</v>
+      </c>
+      <c r="N30" s="43">
+        <v>-0.75</v>
+      </c>
+      <c r="O30" s="6"/>
+      <c r="P30" s="6"/>
       <c r="Q30" s="7">
         <v>120</v>
       </c>
@@ -2922,16 +2973,16 @@
         <v>2023</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>9</v>
@@ -2943,27 +2994,22 @@
         <v>79</v>
       </c>
       <c r="J31" s="10" t="s">
-        <v>42</v>
+        <v>88</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="M31" s="43">
-        <v>-1.25</v>
-      </c>
-      <c r="N31" s="43">
-        <v>-0.75</v>
-      </c>
-      <c r="O31" s="6"/>
-      <c r="P31" s="6"/>
+        <v>81</v>
+      </c>
+      <c r="O31" s="6">
+        <v>1.27</v>
+      </c>
+      <c r="P31" s="6">
+        <v>1.1499999999999999</v>
+      </c>
       <c r="Q31" s="7">
         <v>120</v>
       </c>
       <c r="R31" s="7">
         <v>0</v>
-      </c>
-      <c r="S31" s="7">
-        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.2">
@@ -2971,13 +3017,13 @@
         <v>2023</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>87</v>
@@ -2992,17 +3038,19 @@
         <v>79</v>
       </c>
       <c r="J32" s="10" t="s">
-        <v>88</v>
+        <v>42</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="O32" s="6">
-        <v>1.27</v>
-      </c>
-      <c r="P32" s="6">
-        <v>1.1499999999999999</v>
-      </c>
+      <c r="M32" s="43">
+        <v>-1.25</v>
+      </c>
+      <c r="N32" s="43">
+        <v>-0.75</v>
+      </c>
+      <c r="O32" s="6"/>
+      <c r="P32" s="6"/>
       <c r="Q32" s="7">
         <v>120</v>
       </c>
@@ -3018,16 +3066,16 @@
         <v>2023</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>9</v>
@@ -3039,16 +3087,16 @@
         <v>79</v>
       </c>
       <c r="J33" s="10" t="s">
-        <v>42</v>
+        <v>88</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="M33" s="43">
-        <v>-1.25</v>
-      </c>
-      <c r="N33" s="43">
-        <v>-0.75</v>
+        <v>89</v>
+      </c>
+      <c r="O33" s="6">
+        <v>1.27</v>
+      </c>
+      <c r="P33" s="6">
+        <v>1.1499999999999999</v>
       </c>
       <c r="Q33" s="7">
         <v>120</v>
@@ -3057,7 +3105,7 @@
         <v>0</v>
       </c>
       <c r="S33" s="7">
-        <v>45</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.2">
@@ -3065,13 +3113,13 @@
         <v>2023</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>92</v>
@@ -3086,25 +3134,16 @@
         <v>79</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>88</v>
+        <v>42</v>
       </c>
       <c r="K34" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="L34" s="1">
-        <v>17.77</v>
-      </c>
-      <c r="M34" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="N34" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O34" s="6">
-        <v>1.27</v>
-      </c>
-      <c r="P34" s="6">
-        <v>1.1499999999999999</v>
+      <c r="M34" s="43">
+        <v>-1.25</v>
+      </c>
+      <c r="N34" s="43">
+        <v>-0.75</v>
       </c>
       <c r="Q34" s="7">
         <v>120</v>
@@ -3121,16 +3160,16 @@
         <v>2023</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>9</v>
@@ -3142,10 +3181,10 @@
         <v>79</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>42</v>
+        <v>88</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="L35" s="1">
         <v>17.77</v>
@@ -3156,11 +3195,11 @@
       <c r="N35" s="44" t="s">
         <v>109</v>
       </c>
-      <c r="O35" s="1">
-        <v>0.64</v>
-      </c>
-      <c r="P35" s="1">
-        <v>0.57999999999999996</v>
+      <c r="O35" s="6">
+        <v>1.27</v>
+      </c>
+      <c r="P35" s="6">
+        <v>1.1499999999999999</v>
       </c>
       <c r="Q35" s="7">
         <v>120</v>
@@ -3177,16 +3216,16 @@
         <v>2023</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>152</v>
+        <v>96</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>9</v>
@@ -3198,10 +3237,10 @@
         <v>79</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>88</v>
+        <v>42</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L36" s="1">
         <v>17.77</v>
@@ -3213,18 +3252,18 @@
         <v>109</v>
       </c>
       <c r="O36" s="1">
-        <v>0.95</v>
+        <v>0.64</v>
       </c>
       <c r="P36" s="1">
-        <v>0.86</v>
-      </c>
-      <c r="Q36" s="6">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="Q36" s="7">
         <v>120</v>
       </c>
-      <c r="R36" s="6">
-        <v>0</v>
-      </c>
-      <c r="S36" s="6">
+      <c r="R36" s="7">
+        <v>0</v>
+      </c>
+      <c r="S36" s="7">
         <v>45</v>
       </c>
     </row>
@@ -3233,16 +3272,16 @@
         <v>2023</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>138</v>
+        <v>95</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>133</v>
+        <v>152</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>9</v>
@@ -3254,10 +3293,10 @@
         <v>79</v>
       </c>
       <c r="J37" s="10" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="L37" s="1">
         <v>17.77</v>
@@ -3275,13 +3314,13 @@
         <v>0.86</v>
       </c>
       <c r="Q37" s="6">
-        <v>200</v>
+        <v>120</v>
       </c>
       <c r="R37" s="6">
         <v>0</v>
       </c>
       <c r="S37" s="6">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.2">
@@ -3289,16 +3328,16 @@
         <v>2023</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>9</v>
@@ -3310,10 +3349,10 @@
         <v>79</v>
       </c>
       <c r="J38" s="10" t="s">
-        <v>88</v>
+        <v>43</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="L38" s="1">
         <v>17.77</v>
@@ -3331,7 +3370,7 @@
         <v>0.86</v>
       </c>
       <c r="Q38" s="6">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="R38" s="6">
         <v>0</v>
@@ -3345,16 +3384,16 @@
         <v>2023</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>9</v>
@@ -3366,10 +3405,10 @@
         <v>79</v>
       </c>
       <c r="J39" s="10" t="s">
-        <v>129</v>
+        <v>88</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L39" s="1">
         <v>17.77</v>
@@ -3381,10 +3420,10 @@
         <v>109</v>
       </c>
       <c r="O39" s="1">
-        <v>0.39</v>
+        <v>0.95</v>
       </c>
       <c r="P39" s="1">
-        <v>0.35</v>
+        <v>0.86</v>
       </c>
       <c r="Q39" s="6">
         <v>300</v>
@@ -3401,16 +3440,16 @@
         <v>2023</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>9</v>
@@ -3422,10 +3461,10 @@
         <v>79</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>43</v>
+        <v>129</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="L40" s="1">
         <v>17.77</v>
@@ -3437,19 +3476,19 @@
         <v>109</v>
       </c>
       <c r="O40" s="1">
-        <v>0.77</v>
+        <v>0.39</v>
       </c>
       <c r="P40" s="1">
-        <v>0.69</v>
+        <v>0.35</v>
       </c>
       <c r="Q40" s="6">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="R40" s="6">
         <v>0</v>
       </c>
       <c r="S40" s="6">
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.2">
@@ -3457,16 +3496,16 @@
         <v>2023</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>9</v>
@@ -3478,10 +3517,10 @@
         <v>79</v>
       </c>
       <c r="J41" s="10" t="s">
-        <v>129</v>
+        <v>43</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
       <c r="L41" s="1">
         <v>17.77</v>
@@ -3493,19 +3532,19 @@
         <v>109</v>
       </c>
       <c r="O41" s="1">
-        <v>0.94</v>
+        <v>0.77</v>
       </c>
       <c r="P41" s="1">
-        <v>0.85499999999999998</v>
+        <v>0.69</v>
       </c>
       <c r="Q41" s="6">
-        <v>120</v>
+        <v>400</v>
       </c>
       <c r="R41" s="6">
         <v>0</v>
       </c>
       <c r="S41" s="6">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.2">
@@ -3513,16 +3552,16 @@
         <v>2023</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>9</v>
@@ -3531,7 +3570,7 @@
         <v>10</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>163</v>
+        <v>79</v>
       </c>
       <c r="J42" s="10" t="s">
         <v>129</v>
@@ -3569,16 +3608,16 @@
         <v>2023</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>9</v>
@@ -3625,16 +3664,16 @@
         <v>2023</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>9</v>
@@ -3646,10 +3685,10 @@
         <v>163</v>
       </c>
       <c r="J44" s="10" t="s">
-        <v>16</v>
+        <v>129</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="L44" s="1">
         <v>17.77</v>
@@ -3680,17 +3719,17 @@
       <c r="A45" s="1">
         <v>2023</v>
       </c>
-      <c r="B45" s="50" t="s">
-        <v>170</v>
+      <c r="B45" s="1" t="s">
+        <v>167</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>9</v>
@@ -3699,13 +3738,13 @@
         <v>10</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="J45" s="10" t="s">
         <v>16</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="L45" s="1">
         <v>17.77</v>
@@ -3736,17 +3775,17 @@
       <c r="A46" s="1">
         <v>2023</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>174</v>
+      <c r="B46" s="50" t="s">
+        <v>170</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>199</v>
+        <v>171</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>9</v>
@@ -3761,7 +3800,7 @@
         <v>16</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="L46" s="1">
         <v>17.77</v>
@@ -3773,10 +3812,10 @@
         <v>109</v>
       </c>
       <c r="O46" s="1">
-        <v>0.99</v>
+        <v>0.94</v>
       </c>
       <c r="P46" s="1">
-        <v>0.89</v>
+        <v>0.85499999999999998</v>
       </c>
       <c r="Q46" s="6">
         <v>120</v>
@@ -3793,16 +3832,16 @@
         <v>2023</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>9</v>
@@ -3811,13 +3850,13 @@
         <v>10</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="J47" s="10" t="s">
         <v>16</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="L47" s="1">
         <v>17.77</v>
@@ -3849,16 +3888,16 @@
         <v>2023</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>9</v>
@@ -3870,10 +3909,10 @@
         <v>177</v>
       </c>
       <c r="J48" s="10" t="s">
-        <v>110</v>
+        <v>16</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L48" s="1">
         <v>17.77</v>
@@ -3885,10 +3924,10 @@
         <v>109</v>
       </c>
       <c r="O48" s="1">
-        <v>1.04</v>
+        <v>0.99</v>
       </c>
       <c r="P48" s="1">
-        <v>0.94</v>
+        <v>0.89</v>
       </c>
       <c r="Q48" s="6">
         <v>120</v>
@@ -3904,17 +3943,17 @@
       <c r="A49" s="1">
         <v>2023</v>
       </c>
-      <c r="B49" s="50" t="s">
-        <v>181</v>
+      <c r="B49" s="1" t="s">
+        <v>180</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>9</v>
@@ -3926,10 +3965,10 @@
         <v>177</v>
       </c>
       <c r="J49" s="10" t="s">
-        <v>44</v>
+        <v>110</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="L49" s="1">
         <v>17.77</v>
@@ -3941,36 +3980,36 @@
         <v>109</v>
       </c>
       <c r="O49" s="1">
-        <v>0.99</v>
+        <v>1.04</v>
       </c>
       <c r="P49" s="1">
-        <v>0.89</v>
+        <v>0.94</v>
       </c>
       <c r="Q49" s="6">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="R49" s="6">
         <v>0</v>
       </c>
       <c r="S49" s="6">
-        <v>60</v>
+        <v>45</v>
       </c>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>2023</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>183</v>
+      <c r="B50" s="50" t="s">
+        <v>181</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>9</v>
@@ -3982,10 +4021,10 @@
         <v>177</v>
       </c>
       <c r="J50" s="10" t="s">
-        <v>129</v>
+        <v>44</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="L50" s="1">
         <v>17.77</v>
@@ -3997,10 +4036,10 @@
         <v>109</v>
       </c>
       <c r="O50" s="1">
-        <v>1.04</v>
+        <v>0.99</v>
       </c>
       <c r="P50" s="1">
-        <v>0.94</v>
+        <v>0.89</v>
       </c>
       <c r="Q50" s="6">
         <v>100</v>
@@ -4017,16 +4056,16 @@
         <v>2023</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>9</v>
@@ -4038,10 +4077,10 @@
         <v>177</v>
       </c>
       <c r="J51" s="10" t="s">
-        <v>43</v>
+        <v>129</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="L51" s="1">
         <v>17.77</v>
@@ -4053,19 +4092,19 @@
         <v>109</v>
       </c>
       <c r="O51" s="1">
-        <v>0.99</v>
+        <v>1.04</v>
       </c>
       <c r="P51" s="1">
-        <v>0.89</v>
+        <v>0.94</v>
       </c>
       <c r="Q51" s="6">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="R51" s="6">
         <v>0</v>
       </c>
       <c r="S51" s="6">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.2">
@@ -4073,16 +4112,16 @@
         <v>2023</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>9</v>
@@ -4094,10 +4133,10 @@
         <v>177</v>
       </c>
       <c r="J52" s="10" t="s">
-        <v>88</v>
+        <v>43</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="L52" s="1">
         <v>17.77</v>
@@ -4109,10 +4148,10 @@
         <v>109</v>
       </c>
       <c r="O52" s="1">
-        <v>1.04</v>
+        <v>0.99</v>
       </c>
       <c r="P52" s="1">
-        <v>0.94</v>
+        <v>0.89</v>
       </c>
       <c r="Q52" s="6">
         <v>90</v>
@@ -4129,16 +4168,16 @@
         <v>2023</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>9</v>
@@ -4150,10 +4189,10 @@
         <v>177</v>
       </c>
       <c r="J53" s="10" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="L53" s="1">
         <v>17.77</v>
@@ -4165,19 +4204,19 @@
         <v>109</v>
       </c>
       <c r="O53" s="1">
-        <v>0.99</v>
+        <v>1.04</v>
       </c>
       <c r="P53" s="1">
-        <v>0.89</v>
+        <v>0.94</v>
       </c>
       <c r="Q53" s="6">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="R53" s="6">
         <v>0</v>
       </c>
       <c r="S53" s="6">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.2">
@@ -4185,13 +4224,13 @@
         <v>2023</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>192</v>
@@ -4209,7 +4248,7 @@
         <v>110</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="L54" s="1">
         <v>17.77</v>
@@ -4233,7 +4272,7 @@
         <v>0</v>
       </c>
       <c r="S54" s="6">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.2">
@@ -4241,16 +4280,16 @@
         <v>2023</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>9</v>
@@ -4262,13 +4301,13 @@
         <v>177</v>
       </c>
       <c r="J55" s="10" t="s">
-        <v>43</v>
+        <v>110</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="L55" s="1">
-        <v>16.45</v>
+        <v>17.77</v>
       </c>
       <c r="M55" s="44" t="s">
         <v>109</v>
@@ -4297,16 +4336,16 @@
         <v>2023</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>9</v>
@@ -4321,10 +4360,10 @@
         <v>43</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="L56" s="1">
-        <v>16.61</v>
+        <v>16.45</v>
       </c>
       <c r="M56" s="44" t="s">
         <v>109</v>
@@ -4353,16 +4392,16 @@
         <v>2023</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>9</v>
@@ -4370,17 +4409,14 @@
       <c r="G57" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H57" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="I57" s="1" t="s">
         <v>177</v>
       </c>
       <c r="J57" s="10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="L57" s="1">
         <v>16.61</v>
@@ -4392,10 +4428,10 @@
         <v>109</v>
       </c>
       <c r="O57" s="1">
-        <v>1.04</v>
+        <v>0.99</v>
       </c>
       <c r="P57" s="1">
-        <v>0.94</v>
+        <v>0.89</v>
       </c>
       <c r="Q57" s="6">
         <v>100</v>
@@ -4407,150 +4443,153 @@
         <v>75</v>
       </c>
     </row>
-    <row r="58" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="28">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="J58" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="L58" s="1">
+        <v>16.61</v>
+      </c>
+      <c r="M58" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="N58" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="O58" s="1">
+        <v>1.04</v>
+      </c>
+      <c r="P58" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="Q58" s="6">
+        <v>100</v>
+      </c>
+      <c r="R58" s="6">
+        <v>0</v>
+      </c>
+      <c r="S58" s="6">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="28">
         <v>2025</v>
       </c>
-      <c r="B58" s="28" t="s">
+      <c r="B59" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="C58" s="28" t="s">
+      <c r="C59" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="D58" s="28" t="s">
-        <v>246</v>
-      </c>
-      <c r="E58" s="28" t="s">
+      <c r="D59" s="28" t="s">
+        <v>244</v>
+      </c>
+      <c r="E59" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="H58" s="28" t="s">
+      <c r="H59" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="I58" s="28" t="s">
+      <c r="I59" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="J58" s="29" t="s">
+      <c r="J59" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="M58" s="45"/>
-      <c r="N58" s="45"/>
-      <c r="Q58" s="30"/>
-      <c r="R58" s="30"/>
-      <c r="S58" s="30"/>
-    </row>
-    <row r="59" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="15">
+      <c r="M59" s="45"/>
+      <c r="N59" s="45"/>
+      <c r="Q59" s="30"/>
+      <c r="R59" s="30"/>
+      <c r="S59" s="30"/>
+    </row>
+    <row r="60" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="15">
         <v>2035</v>
       </c>
-      <c r="B59" s="15" t="s">
+      <c r="B60" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="C59" s="15" t="s">
+      <c r="C60" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="D59" s="15" t="s">
-        <v>246</v>
-      </c>
-      <c r="E59" s="15" t="s">
+      <c r="D60" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="E60" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="F59" s="15" t="s">
+      <c r="F60" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="G59" s="18" t="s">
+      <c r="G60" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="H59" s="15" t="s">
+      <c r="H60" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="I59" s="15" t="s">
+      <c r="I60" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="J59" s="16" t="s">
+      <c r="J60" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="K59" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="L59" s="15">
+      <c r="K60" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="L60" s="15">
         <v>15.85</v>
       </c>
-      <c r="M59" s="46">
+      <c r="M60" s="46">
         <v>-0.27</v>
       </c>
-      <c r="N59" s="46">
-        <v>0</v>
-      </c>
-      <c r="O59" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="P59" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q59" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="R59" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="S59" s="17" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="60" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="12">
-        <v>2035</v>
-      </c>
-      <c r="B60" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="C60" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D60" s="12" t="s">
-        <v>245</v>
-      </c>
-      <c r="E60" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="F60" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="G60" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="I60" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="J60" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="K60" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="L60" s="12">
-        <v>15.85</v>
-      </c>
-      <c r="M60" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="N60" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="O60" s="14">
-        <v>1.27</v>
-      </c>
-      <c r="P60" s="14">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="Q60" s="14">
-        <v>120</v>
-      </c>
-      <c r="R60" s="14">
-        <v>0</v>
-      </c>
-      <c r="S60" s="14">
-        <v>45</v>
+      <c r="N60" s="46">
+        <v>0</v>
+      </c>
+      <c r="O60" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="P60" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q60" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="R60" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="S60" s="17" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="61" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
@@ -4558,16 +4597,16 @@
         <v>2035</v>
       </c>
       <c r="B61" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C61" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D61" s="12" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F61" s="12" t="s">
         <v>9</v>
@@ -4579,13 +4618,13 @@
         <v>103</v>
       </c>
       <c r="J61" s="13" t="s">
-        <v>108</v>
+        <v>43</v>
       </c>
       <c r="K61" s="12" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="L61" s="12">
-        <v>18.64</v>
+        <v>15.85</v>
       </c>
       <c r="M61" s="47" t="s">
         <v>109</v>
@@ -4614,16 +4653,16 @@
         <v>2035</v>
       </c>
       <c r="B62" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C62" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E62" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F62" s="12" t="s">
         <v>9</v>
@@ -4635,10 +4674,10 @@
         <v>103</v>
       </c>
       <c r="J62" s="13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K62" s="12" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="L62" s="12">
         <v>18.64</v>
@@ -4656,13 +4695,13 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="Q62" s="14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="R62" s="14">
         <v>0</v>
       </c>
       <c r="S62" s="14">
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="63" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
@@ -4670,16 +4709,16 @@
         <v>2035</v>
       </c>
       <c r="B63" s="12" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="C63" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D63" s="12" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E63" s="12" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="F63" s="12" t="s">
         <v>9</v>
@@ -4691,10 +4730,10 @@
         <v>103</v>
       </c>
       <c r="J63" s="13" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="K63" s="12" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="L63" s="12">
         <v>18.64</v>
@@ -4705,20 +4744,20 @@
       <c r="N63" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="O63" s="12">
-        <v>0.95</v>
-      </c>
-      <c r="P63" s="12">
-        <v>0.86</v>
+      <c r="O63" s="14">
+        <v>1.27</v>
+      </c>
+      <c r="P63" s="14">
+        <v>1.1499999999999999</v>
       </c>
       <c r="Q63" s="14">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="R63" s="14">
         <v>0</v>
       </c>
       <c r="S63" s="14">
-        <v>45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
@@ -4726,16 +4765,16 @@
         <v>2035</v>
       </c>
       <c r="B64" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C64" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D64" s="12" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E64" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F64" s="12" t="s">
         <v>9</v>
@@ -4747,10 +4786,10 @@
         <v>103</v>
       </c>
       <c r="J64" s="13" t="s">
-        <v>42</v>
+        <v>108</v>
       </c>
       <c r="K64" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="L64" s="12">
         <v>18.64</v>
@@ -4768,13 +4807,13 @@
         <v>0.86</v>
       </c>
       <c r="Q64" s="14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="R64" s="14">
         <v>0</v>
       </c>
       <c r="S64" s="14">
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="65" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
@@ -4782,16 +4821,16 @@
         <v>2035</v>
       </c>
       <c r="B65" s="12" t="s">
-        <v>184</v>
+        <v>120</v>
       </c>
       <c r="C65" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D65" s="12" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E65" s="12" t="s">
-        <v>209</v>
+        <v>122</v>
       </c>
       <c r="F65" s="12" t="s">
         <v>9</v>
@@ -4803,10 +4842,10 @@
         <v>103</v>
       </c>
       <c r="J65" s="13" t="s">
-        <v>108</v>
+        <v>42</v>
       </c>
       <c r="K65" s="12" t="s">
-        <v>186</v>
+        <v>123</v>
       </c>
       <c r="L65" s="12">
         <v>18.64</v>
@@ -4838,16 +4877,16 @@
         <v>2035</v>
       </c>
       <c r="B66" s="12" t="s">
-        <v>207</v>
+        <v>184</v>
       </c>
       <c r="C66" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D66" s="12" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E66" s="12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F66" s="12" t="s">
         <v>9</v>
@@ -4859,7 +4898,7 @@
         <v>103</v>
       </c>
       <c r="J66" s="13" t="s">
-        <v>44</v>
+        <v>108</v>
       </c>
       <c r="K66" s="12" t="s">
         <v>186</v>
@@ -4894,22 +4933,22 @@
         <v>2035</v>
       </c>
       <c r="B67" s="12" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C67" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D67" s="12" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E67" s="12" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="F67" s="12" t="s">
-        <v>211</v>
+        <v>9</v>
       </c>
       <c r="G67" s="12" t="s">
-        <v>116</v>
+        <v>10</v>
       </c>
       <c r="I67" s="12" t="s">
         <v>103</v>
@@ -4918,7 +4957,7 @@
         <v>44</v>
       </c>
       <c r="K67" s="12" t="s">
-        <v>212</v>
+        <v>186</v>
       </c>
       <c r="L67" s="12">
         <v>18.64</v>
@@ -4936,13 +4975,13 @@
         <v>0.86</v>
       </c>
       <c r="Q67" s="14">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="R67" s="14">
         <v>0</v>
       </c>
       <c r="S67" s="14">
-        <v>41.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
@@ -4950,16 +4989,16 @@
         <v>2035</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>228</v>
+        <v>206</v>
       </c>
       <c r="C68" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D68" s="12" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E68" s="12" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
       <c r="F68" s="12" t="s">
         <v>211</v>
@@ -4971,13 +5010,13 @@
         <v>103</v>
       </c>
       <c r="J68" s="13" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="K68" s="12" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="L68" s="12">
-        <v>20.55</v>
+        <v>18.64</v>
       </c>
       <c r="M68" s="47" t="s">
         <v>109</v>
@@ -4986,10 +5025,10 @@
         <v>109</v>
       </c>
       <c r="O68" s="12">
-        <v>0.99</v>
+        <v>0.95</v>
       </c>
       <c r="P68" s="12">
-        <v>0.89</v>
+        <v>0.86</v>
       </c>
       <c r="Q68" s="14">
         <v>100</v>
@@ -4998,7 +5037,7 @@
         <v>0</v>
       </c>
       <c r="S68" s="14">
-        <v>75</v>
+        <v>41.25</v>
       </c>
     </row>
     <row r="69" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
@@ -5006,16 +5045,16 @@
         <v>2035</v>
       </c>
       <c r="B69" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C69" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D69" s="12" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E69" s="12" t="s">
-        <v>271</v>
+        <v>226</v>
       </c>
       <c r="F69" s="12" t="s">
         <v>211</v>
@@ -5023,17 +5062,14 @@
       <c r="G69" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="H69" s="12" t="s">
-        <v>11</v>
-      </c>
       <c r="I69" s="12" t="s">
         <v>103</v>
       </c>
       <c r="J69" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K69" s="12" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="L69" s="12">
         <v>20.55</v>
@@ -5065,22 +5101,22 @@
         <v>2035</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C70" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D70" s="12" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E70" s="12" t="s">
-        <v>272</v>
-      </c>
-      <c r="F70" s="53" t="s">
-        <v>232</v>
+        <v>269</v>
+      </c>
+      <c r="F70" s="12" t="s">
+        <v>211</v>
       </c>
       <c r="G70" s="12" t="s">
-        <v>233</v>
+        <v>116</v>
       </c>
       <c r="H70" s="12" t="s">
         <v>11</v>
@@ -5089,10 +5125,10 @@
         <v>103</v>
       </c>
       <c r="J70" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K70" s="12" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="L70" s="12">
         <v>20.55</v>
@@ -5124,22 +5160,22 @@
         <v>2035</v>
       </c>
       <c r="B71" s="12" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C71" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D71" s="12" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E71" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="F71" s="12" t="s">
-        <v>211</v>
+        <v>270</v>
+      </c>
+      <c r="F71" s="53" t="s">
+        <v>232</v>
       </c>
       <c r="G71" s="12" t="s">
-        <v>116</v>
+        <v>233</v>
       </c>
       <c r="H71" s="12" t="s">
         <v>11</v>
@@ -5148,13 +5184,13 @@
         <v>103</v>
       </c>
       <c r="J71" s="13" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="K71" s="12" t="s">
-        <v>236</v>
-      </c>
-      <c r="L71" s="53">
-        <v>15.85</v>
+        <v>234</v>
+      </c>
+      <c r="L71" s="12">
+        <v>20.55</v>
       </c>
       <c r="M71" s="47" t="s">
         <v>109</v>
@@ -5183,16 +5219,16 @@
         <v>2035</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="C72" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D72" s="12" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E72" s="12" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="F72" s="12" t="s">
         <v>211</v>
@@ -5207,13 +5243,13 @@
         <v>103</v>
       </c>
       <c r="J72" s="13" t="s">
-        <v>110</v>
+        <v>16</v>
       </c>
       <c r="K72" s="12" t="s">
-        <v>242</v>
-      </c>
-      <c r="L72" s="12">
-        <v>20.55</v>
+        <v>236</v>
+      </c>
+      <c r="L72" s="53">
+        <v>15.85</v>
       </c>
       <c r="M72" s="47" t="s">
         <v>109</v>
@@ -5227,14 +5263,14 @@
       <c r="P72" s="12">
         <v>0.89</v>
       </c>
-      <c r="Q72" s="52">
-        <v>0</v>
-      </c>
-      <c r="R72" s="52">
-        <v>0</v>
-      </c>
-      <c r="S72" s="52">
-        <v>0</v>
+      <c r="Q72" s="14">
+        <v>100</v>
+      </c>
+      <c r="R72" s="14">
+        <v>0</v>
+      </c>
+      <c r="S72" s="14">
+        <v>75</v>
       </c>
     </row>
     <row r="73" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
@@ -5242,16 +5278,16 @@
         <v>2035</v>
       </c>
       <c r="B73" s="12" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="C73" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D73" s="12" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E73" s="12" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="F73" s="12" t="s">
         <v>211</v>
@@ -5266,10 +5302,10 @@
         <v>103</v>
       </c>
       <c r="J73" s="13" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="K73" s="12" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="L73" s="12">
         <v>20.55</v>
@@ -5286,14 +5322,14 @@
       <c r="P73" s="12">
         <v>0.89</v>
       </c>
-      <c r="Q73" s="14">
-        <v>100</v>
-      </c>
-      <c r="R73" s="14">
-        <v>0</v>
-      </c>
-      <c r="S73" s="14">
-        <v>75</v>
+      <c r="Q73" s="52">
+        <v>0</v>
+      </c>
+      <c r="R73" s="52">
+        <v>0</v>
+      </c>
+      <c r="S73" s="52">
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
@@ -5301,16 +5337,16 @@
         <v>2035</v>
       </c>
       <c r="B74" s="12" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="C74" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D74" s="12" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E74" s="12" t="s">
-        <v>251</v>
+        <v>273</v>
       </c>
       <c r="F74" s="12" t="s">
         <v>211</v>
@@ -5325,10 +5361,10 @@
         <v>103</v>
       </c>
       <c r="J74" s="13" t="s">
-        <v>43</v>
+        <v>129</v>
       </c>
       <c r="K74" s="12" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
       <c r="L74" s="12">
         <v>20.55</v>
@@ -5340,10 +5376,10 @@
         <v>109</v>
       </c>
       <c r="O74" s="12">
-        <v>0.87</v>
+        <v>0.99</v>
       </c>
       <c r="P74" s="12">
-        <v>0.78</v>
+        <v>0.89</v>
       </c>
       <c r="Q74" s="14">
         <v>100</v>
@@ -5360,16 +5396,16 @@
         <v>2035</v>
       </c>
       <c r="B75" s="12" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="C75" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D75" s="12" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E75" s="12" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="F75" s="12" t="s">
         <v>211</v>
@@ -5387,7 +5423,7 @@
         <v>43</v>
       </c>
       <c r="K75" s="12" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="L75" s="12">
         <v>20.55</v>
@@ -5419,16 +5455,16 @@
         <v>2035</v>
       </c>
       <c r="B76" s="12" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="C76" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D76" s="12" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E76" s="12" t="s">
-        <v>239</v>
+        <v>252</v>
       </c>
       <c r="F76" s="12" t="s">
         <v>211</v>
@@ -5443,10 +5479,10 @@
         <v>103</v>
       </c>
       <c r="J76" s="13" t="s">
-        <v>108</v>
+        <v>43</v>
       </c>
       <c r="K76" s="12" t="s">
-        <v>240</v>
+        <v>253</v>
       </c>
       <c r="L76" s="12">
         <v>20.55</v>
@@ -5457,11 +5493,11 @@
       <c r="N76" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="O76" s="53">
-        <v>0.84</v>
-      </c>
-      <c r="P76" s="53">
-        <v>1.59</v>
+      <c r="O76" s="12">
+        <v>0.87</v>
+      </c>
+      <c r="P76" s="12">
+        <v>0.78</v>
       </c>
       <c r="Q76" s="14">
         <v>100</v>
@@ -5478,16 +5514,16 @@
         <v>2035</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C77" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D77" s="12" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E77" s="12" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
       <c r="F77" s="12" t="s">
         <v>211</v>
@@ -5502,10 +5538,10 @@
         <v>103</v>
       </c>
       <c r="J77" s="13" t="s">
-        <v>43</v>
+        <v>108</v>
       </c>
       <c r="K77" s="12" t="s">
-        <v>258</v>
+        <v>240</v>
       </c>
       <c r="L77" s="12">
         <v>20.55</v>
@@ -5516,11 +5552,11 @@
       <c r="N77" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="O77" s="12">
-        <v>0.87</v>
-      </c>
-      <c r="P77" s="12">
-        <v>0.78</v>
+      <c r="O77" s="53">
+        <v>0.84</v>
+      </c>
+      <c r="P77" s="53">
+        <v>1.59</v>
       </c>
       <c r="Q77" s="14">
         <v>100</v>
@@ -5537,16 +5573,16 @@
         <v>2035</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="C78" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D78" s="12" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E78" s="12" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="F78" s="12" t="s">
         <v>211</v>
@@ -5557,14 +5593,14 @@
       <c r="H78" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="I78" s="53" t="s">
-        <v>265</v>
+      <c r="I78" s="12" t="s">
+        <v>103</v>
       </c>
       <c r="J78" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K78" s="12" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="L78" s="12">
         <v>20.55</v>
@@ -5596,16 +5632,16 @@
         <v>2035</v>
       </c>
       <c r="B79" s="12" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C79" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D79" s="12" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E79" s="12" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="F79" s="12" t="s">
         <v>211</v>
@@ -5616,14 +5652,14 @@
       <c r="H79" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="I79" s="12" t="s">
-        <v>103</v>
+      <c r="I79" s="53" t="s">
+        <v>263</v>
       </c>
       <c r="J79" s="13" t="s">
-        <v>129</v>
+        <v>42</v>
       </c>
       <c r="K79" s="12" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="L79" s="12">
         <v>20.55</v>
@@ -5655,16 +5691,16 @@
         <v>2035</v>
       </c>
       <c r="B80" s="12" t="s">
-        <v>276</v>
+        <v>258</v>
       </c>
       <c r="C80" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D80" s="12" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E80" s="12" t="s">
-        <v>277</v>
+        <v>259</v>
       </c>
       <c r="F80" s="12" t="s">
         <v>211</v>
@@ -5679,13 +5715,13 @@
         <v>103</v>
       </c>
       <c r="J80" s="13" t="s">
-        <v>43</v>
+        <v>129</v>
       </c>
       <c r="K80" s="12" t="s">
-        <v>278</v>
-      </c>
-      <c r="L80" s="53">
-        <v>13.68</v>
+        <v>260</v>
+      </c>
+      <c r="L80" s="12">
+        <v>20.55</v>
       </c>
       <c r="M80" s="47" t="s">
         <v>109</v>
@@ -5709,88 +5745,206 @@
         <v>75</v>
       </c>
     </row>
-    <row r="81" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="24">
+    <row r="81" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B81" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="C81" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D81" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="E81" s="12" t="s">
+        <v>275</v>
+      </c>
+      <c r="F81" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="G81" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="H81" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I81" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="J81" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K81" s="12" t="s">
+        <v>276</v>
+      </c>
+      <c r="L81" s="53">
+        <v>13.68</v>
+      </c>
+      <c r="M81" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="N81" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="O81" s="12">
+        <v>0.87</v>
+      </c>
+      <c r="P81" s="12">
+        <v>0.78</v>
+      </c>
+      <c r="Q81" s="14">
+        <v>100</v>
+      </c>
+      <c r="R81" s="14">
+        <v>0</v>
+      </c>
+      <c r="S81" s="14">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="82" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B82" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="C82" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D82" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="E82" s="12" t="s">
+        <v>280</v>
+      </c>
+      <c r="F82" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="G82" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="H82" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I82" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="J82" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K82" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="L82" s="53">
+        <v>14.55</v>
+      </c>
+      <c r="M82" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="N82" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="O82" s="12">
+        <v>0.87</v>
+      </c>
+      <c r="P82" s="12">
+        <v>0.78</v>
+      </c>
+      <c r="Q82" s="14">
+        <v>100</v>
+      </c>
+      <c r="R82" s="14">
+        <v>0</v>
+      </c>
+      <c r="S82" s="14">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="83" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="24">
         <v>2050</v>
       </c>
-      <c r="B81" s="24" t="s">
+      <c r="B83" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="C81" s="24" t="s">
+      <c r="C83" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="D81" s="24" t="s">
-        <v>246</v>
-      </c>
-      <c r="E81" s="24" t="s">
+      <c r="D83" s="24" t="s">
+        <v>244</v>
+      </c>
+      <c r="E83" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="F81" s="24" t="s">
+      <c r="F83" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="G81" s="25" t="s">
+      <c r="G83" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="I81" s="24" t="s">
+      <c r="I83" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="J81" s="26" t="s">
+      <c r="J83" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="K81" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="L81" s="24">
+      <c r="K83" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="L83" s="24">
         <v>17.440000000000001</v>
       </c>
-      <c r="M81" s="48">
+      <c r="M83" s="48">
         <v>-0.33</v>
       </c>
-      <c r="N81" s="48">
-        <v>0</v>
-      </c>
-      <c r="O81" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="P81" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q81" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="R81" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="S81" s="27" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="L83" s="1">
+      <c r="N83" s="48">
+        <v>0</v>
+      </c>
+      <c r="O83" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="P83" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q83" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="R83" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="S83" s="27" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="L85" s="1">
+        <f>L81*2</f>
+        <v>27.36</v>
+      </c>
+      <c r="M85" s="44">
         <f>L80*2</f>
-        <v>27.36</v>
-      </c>
-      <c r="M83" s="44">
-        <f>L79*2</f>
         <v>41.1</v>
       </c>
     </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="L84" s="1">
+    <row r="86" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="L86" s="1">
+        <f>L81*3</f>
+        <v>41.04</v>
+      </c>
+      <c r="M86" s="44">
         <f>L80*3</f>
-        <v>41.04</v>
-      </c>
-      <c r="M84" s="44">
-        <f>L79*3</f>
         <v>61.650000000000006</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="K7" r:id="rId1" xr:uid="{1BE7DD4C-B567-4320-9B69-E8B55CE41797}"/>
-    <hyperlink ref="K8" r:id="rId2" xr:uid="{A52BF015-28DA-4569-A638-6E56CCBD2F4D}"/>
-    <hyperlink ref="K9" r:id="rId3" xr:uid="{70B88B93-E906-4801-9012-B01BCDB48CBF}"/>
+    <hyperlink ref="K8" r:id="rId1" xr:uid="{1BE7DD4C-B567-4320-9B69-E8B55CE41797}"/>
+    <hyperlink ref="K9" r:id="rId2" xr:uid="{A52BF015-28DA-4569-A638-6E56CCBD2F4D}"/>
+    <hyperlink ref="K10" r:id="rId3" xr:uid="{70B88B93-E906-4801-9012-B01BCDB48CBF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>

<commit_message>
Demote 2035_TM160_IPA_13 from current
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9832675-6486-4B09-A540-D6113A1FB1A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014E6DC1-3407-4A16-9BB1-B18EA52F2835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="17010" windowHeight="9855" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="283">
   <si>
     <t>year</t>
   </si>
@@ -1484,7 +1484,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C71" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B82" sqref="B82"/>
+      <selection pane="bottomRight" activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5767,9 +5767,6 @@
       <c r="G81" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="H81" s="12" t="s">
-        <v>11</v>
-      </c>
       <c r="I81" s="12" t="s">
         <v>103</v>
       </c>

</xml_diff>

<commit_message>
Demote 2035_TM160_IPA_11_PBA50wfh from current
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014E6DC1-3407-4A16-9BB1-B18EA52F2835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A6FE78-750B-4ED7-A41D-4FE5C98A03D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="17010" windowHeight="9855" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="283">
   <si>
     <t>year</t>
   </si>
@@ -1484,7 +1484,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C71" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E85" sqref="E85"/>
+      <selection pane="bottomRight" activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5531,9 +5531,6 @@
       <c r="G77" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="H77" s="12" t="s">
-        <v>11</v>
-      </c>
       <c r="I77" s="12" t="s">
         <v>103</v>
       </c>

</xml_diff>

<commit_message>
2023 test runs with lowered Work_Transit_Hesitance
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\config_RTP2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one-master\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDFCCF9D-56D1-45C1-A5E0-B986E8D659FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F418DA-762A-472B-8C98-513FE4588819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5160" yWindow="2940" windowWidth="28230" windowHeight="12750" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelRuns" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="331">
   <si>
     <t>year</t>
   </si>
@@ -999,6 +999,36 @@
   </si>
   <si>
     <t>Sensitivity Test - AOC</t>
+  </si>
+  <si>
+    <t>2023_TM160_IPA_51</t>
+  </si>
+  <si>
+    <t>2023_TM160_IPA_52</t>
+  </si>
+  <si>
+    <t>2023_TM160_IPA_53</t>
+  </si>
+  <si>
+    <t>AOC=16.21, with rail/ferry hes =70</t>
+  </si>
+  <si>
+    <t>AOC=16.21, with rail/ferry hes =65</t>
+  </si>
+  <si>
+    <t>AOC=16.21, with rail/ferry hes =60</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1206685870182016/f</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1206685870182013/f</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1206699871295080/f</t>
+  </si>
+  <si>
+    <t>tbd</t>
   </si>
 </sst>
 </file>
@@ -1296,9 +1326,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1336,7 +1366,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1442,7 +1472,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1584,7 +1614,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1592,35 +1622,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9564CC59-3725-4FDA-8BF2-0F68CB1B6F5A}">
-  <dimension ref="A1:T99"/>
+  <dimension ref="A1:T102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C44" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="H44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B62" sqref="B62"/>
+      <selection pane="bottomRight" activeCell="K72" sqref="K72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="42.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.54296875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="42.26953125" style="1" customWidth="1"/>
     <col min="7" max="7" width="23" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.28515625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" style="10" customWidth="1"/>
-    <col min="12" max="12" width="17.5703125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="8.28515625" style="1" customWidth="1"/>
-    <col min="14" max="15" width="9.28515625" style="44"/>
-    <col min="16" max="16384" width="9.28515625" style="1"/>
+    <col min="8" max="8" width="8.26953125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="6.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.26953125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11.26953125" style="10" customWidth="1"/>
+    <col min="12" max="12" width="17.54296875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="8.26953125" style="1" customWidth="1"/>
+    <col min="14" max="15" width="9.26953125" style="44"/>
+    <col min="16" max="16384" width="9.26953125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" s="5" customFormat="1" ht="39" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1682,7 +1712,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19">
         <v>2005</v>
       </c>
@@ -1735,7 +1765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:20" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="31">
         <v>2005</v>
       </c>
@@ -1791,7 +1821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:20" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="31">
         <v>2005</v>
       </c>
@@ -1846,7 +1876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:20" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="31">
         <v>2005</v>
       </c>
@@ -1901,7 +1931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:20" s="55" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" s="55" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="54">
         <v>2015</v>
       </c>
@@ -1942,7 +1972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:20" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="35">
         <v>2015</v>
       </c>
@@ -1988,7 +2018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:20" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="35">
         <v>2015</v>
       </c>
@@ -2041,7 +2071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:20" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="35">
         <v>2015</v>
       </c>
@@ -2094,7 +2124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:20" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="35">
         <v>2015</v>
       </c>
@@ -2147,7 +2177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:20" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="35">
         <v>2015</v>
       </c>
@@ -2203,7 +2233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:20" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="35">
         <v>2015</v>
       </c>
@@ -2259,7 +2289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:20" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="35">
         <v>2015</v>
       </c>
@@ -2315,7 +2345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:20" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="35">
         <v>2015</v>
       </c>
@@ -2374,7 +2404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>2023</v>
       </c>
@@ -2420,7 +2450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>2023</v>
       </c>
@@ -2466,7 +2496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>2023</v>
       </c>
@@ -2512,7 +2542,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>2023</v>
       </c>
@@ -2558,7 +2588,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>2023</v>
       </c>
@@ -2604,7 +2634,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>2023</v>
       </c>
@@ -2650,7 +2680,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>2023</v>
       </c>
@@ -2696,7 +2726,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>2023</v>
       </c>
@@ -2742,7 +2772,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>2023</v>
       </c>
@@ -2788,7 +2818,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>2023</v>
       </c>
@@ -2834,7 +2864,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>2023</v>
       </c>
@@ -2880,7 +2910,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>2023</v>
       </c>
@@ -2926,7 +2956,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>2023</v>
       </c>
@@ -2972,7 +3002,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>2023</v>
       </c>
@@ -3018,7 +3048,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>2023</v>
       </c>
@@ -3064,7 +3094,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>2023</v>
       </c>
@@ -3110,7 +3140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>2023</v>
       </c>
@@ -3156,7 +3186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>2023</v>
       </c>
@@ -3202,7 +3232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>2023</v>
       </c>
@@ -3246,7 +3276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>2023</v>
       </c>
@@ -3295,7 +3325,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>2023</v>
       </c>
@@ -3342,7 +3372,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>2023</v>
       </c>
@@ -3389,7 +3419,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>2023</v>
       </c>
@@ -3445,7 +3475,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>2023</v>
       </c>
@@ -3501,7 +3531,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>2023</v>
       </c>
@@ -3557,7 +3587,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>2023</v>
       </c>
@@ -3613,7 +3643,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>2023</v>
       </c>
@@ -3669,7 +3699,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>2023</v>
       </c>
@@ -3725,7 +3755,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>2023</v>
       </c>
@@ -3781,7 +3811,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>2023</v>
       </c>
@@ -3837,7 +3867,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>2023</v>
       </c>
@@ -3893,7 +3923,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>2023</v>
       </c>
@@ -3949,7 +3979,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>2023</v>
       </c>
@@ -4005,7 +4035,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>2023</v>
       </c>
@@ -4061,7 +4091,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>2023</v>
       </c>
@@ -4117,7 +4147,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>2023</v>
       </c>
@@ -4173,7 +4203,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>2023</v>
       </c>
@@ -4229,7 +4259,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>2023</v>
       </c>
@@ -4285,7 +4315,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>2023</v>
       </c>
@@ -4341,7 +4371,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>2023</v>
       </c>
@@ -4397,7 +4427,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>2023</v>
       </c>
@@ -4453,7 +4483,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>2023</v>
       </c>
@@ -4509,7 +4539,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>2023</v>
       </c>
@@ -4565,7 +4595,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>2023</v>
       </c>
@@ -4621,7 +4651,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>2023</v>
       </c>
@@ -4677,7 +4707,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>2023</v>
       </c>
@@ -4733,7 +4763,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>2023</v>
       </c>
@@ -4789,7 +4819,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>2023</v>
       </c>
@@ -4851,7 +4881,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>2023</v>
       </c>
@@ -4907,7 +4937,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>2023</v>
       </c>
@@ -4969,7 +4999,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>2023</v>
       </c>
@@ -5031,7 +5061,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>2023</v>
       </c>
@@ -5093,7 +5123,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>2023</v>
       </c>
@@ -5155,7 +5185,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="68" spans="1:20" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:20" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>2023</v>
       </c>
@@ -5211,7 +5241,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:20" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>2023</v>
       </c>
@@ -5267,267 +5297,276 @@
         <v>75</v>
       </c>
     </row>
-    <row r="70" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="28">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A70" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J70" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="K70" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="L70" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="M70" s="1">
+        <v>16.21</v>
+      </c>
+      <c r="N70" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="O70" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="P70" s="1">
+        <v>1.04</v>
+      </c>
+      <c r="Q70" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="R70" s="6">
+        <v>90</v>
+      </c>
+      <c r="S70" s="6">
+        <v>0</v>
+      </c>
+      <c r="T70" s="6">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A71" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I71" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J71" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="K71" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="L71" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="M71" s="1">
+        <v>16.21</v>
+      </c>
+      <c r="N71" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="O71" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="P71" s="1">
+        <v>1.04</v>
+      </c>
+      <c r="Q71" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="R71" s="6">
+        <v>80</v>
+      </c>
+      <c r="S71" s="6">
+        <v>0</v>
+      </c>
+      <c r="T71" s="6">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A72" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I72" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J72" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="K72" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="L72" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="M72" s="1">
+        <v>16.21</v>
+      </c>
+      <c r="N72" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="O72" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="P72" s="1">
+        <v>1.04</v>
+      </c>
+      <c r="Q72" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="R72" s="6">
+        <v>70</v>
+      </c>
+      <c r="S72" s="6">
+        <v>0</v>
+      </c>
+      <c r="T72" s="6">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="28">
         <v>2025</v>
       </c>
-      <c r="B70" s="28" t="s">
+      <c r="B73" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="C70" s="28" t="s">
+      <c r="C73" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="D70" s="28" t="s">
+      <c r="D73" s="28" t="s">
         <v>244</v>
       </c>
-      <c r="F70" s="28" t="s">
+      <c r="F73" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="J70" s="28" t="s">
+      <c r="J73" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="K70" s="29" t="s">
+      <c r="K73" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="N70" s="45"/>
-      <c r="O70" s="45"/>
-      <c r="R70" s="30"/>
-      <c r="S70" s="30"/>
-      <c r="T70" s="30"/>
-    </row>
-    <row r="71" spans="1:20" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="15">
+      <c r="N73" s="45"/>
+      <c r="O73" s="45"/>
+      <c r="R73" s="30"/>
+      <c r="S73" s="30"/>
+      <c r="T73" s="30"/>
+    </row>
+    <row r="74" spans="1:20" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="15">
         <v>2035</v>
       </c>
-      <c r="B71" s="15" t="s">
+      <c r="B74" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="C71" s="15" t="s">
+      <c r="C74" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="D71" s="15" t="s">
+      <c r="D74" s="15" t="s">
         <v>244</v>
       </c>
-      <c r="F71" s="15" t="s">
+      <c r="F74" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="G71" s="15" t="s">
+      <c r="G74" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="H71" s="18" t="s">
+      <c r="H74" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="I71" s="15" t="s">
+      <c r="I74" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="J71" s="15" t="s">
+      <c r="J74" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="K71" s="16" t="s">
+      <c r="K74" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="L71" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="M71" s="15">
+      <c r="L74" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="M74" s="15">
         <v>15.85</v>
       </c>
-      <c r="N71" s="46">
+      <c r="N74" s="46">
         <v>-0.27</v>
       </c>
-      <c r="O71" s="46">
-        <v>0</v>
-      </c>
-      <c r="P71" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q71" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="R71" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="S71" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="T71" s="17" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="72" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="12">
-        <v>2035</v>
-      </c>
-      <c r="B72" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="C72" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D72" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="F72" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="G72" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="H72" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="J72" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="K72" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="L72" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="M72" s="12">
-        <v>15.85</v>
-      </c>
-      <c r="N72" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="O72" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="P72" s="14">
-        <v>1.27</v>
-      </c>
-      <c r="Q72" s="14">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="R72" s="14">
-        <v>120</v>
-      </c>
-      <c r="S72" s="14">
-        <v>0</v>
-      </c>
-      <c r="T72" s="14">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="73" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="12">
-        <v>2035</v>
-      </c>
-      <c r="B73" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="C73" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D73" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="F73" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="G73" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="H73" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="J73" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="K73" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="L73" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="M73" s="12">
-        <v>18.64</v>
-      </c>
-      <c r="N73" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="O73" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="P73" s="14">
-        <v>1.27</v>
-      </c>
-      <c r="Q73" s="14">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="R73" s="14">
-        <v>120</v>
-      </c>
-      <c r="S73" s="14">
-        <v>0</v>
-      </c>
-      <c r="T73" s="14">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="74" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="12">
-        <v>2035</v>
-      </c>
-      <c r="B74" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="C74" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D74" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="F74" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="G74" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="H74" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="J74" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="K74" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="L74" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="M74" s="12">
-        <v>18.64</v>
-      </c>
-      <c r="N74" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="O74" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="P74" s="14">
-        <v>1.27</v>
-      </c>
-      <c r="Q74" s="14">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="R74" s="14">
-        <v>0</v>
-      </c>
-      <c r="S74" s="14">
-        <v>0</v>
-      </c>
-      <c r="T74" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O74" s="46">
+        <v>0</v>
+      </c>
+      <c r="P74" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q74" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="R74" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="S74" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="T74" s="17" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="12">
         <v>2035</v>
       </c>
       <c r="B75" s="12" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="C75" s="12" t="s">
         <v>17</v>
@@ -5536,7 +5575,7 @@
         <v>243</v>
       </c>
       <c r="F75" s="12" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="G75" s="12" t="s">
         <v>9</v>
@@ -5548,13 +5587,13 @@
         <v>103</v>
       </c>
       <c r="K75" s="13" t="s">
-        <v>108</v>
+        <v>43</v>
       </c>
       <c r="L75" s="12" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="M75" s="12">
-        <v>18.64</v>
+        <v>15.85</v>
       </c>
       <c r="N75" s="47" t="s">
         <v>109</v>
@@ -5562,11 +5601,11 @@
       <c r="O75" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="P75" s="12">
-        <v>0.95</v>
-      </c>
-      <c r="Q75" s="12">
-        <v>0.86</v>
+      <c r="P75" s="14">
+        <v>1.27</v>
+      </c>
+      <c r="Q75" s="14">
+        <v>1.1499999999999999</v>
       </c>
       <c r="R75" s="14">
         <v>120</v>
@@ -5578,12 +5617,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="76" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="12">
         <v>2035</v>
       </c>
       <c r="B76" s="12" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="C76" s="12" t="s">
         <v>17</v>
@@ -5592,7 +5631,7 @@
         <v>243</v>
       </c>
       <c r="F76" s="12" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="G76" s="12" t="s">
         <v>9</v>
@@ -5604,10 +5643,10 @@
         <v>103</v>
       </c>
       <c r="K76" s="13" t="s">
-        <v>42</v>
+        <v>108</v>
       </c>
       <c r="L76" s="12" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="M76" s="12">
         <v>18.64</v>
@@ -5618,28 +5657,28 @@
       <c r="O76" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="P76" s="12">
-        <v>0.95</v>
-      </c>
-      <c r="Q76" s="12">
-        <v>0.86</v>
+      <c r="P76" s="14">
+        <v>1.27</v>
+      </c>
+      <c r="Q76" s="14">
+        <v>1.1499999999999999</v>
       </c>
       <c r="R76" s="14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="S76" s="14">
         <v>0</v>
       </c>
       <c r="T76" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="12">
         <v>2035</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>184</v>
+        <v>101</v>
       </c>
       <c r="C77" s="12" t="s">
         <v>17</v>
@@ -5648,7 +5687,7 @@
         <v>243</v>
       </c>
       <c r="F77" s="12" t="s">
-        <v>209</v>
+        <v>106</v>
       </c>
       <c r="G77" s="12" t="s">
         <v>9</v>
@@ -5660,10 +5699,10 @@
         <v>103</v>
       </c>
       <c r="K77" s="13" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="L77" s="12" t="s">
-        <v>186</v>
+        <v>111</v>
       </c>
       <c r="M77" s="12">
         <v>18.64</v>
@@ -5674,11 +5713,11 @@
       <c r="O77" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="P77" s="12">
-        <v>0.95</v>
-      </c>
-      <c r="Q77" s="12">
-        <v>0.86</v>
+      <c r="P77" s="14">
+        <v>1.27</v>
+      </c>
+      <c r="Q77" s="14">
+        <v>1.1499999999999999</v>
       </c>
       <c r="R77" s="14">
         <v>0</v>
@@ -5690,12 +5729,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="12">
         <v>2035</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>207</v>
+        <v>119</v>
       </c>
       <c r="C78" s="12" t="s">
         <v>17</v>
@@ -5704,7 +5743,7 @@
         <v>243</v>
       </c>
       <c r="F78" s="12" t="s">
-        <v>210</v>
+        <v>121</v>
       </c>
       <c r="G78" s="12" t="s">
         <v>9</v>
@@ -5716,10 +5755,10 @@
         <v>103</v>
       </c>
       <c r="K78" s="13" t="s">
-        <v>44</v>
+        <v>108</v>
       </c>
       <c r="L78" s="12" t="s">
-        <v>186</v>
+        <v>124</v>
       </c>
       <c r="M78" s="12">
         <v>18.64</v>
@@ -5737,21 +5776,21 @@
         <v>0.86</v>
       </c>
       <c r="R78" s="14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="S78" s="14">
         <v>0</v>
       </c>
       <c r="T78" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="12">
         <v>2035</v>
       </c>
       <c r="B79" s="12" t="s">
-        <v>206</v>
+        <v>120</v>
       </c>
       <c r="C79" s="12" t="s">
         <v>17</v>
@@ -5760,22 +5799,22 @@
         <v>243</v>
       </c>
       <c r="F79" s="12" t="s">
-        <v>208</v>
+        <v>122</v>
       </c>
       <c r="G79" s="12" t="s">
-        <v>211</v>
+        <v>9</v>
       </c>
       <c r="H79" s="12" t="s">
-        <v>116</v>
+        <v>10</v>
       </c>
       <c r="J79" s="12" t="s">
         <v>103</v>
       </c>
       <c r="K79" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L79" s="12" t="s">
-        <v>212</v>
+        <v>123</v>
       </c>
       <c r="M79" s="12">
         <v>18.64</v>
@@ -5793,21 +5832,21 @@
         <v>0.86</v>
       </c>
       <c r="R79" s="14">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="S79" s="14">
         <v>0</v>
       </c>
       <c r="T79" s="14">
-        <v>41.25</v>
-      </c>
-    </row>
-    <row r="80" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="12">
         <v>2035</v>
       </c>
       <c r="B80" s="12" t="s">
-        <v>228</v>
+        <v>184</v>
       </c>
       <c r="C80" s="12" t="s">
         <v>17</v>
@@ -5816,25 +5855,25 @@
         <v>243</v>
       </c>
       <c r="F80" s="12" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="G80" s="12" t="s">
-        <v>211</v>
+        <v>9</v>
       </c>
       <c r="H80" s="12" t="s">
-        <v>116</v>
+        <v>10</v>
       </c>
       <c r="J80" s="12" t="s">
         <v>103</v>
       </c>
       <c r="K80" s="13" t="s">
-        <v>42</v>
+        <v>108</v>
       </c>
       <c r="L80" s="12" t="s">
-        <v>227</v>
+        <v>186</v>
       </c>
       <c r="M80" s="12">
-        <v>20.55</v>
+        <v>18.64</v>
       </c>
       <c r="N80" s="47" t="s">
         <v>109</v>
@@ -5843,27 +5882,27 @@
         <v>109</v>
       </c>
       <c r="P80" s="12">
-        <v>0.99</v>
+        <v>0.95</v>
       </c>
       <c r="Q80" s="12">
-        <v>0.89</v>
+        <v>0.86</v>
       </c>
       <c r="R80" s="14">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="S80" s="14">
         <v>0</v>
       </c>
       <c r="T80" s="14">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="81" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="12">
         <v>2035</v>
       </c>
       <c r="B81" s="12" t="s">
-        <v>229</v>
+        <v>207</v>
       </c>
       <c r="C81" s="12" t="s">
         <v>17</v>
@@ -5872,25 +5911,25 @@
         <v>243</v>
       </c>
       <c r="F81" s="12" t="s">
-        <v>269</v>
+        <v>210</v>
       </c>
       <c r="G81" s="12" t="s">
-        <v>211</v>
+        <v>9</v>
       </c>
       <c r="H81" s="12" t="s">
-        <v>116</v>
+        <v>10</v>
       </c>
       <c r="J81" s="12" t="s">
         <v>103</v>
       </c>
       <c r="K81" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L81" s="12" t="s">
-        <v>230</v>
+        <v>186</v>
       </c>
       <c r="M81" s="12">
-        <v>20.55</v>
+        <v>18.64</v>
       </c>
       <c r="N81" s="47" t="s">
         <v>109</v>
@@ -5899,27 +5938,27 @@
         <v>109</v>
       </c>
       <c r="P81" s="12">
-        <v>0.99</v>
+        <v>0.95</v>
       </c>
       <c r="Q81" s="12">
-        <v>0.89</v>
+        <v>0.86</v>
       </c>
       <c r="R81" s="14">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="S81" s="14">
         <v>0</v>
       </c>
       <c r="T81" s="14">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="82" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="12">
         <v>2035</v>
       </c>
       <c r="B82" s="12" t="s">
-        <v>231</v>
+        <v>206</v>
       </c>
       <c r="C82" s="12" t="s">
         <v>17</v>
@@ -5928,13 +5967,13 @@
         <v>243</v>
       </c>
       <c r="F82" s="12" t="s">
-        <v>270</v>
-      </c>
-      <c r="G82" s="53" t="s">
-        <v>232</v>
+        <v>208</v>
+      </c>
+      <c r="G82" s="12" t="s">
+        <v>211</v>
       </c>
       <c r="H82" s="12" t="s">
-        <v>233</v>
+        <v>116</v>
       </c>
       <c r="J82" s="12" t="s">
         <v>103</v>
@@ -5943,10 +5982,10 @@
         <v>44</v>
       </c>
       <c r="L82" s="12" t="s">
-        <v>234</v>
+        <v>212</v>
       </c>
       <c r="M82" s="12">
-        <v>20.55</v>
+        <v>18.64</v>
       </c>
       <c r="N82" s="47" t="s">
         <v>109</v>
@@ -5955,10 +5994,10 @@
         <v>109</v>
       </c>
       <c r="P82" s="12">
-        <v>0.99</v>
+        <v>0.95</v>
       </c>
       <c r="Q82" s="12">
-        <v>0.89</v>
+        <v>0.86</v>
       </c>
       <c r="R82" s="14">
         <v>100</v>
@@ -5967,15 +6006,15 @@
         <v>0</v>
       </c>
       <c r="T82" s="14">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="83" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>41.25</v>
+      </c>
+    </row>
+    <row r="83" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="12">
         <v>2035</v>
       </c>
       <c r="B83" s="12" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="C83" s="12" t="s">
         <v>17</v>
@@ -5984,7 +6023,7 @@
         <v>243</v>
       </c>
       <c r="F83" s="12" t="s">
-        <v>271</v>
+        <v>226</v>
       </c>
       <c r="G83" s="12" t="s">
         <v>211</v>
@@ -5996,13 +6035,13 @@
         <v>103</v>
       </c>
       <c r="K83" s="13" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="L83" s="12" t="s">
-        <v>236</v>
-      </c>
-      <c r="M83" s="53">
-        <v>15.85</v>
+        <v>227</v>
+      </c>
+      <c r="M83" s="12">
+        <v>20.55</v>
       </c>
       <c r="N83" s="47" t="s">
         <v>109</v>
@@ -6026,12 +6065,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="84" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A84" s="12">
         <v>2035</v>
       </c>
       <c r="B84" s="12" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="C84" s="12" t="s">
         <v>17</v>
@@ -6040,7 +6079,7 @@
         <v>243</v>
       </c>
       <c r="F84" s="12" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G84" s="12" t="s">
         <v>211</v>
@@ -6052,10 +6091,10 @@
         <v>103</v>
       </c>
       <c r="K84" s="13" t="s">
-        <v>110</v>
+        <v>43</v>
       </c>
       <c r="L84" s="12" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="M84" s="12">
         <v>20.55</v>
@@ -6072,22 +6111,22 @@
       <c r="Q84" s="12">
         <v>0.89</v>
       </c>
-      <c r="R84" s="52">
-        <v>0</v>
-      </c>
-      <c r="S84" s="52">
-        <v>0</v>
-      </c>
-      <c r="T84" s="52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R84" s="14">
+        <v>100</v>
+      </c>
+      <c r="S84" s="14">
+        <v>0</v>
+      </c>
+      <c r="T84" s="14">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="85" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="12">
         <v>2035</v>
       </c>
       <c r="B85" s="12" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C85" s="12" t="s">
         <v>17</v>
@@ -6096,22 +6135,22 @@
         <v>243</v>
       </c>
       <c r="F85" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="G85" s="12" t="s">
-        <v>211</v>
+        <v>270</v>
+      </c>
+      <c r="G85" s="53" t="s">
+        <v>232</v>
       </c>
       <c r="H85" s="12" t="s">
-        <v>116</v>
+        <v>233</v>
       </c>
       <c r="J85" s="12" t="s">
         <v>103</v>
       </c>
       <c r="K85" s="13" t="s">
-        <v>129</v>
+        <v>44</v>
       </c>
       <c r="L85" s="12" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="M85" s="12">
         <v>20.55</v>
@@ -6138,12 +6177,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="86" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" s="12">
         <v>2035</v>
       </c>
       <c r="B86" s="12" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
       <c r="C86" s="12" t="s">
         <v>17</v>
@@ -6152,7 +6191,7 @@
         <v>243</v>
       </c>
       <c r="F86" s="12" t="s">
-        <v>249</v>
+        <v>271</v>
       </c>
       <c r="G86" s="12" t="s">
         <v>211</v>
@@ -6164,13 +6203,13 @@
         <v>103</v>
       </c>
       <c r="K86" s="13" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="L86" s="12" t="s">
-        <v>250</v>
-      </c>
-      <c r="M86" s="12">
-        <v>20.55</v>
+        <v>236</v>
+      </c>
+      <c r="M86" s="53">
+        <v>15.85</v>
       </c>
       <c r="N86" s="47" t="s">
         <v>109</v>
@@ -6179,10 +6218,10 @@
         <v>109</v>
       </c>
       <c r="P86" s="12">
-        <v>0.87</v>
+        <v>0.99</v>
       </c>
       <c r="Q86" s="12">
-        <v>0.78</v>
+        <v>0.89</v>
       </c>
       <c r="R86" s="14">
         <v>100</v>
@@ -6194,12 +6233,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="87" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" s="12">
         <v>2035</v>
       </c>
       <c r="B87" s="12" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="C87" s="12" t="s">
         <v>17</v>
@@ -6208,7 +6247,7 @@
         <v>243</v>
       </c>
       <c r="F87" s="12" t="s">
-        <v>252</v>
+        <v>272</v>
       </c>
       <c r="G87" s="12" t="s">
         <v>211</v>
@@ -6220,10 +6259,10 @@
         <v>103</v>
       </c>
       <c r="K87" s="13" t="s">
-        <v>43</v>
+        <v>110</v>
       </c>
       <c r="L87" s="12" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="M87" s="12">
         <v>20.55</v>
@@ -6235,27 +6274,27 @@
         <v>109</v>
       </c>
       <c r="P87" s="12">
-        <v>0.87</v>
+        <v>0.99</v>
       </c>
       <c r="Q87" s="12">
-        <v>0.78</v>
-      </c>
-      <c r="R87" s="14">
-        <v>100</v>
-      </c>
-      <c r="S87" s="14">
-        <v>0</v>
-      </c>
-      <c r="T87" s="14">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="88" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>0.89</v>
+      </c>
+      <c r="R87" s="52">
+        <v>0</v>
+      </c>
+      <c r="S87" s="52">
+        <v>0</v>
+      </c>
+      <c r="T87" s="52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="12">
         <v>2035</v>
       </c>
       <c r="B88" s="12" t="s">
-        <v>257</v>
+        <v>237</v>
       </c>
       <c r="C88" s="12" t="s">
         <v>17</v>
@@ -6264,7 +6303,7 @@
         <v>243</v>
       </c>
       <c r="F88" s="12" t="s">
-        <v>239</v>
+        <v>273</v>
       </c>
       <c r="G88" s="12" t="s">
         <v>211</v>
@@ -6276,10 +6315,10 @@
         <v>103</v>
       </c>
       <c r="K88" s="13" t="s">
-        <v>108</v>
+        <v>129</v>
       </c>
       <c r="L88" s="12" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="M88" s="12">
         <v>20.55</v>
@@ -6290,11 +6329,11 @@
       <c r="O88" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="P88" s="53">
-        <v>0.84</v>
-      </c>
-      <c r="Q88" s="53">
-        <v>1.59</v>
+      <c r="P88" s="12">
+        <v>0.99</v>
+      </c>
+      <c r="Q88" s="12">
+        <v>0.89</v>
       </c>
       <c r="R88" s="14">
         <v>100</v>
@@ -6306,12 +6345,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="89" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="12">
         <v>2035</v>
       </c>
       <c r="B89" s="12" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="C89" s="12" t="s">
         <v>17</v>
@@ -6320,7 +6359,7 @@
         <v>243</v>
       </c>
       <c r="F89" s="12" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="G89" s="12" t="s">
         <v>211</v>
@@ -6335,7 +6374,7 @@
         <v>43</v>
       </c>
       <c r="L89" s="12" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="M89" s="12">
         <v>20.55</v>
@@ -6362,12 +6401,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="90" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90" s="12">
         <v>2035</v>
       </c>
       <c r="B90" s="12" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="C90" s="12" t="s">
         <v>17</v>
@@ -6376,7 +6415,7 @@
         <v>243</v>
       </c>
       <c r="F90" s="12" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="G90" s="12" t="s">
         <v>211</v>
@@ -6384,14 +6423,14 @@
       <c r="H90" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="J90" s="53" t="s">
-        <v>263</v>
+      <c r="J90" s="12" t="s">
+        <v>103</v>
       </c>
       <c r="K90" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L90" s="12" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="M90" s="12">
         <v>20.55</v>
@@ -6418,12 +6457,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="91" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" s="12">
         <v>2035</v>
       </c>
       <c r="B91" s="12" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C91" s="12" t="s">
         <v>17</v>
@@ -6432,7 +6471,7 @@
         <v>243</v>
       </c>
       <c r="F91" s="12" t="s">
-        <v>259</v>
+        <v>239</v>
       </c>
       <c r="G91" s="12" t="s">
         <v>211</v>
@@ -6444,10 +6483,10 @@
         <v>103</v>
       </c>
       <c r="K91" s="13" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="L91" s="12" t="s">
-        <v>260</v>
+        <v>240</v>
       </c>
       <c r="M91" s="12">
         <v>20.55</v>
@@ -6458,11 +6497,11 @@
       <c r="O91" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="P91" s="12">
-        <v>0.87</v>
-      </c>
-      <c r="Q91" s="12">
-        <v>0.78</v>
+      <c r="P91" s="53">
+        <v>0.84</v>
+      </c>
+      <c r="Q91" s="53">
+        <v>1.59</v>
       </c>
       <c r="R91" s="14">
         <v>100</v>
@@ -6474,12 +6513,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="92" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="12">
         <v>2035</v>
       </c>
       <c r="B92" s="12" t="s">
-        <v>274</v>
+        <v>254</v>
       </c>
       <c r="C92" s="12" t="s">
         <v>17</v>
@@ -6488,7 +6527,7 @@
         <v>243</v>
       </c>
       <c r="F92" s="12" t="s">
-        <v>275</v>
+        <v>255</v>
       </c>
       <c r="G92" s="12" t="s">
         <v>211</v>
@@ -6503,10 +6542,10 @@
         <v>43</v>
       </c>
       <c r="L92" s="12" t="s">
-        <v>276</v>
-      </c>
-      <c r="M92" s="53">
-        <v>13.68</v>
+        <v>256</v>
+      </c>
+      <c r="M92" s="12">
+        <v>20.55</v>
       </c>
       <c r="N92" s="47" t="s">
         <v>109</v>
@@ -6530,12 +6569,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="93" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" s="12">
         <v>2035</v>
       </c>
       <c r="B93" s="12" t="s">
-        <v>282</v>
+        <v>261</v>
       </c>
       <c r="C93" s="12" t="s">
         <v>17</v>
@@ -6544,7 +6583,7 @@
         <v>243</v>
       </c>
       <c r="F93" s="12" t="s">
-        <v>280</v>
+        <v>262</v>
       </c>
       <c r="G93" s="12" t="s">
         <v>211</v>
@@ -6552,17 +6591,17 @@
       <c r="H93" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="J93" s="12" t="s">
-        <v>103</v>
+      <c r="J93" s="53" t="s">
+        <v>263</v>
       </c>
       <c r="K93" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L93" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="M93" s="53">
-        <v>14.55</v>
+        <v>264</v>
+      </c>
+      <c r="M93" s="12">
+        <v>20.55</v>
       </c>
       <c r="N93" s="47" t="s">
         <v>109</v>
@@ -6586,12 +6625,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="94" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" s="12">
         <v>2035</v>
       </c>
       <c r="B94" s="12" t="s">
-        <v>284</v>
+        <v>258</v>
       </c>
       <c r="C94" s="12" t="s">
         <v>17</v>
@@ -6600,7 +6639,7 @@
         <v>243</v>
       </c>
       <c r="F94" s="12" t="s">
-        <v>283</v>
+        <v>259</v>
       </c>
       <c r="G94" s="12" t="s">
         <v>211</v>
@@ -6608,20 +6647,17 @@
       <c r="H94" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="I94" s="12" t="s">
-        <v>243</v>
-      </c>
       <c r="J94" s="12" t="s">
         <v>103</v>
       </c>
       <c r="K94" s="13" t="s">
-        <v>43</v>
+        <v>129</v>
       </c>
       <c r="L94" s="12" t="s">
-        <v>286</v>
-      </c>
-      <c r="M94" s="53">
-        <v>17.579999999999998</v>
+        <v>260</v>
+      </c>
+      <c r="M94" s="12">
+        <v>20.55</v>
       </c>
       <c r="N94" s="47" t="s">
         <v>109</v>
@@ -6645,12 +6681,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="95" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A95" s="12">
         <v>2035</v>
       </c>
       <c r="B95" s="12" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="C95" s="12" t="s">
         <v>17</v>
@@ -6659,7 +6695,7 @@
         <v>243</v>
       </c>
       <c r="F95" s="12" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="G95" s="12" t="s">
         <v>211</v>
@@ -6671,13 +6707,13 @@
         <v>103</v>
       </c>
       <c r="K95" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L95" s="12" t="s">
-        <v>288</v>
+        <v>276</v>
       </c>
       <c r="M95" s="53">
-        <v>15.06</v>
+        <v>13.68</v>
       </c>
       <c r="N95" s="47" t="s">
         <v>109</v>
@@ -6701,79 +6737,250 @@
         <v>75</v>
       </c>
     </row>
-    <row r="96" spans="1:20" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="24">
+    <row r="96" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B96" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="C96" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D96" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="F96" s="12" t="s">
+        <v>280</v>
+      </c>
+      <c r="G96" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="H96" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="J96" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="K96" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="L96" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="M96" s="53">
+        <v>14.55</v>
+      </c>
+      <c r="N96" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="O96" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="P96" s="12">
+        <v>0.87</v>
+      </c>
+      <c r="Q96" s="12">
+        <v>0.78</v>
+      </c>
+      <c r="R96" s="14">
+        <v>100</v>
+      </c>
+      <c r="S96" s="14">
+        <v>0</v>
+      </c>
+      <c r="T96" s="14">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="97" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B97" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="C97" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D97" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="F97" s="12" t="s">
+        <v>283</v>
+      </c>
+      <c r="G97" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="H97" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="I97" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="J97" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="K97" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="L97" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="M97" s="53">
+        <v>17.579999999999998</v>
+      </c>
+      <c r="N97" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="O97" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="P97" s="12">
+        <v>0.87</v>
+      </c>
+      <c r="Q97" s="12">
+        <v>0.78</v>
+      </c>
+      <c r="R97" s="14">
+        <v>100</v>
+      </c>
+      <c r="S97" s="14">
+        <v>0</v>
+      </c>
+      <c r="T97" s="14">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="98" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B98" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="C98" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D98" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="F98" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="G98" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="H98" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="J98" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="K98" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="L98" s="12" t="s">
+        <v>288</v>
+      </c>
+      <c r="M98" s="53">
+        <v>15.06</v>
+      </c>
+      <c r="N98" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="O98" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="P98" s="12">
+        <v>0.87</v>
+      </c>
+      <c r="Q98" s="12">
+        <v>0.78</v>
+      </c>
+      <c r="R98" s="14">
+        <v>100</v>
+      </c>
+      <c r="S98" s="14">
+        <v>0</v>
+      </c>
+      <c r="T98" s="14">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="99" spans="1:20" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="24">
         <v>2050</v>
       </c>
-      <c r="B96" s="24" t="s">
+      <c r="B99" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="C96" s="24" t="s">
+      <c r="C99" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="D96" s="24" t="s">
+      <c r="D99" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="F96" s="24" t="s">
+      <c r="F99" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="G96" s="24" t="s">
+      <c r="G99" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="H96" s="25" t="s">
+      <c r="H99" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="J96" s="24" t="s">
+      <c r="J99" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="K96" s="26" t="s">
+      <c r="K99" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="L96" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="M96" s="24">
+      <c r="L99" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="M99" s="24">
         <v>17.440000000000001</v>
       </c>
-      <c r="N96" s="48">
+      <c r="N99" s="48">
         <v>-0.33</v>
       </c>
-      <c r="O96" s="48">
-        <v>0</v>
-      </c>
-      <c r="P96" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q96" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="R96" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="S96" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="T96" s="27" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="98" spans="13:14" x14ac:dyDescent="0.2">
-      <c r="M98" s="1">
-        <f>M92*2</f>
+      <c r="O99" s="48">
+        <v>0</v>
+      </c>
+      <c r="P99" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q99" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="R99" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="S99" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="T99" s="27" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="101" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="M101" s="1">
+        <f>M95*2</f>
         <v>27.36</v>
       </c>
-      <c r="N98" s="44">
-        <f>M91*2</f>
+      <c r="N101" s="44">
+        <f>M94*2</f>
         <v>41.1</v>
       </c>
     </row>
-    <row r="99" spans="13:14" x14ac:dyDescent="0.2">
-      <c r="M99" s="1">
-        <f>M92*3</f>
+    <row r="102" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="M102" s="1">
+        <f>M95*3</f>
         <v>41.04</v>
       </c>
-      <c r="N99" s="44">
-        <f>M91*3</f>
+      <c r="N102" s="44">
+        <f>M94*3</f>
         <v>61.650000000000006</v>
       </c>
     </row>

</xml_diff>

<commit_message>
correcting descriptions for v51, v52, v53
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one-master\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F418DA-762A-472B-8C98-513FE4588819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAF598D8-000D-4E60-9014-7C6826F64B91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="19200" windowHeight="8600" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelRuns" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="330">
   <si>
     <t>year</t>
   </si>
@@ -1010,15 +1010,6 @@
     <t>2023_TM160_IPA_53</t>
   </si>
   <si>
-    <t>AOC=16.21, with rail/ferry hes =70</t>
-  </si>
-  <si>
-    <t>AOC=16.21, with rail/ferry hes =65</t>
-  </si>
-  <si>
-    <t>AOC=16.21, with rail/ferry hes =60</t>
-  </si>
-  <si>
     <t>https://app.asana.com/0/1204085012544660/1206685870182016/f</t>
   </si>
   <si>
@@ -1028,7 +1019,13 @@
     <t>https://app.asana.com/0/1204085012544660/1206699871295080/f</t>
   </si>
   <si>
-    <t>tbd</t>
+    <t>AOC=16.21, with wrk_trn_hes=90</t>
+  </si>
+  <si>
+    <t>AOC=16.21, with wrk_trn_hes=80</t>
+  </si>
+  <si>
+    <t>AOC=16.21, with wrk_trn_hes=70</t>
   </si>
 </sst>
 </file>
@@ -1625,7 +1622,7 @@
   <dimension ref="A1:T102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="H44" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G60" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="K72" sqref="K72"/>
@@ -5311,7 +5308,7 @@
         <v>245</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="G70" s="1" t="s">
         <v>9</v>
@@ -5326,10 +5323,10 @@
         <v>292</v>
       </c>
       <c r="K70" s="10" t="s">
-        <v>330</v>
+        <v>42</v>
       </c>
       <c r="L70" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="M70" s="1">
         <v>16.21</v>
@@ -5370,7 +5367,7 @@
         <v>245</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="G71" s="1" t="s">
         <v>9</v>
@@ -5385,10 +5382,10 @@
         <v>292</v>
       </c>
       <c r="K71" s="10" t="s">
-        <v>330</v>
+        <v>88</v>
       </c>
       <c r="L71" s="1" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="M71" s="1">
         <v>16.21</v>
@@ -5429,7 +5426,7 @@
         <v>245</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="G72" s="1" t="s">
         <v>9</v>
@@ -5444,10 +5441,10 @@
         <v>292</v>
       </c>
       <c r="K72" s="10" t="s">
-        <v>330</v>
+        <v>16</v>
       </c>
       <c r="L72" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="M72" s="1">
         <v>16.21</v>

</xml_diff>

<commit_message>
add 2023 v54 to the run log
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one-master\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE32E68A-E1A0-424E-A348-A06E06E9D9FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0574D523-497A-4754-B8FE-50CD67E3759F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="165" yWindow="4365" windowWidth="34980" windowHeight="15090" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelRuns" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="340">
   <si>
     <t>year</t>
   </si>
@@ -1062,6 +1062,18 @@
   </si>
   <si>
     <t>2035 IPA</t>
+  </si>
+  <si>
+    <t>2023_TM160_IPA_54</t>
+  </si>
+  <si>
+    <t>AOC=16.21, with wrk_trn_hes=83.3</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1206710598691438/f</t>
+  </si>
+  <si>
+    <t>2023 v54</t>
   </si>
 </sst>
 </file>
@@ -1071,7 +1083,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1111,12 +1123,6 @@
       <color rgb="FFFF0000"/>
       <name val="Consolas"/>
       <family val="3"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="13">
@@ -1372,9 +1378,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1412,7 +1418,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1518,7 +1524,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1660,7 +1666,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1676,35 +1682,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9564CC59-3725-4FDA-8BF2-0F68CB1B6F5A}">
-  <dimension ref="A1:U102"/>
+  <dimension ref="A1:U103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C67" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U98" sqref="U98"/>
+      <selection pane="bottomRight" activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="42.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.54296875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="42.26953125" style="1" customWidth="1"/>
     <col min="7" max="7" width="23" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.28515625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" style="10" customWidth="1"/>
-    <col min="12" max="12" width="17.5703125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="8.28515625" style="1" customWidth="1"/>
-    <col min="14" max="15" width="9.28515625" style="44"/>
-    <col min="16" max="16384" width="9.28515625" style="1"/>
+    <col min="8" max="8" width="8.26953125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="6.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.26953125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11.26953125" style="10" customWidth="1"/>
+    <col min="12" max="12" width="17.54296875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="8.26953125" style="1" customWidth="1"/>
+    <col min="14" max="15" width="9.26953125" style="44"/>
+    <col min="16" max="16384" width="9.26953125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="5" customFormat="1" ht="39" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1769,7 +1775,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19">
         <v>2005</v>
       </c>
@@ -1822,7 +1828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="31">
         <v>2005</v>
       </c>
@@ -1878,7 +1884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="31">
         <v>2005</v>
       </c>
@@ -1933,7 +1939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:21" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="31">
         <v>2005</v>
       </c>
@@ -1988,7 +1994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:21" s="55" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" s="55" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="54">
         <v>2015</v>
       </c>
@@ -2029,7 +2035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="35">
         <v>2015</v>
       </c>
@@ -2075,7 +2081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="35">
         <v>2015</v>
       </c>
@@ -2128,7 +2134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="35">
         <v>2015</v>
       </c>
@@ -2181,7 +2187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="35">
         <v>2015</v>
       </c>
@@ -2234,7 +2240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="35">
         <v>2015</v>
       </c>
@@ -2290,7 +2296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="35">
         <v>2015</v>
       </c>
@@ -2346,7 +2352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="35">
         <v>2015</v>
       </c>
@@ -2402,7 +2408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="35">
         <v>2015</v>
       </c>
@@ -2464,7 +2470,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>2023</v>
       </c>
@@ -2510,7 +2516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>2023</v>
       </c>
@@ -2556,7 +2562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>2023</v>
       </c>
@@ -2602,7 +2608,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>2023</v>
       </c>
@@ -2648,7 +2654,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>2023</v>
       </c>
@@ -2694,7 +2700,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>2023</v>
       </c>
@@ -2740,7 +2746,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>2023</v>
       </c>
@@ -2786,7 +2792,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>2023</v>
       </c>
@@ -2832,7 +2838,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>2023</v>
       </c>
@@ -2878,7 +2884,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>2023</v>
       </c>
@@ -2924,7 +2930,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>2023</v>
       </c>
@@ -2970,7 +2976,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>2023</v>
       </c>
@@ -3016,7 +3022,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>2023</v>
       </c>
@@ -3062,7 +3068,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>2023</v>
       </c>
@@ -3108,7 +3114,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>2023</v>
       </c>
@@ -3154,7 +3160,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>2023</v>
       </c>
@@ -3200,7 +3206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>2023</v>
       </c>
@@ -3246,7 +3252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>2023</v>
       </c>
@@ -3292,7 +3298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>2023</v>
       </c>
@@ -3336,7 +3342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>2023</v>
       </c>
@@ -3385,7 +3391,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>2023</v>
       </c>
@@ -3432,7 +3438,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>2023</v>
       </c>
@@ -3479,7 +3485,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>2023</v>
       </c>
@@ -3535,7 +3541,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>2023</v>
       </c>
@@ -3591,7 +3597,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>2023</v>
       </c>
@@ -3647,7 +3653,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>2023</v>
       </c>
@@ -3703,7 +3709,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>2023</v>
       </c>
@@ -3759,7 +3765,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>2023</v>
       </c>
@@ -3815,7 +3821,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>2023</v>
       </c>
@@ -3871,7 +3877,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>2023</v>
       </c>
@@ -3927,7 +3933,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>2023</v>
       </c>
@@ -3983,7 +3989,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>2023</v>
       </c>
@@ -4039,7 +4045,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>2023</v>
       </c>
@@ -4095,7 +4101,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>2023</v>
       </c>
@@ -4151,7 +4157,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>2023</v>
       </c>
@@ -4207,7 +4213,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>2023</v>
       </c>
@@ -4263,7 +4269,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>2023</v>
       </c>
@@ -4319,7 +4325,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>2023</v>
       </c>
@@ -4375,7 +4381,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>2023</v>
       </c>
@@ -4431,7 +4437,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>2023</v>
       </c>
@@ -4487,7 +4493,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>2023</v>
       </c>
@@ -4543,7 +4549,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>2023</v>
       </c>
@@ -4599,7 +4605,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>2023</v>
       </c>
@@ -4655,7 +4661,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>2023</v>
       </c>
@@ -4711,7 +4717,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>2023</v>
       </c>
@@ -4767,7 +4773,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>2023</v>
       </c>
@@ -4823,7 +4829,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>2023</v>
       </c>
@@ -4879,7 +4885,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>2023</v>
       </c>
@@ -4941,7 +4947,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>2023</v>
       </c>
@@ -4997,7 +5003,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>2023</v>
       </c>
@@ -5059,7 +5065,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>2023</v>
       </c>
@@ -5121,7 +5127,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>2023</v>
       </c>
@@ -5183,7 +5189,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>2023</v>
       </c>
@@ -5245,7 +5251,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="68" spans="1:21" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:21" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>2023</v>
       </c>
@@ -5301,7 +5307,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="69" spans="1:21" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:21" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>2023</v>
       </c>
@@ -5357,7 +5363,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>2023</v>
       </c>
@@ -5419,7 +5425,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>2023</v>
       </c>
@@ -5481,7 +5487,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>2023</v>
       </c>
@@ -5543,155 +5549,161 @@
         <v>334</v>
       </c>
     </row>
-    <row r="73" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="28">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A73" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I73" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J73" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="K73" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="L73" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="M73" s="1">
+        <v>16.21</v>
+      </c>
+      <c r="N73" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="O73" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="P73" s="1">
+        <v>1.04</v>
+      </c>
+      <c r="Q73" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="R73" s="6">
+        <v>83.3</v>
+      </c>
+      <c r="S73" s="6">
+        <v>0</v>
+      </c>
+      <c r="T73" s="6">
+        <v>75</v>
+      </c>
+      <c r="U73" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="74" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="28">
         <v>2025</v>
       </c>
-      <c r="B73" s="28" t="s">
+      <c r="B74" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="C73" s="28" t="s">
+      <c r="C74" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="D73" s="28" t="s">
+      <c r="D74" s="28" t="s">
         <v>244</v>
       </c>
-      <c r="F73" s="28" t="s">
+      <c r="F74" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="J73" s="28" t="s">
+      <c r="J74" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="K73" s="29" t="s">
+      <c r="K74" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="N73" s="45"/>
-      <c r="O73" s="45"/>
-      <c r="R73" s="30"/>
-      <c r="S73" s="30"/>
-      <c r="T73" s="30"/>
-    </row>
-    <row r="74" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="15">
+      <c r="N74" s="45"/>
+      <c r="O74" s="45"/>
+      <c r="R74" s="30"/>
+      <c r="S74" s="30"/>
+      <c r="T74" s="30"/>
+    </row>
+    <row r="75" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="15">
         <v>2035</v>
       </c>
-      <c r="B74" s="15" t="s">
+      <c r="B75" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="C74" s="15" t="s">
+      <c r="C75" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="D74" s="15" t="s">
+      <c r="D75" s="15" t="s">
         <v>244</v>
       </c>
-      <c r="F74" s="15" t="s">
+      <c r="F75" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="G74" s="15" t="s">
+      <c r="G75" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="H74" s="18" t="s">
+      <c r="H75" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="I74" s="15" t="s">
+      <c r="I75" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="J74" s="15" t="s">
+      <c r="J75" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="K74" s="16" t="s">
+      <c r="K75" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="L74" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="M74" s="15">
+      <c r="L75" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="M75" s="15">
         <v>15.85</v>
       </c>
-      <c r="N74" s="46">
+      <c r="N75" s="46">
         <v>-0.27</v>
       </c>
-      <c r="O74" s="46">
-        <v>0</v>
-      </c>
-      <c r="P74" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q74" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="R74" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="S74" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="T74" s="17" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="75" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="12">
-        <v>2035</v>
-      </c>
-      <c r="B75" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="C75" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D75" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="F75" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="G75" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="H75" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="J75" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="K75" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="L75" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="M75" s="12">
-        <v>15.85</v>
-      </c>
-      <c r="N75" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="O75" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="P75" s="14">
-        <v>1.27</v>
-      </c>
-      <c r="Q75" s="14">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="R75" s="14">
-        <v>120</v>
-      </c>
-      <c r="S75" s="14">
-        <v>0</v>
-      </c>
-      <c r="T75" s="14">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="76" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O75" s="46">
+        <v>0</v>
+      </c>
+      <c r="P75" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q75" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="R75" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="S75" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="T75" s="17" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="76" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="12">
         <v>2035</v>
       </c>
       <c r="B76" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C76" s="12" t="s">
         <v>17</v>
@@ -5700,7 +5712,7 @@
         <v>243</v>
       </c>
       <c r="F76" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G76" s="12" t="s">
         <v>9</v>
@@ -5712,13 +5724,13 @@
         <v>103</v>
       </c>
       <c r="K76" s="13" t="s">
-        <v>108</v>
+        <v>43</v>
       </c>
       <c r="L76" s="12" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="M76" s="12">
-        <v>18.64</v>
+        <v>15.85</v>
       </c>
       <c r="N76" s="47" t="s">
         <v>109</v>
@@ -5742,12 +5754,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="77" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="12">
         <v>2035</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C77" s="12" t="s">
         <v>17</v>
@@ -5756,7 +5768,7 @@
         <v>243</v>
       </c>
       <c r="F77" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G77" s="12" t="s">
         <v>9</v>
@@ -5768,10 +5780,10 @@
         <v>103</v>
       </c>
       <c r="K77" s="13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L77" s="12" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="M77" s="12">
         <v>18.64</v>
@@ -5789,21 +5801,21 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="R77" s="14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="S77" s="14">
         <v>0</v>
       </c>
       <c r="T77" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="12">
         <v>2035</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="C78" s="12" t="s">
         <v>17</v>
@@ -5812,7 +5824,7 @@
         <v>243</v>
       </c>
       <c r="F78" s="12" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="G78" s="12" t="s">
         <v>9</v>
@@ -5824,10 +5836,10 @@
         <v>103</v>
       </c>
       <c r="K78" s="13" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="L78" s="12" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="M78" s="12">
         <v>18.64</v>
@@ -5838,28 +5850,28 @@
       <c r="O78" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="P78" s="12">
-        <v>0.95</v>
-      </c>
-      <c r="Q78" s="12">
-        <v>0.86</v>
+      <c r="P78" s="14">
+        <v>1.27</v>
+      </c>
+      <c r="Q78" s="14">
+        <v>1.1499999999999999</v>
       </c>
       <c r="R78" s="14">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="S78" s="14">
         <v>0</v>
       </c>
       <c r="T78" s="14">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="79" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="12">
         <v>2035</v>
       </c>
       <c r="B79" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C79" s="12" t="s">
         <v>17</v>
@@ -5868,7 +5880,7 @@
         <v>243</v>
       </c>
       <c r="F79" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G79" s="12" t="s">
         <v>9</v>
@@ -5880,10 +5892,10 @@
         <v>103</v>
       </c>
       <c r="K79" s="13" t="s">
-        <v>42</v>
+        <v>108</v>
       </c>
       <c r="L79" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="M79" s="12">
         <v>18.64</v>
@@ -5901,21 +5913,21 @@
         <v>0.86</v>
       </c>
       <c r="R79" s="14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="S79" s="14">
         <v>0</v>
       </c>
       <c r="T79" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="80" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="12">
         <v>2035</v>
       </c>
       <c r="B80" s="12" t="s">
-        <v>184</v>
+        <v>120</v>
       </c>
       <c r="C80" s="12" t="s">
         <v>17</v>
@@ -5924,7 +5936,7 @@
         <v>243</v>
       </c>
       <c r="F80" s="12" t="s">
-        <v>209</v>
+        <v>122</v>
       </c>
       <c r="G80" s="12" t="s">
         <v>9</v>
@@ -5936,10 +5948,10 @@
         <v>103</v>
       </c>
       <c r="K80" s="13" t="s">
-        <v>108</v>
+        <v>42</v>
       </c>
       <c r="L80" s="12" t="s">
-        <v>186</v>
+        <v>123</v>
       </c>
       <c r="M80" s="12">
         <v>18.64</v>
@@ -5966,12 +5978,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="12">
         <v>2035</v>
       </c>
       <c r="B81" s="12" t="s">
-        <v>207</v>
+        <v>184</v>
       </c>
       <c r="C81" s="12" t="s">
         <v>17</v>
@@ -5980,7 +5992,7 @@
         <v>243</v>
       </c>
       <c r="F81" s="12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G81" s="12" t="s">
         <v>9</v>
@@ -5992,7 +6004,7 @@
         <v>103</v>
       </c>
       <c r="K81" s="13" t="s">
-        <v>44</v>
+        <v>108</v>
       </c>
       <c r="L81" s="12" t="s">
         <v>186</v>
@@ -6022,12 +6034,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="12">
         <v>2035</v>
       </c>
       <c r="B82" s="12" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C82" s="12" t="s">
         <v>17</v>
@@ -6036,13 +6048,13 @@
         <v>243</v>
       </c>
       <c r="F82" s="12" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="G82" s="12" t="s">
-        <v>211</v>
+        <v>9</v>
       </c>
       <c r="H82" s="12" t="s">
-        <v>116</v>
+        <v>10</v>
       </c>
       <c r="J82" s="12" t="s">
         <v>103</v>
@@ -6051,7 +6063,7 @@
         <v>44</v>
       </c>
       <c r="L82" s="12" t="s">
-        <v>212</v>
+        <v>186</v>
       </c>
       <c r="M82" s="12">
         <v>18.64</v>
@@ -6069,21 +6081,21 @@
         <v>0.86</v>
       </c>
       <c r="R82" s="14">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="S82" s="14">
         <v>0</v>
       </c>
       <c r="T82" s="14">
-        <v>41.25</v>
-      </c>
-    </row>
-    <row r="83" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="12">
         <v>2035</v>
       </c>
       <c r="B83" s="12" t="s">
-        <v>228</v>
+        <v>206</v>
       </c>
       <c r="C83" s="12" t="s">
         <v>17</v>
@@ -6092,7 +6104,7 @@
         <v>243</v>
       </c>
       <c r="F83" s="12" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
       <c r="G83" s="12" t="s">
         <v>211</v>
@@ -6104,13 +6116,13 @@
         <v>103</v>
       </c>
       <c r="K83" s="13" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L83" s="12" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="M83" s="12">
-        <v>20.55</v>
+        <v>18.64</v>
       </c>
       <c r="N83" s="47" t="s">
         <v>109</v>
@@ -6119,10 +6131,10 @@
         <v>109</v>
       </c>
       <c r="P83" s="12">
-        <v>0.99</v>
+        <v>0.95</v>
       </c>
       <c r="Q83" s="12">
-        <v>0.89</v>
+        <v>0.86</v>
       </c>
       <c r="R83" s="14">
         <v>100</v>
@@ -6131,15 +6143,15 @@
         <v>0</v>
       </c>
       <c r="T83" s="14">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="84" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>41.25</v>
+      </c>
+    </row>
+    <row r="84" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A84" s="12">
         <v>2035</v>
       </c>
       <c r="B84" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C84" s="12" t="s">
         <v>17</v>
@@ -6148,7 +6160,7 @@
         <v>243</v>
       </c>
       <c r="F84" s="12" t="s">
-        <v>269</v>
+        <v>226</v>
       </c>
       <c r="G84" s="12" t="s">
         <v>211</v>
@@ -6160,10 +6172,10 @@
         <v>103</v>
       </c>
       <c r="K84" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L84" s="12" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="M84" s="12">
         <v>20.55</v>
@@ -6190,12 +6202,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="85" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="12">
         <v>2035</v>
       </c>
       <c r="B85" s="12" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C85" s="12" t="s">
         <v>17</v>
@@ -6204,22 +6216,22 @@
         <v>243</v>
       </c>
       <c r="F85" s="12" t="s">
-        <v>270</v>
-      </c>
-      <c r="G85" s="53" t="s">
-        <v>232</v>
+        <v>269</v>
+      </c>
+      <c r="G85" s="12" t="s">
+        <v>211</v>
       </c>
       <c r="H85" s="12" t="s">
-        <v>233</v>
+        <v>116</v>
       </c>
       <c r="J85" s="12" t="s">
         <v>103</v>
       </c>
       <c r="K85" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L85" s="12" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="M85" s="12">
         <v>20.55</v>
@@ -6246,12 +6258,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="86" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" s="12">
         <v>2035</v>
       </c>
       <c r="B86" s="12" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C86" s="12" t="s">
         <v>17</v>
@@ -6260,25 +6272,25 @@
         <v>243</v>
       </c>
       <c r="F86" s="12" t="s">
-        <v>271</v>
-      </c>
-      <c r="G86" s="12" t="s">
-        <v>211</v>
+        <v>270</v>
+      </c>
+      <c r="G86" s="53" t="s">
+        <v>232</v>
       </c>
       <c r="H86" s="12" t="s">
-        <v>116</v>
+        <v>233</v>
       </c>
       <c r="J86" s="12" t="s">
         <v>103</v>
       </c>
       <c r="K86" s="13" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="L86" s="12" t="s">
-        <v>236</v>
-      </c>
-      <c r="M86" s="53">
-        <v>15.85</v>
+        <v>234</v>
+      </c>
+      <c r="M86" s="12">
+        <v>20.55</v>
       </c>
       <c r="N86" s="47" t="s">
         <v>109</v>
@@ -6302,12 +6314,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="87" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" s="12">
         <v>2035</v>
       </c>
       <c r="B87" s="12" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="C87" s="12" t="s">
         <v>17</v>
@@ -6316,7 +6328,7 @@
         <v>243</v>
       </c>
       <c r="F87" s="12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G87" s="12" t="s">
         <v>211</v>
@@ -6328,13 +6340,13 @@
         <v>103</v>
       </c>
       <c r="K87" s="13" t="s">
-        <v>110</v>
+        <v>16</v>
       </c>
       <c r="L87" s="12" t="s">
-        <v>242</v>
-      </c>
-      <c r="M87" s="12">
-        <v>20.55</v>
+        <v>236</v>
+      </c>
+      <c r="M87" s="53">
+        <v>15.85</v>
       </c>
       <c r="N87" s="47" t="s">
         <v>109</v>
@@ -6348,22 +6360,22 @@
       <c r="Q87" s="12">
         <v>0.89</v>
       </c>
-      <c r="R87" s="52">
-        <v>0</v>
-      </c>
-      <c r="S87" s="52">
-        <v>0</v>
-      </c>
-      <c r="T87" s="52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R87" s="14">
+        <v>100</v>
+      </c>
+      <c r="S87" s="14">
+        <v>0</v>
+      </c>
+      <c r="T87" s="14">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="88" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="12">
         <v>2035</v>
       </c>
       <c r="B88" s="12" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="C88" s="12" t="s">
         <v>17</v>
@@ -6372,7 +6384,7 @@
         <v>243</v>
       </c>
       <c r="F88" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G88" s="12" t="s">
         <v>211</v>
@@ -6384,10 +6396,10 @@
         <v>103</v>
       </c>
       <c r="K88" s="13" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="L88" s="12" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="M88" s="12">
         <v>20.55</v>
@@ -6404,22 +6416,22 @@
       <c r="Q88" s="12">
         <v>0.89</v>
       </c>
-      <c r="R88" s="14">
-        <v>100</v>
-      </c>
-      <c r="S88" s="14">
-        <v>0</v>
-      </c>
-      <c r="T88" s="14">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="89" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R88" s="52">
+        <v>0</v>
+      </c>
+      <c r="S88" s="52">
+        <v>0</v>
+      </c>
+      <c r="T88" s="52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="12">
         <v>2035</v>
       </c>
       <c r="B89" s="12" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="C89" s="12" t="s">
         <v>17</v>
@@ -6428,7 +6440,7 @@
         <v>243</v>
       </c>
       <c r="F89" s="12" t="s">
-        <v>249</v>
+        <v>273</v>
       </c>
       <c r="G89" s="12" t="s">
         <v>211</v>
@@ -6440,10 +6452,10 @@
         <v>103</v>
       </c>
       <c r="K89" s="13" t="s">
-        <v>43</v>
+        <v>129</v>
       </c>
       <c r="L89" s="12" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="M89" s="12">
         <v>20.55</v>
@@ -6455,10 +6467,10 @@
         <v>109</v>
       </c>
       <c r="P89" s="12">
-        <v>0.87</v>
+        <v>0.99</v>
       </c>
       <c r="Q89" s="12">
-        <v>0.78</v>
+        <v>0.89</v>
       </c>
       <c r="R89" s="14">
         <v>100</v>
@@ -6470,12 +6482,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="90" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90" s="12">
         <v>2035</v>
       </c>
       <c r="B90" s="12" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C90" s="12" t="s">
         <v>17</v>
@@ -6484,7 +6496,7 @@
         <v>243</v>
       </c>
       <c r="F90" s="12" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G90" s="12" t="s">
         <v>211</v>
@@ -6499,7 +6511,7 @@
         <v>43</v>
       </c>
       <c r="L90" s="12" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="M90" s="12">
         <v>20.55</v>
@@ -6526,12 +6538,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="91" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" s="12">
         <v>2035</v>
       </c>
       <c r="B91" s="12" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="C91" s="12" t="s">
         <v>17</v>
@@ -6540,7 +6552,7 @@
         <v>243</v>
       </c>
       <c r="F91" s="12" t="s">
-        <v>239</v>
+        <v>252</v>
       </c>
       <c r="G91" s="12" t="s">
         <v>211</v>
@@ -6552,10 +6564,10 @@
         <v>103</v>
       </c>
       <c r="K91" s="13" t="s">
-        <v>108</v>
+        <v>43</v>
       </c>
       <c r="L91" s="12" t="s">
-        <v>240</v>
+        <v>253</v>
       </c>
       <c r="M91" s="12">
         <v>20.55</v>
@@ -6566,11 +6578,11 @@
       <c r="O91" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="P91" s="53">
-        <v>0.84</v>
-      </c>
-      <c r="Q91" s="53">
-        <v>1.59</v>
+      <c r="P91" s="12">
+        <v>0.87</v>
+      </c>
+      <c r="Q91" s="12">
+        <v>0.78</v>
       </c>
       <c r="R91" s="14">
         <v>100</v>
@@ -6582,12 +6594,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="92" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="12">
         <v>2035</v>
       </c>
       <c r="B92" s="12" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C92" s="12" t="s">
         <v>17</v>
@@ -6596,7 +6608,7 @@
         <v>243</v>
       </c>
       <c r="F92" s="12" t="s">
-        <v>255</v>
+        <v>239</v>
       </c>
       <c r="G92" s="12" t="s">
         <v>211</v>
@@ -6608,10 +6620,10 @@
         <v>103</v>
       </c>
       <c r="K92" s="13" t="s">
-        <v>43</v>
+        <v>108</v>
       </c>
       <c r="L92" s="12" t="s">
-        <v>256</v>
+        <v>240</v>
       </c>
       <c r="M92" s="12">
         <v>20.55</v>
@@ -6622,11 +6634,11 @@
       <c r="O92" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="P92" s="12">
-        <v>0.87</v>
-      </c>
-      <c r="Q92" s="12">
-        <v>0.78</v>
+      <c r="P92" s="53">
+        <v>0.84</v>
+      </c>
+      <c r="Q92" s="53">
+        <v>1.59</v>
       </c>
       <c r="R92" s="14">
         <v>100</v>
@@ -6638,12 +6650,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="93" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" s="12">
         <v>2035</v>
       </c>
       <c r="B93" s="12" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="C93" s="12" t="s">
         <v>17</v>
@@ -6652,7 +6664,7 @@
         <v>243</v>
       </c>
       <c r="F93" s="12" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="G93" s="12" t="s">
         <v>211</v>
@@ -6660,14 +6672,14 @@
       <c r="H93" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="J93" s="53" t="s">
-        <v>263</v>
+      <c r="J93" s="12" t="s">
+        <v>103</v>
       </c>
       <c r="K93" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L93" s="12" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="M93" s="12">
         <v>20.55</v>
@@ -6694,12 +6706,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="94" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" s="12">
         <v>2035</v>
       </c>
       <c r="B94" s="12" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="C94" s="12" t="s">
         <v>17</v>
@@ -6708,7 +6720,7 @@
         <v>243</v>
       </c>
       <c r="F94" s="12" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="G94" s="12" t="s">
         <v>211</v>
@@ -6716,14 +6728,14 @@
       <c r="H94" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="J94" s="12" t="s">
-        <v>103</v>
+      <c r="J94" s="53" t="s">
+        <v>263</v>
       </c>
       <c r="K94" s="13" t="s">
-        <v>129</v>
+        <v>42</v>
       </c>
       <c r="L94" s="12" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="M94" s="12">
         <v>20.55</v>
@@ -6750,12 +6762,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="95" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A95" s="12">
         <v>2035</v>
       </c>
       <c r="B95" s="12" t="s">
-        <v>274</v>
+        <v>258</v>
       </c>
       <c r="C95" s="12" t="s">
         <v>17</v>
@@ -6764,7 +6776,7 @@
         <v>243</v>
       </c>
       <c r="F95" s="12" t="s">
-        <v>275</v>
+        <v>259</v>
       </c>
       <c r="G95" s="12" t="s">
         <v>211</v>
@@ -6776,13 +6788,13 @@
         <v>103</v>
       </c>
       <c r="K95" s="13" t="s">
-        <v>43</v>
+        <v>129</v>
       </c>
       <c r="L95" s="12" t="s">
-        <v>276</v>
-      </c>
-      <c r="M95" s="53">
-        <v>13.68</v>
+        <v>260</v>
+      </c>
+      <c r="M95" s="12">
+        <v>20.55</v>
       </c>
       <c r="N95" s="47" t="s">
         <v>109</v>
@@ -6806,12 +6818,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="96" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A96" s="12">
         <v>2035</v>
       </c>
       <c r="B96" s="12" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="C96" s="12" t="s">
         <v>17</v>
@@ -6820,7 +6832,7 @@
         <v>243</v>
       </c>
       <c r="F96" s="12" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="G96" s="12" t="s">
         <v>211</v>
@@ -6835,10 +6847,10 @@
         <v>43</v>
       </c>
       <c r="L96" s="12" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="M96" s="53">
-        <v>14.55</v>
+        <v>13.68</v>
       </c>
       <c r="N96" s="47" t="s">
         <v>109</v>
@@ -6862,12 +6874,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="97" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A97" s="12">
         <v>2035</v>
       </c>
       <c r="B97" s="12" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C97" s="12" t="s">
         <v>17</v>
@@ -6876,7 +6888,7 @@
         <v>243</v>
       </c>
       <c r="F97" s="12" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="G97" s="12" t="s">
         <v>211</v>
@@ -6884,9 +6896,6 @@
       <c r="H97" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="I97" s="12" t="s">
-        <v>11</v>
-      </c>
       <c r="J97" s="12" t="s">
         <v>103</v>
       </c>
@@ -6894,10 +6903,10 @@
         <v>43</v>
       </c>
       <c r="L97" s="12" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="M97" s="53">
-        <v>17.579999999999998</v>
+        <v>14.55</v>
       </c>
       <c r="N97" s="47" t="s">
         <v>109</v>
@@ -6920,16 +6929,13 @@
       <c r="T97" s="14">
         <v>75</v>
       </c>
-      <c r="U97" s="12" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="98" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="98" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" s="12">
         <v>2035</v>
       </c>
       <c r="B98" s="12" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C98" s="12" t="s">
         <v>17</v>
@@ -6938,7 +6944,7 @@
         <v>243</v>
       </c>
       <c r="F98" s="12" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="G98" s="12" t="s">
         <v>211</v>
@@ -6946,17 +6952,20 @@
       <c r="H98" s="12" t="s">
         <v>116</v>
       </c>
+      <c r="I98" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="J98" s="12" t="s">
         <v>103</v>
       </c>
       <c r="K98" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L98" s="12" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="M98" s="53">
-        <v>15.06</v>
+        <v>17.579999999999998</v>
       </c>
       <c r="N98" s="47" t="s">
         <v>109</v>
@@ -6979,80 +6988,139 @@
       <c r="T98" s="14">
         <v>75</v>
       </c>
-    </row>
-    <row r="99" spans="1:21" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="24">
+      <c r="U98" s="12" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="99" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B99" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="C99" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D99" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="F99" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="G99" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="H99" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="J99" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="K99" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="L99" s="12" t="s">
+        <v>288</v>
+      </c>
+      <c r="M99" s="53">
+        <v>15.06</v>
+      </c>
+      <c r="N99" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="O99" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="P99" s="12">
+        <v>0.87</v>
+      </c>
+      <c r="Q99" s="12">
+        <v>0.78</v>
+      </c>
+      <c r="R99" s="14">
+        <v>100</v>
+      </c>
+      <c r="S99" s="14">
+        <v>0</v>
+      </c>
+      <c r="T99" s="14">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="100" spans="1:21" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="24">
         <v>2050</v>
       </c>
-      <c r="B99" s="24" t="s">
+      <c r="B100" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="C99" s="24" t="s">
+      <c r="C100" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="D99" s="24" t="s">
+      <c r="D100" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="F99" s="24" t="s">
+      <c r="F100" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="G99" s="24" t="s">
+      <c r="G100" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="H99" s="25" t="s">
+      <c r="H100" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="J99" s="24" t="s">
+      <c r="J100" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="K99" s="26" t="s">
+      <c r="K100" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="L99" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="M99" s="24">
+      <c r="L100" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="M100" s="24">
         <v>17.440000000000001</v>
       </c>
-      <c r="N99" s="48">
+      <c r="N100" s="48">
         <v>-0.33</v>
       </c>
-      <c r="O99" s="48">
-        <v>0</v>
-      </c>
-      <c r="P99" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q99" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="R99" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="S99" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="T99" s="27" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="101" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="M101" s="1">
+      <c r="O100" s="48">
+        <v>0</v>
+      </c>
+      <c r="P100" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q100" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="R100" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="S100" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="T100" s="27" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="102" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="M102" s="1">
+        <f>M96*2</f>
+        <v>27.36</v>
+      </c>
+      <c r="N102" s="44">
         <f>M95*2</f>
-        <v>27.36</v>
-      </c>
-      <c r="N101" s="44">
-        <f>M94*2</f>
         <v>41.1</v>
       </c>
     </row>
-    <row r="102" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="M102" s="1">
+    <row r="103" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="M103" s="1">
+        <f>M96*3</f>
+        <v>41.04</v>
+      </c>
+      <c r="N103" s="44">
         <f>M95*3</f>
-        <v>41.04</v>
-      </c>
-      <c r="N102" s="44">
-        <f>M94*3</f>
         <v>61.650000000000006</v>
       </c>
     </row>

</xml_diff>

<commit_message>
lower BART_Transit_Hesitance slightly (to 72.0 minutes)
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one-master\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0574D523-497A-4754-B8FE-50CD67E3759F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21AB7249-C4EE-43EA-8845-CA1E8F35EA8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="341">
   <si>
     <t>year</t>
   </si>
@@ -1052,15 +1052,6 @@
     <t>2015</t>
   </si>
   <si>
-    <t>2023 v51</t>
-  </si>
-  <si>
-    <t>2023 v52</t>
-  </si>
-  <si>
-    <t>2023 v53</t>
-  </si>
-  <si>
     <t>2035 IPA</t>
   </si>
   <si>
@@ -1074,6 +1065,18 @@
   </si>
   <si>
     <t>2023 v54</t>
+  </si>
+  <si>
+    <t>2023_TM160_IPA_55</t>
+  </si>
+  <si>
+    <t>AOC=16.21, with BART_Transit_Hesitance=70</t>
+  </si>
+  <si>
+    <t>tbd</t>
+  </si>
+  <si>
+    <t>2023 v55</t>
   </si>
 </sst>
 </file>
@@ -1682,13 +1685,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9564CC59-3725-4FDA-8BF2-0F68CB1B6F5A}">
-  <dimension ref="A1:U103"/>
+  <dimension ref="A1:U104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A73" sqref="A73"/>
+      <selection pane="bottomRight" activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -5385,9 +5388,6 @@
       <c r="H70" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I70" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="J70" s="1" t="s">
         <v>292</v>
       </c>
@@ -5420,9 +5420,6 @@
       </c>
       <c r="T70" s="6">
         <v>75</v>
-      </c>
-      <c r="U70" s="1" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.3">
@@ -5447,9 +5444,6 @@
       <c r="H71" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I71" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="J71" s="1" t="s">
         <v>292</v>
       </c>
@@ -5482,9 +5476,6 @@
       </c>
       <c r="T71" s="6">
         <v>75</v>
-      </c>
-      <c r="U71" s="1" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.3">
@@ -5509,9 +5500,6 @@
       <c r="H72" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I72" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="J72" s="1" t="s">
         <v>292</v>
       </c>
@@ -5544,9 +5532,6 @@
       </c>
       <c r="T72" s="6">
         <v>75</v>
-      </c>
-      <c r="U72" s="1" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="73" spans="1:21" x14ac:dyDescent="0.3">
@@ -5554,7 +5539,7 @@
         <v>2023</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>17</v>
@@ -5563,7 +5548,7 @@
         <v>245</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="G73" s="1" t="s">
         <v>9</v>
@@ -5581,7 +5566,7 @@
         <v>16</v>
       </c>
       <c r="L73" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="M73" s="1">
         <v>16.21</v>
@@ -5608,150 +5593,156 @@
         <v>75</v>
       </c>
       <c r="U73" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="74" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A74" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I74" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J74" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="K74" s="10" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="74" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="28">
+      <c r="L74" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="M74" s="1">
+        <v>16.21</v>
+      </c>
+      <c r="N74" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="O74" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="P74" s="1">
+        <v>1.04</v>
+      </c>
+      <c r="Q74" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="R74" s="6">
+        <v>83.3</v>
+      </c>
+      <c r="S74" s="6">
+        <v>0</v>
+      </c>
+      <c r="T74" s="6">
+        <v>72</v>
+      </c>
+      <c r="U74" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="75" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="28">
         <v>2025</v>
       </c>
-      <c r="B74" s="28" t="s">
+      <c r="B75" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="C74" s="28" t="s">
+      <c r="C75" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="D74" s="28" t="s">
+      <c r="D75" s="28" t="s">
         <v>244</v>
       </c>
-      <c r="F74" s="28" t="s">
+      <c r="F75" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="J74" s="28" t="s">
+      <c r="J75" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="K74" s="29" t="s">
+      <c r="K75" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="N74" s="45"/>
-      <c r="O74" s="45"/>
-      <c r="R74" s="30"/>
-      <c r="S74" s="30"/>
-      <c r="T74" s="30"/>
-    </row>
-    <row r="75" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="15">
+      <c r="N75" s="45"/>
+      <c r="O75" s="45"/>
+      <c r="R75" s="30"/>
+      <c r="S75" s="30"/>
+      <c r="T75" s="30"/>
+    </row>
+    <row r="76" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="15">
         <v>2035</v>
       </c>
-      <c r="B75" s="15" t="s">
+      <c r="B76" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="C75" s="15" t="s">
+      <c r="C76" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="D75" s="15" t="s">
+      <c r="D76" s="15" t="s">
         <v>244</v>
       </c>
-      <c r="F75" s="15" t="s">
+      <c r="F76" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="G75" s="15" t="s">
+      <c r="G76" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="H75" s="18" t="s">
+      <c r="H76" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="I75" s="15" t="s">
+      <c r="I76" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="J75" s="15" t="s">
+      <c r="J76" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="K75" s="16" t="s">
+      <c r="K76" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="L75" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="M75" s="15">
+      <c r="L76" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="M76" s="15">
         <v>15.85</v>
       </c>
-      <c r="N75" s="46">
+      <c r="N76" s="46">
         <v>-0.27</v>
       </c>
-      <c r="O75" s="46">
-        <v>0</v>
-      </c>
-      <c r="P75" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q75" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="R75" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="S75" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="T75" s="17" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="76" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="12">
-        <v>2035</v>
-      </c>
-      <c r="B76" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="C76" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D76" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="F76" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="G76" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="H76" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="J76" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="K76" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="L76" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="M76" s="12">
-        <v>15.85</v>
-      </c>
-      <c r="N76" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="O76" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="P76" s="14">
-        <v>1.27</v>
-      </c>
-      <c r="Q76" s="14">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="R76" s="14">
-        <v>120</v>
-      </c>
-      <c r="S76" s="14">
-        <v>0</v>
-      </c>
-      <c r="T76" s="14">
-        <v>45</v>
+      <c r="O76" s="46">
+        <v>0</v>
+      </c>
+      <c r="P76" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q76" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="R76" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="S76" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="T76" s="17" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="77" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -5759,7 +5750,7 @@
         <v>2035</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C77" s="12" t="s">
         <v>17</v>
@@ -5768,7 +5759,7 @@
         <v>243</v>
       </c>
       <c r="F77" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G77" s="12" t="s">
         <v>9</v>
@@ -5780,13 +5771,13 @@
         <v>103</v>
       </c>
       <c r="K77" s="13" t="s">
-        <v>108</v>
+        <v>43</v>
       </c>
       <c r="L77" s="12" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="M77" s="12">
-        <v>18.64</v>
+        <v>15.85</v>
       </c>
       <c r="N77" s="47" t="s">
         <v>109</v>
@@ -5815,7 +5806,7 @@
         <v>2035</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C78" s="12" t="s">
         <v>17</v>
@@ -5824,7 +5815,7 @@
         <v>243</v>
       </c>
       <c r="F78" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G78" s="12" t="s">
         <v>9</v>
@@ -5836,10 +5827,10 @@
         <v>103</v>
       </c>
       <c r="K78" s="13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L78" s="12" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="M78" s="12">
         <v>18.64</v>
@@ -5857,13 +5848,13 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="R78" s="14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="S78" s="14">
         <v>0</v>
       </c>
       <c r="T78" s="14">
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="79" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -5871,7 +5862,7 @@
         <v>2035</v>
       </c>
       <c r="B79" s="12" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="C79" s="12" t="s">
         <v>17</v>
@@ -5880,7 +5871,7 @@
         <v>243</v>
       </c>
       <c r="F79" s="12" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="G79" s="12" t="s">
         <v>9</v>
@@ -5892,10 +5883,10 @@
         <v>103</v>
       </c>
       <c r="K79" s="13" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="L79" s="12" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="M79" s="12">
         <v>18.64</v>
@@ -5906,20 +5897,20 @@
       <c r="O79" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="P79" s="12">
-        <v>0.95</v>
-      </c>
-      <c r="Q79" s="12">
-        <v>0.86</v>
+      <c r="P79" s="14">
+        <v>1.27</v>
+      </c>
+      <c r="Q79" s="14">
+        <v>1.1499999999999999</v>
       </c>
       <c r="R79" s="14">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="S79" s="14">
         <v>0</v>
       </c>
       <c r="T79" s="14">
-        <v>45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -5927,7 +5918,7 @@
         <v>2035</v>
       </c>
       <c r="B80" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C80" s="12" t="s">
         <v>17</v>
@@ -5936,7 +5927,7 @@
         <v>243</v>
       </c>
       <c r="F80" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G80" s="12" t="s">
         <v>9</v>
@@ -5948,10 +5939,10 @@
         <v>103</v>
       </c>
       <c r="K80" s="13" t="s">
-        <v>42</v>
+        <v>108</v>
       </c>
       <c r="L80" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="M80" s="12">
         <v>18.64</v>
@@ -5969,13 +5960,13 @@
         <v>0.86</v>
       </c>
       <c r="R80" s="14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="S80" s="14">
         <v>0</v>
       </c>
       <c r="T80" s="14">
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="81" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -5983,7 +5974,7 @@
         <v>2035</v>
       </c>
       <c r="B81" s="12" t="s">
-        <v>184</v>
+        <v>120</v>
       </c>
       <c r="C81" s="12" t="s">
         <v>17</v>
@@ -5992,7 +5983,7 @@
         <v>243</v>
       </c>
       <c r="F81" s="12" t="s">
-        <v>209</v>
+        <v>122</v>
       </c>
       <c r="G81" s="12" t="s">
         <v>9</v>
@@ -6004,10 +5995,10 @@
         <v>103</v>
       </c>
       <c r="K81" s="13" t="s">
-        <v>108</v>
+        <v>42</v>
       </c>
       <c r="L81" s="12" t="s">
-        <v>186</v>
+        <v>123</v>
       </c>
       <c r="M81" s="12">
         <v>18.64</v>
@@ -6039,7 +6030,7 @@
         <v>2035</v>
       </c>
       <c r="B82" s="12" t="s">
-        <v>207</v>
+        <v>184</v>
       </c>
       <c r="C82" s="12" t="s">
         <v>17</v>
@@ -6048,7 +6039,7 @@
         <v>243</v>
       </c>
       <c r="F82" s="12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G82" s="12" t="s">
         <v>9</v>
@@ -6060,7 +6051,7 @@
         <v>103</v>
       </c>
       <c r="K82" s="13" t="s">
-        <v>44</v>
+        <v>108</v>
       </c>
       <c r="L82" s="12" t="s">
         <v>186</v>
@@ -6095,7 +6086,7 @@
         <v>2035</v>
       </c>
       <c r="B83" s="12" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C83" s="12" t="s">
         <v>17</v>
@@ -6104,13 +6095,13 @@
         <v>243</v>
       </c>
       <c r="F83" s="12" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="G83" s="12" t="s">
-        <v>211</v>
+        <v>9</v>
       </c>
       <c r="H83" s="12" t="s">
-        <v>116</v>
+        <v>10</v>
       </c>
       <c r="J83" s="12" t="s">
         <v>103</v>
@@ -6119,7 +6110,7 @@
         <v>44</v>
       </c>
       <c r="L83" s="12" t="s">
-        <v>212</v>
+        <v>186</v>
       </c>
       <c r="M83" s="12">
         <v>18.64</v>
@@ -6137,13 +6128,13 @@
         <v>0.86</v>
       </c>
       <c r="R83" s="14">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="S83" s="14">
         <v>0</v>
       </c>
       <c r="T83" s="14">
-        <v>41.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -6151,7 +6142,7 @@
         <v>2035</v>
       </c>
       <c r="B84" s="12" t="s">
-        <v>228</v>
+        <v>206</v>
       </c>
       <c r="C84" s="12" t="s">
         <v>17</v>
@@ -6160,7 +6151,7 @@
         <v>243</v>
       </c>
       <c r="F84" s="12" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
       <c r="G84" s="12" t="s">
         <v>211</v>
@@ -6172,13 +6163,13 @@
         <v>103</v>
       </c>
       <c r="K84" s="13" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L84" s="12" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="M84" s="12">
-        <v>20.55</v>
+        <v>18.64</v>
       </c>
       <c r="N84" s="47" t="s">
         <v>109</v>
@@ -6187,10 +6178,10 @@
         <v>109</v>
       </c>
       <c r="P84" s="12">
-        <v>0.99</v>
+        <v>0.95</v>
       </c>
       <c r="Q84" s="12">
-        <v>0.89</v>
+        <v>0.86</v>
       </c>
       <c r="R84" s="14">
         <v>100</v>
@@ -6199,7 +6190,7 @@
         <v>0</v>
       </c>
       <c r="T84" s="14">
-        <v>75</v>
+        <v>41.25</v>
       </c>
     </row>
     <row r="85" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -6207,7 +6198,7 @@
         <v>2035</v>
       </c>
       <c r="B85" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C85" s="12" t="s">
         <v>17</v>
@@ -6216,7 +6207,7 @@
         <v>243</v>
       </c>
       <c r="F85" s="12" t="s">
-        <v>269</v>
+        <v>226</v>
       </c>
       <c r="G85" s="12" t="s">
         <v>211</v>
@@ -6228,10 +6219,10 @@
         <v>103</v>
       </c>
       <c r="K85" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L85" s="12" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="M85" s="12">
         <v>20.55</v>
@@ -6263,7 +6254,7 @@
         <v>2035</v>
       </c>
       <c r="B86" s="12" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C86" s="12" t="s">
         <v>17</v>
@@ -6272,22 +6263,22 @@
         <v>243</v>
       </c>
       <c r="F86" s="12" t="s">
-        <v>270</v>
-      </c>
-      <c r="G86" s="53" t="s">
-        <v>232</v>
+        <v>269</v>
+      </c>
+      <c r="G86" s="12" t="s">
+        <v>211</v>
       </c>
       <c r="H86" s="12" t="s">
-        <v>233</v>
+        <v>116</v>
       </c>
       <c r="J86" s="12" t="s">
         <v>103</v>
       </c>
       <c r="K86" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L86" s="12" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="M86" s="12">
         <v>20.55</v>
@@ -6319,7 +6310,7 @@
         <v>2035</v>
       </c>
       <c r="B87" s="12" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C87" s="12" t="s">
         <v>17</v>
@@ -6328,25 +6319,25 @@
         <v>243</v>
       </c>
       <c r="F87" s="12" t="s">
-        <v>271</v>
-      </c>
-      <c r="G87" s="12" t="s">
-        <v>211</v>
+        <v>270</v>
+      </c>
+      <c r="G87" s="53" t="s">
+        <v>232</v>
       </c>
       <c r="H87" s="12" t="s">
-        <v>116</v>
+        <v>233</v>
       </c>
       <c r="J87" s="12" t="s">
         <v>103</v>
       </c>
       <c r="K87" s="13" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="L87" s="12" t="s">
-        <v>236</v>
-      </c>
-      <c r="M87" s="53">
-        <v>15.85</v>
+        <v>234</v>
+      </c>
+      <c r="M87" s="12">
+        <v>20.55</v>
       </c>
       <c r="N87" s="47" t="s">
         <v>109</v>
@@ -6375,7 +6366,7 @@
         <v>2035</v>
       </c>
       <c r="B88" s="12" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="C88" s="12" t="s">
         <v>17</v>
@@ -6384,7 +6375,7 @@
         <v>243</v>
       </c>
       <c r="F88" s="12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G88" s="12" t="s">
         <v>211</v>
@@ -6396,13 +6387,13 @@
         <v>103</v>
       </c>
       <c r="K88" s="13" t="s">
-        <v>110</v>
+        <v>16</v>
       </c>
       <c r="L88" s="12" t="s">
-        <v>242</v>
-      </c>
-      <c r="M88" s="12">
-        <v>20.55</v>
+        <v>236</v>
+      </c>
+      <c r="M88" s="53">
+        <v>15.85</v>
       </c>
       <c r="N88" s="47" t="s">
         <v>109</v>
@@ -6416,14 +6407,14 @@
       <c r="Q88" s="12">
         <v>0.89</v>
       </c>
-      <c r="R88" s="52">
-        <v>0</v>
-      </c>
-      <c r="S88" s="52">
-        <v>0</v>
-      </c>
-      <c r="T88" s="52">
-        <v>0</v>
+      <c r="R88" s="14">
+        <v>100</v>
+      </c>
+      <c r="S88" s="14">
+        <v>0</v>
+      </c>
+      <c r="T88" s="14">
+        <v>75</v>
       </c>
     </row>
     <row r="89" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -6431,7 +6422,7 @@
         <v>2035</v>
       </c>
       <c r="B89" s="12" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="C89" s="12" t="s">
         <v>17</v>
@@ -6440,7 +6431,7 @@
         <v>243</v>
       </c>
       <c r="F89" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G89" s="12" t="s">
         <v>211</v>
@@ -6452,10 +6443,10 @@
         <v>103</v>
       </c>
       <c r="K89" s="13" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="L89" s="12" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="M89" s="12">
         <v>20.55</v>
@@ -6472,14 +6463,14 @@
       <c r="Q89" s="12">
         <v>0.89</v>
       </c>
-      <c r="R89" s="14">
-        <v>100</v>
-      </c>
-      <c r="S89" s="14">
-        <v>0</v>
-      </c>
-      <c r="T89" s="14">
-        <v>75</v>
+      <c r="R89" s="52">
+        <v>0</v>
+      </c>
+      <c r="S89" s="52">
+        <v>0</v>
+      </c>
+      <c r="T89" s="52">
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -6487,7 +6478,7 @@
         <v>2035</v>
       </c>
       <c r="B90" s="12" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="C90" s="12" t="s">
         <v>17</v>
@@ -6496,7 +6487,7 @@
         <v>243</v>
       </c>
       <c r="F90" s="12" t="s">
-        <v>249</v>
+        <v>273</v>
       </c>
       <c r="G90" s="12" t="s">
         <v>211</v>
@@ -6508,10 +6499,10 @@
         <v>103</v>
       </c>
       <c r="K90" s="13" t="s">
-        <v>43</v>
+        <v>129</v>
       </c>
       <c r="L90" s="12" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="M90" s="12">
         <v>20.55</v>
@@ -6523,10 +6514,10 @@
         <v>109</v>
       </c>
       <c r="P90" s="12">
-        <v>0.87</v>
+        <v>0.99</v>
       </c>
       <c r="Q90" s="12">
-        <v>0.78</v>
+        <v>0.89</v>
       </c>
       <c r="R90" s="14">
         <v>100</v>
@@ -6543,7 +6534,7 @@
         <v>2035</v>
       </c>
       <c r="B91" s="12" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C91" s="12" t="s">
         <v>17</v>
@@ -6552,7 +6543,7 @@
         <v>243</v>
       </c>
       <c r="F91" s="12" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G91" s="12" t="s">
         <v>211</v>
@@ -6567,7 +6558,7 @@
         <v>43</v>
       </c>
       <c r="L91" s="12" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="M91" s="12">
         <v>20.55</v>
@@ -6599,7 +6590,7 @@
         <v>2035</v>
       </c>
       <c r="B92" s="12" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="C92" s="12" t="s">
         <v>17</v>
@@ -6608,7 +6599,7 @@
         <v>243</v>
       </c>
       <c r="F92" s="12" t="s">
-        <v>239</v>
+        <v>252</v>
       </c>
       <c r="G92" s="12" t="s">
         <v>211</v>
@@ -6620,10 +6611,10 @@
         <v>103</v>
       </c>
       <c r="K92" s="13" t="s">
-        <v>108</v>
+        <v>43</v>
       </c>
       <c r="L92" s="12" t="s">
-        <v>240</v>
+        <v>253</v>
       </c>
       <c r="M92" s="12">
         <v>20.55</v>
@@ -6634,11 +6625,11 @@
       <c r="O92" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="P92" s="53">
-        <v>0.84</v>
-      </c>
-      <c r="Q92" s="53">
-        <v>1.59</v>
+      <c r="P92" s="12">
+        <v>0.87</v>
+      </c>
+      <c r="Q92" s="12">
+        <v>0.78</v>
       </c>
       <c r="R92" s="14">
         <v>100</v>
@@ -6655,7 +6646,7 @@
         <v>2035</v>
       </c>
       <c r="B93" s="12" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C93" s="12" t="s">
         <v>17</v>
@@ -6664,7 +6655,7 @@
         <v>243</v>
       </c>
       <c r="F93" s="12" t="s">
-        <v>255</v>
+        <v>239</v>
       </c>
       <c r="G93" s="12" t="s">
         <v>211</v>
@@ -6676,10 +6667,10 @@
         <v>103</v>
       </c>
       <c r="K93" s="13" t="s">
-        <v>43</v>
+        <v>108</v>
       </c>
       <c r="L93" s="12" t="s">
-        <v>256</v>
+        <v>240</v>
       </c>
       <c r="M93" s="12">
         <v>20.55</v>
@@ -6690,11 +6681,11 @@
       <c r="O93" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="P93" s="12">
-        <v>0.87</v>
-      </c>
-      <c r="Q93" s="12">
-        <v>0.78</v>
+      <c r="P93" s="53">
+        <v>0.84</v>
+      </c>
+      <c r="Q93" s="53">
+        <v>1.59</v>
       </c>
       <c r="R93" s="14">
         <v>100</v>
@@ -6711,7 +6702,7 @@
         <v>2035</v>
       </c>
       <c r="B94" s="12" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="C94" s="12" t="s">
         <v>17</v>
@@ -6720,7 +6711,7 @@
         <v>243</v>
       </c>
       <c r="F94" s="12" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="G94" s="12" t="s">
         <v>211</v>
@@ -6728,14 +6719,14 @@
       <c r="H94" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="J94" s="53" t="s">
-        <v>263</v>
+      <c r="J94" s="12" t="s">
+        <v>103</v>
       </c>
       <c r="K94" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L94" s="12" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="M94" s="12">
         <v>20.55</v>
@@ -6767,7 +6758,7 @@
         <v>2035</v>
       </c>
       <c r="B95" s="12" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="C95" s="12" t="s">
         <v>17</v>
@@ -6776,7 +6767,7 @@
         <v>243</v>
       </c>
       <c r="F95" s="12" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="G95" s="12" t="s">
         <v>211</v>
@@ -6784,14 +6775,14 @@
       <c r="H95" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="J95" s="12" t="s">
-        <v>103</v>
+      <c r="J95" s="53" t="s">
+        <v>263</v>
       </c>
       <c r="K95" s="13" t="s">
-        <v>129</v>
+        <v>42</v>
       </c>
       <c r="L95" s="12" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="M95" s="12">
         <v>20.55</v>
@@ -6823,7 +6814,7 @@
         <v>2035</v>
       </c>
       <c r="B96" s="12" t="s">
-        <v>274</v>
+        <v>258</v>
       </c>
       <c r="C96" s="12" t="s">
         <v>17</v>
@@ -6832,7 +6823,7 @@
         <v>243</v>
       </c>
       <c r="F96" s="12" t="s">
-        <v>275</v>
+        <v>259</v>
       </c>
       <c r="G96" s="12" t="s">
         <v>211</v>
@@ -6844,13 +6835,13 @@
         <v>103</v>
       </c>
       <c r="K96" s="13" t="s">
-        <v>43</v>
+        <v>129</v>
       </c>
       <c r="L96" s="12" t="s">
-        <v>276</v>
-      </c>
-      <c r="M96" s="53">
-        <v>13.68</v>
+        <v>260</v>
+      </c>
+      <c r="M96" s="12">
+        <v>20.55</v>
       </c>
       <c r="N96" s="47" t="s">
         <v>109</v>
@@ -6879,7 +6870,7 @@
         <v>2035</v>
       </c>
       <c r="B97" s="12" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="C97" s="12" t="s">
         <v>17</v>
@@ -6888,7 +6879,7 @@
         <v>243</v>
       </c>
       <c r="F97" s="12" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="G97" s="12" t="s">
         <v>211</v>
@@ -6903,10 +6894,10 @@
         <v>43</v>
       </c>
       <c r="L97" s="12" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="M97" s="53">
-        <v>14.55</v>
+        <v>13.68</v>
       </c>
       <c r="N97" s="47" t="s">
         <v>109</v>
@@ -6935,7 +6926,7 @@
         <v>2035</v>
       </c>
       <c r="B98" s="12" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C98" s="12" t="s">
         <v>17</v>
@@ -6944,7 +6935,7 @@
         <v>243</v>
       </c>
       <c r="F98" s="12" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="G98" s="12" t="s">
         <v>211</v>
@@ -6952,9 +6943,6 @@
       <c r="H98" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="I98" s="12" t="s">
-        <v>11</v>
-      </c>
       <c r="J98" s="12" t="s">
         <v>103</v>
       </c>
@@ -6962,10 +6950,10 @@
         <v>43</v>
       </c>
       <c r="L98" s="12" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="M98" s="53">
-        <v>17.579999999999998</v>
+        <v>14.55</v>
       </c>
       <c r="N98" s="47" t="s">
         <v>109</v>
@@ -6987,9 +6975,6 @@
       </c>
       <c r="T98" s="14">
         <v>75</v>
-      </c>
-      <c r="U98" s="12" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="99" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -6997,7 +6982,7 @@
         <v>2035</v>
       </c>
       <c r="B99" s="12" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C99" s="12" t="s">
         <v>17</v>
@@ -7006,7 +6991,7 @@
         <v>243</v>
       </c>
       <c r="F99" s="12" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="G99" s="12" t="s">
         <v>211</v>
@@ -7014,17 +6999,20 @@
       <c r="H99" s="12" t="s">
         <v>116</v>
       </c>
+      <c r="I99" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="J99" s="12" t="s">
         <v>103</v>
       </c>
       <c r="K99" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L99" s="12" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="M99" s="53">
-        <v>15.06</v>
+        <v>17.579999999999998</v>
       </c>
       <c r="N99" s="47" t="s">
         <v>109</v>
@@ -7047,80 +7035,139 @@
       <c r="T99" s="14">
         <v>75</v>
       </c>
-    </row>
-    <row r="100" spans="1:21" s="24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="24">
+      <c r="U99" s="12" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="100" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B100" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="C100" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D100" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="F100" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="G100" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="H100" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="J100" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="K100" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="L100" s="12" t="s">
+        <v>288</v>
+      </c>
+      <c r="M100" s="53">
+        <v>15.06</v>
+      </c>
+      <c r="N100" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="O100" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="P100" s="12">
+        <v>0.87</v>
+      </c>
+      <c r="Q100" s="12">
+        <v>0.78</v>
+      </c>
+      <c r="R100" s="14">
+        <v>100</v>
+      </c>
+      <c r="S100" s="14">
+        <v>0</v>
+      </c>
+      <c r="T100" s="14">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="101" spans="1:21" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="24">
         <v>2050</v>
       </c>
-      <c r="B100" s="24" t="s">
+      <c r="B101" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="C100" s="24" t="s">
+      <c r="C101" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="D100" s="24" t="s">
+      <c r="D101" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="F100" s="24" t="s">
+      <c r="F101" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="G100" s="24" t="s">
+      <c r="G101" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="H100" s="25" t="s">
+      <c r="H101" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="J100" s="24" t="s">
+      <c r="J101" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="K100" s="26" t="s">
+      <c r="K101" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="L100" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="M100" s="24">
+      <c r="L101" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="M101" s="24">
         <v>17.440000000000001</v>
       </c>
-      <c r="N100" s="48">
+      <c r="N101" s="48">
         <v>-0.33</v>
       </c>
-      <c r="O100" s="48">
-        <v>0</v>
-      </c>
-      <c r="P100" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q100" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="R100" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="S100" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="T100" s="27" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="102" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="M102" s="1">
-        <f>M96*2</f>
-        <v>27.36</v>
-      </c>
-      <c r="N102" s="44">
-        <f>M95*2</f>
-        <v>41.1</v>
+      <c r="O101" s="48">
+        <v>0</v>
+      </c>
+      <c r="P101" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q101" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="R101" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="S101" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="T101" s="27" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="103" spans="1:21" x14ac:dyDescent="0.3">
       <c r="M103" s="1">
+        <f>M97*2</f>
+        <v>27.36</v>
+      </c>
+      <c r="N103" s="44">
+        <f>M96*2</f>
+        <v>41.1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="M104" s="1">
+        <f>M97*3</f>
+        <v>41.04</v>
+      </c>
+      <c r="N104" s="44">
         <f>M96*3</f>
-        <v>41.04</v>
-      </c>
-      <c r="N103" s="44">
-        <f>M95*3</f>
         <v>61.650000000000006</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Draft Blueprint v01 runs
[NoProject, Plan] x [2035,2050]
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one-master\utilities\RTP\config_RTP2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21AB7249-C4EE-43EA-8845-CA1E8F35EA8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4AC3160-7C91-4DF2-B491-37EFC2872B87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
+    <workbookView xWindow="2055" yWindow="690" windowWidth="27345" windowHeight="20055" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelRuns" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1142" uniqueCount="366">
   <si>
     <t>year</t>
   </si>
@@ -1077,6 +1077,81 @@
   </si>
   <si>
     <t>2023 v55</t>
+  </si>
+  <si>
+    <t>2035_TM160_DBP_NoProject_01</t>
+  </si>
+  <si>
+    <t>RTP2025</t>
+  </si>
+  <si>
+    <t>DBP</t>
+  </si>
+  <si>
+    <t>Initial 2035 NoProject Run</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1206676779097787/f</t>
+  </si>
+  <si>
+    <t>M:\urban_modeling\baus\PBA50Plus\PBA50Plus_NP_InitialRun\outputs\PBA50Plus_NP_InitialRun_v8</t>
+  </si>
+  <si>
+    <t>PBA50Plus_NP_InitialRun_v8</t>
+  </si>
+  <si>
+    <t>BlueprintNetworks_v16\net_2030_Baseline</t>
+  </si>
+  <si>
+    <t>2035 NoProject</t>
+  </si>
+  <si>
+    <t>2035_TM160_DBP_Plan_01</t>
+  </si>
+  <si>
+    <t>Initial 2035 Plan Run</t>
+  </si>
+  <si>
+    <t>M:\urban_modeling\baus\PBA50Plus\PBA50Plus_Preservation</t>
+  </si>
+  <si>
+    <t>PBA50Plus_Preservation</t>
+  </si>
+  <si>
+    <t>BlueprintNetworks_v16\net_2035_Blueprint</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1206676779097785/f</t>
+  </si>
+  <si>
+    <t>2050_TM160_DBP_NoProject_01</t>
+  </si>
+  <si>
+    <t>2050_TM160_DBP_Plan_01</t>
+  </si>
+  <si>
+    <t>Initial 2050 NoProject Run</t>
+  </si>
+  <si>
+    <t>Initial 2050 Plan Run</t>
+  </si>
+  <si>
+    <t>BlueprintNetworks_v16\net_2050_Blueprint</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1206676779097791/f</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1206676779097789/f</t>
+  </si>
+  <si>
+    <t>2050 NoProject</t>
+  </si>
+  <si>
+    <t>2050 Plan</t>
+  </si>
+  <si>
+    <t>2035 Plan</t>
   </si>
 </sst>
 </file>
@@ -1086,7 +1161,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1127,8 +1202,19 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1201,6 +1287,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -1232,7 +1336,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1288,7 +1392,6 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1357,6 +1460,44 @@
     </xf>
     <xf numFmtId="2" fontId="4" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1381,9 +1522,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1421,7 +1562,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1527,7 +1668,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1669,7 +1810,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1685,35 +1826,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9564CC59-3725-4FDA-8BF2-0F68CB1B6F5A}">
-  <dimension ref="A1:U104"/>
+  <dimension ref="A1:U108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C50" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C53" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A74" sqref="A74"/>
+      <selection pane="bottomRight" activeCell="U103" sqref="U103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.81640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.54296875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="42.26953125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="42.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="23" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.26953125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.26953125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="11.26953125" style="10" customWidth="1"/>
-    <col min="12" max="12" width="17.54296875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="8.26953125" style="1" customWidth="1"/>
-    <col min="14" max="15" width="9.26953125" style="44"/>
-    <col min="16" max="16384" width="9.26953125" style="1"/>
+    <col min="8" max="8" width="8.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" style="10" customWidth="1"/>
+    <col min="12" max="12" width="17.5703125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="8.28515625" style="1" customWidth="1"/>
+    <col min="14" max="15" width="9.28515625" style="43"/>
+    <col min="16" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="5" customFormat="1" ht="39" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1753,10 +1894,10 @@
       <c r="M1" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="N1" s="39" t="s">
+      <c r="N1" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="O1" s="39" t="s">
+      <c r="O1" s="38" t="s">
         <v>38</v>
       </c>
       <c r="P1" s="4" t="s">
@@ -1778,7 +1919,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="19">
         <v>2005</v>
       </c>
@@ -1809,10 +1950,10 @@
       <c r="M2" s="21">
         <v>14.87</v>
       </c>
-      <c r="N2" s="40" t="s">
-        <v>109</v>
-      </c>
-      <c r="O2" s="40" t="s">
+      <c r="N2" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="O2" s="39" t="s">
         <v>109</v>
       </c>
       <c r="P2" s="23">
@@ -1831,649 +1972,649 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="32" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="31">
+    <row r="3" spans="1:21" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="30">
         <v>2005</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="C3" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="32" t="s">
+      <c r="C3" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="31" t="s">
         <v>247</v>
       </c>
-      <c r="F3" s="32" t="s">
+      <c r="F3" s="31" t="s">
         <v>150</v>
       </c>
-      <c r="G3" s="32" t="s">
+      <c r="G3" s="31" t="s">
         <v>277</v>
       </c>
-      <c r="H3" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="32" t="s">
+      <c r="H3" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="31" t="s">
         <v>224</v>
       </c>
-      <c r="K3" s="33" t="s">
+      <c r="K3" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="L3" s="32" t="s">
+      <c r="L3" s="31" t="s">
         <v>151</v>
       </c>
-      <c r="M3" s="32">
+      <c r="M3" s="31">
         <v>14.87</v>
       </c>
-      <c r="N3" s="41" t="s">
-        <v>109</v>
-      </c>
-      <c r="O3" s="41" t="s">
-        <v>109</v>
-      </c>
-      <c r="P3" s="34">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="34">
-        <v>0</v>
-      </c>
-      <c r="R3" s="34">
-        <v>0</v>
-      </c>
-      <c r="S3" s="34">
-        <v>0</v>
-      </c>
-      <c r="T3" s="34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" s="32" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="31">
+      <c r="N3" s="40" t="s">
+        <v>109</v>
+      </c>
+      <c r="O3" s="40" t="s">
+        <v>109</v>
+      </c>
+      <c r="P3" s="33">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="33">
+        <v>0</v>
+      </c>
+      <c r="R3" s="33">
+        <v>0</v>
+      </c>
+      <c r="S3" s="33">
+        <v>0</v>
+      </c>
+      <c r="T3" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="30">
         <v>2005</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="31" t="s">
         <v>222</v>
       </c>
-      <c r="C4" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="32" t="s">
+      <c r="C4" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="31" t="s">
         <v>247</v>
       </c>
-      <c r="F4" s="32" t="s">
+      <c r="F4" s="31" t="s">
         <v>223</v>
       </c>
-      <c r="G4" s="32" t="s">
+      <c r="G4" s="31" t="s">
         <v>267</v>
       </c>
-      <c r="H4" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="32" t="s">
+      <c r="H4" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="32" t="s">
+      <c r="J4" s="31" t="s">
         <v>224</v>
       </c>
-      <c r="K4" s="33" t="s">
+      <c r="K4" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="L4" s="32" t="s">
+      <c r="L4" s="31" t="s">
         <v>225</v>
       </c>
-      <c r="M4" s="32">
+      <c r="M4" s="31">
         <v>14.87</v>
       </c>
-      <c r="N4" s="41" t="s">
-        <v>109</v>
-      </c>
-      <c r="O4" s="41" t="s">
-        <v>109</v>
-      </c>
-      <c r="P4" s="34"/>
-      <c r="Q4" s="34"/>
-      <c r="R4" s="34">
-        <v>0</v>
-      </c>
-      <c r="S4" s="34">
-        <v>0</v>
-      </c>
-      <c r="T4" s="34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" s="32" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="31">
+      <c r="N4" s="40" t="s">
+        <v>109</v>
+      </c>
+      <c r="O4" s="40" t="s">
+        <v>109</v>
+      </c>
+      <c r="P4" s="33"/>
+      <c r="Q4" s="33"/>
+      <c r="R4" s="33">
+        <v>0</v>
+      </c>
+      <c r="S4" s="33">
+        <v>0</v>
+      </c>
+      <c r="T4" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="30">
         <v>2005</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="31" t="s">
         <v>265</v>
       </c>
-      <c r="C5" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="32" t="s">
+      <c r="C5" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="31" t="s">
         <v>247</v>
       </c>
-      <c r="F5" s="32" t="s">
+      <c r="F5" s="31" t="s">
         <v>266</v>
       </c>
-      <c r="G5" s="32" t="s">
+      <c r="G5" s="31" t="s">
         <v>267</v>
       </c>
-      <c r="H5" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="32" t="s">
+      <c r="H5" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="32" t="s">
+      <c r="J5" s="31" t="s">
         <v>224</v>
       </c>
-      <c r="K5" s="33" t="s">
+      <c r="K5" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="L5" s="32" t="s">
+      <c r="L5" s="31" t="s">
         <v>268</v>
       </c>
-      <c r="M5" s="32">
+      <c r="M5" s="31">
         <v>14.87</v>
       </c>
-      <c r="N5" s="41" t="s">
-        <v>109</v>
-      </c>
-      <c r="O5" s="41" t="s">
-        <v>109</v>
-      </c>
-      <c r="P5" s="34"/>
-      <c r="Q5" s="34"/>
-      <c r="R5" s="34">
-        <v>0</v>
-      </c>
-      <c r="S5" s="34">
-        <v>0</v>
-      </c>
-      <c r="T5" s="34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" s="55" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="54">
+      <c r="N5" s="40" t="s">
+        <v>109</v>
+      </c>
+      <c r="O5" s="40" t="s">
+        <v>109</v>
+      </c>
+      <c r="P5" s="33"/>
+      <c r="Q5" s="33"/>
+      <c r="R5" s="33">
+        <v>0</v>
+      </c>
+      <c r="S5" s="33">
+        <v>0</v>
+      </c>
+      <c r="T5" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="53">
         <v>2015</v>
       </c>
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="54" t="s">
         <v>278</v>
       </c>
-      <c r="C6" s="55" t="s">
+      <c r="C6" s="54" t="s">
         <v>113</v>
       </c>
-      <c r="D6" s="55" t="s">
+      <c r="D6" s="54" t="s">
         <v>246</v>
       </c>
-      <c r="F6" s="55" t="s">
+      <c r="F6" s="54" t="s">
         <v>279</v>
       </c>
-      <c r="G6" s="55" t="s">
+      <c r="G6" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="55" t="s">
-        <v>10</v>
-      </c>
-      <c r="K6" s="56"/>
-      <c r="M6" s="55">
+      <c r="H6" s="54" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="55"/>
+      <c r="M6" s="54">
         <v>13.73</v>
       </c>
-      <c r="N6" s="57">
+      <c r="N6" s="56">
         <v>-0.09</v>
       </c>
-      <c r="O6" s="57">
+      <c r="O6" s="56">
         <v>0.9</v>
       </c>
-      <c r="P6" s="58"/>
-      <c r="Q6" s="58"/>
-      <c r="R6" s="58">
-        <v>0</v>
-      </c>
-      <c r="S6" s="58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="35">
+      <c r="P6" s="57"/>
+      <c r="Q6" s="57"/>
+      <c r="R6" s="57">
+        <v>0</v>
+      </c>
+      <c r="S6" s="57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="34">
         <v>2015</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="36" t="s">
+      <c r="C7" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="35" t="s">
         <v>246</v>
       </c>
-      <c r="F7" s="36" t="s">
+      <c r="F7" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="36" t="s">
+      <c r="G7" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="J7" s="36" t="s">
+      <c r="H7" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="37" t="s">
+      <c r="K7" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="L7" s="36" t="s">
+      <c r="L7" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="N7" s="42">
+      <c r="N7" s="41">
         <v>-0.09</v>
       </c>
-      <c r="O7" s="42">
+      <c r="O7" s="41">
         <v>0.9</v>
       </c>
-      <c r="P7" s="38"/>
-      <c r="Q7" s="38"/>
-      <c r="R7" s="38">
-        <v>0</v>
-      </c>
-      <c r="S7" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="35">
+      <c r="P7" s="37"/>
+      <c r="Q7" s="37"/>
+      <c r="R7" s="37">
+        <v>0</v>
+      </c>
+      <c r="S7" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="34">
         <v>2015</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="35" t="s">
         <v>145</v>
       </c>
-      <c r="C8" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="36" t="s">
+      <c r="C8" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="35" t="s">
         <v>246</v>
       </c>
-      <c r="F8" s="36" t="s">
+      <c r="F8" s="35" t="s">
         <v>149</v>
       </c>
-      <c r="G8" s="36" t="s">
+      <c r="G8" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="J8" s="36" t="s">
+      <c r="H8" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="35" t="s">
         <v>146</v>
       </c>
-      <c r="K8" s="37" t="s">
+      <c r="K8" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="L8" s="36" t="s">
+      <c r="L8" s="35" t="s">
         <v>147</v>
       </c>
-      <c r="N8" s="42" t="s">
-        <v>109</v>
-      </c>
-      <c r="O8" s="42" t="s">
-        <v>109</v>
-      </c>
-      <c r="P8" s="38">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="38">
-        <v>0</v>
-      </c>
-      <c r="R8" s="38">
-        <v>0</v>
-      </c>
-      <c r="S8" s="38">
-        <v>0</v>
-      </c>
-      <c r="T8" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="35">
+      <c r="N8" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="O8" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="P8" s="37">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="37">
+        <v>0</v>
+      </c>
+      <c r="R8" s="37">
+        <v>0</v>
+      </c>
+      <c r="S8" s="37">
+        <v>0</v>
+      </c>
+      <c r="T8" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="34">
         <v>2015</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="35" t="s">
         <v>154</v>
       </c>
-      <c r="C9" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="36" t="s">
+      <c r="C9" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="35" t="s">
         <v>246</v>
       </c>
-      <c r="F9" s="36" t="s">
+      <c r="F9" s="35" t="s">
         <v>153</v>
       </c>
-      <c r="G9" s="36" t="s">
+      <c r="G9" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="J9" s="36" t="s">
+      <c r="H9" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="35" t="s">
         <v>146</v>
       </c>
-      <c r="K9" s="37" t="s">
+      <c r="K9" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="L9" s="36" t="s">
+      <c r="L9" s="35" t="s">
         <v>147</v>
       </c>
-      <c r="N9" s="42" t="s">
-        <v>109</v>
-      </c>
-      <c r="O9" s="42" t="s">
-        <v>109</v>
-      </c>
-      <c r="P9" s="38">
+      <c r="N9" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="O9" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="P9" s="37">
         <v>0.32</v>
       </c>
-      <c r="Q9" s="38">
+      <c r="Q9" s="37">
         <v>0.28000000000000003</v>
       </c>
-      <c r="R9" s="38">
-        <v>0</v>
-      </c>
-      <c r="S9" s="38">
-        <v>0</v>
-      </c>
-      <c r="T9" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="35">
+      <c r="R9" s="37">
+        <v>0</v>
+      </c>
+      <c r="S9" s="37">
+        <v>0</v>
+      </c>
+      <c r="T9" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="34">
         <v>2015</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="35" t="s">
         <v>155</v>
       </c>
-      <c r="C10" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="36" t="s">
+      <c r="C10" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="35" t="s">
         <v>246</v>
       </c>
-      <c r="F10" s="36" t="s">
+      <c r="F10" s="35" t="s">
         <v>153</v>
       </c>
-      <c r="G10" s="36" t="s">
+      <c r="G10" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="J10" s="36" t="s">
+      <c r="H10" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="35" t="s">
         <v>146</v>
       </c>
-      <c r="K10" s="37" t="s">
+      <c r="K10" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="L10" s="36" t="s">
+      <c r="L10" s="35" t="s">
         <v>147</v>
       </c>
-      <c r="N10" s="42" t="s">
-        <v>109</v>
-      </c>
-      <c r="O10" s="42" t="s">
-        <v>109</v>
-      </c>
-      <c r="P10" s="38">
+      <c r="N10" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="O10" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="P10" s="37">
         <v>0.32</v>
       </c>
-      <c r="Q10" s="38">
+      <c r="Q10" s="37">
         <v>0.28000000000000003</v>
       </c>
-      <c r="R10" s="38">
-        <v>0</v>
-      </c>
-      <c r="S10" s="38">
-        <v>0</v>
-      </c>
-      <c r="T10" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="35">
+      <c r="R10" s="37">
+        <v>0</v>
+      </c>
+      <c r="S10" s="37">
+        <v>0</v>
+      </c>
+      <c r="T10" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="34">
         <v>2015</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="35" t="s">
         <v>156</v>
       </c>
-      <c r="C11" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="36" t="s">
+      <c r="C11" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="35" t="s">
         <v>246</v>
       </c>
-      <c r="F11" s="36" t="s">
+      <c r="F11" s="35" t="s">
         <v>157</v>
       </c>
-      <c r="G11" s="36" t="s">
+      <c r="G11" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="H11" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="J11" s="36" t="s">
+      <c r="H11" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="35" t="s">
         <v>146</v>
       </c>
-      <c r="K11" s="37" t="s">
+      <c r="K11" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="L11" s="36" t="s">
+      <c r="L11" s="35" t="s">
         <v>158</v>
       </c>
-      <c r="M11" s="51">
+      <c r="M11" s="50">
         <v>15.1</v>
       </c>
-      <c r="N11" s="42" t="s">
-        <v>109</v>
-      </c>
-      <c r="O11" s="42" t="s">
-        <v>109</v>
-      </c>
-      <c r="P11" s="38">
+      <c r="N11" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="O11" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="P11" s="37">
         <v>0.32300000000000001</v>
       </c>
-      <c r="Q11" s="49">
+      <c r="Q11" s="48">
         <v>0.83099999999999996</v>
       </c>
-      <c r="R11" s="38">
-        <v>0</v>
-      </c>
-      <c r="S11" s="38">
-        <v>0</v>
-      </c>
-      <c r="T11" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="35">
+      <c r="R11" s="37">
+        <v>0</v>
+      </c>
+      <c r="S11" s="37">
+        <v>0</v>
+      </c>
+      <c r="T11" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="34">
         <v>2015</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="35" t="s">
         <v>213</v>
       </c>
-      <c r="C12" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="36" t="s">
+      <c r="C12" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="35" t="s">
         <v>246</v>
       </c>
-      <c r="F12" s="36" t="s">
+      <c r="F12" s="35" t="s">
         <v>215</v>
       </c>
-      <c r="G12" s="36" t="s">
+      <c r="G12" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="J12" s="36" t="s">
+      <c r="H12" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="J12" s="35" t="s">
         <v>146</v>
       </c>
-      <c r="K12" s="37" t="s">
+      <c r="K12" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="L12" s="36" t="s">
+      <c r="L12" s="35" t="s">
         <v>214</v>
       </c>
-      <c r="M12" s="36">
+      <c r="M12" s="35">
         <v>13.73</v>
       </c>
-      <c r="N12" s="42" t="s">
-        <v>109</v>
-      </c>
-      <c r="O12" s="42" t="s">
-        <v>109</v>
-      </c>
-      <c r="P12" s="38">
+      <c r="N12" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="O12" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="P12" s="37">
         <v>0.32300000000000001</v>
       </c>
-      <c r="Q12" s="49">
+      <c r="Q12" s="48">
         <v>0.83099999999999996</v>
       </c>
-      <c r="R12" s="38">
-        <v>0</v>
-      </c>
-      <c r="S12" s="38">
-        <v>0</v>
-      </c>
-      <c r="T12" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="35">
+      <c r="R12" s="37">
+        <v>0</v>
+      </c>
+      <c r="S12" s="37">
+        <v>0</v>
+      </c>
+      <c r="T12" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="34">
         <v>2015</v>
       </c>
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="35" t="s">
         <v>314</v>
       </c>
-      <c r="C13" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="36" t="s">
+      <c r="C13" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="35" t="s">
         <v>246</v>
       </c>
-      <c r="F13" s="36" t="s">
+      <c r="F13" s="35" t="s">
         <v>316</v>
       </c>
-      <c r="G13" s="36" t="s">
+      <c r="G13" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="J13" s="36" t="s">
+      <c r="H13" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13" s="35" t="s">
         <v>146</v>
       </c>
-      <c r="K13" s="37" t="s">
+      <c r="K13" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="L13" s="36" t="s">
+      <c r="L13" s="35" t="s">
         <v>317</v>
       </c>
-      <c r="M13" s="36">
+      <c r="M13" s="35">
         <v>13.73</v>
       </c>
-      <c r="N13" s="42" t="s">
-        <v>109</v>
-      </c>
-      <c r="O13" s="42" t="s">
-        <v>109</v>
-      </c>
-      <c r="P13" s="38">
+      <c r="N13" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="O13" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="P13" s="37">
         <v>0.32300000000000001</v>
       </c>
-      <c r="Q13" s="49">
+      <c r="Q13" s="48">
         <v>0.83099999999999996</v>
       </c>
-      <c r="R13" s="38">
-        <v>0</v>
-      </c>
-      <c r="S13" s="38">
-        <v>0</v>
-      </c>
-      <c r="T13" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="35">
+      <c r="R13" s="37">
+        <v>0</v>
+      </c>
+      <c r="S13" s="37">
+        <v>0</v>
+      </c>
+      <c r="T13" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="34">
         <v>2015</v>
       </c>
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="35" t="s">
         <v>315</v>
       </c>
-      <c r="C14" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="36" t="s">
+      <c r="C14" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="35" t="s">
         <v>246</v>
       </c>
-      <c r="F14" s="36" t="s">
+      <c r="F14" s="35" t="s">
         <v>318</v>
       </c>
-      <c r="G14" s="36" t="s">
+      <c r="G14" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="H14" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="I14" s="36" t="s">
+      <c r="H14" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="J14" s="36" t="s">
+      <c r="J14" s="35" t="s">
         <v>146</v>
       </c>
-      <c r="K14" s="37" t="s">
+      <c r="K14" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="L14" s="36" t="s">
+      <c r="L14" s="35" t="s">
         <v>317</v>
       </c>
-      <c r="M14" s="36">
+      <c r="M14" s="35">
         <v>13.73</v>
       </c>
-      <c r="N14" s="42" t="s">
-        <v>109</v>
-      </c>
-      <c r="O14" s="42" t="s">
-        <v>109</v>
-      </c>
-      <c r="P14" s="38">
+      <c r="N14" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="O14" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="P14" s="37">
         <v>0.32300000000000001</v>
       </c>
-      <c r="Q14" s="49">
+      <c r="Q14" s="48">
         <v>0.83099999999999996</v>
       </c>
-      <c r="R14" s="38">
-        <v>0</v>
-      </c>
-      <c r="S14" s="38">
-        <v>0</v>
-      </c>
-      <c r="T14" s="38">
-        <v>0</v>
-      </c>
-      <c r="U14" s="59" t="s">
+      <c r="R14" s="37">
+        <v>0</v>
+      </c>
+      <c r="S14" s="37">
+        <v>0</v>
+      </c>
+      <c r="T14" s="37">
+        <v>0</v>
+      </c>
+      <c r="U14" s="58" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>2023</v>
       </c>
@@ -2504,10 +2645,10 @@
       <c r="L15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="N15" s="43">
+      <c r="N15" s="42">
         <v>-0.44</v>
       </c>
-      <c r="O15" s="43">
+      <c r="O15" s="42">
         <v>-0.23</v>
       </c>
       <c r="P15" s="6"/>
@@ -2519,7 +2660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>2023</v>
       </c>
@@ -2550,10 +2691,10 @@
       <c r="L16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="N16" s="43">
+      <c r="N16" s="42">
         <v>-1.25</v>
       </c>
-      <c r="O16" s="43">
+      <c r="O16" s="42">
         <v>-0.75</v>
       </c>
       <c r="P16" s="6"/>
@@ -2565,7 +2706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>2023</v>
       </c>
@@ -2596,10 +2737,10 @@
       <c r="L17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N17" s="43">
+      <c r="N17" s="42">
         <v>-1.25</v>
       </c>
-      <c r="O17" s="43">
+      <c r="O17" s="42">
         <v>-0.75</v>
       </c>
       <c r="P17" s="6"/>
@@ -2611,7 +2752,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>2023</v>
       </c>
@@ -2642,10 +2783,10 @@
       <c r="L18" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="N18" s="43">
+      <c r="N18" s="42">
         <v>-1.25</v>
       </c>
-      <c r="O18" s="43">
+      <c r="O18" s="42">
         <v>-0.75</v>
       </c>
       <c r="P18" s="6"/>
@@ -2657,7 +2798,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>2023</v>
       </c>
@@ -2688,10 +2829,10 @@
       <c r="L19" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N19" s="43">
+      <c r="N19" s="42">
         <v>-1.25</v>
       </c>
-      <c r="O19" s="43">
+      <c r="O19" s="42">
         <v>-0.75</v>
       </c>
       <c r="P19" s="6"/>
@@ -2703,7 +2844,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>2023</v>
       </c>
@@ -2734,10 +2875,10 @@
       <c r="L20" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N20" s="43">
+      <c r="N20" s="42">
         <v>-1.25</v>
       </c>
-      <c r="O20" s="43">
+      <c r="O20" s="42">
         <v>-0.75</v>
       </c>
       <c r="P20" s="6"/>
@@ -2749,7 +2890,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>2023</v>
       </c>
@@ -2780,10 +2921,10 @@
       <c r="L21" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N21" s="43">
+      <c r="N21" s="42">
         <v>-1.25</v>
       </c>
-      <c r="O21" s="43">
+      <c r="O21" s="42">
         <v>-0.75</v>
       </c>
       <c r="P21" s="6"/>
@@ -2795,7 +2936,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>2023</v>
       </c>
@@ -2826,10 +2967,10 @@
       <c r="L22" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N22" s="43">
+      <c r="N22" s="42">
         <v>-1.25</v>
       </c>
-      <c r="O22" s="43">
+      <c r="O22" s="42">
         <v>-0.75</v>
       </c>
       <c r="P22" s="6"/>
@@ -2841,7 +2982,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>2023</v>
       </c>
@@ -2872,10 +3013,10 @@
       <c r="L23" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="N23" s="43">
+      <c r="N23" s="42">
         <v>-1.25</v>
       </c>
-      <c r="O23" s="43">
+      <c r="O23" s="42">
         <v>-0.75</v>
       </c>
       <c r="P23" s="6"/>
@@ -2887,7 +3028,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>2023</v>
       </c>
@@ -2918,10 +3059,10 @@
       <c r="L24" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="N24" s="43">
+      <c r="N24" s="42">
         <v>-1.25</v>
       </c>
-      <c r="O24" s="43">
+      <c r="O24" s="42">
         <v>-0.75</v>
       </c>
       <c r="P24" s="6"/>
@@ -2933,7 +3074,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>2023</v>
       </c>
@@ -2964,10 +3105,10 @@
       <c r="L25" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="N25" s="43">
+      <c r="N25" s="42">
         <v>-1.25</v>
       </c>
-      <c r="O25" s="43">
+      <c r="O25" s="42">
         <v>-0.75</v>
       </c>
       <c r="P25" s="6"/>
@@ -2979,7 +3120,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>2023</v>
       </c>
@@ -3010,10 +3151,10 @@
       <c r="L26" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="N26" s="43">
+      <c r="N26" s="42">
         <v>-1.25</v>
       </c>
-      <c r="O26" s="43">
+      <c r="O26" s="42">
         <v>-0.75</v>
       </c>
       <c r="P26" s="6"/>
@@ -3025,7 +3166,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>2023</v>
       </c>
@@ -3056,10 +3197,10 @@
       <c r="L27" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="N27" s="43">
+      <c r="N27" s="42">
         <v>-1.25</v>
       </c>
-      <c r="O27" s="43">
+      <c r="O27" s="42">
         <v>-0.75</v>
       </c>
       <c r="P27" s="6"/>
@@ -3071,7 +3212,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>2023</v>
       </c>
@@ -3102,10 +3243,10 @@
       <c r="L28" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="N28" s="43">
+      <c r="N28" s="42">
         <v>-1.25</v>
       </c>
-      <c r="O28" s="43">
+      <c r="O28" s="42">
         <v>-0.75</v>
       </c>
       <c r="P28" s="6"/>
@@ -3117,7 +3258,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>2023</v>
       </c>
@@ -3148,10 +3289,10 @@
       <c r="L29" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="N29" s="43">
+      <c r="N29" s="42">
         <v>-1.25</v>
       </c>
-      <c r="O29" s="43">
+      <c r="O29" s="42">
         <v>-0.75</v>
       </c>
       <c r="P29" s="6"/>
@@ -3163,7 +3304,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>2023</v>
       </c>
@@ -3194,10 +3335,10 @@
       <c r="L30" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="N30" s="43">
+      <c r="N30" s="42">
         <v>-1.25</v>
       </c>
-      <c r="O30" s="43">
+      <c r="O30" s="42">
         <v>-0.75</v>
       </c>
       <c r="P30" s="6"/>
@@ -3209,7 +3350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>2023</v>
       </c>
@@ -3240,10 +3381,10 @@
       <c r="L31" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="N31" s="43">
+      <c r="N31" s="42">
         <v>-1.25</v>
       </c>
-      <c r="O31" s="43">
+      <c r="O31" s="42">
         <v>-0.75</v>
       </c>
       <c r="P31" s="6"/>
@@ -3255,7 +3396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>2023</v>
       </c>
@@ -3286,10 +3427,10 @@
       <c r="L32" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="N32" s="43">
+      <c r="N32" s="42">
         <v>-1.25</v>
       </c>
-      <c r="O32" s="43">
+      <c r="O32" s="42">
         <v>-0.75</v>
       </c>
       <c r="P32" s="6"/>
@@ -3301,7 +3442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>2023</v>
       </c>
@@ -3345,7 +3486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>2023</v>
       </c>
@@ -3376,10 +3517,10 @@
       <c r="L34" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="N34" s="43">
+      <c r="N34" s="42">
         <v>-1.25</v>
       </c>
-      <c r="O34" s="43">
+      <c r="O34" s="42">
         <v>-0.75</v>
       </c>
       <c r="P34" s="6"/>
@@ -3394,7 +3535,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>2023</v>
       </c>
@@ -3441,7 +3582,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>2023</v>
       </c>
@@ -3472,10 +3613,10 @@
       <c r="L36" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="N36" s="43">
+      <c r="N36" s="42">
         <v>-1.25</v>
       </c>
-      <c r="O36" s="43">
+      <c r="O36" s="42">
         <v>-0.75</v>
       </c>
       <c r="R36" s="7">
@@ -3488,7 +3629,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>2023</v>
       </c>
@@ -3522,10 +3663,10 @@
       <c r="M37" s="1">
         <v>17.77</v>
       </c>
-      <c r="N37" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O37" s="44" t="s">
+      <c r="N37" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="O37" s="43" t="s">
         <v>109</v>
       </c>
       <c r="P37" s="6">
@@ -3544,7 +3685,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>2023</v>
       </c>
@@ -3578,10 +3719,10 @@
       <c r="M38" s="1">
         <v>17.77</v>
       </c>
-      <c r="N38" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O38" s="44" t="s">
+      <c r="N38" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="O38" s="43" t="s">
         <v>109</v>
       </c>
       <c r="P38" s="1">
@@ -3600,7 +3741,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>2023</v>
       </c>
@@ -3634,10 +3775,10 @@
       <c r="M39" s="1">
         <v>17.77</v>
       </c>
-      <c r="N39" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O39" s="44" t="s">
+      <c r="N39" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="O39" s="43" t="s">
         <v>109</v>
       </c>
       <c r="P39" s="1">
@@ -3656,7 +3797,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>2023</v>
       </c>
@@ -3690,10 +3831,10 @@
       <c r="M40" s="1">
         <v>17.77</v>
       </c>
-      <c r="N40" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O40" s="44" t="s">
+      <c r="N40" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="O40" s="43" t="s">
         <v>109</v>
       </c>
       <c r="P40" s="1">
@@ -3712,7 +3853,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>2023</v>
       </c>
@@ -3746,10 +3887,10 @@
       <c r="M41" s="1">
         <v>17.77</v>
       </c>
-      <c r="N41" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O41" s="44" t="s">
+      <c r="N41" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="O41" s="43" t="s">
         <v>109</v>
       </c>
       <c r="P41" s="1">
@@ -3768,7 +3909,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>2023</v>
       </c>
@@ -3802,10 +3943,10 @@
       <c r="M42" s="1">
         <v>17.77</v>
       </c>
-      <c r="N42" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O42" s="44" t="s">
+      <c r="N42" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="O42" s="43" t="s">
         <v>109</v>
       </c>
       <c r="P42" s="1">
@@ -3824,7 +3965,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>2023</v>
       </c>
@@ -3858,10 +3999,10 @@
       <c r="M43" s="1">
         <v>17.77</v>
       </c>
-      <c r="N43" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O43" s="44" t="s">
+      <c r="N43" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="O43" s="43" t="s">
         <v>109</v>
       </c>
       <c r="P43" s="1">
@@ -3880,7 +4021,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>2023</v>
       </c>
@@ -3914,10 +4055,10 @@
       <c r="M44" s="1">
         <v>17.77</v>
       </c>
-      <c r="N44" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O44" s="44" t="s">
+      <c r="N44" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="O44" s="43" t="s">
         <v>109</v>
       </c>
       <c r="P44" s="1">
@@ -3936,7 +4077,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>2023</v>
       </c>
@@ -3970,10 +4111,10 @@
       <c r="M45" s="1">
         <v>17.77</v>
       </c>
-      <c r="N45" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O45" s="44" t="s">
+      <c r="N45" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="O45" s="43" t="s">
         <v>109</v>
       </c>
       <c r="P45" s="1">
@@ -3992,7 +4133,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>2023</v>
       </c>
@@ -4026,10 +4167,10 @@
       <c r="M46" s="1">
         <v>17.77</v>
       </c>
-      <c r="N46" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O46" s="44" t="s">
+      <c r="N46" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="O46" s="43" t="s">
         <v>109</v>
       </c>
       <c r="P46" s="1">
@@ -4048,7 +4189,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>2023</v>
       </c>
@@ -4082,10 +4223,10 @@
       <c r="M47" s="1">
         <v>17.77</v>
       </c>
-      <c r="N47" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O47" s="44" t="s">
+      <c r="N47" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="O47" s="43" t="s">
         <v>109</v>
       </c>
       <c r="P47" s="1">
@@ -4104,11 +4245,11 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>2023</v>
       </c>
-      <c r="B48" s="50" t="s">
+      <c r="B48" s="49" t="s">
         <v>170</v>
       </c>
       <c r="C48" s="1" t="s">
@@ -4138,10 +4279,10 @@
       <c r="M48" s="1">
         <v>17.77</v>
       </c>
-      <c r="N48" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O48" s="44" t="s">
+      <c r="N48" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="O48" s="43" t="s">
         <v>109</v>
       </c>
       <c r="P48" s="1">
@@ -4160,7 +4301,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>2023</v>
       </c>
@@ -4194,10 +4335,10 @@
       <c r="M49" s="1">
         <v>17.77</v>
       </c>
-      <c r="N49" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O49" s="44" t="s">
+      <c r="N49" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="O49" s="43" t="s">
         <v>109</v>
       </c>
       <c r="P49" s="1">
@@ -4216,7 +4357,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>2023</v>
       </c>
@@ -4250,10 +4391,10 @@
       <c r="M50" s="1">
         <v>17.77</v>
       </c>
-      <c r="N50" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O50" s="44" t="s">
+      <c r="N50" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="O50" s="43" t="s">
         <v>109</v>
       </c>
       <c r="P50" s="1">
@@ -4272,7 +4413,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>2023</v>
       </c>
@@ -4306,10 +4447,10 @@
       <c r="M51" s="1">
         <v>17.77</v>
       </c>
-      <c r="N51" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O51" s="44" t="s">
+      <c r="N51" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="O51" s="43" t="s">
         <v>109</v>
       </c>
       <c r="P51" s="1">
@@ -4328,11 +4469,11 @@
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>2023</v>
       </c>
-      <c r="B52" s="50" t="s">
+      <c r="B52" s="49" t="s">
         <v>181</v>
       </c>
       <c r="C52" s="1" t="s">
@@ -4362,10 +4503,10 @@
       <c r="M52" s="1">
         <v>17.77</v>
       </c>
-      <c r="N52" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O52" s="44" t="s">
+      <c r="N52" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="O52" s="43" t="s">
         <v>109</v>
       </c>
       <c r="P52" s="1">
@@ -4384,7 +4525,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>2023</v>
       </c>
@@ -4418,10 +4559,10 @@
       <c r="M53" s="1">
         <v>17.77</v>
       </c>
-      <c r="N53" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O53" s="44" t="s">
+      <c r="N53" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="O53" s="43" t="s">
         <v>109</v>
       </c>
       <c r="P53" s="1">
@@ -4440,7 +4581,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>2023</v>
       </c>
@@ -4474,10 +4615,10 @@
       <c r="M54" s="1">
         <v>17.77</v>
       </c>
-      <c r="N54" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O54" s="44" t="s">
+      <c r="N54" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="O54" s="43" t="s">
         <v>109</v>
       </c>
       <c r="P54" s="1">
@@ -4496,7 +4637,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>2023</v>
       </c>
@@ -4530,10 +4671,10 @@
       <c r="M55" s="1">
         <v>17.77</v>
       </c>
-      <c r="N55" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O55" s="44" t="s">
+      <c r="N55" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="O55" s="43" t="s">
         <v>109</v>
       </c>
       <c r="P55" s="1">
@@ -4552,7 +4693,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>2023</v>
       </c>
@@ -4586,10 +4727,10 @@
       <c r="M56" s="1">
         <v>17.77</v>
       </c>
-      <c r="N56" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O56" s="44" t="s">
+      <c r="N56" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="O56" s="43" t="s">
         <v>109</v>
       </c>
       <c r="P56" s="1">
@@ -4608,7 +4749,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>2023</v>
       </c>
@@ -4642,10 +4783,10 @@
       <c r="M57" s="1">
         <v>17.77</v>
       </c>
-      <c r="N57" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O57" s="44" t="s">
+      <c r="N57" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="O57" s="43" t="s">
         <v>109</v>
       </c>
       <c r="P57" s="1">
@@ -4664,7 +4805,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>2023</v>
       </c>
@@ -4698,10 +4839,10 @@
       <c r="M58" s="1">
         <v>16.45</v>
       </c>
-      <c r="N58" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O58" s="44" t="s">
+      <c r="N58" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="O58" s="43" t="s">
         <v>109</v>
       </c>
       <c r="P58" s="1">
@@ -4720,7 +4861,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>2023</v>
       </c>
@@ -4754,10 +4895,10 @@
       <c r="M59" s="1">
         <v>16.61</v>
       </c>
-      <c r="N59" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O59" s="44" t="s">
+      <c r="N59" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="O59" s="43" t="s">
         <v>109</v>
       </c>
       <c r="P59" s="1">
@@ -4776,7 +4917,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>2023</v>
       </c>
@@ -4810,10 +4951,10 @@
       <c r="M60" s="1">
         <v>16.61</v>
       </c>
-      <c r="N60" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O60" s="44" t="s">
+      <c r="N60" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="O60" s="43" t="s">
         <v>109</v>
       </c>
       <c r="P60" s="1">
@@ -4832,7 +4973,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>2023</v>
       </c>
@@ -4866,10 +5007,10 @@
       <c r="M61" s="1">
         <v>16.61</v>
       </c>
-      <c r="N61" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O61" s="44" t="s">
+      <c r="N61" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="O61" s="43" t="s">
         <v>109</v>
       </c>
       <c r="P61" s="1">
@@ -4888,7 +5029,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>2023</v>
       </c>
@@ -4928,10 +5069,10 @@
       <c r="M62" s="1">
         <v>16.21</v>
       </c>
-      <c r="N62" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O62" s="44" t="s">
+      <c r="N62" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="O62" s="43" t="s">
         <v>109</v>
       </c>
       <c r="P62" s="1">
@@ -4950,7 +5091,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>2023</v>
       </c>
@@ -4984,10 +5125,10 @@
       <c r="M63" s="1">
         <v>15.16</v>
       </c>
-      <c r="N63" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O63" s="44" t="s">
+      <c r="N63" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="O63" s="43" t="s">
         <v>109</v>
       </c>
       <c r="P63" s="1">
@@ -5006,7 +5147,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>2023</v>
       </c>
@@ -5046,10 +5187,10 @@
       <c r="M64" s="1">
         <v>17.84</v>
       </c>
-      <c r="N64" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O64" s="44" t="s">
+      <c r="N64" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="O64" s="43" t="s">
         <v>109</v>
       </c>
       <c r="P64" s="1">
@@ -5068,7 +5209,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>2023</v>
       </c>
@@ -5108,10 +5249,10 @@
       <c r="M65" s="1">
         <v>19.46</v>
       </c>
-      <c r="N65" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O65" s="44" t="s">
+      <c r="N65" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="O65" s="43" t="s">
         <v>109</v>
       </c>
       <c r="P65" s="1">
@@ -5130,7 +5271,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>2023</v>
       </c>
@@ -5170,10 +5311,10 @@
       <c r="M66" s="1">
         <v>14.59</v>
       </c>
-      <c r="N66" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O66" s="44" t="s">
+      <c r="N66" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="O66" s="43" t="s">
         <v>109</v>
       </c>
       <c r="P66" s="1">
@@ -5192,7 +5333,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>2023</v>
       </c>
@@ -5232,10 +5373,10 @@
       <c r="M67" s="1">
         <v>12.97</v>
       </c>
-      <c r="N67" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O67" s="44" t="s">
+      <c r="N67" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="O67" s="43" t="s">
         <v>109</v>
       </c>
       <c r="P67" s="1">
@@ -5254,7 +5395,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="68" spans="1:21" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:21" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>2023</v>
       </c>
@@ -5288,10 +5429,10 @@
       <c r="M68" s="1">
         <v>16.61</v>
       </c>
-      <c r="N68" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O68" s="44" t="s">
+      <c r="N68" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="O68" s="43" t="s">
         <v>109</v>
       </c>
       <c r="P68" s="1">
@@ -5310,7 +5451,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="69" spans="1:21" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:21" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>2023</v>
       </c>
@@ -5344,10 +5485,10 @@
       <c r="M69" s="1">
         <v>15.16</v>
       </c>
-      <c r="N69" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O69" s="44" t="s">
+      <c r="N69" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="O69" s="43" t="s">
         <v>109</v>
       </c>
       <c r="P69" s="1">
@@ -5366,7 +5507,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>2023</v>
       </c>
@@ -5400,10 +5541,10 @@
       <c r="M70" s="1">
         <v>16.21</v>
       </c>
-      <c r="N70" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O70" s="44" t="s">
+      <c r="N70" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="O70" s="43" t="s">
         <v>109</v>
       </c>
       <c r="P70" s="1">
@@ -5422,7 +5563,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>2023</v>
       </c>
@@ -5456,10 +5597,10 @@
       <c r="M71" s="1">
         <v>16.21</v>
       </c>
-      <c r="N71" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O71" s="44" t="s">
+      <c r="N71" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="O71" s="43" t="s">
         <v>109</v>
       </c>
       <c r="P71" s="1">
@@ -5478,7 +5619,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>2023</v>
       </c>
@@ -5512,10 +5653,10 @@
       <c r="M72" s="1">
         <v>16.21</v>
       </c>
-      <c r="N72" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O72" s="44" t="s">
+      <c r="N72" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="O72" s="43" t="s">
         <v>109</v>
       </c>
       <c r="P72" s="1">
@@ -5534,7 +5675,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>2023</v>
       </c>
@@ -5571,10 +5712,10 @@
       <c r="M73" s="1">
         <v>16.21</v>
       </c>
-      <c r="N73" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O73" s="44" t="s">
+      <c r="N73" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="O73" s="43" t="s">
         <v>109</v>
       </c>
       <c r="P73" s="1">
@@ -5596,7 +5737,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>2023</v>
       </c>
@@ -5633,10 +5774,10 @@
       <c r="M74" s="1">
         <v>16.21</v>
       </c>
-      <c r="N74" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O74" s="44" t="s">
+      <c r="N74" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="O74" s="43" t="s">
         <v>109</v>
       </c>
       <c r="P74" s="1">
@@ -5658,35 +5799,35 @@
         <v>340</v>
       </c>
     </row>
-    <row r="75" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="28">
+    <row r="75" spans="1:21" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="27">
         <v>2025</v>
       </c>
-      <c r="B75" s="28" t="s">
+      <c r="B75" s="27" t="s">
         <v>130</v>
       </c>
-      <c r="C75" s="28" t="s">
+      <c r="C75" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="D75" s="28" t="s">
+      <c r="D75" s="27" t="s">
         <v>244</v>
       </c>
-      <c r="F75" s="28" t="s">
+      <c r="F75" s="27" t="s">
         <v>131</v>
       </c>
-      <c r="J75" s="28" t="s">
+      <c r="J75" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="K75" s="29" t="s">
+      <c r="K75" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="N75" s="45"/>
-      <c r="O75" s="45"/>
-      <c r="R75" s="30"/>
-      <c r="S75" s="30"/>
-      <c r="T75" s="30"/>
-    </row>
-    <row r="76" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N75" s="44"/>
+      <c r="O75" s="44"/>
+      <c r="R75" s="29"/>
+      <c r="S75" s="29"/>
+      <c r="T75" s="29"/>
+    </row>
+    <row r="76" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="15">
         <v>2035</v>
       </c>
@@ -5723,10 +5864,10 @@
       <c r="M76" s="15">
         <v>15.85</v>
       </c>
-      <c r="N76" s="46">
+      <c r="N76" s="45">
         <v>-0.27</v>
       </c>
-      <c r="O76" s="46">
+      <c r="O76" s="45">
         <v>0</v>
       </c>
       <c r="P76" s="15" t="s">
@@ -5745,7 +5886,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="77" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="12">
         <v>2035</v>
       </c>
@@ -5779,10 +5920,10 @@
       <c r="M77" s="12">
         <v>15.85</v>
       </c>
-      <c r="N77" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="O77" s="47" t="s">
+      <c r="N77" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="O77" s="46" t="s">
         <v>109</v>
       </c>
       <c r="P77" s="14">
@@ -5801,7 +5942,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="78" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="12">
         <v>2035</v>
       </c>
@@ -5835,10 +5976,10 @@
       <c r="M78" s="12">
         <v>18.64</v>
       </c>
-      <c r="N78" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="O78" s="47" t="s">
+      <c r="N78" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="O78" s="46" t="s">
         <v>109</v>
       </c>
       <c r="P78" s="14">
@@ -5857,7 +5998,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="79" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="12">
         <v>2035</v>
       </c>
@@ -5891,10 +6032,10 @@
       <c r="M79" s="12">
         <v>18.64</v>
       </c>
-      <c r="N79" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="O79" s="47" t="s">
+      <c r="N79" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="O79" s="46" t="s">
         <v>109</v>
       </c>
       <c r="P79" s="14">
@@ -5913,7 +6054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="12">
         <v>2035</v>
       </c>
@@ -5947,10 +6088,10 @@
       <c r="M80" s="12">
         <v>18.64</v>
       </c>
-      <c r="N80" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="O80" s="47" t="s">
+      <c r="N80" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="O80" s="46" t="s">
         <v>109</v>
       </c>
       <c r="P80" s="12">
@@ -5969,7 +6110,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="81" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="12">
         <v>2035</v>
       </c>
@@ -6003,10 +6144,10 @@
       <c r="M81" s="12">
         <v>18.64</v>
       </c>
-      <c r="N81" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="O81" s="47" t="s">
+      <c r="N81" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="O81" s="46" t="s">
         <v>109</v>
       </c>
       <c r="P81" s="12">
@@ -6025,7 +6166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="12">
         <v>2035</v>
       </c>
@@ -6059,10 +6200,10 @@
       <c r="M82" s="12">
         <v>18.64</v>
       </c>
-      <c r="N82" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="O82" s="47" t="s">
+      <c r="N82" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="O82" s="46" t="s">
         <v>109</v>
       </c>
       <c r="P82" s="12">
@@ -6081,7 +6222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="12">
         <v>2035</v>
       </c>
@@ -6115,10 +6256,10 @@
       <c r="M83" s="12">
         <v>18.64</v>
       </c>
-      <c r="N83" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="O83" s="47" t="s">
+      <c r="N83" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="O83" s="46" t="s">
         <v>109</v>
       </c>
       <c r="P83" s="12">
@@ -6137,7 +6278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="12">
         <v>2035</v>
       </c>
@@ -6171,10 +6312,10 @@
       <c r="M84" s="12">
         <v>18.64</v>
       </c>
-      <c r="N84" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="O84" s="47" t="s">
+      <c r="N84" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="O84" s="46" t="s">
         <v>109</v>
       </c>
       <c r="P84" s="12">
@@ -6193,7 +6334,7 @@
         <v>41.25</v>
       </c>
     </row>
-    <row r="85" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="12">
         <v>2035</v>
       </c>
@@ -6227,10 +6368,10 @@
       <c r="M85" s="12">
         <v>20.55</v>
       </c>
-      <c r="N85" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="O85" s="47" t="s">
+      <c r="N85" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="O85" s="46" t="s">
         <v>109</v>
       </c>
       <c r="P85" s="12">
@@ -6249,7 +6390,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="86" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="12">
         <v>2035</v>
       </c>
@@ -6283,10 +6424,10 @@
       <c r="M86" s="12">
         <v>20.55</v>
       </c>
-      <c r="N86" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="O86" s="47" t="s">
+      <c r="N86" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="O86" s="46" t="s">
         <v>109</v>
       </c>
       <c r="P86" s="12">
@@ -6305,7 +6446,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="87" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="12">
         <v>2035</v>
       </c>
@@ -6321,7 +6462,7 @@
       <c r="F87" s="12" t="s">
         <v>270</v>
       </c>
-      <c r="G87" s="53" t="s">
+      <c r="G87" s="52" t="s">
         <v>232</v>
       </c>
       <c r="H87" s="12" t="s">
@@ -6339,10 +6480,10 @@
       <c r="M87" s="12">
         <v>20.55</v>
       </c>
-      <c r="N87" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="O87" s="47" t="s">
+      <c r="N87" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="O87" s="46" t="s">
         <v>109</v>
       </c>
       <c r="P87" s="12">
@@ -6361,7 +6502,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="88" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A88" s="12">
         <v>2035</v>
       </c>
@@ -6392,13 +6533,13 @@
       <c r="L88" s="12" t="s">
         <v>236</v>
       </c>
-      <c r="M88" s="53">
+      <c r="M88" s="52">
         <v>15.85</v>
       </c>
-      <c r="N88" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="O88" s="47" t="s">
+      <c r="N88" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="O88" s="46" t="s">
         <v>109</v>
       </c>
       <c r="P88" s="12">
@@ -6417,7 +6558,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="89" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" s="12">
         <v>2035</v>
       </c>
@@ -6451,10 +6592,10 @@
       <c r="M89" s="12">
         <v>20.55</v>
       </c>
-      <c r="N89" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="O89" s="47" t="s">
+      <c r="N89" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="O89" s="46" t="s">
         <v>109</v>
       </c>
       <c r="P89" s="12">
@@ -6463,17 +6604,17 @@
       <c r="Q89" s="12">
         <v>0.89</v>
       </c>
-      <c r="R89" s="52">
-        <v>0</v>
-      </c>
-      <c r="S89" s="52">
-        <v>0</v>
-      </c>
-      <c r="T89" s="52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="R89" s="51">
+        <v>0</v>
+      </c>
+      <c r="S89" s="51">
+        <v>0</v>
+      </c>
+      <c r="T89" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A90" s="12">
         <v>2035</v>
       </c>
@@ -6507,10 +6648,10 @@
       <c r="M90" s="12">
         <v>20.55</v>
       </c>
-      <c r="N90" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="O90" s="47" t="s">
+      <c r="N90" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="O90" s="46" t="s">
         <v>109</v>
       </c>
       <c r="P90" s="12">
@@ -6529,7 +6670,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="91" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="12">
         <v>2035</v>
       </c>
@@ -6563,10 +6704,10 @@
       <c r="M91" s="12">
         <v>20.55</v>
       </c>
-      <c r="N91" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="O91" s="47" t="s">
+      <c r="N91" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="O91" s="46" t="s">
         <v>109</v>
       </c>
       <c r="P91" s="12">
@@ -6585,7 +6726,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="92" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="12">
         <v>2035</v>
       </c>
@@ -6619,10 +6760,10 @@
       <c r="M92" s="12">
         <v>20.55</v>
       </c>
-      <c r="N92" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="O92" s="47" t="s">
+      <c r="N92" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="O92" s="46" t="s">
         <v>109</v>
       </c>
       <c r="P92" s="12">
@@ -6641,7 +6782,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="93" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A93" s="12">
         <v>2035</v>
       </c>
@@ -6675,16 +6816,16 @@
       <c r="M93" s="12">
         <v>20.55</v>
       </c>
-      <c r="N93" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="O93" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="P93" s="53">
+      <c r="N93" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="O93" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="P93" s="52">
         <v>0.84</v>
       </c>
-      <c r="Q93" s="53">
+      <c r="Q93" s="52">
         <v>1.59</v>
       </c>
       <c r="R93" s="14">
@@ -6697,7 +6838,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="94" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A94" s="12">
         <v>2035</v>
       </c>
@@ -6731,10 +6872,10 @@
       <c r="M94" s="12">
         <v>20.55</v>
       </c>
-      <c r="N94" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="O94" s="47" t="s">
+      <c r="N94" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="O94" s="46" t="s">
         <v>109</v>
       </c>
       <c r="P94" s="12">
@@ -6753,7 +6894,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="95" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A95" s="12">
         <v>2035</v>
       </c>
@@ -6775,7 +6916,7 @@
       <c r="H95" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="J95" s="53" t="s">
+      <c r="J95" s="52" t="s">
         <v>263</v>
       </c>
       <c r="K95" s="13" t="s">
@@ -6787,10 +6928,10 @@
       <c r="M95" s="12">
         <v>20.55</v>
       </c>
-      <c r="N95" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="O95" s="47" t="s">
+      <c r="N95" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="O95" s="46" t="s">
         <v>109</v>
       </c>
       <c r="P95" s="12">
@@ -6809,7 +6950,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="96" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A96" s="12">
         <v>2035</v>
       </c>
@@ -6843,10 +6984,10 @@
       <c r="M96" s="12">
         <v>20.55</v>
       </c>
-      <c r="N96" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="O96" s="47" t="s">
+      <c r="N96" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="O96" s="46" t="s">
         <v>109</v>
       </c>
       <c r="P96" s="12">
@@ -6865,7 +7006,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="97" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A97" s="12">
         <v>2035</v>
       </c>
@@ -6896,13 +7037,13 @@
       <c r="L97" s="12" t="s">
         <v>276</v>
       </c>
-      <c r="M97" s="53">
+      <c r="M97" s="52">
         <v>13.68</v>
       </c>
-      <c r="N97" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="O97" s="47" t="s">
+      <c r="N97" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="O97" s="46" t="s">
         <v>109</v>
       </c>
       <c r="P97" s="12">
@@ -6921,7 +7062,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="98" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="12">
         <v>2035</v>
       </c>
@@ -6952,13 +7093,13 @@
       <c r="L98" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="M98" s="53">
+      <c r="M98" s="52">
         <v>14.55</v>
       </c>
-      <c r="N98" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="O98" s="47" t="s">
+      <c r="N98" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="O98" s="46" t="s">
         <v>109</v>
       </c>
       <c r="P98" s="12">
@@ -6977,7 +7118,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="99" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A99" s="12">
         <v>2035</v>
       </c>
@@ -7011,13 +7152,13 @@
       <c r="L99" s="12" t="s">
         <v>286</v>
       </c>
-      <c r="M99" s="53">
+      <c r="M99" s="52">
         <v>17.579999999999998</v>
       </c>
-      <c r="N99" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="O99" s="47" t="s">
+      <c r="N99" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="O99" s="46" t="s">
         <v>109</v>
       </c>
       <c r="P99" s="12">
@@ -7039,7 +7180,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="100" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A100" s="12">
         <v>2035</v>
       </c>
@@ -7070,13 +7211,13 @@
       <c r="L100" s="12" t="s">
         <v>288</v>
       </c>
-      <c r="M100" s="53">
+      <c r="M100" s="52">
         <v>15.06</v>
       </c>
-      <c r="N100" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="O100" s="47" t="s">
+      <c r="N100" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="O100" s="46" t="s">
         <v>109</v>
       </c>
       <c r="P100" s="12">
@@ -7095,78 +7236,326 @@
         <v>75</v>
       </c>
     </row>
-    <row r="101" spans="1:21" s="24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="24">
+    <row r="101" spans="1:21" s="59" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="59">
+        <v>2035</v>
+      </c>
+      <c r="B101" s="59" t="s">
+        <v>341</v>
+      </c>
+      <c r="C101" s="59" t="s">
+        <v>342</v>
+      </c>
+      <c r="D101" s="59" t="s">
+        <v>343</v>
+      </c>
+      <c r="F101" s="59" t="s">
+        <v>344</v>
+      </c>
+      <c r="G101" s="59" t="s">
+        <v>346</v>
+      </c>
+      <c r="H101" s="59" t="s">
+        <v>347</v>
+      </c>
+      <c r="I101" s="59" t="s">
+        <v>11</v>
+      </c>
+      <c r="J101" s="59" t="s">
+        <v>348</v>
+      </c>
+      <c r="K101" s="60" t="s">
+        <v>110</v>
+      </c>
+      <c r="L101" s="63" t="s">
+        <v>345</v>
+      </c>
+      <c r="M101" s="59">
+        <v>17.579999999999998</v>
+      </c>
+      <c r="N101" s="61" t="s">
+        <v>109</v>
+      </c>
+      <c r="O101" s="61" t="s">
+        <v>109</v>
+      </c>
+      <c r="P101" s="59">
+        <v>0.87</v>
+      </c>
+      <c r="Q101" s="59">
+        <v>0.78</v>
+      </c>
+      <c r="R101" s="62">
+        <v>83.3</v>
+      </c>
+      <c r="S101" s="62">
+        <v>0</v>
+      </c>
+      <c r="T101" s="62">
+        <v>72</v>
+      </c>
+      <c r="U101" s="59" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="102" spans="1:21" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="64">
+        <v>2035</v>
+      </c>
+      <c r="B102" s="64" t="s">
+        <v>350</v>
+      </c>
+      <c r="C102" s="65" t="s">
+        <v>342</v>
+      </c>
+      <c r="D102" s="64" t="s">
+        <v>343</v>
+      </c>
+      <c r="F102" s="64" t="s">
+        <v>351</v>
+      </c>
+      <c r="G102" s="64" t="s">
+        <v>352</v>
+      </c>
+      <c r="H102" s="64" t="s">
+        <v>353</v>
+      </c>
+      <c r="I102" s="64" t="s">
+        <v>11</v>
+      </c>
+      <c r="J102" s="64" t="s">
+        <v>354</v>
+      </c>
+      <c r="K102" s="66" t="s">
+        <v>129</v>
+      </c>
+      <c r="L102" s="65" t="s">
+        <v>355</v>
+      </c>
+      <c r="M102" s="64">
+        <v>17.579999999999998</v>
+      </c>
+      <c r="N102" s="67" t="s">
+        <v>109</v>
+      </c>
+      <c r="O102" s="67" t="s">
+        <v>109</v>
+      </c>
+      <c r="P102" s="64">
+        <v>0.87</v>
+      </c>
+      <c r="Q102" s="64">
+        <v>0.78</v>
+      </c>
+      <c r="R102" s="68">
+        <v>83.3</v>
+      </c>
+      <c r="S102" s="68">
+        <v>0</v>
+      </c>
+      <c r="T102" s="68">
+        <v>72</v>
+      </c>
+      <c r="U102" s="64" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="103" spans="1:21" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="24">
         <v>2050</v>
       </c>
-      <c r="B101" s="24" t="s">
+      <c r="B103" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="C101" s="24" t="s">
+      <c r="C103" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="D101" s="24" t="s">
+      <c r="D103" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="F101" s="24" t="s">
+      <c r="F103" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="G101" s="24" t="s">
+      <c r="G103" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="H101" s="25" t="s">
+      <c r="H103" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="J101" s="24" t="s">
+      <c r="J103" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="K101" s="26" t="s">
+      <c r="K103" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="L101" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="M101" s="24">
+      <c r="L103" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="M103" s="24">
         <v>17.440000000000001</v>
       </c>
-      <c r="N101" s="48">
+      <c r="N103" s="47">
         <v>-0.33</v>
       </c>
-      <c r="O101" s="48">
-        <v>0</v>
-      </c>
-      <c r="P101" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q101" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="R101" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="S101" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="T101" s="27" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="103" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="M103" s="1">
+      <c r="O103" s="47">
+        <v>0</v>
+      </c>
+      <c r="P103" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q103" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="R103" s="76" t="s">
+        <v>109</v>
+      </c>
+      <c r="S103" s="76" t="s">
+        <v>109</v>
+      </c>
+      <c r="T103" s="76" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="104" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="54">
+        <v>2050</v>
+      </c>
+      <c r="B104" s="54" t="s">
+        <v>356</v>
+      </c>
+      <c r="C104" s="54" t="s">
+        <v>342</v>
+      </c>
+      <c r="D104" s="54" t="s">
+        <v>343</v>
+      </c>
+      <c r="F104" s="54" t="s">
+        <v>358</v>
+      </c>
+      <c r="G104" s="54" t="s">
+        <v>346</v>
+      </c>
+      <c r="H104" s="69" t="s">
+        <v>347</v>
+      </c>
+      <c r="I104" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="J104" s="54" t="s">
+        <v>348</v>
+      </c>
+      <c r="K104" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="L104" s="54" t="s">
+        <v>361</v>
+      </c>
+      <c r="M104" s="54">
+        <v>19.13</v>
+      </c>
+      <c r="N104" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="O104" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="P104" s="54">
+        <v>0.87</v>
+      </c>
+      <c r="Q104" s="54">
+        <v>0.78</v>
+      </c>
+      <c r="R104" s="57">
+        <v>83.3</v>
+      </c>
+      <c r="S104" s="57">
+        <v>0</v>
+      </c>
+      <c r="T104" s="57">
+        <v>72</v>
+      </c>
+      <c r="U104" s="54" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="105" spans="1:21" s="71" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="71">
+        <v>2050</v>
+      </c>
+      <c r="B105" s="71" t="s">
+        <v>357</v>
+      </c>
+      <c r="C105" s="71" t="s">
+        <v>342</v>
+      </c>
+      <c r="D105" s="71" t="s">
+        <v>343</v>
+      </c>
+      <c r="F105" s="71" t="s">
+        <v>359</v>
+      </c>
+      <c r="G105" s="71" t="s">
+        <v>352</v>
+      </c>
+      <c r="H105" s="72" t="s">
+        <v>353</v>
+      </c>
+      <c r="I105" s="71" t="s">
+        <v>11</v>
+      </c>
+      <c r="J105" s="71" t="s">
+        <v>360</v>
+      </c>
+      <c r="K105" s="73" t="s">
+        <v>44</v>
+      </c>
+      <c r="L105" s="71" t="s">
+        <v>362</v>
+      </c>
+      <c r="M105" s="71">
+        <v>19.13</v>
+      </c>
+      <c r="N105" s="74" t="s">
+        <v>109</v>
+      </c>
+      <c r="O105" s="74" t="s">
+        <v>109</v>
+      </c>
+      <c r="P105" s="71">
+        <v>0.87</v>
+      </c>
+      <c r="Q105" s="71">
+        <v>0.78</v>
+      </c>
+      <c r="R105" s="75">
+        <v>83.3</v>
+      </c>
+      <c r="S105" s="75">
+        <v>0</v>
+      </c>
+      <c r="T105" s="75">
+        <v>72</v>
+      </c>
+      <c r="U105" s="71" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="107" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="M107" s="1">
         <f>M97*2</f>
         <v>27.36</v>
       </c>
-      <c r="N103" s="44">
+      <c r="N107" s="43">
         <f>M96*2</f>
         <v>41.1</v>
       </c>
     </row>
-    <row r="104" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="M104" s="1">
+    <row r="108" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="M108" s="1">
         <f>M97*3</f>
         <v>41.04</v>
       </c>
-      <c r="N104" s="44">
+      <c r="N108" s="43">
         <f>M96*3</f>
         <v>61.650000000000006</v>
       </c>

</xml_diff>

<commit_message>
Added missing details for 2035_TM160_IPA_17
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E63002-7EA5-4675-9B3F-E42EB810A6D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AA5F989-3DA7-4FA8-853F-B0FEA58FD6EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8040" yWindow="3750" windowWidth="24885" windowHeight="11385" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="28800" windowHeight="15435" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelRuns" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="376">
   <si>
     <t>year</t>
   </si>
@@ -1854,10 +1854,10 @@
   <dimension ref="A1:U109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E95" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C87" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M104" sqref="M104"/>
+      <selection pane="bottomRight" activeCell="D117" sqref="D117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7430,9 +7430,6 @@
       <c r="T103" s="14">
         <v>75</v>
       </c>
-      <c r="U103" s="12" t="s">
-        <v>332</v>
-      </c>
     </row>
     <row r="104" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A104" s="12">
@@ -7441,6 +7438,12 @@
       <c r="B104" s="12" t="s">
         <v>373</v>
       </c>
+      <c r="C104" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D104" s="12" t="s">
+        <v>243</v>
+      </c>
       <c r="F104" s="12" t="s">
         <v>374</v>
       </c>
@@ -7462,12 +7465,33 @@
       <c r="L104" s="12" t="s">
         <v>375</v>
       </c>
-      <c r="M104" s="52"/>
-      <c r="N104" s="46"/>
-      <c r="O104" s="46"/>
-      <c r="R104" s="14"/>
-      <c r="S104" s="14"/>
-      <c r="T104" s="14"/>
+      <c r="M104" s="52">
+        <v>16.82</v>
+      </c>
+      <c r="N104" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="O104" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="P104" s="12">
+        <v>0.87</v>
+      </c>
+      <c r="Q104" s="12">
+        <v>0.78</v>
+      </c>
+      <c r="R104" s="14">
+        <v>100</v>
+      </c>
+      <c r="S104" s="14">
+        <v>0</v>
+      </c>
+      <c r="T104" s="14">
+        <v>75</v>
+      </c>
+      <c r="U104" s="12" t="s">
+        <v>332</v>
+      </c>
     </row>
     <row r="105" spans="1:21" s="59" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A105" s="59">

</xml_diff>

<commit_message>
minor fix to the description of v56
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one-master\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D0618A8-28AB-4FA3-8272-6F76E50EB0ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED67816-3A07-4045-9510-326E8DF486BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4530" yWindow="3645" windowWidth="28800" windowHeight="15435" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelRuns" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1233" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1233" uniqueCount="385">
   <si>
     <t>year</t>
   </si>
@@ -1206,6 +1206,9 @@
   </si>
   <si>
     <t>2050_TM160_DBP_Plan_02</t>
+  </si>
+  <si>
+    <t>AOC=15.28, with BART_Transit_Hesitance=70</t>
   </si>
 </sst>
 </file>
@@ -1384,7 +1387,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1540,7 +1543,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1872,32 +1874,32 @@
   <dimension ref="A1:U113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C87" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C62" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A113" sqref="A113"/>
+      <selection pane="bottomRight" activeCell="F78" sqref="F78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="42.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.54296875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="42.26953125" style="1" customWidth="1"/>
     <col min="7" max="7" width="23" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.28515625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" style="10" customWidth="1"/>
-    <col min="12" max="12" width="17.5703125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="8.28515625" style="1" customWidth="1"/>
-    <col min="14" max="15" width="9.28515625" style="43"/>
-    <col min="16" max="16384" width="9.28515625" style="1"/>
+    <col min="8" max="8" width="8.26953125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="6.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.26953125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11.26953125" style="10" customWidth="1"/>
+    <col min="12" max="12" width="17.54296875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="8.26953125" style="1" customWidth="1"/>
+    <col min="14" max="15" width="9.26953125" style="43"/>
+    <col min="16" max="16384" width="9.26953125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="5" customFormat="1" ht="39" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1962,7 +1964,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19">
         <v>2005</v>
       </c>
@@ -2015,7 +2017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="30">
         <v>2005</v>
       </c>
@@ -2071,7 +2073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30">
         <v>2005</v>
       </c>
@@ -2126,7 +2128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:21" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="30">
         <v>2005</v>
       </c>
@@ -2181,7 +2183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:21" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="30">
         <v>2005</v>
       </c>
@@ -2240,7 +2242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="53">
         <v>2015</v>
       </c>
@@ -2281,7 +2283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="34">
         <v>2015</v>
       </c>
@@ -2327,7 +2329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="34">
         <v>2015</v>
       </c>
@@ -2380,7 +2382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="34">
         <v>2015</v>
       </c>
@@ -2433,7 +2435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="34">
         <v>2015</v>
       </c>
@@ -2486,7 +2488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="34">
         <v>2015</v>
       </c>
@@ -2542,7 +2544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="34">
         <v>2015</v>
       </c>
@@ -2598,7 +2600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="34">
         <v>2015</v>
       </c>
@@ -2654,7 +2656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="34">
         <v>2015</v>
       </c>
@@ -2714,7 +2716,7 @@
       </c>
       <c r="U15" s="58"/>
     </row>
-    <row r="16" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="34">
         <v>2015</v>
       </c>
@@ -2776,7 +2778,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>2023</v>
       </c>
@@ -2822,7 +2824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>2023</v>
       </c>
@@ -2868,7 +2870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>2023</v>
       </c>
@@ -2914,7 +2916,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>2023</v>
       </c>
@@ -2960,7 +2962,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>2023</v>
       </c>
@@ -3006,7 +3008,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>2023</v>
       </c>
@@ -3052,7 +3054,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>2023</v>
       </c>
@@ -3098,7 +3100,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>2023</v>
       </c>
@@ -3144,7 +3146,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>2023</v>
       </c>
@@ -3190,7 +3192,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>2023</v>
       </c>
@@ -3236,7 +3238,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>2023</v>
       </c>
@@ -3282,7 +3284,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>2023</v>
       </c>
@@ -3328,7 +3330,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>2023</v>
       </c>
@@ -3374,7 +3376,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>2023</v>
       </c>
@@ -3420,7 +3422,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>2023</v>
       </c>
@@ -3466,7 +3468,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>2023</v>
       </c>
@@ -3512,7 +3514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>2023</v>
       </c>
@@ -3558,7 +3560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>2023</v>
       </c>
@@ -3604,7 +3606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>2023</v>
       </c>
@@ -3648,7 +3650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>2023</v>
       </c>
@@ -3697,7 +3699,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>2023</v>
       </c>
@@ -3744,7 +3746,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>2023</v>
       </c>
@@ -3791,7 +3793,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>2023</v>
       </c>
@@ -3847,7 +3849,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>2023</v>
       </c>
@@ -3903,7 +3905,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>2023</v>
       </c>
@@ -3959,7 +3961,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>2023</v>
       </c>
@@ -4015,7 +4017,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>2023</v>
       </c>
@@ -4071,7 +4073,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>2023</v>
       </c>
@@ -4127,7 +4129,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>2023</v>
       </c>
@@ -4183,7 +4185,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>2023</v>
       </c>
@@ -4239,7 +4241,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>2023</v>
       </c>
@@ -4295,7 +4297,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>2023</v>
       </c>
@@ -4351,7 +4353,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>2023</v>
       </c>
@@ -4407,7 +4409,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>2023</v>
       </c>
@@ -4463,7 +4465,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>2023</v>
       </c>
@@ -4519,7 +4521,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>2023</v>
       </c>
@@ -4575,7 +4577,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>2023</v>
       </c>
@@ -4631,7 +4633,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>2023</v>
       </c>
@@ -4687,7 +4689,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>2023</v>
       </c>
@@ -4743,7 +4745,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>2023</v>
       </c>
@@ -4799,7 +4801,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>2023</v>
       </c>
@@ -4855,7 +4857,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>2023</v>
       </c>
@@ -4911,7 +4913,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>2023</v>
       </c>
@@ -4967,7 +4969,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>2023</v>
       </c>
@@ -5023,7 +5025,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>2023</v>
       </c>
@@ -5079,7 +5081,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>2023</v>
       </c>
@@ -5135,7 +5137,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>2023</v>
       </c>
@@ -5191,7 +5193,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>2023</v>
       </c>
@@ -5253,7 +5255,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>2023</v>
       </c>
@@ -5309,7 +5311,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>2023</v>
       </c>
@@ -5371,7 +5373,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>2023</v>
       </c>
@@ -5433,7 +5435,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>2023</v>
       </c>
@@ -5495,7 +5497,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>2023</v>
       </c>
@@ -5557,7 +5559,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="70" spans="1:21" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:21" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>2023</v>
       </c>
@@ -5613,7 +5615,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="71" spans="1:21" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:21" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>2023</v>
       </c>
@@ -5669,7 +5671,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>2023</v>
       </c>
@@ -5725,7 +5727,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>2023</v>
       </c>
@@ -5781,7 +5783,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>2023</v>
       </c>
@@ -5837,7 +5839,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>2023</v>
       </c>
@@ -5896,7 +5898,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>2023</v>
       </c>
@@ -5956,7 +5958,7 @@
       </c>
       <c r="U76" s="74"/>
     </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>2023</v>
       </c>
@@ -5970,7 +5972,7 @@
         <v>245</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>337</v>
+        <v>384</v>
       </c>
       <c r="G77" s="1" t="s">
         <v>9</v>
@@ -6018,7 +6020,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="78" spans="1:21" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:21" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="27">
         <v>2025</v>
       </c>
@@ -6046,7 +6048,7 @@
       <c r="S78" s="29"/>
       <c r="T78" s="29"/>
     </row>
-    <row r="79" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="15">
         <v>2035</v>
       </c>
@@ -6105,7 +6107,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="80" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="12">
         <v>2035</v>
       </c>
@@ -6161,7 +6163,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="81" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="12">
         <v>2035</v>
       </c>
@@ -6217,7 +6219,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="82" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="12">
         <v>2035</v>
       </c>
@@ -6273,7 +6275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="12">
         <v>2035</v>
       </c>
@@ -6329,7 +6331,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="84" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A84" s="12">
         <v>2035</v>
       </c>
@@ -6385,7 +6387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="12">
         <v>2035</v>
       </c>
@@ -6441,7 +6443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" s="12">
         <v>2035</v>
       </c>
@@ -6497,7 +6499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" s="12">
         <v>2035</v>
       </c>
@@ -6553,7 +6555,7 @@
         <v>41.25</v>
       </c>
     </row>
-    <row r="88" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="12">
         <v>2035</v>
       </c>
@@ -6609,7 +6611,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="89" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="12">
         <v>2035</v>
       </c>
@@ -6665,7 +6667,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="90" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90" s="12">
         <v>2035</v>
       </c>
@@ -6721,7 +6723,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="91" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" s="12">
         <v>2035</v>
       </c>
@@ -6777,7 +6779,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="92" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="12">
         <v>2035</v>
       </c>
@@ -6833,7 +6835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" s="12">
         <v>2035</v>
       </c>
@@ -6889,7 +6891,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="94" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" s="12">
         <v>2035</v>
       </c>
@@ -6945,7 +6947,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="95" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A95" s="12">
         <v>2035</v>
       </c>
@@ -7001,7 +7003,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="96" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A96" s="12">
         <v>2035</v>
       </c>
@@ -7057,7 +7059,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="97" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A97" s="12">
         <v>2035</v>
       </c>
@@ -7113,7 +7115,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="98" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" s="12">
         <v>2035</v>
       </c>
@@ -7169,7 +7171,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="99" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A99" s="12">
         <v>2035</v>
       </c>
@@ -7225,7 +7227,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="100" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A100" s="12">
         <v>2035</v>
       </c>
@@ -7281,7 +7283,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="101" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A101" s="12">
         <v>2035</v>
       </c>
@@ -7337,7 +7339,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="102" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A102" s="12">
         <v>2035</v>
       </c>
@@ -7393,7 +7395,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="103" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A103" s="12">
         <v>2035</v>
       </c>
@@ -7449,7 +7451,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="104" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A104" s="12">
         <v>2035</v>
       </c>
@@ -7511,7 +7513,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="105" spans="1:21" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:21" s="59" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A105" s="59">
         <v>2035</v>
       </c>
@@ -7539,7 +7541,7 @@
       <c r="K105" s="60" t="s">
         <v>110</v>
       </c>
-      <c r="L105" s="75" t="s">
+      <c r="L105" s="59" t="s">
         <v>342</v>
       </c>
       <c r="M105" s="59">
@@ -7567,7 +7569,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="106" spans="1:21" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:21" s="59" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A106" s="59">
         <v>2035</v>
       </c>
@@ -7598,7 +7600,7 @@
       <c r="K106" s="60" t="s">
         <v>110</v>
       </c>
-      <c r="L106" s="75" t="s">
+      <c r="L106" s="59" t="s">
         <v>378</v>
       </c>
       <c r="M106" s="59">
@@ -7629,7 +7631,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="107" spans="1:21" s="63" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:21" s="63" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A107" s="63">
         <v>2035</v>
       </c>
@@ -7685,7 +7687,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="108" spans="1:21" s="63" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:21" s="63" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A108" s="63">
         <v>2035</v>
       </c>
@@ -7747,7 +7749,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="109" spans="1:21" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:21" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A109" s="24">
         <v>2050</v>
       </c>
@@ -7803,7 +7805,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="110" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A110" s="54">
         <v>2050</v>
       </c>
@@ -7859,7 +7861,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="111" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A111" s="54">
         <v>2050</v>
       </c>
@@ -7921,7 +7923,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="112" spans="1:21" s="69" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:21" s="69" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A112" s="69">
         <v>2050</v>
       </c>
@@ -7980,7 +7982,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="113" spans="1:21" s="69" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:21" s="69" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A113" s="69">
         <v>2050</v>
       </c>

</xml_diff>

<commit_message>
Demote some runs from current and fix model run ID typo
(there is no TM161)
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one-master\utilities\RTP\config_RTP2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED67816-3A07-4045-9510-326E8DF486BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923A236D-8178-4D35-8BFF-76CACFEF60AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
+    <workbookView xWindow="4665" yWindow="3690" windowWidth="24150" windowHeight="13290" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelRuns" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1233" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1227" uniqueCount="385">
   <si>
     <t>year</t>
   </si>
@@ -923,9 +923,6 @@
     <t>https://app.asana.com/0/1204085012544660/1206323265669539/f</t>
   </si>
   <si>
-    <t>2023_TM161_IPA_50</t>
-  </si>
-  <si>
     <t>https://app.asana.com/0/1204085012544660/1206579347148152/f</t>
   </si>
   <si>
@@ -1209,6 +1206,9 @@
   </si>
   <si>
     <t>AOC=15.28, with BART_Transit_Hesitance=70</t>
+  </si>
+  <si>
+    <t>2023_TM160_IPA_50</t>
   </si>
 </sst>
 </file>
@@ -1874,32 +1874,32 @@
   <dimension ref="A1:U113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C62" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C67" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F78" sqref="F78"/>
+      <selection pane="bottomRight" activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.81640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.54296875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="42.26953125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="42.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="23" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.26953125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.26953125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="11.26953125" style="10" customWidth="1"/>
-    <col min="12" max="12" width="17.54296875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="8.26953125" style="1" customWidth="1"/>
-    <col min="14" max="15" width="9.26953125" style="43"/>
-    <col min="16" max="16384" width="9.26953125" style="1"/>
+    <col min="8" max="8" width="8.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" style="10" customWidth="1"/>
+    <col min="12" max="12" width="17.5703125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="8.28515625" style="1" customWidth="1"/>
+    <col min="14" max="15" width="9.28515625" style="43"/>
+    <col min="16" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="5" customFormat="1" ht="39" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1913,7 +1913,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>18</v>
@@ -1961,10 +1961,10 @@
         <v>84</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.3">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="19">
         <v>2005</v>
       </c>
@@ -2017,7 +2017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="30">
         <v>2005</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="30">
         <v>2005</v>
       </c>
@@ -2128,7 +2128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:21" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="30">
         <v>2005</v>
       </c>
@@ -2183,12 +2183,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:21" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="30">
         <v>2005</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C6" s="31" t="s">
         <v>17</v>
@@ -2197,7 +2197,7 @@
         <v>247</v>
       </c>
       <c r="F6" s="31" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G6" s="31" t="s">
         <v>267</v>
@@ -2215,7 +2215,7 @@
         <v>43</v>
       </c>
       <c r="L6" s="31" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="M6" s="31">
         <v>14.07</v>
@@ -2242,7 +2242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="53">
         <v>2015</v>
       </c>
@@ -2283,7 +2283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="34">
         <v>2015</v>
       </c>
@@ -2329,7 +2329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="34">
         <v>2015</v>
       </c>
@@ -2382,7 +2382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="34">
         <v>2015</v>
       </c>
@@ -2435,7 +2435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="34">
         <v>2015</v>
       </c>
@@ -2488,7 +2488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="34">
         <v>2015</v>
       </c>
@@ -2544,7 +2544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="34">
         <v>2015</v>
       </c>
@@ -2600,12 +2600,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="34">
         <v>2015</v>
       </c>
       <c r="B14" s="35" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C14" s="35" t="s">
         <v>17</v>
@@ -2614,7 +2614,7 @@
         <v>246</v>
       </c>
       <c r="F14" s="35" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G14" s="35" t="s">
         <v>9</v>
@@ -2629,7 +2629,7 @@
         <v>16</v>
       </c>
       <c r="L14" s="35" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="M14" s="35">
         <v>13.73</v>
@@ -2656,12 +2656,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="34">
         <v>2015</v>
       </c>
       <c r="B15" s="35" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C15" s="35" t="s">
         <v>17</v>
@@ -2670,7 +2670,7 @@
         <v>246</v>
       </c>
       <c r="F15" s="35" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G15" s="35" t="s">
         <v>9</v>
@@ -2688,7 +2688,7 @@
         <v>16</v>
       </c>
       <c r="L15" s="35" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="M15" s="35">
         <v>13.73</v>
@@ -2716,12 +2716,12 @@
       </c>
       <c r="U15" s="58"/>
     </row>
-    <row r="16" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="34">
         <v>2015</v>
       </c>
       <c r="B16" s="35" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C16" s="35" t="s">
         <v>17</v>
@@ -2730,7 +2730,7 @@
         <v>246</v>
       </c>
       <c r="F16" s="35" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G16" s="35" t="s">
         <v>9</v>
@@ -2748,7 +2748,7 @@
         <v>16</v>
       </c>
       <c r="L16" s="35" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="M16" s="35">
         <v>15.28</v>
@@ -2775,10 +2775,10 @@
         <v>0</v>
       </c>
       <c r="U16" s="58" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>2023</v>
       </c>
@@ -2824,7 +2824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>2023</v>
       </c>
@@ -2870,7 +2870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>2023</v>
       </c>
@@ -2916,7 +2916,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>2023</v>
       </c>
@@ -2962,7 +2962,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>2023</v>
       </c>
@@ -3008,7 +3008,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>2023</v>
       </c>
@@ -3054,7 +3054,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>2023</v>
       </c>
@@ -3100,7 +3100,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>2023</v>
       </c>
@@ -3146,7 +3146,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>2023</v>
       </c>
@@ -3192,7 +3192,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>2023</v>
       </c>
@@ -3238,7 +3238,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>2023</v>
       </c>
@@ -3284,7 +3284,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>2023</v>
       </c>
@@ -3330,7 +3330,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>2023</v>
       </c>
@@ -3376,7 +3376,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>2023</v>
       </c>
@@ -3422,7 +3422,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>2023</v>
       </c>
@@ -3468,7 +3468,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>2023</v>
       </c>
@@ -3514,7 +3514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>2023</v>
       </c>
@@ -3560,7 +3560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>2023</v>
       </c>
@@ -3606,7 +3606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>2023</v>
       </c>
@@ -3650,7 +3650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>2023</v>
       </c>
@@ -3699,7 +3699,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>2023</v>
       </c>
@@ -3746,7 +3746,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>2023</v>
       </c>
@@ -3793,7 +3793,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>2023</v>
       </c>
@@ -3849,7 +3849,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>2023</v>
       </c>
@@ -3905,7 +3905,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>2023</v>
       </c>
@@ -3961,7 +3961,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>2023</v>
       </c>
@@ -4017,7 +4017,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>2023</v>
       </c>
@@ -4073,7 +4073,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>2023</v>
       </c>
@@ -4129,7 +4129,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>2023</v>
       </c>
@@ -4185,7 +4185,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>2023</v>
       </c>
@@ -4241,7 +4241,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>2023</v>
       </c>
@@ -4297,7 +4297,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>2023</v>
       </c>
@@ -4353,7 +4353,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>2023</v>
       </c>
@@ -4409,7 +4409,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>2023</v>
       </c>
@@ -4465,7 +4465,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>2023</v>
       </c>
@@ -4521,7 +4521,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>2023</v>
       </c>
@@ -4577,7 +4577,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>2023</v>
       </c>
@@ -4633,7 +4633,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>2023</v>
       </c>
@@ -4689,7 +4689,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>2023</v>
       </c>
@@ -4745,7 +4745,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>2023</v>
       </c>
@@ -4801,7 +4801,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>2023</v>
       </c>
@@ -4857,7 +4857,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>2023</v>
       </c>
@@ -4913,7 +4913,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>2023</v>
       </c>
@@ -4969,7 +4969,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>2023</v>
       </c>
@@ -5025,7 +5025,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>2023</v>
       </c>
@@ -5081,7 +5081,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>2023</v>
       </c>
@@ -5137,12 +5137,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>2023</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>17</v>
@@ -5151,7 +5151,7 @@
         <v>245</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G63" s="1" t="s">
         <v>9</v>
@@ -5160,13 +5160,13 @@
         <v>10</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K63" s="10" t="s">
         <v>129</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M63" s="1">
         <v>16.61</v>
@@ -5193,12 +5193,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>2023</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>17</v>
@@ -5207,10 +5207,10 @@
         <v>245</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>9</v>
@@ -5218,17 +5218,14 @@
       <c r="H64" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I64" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="J64" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K64" s="10" t="s">
         <v>129</v>
       </c>
       <c r="L64" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="M64" s="1">
         <v>16.21</v>
@@ -5255,12 +5252,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>2023</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>17</v>
@@ -5269,7 +5266,7 @@
         <v>245</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>9</v>
@@ -5278,13 +5275,13 @@
         <v>10</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K65" s="10" t="s">
         <v>42</v>
       </c>
       <c r="L65" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="M65" s="1">
         <v>15.16</v>
@@ -5311,12 +5308,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>2023</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>17</v>
@@ -5325,10 +5322,10 @@
         <v>245</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>9</v>
@@ -5336,17 +5333,14 @@
       <c r="H66" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I66" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="J66" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K66" s="10" t="s">
         <v>108</v>
       </c>
       <c r="L66" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M66" s="1">
         <v>17.84</v>
@@ -5373,12 +5367,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>2023</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>17</v>
@@ -5387,10 +5381,10 @@
         <v>245</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>9</v>
@@ -5398,17 +5392,14 @@
       <c r="H67" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I67" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="J67" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K67" s="10" t="s">
         <v>43</v>
       </c>
       <c r="L67" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M67" s="1">
         <v>19.46</v>
@@ -5435,12 +5426,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>2023</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>17</v>
@@ -5449,10 +5440,10 @@
         <v>245</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>9</v>
@@ -5460,17 +5451,14 @@
       <c r="H68" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I68" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="J68" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K68" s="10" t="s">
         <v>108</v>
       </c>
       <c r="L68" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M68" s="1">
         <v>14.59</v>
@@ -5497,12 +5485,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>2023</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>17</v>
@@ -5511,10 +5499,10 @@
         <v>245</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G69" s="1" t="s">
         <v>9</v>
@@ -5522,17 +5510,14 @@
       <c r="H69" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I69" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="J69" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K69" s="10" t="s">
         <v>43</v>
       </c>
       <c r="L69" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M69" s="1">
         <v>12.97</v>
@@ -5559,12 +5544,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="70" spans="1:21" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:21" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>2023</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>289</v>
+        <v>384</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>17</v>
@@ -5573,7 +5558,7 @@
         <v>245</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G70" s="1" t="s">
         <v>9</v>
@@ -5582,13 +5567,13 @@
         <v>10</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K70" s="10" t="s">
         <v>108</v>
       </c>
       <c r="L70" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="M70" s="1">
         <v>16.61</v>
@@ -5615,12 +5600,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="71" spans="1:21" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:21" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>2023</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>17</v>
@@ -5629,7 +5614,7 @@
         <v>245</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G71" s="1" t="s">
         <v>9</v>
@@ -5638,13 +5623,13 @@
         <v>10</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K71" s="10" t="s">
         <v>108</v>
       </c>
       <c r="L71" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="M71" s="1">
         <v>15.16</v>
@@ -5671,12 +5656,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>2023</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>17</v>
@@ -5685,7 +5670,7 @@
         <v>245</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G72" s="1" t="s">
         <v>9</v>
@@ -5694,13 +5679,13 @@
         <v>10</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K72" s="10" t="s">
         <v>42</v>
       </c>
       <c r="L72" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="M72" s="1">
         <v>16.21</v>
@@ -5727,12 +5712,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>2023</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>17</v>
@@ -5741,7 +5726,7 @@
         <v>245</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G73" s="1" t="s">
         <v>9</v>
@@ -5750,13 +5735,13 @@
         <v>10</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K73" s="10" t="s">
         <v>88</v>
       </c>
       <c r="L73" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="M73" s="1">
         <v>16.21</v>
@@ -5783,12 +5768,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>2023</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>17</v>
@@ -5797,7 +5782,7 @@
         <v>245</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G74" s="1" t="s">
         <v>9</v>
@@ -5806,13 +5791,13 @@
         <v>10</v>
       </c>
       <c r="J74" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K74" s="10" t="s">
         <v>16</v>
       </c>
       <c r="L74" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="M74" s="1">
         <v>16.21</v>
@@ -5839,12 +5824,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>2023</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>17</v>
@@ -5853,7 +5838,7 @@
         <v>245</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G75" s="1" t="s">
         <v>9</v>
@@ -5865,13 +5850,13 @@
         <v>11</v>
       </c>
       <c r="J75" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K75" s="10" t="s">
         <v>16</v>
       </c>
       <c r="L75" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="M75" s="1">
         <v>16.21</v>
@@ -5898,12 +5883,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>2023</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>17</v>
@@ -5912,7 +5897,7 @@
         <v>245</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G76" s="1" t="s">
         <v>9</v>
@@ -5924,13 +5909,13 @@
         <v>11</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K76" s="10" t="s">
         <v>16</v>
       </c>
       <c r="L76" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="M76" s="1">
         <v>16.21</v>
@@ -5958,12 +5943,12 @@
       </c>
       <c r="U76" s="74"/>
     </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>2023</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>17</v>
@@ -5972,7 +5957,7 @@
         <v>245</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="G77" s="1" t="s">
         <v>9</v>
@@ -5984,13 +5969,13 @@
         <v>11</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K77" s="10" t="s">
         <v>44</v>
       </c>
       <c r="L77" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="M77" s="1">
         <v>15.28</v>
@@ -6017,10 +6002,10 @@
         <v>72</v>
       </c>
       <c r="U77" s="74" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="78" spans="1:21" s="27" customFormat="1" x14ac:dyDescent="0.3">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="27">
         <v>2025</v>
       </c>
@@ -6048,7 +6033,7 @@
       <c r="S78" s="29"/>
       <c r="T78" s="29"/>
     </row>
-    <row r="79" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="15">
         <v>2035</v>
       </c>
@@ -6107,7 +6092,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="80" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="12">
         <v>2035</v>
       </c>
@@ -6163,7 +6148,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="81" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="12">
         <v>2035</v>
       </c>
@@ -6219,7 +6204,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="82" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="12">
         <v>2035</v>
       </c>
@@ -6275,7 +6260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="12">
         <v>2035</v>
       </c>
@@ -6331,7 +6316,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="84" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="12">
         <v>2035</v>
       </c>
@@ -6387,7 +6372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="12">
         <v>2035</v>
       </c>
@@ -6443,7 +6428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="12">
         <v>2035</v>
       </c>
@@ -6499,7 +6484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="12">
         <v>2035</v>
       </c>
@@ -6555,7 +6540,7 @@
         <v>41.25</v>
       </c>
     </row>
-    <row r="88" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A88" s="12">
         <v>2035</v>
       </c>
@@ -6611,7 +6596,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="89" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" s="12">
         <v>2035</v>
       </c>
@@ -6667,7 +6652,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="90" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A90" s="12">
         <v>2035</v>
       </c>
@@ -6723,7 +6708,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="91" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="12">
         <v>2035</v>
       </c>
@@ -6779,7 +6764,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="92" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="12">
         <v>2035</v>
       </c>
@@ -6835,7 +6820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A93" s="12">
         <v>2035</v>
       </c>
@@ -6891,7 +6876,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="94" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A94" s="12">
         <v>2035</v>
       </c>
@@ -6947,7 +6932,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="95" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A95" s="12">
         <v>2035</v>
       </c>
@@ -7003,7 +6988,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="96" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A96" s="12">
         <v>2035</v>
       </c>
@@ -7059,7 +7044,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="97" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A97" s="12">
         <v>2035</v>
       </c>
@@ -7115,7 +7100,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="98" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="12">
         <v>2035</v>
       </c>
@@ -7171,7 +7156,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="99" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A99" s="12">
         <v>2035</v>
       </c>
@@ -7227,7 +7212,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="100" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A100" s="12">
         <v>2035</v>
       </c>
@@ -7283,7 +7268,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="101" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A101" s="12">
         <v>2035</v>
       </c>
@@ -7339,7 +7324,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="102" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A102" s="12">
         <v>2035</v>
       </c>
@@ -7395,7 +7380,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="103" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A103" s="12">
         <v>2035</v>
       </c>
@@ -7451,12 +7436,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="104" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A104" s="12">
         <v>2035</v>
       </c>
       <c r="B104" s="12" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C104" s="12" t="s">
         <v>17</v>
@@ -7465,7 +7450,7 @@
         <v>243</v>
       </c>
       <c r="F104" s="12" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G104" s="12" t="s">
         <v>211</v>
@@ -7483,7 +7468,7 @@
         <v>42</v>
       </c>
       <c r="L104" s="12" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="M104" s="52">
         <v>16.82</v>
@@ -7510,39 +7495,39 @@
         <v>75</v>
       </c>
       <c r="U104" s="12" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="105" spans="1:21" s="59" customFormat="1" x14ac:dyDescent="0.3">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="105" spans="1:21" s="59" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A105" s="59">
         <v>2035</v>
       </c>
       <c r="B105" s="59" t="s">
+        <v>337</v>
+      </c>
+      <c r="C105" s="59" t="s">
         <v>338</v>
       </c>
-      <c r="C105" s="59" t="s">
+      <c r="D105" s="59" t="s">
         <v>339</v>
       </c>
-      <c r="D105" s="59" t="s">
+      <c r="F105" s="59" t="s">
         <v>340</v>
       </c>
-      <c r="F105" s="59" t="s">
-        <v>341</v>
-      </c>
       <c r="G105" s="59" t="s">
+        <v>342</v>
+      </c>
+      <c r="H105" s="59" t="s">
         <v>343</v>
       </c>
-      <c r="H105" s="59" t="s">
+      <c r="J105" s="59" t="s">
         <v>344</v>
-      </c>
-      <c r="J105" s="59" t="s">
-        <v>345</v>
       </c>
       <c r="K105" s="60" t="s">
         <v>110</v>
       </c>
       <c r="L105" s="59" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="M105" s="59">
         <v>17.579999999999998</v>
@@ -7569,39 +7554,39 @@
         <v>72</v>
       </c>
     </row>
-    <row r="106" spans="1:21" s="59" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:21" s="59" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A106" s="59">
         <v>2035</v>
       </c>
       <c r="B106" s="59" t="s">
+        <v>375</v>
+      </c>
+      <c r="C106" s="59" t="s">
+        <v>338</v>
+      </c>
+      <c r="D106" s="59" t="s">
+        <v>339</v>
+      </c>
+      <c r="F106" s="59" t="s">
         <v>376</v>
       </c>
-      <c r="C106" s="59" t="s">
-        <v>339</v>
-      </c>
-      <c r="D106" s="59" t="s">
-        <v>340</v>
-      </c>
-      <c r="F106" s="59" t="s">
-        <v>377</v>
-      </c>
       <c r="G106" s="59" t="s">
+        <v>342</v>
+      </c>
+      <c r="H106" s="59" t="s">
         <v>343</v>
-      </c>
-      <c r="H106" s="59" t="s">
-        <v>344</v>
       </c>
       <c r="I106" s="59" t="s">
         <v>11</v>
       </c>
       <c r="J106" s="59" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K106" s="60" t="s">
         <v>110</v>
       </c>
       <c r="L106" s="59" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="M106" s="59">
         <v>16.82</v>
@@ -7628,39 +7613,39 @@
         <v>72</v>
       </c>
       <c r="U106" s="59" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="107" spans="1:21" s="63" customFormat="1" x14ac:dyDescent="0.3">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="107" spans="1:21" s="63" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A107" s="63">
         <v>2035</v>
       </c>
       <c r="B107" s="63" t="s">
+        <v>345</v>
+      </c>
+      <c r="C107" s="64" t="s">
+        <v>338</v>
+      </c>
+      <c r="D107" s="63" t="s">
+        <v>339</v>
+      </c>
+      <c r="F107" s="63" t="s">
         <v>346</v>
       </c>
-      <c r="C107" s="64" t="s">
-        <v>339</v>
-      </c>
-      <c r="D107" s="63" t="s">
-        <v>340</v>
-      </c>
-      <c r="F107" s="63" t="s">
+      <c r="G107" s="63" t="s">
         <v>347</v>
       </c>
-      <c r="G107" s="63" t="s">
+      <c r="H107" s="63" t="s">
         <v>348</v>
       </c>
-      <c r="H107" s="63" t="s">
+      <c r="J107" s="63" t="s">
         <v>349</v>
-      </c>
-      <c r="J107" s="63" t="s">
-        <v>350</v>
       </c>
       <c r="K107" s="65" t="s">
         <v>129</v>
       </c>
       <c r="L107" s="64" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="M107" s="63">
         <v>17.579999999999998</v>
@@ -7687,39 +7672,39 @@
         <v>72</v>
       </c>
     </row>
-    <row r="108" spans="1:21" s="63" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:21" s="63" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A108" s="63">
         <v>2035</v>
       </c>
       <c r="B108" s="63" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C108" s="64" t="s">
+        <v>338</v>
+      </c>
+      <c r="D108" s="63" t="s">
         <v>339</v>
       </c>
-      <c r="D108" s="63" t="s">
-        <v>340</v>
-      </c>
       <c r="F108" s="63" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G108" s="63" t="s">
+        <v>347</v>
+      </c>
+      <c r="H108" s="63" t="s">
         <v>348</v>
-      </c>
-      <c r="H108" s="63" t="s">
-        <v>349</v>
       </c>
       <c r="I108" s="63" t="s">
         <v>11</v>
       </c>
       <c r="J108" s="63" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K108" s="65" t="s">
         <v>129</v>
       </c>
       <c r="L108" s="64" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="M108" s="63">
         <v>16.82</v>
@@ -7746,10 +7731,10 @@
         <v>72</v>
       </c>
       <c r="U108" s="63" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="109" spans="1:21" s="24" customFormat="1" x14ac:dyDescent="0.3">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="109" spans="1:21" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A109" s="24">
         <v>2050</v>
       </c>
@@ -7805,36 +7790,36 @@
         <v>109</v>
       </c>
     </row>
-    <row r="110" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A110" s="54">
         <v>2050</v>
       </c>
       <c r="B110" s="54" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C110" s="54" t="s">
+        <v>338</v>
+      </c>
+      <c r="D110" s="54" t="s">
         <v>339</v>
       </c>
-      <c r="D110" s="54" t="s">
-        <v>340</v>
-      </c>
       <c r="F110" s="54" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G110" s="54" t="s">
+        <v>342</v>
+      </c>
+      <c r="H110" s="53" t="s">
         <v>343</v>
       </c>
-      <c r="H110" s="53" t="s">
+      <c r="J110" s="54" t="s">
         <v>344</v>
-      </c>
-      <c r="J110" s="54" t="s">
-        <v>345</v>
       </c>
       <c r="K110" s="53" t="s">
         <v>16</v>
       </c>
       <c r="L110" s="54" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="M110" s="54">
         <v>19.13</v>
@@ -7861,39 +7846,39 @@
         <v>72</v>
       </c>
     </row>
-    <row r="111" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A111" s="54">
         <v>2050</v>
       </c>
       <c r="B111" s="54" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C111" s="54" t="s">
+        <v>338</v>
+      </c>
+      <c r="D111" s="54" t="s">
         <v>339</v>
       </c>
-      <c r="D111" s="54" t="s">
-        <v>340</v>
-      </c>
       <c r="F111" s="54" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G111" s="54" t="s">
+        <v>342</v>
+      </c>
+      <c r="H111" s="53" t="s">
         <v>343</v>
-      </c>
-      <c r="H111" s="53" t="s">
-        <v>344</v>
       </c>
       <c r="I111" s="54" t="s">
         <v>11</v>
       </c>
       <c r="J111" s="54" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K111" s="53" t="s">
         <v>16</v>
       </c>
       <c r="L111" s="54" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="M111" s="54">
         <v>18.420000000000002</v>
@@ -7920,42 +7905,39 @@
         <v>72</v>
       </c>
       <c r="U111" s="54" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="112" spans="1:21" s="69" customFormat="1" x14ac:dyDescent="0.3">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="112" spans="1:21" s="69" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A112" s="69">
         <v>2050</v>
       </c>
       <c r="B112" s="69" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C112" s="69" t="s">
+        <v>338</v>
+      </c>
+      <c r="D112" s="69" t="s">
         <v>339</v>
       </c>
-      <c r="D112" s="69" t="s">
-        <v>340</v>
-      </c>
       <c r="F112" s="69" t="s">
+        <v>354</v>
+      </c>
+      <c r="G112" s="69" t="s">
+        <v>347</v>
+      </c>
+      <c r="H112" s="70" t="s">
+        <v>348</v>
+      </c>
+      <c r="J112" s="69" t="s">
         <v>355</v>
-      </c>
-      <c r="G112" s="69" t="s">
-        <v>348</v>
-      </c>
-      <c r="H112" s="70" t="s">
-        <v>349</v>
-      </c>
-      <c r="I112" s="69" t="s">
-        <v>11</v>
-      </c>
-      <c r="J112" s="69" t="s">
-        <v>356</v>
       </c>
       <c r="K112" s="70" t="s">
         <v>44</v>
       </c>
       <c r="L112" s="69" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="M112" s="69">
         <v>19.13</v>
@@ -7982,39 +7964,39 @@
         <v>72</v>
       </c>
     </row>
-    <row r="113" spans="1:21" s="69" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:21" s="69" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A113" s="69">
         <v>2050</v>
       </c>
       <c r="B113" s="69" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C113" s="69" t="s">
+        <v>338</v>
+      </c>
+      <c r="D113" s="69" t="s">
         <v>339</v>
       </c>
-      <c r="D113" s="69" t="s">
-        <v>340</v>
-      </c>
       <c r="F113" s="69" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G113" s="69" t="s">
+        <v>347</v>
+      </c>
+      <c r="H113" s="70" t="s">
         <v>348</v>
-      </c>
-      <c r="H113" s="70" t="s">
-        <v>349</v>
       </c>
       <c r="I113" s="69" t="s">
         <v>11</v>
       </c>
       <c r="J113" s="69" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="K113" s="70" t="s">
         <v>44</v>
       </c>
       <c r="L113" s="69" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="M113" s="69">
         <v>18.420000000000002</v>
@@ -8041,7 +8023,7 @@
         <v>72</v>
       </c>
       <c r="U113" s="69" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding round3 DBP runs and making current
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923A236D-8178-4D35-8BFF-76CACFEF60AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FCD9711-7E68-4EBD-A3F4-3A3A9D94052B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4665" yWindow="3690" windowWidth="24150" windowHeight="13290" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
+    <workbookView xWindow="30" yWindow="30" windowWidth="21570" windowHeight="12870" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelRuns" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1227" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1271" uniqueCount="401">
   <si>
     <t>year</t>
   </si>
@@ -1209,6 +1209,54 @@
   </si>
   <si>
     <t>2023_TM160_IPA_50</t>
+  </si>
+  <si>
+    <t>2035_TM160_DBP_NoProject_03</t>
+  </si>
+  <si>
+    <t>Updated landuse/popsyn and small network updates</t>
+  </si>
+  <si>
+    <t>M:\urban_modeling\baus\PBA50Plus\PBA50Plus_2020Validation_HE_BOC_v2</t>
+  </si>
+  <si>
+    <t>2050_TM160_DBP_NoProject_03</t>
+  </si>
+  <si>
+    <t>2050_TM160_DBP_Plan_03</t>
+  </si>
+  <si>
+    <t>2035_TM160_DBP_Plan_03</t>
+  </si>
+  <si>
+    <t>M:\urban_modeling\baus\PBA50Plus\PBA50Plus_InclusionaryZoning_v2</t>
+  </si>
+  <si>
+    <t>PBA50Plus_2020Validation_HE_BOC_v2</t>
+  </si>
+  <si>
+    <t>PBA50Plus_InclusionaryZoning_v2</t>
+  </si>
+  <si>
+    <t>BlueprintNetworks_v17\net_2030_Baseline</t>
+  </si>
+  <si>
+    <t>BlueprintNetworks_v17\net_2050_Blueprint</t>
+  </si>
+  <si>
+    <t>BlueprintNetworks_v17\net_2035_Blueprint</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1206926596430568/f</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1206926596430572/f</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1206926596430570/f</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1206926596430574/f</t>
   </si>
 </sst>
 </file>
@@ -1871,13 +1919,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9564CC59-3725-4FDA-8BF2-0F68CB1B6F5A}">
-  <dimension ref="A1:U113"/>
+  <dimension ref="A1:U117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C67" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C91" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B71" sqref="B71"/>
+      <selection pane="bottomRight" activeCell="K114" sqref="K114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7576,9 +7624,6 @@
       <c r="H106" s="59" t="s">
         <v>343</v>
       </c>
-      <c r="I106" s="59" t="s">
-        <v>11</v>
-      </c>
       <c r="J106" s="59" t="s">
         <v>344</v>
       </c>
@@ -7612,64 +7657,67 @@
       <c r="T106" s="62">
         <v>72</v>
       </c>
-      <c r="U106" s="59" t="s">
+    </row>
+    <row r="107" spans="1:21" s="59" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="59">
+        <v>2035</v>
+      </c>
+      <c r="B107" s="59" t="s">
+        <v>385</v>
+      </c>
+      <c r="C107" s="59" t="s">
+        <v>338</v>
+      </c>
+      <c r="D107" s="59" t="s">
+        <v>339</v>
+      </c>
+      <c r="F107" s="59" t="s">
+        <v>386</v>
+      </c>
+      <c r="G107" s="59" t="s">
+        <v>387</v>
+      </c>
+      <c r="H107" s="59" t="s">
+        <v>392</v>
+      </c>
+      <c r="I107" s="59" t="s">
+        <v>11</v>
+      </c>
+      <c r="J107" s="59" t="s">
+        <v>394</v>
+      </c>
+      <c r="K107" s="60" t="s">
+        <v>110</v>
+      </c>
+      <c r="L107" s="59" t="s">
+        <v>399</v>
+      </c>
+      <c r="M107" s="59">
+        <v>16.82</v>
+      </c>
+      <c r="N107" s="61" t="s">
+        <v>109</v>
+      </c>
+      <c r="O107" s="61" t="s">
+        <v>109</v>
+      </c>
+      <c r="P107" s="59">
+        <v>0.87</v>
+      </c>
+      <c r="Q107" s="59">
+        <v>0.78</v>
+      </c>
+      <c r="R107" s="62">
+        <v>83.3</v>
+      </c>
+      <c r="S107" s="62">
+        <v>0</v>
+      </c>
+      <c r="T107" s="62">
+        <v>72</v>
+      </c>
+      <c r="U107" s="59" t="s">
         <v>361</v>
-      </c>
-    </row>
-    <row r="107" spans="1:21" s="63" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="63">
-        <v>2035</v>
-      </c>
-      <c r="B107" s="63" t="s">
-        <v>345</v>
-      </c>
-      <c r="C107" s="64" t="s">
-        <v>338</v>
-      </c>
-      <c r="D107" s="63" t="s">
-        <v>339</v>
-      </c>
-      <c r="F107" s="63" t="s">
-        <v>346</v>
-      </c>
-      <c r="G107" s="63" t="s">
-        <v>347</v>
-      </c>
-      <c r="H107" s="63" t="s">
-        <v>348</v>
-      </c>
-      <c r="J107" s="63" t="s">
-        <v>349</v>
-      </c>
-      <c r="K107" s="65" t="s">
-        <v>129</v>
-      </c>
-      <c r="L107" s="64" t="s">
-        <v>350</v>
-      </c>
-      <c r="M107" s="63">
-        <v>17.579999999999998</v>
-      </c>
-      <c r="N107" s="66" t="s">
-        <v>109</v>
-      </c>
-      <c r="O107" s="66" t="s">
-        <v>109</v>
-      </c>
-      <c r="P107" s="63">
-        <v>0.87</v>
-      </c>
-      <c r="Q107" s="63">
-        <v>0.78</v>
-      </c>
-      <c r="R107" s="67">
-        <v>83.3</v>
-      </c>
-      <c r="S107" s="67">
-        <v>0</v>
-      </c>
-      <c r="T107" s="67">
-        <v>72</v>
       </c>
     </row>
     <row r="108" spans="1:21" s="63" customFormat="1" x14ac:dyDescent="0.2">
@@ -7677,7 +7725,7 @@
         <v>2035</v>
       </c>
       <c r="B108" s="63" t="s">
-        <v>378</v>
+        <v>345</v>
       </c>
       <c r="C108" s="64" t="s">
         <v>338</v>
@@ -7686,7 +7734,7 @@
         <v>339</v>
       </c>
       <c r="F108" s="63" t="s">
-        <v>376</v>
+        <v>346</v>
       </c>
       <c r="G108" s="63" t="s">
         <v>347</v>
@@ -7694,9 +7742,6 @@
       <c r="H108" s="63" t="s">
         <v>348</v>
       </c>
-      <c r="I108" s="63" t="s">
-        <v>11</v>
-      </c>
       <c r="J108" s="63" t="s">
         <v>349</v>
       </c>
@@ -7704,10 +7749,10 @@
         <v>129</v>
       </c>
       <c r="L108" s="64" t="s">
-        <v>379</v>
+        <v>350</v>
       </c>
       <c r="M108" s="63">
-        <v>16.82</v>
+        <v>17.579999999999998</v>
       </c>
       <c r="N108" s="66" t="s">
         <v>109</v>
@@ -7730,299 +7775,526 @@
       <c r="T108" s="67">
         <v>72</v>
       </c>
-      <c r="U108" s="63" t="s">
+    </row>
+    <row r="109" spans="1:21" s="63" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="63">
+        <v>2035</v>
+      </c>
+      <c r="B109" s="63" t="s">
+        <v>378</v>
+      </c>
+      <c r="C109" s="64" t="s">
+        <v>338</v>
+      </c>
+      <c r="D109" s="63" t="s">
+        <v>339</v>
+      </c>
+      <c r="F109" s="63" t="s">
+        <v>376</v>
+      </c>
+      <c r="G109" s="63" t="s">
+        <v>347</v>
+      </c>
+      <c r="H109" s="63" t="s">
+        <v>348</v>
+      </c>
+      <c r="J109" s="63" t="s">
+        <v>349</v>
+      </c>
+      <c r="K109" s="65" t="s">
+        <v>129</v>
+      </c>
+      <c r="L109" s="64" t="s">
+        <v>379</v>
+      </c>
+      <c r="M109" s="63">
+        <v>16.82</v>
+      </c>
+      <c r="N109" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="O109" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="P109" s="63">
+        <v>0.87</v>
+      </c>
+      <c r="Q109" s="63">
+        <v>0.78</v>
+      </c>
+      <c r="R109" s="67">
+        <v>83.3</v>
+      </c>
+      <c r="S109" s="67">
+        <v>0</v>
+      </c>
+      <c r="T109" s="67">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="110" spans="1:21" s="63" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="63">
+        <v>2035</v>
+      </c>
+      <c r="B110" s="63" t="s">
+        <v>390</v>
+      </c>
+      <c r="C110" s="64" t="s">
+        <v>338</v>
+      </c>
+      <c r="D110" s="63" t="s">
+        <v>339</v>
+      </c>
+      <c r="F110" s="63" t="s">
+        <v>386</v>
+      </c>
+      <c r="G110" s="63" t="s">
+        <v>391</v>
+      </c>
+      <c r="H110" s="63" t="s">
+        <v>393</v>
+      </c>
+      <c r="I110" s="63" t="s">
+        <v>11</v>
+      </c>
+      <c r="J110" s="63" t="s">
+        <v>396</v>
+      </c>
+      <c r="K110" s="65" t="s">
+        <v>129</v>
+      </c>
+      <c r="L110" s="64" t="s">
+        <v>397</v>
+      </c>
+      <c r="M110" s="63">
+        <v>16.82</v>
+      </c>
+      <c r="N110" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="O110" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="P110" s="63">
+        <v>0.87</v>
+      </c>
+      <c r="Q110" s="63">
+        <v>0.78</v>
+      </c>
+      <c r="R110" s="67">
+        <v>83.3</v>
+      </c>
+      <c r="S110" s="67">
+        <v>0</v>
+      </c>
+      <c r="T110" s="67">
+        <v>72</v>
+      </c>
+      <c r="U110" s="63" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="109" spans="1:21" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="24">
+    <row r="111" spans="1:21" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="24">
         <v>2050</v>
       </c>
-      <c r="B109" s="24" t="s">
+      <c r="B111" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="C109" s="24" t="s">
+      <c r="C111" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="D109" s="24" t="s">
+      <c r="D111" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="F109" s="24" t="s">
+      <c r="F111" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="G109" s="24" t="s">
+      <c r="G111" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="H109" s="25" t="s">
+      <c r="H111" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="J109" s="24" t="s">
+      <c r="J111" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="K109" s="26" t="s">
+      <c r="K111" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="L109" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="M109" s="24">
+      <c r="L111" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="M111" s="24">
         <v>17.440000000000001</v>
       </c>
-      <c r="N109" s="47">
+      <c r="N111" s="47">
         <v>-0.33</v>
       </c>
-      <c r="O109" s="47">
-        <v>0</v>
-      </c>
-      <c r="P109" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q109" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="R109" s="73" t="s">
-        <v>109</v>
-      </c>
-      <c r="S109" s="73" t="s">
-        <v>109</v>
-      </c>
-      <c r="T109" s="73" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="110" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="54">
+      <c r="O111" s="47">
+        <v>0</v>
+      </c>
+      <c r="P111" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q111" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="R111" s="73" t="s">
+        <v>109</v>
+      </c>
+      <c r="S111" s="73" t="s">
+        <v>109</v>
+      </c>
+      <c r="T111" s="73" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="112" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="54">
         <v>2050</v>
       </c>
-      <c r="B110" s="54" t="s">
+      <c r="B112" s="54" t="s">
         <v>351</v>
       </c>
-      <c r="C110" s="54" t="s">
+      <c r="C112" s="54" t="s">
         <v>338</v>
       </c>
-      <c r="D110" s="54" t="s">
+      <c r="D112" s="54" t="s">
         <v>339</v>
       </c>
-      <c r="F110" s="54" t="s">
+      <c r="F112" s="54" t="s">
         <v>353</v>
       </c>
-      <c r="G110" s="54" t="s">
+      <c r="G112" s="54" t="s">
         <v>342</v>
       </c>
-      <c r="H110" s="53" t="s">
+      <c r="H112" s="53" t="s">
         <v>343</v>
       </c>
-      <c r="J110" s="54" t="s">
+      <c r="J112" s="54" t="s">
         <v>344</v>
       </c>
-      <c r="K110" s="53" t="s">
+      <c r="K112" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="L110" s="54" t="s">
+      <c r="L112" s="54" t="s">
         <v>356</v>
       </c>
-      <c r="M110" s="54">
+      <c r="M112" s="54">
         <v>19.13</v>
       </c>
-      <c r="N110" s="68" t="s">
-        <v>109</v>
-      </c>
-      <c r="O110" s="68" t="s">
-        <v>109</v>
-      </c>
-      <c r="P110" s="54">
+      <c r="N112" s="68" t="s">
+        <v>109</v>
+      </c>
+      <c r="O112" s="68" t="s">
+        <v>109</v>
+      </c>
+      <c r="P112" s="54">
         <v>0.87</v>
       </c>
-      <c r="Q110" s="54">
+      <c r="Q112" s="54">
         <v>0.78</v>
       </c>
-      <c r="R110" s="57">
+      <c r="R112" s="57">
         <v>83.3</v>
       </c>
-      <c r="S110" s="57">
-        <v>0</v>
-      </c>
-      <c r="T110" s="57">
+      <c r="S112" s="57">
+        <v>0</v>
+      </c>
+      <c r="T112" s="57">
         <v>72</v>
       </c>
     </row>
-    <row r="111" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="54">
+    <row r="113" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="54">
         <v>2050</v>
       </c>
-      <c r="B111" s="54" t="s">
+      <c r="B113" s="54" t="s">
         <v>380</v>
       </c>
-      <c r="C111" s="54" t="s">
+      <c r="C113" s="54" t="s">
         <v>338</v>
       </c>
-      <c r="D111" s="54" t="s">
+      <c r="D113" s="54" t="s">
         <v>339</v>
       </c>
-      <c r="F111" s="54" t="s">
+      <c r="F113" s="54" t="s">
         <v>376</v>
       </c>
-      <c r="G111" s="54" t="s">
+      <c r="G113" s="54" t="s">
         <v>342</v>
       </c>
-      <c r="H111" s="53" t="s">
+      <c r="H113" s="53" t="s">
         <v>343</v>
       </c>
-      <c r="I111" s="54" t="s">
+      <c r="J113" s="54" t="s">
+        <v>344</v>
+      </c>
+      <c r="K113" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="L113" s="54" t="s">
+        <v>381</v>
+      </c>
+      <c r="M113" s="54">
+        <v>18.420000000000002</v>
+      </c>
+      <c r="N113" s="68" t="s">
+        <v>109</v>
+      </c>
+      <c r="O113" s="68" t="s">
+        <v>109</v>
+      </c>
+      <c r="P113" s="54">
+        <v>0.87</v>
+      </c>
+      <c r="Q113" s="54">
+        <v>0.78</v>
+      </c>
+      <c r="R113" s="57">
+        <v>83.3</v>
+      </c>
+      <c r="S113" s="57">
+        <v>0</v>
+      </c>
+      <c r="T113" s="57">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="114" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="54">
+        <v>2050</v>
+      </c>
+      <c r="B114" s="54" t="s">
+        <v>388</v>
+      </c>
+      <c r="C114" s="54" t="s">
+        <v>338</v>
+      </c>
+      <c r="D114" s="54" t="s">
+        <v>339</v>
+      </c>
+      <c r="F114" s="54" t="s">
+        <v>386</v>
+      </c>
+      <c r="G114" s="54" t="s">
+        <v>387</v>
+      </c>
+      <c r="H114" s="53" t="s">
+        <v>392</v>
+      </c>
+      <c r="I114" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="J111" s="54" t="s">
-        <v>344</v>
-      </c>
-      <c r="K111" s="53" t="s">
+      <c r="J114" s="54" t="s">
+        <v>394</v>
+      </c>
+      <c r="K114" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="L111" s="54" t="s">
-        <v>381</v>
-      </c>
-      <c r="M111" s="54">
+      <c r="L114" s="54" t="s">
+        <v>400</v>
+      </c>
+      <c r="M114" s="54">
         <v>18.420000000000002</v>
       </c>
-      <c r="N111" s="68" t="s">
-        <v>109</v>
-      </c>
-      <c r="O111" s="68" t="s">
-        <v>109</v>
-      </c>
-      <c r="P111" s="54">
+      <c r="N114" s="68" t="s">
+        <v>109</v>
+      </c>
+      <c r="O114" s="68" t="s">
+        <v>109</v>
+      </c>
+      <c r="P114" s="54">
         <v>0.87</v>
       </c>
-      <c r="Q111" s="54">
+      <c r="Q114" s="54">
         <v>0.78</v>
       </c>
-      <c r="R111" s="57">
+      <c r="R114" s="57">
         <v>83.3</v>
       </c>
-      <c r="S111" s="57">
-        <v>0</v>
-      </c>
-      <c r="T111" s="57">
+      <c r="S114" s="57">
+        <v>0</v>
+      </c>
+      <c r="T114" s="57">
         <v>72</v>
       </c>
-      <c r="U111" s="54" t="s">
+      <c r="U114" s="54" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="112" spans="1:21" s="69" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="69">
+    <row r="115" spans="1:21" s="69" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="69">
         <v>2050</v>
       </c>
-      <c r="B112" s="69" t="s">
+      <c r="B115" s="69" t="s">
         <v>352</v>
       </c>
-      <c r="C112" s="69" t="s">
+      <c r="C115" s="69" t="s">
         <v>338</v>
       </c>
-      <c r="D112" s="69" t="s">
+      <c r="D115" s="69" t="s">
         <v>339</v>
       </c>
-      <c r="F112" s="69" t="s">
+      <c r="F115" s="69" t="s">
         <v>354</v>
       </c>
-      <c r="G112" s="69" t="s">
+      <c r="G115" s="69" t="s">
         <v>347</v>
       </c>
-      <c r="H112" s="70" t="s">
+      <c r="H115" s="70" t="s">
         <v>348</v>
       </c>
-      <c r="J112" s="69" t="s">
+      <c r="J115" s="69" t="s">
         <v>355</v>
       </c>
-      <c r="K112" s="70" t="s">
+      <c r="K115" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="L112" s="69" t="s">
+      <c r="L115" s="69" t="s">
         <v>357</v>
       </c>
-      <c r="M112" s="69">
+      <c r="M115" s="69">
         <v>19.13</v>
       </c>
-      <c r="N112" s="71" t="s">
-        <v>109</v>
-      </c>
-      <c r="O112" s="71" t="s">
-        <v>109</v>
-      </c>
-      <c r="P112" s="69">
+      <c r="N115" s="71" t="s">
+        <v>109</v>
+      </c>
+      <c r="O115" s="71" t="s">
+        <v>109</v>
+      </c>
+      <c r="P115" s="69">
         <v>0.87</v>
       </c>
-      <c r="Q112" s="69">
+      <c r="Q115" s="69">
         <v>0.78</v>
       </c>
-      <c r="R112" s="72">
+      <c r="R115" s="72">
         <v>83.3</v>
       </c>
-      <c r="S112" s="72">
-        <v>0</v>
-      </c>
-      <c r="T112" s="72">
+      <c r="S115" s="72">
+        <v>0</v>
+      </c>
+      <c r="T115" s="72">
         <v>72</v>
       </c>
     </row>
-    <row r="113" spans="1:21" s="69" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="69">
+    <row r="116" spans="1:21" s="69" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="69">
         <v>2050</v>
       </c>
-      <c r="B113" s="69" t="s">
+      <c r="B116" s="69" t="s">
         <v>382</v>
       </c>
-      <c r="C113" s="69" t="s">
+      <c r="C116" s="69" t="s">
         <v>338</v>
       </c>
-      <c r="D113" s="69" t="s">
+      <c r="D116" s="69" t="s">
         <v>339</v>
       </c>
-      <c r="F113" s="69" t="s">
+      <c r="F116" s="69" t="s">
         <v>354</v>
       </c>
-      <c r="G113" s="69" t="s">
+      <c r="G116" s="69" t="s">
         <v>347</v>
       </c>
-      <c r="H113" s="70" t="s">
+      <c r="H116" s="70" t="s">
         <v>348</v>
       </c>
-      <c r="I113" s="69" t="s">
+      <c r="J116" s="69" t="s">
+        <v>355</v>
+      </c>
+      <c r="K116" s="70" t="s">
+        <v>44</v>
+      </c>
+      <c r="L116" s="69" t="s">
+        <v>357</v>
+      </c>
+      <c r="M116" s="69">
+        <v>18.420000000000002</v>
+      </c>
+      <c r="N116" s="71" t="s">
+        <v>109</v>
+      </c>
+      <c r="O116" s="71" t="s">
+        <v>109</v>
+      </c>
+      <c r="P116" s="69">
+        <v>0.87</v>
+      </c>
+      <c r="Q116" s="69">
+        <v>0.78</v>
+      </c>
+      <c r="R116" s="72">
+        <v>83.3</v>
+      </c>
+      <c r="S116" s="72">
+        <v>0</v>
+      </c>
+      <c r="T116" s="72">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="117" spans="1:21" s="69" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="69">
+        <v>2050</v>
+      </c>
+      <c r="B117" s="69" t="s">
+        <v>389</v>
+      </c>
+      <c r="C117" s="69" t="s">
+        <v>338</v>
+      </c>
+      <c r="D117" s="69" t="s">
+        <v>339</v>
+      </c>
+      <c r="F117" s="69" t="s">
+        <v>386</v>
+      </c>
+      <c r="G117" s="69" t="s">
+        <v>391</v>
+      </c>
+      <c r="H117" s="70" t="s">
+        <v>393</v>
+      </c>
+      <c r="I117" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="J113" s="69" t="s">
-        <v>355</v>
-      </c>
-      <c r="K113" s="70" t="s">
+      <c r="J117" s="69" t="s">
+        <v>395</v>
+      </c>
+      <c r="K117" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="L113" s="69" t="s">
-        <v>357</v>
-      </c>
-      <c r="M113" s="69">
+      <c r="L117" s="69" t="s">
+        <v>398</v>
+      </c>
+      <c r="M117" s="69">
         <v>18.420000000000002</v>
       </c>
-      <c r="N113" s="71" t="s">
-        <v>109</v>
-      </c>
-      <c r="O113" s="71" t="s">
-        <v>109</v>
-      </c>
-      <c r="P113" s="69">
+      <c r="N117" s="71" t="s">
+        <v>109</v>
+      </c>
+      <c r="O117" s="71" t="s">
+        <v>109</v>
+      </c>
+      <c r="P117" s="69">
         <v>0.87</v>
       </c>
-      <c r="Q113" s="69">
+      <c r="Q117" s="69">
         <v>0.78</v>
       </c>
-      <c r="R113" s="72">
+      <c r="R117" s="72">
         <v>83.3</v>
       </c>
-      <c r="S113" s="72">
-        <v>0</v>
-      </c>
-      <c r="T113" s="72">
+      <c r="S117" s="72">
+        <v>0</v>
+      </c>
+      <c r="T117" s="72">
         <v>72</v>
       </c>
-      <c r="U113" s="69" t="s">
+      <c r="U117" s="69" t="s">
         <v>358</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding an old TM152 2023 run
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\config_RTP2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one-master\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FCD9711-7E68-4EBD-A3F4-3A3A9D94052B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11106E5B-DFEC-4D97-A2F2-8CF51D1E5D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="30" windowWidth="21570" windowHeight="12870" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelRuns" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1271" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1277" uniqueCount="405">
   <si>
     <t>year</t>
   </si>
@@ -1257,6 +1257,18 @@
   </si>
   <si>
     <t>https://app.asana.com/0/1204085012544660/1206926596430574/f</t>
+  </si>
+  <si>
+    <t>2023_TM152_FBP_Plus_22</t>
+  </si>
+  <si>
+    <t>External_requests\SACOG_Air_Quality_Plan</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/310827677834656/1201494979354388/f</t>
+  </si>
+  <si>
+    <t>ext_req</t>
   </si>
 </sst>
 </file>
@@ -1435,7 +1447,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1591,6 +1603,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1919,35 +1932,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9564CC59-3725-4FDA-8BF2-0F68CB1B6F5A}">
-  <dimension ref="A1:U117"/>
+  <dimension ref="A1:U118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C91" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K114" sqref="K114"/>
+      <selection pane="bottomRight" activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="42.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.54296875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="42.26953125" style="1" customWidth="1"/>
     <col min="7" max="7" width="23" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.28515625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" style="10" customWidth="1"/>
-    <col min="12" max="12" width="17.5703125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="8.28515625" style="1" customWidth="1"/>
-    <col min="14" max="15" width="9.28515625" style="43"/>
-    <col min="16" max="16384" width="9.28515625" style="1"/>
+    <col min="8" max="8" width="8.26953125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="6.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.26953125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11.26953125" style="10" customWidth="1"/>
+    <col min="12" max="12" width="17.54296875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="8.26953125" style="1" customWidth="1"/>
+    <col min="14" max="15" width="9.26953125" style="43"/>
+    <col min="16" max="16384" width="9.26953125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="5" customFormat="1" ht="39" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2012,7 +2025,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19">
         <v>2005</v>
       </c>
@@ -2065,7 +2078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="30">
         <v>2005</v>
       </c>
@@ -2121,7 +2134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30">
         <v>2005</v>
       </c>
@@ -2176,7 +2189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:21" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="30">
         <v>2005</v>
       </c>
@@ -2231,7 +2244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:21" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="30">
         <v>2005</v>
       </c>
@@ -2290,7 +2303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="53">
         <v>2015</v>
       </c>
@@ -2331,7 +2344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="34">
         <v>2015</v>
       </c>
@@ -2377,7 +2390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="34">
         <v>2015</v>
       </c>
@@ -2430,7 +2443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="34">
         <v>2015</v>
       </c>
@@ -2483,7 +2496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="34">
         <v>2015</v>
       </c>
@@ -2536,7 +2549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="34">
         <v>2015</v>
       </c>
@@ -2592,7 +2605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="34">
         <v>2015</v>
       </c>
@@ -2648,7 +2661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="34">
         <v>2015</v>
       </c>
@@ -2704,7 +2717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="34">
         <v>2015</v>
       </c>
@@ -2764,7 +2777,7 @@
       </c>
       <c r="U15" s="58"/>
     </row>
-    <row r="16" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="34">
         <v>2015</v>
       </c>
@@ -2826,7 +2839,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>2023</v>
       </c>
@@ -2872,7 +2885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>2023</v>
       </c>
@@ -2918,7 +2931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>2023</v>
       </c>
@@ -2964,7 +2977,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>2023</v>
       </c>
@@ -3010,7 +3023,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>2023</v>
       </c>
@@ -3056,7 +3069,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>2023</v>
       </c>
@@ -3102,7 +3115,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>2023</v>
       </c>
@@ -3148,7 +3161,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>2023</v>
       </c>
@@ -3194,7 +3207,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>2023</v>
       </c>
@@ -3240,7 +3253,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>2023</v>
       </c>
@@ -3286,7 +3299,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>2023</v>
       </c>
@@ -3332,7 +3345,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>2023</v>
       </c>
@@ -3378,7 +3391,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>2023</v>
       </c>
@@ -3424,7 +3437,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>2023</v>
       </c>
@@ -3470,7 +3483,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>2023</v>
       </c>
@@ -3516,7 +3529,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>2023</v>
       </c>
@@ -3562,7 +3575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>2023</v>
       </c>
@@ -3608,7 +3621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>2023</v>
       </c>
@@ -3654,7 +3667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>2023</v>
       </c>
@@ -3698,7 +3711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>2023</v>
       </c>
@@ -3747,7 +3760,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>2023</v>
       </c>
@@ -3794,7 +3807,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>2023</v>
       </c>
@@ -3841,7 +3854,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>2023</v>
       </c>
@@ -3897,7 +3910,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>2023</v>
       </c>
@@ -3953,7 +3966,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>2023</v>
       </c>
@@ -4009,7 +4022,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>2023</v>
       </c>
@@ -4065,7 +4078,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>2023</v>
       </c>
@@ -4121,7 +4134,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>2023</v>
       </c>
@@ -4177,7 +4190,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>2023</v>
       </c>
@@ -4233,7 +4246,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>2023</v>
       </c>
@@ -4289,7 +4302,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>2023</v>
       </c>
@@ -4345,7 +4358,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>2023</v>
       </c>
@@ -4401,7 +4414,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>2023</v>
       </c>
@@ -4457,7 +4470,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>2023</v>
       </c>
@@ -4513,7 +4526,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>2023</v>
       </c>
@@ -4569,7 +4582,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>2023</v>
       </c>
@@ -4625,7 +4638,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>2023</v>
       </c>
@@ -4681,7 +4694,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>2023</v>
       </c>
@@ -4737,7 +4750,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>2023</v>
       </c>
@@ -4793,7 +4806,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>2023</v>
       </c>
@@ -4849,7 +4862,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>2023</v>
       </c>
@@ -4905,7 +4918,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>2023</v>
       </c>
@@ -4961,7 +4974,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>2023</v>
       </c>
@@ -5017,7 +5030,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>2023</v>
       </c>
@@ -5073,7 +5086,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>2023</v>
       </c>
@@ -5129,7 +5142,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>2023</v>
       </c>
@@ -5185,7 +5198,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>2023</v>
       </c>
@@ -5241,7 +5254,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>2023</v>
       </c>
@@ -5300,7 +5313,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>2023</v>
       </c>
@@ -5356,7 +5369,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>2023</v>
       </c>
@@ -5415,7 +5428,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>2023</v>
       </c>
@@ -5474,7 +5487,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>2023</v>
       </c>
@@ -5533,7 +5546,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>2023</v>
       </c>
@@ -5592,7 +5605,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="70" spans="1:21" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:21" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>2023</v>
       </c>
@@ -5648,7 +5661,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="71" spans="1:21" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:21" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>2023</v>
       </c>
@@ -5704,7 +5717,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>2023</v>
       </c>
@@ -5760,7 +5773,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>2023</v>
       </c>
@@ -5816,7 +5829,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>2023</v>
       </c>
@@ -5872,7 +5885,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>2023</v>
       </c>
@@ -5931,7 +5944,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>2023</v>
       </c>
@@ -5991,7 +6004,7 @@
       </c>
       <c r="U76" s="74"/>
     </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>2023</v>
       </c>
@@ -6053,155 +6066,128 @@
         <v>360</v>
       </c>
     </row>
-    <row r="78" spans="1:21" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:21" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="27">
-        <v>2025</v>
+        <v>2023</v>
       </c>
       <c r="B78" s="27" t="s">
-        <v>130</v>
+        <v>401</v>
       </c>
       <c r="C78" s="27" t="s">
-        <v>113</v>
+        <v>404</v>
       </c>
       <c r="D78" s="27" t="s">
         <v>244</v>
       </c>
       <c r="F78" s="27" t="s">
-        <v>131</v>
+        <v>402</v>
       </c>
       <c r="J78" s="27" t="s">
         <v>132</v>
       </c>
       <c r="K78" s="28" t="s">
         <v>16</v>
+      </c>
+      <c r="L78" s="27" t="s">
+        <v>403</v>
       </c>
       <c r="N78" s="44"/>
       <c r="O78" s="44"/>
       <c r="R78" s="29"/>
       <c r="S78" s="29"/>
       <c r="T78" s="29"/>
-    </row>
-    <row r="79" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="15">
+      <c r="U78" s="75"/>
+    </row>
+    <row r="79" spans="1:21" s="27" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="27">
+        <v>2025</v>
+      </c>
+      <c r="B79" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="C79" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="D79" s="27" t="s">
+        <v>244</v>
+      </c>
+      <c r="F79" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="K79" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="N79" s="44"/>
+      <c r="O79" s="44"/>
+      <c r="R79" s="29"/>
+      <c r="S79" s="29"/>
+      <c r="T79" s="29"/>
+    </row>
+    <row r="80" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="15">
         <v>2035</v>
       </c>
-      <c r="B79" s="15" t="s">
+      <c r="B80" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="C79" s="15" t="s">
+      <c r="C80" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="D79" s="15" t="s">
+      <c r="D80" s="15" t="s">
         <v>244</v>
       </c>
-      <c r="F79" s="15" t="s">
+      <c r="F80" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="G79" s="15" t="s">
+      <c r="G80" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="H79" s="18" t="s">
+      <c r="H80" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="I79" s="15" t="s">
+      <c r="I80" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="J79" s="15" t="s">
+      <c r="J80" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="K79" s="16" t="s">
+      <c r="K80" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="L79" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="M79" s="15">
+      <c r="L80" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="M80" s="15">
         <v>15.85</v>
       </c>
-      <c r="N79" s="45">
+      <c r="N80" s="45">
         <v>-0.27</v>
       </c>
-      <c r="O79" s="45">
-        <v>0</v>
-      </c>
-      <c r="P79" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q79" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="R79" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="S79" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="T79" s="17" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="80" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="12">
-        <v>2035</v>
-      </c>
-      <c r="B80" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="C80" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D80" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="F80" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="G80" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="H80" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="J80" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="K80" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="L80" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="M80" s="12">
-        <v>15.85</v>
-      </c>
-      <c r="N80" s="46" t="s">
-        <v>109</v>
-      </c>
-      <c r="O80" s="46" t="s">
-        <v>109</v>
-      </c>
-      <c r="P80" s="14">
-        <v>1.27</v>
-      </c>
-      <c r="Q80" s="14">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="R80" s="14">
-        <v>120</v>
-      </c>
-      <c r="S80" s="14">
-        <v>0</v>
-      </c>
-      <c r="T80" s="14">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="81" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O80" s="45">
+        <v>0</v>
+      </c>
+      <c r="P80" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q80" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="R80" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="S80" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="T80" s="17" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="81" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="12">
         <v>2035</v>
       </c>
       <c r="B81" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C81" s="12" t="s">
         <v>17</v>
@@ -6210,7 +6196,7 @@
         <v>243</v>
       </c>
       <c r="F81" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G81" s="12" t="s">
         <v>9</v>
@@ -6222,13 +6208,13 @@
         <v>103</v>
       </c>
       <c r="K81" s="13" t="s">
-        <v>108</v>
+        <v>43</v>
       </c>
       <c r="L81" s="12" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="M81" s="12">
-        <v>18.64</v>
+        <v>15.85</v>
       </c>
       <c r="N81" s="46" t="s">
         <v>109</v>
@@ -6252,12 +6238,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="82" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="12">
         <v>2035</v>
       </c>
       <c r="B82" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C82" s="12" t="s">
         <v>17</v>
@@ -6266,7 +6252,7 @@
         <v>243</v>
       </c>
       <c r="F82" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G82" s="12" t="s">
         <v>9</v>
@@ -6278,10 +6264,10 @@
         <v>103</v>
       </c>
       <c r="K82" s="13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L82" s="12" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="M82" s="12">
         <v>18.64</v>
@@ -6299,21 +6285,21 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="R82" s="14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="S82" s="14">
         <v>0</v>
       </c>
       <c r="T82" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="83" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="12">
         <v>2035</v>
       </c>
       <c r="B83" s="12" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="C83" s="12" t="s">
         <v>17</v>
@@ -6322,7 +6308,7 @@
         <v>243</v>
       </c>
       <c r="F83" s="12" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="G83" s="12" t="s">
         <v>9</v>
@@ -6334,10 +6320,10 @@
         <v>103</v>
       </c>
       <c r="K83" s="13" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="L83" s="12" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="M83" s="12">
         <v>18.64</v>
@@ -6348,28 +6334,28 @@
       <c r="O83" s="46" t="s">
         <v>109</v>
       </c>
-      <c r="P83" s="12">
-        <v>0.95</v>
-      </c>
-      <c r="Q83" s="12">
-        <v>0.86</v>
+      <c r="P83" s="14">
+        <v>1.27</v>
+      </c>
+      <c r="Q83" s="14">
+        <v>1.1499999999999999</v>
       </c>
       <c r="R83" s="14">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="S83" s="14">
         <v>0</v>
       </c>
       <c r="T83" s="14">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="84" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A84" s="12">
         <v>2035</v>
       </c>
       <c r="B84" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C84" s="12" t="s">
         <v>17</v>
@@ -6378,7 +6364,7 @@
         <v>243</v>
       </c>
       <c r="F84" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G84" s="12" t="s">
         <v>9</v>
@@ -6390,10 +6376,10 @@
         <v>103</v>
       </c>
       <c r="K84" s="13" t="s">
-        <v>42</v>
+        <v>108</v>
       </c>
       <c r="L84" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="M84" s="12">
         <v>18.64</v>
@@ -6411,21 +6397,21 @@
         <v>0.86</v>
       </c>
       <c r="R84" s="14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="S84" s="14">
         <v>0</v>
       </c>
       <c r="T84" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="85" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="12">
         <v>2035</v>
       </c>
       <c r="B85" s="12" t="s">
-        <v>184</v>
+        <v>120</v>
       </c>
       <c r="C85" s="12" t="s">
         <v>17</v>
@@ -6434,7 +6420,7 @@
         <v>243</v>
       </c>
       <c r="F85" s="12" t="s">
-        <v>209</v>
+        <v>122</v>
       </c>
       <c r="G85" s="12" t="s">
         <v>9</v>
@@ -6446,10 +6432,10 @@
         <v>103</v>
       </c>
       <c r="K85" s="13" t="s">
-        <v>108</v>
+        <v>42</v>
       </c>
       <c r="L85" s="12" t="s">
-        <v>186</v>
+        <v>123</v>
       </c>
       <c r="M85" s="12">
         <v>18.64</v>
@@ -6476,12 +6462,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" s="12">
         <v>2035</v>
       </c>
       <c r="B86" s="12" t="s">
-        <v>207</v>
+        <v>184</v>
       </c>
       <c r="C86" s="12" t="s">
         <v>17</v>
@@ -6490,7 +6476,7 @@
         <v>243</v>
       </c>
       <c r="F86" s="12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G86" s="12" t="s">
         <v>9</v>
@@ -6502,7 +6488,7 @@
         <v>103</v>
       </c>
       <c r="K86" s="13" t="s">
-        <v>44</v>
+        <v>108</v>
       </c>
       <c r="L86" s="12" t="s">
         <v>186</v>
@@ -6532,12 +6518,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" s="12">
         <v>2035</v>
       </c>
       <c r="B87" s="12" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C87" s="12" t="s">
         <v>17</v>
@@ -6546,13 +6532,13 @@
         <v>243</v>
       </c>
       <c r="F87" s="12" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="G87" s="12" t="s">
-        <v>211</v>
+        <v>9</v>
       </c>
       <c r="H87" s="12" t="s">
-        <v>116</v>
+        <v>10</v>
       </c>
       <c r="J87" s="12" t="s">
         <v>103</v>
@@ -6561,7 +6547,7 @@
         <v>44</v>
       </c>
       <c r="L87" s="12" t="s">
-        <v>212</v>
+        <v>186</v>
       </c>
       <c r="M87" s="12">
         <v>18.64</v>
@@ -6579,21 +6565,21 @@
         <v>0.86</v>
       </c>
       <c r="R87" s="14">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="S87" s="14">
         <v>0</v>
       </c>
       <c r="T87" s="14">
-        <v>41.25</v>
-      </c>
-    </row>
-    <row r="88" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="12">
         <v>2035</v>
       </c>
       <c r="B88" s="12" t="s">
-        <v>228</v>
+        <v>206</v>
       </c>
       <c r="C88" s="12" t="s">
         <v>17</v>
@@ -6602,7 +6588,7 @@
         <v>243</v>
       </c>
       <c r="F88" s="12" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
       <c r="G88" s="12" t="s">
         <v>211</v>
@@ -6614,13 +6600,13 @@
         <v>103</v>
       </c>
       <c r="K88" s="13" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L88" s="12" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="M88" s="12">
-        <v>20.55</v>
+        <v>18.64</v>
       </c>
       <c r="N88" s="46" t="s">
         <v>109</v>
@@ -6629,10 +6615,10 @@
         <v>109</v>
       </c>
       <c r="P88" s="12">
-        <v>0.99</v>
+        <v>0.95</v>
       </c>
       <c r="Q88" s="12">
-        <v>0.89</v>
+        <v>0.86</v>
       </c>
       <c r="R88" s="14">
         <v>100</v>
@@ -6641,15 +6627,15 @@
         <v>0</v>
       </c>
       <c r="T88" s="14">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="89" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>41.25</v>
+      </c>
+    </row>
+    <row r="89" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="12">
         <v>2035</v>
       </c>
       <c r="B89" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C89" s="12" t="s">
         <v>17</v>
@@ -6658,7 +6644,7 @@
         <v>243</v>
       </c>
       <c r="F89" s="12" t="s">
-        <v>269</v>
+        <v>226</v>
       </c>
       <c r="G89" s="12" t="s">
         <v>211</v>
@@ -6670,10 +6656,10 @@
         <v>103</v>
       </c>
       <c r="K89" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L89" s="12" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="M89" s="12">
         <v>20.55</v>
@@ -6700,12 +6686,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="90" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90" s="12">
         <v>2035</v>
       </c>
       <c r="B90" s="12" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C90" s="12" t="s">
         <v>17</v>
@@ -6714,22 +6700,22 @@
         <v>243</v>
       </c>
       <c r="F90" s="12" t="s">
-        <v>270</v>
-      </c>
-      <c r="G90" s="52" t="s">
-        <v>232</v>
+        <v>269</v>
+      </c>
+      <c r="G90" s="12" t="s">
+        <v>211</v>
       </c>
       <c r="H90" s="12" t="s">
-        <v>233</v>
+        <v>116</v>
       </c>
       <c r="J90" s="12" t="s">
         <v>103</v>
       </c>
       <c r="K90" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L90" s="12" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="M90" s="12">
         <v>20.55</v>
@@ -6756,12 +6742,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="91" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" s="12">
         <v>2035</v>
       </c>
       <c r="B91" s="12" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C91" s="12" t="s">
         <v>17</v>
@@ -6770,25 +6756,25 @@
         <v>243</v>
       </c>
       <c r="F91" s="12" t="s">
-        <v>271</v>
-      </c>
-      <c r="G91" s="12" t="s">
-        <v>211</v>
+        <v>270</v>
+      </c>
+      <c r="G91" s="52" t="s">
+        <v>232</v>
       </c>
       <c r="H91" s="12" t="s">
-        <v>116</v>
+        <v>233</v>
       </c>
       <c r="J91" s="12" t="s">
         <v>103</v>
       </c>
       <c r="K91" s="13" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="L91" s="12" t="s">
-        <v>236</v>
-      </c>
-      <c r="M91" s="52">
-        <v>15.85</v>
+        <v>234</v>
+      </c>
+      <c r="M91" s="12">
+        <v>20.55</v>
       </c>
       <c r="N91" s="46" t="s">
         <v>109</v>
@@ -6812,12 +6798,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="92" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="12">
         <v>2035</v>
       </c>
       <c r="B92" s="12" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="C92" s="12" t="s">
         <v>17</v>
@@ -6826,7 +6812,7 @@
         <v>243</v>
       </c>
       <c r="F92" s="12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G92" s="12" t="s">
         <v>211</v>
@@ -6838,13 +6824,13 @@
         <v>103</v>
       </c>
       <c r="K92" s="13" t="s">
-        <v>110</v>
+        <v>16</v>
       </c>
       <c r="L92" s="12" t="s">
-        <v>242</v>
-      </c>
-      <c r="M92" s="12">
-        <v>20.55</v>
+        <v>236</v>
+      </c>
+      <c r="M92" s="52">
+        <v>15.85</v>
       </c>
       <c r="N92" s="46" t="s">
         <v>109</v>
@@ -6858,22 +6844,22 @@
       <c r="Q92" s="12">
         <v>0.89</v>
       </c>
-      <c r="R92" s="51">
-        <v>0</v>
-      </c>
-      <c r="S92" s="51">
-        <v>0</v>
-      </c>
-      <c r="T92" s="51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R92" s="14">
+        <v>100</v>
+      </c>
+      <c r="S92" s="14">
+        <v>0</v>
+      </c>
+      <c r="T92" s="14">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="93" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" s="12">
         <v>2035</v>
       </c>
       <c r="B93" s="12" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="C93" s="12" t="s">
         <v>17</v>
@@ -6882,7 +6868,7 @@
         <v>243</v>
       </c>
       <c r="F93" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G93" s="12" t="s">
         <v>211</v>
@@ -6894,10 +6880,10 @@
         <v>103</v>
       </c>
       <c r="K93" s="13" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="L93" s="12" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="M93" s="12">
         <v>20.55</v>
@@ -6914,22 +6900,22 @@
       <c r="Q93" s="12">
         <v>0.89</v>
       </c>
-      <c r="R93" s="14">
-        <v>100</v>
-      </c>
-      <c r="S93" s="14">
-        <v>0</v>
-      </c>
-      <c r="T93" s="14">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="94" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R93" s="51">
+        <v>0</v>
+      </c>
+      <c r="S93" s="51">
+        <v>0</v>
+      </c>
+      <c r="T93" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" s="12">
         <v>2035</v>
       </c>
       <c r="B94" s="12" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="C94" s="12" t="s">
         <v>17</v>
@@ -6938,7 +6924,7 @@
         <v>243</v>
       </c>
       <c r="F94" s="12" t="s">
-        <v>249</v>
+        <v>273</v>
       </c>
       <c r="G94" s="12" t="s">
         <v>211</v>
@@ -6950,10 +6936,10 @@
         <v>103</v>
       </c>
       <c r="K94" s="13" t="s">
-        <v>43</v>
+        <v>129</v>
       </c>
       <c r="L94" s="12" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="M94" s="12">
         <v>20.55</v>
@@ -6965,10 +6951,10 @@
         <v>109</v>
       </c>
       <c r="P94" s="12">
-        <v>0.87</v>
+        <v>0.99</v>
       </c>
       <c r="Q94" s="12">
-        <v>0.78</v>
+        <v>0.89</v>
       </c>
       <c r="R94" s="14">
         <v>100</v>
@@ -6980,12 +6966,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="95" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A95" s="12">
         <v>2035</v>
       </c>
       <c r="B95" s="12" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C95" s="12" t="s">
         <v>17</v>
@@ -6994,7 +6980,7 @@
         <v>243</v>
       </c>
       <c r="F95" s="12" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G95" s="12" t="s">
         <v>211</v>
@@ -7009,7 +6995,7 @@
         <v>43</v>
       </c>
       <c r="L95" s="12" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="M95" s="12">
         <v>20.55</v>
@@ -7036,12 +7022,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="96" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A96" s="12">
         <v>2035</v>
       </c>
       <c r="B96" s="12" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="C96" s="12" t="s">
         <v>17</v>
@@ -7050,7 +7036,7 @@
         <v>243</v>
       </c>
       <c r="F96" s="12" t="s">
-        <v>239</v>
+        <v>252</v>
       </c>
       <c r="G96" s="12" t="s">
         <v>211</v>
@@ -7062,10 +7048,10 @@
         <v>103</v>
       </c>
       <c r="K96" s="13" t="s">
-        <v>108</v>
+        <v>43</v>
       </c>
       <c r="L96" s="12" t="s">
-        <v>240</v>
+        <v>253</v>
       </c>
       <c r="M96" s="12">
         <v>20.55</v>
@@ -7076,11 +7062,11 @@
       <c r="O96" s="46" t="s">
         <v>109</v>
       </c>
-      <c r="P96" s="52">
-        <v>0.84</v>
-      </c>
-      <c r="Q96" s="52">
-        <v>1.59</v>
+      <c r="P96" s="12">
+        <v>0.87</v>
+      </c>
+      <c r="Q96" s="12">
+        <v>0.78</v>
       </c>
       <c r="R96" s="14">
         <v>100</v>
@@ -7092,12 +7078,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="97" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A97" s="12">
         <v>2035</v>
       </c>
       <c r="B97" s="12" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C97" s="12" t="s">
         <v>17</v>
@@ -7106,7 +7092,7 @@
         <v>243</v>
       </c>
       <c r="F97" s="12" t="s">
-        <v>255</v>
+        <v>239</v>
       </c>
       <c r="G97" s="12" t="s">
         <v>211</v>
@@ -7118,10 +7104,10 @@
         <v>103</v>
       </c>
       <c r="K97" s="13" t="s">
-        <v>43</v>
+        <v>108</v>
       </c>
       <c r="L97" s="12" t="s">
-        <v>256</v>
+        <v>240</v>
       </c>
       <c r="M97" s="12">
         <v>20.55</v>
@@ -7132,11 +7118,11 @@
       <c r="O97" s="46" t="s">
         <v>109</v>
       </c>
-      <c r="P97" s="12">
-        <v>0.87</v>
-      </c>
-      <c r="Q97" s="12">
-        <v>0.78</v>
+      <c r="P97" s="52">
+        <v>0.84</v>
+      </c>
+      <c r="Q97" s="52">
+        <v>1.59</v>
       </c>
       <c r="R97" s="14">
         <v>100</v>
@@ -7148,12 +7134,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="98" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" s="12">
         <v>2035</v>
       </c>
       <c r="B98" s="12" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="C98" s="12" t="s">
         <v>17</v>
@@ -7162,7 +7148,7 @@
         <v>243</v>
       </c>
       <c r="F98" s="12" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="G98" s="12" t="s">
         <v>211</v>
@@ -7170,14 +7156,14 @@
       <c r="H98" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="J98" s="52" t="s">
-        <v>263</v>
+      <c r="J98" s="12" t="s">
+        <v>103</v>
       </c>
       <c r="K98" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L98" s="12" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="M98" s="12">
         <v>20.55</v>
@@ -7204,12 +7190,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="99" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A99" s="12">
         <v>2035</v>
       </c>
       <c r="B99" s="12" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="C99" s="12" t="s">
         <v>17</v>
@@ -7218,7 +7204,7 @@
         <v>243</v>
       </c>
       <c r="F99" s="12" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="G99" s="12" t="s">
         <v>211</v>
@@ -7226,14 +7212,14 @@
       <c r="H99" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="J99" s="12" t="s">
-        <v>103</v>
+      <c r="J99" s="52" t="s">
+        <v>263</v>
       </c>
       <c r="K99" s="13" t="s">
-        <v>129</v>
+        <v>42</v>
       </c>
       <c r="L99" s="12" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="M99" s="12">
         <v>20.55</v>
@@ -7260,12 +7246,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="100" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A100" s="12">
         <v>2035</v>
       </c>
       <c r="B100" s="12" t="s">
-        <v>274</v>
+        <v>258</v>
       </c>
       <c r="C100" s="12" t="s">
         <v>17</v>
@@ -7274,7 +7260,7 @@
         <v>243</v>
       </c>
       <c r="F100" s="12" t="s">
-        <v>275</v>
+        <v>259</v>
       </c>
       <c r="G100" s="12" t="s">
         <v>211</v>
@@ -7286,13 +7272,13 @@
         <v>103</v>
       </c>
       <c r="K100" s="13" t="s">
-        <v>43</v>
+        <v>129</v>
       </c>
       <c r="L100" s="12" t="s">
-        <v>276</v>
-      </c>
-      <c r="M100" s="52">
-        <v>13.68</v>
+        <v>260</v>
+      </c>
+      <c r="M100" s="12">
+        <v>20.55</v>
       </c>
       <c r="N100" s="46" t="s">
         <v>109</v>
@@ -7316,12 +7302,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="101" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A101" s="12">
         <v>2035</v>
       </c>
       <c r="B101" s="12" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="C101" s="12" t="s">
         <v>17</v>
@@ -7330,7 +7316,7 @@
         <v>243</v>
       </c>
       <c r="F101" s="12" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="G101" s="12" t="s">
         <v>211</v>
@@ -7345,10 +7331,10 @@
         <v>43</v>
       </c>
       <c r="L101" s="12" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="M101" s="52">
-        <v>14.55</v>
+        <v>13.68</v>
       </c>
       <c r="N101" s="46" t="s">
         <v>109</v>
@@ -7372,12 +7358,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="102" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A102" s="12">
         <v>2035</v>
       </c>
       <c r="B102" s="12" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C102" s="12" t="s">
         <v>17</v>
@@ -7386,7 +7372,7 @@
         <v>243</v>
       </c>
       <c r="F102" s="12" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="G102" s="12" t="s">
         <v>211</v>
@@ -7401,10 +7387,10 @@
         <v>43</v>
       </c>
       <c r="L102" s="12" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="M102" s="52">
-        <v>17.579999999999998</v>
+        <v>14.55</v>
       </c>
       <c r="N102" s="46" t="s">
         <v>109</v>
@@ -7428,12 +7414,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="103" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A103" s="12">
         <v>2035</v>
       </c>
       <c r="B103" s="12" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C103" s="12" t="s">
         <v>17</v>
@@ -7442,7 +7428,7 @@
         <v>243</v>
       </c>
       <c r="F103" s="12" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="G103" s="12" t="s">
         <v>211</v>
@@ -7454,13 +7440,13 @@
         <v>103</v>
       </c>
       <c r="K103" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L103" s="12" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="M103" s="52">
-        <v>15.06</v>
+        <v>17.579999999999998</v>
       </c>
       <c r="N103" s="46" t="s">
         <v>109</v>
@@ -7484,12 +7470,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="104" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A104" s="12">
         <v>2035</v>
       </c>
       <c r="B104" s="12" t="s">
-        <v>372</v>
+        <v>285</v>
       </c>
       <c r="C104" s="12" t="s">
         <v>17</v>
@@ -7498,7 +7484,7 @@
         <v>243</v>
       </c>
       <c r="F104" s="12" t="s">
-        <v>373</v>
+        <v>287</v>
       </c>
       <c r="G104" s="12" t="s">
         <v>211</v>
@@ -7506,9 +7492,6 @@
       <c r="H104" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="I104" s="12" t="s">
-        <v>11</v>
-      </c>
       <c r="J104" s="12" t="s">
         <v>103</v>
       </c>
@@ -7516,10 +7499,10 @@
         <v>42</v>
       </c>
       <c r="L104" s="12" t="s">
-        <v>374</v>
+        <v>288</v>
       </c>
       <c r="M104" s="52">
-        <v>16.82</v>
+        <v>15.06</v>
       </c>
       <c r="N104" s="46" t="s">
         <v>109</v>
@@ -7542,72 +7525,75 @@
       <c r="T104" s="14">
         <v>75</v>
       </c>
-      <c r="U104" s="12" t="s">
+    </row>
+    <row r="105" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="12">
+        <v>2035</v>
+      </c>
+      <c r="B105" s="12" t="s">
+        <v>372</v>
+      </c>
+      <c r="C105" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D105" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="F105" s="12" t="s">
+        <v>373</v>
+      </c>
+      <c r="G105" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="H105" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="I105" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="J105" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="K105" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="L105" s="12" t="s">
+        <v>374</v>
+      </c>
+      <c r="M105" s="52">
+        <v>16.82</v>
+      </c>
+      <c r="N105" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="O105" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="P105" s="12">
+        <v>0.87</v>
+      </c>
+      <c r="Q105" s="12">
+        <v>0.78</v>
+      </c>
+      <c r="R105" s="14">
+        <v>100</v>
+      </c>
+      <c r="S105" s="14">
+        <v>0</v>
+      </c>
+      <c r="T105" s="14">
+        <v>75</v>
+      </c>
+      <c r="U105" s="12" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="105" spans="1:21" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="59">
-        <v>2035</v>
-      </c>
-      <c r="B105" s="59" t="s">
-        <v>337</v>
-      </c>
-      <c r="C105" s="59" t="s">
-        <v>338</v>
-      </c>
-      <c r="D105" s="59" t="s">
-        <v>339</v>
-      </c>
-      <c r="F105" s="59" t="s">
-        <v>340</v>
-      </c>
-      <c r="G105" s="59" t="s">
-        <v>342</v>
-      </c>
-      <c r="H105" s="59" t="s">
-        <v>343</v>
-      </c>
-      <c r="J105" s="59" t="s">
-        <v>344</v>
-      </c>
-      <c r="K105" s="60" t="s">
-        <v>110</v>
-      </c>
-      <c r="L105" s="59" t="s">
-        <v>341</v>
-      </c>
-      <c r="M105" s="59">
-        <v>17.579999999999998</v>
-      </c>
-      <c r="N105" s="61" t="s">
-        <v>109</v>
-      </c>
-      <c r="O105" s="61" t="s">
-        <v>109</v>
-      </c>
-      <c r="P105" s="59">
-        <v>0.87</v>
-      </c>
-      <c r="Q105" s="59">
-        <v>0.78</v>
-      </c>
-      <c r="R105" s="62">
-        <v>83.3</v>
-      </c>
-      <c r="S105" s="62">
-        <v>0</v>
-      </c>
-      <c r="T105" s="62">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="106" spans="1:21" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:21" s="59" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A106" s="59">
         <v>2035</v>
       </c>
       <c r="B106" s="59" t="s">
-        <v>375</v>
+        <v>337</v>
       </c>
       <c r="C106" s="59" t="s">
         <v>338</v>
@@ -7616,7 +7602,7 @@
         <v>339</v>
       </c>
       <c r="F106" s="59" t="s">
-        <v>376</v>
+        <v>340</v>
       </c>
       <c r="G106" s="59" t="s">
         <v>342</v>
@@ -7631,10 +7617,10 @@
         <v>110</v>
       </c>
       <c r="L106" s="59" t="s">
-        <v>377</v>
+        <v>341</v>
       </c>
       <c r="M106" s="59">
-        <v>16.82</v>
+        <v>17.579999999999998</v>
       </c>
       <c r="N106" s="61" t="s">
         <v>109</v>
@@ -7658,12 +7644,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="107" spans="1:21" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:21" s="59" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A107" s="59">
         <v>2035</v>
       </c>
       <c r="B107" s="59" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="C107" s="59" t="s">
         <v>338</v>
@@ -7672,25 +7658,22 @@
         <v>339</v>
       </c>
       <c r="F107" s="59" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="G107" s="59" t="s">
-        <v>387</v>
+        <v>342</v>
       </c>
       <c r="H107" s="59" t="s">
-        <v>392</v>
-      </c>
-      <c r="I107" s="59" t="s">
-        <v>11</v>
+        <v>343</v>
       </c>
       <c r="J107" s="59" t="s">
-        <v>394</v>
+        <v>344</v>
       </c>
       <c r="K107" s="60" t="s">
         <v>110</v>
       </c>
       <c r="L107" s="59" t="s">
-        <v>399</v>
+        <v>377</v>
       </c>
       <c r="M107" s="59">
         <v>16.82</v>
@@ -7716,72 +7699,75 @@
       <c r="T107" s="62">
         <v>72</v>
       </c>
-      <c r="U107" s="59" t="s">
+    </row>
+    <row r="108" spans="1:21" s="59" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="59">
+        <v>2035</v>
+      </c>
+      <c r="B108" s="59" t="s">
+        <v>385</v>
+      </c>
+      <c r="C108" s="59" t="s">
+        <v>338</v>
+      </c>
+      <c r="D108" s="59" t="s">
+        <v>339</v>
+      </c>
+      <c r="F108" s="59" t="s">
+        <v>386</v>
+      </c>
+      <c r="G108" s="59" t="s">
+        <v>387</v>
+      </c>
+      <c r="H108" s="59" t="s">
+        <v>392</v>
+      </c>
+      <c r="I108" s="59" t="s">
+        <v>11</v>
+      </c>
+      <c r="J108" s="59" t="s">
+        <v>394</v>
+      </c>
+      <c r="K108" s="60" t="s">
+        <v>110</v>
+      </c>
+      <c r="L108" s="59" t="s">
+        <v>399</v>
+      </c>
+      <c r="M108" s="59">
+        <v>16.82</v>
+      </c>
+      <c r="N108" s="61" t="s">
+        <v>109</v>
+      </c>
+      <c r="O108" s="61" t="s">
+        <v>109</v>
+      </c>
+      <c r="P108" s="59">
+        <v>0.87</v>
+      </c>
+      <c r="Q108" s="59">
+        <v>0.78</v>
+      </c>
+      <c r="R108" s="62">
+        <v>83.3</v>
+      </c>
+      <c r="S108" s="62">
+        <v>0</v>
+      </c>
+      <c r="T108" s="62">
+        <v>72</v>
+      </c>
+      <c r="U108" s="59" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="108" spans="1:21" s="63" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="63">
-        <v>2035</v>
-      </c>
-      <c r="B108" s="63" t="s">
-        <v>345</v>
-      </c>
-      <c r="C108" s="64" t="s">
-        <v>338</v>
-      </c>
-      <c r="D108" s="63" t="s">
-        <v>339</v>
-      </c>
-      <c r="F108" s="63" t="s">
-        <v>346</v>
-      </c>
-      <c r="G108" s="63" t="s">
-        <v>347</v>
-      </c>
-      <c r="H108" s="63" t="s">
-        <v>348</v>
-      </c>
-      <c r="J108" s="63" t="s">
-        <v>349</v>
-      </c>
-      <c r="K108" s="65" t="s">
-        <v>129</v>
-      </c>
-      <c r="L108" s="64" t="s">
-        <v>350</v>
-      </c>
-      <c r="M108" s="63">
-        <v>17.579999999999998</v>
-      </c>
-      <c r="N108" s="66" t="s">
-        <v>109</v>
-      </c>
-      <c r="O108" s="66" t="s">
-        <v>109</v>
-      </c>
-      <c r="P108" s="63">
-        <v>0.87</v>
-      </c>
-      <c r="Q108" s="63">
-        <v>0.78</v>
-      </c>
-      <c r="R108" s="67">
-        <v>83.3</v>
-      </c>
-      <c r="S108" s="67">
-        <v>0</v>
-      </c>
-      <c r="T108" s="67">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="109" spans="1:21" s="63" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:21" s="63" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A109" s="63">
         <v>2035</v>
       </c>
       <c r="B109" s="63" t="s">
-        <v>378</v>
+        <v>345</v>
       </c>
       <c r="C109" s="64" t="s">
         <v>338</v>
@@ -7790,7 +7776,7 @@
         <v>339</v>
       </c>
       <c r="F109" s="63" t="s">
-        <v>376</v>
+        <v>346</v>
       </c>
       <c r="G109" s="63" t="s">
         <v>347</v>
@@ -7805,10 +7791,10 @@
         <v>129</v>
       </c>
       <c r="L109" s="64" t="s">
-        <v>379</v>
+        <v>350</v>
       </c>
       <c r="M109" s="63">
-        <v>16.82</v>
+        <v>17.579999999999998</v>
       </c>
       <c r="N109" s="66" t="s">
         <v>109</v>
@@ -7832,12 +7818,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="110" spans="1:21" s="63" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:21" s="63" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A110" s="63">
         <v>2035</v>
       </c>
       <c r="B110" s="63" t="s">
-        <v>390</v>
+        <v>378</v>
       </c>
       <c r="C110" s="64" t="s">
         <v>338</v>
@@ -7846,25 +7832,22 @@
         <v>339</v>
       </c>
       <c r="F110" s="63" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="G110" s="63" t="s">
-        <v>391</v>
+        <v>347</v>
       </c>
       <c r="H110" s="63" t="s">
-        <v>393</v>
-      </c>
-      <c r="I110" s="63" t="s">
-        <v>11</v>
+        <v>348</v>
       </c>
       <c r="J110" s="63" t="s">
-        <v>396</v>
+        <v>349</v>
       </c>
       <c r="K110" s="65" t="s">
         <v>129</v>
       </c>
       <c r="L110" s="64" t="s">
-        <v>397</v>
+        <v>379</v>
       </c>
       <c r="M110" s="63">
         <v>16.82</v>
@@ -7890,128 +7873,131 @@
       <c r="T110" s="67">
         <v>72</v>
       </c>
-      <c r="U110" s="63" t="s">
+    </row>
+    <row r="111" spans="1:21" s="63" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="63">
+        <v>2035</v>
+      </c>
+      <c r="B111" s="63" t="s">
+        <v>390</v>
+      </c>
+      <c r="C111" s="64" t="s">
+        <v>338</v>
+      </c>
+      <c r="D111" s="63" t="s">
+        <v>339</v>
+      </c>
+      <c r="F111" s="63" t="s">
+        <v>386</v>
+      </c>
+      <c r="G111" s="63" t="s">
+        <v>391</v>
+      </c>
+      <c r="H111" s="63" t="s">
+        <v>393</v>
+      </c>
+      <c r="I111" s="63" t="s">
+        <v>11</v>
+      </c>
+      <c r="J111" s="63" t="s">
+        <v>396</v>
+      </c>
+      <c r="K111" s="65" t="s">
+        <v>129</v>
+      </c>
+      <c r="L111" s="64" t="s">
+        <v>397</v>
+      </c>
+      <c r="M111" s="63">
+        <v>16.82</v>
+      </c>
+      <c r="N111" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="O111" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="P111" s="63">
+        <v>0.87</v>
+      </c>
+      <c r="Q111" s="63">
+        <v>0.78</v>
+      </c>
+      <c r="R111" s="67">
+        <v>83.3</v>
+      </c>
+      <c r="S111" s="67">
+        <v>0</v>
+      </c>
+      <c r="T111" s="67">
+        <v>72</v>
+      </c>
+      <c r="U111" s="63" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="111" spans="1:21" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="24">
+    <row r="112" spans="1:21" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="24">
         <v>2050</v>
       </c>
-      <c r="B111" s="24" t="s">
+      <c r="B112" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="C111" s="24" t="s">
+      <c r="C112" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="D111" s="24" t="s">
+      <c r="D112" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="F111" s="24" t="s">
+      <c r="F112" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="G111" s="24" t="s">
+      <c r="G112" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="H111" s="25" t="s">
+      <c r="H112" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="J111" s="24" t="s">
+      <c r="J112" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="K111" s="26" t="s">
+      <c r="K112" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="L111" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="M111" s="24">
+      <c r="L112" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="M112" s="24">
         <v>17.440000000000001</v>
       </c>
-      <c r="N111" s="47">
+      <c r="N112" s="47">
         <v>-0.33</v>
       </c>
-      <c r="O111" s="47">
-        <v>0</v>
-      </c>
-      <c r="P111" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q111" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="R111" s="73" t="s">
-        <v>109</v>
-      </c>
-      <c r="S111" s="73" t="s">
-        <v>109</v>
-      </c>
-      <c r="T111" s="73" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="112" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="54">
-        <v>2050</v>
-      </c>
-      <c r="B112" s="54" t="s">
-        <v>351</v>
-      </c>
-      <c r="C112" s="54" t="s">
-        <v>338</v>
-      </c>
-      <c r="D112" s="54" t="s">
-        <v>339</v>
-      </c>
-      <c r="F112" s="54" t="s">
-        <v>353</v>
-      </c>
-      <c r="G112" s="54" t="s">
-        <v>342</v>
-      </c>
-      <c r="H112" s="53" t="s">
-        <v>343</v>
-      </c>
-      <c r="J112" s="54" t="s">
-        <v>344</v>
-      </c>
-      <c r="K112" s="53" t="s">
-        <v>16</v>
-      </c>
-      <c r="L112" s="54" t="s">
-        <v>356</v>
-      </c>
-      <c r="M112" s="54">
-        <v>19.13</v>
-      </c>
-      <c r="N112" s="68" t="s">
-        <v>109</v>
-      </c>
-      <c r="O112" s="68" t="s">
-        <v>109</v>
-      </c>
-      <c r="P112" s="54">
-        <v>0.87</v>
-      </c>
-      <c r="Q112" s="54">
-        <v>0.78</v>
-      </c>
-      <c r="R112" s="57">
-        <v>83.3</v>
-      </c>
-      <c r="S112" s="57">
-        <v>0</v>
-      </c>
-      <c r="T112" s="57">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="113" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O112" s="47">
+        <v>0</v>
+      </c>
+      <c r="P112" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q112" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="R112" s="73" t="s">
+        <v>109</v>
+      </c>
+      <c r="S112" s="73" t="s">
+        <v>109</v>
+      </c>
+      <c r="T112" s="73" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="113" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A113" s="54">
         <v>2050</v>
       </c>
       <c r="B113" s="54" t="s">
-        <v>380</v>
+        <v>351</v>
       </c>
       <c r="C113" s="54" t="s">
         <v>338</v>
@@ -8020,7 +8006,7 @@
         <v>339</v>
       </c>
       <c r="F113" s="54" t="s">
-        <v>376</v>
+        <v>353</v>
       </c>
       <c r="G113" s="54" t="s">
         <v>342</v>
@@ -8035,10 +8021,10 @@
         <v>16</v>
       </c>
       <c r="L113" s="54" t="s">
-        <v>381</v>
+        <v>356</v>
       </c>
       <c r="M113" s="54">
-        <v>18.420000000000002</v>
+        <v>19.13</v>
       </c>
       <c r="N113" s="68" t="s">
         <v>109</v>
@@ -8062,12 +8048,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="114" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A114" s="54">
         <v>2050</v>
       </c>
       <c r="B114" s="54" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="C114" s="54" t="s">
         <v>338</v>
@@ -8076,25 +8062,22 @@
         <v>339</v>
       </c>
       <c r="F114" s="54" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="G114" s="54" t="s">
-        <v>387</v>
+        <v>342</v>
       </c>
       <c r="H114" s="53" t="s">
-        <v>392</v>
-      </c>
-      <c r="I114" s="54" t="s">
-        <v>11</v>
+        <v>343</v>
       </c>
       <c r="J114" s="54" t="s">
-        <v>394</v>
+        <v>344</v>
       </c>
       <c r="K114" s="53" t="s">
         <v>16</v>
       </c>
       <c r="L114" s="54" t="s">
-        <v>400</v>
+        <v>381</v>
       </c>
       <c r="M114" s="54">
         <v>18.420000000000002</v>
@@ -8120,72 +8103,75 @@
       <c r="T114" s="57">
         <v>72</v>
       </c>
-      <c r="U114" s="54" t="s">
+    </row>
+    <row r="115" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="54">
+        <v>2050</v>
+      </c>
+      <c r="B115" s="54" t="s">
+        <v>388</v>
+      </c>
+      <c r="C115" s="54" t="s">
+        <v>338</v>
+      </c>
+      <c r="D115" s="54" t="s">
+        <v>339</v>
+      </c>
+      <c r="F115" s="54" t="s">
+        <v>386</v>
+      </c>
+      <c r="G115" s="54" t="s">
+        <v>387</v>
+      </c>
+      <c r="H115" s="53" t="s">
+        <v>392</v>
+      </c>
+      <c r="I115" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="J115" s="54" t="s">
+        <v>394</v>
+      </c>
+      <c r="K115" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="L115" s="54" t="s">
+        <v>400</v>
+      </c>
+      <c r="M115" s="54">
+        <v>18.420000000000002</v>
+      </c>
+      <c r="N115" s="68" t="s">
+        <v>109</v>
+      </c>
+      <c r="O115" s="68" t="s">
+        <v>109</v>
+      </c>
+      <c r="P115" s="54">
+        <v>0.87</v>
+      </c>
+      <c r="Q115" s="54">
+        <v>0.78</v>
+      </c>
+      <c r="R115" s="57">
+        <v>83.3</v>
+      </c>
+      <c r="S115" s="57">
+        <v>0</v>
+      </c>
+      <c r="T115" s="57">
+        <v>72</v>
+      </c>
+      <c r="U115" s="54" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="115" spans="1:21" s="69" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="69">
-        <v>2050</v>
-      </c>
-      <c r="B115" s="69" t="s">
-        <v>352</v>
-      </c>
-      <c r="C115" s="69" t="s">
-        <v>338</v>
-      </c>
-      <c r="D115" s="69" t="s">
-        <v>339</v>
-      </c>
-      <c r="F115" s="69" t="s">
-        <v>354</v>
-      </c>
-      <c r="G115" s="69" t="s">
-        <v>347</v>
-      </c>
-      <c r="H115" s="70" t="s">
-        <v>348</v>
-      </c>
-      <c r="J115" s="69" t="s">
-        <v>355</v>
-      </c>
-      <c r="K115" s="70" t="s">
-        <v>44</v>
-      </c>
-      <c r="L115" s="69" t="s">
-        <v>357</v>
-      </c>
-      <c r="M115" s="69">
-        <v>19.13</v>
-      </c>
-      <c r="N115" s="71" t="s">
-        <v>109</v>
-      </c>
-      <c r="O115" s="71" t="s">
-        <v>109</v>
-      </c>
-      <c r="P115" s="69">
-        <v>0.87</v>
-      </c>
-      <c r="Q115" s="69">
-        <v>0.78</v>
-      </c>
-      <c r="R115" s="72">
-        <v>83.3</v>
-      </c>
-      <c r="S115" s="72">
-        <v>0</v>
-      </c>
-      <c r="T115" s="72">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="116" spans="1:21" s="69" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:21" s="69" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A116" s="69">
         <v>2050</v>
       </c>
       <c r="B116" s="69" t="s">
-        <v>382</v>
+        <v>352</v>
       </c>
       <c r="C116" s="69" t="s">
         <v>338</v>
@@ -8212,7 +8198,7 @@
         <v>357</v>
       </c>
       <c r="M116" s="69">
-        <v>18.420000000000002</v>
+        <v>19.13</v>
       </c>
       <c r="N116" s="71" t="s">
         <v>109</v>
@@ -8236,12 +8222,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="117" spans="1:21" s="69" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:21" s="69" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A117" s="69">
         <v>2050</v>
       </c>
       <c r="B117" s="69" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="C117" s="69" t="s">
         <v>338</v>
@@ -8250,25 +8236,22 @@
         <v>339</v>
       </c>
       <c r="F117" s="69" t="s">
-        <v>386</v>
+        <v>354</v>
       </c>
       <c r="G117" s="69" t="s">
-        <v>391</v>
+        <v>347</v>
       </c>
       <c r="H117" s="70" t="s">
-        <v>393</v>
-      </c>
-      <c r="I117" s="69" t="s">
-        <v>11</v>
+        <v>348</v>
       </c>
       <c r="J117" s="69" t="s">
-        <v>395</v>
+        <v>355</v>
       </c>
       <c r="K117" s="70" t="s">
         <v>44</v>
       </c>
       <c r="L117" s="69" t="s">
-        <v>398</v>
+        <v>357</v>
       </c>
       <c r="M117" s="69">
         <v>18.420000000000002</v>
@@ -8294,7 +8277,66 @@
       <c r="T117" s="72">
         <v>72</v>
       </c>
-      <c r="U117" s="69" t="s">
+    </row>
+    <row r="118" spans="1:21" s="69" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="69">
+        <v>2050</v>
+      </c>
+      <c r="B118" s="69" t="s">
+        <v>389</v>
+      </c>
+      <c r="C118" s="69" t="s">
+        <v>338</v>
+      </c>
+      <c r="D118" s="69" t="s">
+        <v>339</v>
+      </c>
+      <c r="F118" s="69" t="s">
+        <v>386</v>
+      </c>
+      <c r="G118" s="69" t="s">
+        <v>391</v>
+      </c>
+      <c r="H118" s="70" t="s">
+        <v>393</v>
+      </c>
+      <c r="I118" s="69" t="s">
+        <v>11</v>
+      </c>
+      <c r="J118" s="69" t="s">
+        <v>395</v>
+      </c>
+      <c r="K118" s="70" t="s">
+        <v>44</v>
+      </c>
+      <c r="L118" s="69" t="s">
+        <v>398</v>
+      </c>
+      <c r="M118" s="69">
+        <v>18.420000000000002</v>
+      </c>
+      <c r="N118" s="71" t="s">
+        <v>109</v>
+      </c>
+      <c r="O118" s="71" t="s">
+        <v>109</v>
+      </c>
+      <c r="P118" s="69">
+        <v>0.87</v>
+      </c>
+      <c r="Q118" s="69">
+        <v>0.78</v>
+      </c>
+      <c r="R118" s="72">
+        <v>83.3</v>
+      </c>
+      <c r="S118" s="72">
+        <v>0</v>
+      </c>
+      <c r="T118" s="72">
+        <v>72</v>
+      </c>
+      <c r="U118" s="69" t="s">
         <v>358</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add v05 DBP series and promote to current
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\config_RTP2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F320BBF-2C06-42FA-BE02-A6F49AA0CB5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA41A7A1-85DB-44B4-B824-CD7217ECD56C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6510" yWindow="3810" windowWidth="28800" windowHeight="11385" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
+    <workbookView xWindow="5490" yWindow="2790" windowWidth="31425" windowHeight="11175" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelRuns" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1318" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1363" uniqueCount="434">
   <si>
     <t>year</t>
   </si>
@@ -1311,6 +1311,51 @@
   </si>
   <si>
     <t>https://app.asana.com/0/1204085012544660/1206985522676097/f</t>
+  </si>
+  <si>
+    <t>2005</t>
+  </si>
+  <si>
+    <t>2035_TM160_DBP_NoProject_05</t>
+  </si>
+  <si>
+    <t>Updated landuse/popsyn (fix too many persons)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M:\urban_modeling\baus\PBA50Plus\PBA50Plus_NoProject_v4dem </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PBA50Plus_NoProject_v4dem </t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1207070817758664/f</t>
+  </si>
+  <si>
+    <t>2035_TM160_DBP_Plan_05</t>
+  </si>
+  <si>
+    <t>Update landuse/popsyn (fix too many persons); add back T8 Complete Streets</t>
+  </si>
+  <si>
+    <t>PBA50Plus_Draft_Blueprint_v2b</t>
+  </si>
+  <si>
+    <t>M:\urban_modeling\baus\PBA50Plus\PBA50Plus_DBP_InitialRun\outputs\PBA50Plus_Draft_Blueprint_v2b</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1207012741527409/f</t>
+  </si>
+  <si>
+    <t>2050_TM160_DBP_NoProject_05</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1207070817758666/f</t>
+  </si>
+  <si>
+    <t>2050_TM160_DBP_Plan_05</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1204085012544660/1207012741527411/f</t>
   </si>
 </sst>
 </file>
@@ -1638,7 +1683,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1967,13 +2012,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9564CC59-3725-4FDA-8BF2-0F68CB1B6F5A}">
-  <dimension ref="A1:V121"/>
+  <dimension ref="A1:V125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C104" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C107" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B121" sqref="B121"/>
+      <selection pane="bottomRight" activeCell="I125" sqref="I125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2344,6 +2389,9 @@
       <c r="U6" s="33">
         <v>0</v>
       </c>
+      <c r="V6" s="74" t="s">
+        <v>419</v>
+      </c>
     </row>
     <row r="7" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="52">
@@ -4516,7 +4564,7 @@
       <c r="A50" s="1">
         <v>2023</v>
       </c>
-      <c r="B50" s="74" t="s">
+      <c r="B50" s="1" t="s">
         <v>170</v>
       </c>
       <c r="C50" s="1" t="s">
@@ -4740,7 +4788,7 @@
       <c r="A54" s="1">
         <v>2023</v>
       </c>
-      <c r="B54" s="74" t="s">
+      <c r="B54" s="1" t="s">
         <v>181</v>
       </c>
       <c r="C54" s="1" t="s">
@@ -7794,9 +7842,6 @@
       <c r="H108" s="58" t="s">
         <v>406</v>
       </c>
-      <c r="I108" s="58" t="s">
-        <v>11</v>
-      </c>
       <c r="K108" s="58" t="s">
         <v>404</v>
       </c>
@@ -7830,64 +7875,67 @@
       <c r="U108" s="61">
         <v>72</v>
       </c>
-      <c r="V108" s="58" t="s">
+    </row>
+    <row r="109" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="58">
+        <v>2035</v>
+      </c>
+      <c r="B109" s="58" t="s">
+        <v>420</v>
+      </c>
+      <c r="C109" s="58" t="s">
+        <v>338</v>
+      </c>
+      <c r="D109" s="58" t="s">
+        <v>339</v>
+      </c>
+      <c r="F109" s="58" t="s">
+        <v>421</v>
+      </c>
+      <c r="G109" s="58" t="s">
+        <v>422</v>
+      </c>
+      <c r="H109" s="58" t="s">
+        <v>423</v>
+      </c>
+      <c r="I109" s="58" t="s">
+        <v>11</v>
+      </c>
+      <c r="K109" s="58" t="s">
+        <v>404</v>
+      </c>
+      <c r="L109" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="M109" s="58" t="s">
+        <v>424</v>
+      </c>
+      <c r="N109" s="58">
+        <v>16.82</v>
+      </c>
+      <c r="O109" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="P109" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q109" s="58">
+        <v>0.87</v>
+      </c>
+      <c r="R109" s="58">
+        <v>0.78</v>
+      </c>
+      <c r="S109" s="61">
+        <v>83.3</v>
+      </c>
+      <c r="T109" s="61">
+        <v>0</v>
+      </c>
+      <c r="U109" s="61">
+        <v>72</v>
+      </c>
+      <c r="V109" s="58" t="s">
         <v>361</v>
-      </c>
-    </row>
-    <row r="109" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="62">
-        <v>2035</v>
-      </c>
-      <c r="B109" s="62" t="s">
-        <v>345</v>
-      </c>
-      <c r="C109" s="63" t="s">
-        <v>338</v>
-      </c>
-      <c r="D109" s="62" t="s">
-        <v>339</v>
-      </c>
-      <c r="F109" s="62" t="s">
-        <v>346</v>
-      </c>
-      <c r="G109" s="62" t="s">
-        <v>347</v>
-      </c>
-      <c r="H109" s="62" t="s">
-        <v>348</v>
-      </c>
-      <c r="K109" s="62" t="s">
-        <v>349</v>
-      </c>
-      <c r="L109" s="64" t="s">
-        <v>129</v>
-      </c>
-      <c r="M109" s="63" t="s">
-        <v>350</v>
-      </c>
-      <c r="N109" s="62">
-        <v>17.579999999999998</v>
-      </c>
-      <c r="O109" s="65" t="s">
-        <v>109</v>
-      </c>
-      <c r="P109" s="65" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q109" s="62">
-        <v>0.87</v>
-      </c>
-      <c r="R109" s="62">
-        <v>0.78</v>
-      </c>
-      <c r="S109" s="66">
-        <v>83.3</v>
-      </c>
-      <c r="T109" s="66">
-        <v>0</v>
-      </c>
-      <c r="U109" s="66">
-        <v>72</v>
       </c>
     </row>
     <row r="110" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.2">
@@ -7895,7 +7943,7 @@
         <v>2035</v>
       </c>
       <c r="B110" s="62" t="s">
-        <v>378</v>
+        <v>345</v>
       </c>
       <c r="C110" s="63" t="s">
         <v>338</v>
@@ -7904,7 +7952,7 @@
         <v>339</v>
       </c>
       <c r="F110" s="62" t="s">
-        <v>376</v>
+        <v>346</v>
       </c>
       <c r="G110" s="62" t="s">
         <v>347</v>
@@ -7919,10 +7967,10 @@
         <v>129</v>
       </c>
       <c r="M110" s="63" t="s">
-        <v>379</v>
+        <v>350</v>
       </c>
       <c r="N110" s="62">
-        <v>16.82</v>
+        <v>17.579999999999998</v>
       </c>
       <c r="O110" s="65" t="s">
         <v>109</v>
@@ -7951,7 +7999,7 @@
         <v>2035</v>
       </c>
       <c r="B111" s="62" t="s">
-        <v>390</v>
+        <v>378</v>
       </c>
       <c r="C111" s="63" t="s">
         <v>338</v>
@@ -7960,22 +8008,22 @@
         <v>339</v>
       </c>
       <c r="F111" s="62" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="G111" s="62" t="s">
-        <v>391</v>
+        <v>347</v>
       </c>
       <c r="H111" s="62" t="s">
-        <v>393</v>
+        <v>348</v>
       </c>
       <c r="K111" s="62" t="s">
-        <v>396</v>
+        <v>349</v>
       </c>
       <c r="L111" s="64" t="s">
         <v>129</v>
       </c>
       <c r="M111" s="63" t="s">
-        <v>397</v>
+        <v>379</v>
       </c>
       <c r="N111" s="62">
         <v>16.82</v>
@@ -8007,7 +8055,7 @@
         <v>2035</v>
       </c>
       <c r="B112" s="62" t="s">
-        <v>408</v>
+        <v>390</v>
       </c>
       <c r="C112" s="63" t="s">
         <v>338</v>
@@ -8016,25 +8064,22 @@
         <v>339</v>
       </c>
       <c r="F112" s="62" t="s">
-        <v>409</v>
+        <v>386</v>
       </c>
       <c r="G112" s="62" t="s">
-        <v>410</v>
+        <v>391</v>
       </c>
       <c r="H112" s="62" t="s">
-        <v>411</v>
-      </c>
-      <c r="I112" s="62" t="s">
-        <v>11</v>
+        <v>393</v>
       </c>
       <c r="K112" s="62" t="s">
-        <v>412</v>
+        <v>396</v>
       </c>
       <c r="L112" s="64" t="s">
-        <v>43</v>
+        <v>129</v>
       </c>
       <c r="M112" s="63" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="N112" s="62">
         <v>16.82</v>
@@ -8060,176 +8105,179 @@
       <c r="U112" s="66">
         <v>72</v>
       </c>
-      <c r="V112" s="62" t="s">
+    </row>
+    <row r="113" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="62">
+        <v>2035</v>
+      </c>
+      <c r="B113" s="62" t="s">
+        <v>408</v>
+      </c>
+      <c r="C113" s="63" t="s">
+        <v>338</v>
+      </c>
+      <c r="D113" s="62" t="s">
+        <v>339</v>
+      </c>
+      <c r="F113" s="62" t="s">
+        <v>409</v>
+      </c>
+      <c r="G113" s="62" t="s">
+        <v>410</v>
+      </c>
+      <c r="H113" s="62" t="s">
+        <v>411</v>
+      </c>
+      <c r="K113" s="62" t="s">
+        <v>412</v>
+      </c>
+      <c r="L113" s="64" t="s">
+        <v>43</v>
+      </c>
+      <c r="M113" s="63" t="s">
+        <v>413</v>
+      </c>
+      <c r="N113" s="62">
+        <v>16.82</v>
+      </c>
+      <c r="O113" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="P113" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q113" s="62">
+        <v>0.87</v>
+      </c>
+      <c r="R113" s="62">
+        <v>0.78</v>
+      </c>
+      <c r="S113" s="66">
+        <v>83.3</v>
+      </c>
+      <c r="T113" s="66">
+        <v>0</v>
+      </c>
+      <c r="U113" s="66">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="114" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="62">
+        <v>2035</v>
+      </c>
+      <c r="B114" s="62" t="s">
+        <v>425</v>
+      </c>
+      <c r="C114" s="63" t="s">
+        <v>338</v>
+      </c>
+      <c r="D114" s="62" t="s">
+        <v>339</v>
+      </c>
+      <c r="F114" s="62" t="s">
+        <v>426</v>
+      </c>
+      <c r="G114" s="62" t="s">
+        <v>428</v>
+      </c>
+      <c r="H114" s="62" t="s">
+        <v>427</v>
+      </c>
+      <c r="I114" s="62" t="s">
+        <v>11</v>
+      </c>
+      <c r="K114" s="62" t="s">
+        <v>412</v>
+      </c>
+      <c r="L114" s="64" t="s">
+        <v>43</v>
+      </c>
+      <c r="M114" s="63" t="s">
+        <v>429</v>
+      </c>
+      <c r="N114" s="62">
+        <v>16.82</v>
+      </c>
+      <c r="O114" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="P114" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q114" s="62">
+        <v>0.87</v>
+      </c>
+      <c r="R114" s="62">
+        <v>0.78</v>
+      </c>
+      <c r="S114" s="66">
+        <v>83.3</v>
+      </c>
+      <c r="T114" s="66">
+        <v>0</v>
+      </c>
+      <c r="U114" s="66">
+        <v>72</v>
+      </c>
+      <c r="V114" s="62" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="113" spans="1:22" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="24">
+    <row r="115" spans="1:22" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="24">
         <v>2050</v>
       </c>
-      <c r="B113" s="24" t="s">
+      <c r="B115" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="C113" s="24" t="s">
+      <c r="C115" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="D113" s="24" t="s">
+      <c r="D115" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="F113" s="24" t="s">
+      <c r="F115" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="G113" s="24" t="s">
+      <c r="G115" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="H113" s="25" t="s">
+      <c r="H115" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="K113" s="24" t="s">
+      <c r="K115" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="L113" s="26" t="s">
+      <c r="L115" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="M113" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="N113" s="24">
+      <c r="M115" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="N115" s="24">
         <v>17.440000000000001</v>
       </c>
-      <c r="O113" s="47">
+      <c r="O115" s="47">
         <v>-0.33</v>
       </c>
-      <c r="P113" s="47">
-        <v>0</v>
-      </c>
-      <c r="Q113" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="R113" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="S113" s="72" t="s">
-        <v>109</v>
-      </c>
-      <c r="T113" s="72" t="s">
-        <v>109</v>
-      </c>
-      <c r="U113" s="72" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="114" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="53">
-        <v>2050</v>
-      </c>
-      <c r="B114" s="53" t="s">
-        <v>351</v>
-      </c>
-      <c r="C114" s="53" t="s">
-        <v>338</v>
-      </c>
-      <c r="D114" s="53" t="s">
-        <v>339</v>
-      </c>
-      <c r="F114" s="53" t="s">
-        <v>353</v>
-      </c>
-      <c r="G114" s="53" t="s">
-        <v>342</v>
-      </c>
-      <c r="H114" s="52" t="s">
-        <v>343</v>
-      </c>
-      <c r="K114" s="53" t="s">
-        <v>344</v>
-      </c>
-      <c r="L114" s="52" t="s">
-        <v>16</v>
-      </c>
-      <c r="M114" s="53" t="s">
-        <v>356</v>
-      </c>
-      <c r="N114" s="53">
-        <v>19.13</v>
-      </c>
-      <c r="O114" s="67" t="s">
-        <v>109</v>
-      </c>
-      <c r="P114" s="67" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q114" s="53">
-        <v>0.87</v>
-      </c>
-      <c r="R114" s="53">
-        <v>0.78</v>
-      </c>
-      <c r="S114" s="56">
-        <v>83.3</v>
-      </c>
-      <c r="T114" s="56">
-        <v>0</v>
-      </c>
-      <c r="U114" s="56">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="115" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="53">
-        <v>2050</v>
-      </c>
-      <c r="B115" s="53" t="s">
-        <v>380</v>
-      </c>
-      <c r="C115" s="53" t="s">
-        <v>338</v>
-      </c>
-      <c r="D115" s="53" t="s">
-        <v>339</v>
-      </c>
-      <c r="F115" s="53" t="s">
-        <v>376</v>
-      </c>
-      <c r="G115" s="53" t="s">
-        <v>342</v>
-      </c>
-      <c r="H115" s="52" t="s">
-        <v>343</v>
-      </c>
-      <c r="K115" s="53" t="s">
-        <v>344</v>
-      </c>
-      <c r="L115" s="52" t="s">
-        <v>16</v>
-      </c>
-      <c r="M115" s="53" t="s">
-        <v>381</v>
-      </c>
-      <c r="N115" s="53">
-        <v>18.420000000000002</v>
-      </c>
-      <c r="O115" s="67" t="s">
-        <v>109</v>
-      </c>
-      <c r="P115" s="67" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q115" s="53">
-        <v>0.87</v>
-      </c>
-      <c r="R115" s="53">
-        <v>0.78</v>
-      </c>
-      <c r="S115" s="56">
-        <v>83.3</v>
-      </c>
-      <c r="T115" s="56">
-        <v>0</v>
-      </c>
-      <c r="U115" s="56">
-        <v>72</v>
+      <c r="P115" s="47">
+        <v>0</v>
+      </c>
+      <c r="Q115" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="R115" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="S115" s="72" t="s">
+        <v>109</v>
+      </c>
+      <c r="T115" s="72" t="s">
+        <v>109</v>
+      </c>
+      <c r="U115" s="72" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="116" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.2">
@@ -8237,7 +8285,7 @@
         <v>2050</v>
       </c>
       <c r="B116" s="53" t="s">
-        <v>388</v>
+        <v>351</v>
       </c>
       <c r="C116" s="53" t="s">
         <v>338</v>
@@ -8246,25 +8294,25 @@
         <v>339</v>
       </c>
       <c r="F116" s="53" t="s">
-        <v>386</v>
+        <v>353</v>
       </c>
       <c r="G116" s="53" t="s">
-        <v>387</v>
+        <v>342</v>
       </c>
       <c r="H116" s="52" t="s">
-        <v>392</v>
+        <v>343</v>
       </c>
       <c r="K116" s="53" t="s">
-        <v>394</v>
+        <v>344</v>
       </c>
       <c r="L116" s="52" t="s">
         <v>16</v>
       </c>
       <c r="M116" s="53" t="s">
-        <v>400</v>
+        <v>356</v>
       </c>
       <c r="N116" s="53">
-        <v>18.420000000000002</v>
+        <v>19.13</v>
       </c>
       <c r="O116" s="67" t="s">
         <v>109</v>
@@ -8293,7 +8341,7 @@
         <v>2050</v>
       </c>
       <c r="B117" s="53" t="s">
-        <v>414</v>
+        <v>380</v>
       </c>
       <c r="C117" s="53" t="s">
         <v>338</v>
@@ -8302,25 +8350,22 @@
         <v>339</v>
       </c>
       <c r="F117" s="53" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="G117" s="53" t="s">
-        <v>407</v>
+        <v>342</v>
       </c>
       <c r="H117" s="52" t="s">
-        <v>406</v>
-      </c>
-      <c r="I117" s="53" t="s">
-        <v>11</v>
+        <v>343</v>
       </c>
       <c r="K117" s="53" t="s">
-        <v>404</v>
+        <v>344</v>
       </c>
       <c r="L117" s="52" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="M117" s="53" t="s">
-        <v>418</v>
+        <v>381</v>
       </c>
       <c r="N117" s="53">
         <v>18.420000000000002</v>
@@ -8346,176 +8391,179 @@
       <c r="U117" s="56">
         <v>72</v>
       </c>
-      <c r="V117" s="53" t="s">
+    </row>
+    <row r="118" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="53">
+        <v>2050</v>
+      </c>
+      <c r="B118" s="53" t="s">
+        <v>388</v>
+      </c>
+      <c r="C118" s="53" t="s">
+        <v>338</v>
+      </c>
+      <c r="D118" s="53" t="s">
+        <v>339</v>
+      </c>
+      <c r="F118" s="53" t="s">
+        <v>386</v>
+      </c>
+      <c r="G118" s="53" t="s">
+        <v>387</v>
+      </c>
+      <c r="H118" s="52" t="s">
+        <v>392</v>
+      </c>
+      <c r="K118" s="53" t="s">
+        <v>394</v>
+      </c>
+      <c r="L118" s="52" t="s">
+        <v>16</v>
+      </c>
+      <c r="M118" s="53" t="s">
+        <v>400</v>
+      </c>
+      <c r="N118" s="53">
+        <v>18.420000000000002</v>
+      </c>
+      <c r="O118" s="67" t="s">
+        <v>109</v>
+      </c>
+      <c r="P118" s="67" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q118" s="53">
+        <v>0.87</v>
+      </c>
+      <c r="R118" s="53">
+        <v>0.78</v>
+      </c>
+      <c r="S118" s="56">
+        <v>83.3</v>
+      </c>
+      <c r="T118" s="56">
+        <v>0</v>
+      </c>
+      <c r="U118" s="56">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="119" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A119" s="53">
+        <v>2050</v>
+      </c>
+      <c r="B119" s="53" t="s">
+        <v>414</v>
+      </c>
+      <c r="C119" s="53" t="s">
+        <v>338</v>
+      </c>
+      <c r="D119" s="53" t="s">
+        <v>339</v>
+      </c>
+      <c r="F119" s="53" t="s">
+        <v>386</v>
+      </c>
+      <c r="G119" s="53" t="s">
+        <v>407</v>
+      </c>
+      <c r="H119" s="52" t="s">
+        <v>406</v>
+      </c>
+      <c r="K119" s="53" t="s">
+        <v>404</v>
+      </c>
+      <c r="L119" s="52" t="s">
+        <v>42</v>
+      </c>
+      <c r="M119" s="53" t="s">
+        <v>418</v>
+      </c>
+      <c r="N119" s="53">
+        <v>18.420000000000002</v>
+      </c>
+      <c r="O119" s="67" t="s">
+        <v>109</v>
+      </c>
+      <c r="P119" s="67" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q119" s="53">
+        <v>0.87</v>
+      </c>
+      <c r="R119" s="53">
+        <v>0.78</v>
+      </c>
+      <c r="S119" s="56">
+        <v>83.3</v>
+      </c>
+      <c r="T119" s="56">
+        <v>0</v>
+      </c>
+      <c r="U119" s="56">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="120" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="53">
+        <v>2050</v>
+      </c>
+      <c r="B120" s="53" t="s">
+        <v>430</v>
+      </c>
+      <c r="C120" s="53" t="s">
+        <v>338</v>
+      </c>
+      <c r="D120" s="53" t="s">
+        <v>339</v>
+      </c>
+      <c r="F120" s="53" t="s">
+        <v>426</v>
+      </c>
+      <c r="G120" s="53" t="s">
+        <v>428</v>
+      </c>
+      <c r="H120" s="52" t="s">
+        <v>427</v>
+      </c>
+      <c r="I120" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="K120" s="53" t="s">
+        <v>404</v>
+      </c>
+      <c r="L120" s="52" t="s">
+        <v>42</v>
+      </c>
+      <c r="M120" s="53" t="s">
+        <v>431</v>
+      </c>
+      <c r="N120" s="53">
+        <v>18.420000000000002</v>
+      </c>
+      <c r="O120" s="67" t="s">
+        <v>109</v>
+      </c>
+      <c r="P120" s="67" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q120" s="53">
+        <v>0.87</v>
+      </c>
+      <c r="R120" s="53">
+        <v>0.78</v>
+      </c>
+      <c r="S120" s="56">
+        <v>83.3</v>
+      </c>
+      <c r="T120" s="56">
+        <v>0</v>
+      </c>
+      <c r="U120" s="56">
+        <v>72</v>
+      </c>
+      <c r="V120" s="53" t="s">
         <v>362</v>
-      </c>
-    </row>
-    <row r="118" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="68">
-        <v>2050</v>
-      </c>
-      <c r="B118" s="68" t="s">
-        <v>352</v>
-      </c>
-      <c r="C118" s="68" t="s">
-        <v>338</v>
-      </c>
-      <c r="D118" s="68" t="s">
-        <v>339</v>
-      </c>
-      <c r="F118" s="68" t="s">
-        <v>354</v>
-      </c>
-      <c r="G118" s="68" t="s">
-        <v>347</v>
-      </c>
-      <c r="H118" s="69" t="s">
-        <v>348</v>
-      </c>
-      <c r="K118" s="68" t="s">
-        <v>355</v>
-      </c>
-      <c r="L118" s="69" t="s">
-        <v>44</v>
-      </c>
-      <c r="M118" s="68" t="s">
-        <v>357</v>
-      </c>
-      <c r="N118" s="68">
-        <v>19.13</v>
-      </c>
-      <c r="O118" s="70" t="s">
-        <v>109</v>
-      </c>
-      <c r="P118" s="70" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q118" s="68">
-        <v>0.87</v>
-      </c>
-      <c r="R118" s="68">
-        <v>0.78</v>
-      </c>
-      <c r="S118" s="71">
-        <v>83.3</v>
-      </c>
-      <c r="T118" s="71">
-        <v>0</v>
-      </c>
-      <c r="U118" s="71">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="119" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="68">
-        <v>2050</v>
-      </c>
-      <c r="B119" s="68" t="s">
-        <v>382</v>
-      </c>
-      <c r="C119" s="68" t="s">
-        <v>338</v>
-      </c>
-      <c r="D119" s="68" t="s">
-        <v>339</v>
-      </c>
-      <c r="F119" s="68" t="s">
-        <v>354</v>
-      </c>
-      <c r="G119" s="68" t="s">
-        <v>347</v>
-      </c>
-      <c r="H119" s="69" t="s">
-        <v>348</v>
-      </c>
-      <c r="K119" s="68" t="s">
-        <v>355</v>
-      </c>
-      <c r="L119" s="69" t="s">
-        <v>44</v>
-      </c>
-      <c r="M119" s="68" t="s">
-        <v>357</v>
-      </c>
-      <c r="N119" s="68">
-        <v>18.420000000000002</v>
-      </c>
-      <c r="O119" s="70" t="s">
-        <v>109</v>
-      </c>
-      <c r="P119" s="70" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q119" s="68">
-        <v>0.87</v>
-      </c>
-      <c r="R119" s="68">
-        <v>0.78</v>
-      </c>
-      <c r="S119" s="71">
-        <v>83.3</v>
-      </c>
-      <c r="T119" s="71">
-        <v>0</v>
-      </c>
-      <c r="U119" s="71">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="120" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="68">
-        <v>2050</v>
-      </c>
-      <c r="B120" s="68" t="s">
-        <v>389</v>
-      </c>
-      <c r="C120" s="68" t="s">
-        <v>338</v>
-      </c>
-      <c r="D120" s="68" t="s">
-        <v>339</v>
-      </c>
-      <c r="F120" s="68" t="s">
-        <v>386</v>
-      </c>
-      <c r="G120" s="68" t="s">
-        <v>391</v>
-      </c>
-      <c r="H120" s="69" t="s">
-        <v>393</v>
-      </c>
-      <c r="K120" s="68" t="s">
-        <v>395</v>
-      </c>
-      <c r="L120" s="69" t="s">
-        <v>44</v>
-      </c>
-      <c r="M120" s="68" t="s">
-        <v>398</v>
-      </c>
-      <c r="N120" s="68">
-        <v>18.420000000000002</v>
-      </c>
-      <c r="O120" s="70" t="s">
-        <v>109</v>
-      </c>
-      <c r="P120" s="70" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q120" s="68">
-        <v>0.87</v>
-      </c>
-      <c r="R120" s="68">
-        <v>0.78</v>
-      </c>
-      <c r="S120" s="71">
-        <v>83.3</v>
-      </c>
-      <c r="T120" s="71">
-        <v>0</v>
-      </c>
-      <c r="U120" s="71">
-        <v>72</v>
       </c>
     </row>
     <row r="121" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
@@ -8523,7 +8571,7 @@
         <v>2050</v>
       </c>
       <c r="B121" s="68" t="s">
-        <v>415</v>
+        <v>352</v>
       </c>
       <c r="C121" s="68" t="s">
         <v>338</v>
@@ -8532,28 +8580,25 @@
         <v>339</v>
       </c>
       <c r="F121" s="68" t="s">
-        <v>386</v>
+        <v>354</v>
       </c>
       <c r="G121" s="68" t="s">
-        <v>410</v>
+        <v>347</v>
       </c>
       <c r="H121" s="69" t="s">
-        <v>411</v>
-      </c>
-      <c r="I121" s="68" t="s">
-        <v>11</v>
+        <v>348</v>
       </c>
       <c r="K121" s="68" t="s">
-        <v>416</v>
+        <v>355</v>
       </c>
       <c r="L121" s="69" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M121" s="68" t="s">
-        <v>417</v>
+        <v>357</v>
       </c>
       <c r="N121" s="68">
-        <v>18.420000000000002</v>
+        <v>19.13</v>
       </c>
       <c r="O121" s="70" t="s">
         <v>109</v>
@@ -8576,7 +8621,234 @@
       <c r="U121" s="71">
         <v>72</v>
       </c>
-      <c r="V121" s="68" t="s">
+    </row>
+    <row r="122" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="68">
+        <v>2050</v>
+      </c>
+      <c r="B122" s="68" t="s">
+        <v>382</v>
+      </c>
+      <c r="C122" s="68" t="s">
+        <v>338</v>
+      </c>
+      <c r="D122" s="68" t="s">
+        <v>339</v>
+      </c>
+      <c r="F122" s="68" t="s">
+        <v>354</v>
+      </c>
+      <c r="G122" s="68" t="s">
+        <v>347</v>
+      </c>
+      <c r="H122" s="69" t="s">
+        <v>348</v>
+      </c>
+      <c r="K122" s="68" t="s">
+        <v>355</v>
+      </c>
+      <c r="L122" s="69" t="s">
+        <v>44</v>
+      </c>
+      <c r="M122" s="68" t="s">
+        <v>357</v>
+      </c>
+      <c r="N122" s="68">
+        <v>18.420000000000002</v>
+      </c>
+      <c r="O122" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="P122" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q122" s="68">
+        <v>0.87</v>
+      </c>
+      <c r="R122" s="68">
+        <v>0.78</v>
+      </c>
+      <c r="S122" s="71">
+        <v>83.3</v>
+      </c>
+      <c r="T122" s="71">
+        <v>0</v>
+      </c>
+      <c r="U122" s="71">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="123" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="68">
+        <v>2050</v>
+      </c>
+      <c r="B123" s="68" t="s">
+        <v>389</v>
+      </c>
+      <c r="C123" s="68" t="s">
+        <v>338</v>
+      </c>
+      <c r="D123" s="68" t="s">
+        <v>339</v>
+      </c>
+      <c r="F123" s="68" t="s">
+        <v>386</v>
+      </c>
+      <c r="G123" s="68" t="s">
+        <v>391</v>
+      </c>
+      <c r="H123" s="69" t="s">
+        <v>393</v>
+      </c>
+      <c r="K123" s="68" t="s">
+        <v>395</v>
+      </c>
+      <c r="L123" s="69" t="s">
+        <v>44</v>
+      </c>
+      <c r="M123" s="68" t="s">
+        <v>398</v>
+      </c>
+      <c r="N123" s="68">
+        <v>18.420000000000002</v>
+      </c>
+      <c r="O123" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="P123" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q123" s="68">
+        <v>0.87</v>
+      </c>
+      <c r="R123" s="68">
+        <v>0.78</v>
+      </c>
+      <c r="S123" s="71">
+        <v>83.3</v>
+      </c>
+      <c r="T123" s="71">
+        <v>0</v>
+      </c>
+      <c r="U123" s="71">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="124" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="68">
+        <v>2050</v>
+      </c>
+      <c r="B124" s="68" t="s">
+        <v>415</v>
+      </c>
+      <c r="C124" s="68" t="s">
+        <v>338</v>
+      </c>
+      <c r="D124" s="68" t="s">
+        <v>339</v>
+      </c>
+      <c r="F124" s="68" t="s">
+        <v>386</v>
+      </c>
+      <c r="G124" s="68" t="s">
+        <v>410</v>
+      </c>
+      <c r="H124" s="69" t="s">
+        <v>411</v>
+      </c>
+      <c r="K124" s="68" t="s">
+        <v>416</v>
+      </c>
+      <c r="L124" s="69" t="s">
+        <v>42</v>
+      </c>
+      <c r="M124" s="68" t="s">
+        <v>417</v>
+      </c>
+      <c r="N124" s="68">
+        <v>18.420000000000002</v>
+      </c>
+      <c r="O124" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="P124" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q124" s="68">
+        <v>0.87</v>
+      </c>
+      <c r="R124" s="68">
+        <v>0.78</v>
+      </c>
+      <c r="S124" s="71">
+        <v>83.3</v>
+      </c>
+      <c r="T124" s="71">
+        <v>0</v>
+      </c>
+      <c r="U124" s="71">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="125" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="68">
+        <v>2050</v>
+      </c>
+      <c r="B125" s="68" t="s">
+        <v>432</v>
+      </c>
+      <c r="C125" s="68" t="s">
+        <v>338</v>
+      </c>
+      <c r="D125" s="68" t="s">
+        <v>339</v>
+      </c>
+      <c r="F125" s="68" t="s">
+        <v>426</v>
+      </c>
+      <c r="G125" s="68" t="s">
+        <v>428</v>
+      </c>
+      <c r="H125" s="69" t="s">
+        <v>427</v>
+      </c>
+      <c r="I125" s="68" t="s">
+        <v>11</v>
+      </c>
+      <c r="K125" s="68" t="s">
+        <v>416</v>
+      </c>
+      <c r="L125" s="69" t="s">
+        <v>42</v>
+      </c>
+      <c r="M125" s="68" t="s">
+        <v>433</v>
+      </c>
+      <c r="N125" s="68">
+        <v>18.420000000000002</v>
+      </c>
+      <c r="O125" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="P125" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q125" s="68">
+        <v>0.87</v>
+      </c>
+      <c r="R125" s="68">
+        <v>0.78</v>
+      </c>
+      <c r="S125" s="71">
+        <v>83.3</v>
+      </c>
+      <c r="T125" s="71">
+        <v>0</v>
+      </c>
+      <c r="U125" s="71">
+        <v>72</v>
+      </c>
+      <c r="V125" s="68" t="s">
         <v>358</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add NoProject 05b, Plan 06, 06b
But 2050_TM160_DBP_NoProject_05b isn't current yet
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\config_RTP2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64695671-E56D-43A5-BF1A-F8A59C6E22EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CFF8313-2D0C-4619-8C8A-5A457B0B0A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2388" yWindow="3252" windowWidth="23016" windowHeight="12960" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
+    <workbookView xWindow="1215" yWindow="4290" windowWidth="19710" windowHeight="9855" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelRuns" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1372" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1439" uniqueCount="452">
   <si>
     <t>year</t>
   </si>
@@ -1356,6 +1356,60 @@
   </si>
   <si>
     <t>https://app.asana.com/0/1204085012544660/1207012741527411/f</t>
+  </si>
+  <si>
+    <t>2035_TM160_DBP_NoProject_05b</t>
+  </si>
+  <si>
+    <t>Updated landuse/popsyn (fix too many persons), orig AOC</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1182463234225195/1207086029250362/f</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1182463234225195/1207095052585768/f</t>
+  </si>
+  <si>
+    <t>2050_TM160_DBP_NoProject_05b</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1182463234225195/1207094549470908/f</t>
+  </si>
+  <si>
+    <t>running</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1182463234225195/1207094551343878/f</t>
+  </si>
+  <si>
+    <t>2035_TM160_DBP_Plan_06</t>
+  </si>
+  <si>
+    <t>2035_TM160_DBP_Plan_06b</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1182463234225195/1207094549470912/f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PBA50Plus_Draft_Blueprint_v2b_zoningclip </t>
+  </si>
+  <si>
+    <t>M:\urban_modeling\baus\PBA50Plus\PBA50Plus_DBP_InitialRun\outputs\PBA50Plus_Draft_Blueprint_v2b_zoningclip</t>
+  </si>
+  <si>
+    <t>Update landuse/popsyn</t>
+  </si>
+  <si>
+    <t>Original AOC</t>
+  </si>
+  <si>
+    <t>2050_TM160_DBP_Plan_06</t>
+  </si>
+  <si>
+    <t>2050_TM160_DBP_Plan_06b</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1182463234225195/1207094549470916/f</t>
   </si>
 </sst>
 </file>
@@ -1418,7 +1472,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1497,6 +1551,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -1528,7 +1588,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1684,6 +1744,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2012,36 +2073,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9564CC59-3725-4FDA-8BF2-0F68CB1B6F5A}">
-  <dimension ref="A1:V125"/>
+  <dimension ref="A1:V131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C111" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J6" sqref="J6"/>
+      <selection pane="bottomRight" activeCell="A131" sqref="A131"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="7" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="42.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="42.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="23" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="6.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="22.33203125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11.33203125" style="10" customWidth="1"/>
-    <col min="13" max="13" width="17.5546875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="8.33203125" style="1" customWidth="1"/>
-    <col min="15" max="16" width="9.33203125" style="43"/>
-    <col min="17" max="16384" width="9.33203125" style="1"/>
+    <col min="8" max="8" width="8.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="6.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="22.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" style="10" customWidth="1"/>
+    <col min="13" max="13" width="17.5703125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="8.28515625" style="1" customWidth="1"/>
+    <col min="15" max="16" width="9.28515625" style="43"/>
+    <col min="17" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="5" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2109,7 +2170,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="2" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="19">
         <v>2005</v>
       </c>
@@ -2162,7 +2223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="30">
         <v>2005</v>
       </c>
@@ -2218,7 +2279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="30">
         <v>2005</v>
       </c>
@@ -2273,7 +2334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="30">
         <v>2005</v>
       </c>
@@ -2328,7 +2389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="30">
         <v>2005</v>
       </c>
@@ -2393,7 +2454,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="7" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="52">
         <v>2015</v>
       </c>
@@ -2434,7 +2495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="34">
         <v>2015</v>
       </c>
@@ -2480,7 +2541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="34">
         <v>2015</v>
       </c>
@@ -2533,7 +2594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="34">
         <v>2015</v>
       </c>
@@ -2586,7 +2647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="34">
         <v>2015</v>
       </c>
@@ -2639,7 +2700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="34">
         <v>2015</v>
       </c>
@@ -2695,7 +2756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="34">
         <v>2015</v>
       </c>
@@ -2751,7 +2812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="34">
         <v>2015</v>
       </c>
@@ -2807,7 +2868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="34">
         <v>2015</v>
       </c>
@@ -2867,7 +2928,7 @@
       </c>
       <c r="V15" s="57"/>
     </row>
-    <row r="16" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="34">
         <v>2015</v>
       </c>
@@ -2929,7 +2990,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>2023</v>
       </c>
@@ -2975,7 +3036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>2023</v>
       </c>
@@ -3021,7 +3082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>2023</v>
       </c>
@@ -3067,7 +3128,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>2023</v>
       </c>
@@ -3113,7 +3174,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>2023</v>
       </c>
@@ -3159,7 +3220,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>2023</v>
       </c>
@@ -3205,7 +3266,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>2023</v>
       </c>
@@ -3251,7 +3312,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>2023</v>
       </c>
@@ -3297,7 +3358,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>2023</v>
       </c>
@@ -3343,7 +3404,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>2023</v>
       </c>
@@ -3389,7 +3450,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>2023</v>
       </c>
@@ -3435,7 +3496,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>2023</v>
       </c>
@@ -3481,7 +3542,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>2023</v>
       </c>
@@ -3527,7 +3588,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>2023</v>
       </c>
@@ -3573,7 +3634,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>2023</v>
       </c>
@@ -3619,7 +3680,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>2023</v>
       </c>
@@ -3665,7 +3726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>2023</v>
       </c>
@@ -3711,7 +3772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>2023</v>
       </c>
@@ -3757,7 +3818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>2023</v>
       </c>
@@ -3801,7 +3862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>2023</v>
       </c>
@@ -3850,7 +3911,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>2023</v>
       </c>
@@ -3897,7 +3958,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>2023</v>
       </c>
@@ -3944,7 +4005,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>2023</v>
       </c>
@@ -4000,7 +4061,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>2023</v>
       </c>
@@ -4056,7 +4117,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>2023</v>
       </c>
@@ -4112,7 +4173,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>2023</v>
       </c>
@@ -4168,7 +4229,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>2023</v>
       </c>
@@ -4224,7 +4285,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>2023</v>
       </c>
@@ -4280,7 +4341,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>2023</v>
       </c>
@@ -4336,7 +4397,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>2023</v>
       </c>
@@ -4392,7 +4453,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>2023</v>
       </c>
@@ -4448,7 +4509,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>2023</v>
       </c>
@@ -4504,7 +4565,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>2023</v>
       </c>
@@ -4560,7 +4621,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>2023</v>
       </c>
@@ -4616,7 +4677,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>2023</v>
       </c>
@@ -4672,7 +4733,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>2023</v>
       </c>
@@ -4728,7 +4789,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>2023</v>
       </c>
@@ -4784,7 +4845,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>2023</v>
       </c>
@@ -4840,7 +4901,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>2023</v>
       </c>
@@ -4896,7 +4957,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>2023</v>
       </c>
@@ -4952,7 +5013,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>2023</v>
       </c>
@@ -5008,7 +5069,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>2023</v>
       </c>
@@ -5064,7 +5125,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>2023</v>
       </c>
@@ -5120,7 +5181,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>2023</v>
       </c>
@@ -5176,7 +5237,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>2023</v>
       </c>
@@ -5232,7 +5293,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>2023</v>
       </c>
@@ -5288,7 +5349,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>2023</v>
       </c>
@@ -5344,7 +5405,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>2023</v>
       </c>
@@ -5403,7 +5464,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>2023</v>
       </c>
@@ -5459,7 +5520,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>2023</v>
       </c>
@@ -5518,7 +5579,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>2023</v>
       </c>
@@ -5577,7 +5638,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>2023</v>
       </c>
@@ -5636,7 +5697,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>2023</v>
       </c>
@@ -5695,7 +5756,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="70" spans="1:22" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:22" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>2023</v>
       </c>
@@ -5751,7 +5812,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="71" spans="1:22" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:22" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>2023</v>
       </c>
@@ -5807,7 +5868,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>2023</v>
       </c>
@@ -5863,7 +5924,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>2023</v>
       </c>
@@ -5919,7 +5980,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>2023</v>
       </c>
@@ -5975,7 +6036,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>2023</v>
       </c>
@@ -6034,7 +6095,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>2023</v>
       </c>
@@ -6094,7 +6155,7 @@
       </c>
       <c r="V76" s="73"/>
     </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>2023</v>
       </c>
@@ -6156,7 +6217,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="78" spans="1:22" s="27" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:22" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="27">
         <v>2025</v>
       </c>
@@ -6184,7 +6245,7 @@
       <c r="T78" s="29"/>
       <c r="U78" s="29"/>
     </row>
-    <row r="79" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="15">
         <v>2035</v>
       </c>
@@ -6243,7 +6304,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="80" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="12">
         <v>2035</v>
       </c>
@@ -6299,7 +6360,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="81" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="12">
         <v>2035</v>
       </c>
@@ -6355,7 +6416,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="82" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="12">
         <v>2035</v>
       </c>
@@ -6411,7 +6472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="12">
         <v>2035</v>
       </c>
@@ -6467,7 +6528,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="84" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="12">
         <v>2035</v>
       </c>
@@ -6523,7 +6584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="12">
         <v>2035</v>
       </c>
@@ -6579,7 +6640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="12">
         <v>2035</v>
       </c>
@@ -6635,7 +6696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="12">
         <v>2035</v>
       </c>
@@ -6691,7 +6752,7 @@
         <v>41.25</v>
       </c>
     </row>
-    <row r="88" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A88" s="12">
         <v>2035</v>
       </c>
@@ -6747,7 +6808,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="89" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" s="12">
         <v>2035</v>
       </c>
@@ -6803,7 +6864,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="90" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A90" s="12">
         <v>2035</v>
       </c>
@@ -6859,7 +6920,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="91" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="12">
         <v>2035</v>
       </c>
@@ -6915,7 +6976,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="92" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="12">
         <v>2035</v>
       </c>
@@ -6971,7 +7032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A93" s="12">
         <v>2035</v>
       </c>
@@ -7027,7 +7088,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="94" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A94" s="12">
         <v>2035</v>
       </c>
@@ -7083,7 +7144,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="95" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A95" s="12">
         <v>2035</v>
       </c>
@@ -7139,7 +7200,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="96" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A96" s="12">
         <v>2035</v>
       </c>
@@ -7195,7 +7256,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="97" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A97" s="12">
         <v>2035</v>
       </c>
@@ -7251,7 +7312,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="98" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="12">
         <v>2035</v>
       </c>
@@ -7307,7 +7368,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="99" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A99" s="12">
         <v>2035</v>
       </c>
@@ -7363,7 +7424,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="100" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A100" s="12">
         <v>2035</v>
       </c>
@@ -7419,7 +7480,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="101" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A101" s="12">
         <v>2035</v>
       </c>
@@ -7475,7 +7536,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="102" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A102" s="12">
         <v>2035</v>
       </c>
@@ -7534,7 +7595,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="103" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A103" s="12">
         <v>2035</v>
       </c>
@@ -7590,7 +7651,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="104" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A104" s="12">
         <v>2035</v>
       </c>
@@ -7655,7 +7716,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="105" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A105" s="58">
         <v>2035</v>
       </c>
@@ -7711,7 +7772,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="106" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A106" s="58">
         <v>2035</v>
       </c>
@@ -7767,7 +7828,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="107" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A107" s="58">
         <v>2035</v>
       </c>
@@ -7823,7 +7884,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="108" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A108" s="58">
         <v>2035</v>
       </c>
@@ -7882,7 +7943,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="109" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A109" s="58">
         <v>2035</v>
       </c>
@@ -7904,9 +7965,6 @@
       <c r="H109" s="58" t="s">
         <v>423</v>
       </c>
-      <c r="I109" s="58" t="s">
-        <v>11</v>
-      </c>
       <c r="J109" s="58" t="s">
         <v>402</v>
       </c>
@@ -7943,72 +8001,75 @@
       <c r="U109" s="61">
         <v>72</v>
       </c>
-      <c r="V109" s="58" t="s">
+    </row>
+    <row r="110" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="58">
+        <v>2035</v>
+      </c>
+      <c r="B110" s="58" t="s">
+        <v>434</v>
+      </c>
+      <c r="C110" s="58" t="s">
+        <v>338</v>
+      </c>
+      <c r="D110" s="58" t="s">
+        <v>339</v>
+      </c>
+      <c r="F110" s="58" t="s">
+        <v>435</v>
+      </c>
+      <c r="G110" s="58" t="s">
+        <v>422</v>
+      </c>
+      <c r="H110" s="58" t="s">
+        <v>423</v>
+      </c>
+      <c r="I110" s="58" t="s">
+        <v>11</v>
+      </c>
+      <c r="K110" s="58" t="s">
+        <v>404</v>
+      </c>
+      <c r="L110" s="59" t="s">
+        <v>110</v>
+      </c>
+      <c r="M110" s="58" t="s">
+        <v>436</v>
+      </c>
+      <c r="N110" s="58">
+        <v>17.579999999999998</v>
+      </c>
+      <c r="O110" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="P110" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q110" s="58">
+        <v>0.87</v>
+      </c>
+      <c r="R110" s="58">
+        <v>0.78</v>
+      </c>
+      <c r="S110" s="61">
+        <v>83.3</v>
+      </c>
+      <c r="T110" s="61">
+        <v>0</v>
+      </c>
+      <c r="U110" s="61">
+        <v>72</v>
+      </c>
+      <c r="V110" s="58" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="110" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="62">
-        <v>2035</v>
-      </c>
-      <c r="B110" s="62" t="s">
-        <v>345</v>
-      </c>
-      <c r="C110" s="63" t="s">
-        <v>338</v>
-      </c>
-      <c r="D110" s="62" t="s">
-        <v>339</v>
-      </c>
-      <c r="F110" s="62" t="s">
-        <v>346</v>
-      </c>
-      <c r="G110" s="62" t="s">
-        <v>347</v>
-      </c>
-      <c r="H110" s="62" t="s">
-        <v>348</v>
-      </c>
-      <c r="K110" s="62" t="s">
-        <v>349</v>
-      </c>
-      <c r="L110" s="64" t="s">
-        <v>129</v>
-      </c>
-      <c r="M110" s="63" t="s">
-        <v>350</v>
-      </c>
-      <c r="N110" s="62">
-        <v>17.579999999999998</v>
-      </c>
-      <c r="O110" s="65" t="s">
-        <v>109</v>
-      </c>
-      <c r="P110" s="65" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q110" s="62">
-        <v>0.87</v>
-      </c>
-      <c r="R110" s="62">
-        <v>0.78</v>
-      </c>
-      <c r="S110" s="66">
-        <v>83.3</v>
-      </c>
-      <c r="T110" s="66">
-        <v>0</v>
-      </c>
-      <c r="U110" s="66">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="111" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A111" s="62">
         <v>2035</v>
       </c>
       <c r="B111" s="62" t="s">
-        <v>378</v>
+        <v>345</v>
       </c>
       <c r="C111" s="63" t="s">
         <v>338</v>
@@ -8017,7 +8078,7 @@
         <v>339</v>
       </c>
       <c r="F111" s="62" t="s">
-        <v>376</v>
+        <v>346</v>
       </c>
       <c r="G111" s="62" t="s">
         <v>347</v>
@@ -8032,10 +8093,10 @@
         <v>129</v>
       </c>
       <c r="M111" s="63" t="s">
-        <v>379</v>
+        <v>350</v>
       </c>
       <c r="N111" s="62">
-        <v>16.82</v>
+        <v>17.579999999999998</v>
       </c>
       <c r="O111" s="65" t="s">
         <v>109</v>
@@ -8059,12 +8120,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="112" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A112" s="62">
         <v>2035</v>
       </c>
       <c r="B112" s="62" t="s">
-        <v>390</v>
+        <v>378</v>
       </c>
       <c r="C112" s="63" t="s">
         <v>338</v>
@@ -8073,22 +8134,22 @@
         <v>339</v>
       </c>
       <c r="F112" s="62" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="G112" s="62" t="s">
-        <v>391</v>
+        <v>347</v>
       </c>
       <c r="H112" s="62" t="s">
-        <v>393</v>
+        <v>348</v>
       </c>
       <c r="K112" s="62" t="s">
-        <v>396</v>
+        <v>349</v>
       </c>
       <c r="L112" s="64" t="s">
         <v>129</v>
       </c>
       <c r="M112" s="63" t="s">
-        <v>397</v>
+        <v>379</v>
       </c>
       <c r="N112" s="62">
         <v>16.82</v>
@@ -8115,12 +8176,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="113" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A113" s="62">
         <v>2035</v>
       </c>
       <c r="B113" s="62" t="s">
-        <v>408</v>
+        <v>390</v>
       </c>
       <c r="C113" s="63" t="s">
         <v>338</v>
@@ -8129,25 +8190,22 @@
         <v>339</v>
       </c>
       <c r="F113" s="62" t="s">
-        <v>409</v>
+        <v>386</v>
       </c>
       <c r="G113" s="62" t="s">
-        <v>410</v>
+        <v>391</v>
       </c>
       <c r="H113" s="62" t="s">
-        <v>411</v>
-      </c>
-      <c r="J113" s="62" t="s">
-        <v>402</v>
+        <v>393</v>
       </c>
       <c r="K113" s="62" t="s">
-        <v>412</v>
+        <v>396</v>
       </c>
       <c r="L113" s="64" t="s">
-        <v>43</v>
+        <v>129</v>
       </c>
       <c r="M113" s="63" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="N113" s="62">
         <v>16.82</v>
@@ -8174,12 +8232,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="114" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A114" s="62">
         <v>2035</v>
       </c>
       <c r="B114" s="62" t="s">
-        <v>425</v>
+        <v>408</v>
       </c>
       <c r="C114" s="63" t="s">
         <v>338</v>
@@ -8188,16 +8246,13 @@
         <v>339</v>
       </c>
       <c r="F114" s="62" t="s">
-        <v>426</v>
+        <v>409</v>
       </c>
       <c r="G114" s="62" t="s">
-        <v>428</v>
+        <v>410</v>
       </c>
       <c r="H114" s="62" t="s">
-        <v>427</v>
-      </c>
-      <c r="I114" s="62" t="s">
-        <v>11</v>
+        <v>411</v>
       </c>
       <c r="J114" s="62" t="s">
         <v>402</v>
@@ -8209,7 +8264,7 @@
         <v>43</v>
       </c>
       <c r="M114" s="63" t="s">
-        <v>429</v>
+        <v>413</v>
       </c>
       <c r="N114" s="62">
         <v>16.82</v>
@@ -8235,240 +8290,246 @@
       <c r="U114" s="66">
         <v>72</v>
       </c>
-      <c r="V114" s="62" t="s">
+    </row>
+    <row r="115" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="62">
+        <v>2035</v>
+      </c>
+      <c r="B115" s="62" t="s">
+        <v>425</v>
+      </c>
+      <c r="C115" s="63" t="s">
+        <v>338</v>
+      </c>
+      <c r="D115" s="62" t="s">
+        <v>339</v>
+      </c>
+      <c r="F115" s="62" t="s">
+        <v>426</v>
+      </c>
+      <c r="G115" s="62" t="s">
+        <v>428</v>
+      </c>
+      <c r="H115" s="62" t="s">
+        <v>427</v>
+      </c>
+      <c r="J115" s="62" t="s">
+        <v>402</v>
+      </c>
+      <c r="K115" s="62" t="s">
+        <v>412</v>
+      </c>
+      <c r="L115" s="64" t="s">
+        <v>43</v>
+      </c>
+      <c r="M115" s="63" t="s">
+        <v>429</v>
+      </c>
+      <c r="N115" s="62">
+        <v>16.82</v>
+      </c>
+      <c r="O115" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="P115" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q115" s="62">
+        <v>0.87</v>
+      </c>
+      <c r="R115" s="62">
+        <v>0.78</v>
+      </c>
+      <c r="S115" s="66">
+        <v>83.3</v>
+      </c>
+      <c r="T115" s="66">
+        <v>0</v>
+      </c>
+      <c r="U115" s="66">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="116" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="62">
+        <v>2035</v>
+      </c>
+      <c r="B116" s="62" t="s">
+        <v>442</v>
+      </c>
+      <c r="C116" s="63" t="s">
+        <v>338</v>
+      </c>
+      <c r="D116" s="62" t="s">
+        <v>339</v>
+      </c>
+      <c r="F116" s="62" t="s">
+        <v>447</v>
+      </c>
+      <c r="G116" s="62" t="s">
+        <v>446</v>
+      </c>
+      <c r="H116" s="62" t="s">
+        <v>445</v>
+      </c>
+      <c r="K116" s="62" t="s">
+        <v>412</v>
+      </c>
+      <c r="L116" s="64" t="s">
+        <v>43</v>
+      </c>
+      <c r="M116" s="63" t="s">
+        <v>444</v>
+      </c>
+      <c r="N116" s="62">
+        <v>16.82</v>
+      </c>
+      <c r="O116" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="P116" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q116" s="62">
+        <v>0.87</v>
+      </c>
+      <c r="R116" s="62">
+        <v>0.78</v>
+      </c>
+      <c r="S116" s="66">
+        <v>83.3</v>
+      </c>
+      <c r="T116" s="66">
+        <v>0</v>
+      </c>
+      <c r="U116" s="66">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="117" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="62">
+        <v>2035</v>
+      </c>
+      <c r="B117" s="62" t="s">
+        <v>443</v>
+      </c>
+      <c r="C117" s="63" t="s">
+        <v>338</v>
+      </c>
+      <c r="D117" s="62" t="s">
+        <v>339</v>
+      </c>
+      <c r="F117" s="62" t="s">
+        <v>448</v>
+      </c>
+      <c r="G117" s="62" t="s">
+        <v>446</v>
+      </c>
+      <c r="H117" s="62" t="s">
+        <v>445</v>
+      </c>
+      <c r="I117" s="62" t="s">
+        <v>11</v>
+      </c>
+      <c r="K117" s="62" t="s">
+        <v>412</v>
+      </c>
+      <c r="L117" s="64" t="s">
+        <v>43</v>
+      </c>
+      <c r="M117" s="63" t="s">
+        <v>437</v>
+      </c>
+      <c r="N117" s="62">
+        <v>18.03</v>
+      </c>
+      <c r="O117" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="P117" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q117" s="62">
+        <v>0.87</v>
+      </c>
+      <c r="R117" s="62">
+        <v>0.78</v>
+      </c>
+      <c r="S117" s="66">
+        <v>83.3</v>
+      </c>
+      <c r="T117" s="66">
+        <v>0</v>
+      </c>
+      <c r="U117" s="66">
+        <v>72</v>
+      </c>
+      <c r="V117" s="62" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="115" spans="1:22" s="24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="24">
+    <row r="118" spans="1:22" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="24">
         <v>2050</v>
       </c>
-      <c r="B115" s="24" t="s">
+      <c r="B118" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="C115" s="24" t="s">
+      <c r="C118" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="D115" s="24" t="s">
+      <c r="D118" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="F115" s="24" t="s">
+      <c r="F118" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="G115" s="24" t="s">
+      <c r="G118" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="H115" s="25" t="s">
+      <c r="H118" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="K115" s="24" t="s">
+      <c r="K118" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="L115" s="26" t="s">
+      <c r="L118" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="M115" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="N115" s="24">
+      <c r="M118" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="N118" s="24">
         <v>17.440000000000001</v>
       </c>
-      <c r="O115" s="47">
+      <c r="O118" s="47">
         <v>-0.33</v>
       </c>
-      <c r="P115" s="47">
-        <v>0</v>
-      </c>
-      <c r="Q115" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="R115" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="S115" s="72" t="s">
-        <v>109</v>
-      </c>
-      <c r="T115" s="72" t="s">
-        <v>109</v>
-      </c>
-      <c r="U115" s="72" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="116" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="53">
-        <v>2050</v>
-      </c>
-      <c r="B116" s="53" t="s">
-        <v>351</v>
-      </c>
-      <c r="C116" s="53" t="s">
-        <v>338</v>
-      </c>
-      <c r="D116" s="53" t="s">
-        <v>339</v>
-      </c>
-      <c r="F116" s="53" t="s">
-        <v>353</v>
-      </c>
-      <c r="G116" s="53" t="s">
-        <v>342</v>
-      </c>
-      <c r="H116" s="52" t="s">
-        <v>343</v>
-      </c>
-      <c r="K116" s="53" t="s">
-        <v>344</v>
-      </c>
-      <c r="L116" s="52" t="s">
-        <v>16</v>
-      </c>
-      <c r="M116" s="53" t="s">
-        <v>356</v>
-      </c>
-      <c r="N116" s="53">
-        <v>19.13</v>
-      </c>
-      <c r="O116" s="67" t="s">
-        <v>109</v>
-      </c>
-      <c r="P116" s="67" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q116" s="53">
-        <v>0.87</v>
-      </c>
-      <c r="R116" s="53">
-        <v>0.78</v>
-      </c>
-      <c r="S116" s="56">
-        <v>83.3</v>
-      </c>
-      <c r="T116" s="56">
-        <v>0</v>
-      </c>
-      <c r="U116" s="56">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="117" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="53">
-        <v>2050</v>
-      </c>
-      <c r="B117" s="53" t="s">
-        <v>380</v>
-      </c>
-      <c r="C117" s="53" t="s">
-        <v>338</v>
-      </c>
-      <c r="D117" s="53" t="s">
-        <v>339</v>
-      </c>
-      <c r="F117" s="53" t="s">
-        <v>376</v>
-      </c>
-      <c r="G117" s="53" t="s">
-        <v>342</v>
-      </c>
-      <c r="H117" s="52" t="s">
-        <v>343</v>
-      </c>
-      <c r="K117" s="53" t="s">
-        <v>344</v>
-      </c>
-      <c r="L117" s="52" t="s">
-        <v>16</v>
-      </c>
-      <c r="M117" s="53" t="s">
-        <v>381</v>
-      </c>
-      <c r="N117" s="53">
-        <v>18.420000000000002</v>
-      </c>
-      <c r="O117" s="67" t="s">
-        <v>109</v>
-      </c>
-      <c r="P117" s="67" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q117" s="53">
-        <v>0.87</v>
-      </c>
-      <c r="R117" s="53">
-        <v>0.78</v>
-      </c>
-      <c r="S117" s="56">
-        <v>83.3</v>
-      </c>
-      <c r="T117" s="56">
-        <v>0</v>
-      </c>
-      <c r="U117" s="56">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="118" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="53">
-        <v>2050</v>
-      </c>
-      <c r="B118" s="53" t="s">
-        <v>388</v>
-      </c>
-      <c r="C118" s="53" t="s">
-        <v>338</v>
-      </c>
-      <c r="D118" s="53" t="s">
-        <v>339</v>
-      </c>
-      <c r="F118" s="53" t="s">
-        <v>386</v>
-      </c>
-      <c r="G118" s="53" t="s">
-        <v>387</v>
-      </c>
-      <c r="H118" s="52" t="s">
-        <v>392</v>
-      </c>
-      <c r="K118" s="53" t="s">
-        <v>394</v>
-      </c>
-      <c r="L118" s="52" t="s">
-        <v>16</v>
-      </c>
-      <c r="M118" s="53" t="s">
-        <v>400</v>
-      </c>
-      <c r="N118" s="53">
-        <v>18.420000000000002</v>
-      </c>
-      <c r="O118" s="67" t="s">
-        <v>109</v>
-      </c>
-      <c r="P118" s="67" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q118" s="53">
-        <v>0.87</v>
-      </c>
-      <c r="R118" s="53">
-        <v>0.78</v>
-      </c>
-      <c r="S118" s="56">
-        <v>83.3</v>
-      </c>
-      <c r="T118" s="56">
-        <v>0</v>
-      </c>
-      <c r="U118" s="56">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="119" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P118" s="47">
+        <v>0</v>
+      </c>
+      <c r="Q118" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="R118" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="S118" s="72" t="s">
+        <v>109</v>
+      </c>
+      <c r="T118" s="72" t="s">
+        <v>109</v>
+      </c>
+      <c r="U118" s="72" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="119" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A119" s="53">
         <v>2050</v>
       </c>
       <c r="B119" s="53" t="s">
-        <v>414</v>
+        <v>351</v>
       </c>
       <c r="C119" s="53" t="s">
         <v>338</v>
@@ -8477,28 +8538,25 @@
         <v>339</v>
       </c>
       <c r="F119" s="53" t="s">
-        <v>386</v>
+        <v>353</v>
       </c>
       <c r="G119" s="53" t="s">
-        <v>407</v>
+        <v>342</v>
       </c>
       <c r="H119" s="52" t="s">
-        <v>406</v>
-      </c>
-      <c r="J119" s="53" t="s">
-        <v>402</v>
+        <v>343</v>
       </c>
       <c r="K119" s="53" t="s">
-        <v>404</v>
+        <v>344</v>
       </c>
       <c r="L119" s="52" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="M119" s="53" t="s">
-        <v>418</v>
+        <v>356</v>
       </c>
       <c r="N119" s="53">
-        <v>18.420000000000002</v>
+        <v>19.13</v>
       </c>
       <c r="O119" s="67" t="s">
         <v>109</v>
@@ -8522,12 +8580,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="120" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A120" s="53">
         <v>2050</v>
       </c>
       <c r="B120" s="53" t="s">
-        <v>430</v>
+        <v>380</v>
       </c>
       <c r="C120" s="53" t="s">
         <v>338</v>
@@ -8536,28 +8594,22 @@
         <v>339</v>
       </c>
       <c r="F120" s="53" t="s">
-        <v>426</v>
+        <v>376</v>
       </c>
       <c r="G120" s="53" t="s">
-        <v>428</v>
+        <v>342</v>
       </c>
       <c r="H120" s="52" t="s">
-        <v>427</v>
-      </c>
-      <c r="I120" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="J120" s="53" t="s">
-        <v>402</v>
+        <v>343</v>
       </c>
       <c r="K120" s="53" t="s">
-        <v>404</v>
+        <v>344</v>
       </c>
       <c r="L120" s="52" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="M120" s="53" t="s">
-        <v>431</v>
+        <v>381</v>
       </c>
       <c r="N120" s="53">
         <v>18.420000000000002</v>
@@ -8583,243 +8635,252 @@
       <c r="U120" s="56">
         <v>72</v>
       </c>
-      <c r="V120" s="53" t="s">
+    </row>
+    <row r="121" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="53">
+        <v>2050</v>
+      </c>
+      <c r="B121" s="53" t="s">
+        <v>388</v>
+      </c>
+      <c r="C121" s="53" t="s">
+        <v>338</v>
+      </c>
+      <c r="D121" s="53" t="s">
+        <v>339</v>
+      </c>
+      <c r="F121" s="53" t="s">
+        <v>386</v>
+      </c>
+      <c r="G121" s="53" t="s">
+        <v>387</v>
+      </c>
+      <c r="H121" s="52" t="s">
+        <v>392</v>
+      </c>
+      <c r="K121" s="53" t="s">
+        <v>394</v>
+      </c>
+      <c r="L121" s="52" t="s">
+        <v>16</v>
+      </c>
+      <c r="M121" s="53" t="s">
+        <v>400</v>
+      </c>
+      <c r="N121" s="53">
+        <v>18.420000000000002</v>
+      </c>
+      <c r="O121" s="67" t="s">
+        <v>109</v>
+      </c>
+      <c r="P121" s="67" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q121" s="53">
+        <v>0.87</v>
+      </c>
+      <c r="R121" s="53">
+        <v>0.78</v>
+      </c>
+      <c r="S121" s="56">
+        <v>83.3</v>
+      </c>
+      <c r="T121" s="56">
+        <v>0</v>
+      </c>
+      <c r="U121" s="56">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="122" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="53">
+        <v>2050</v>
+      </c>
+      <c r="B122" s="53" t="s">
+        <v>414</v>
+      </c>
+      <c r="C122" s="53" t="s">
+        <v>338</v>
+      </c>
+      <c r="D122" s="53" t="s">
+        <v>339</v>
+      </c>
+      <c r="F122" s="53" t="s">
+        <v>386</v>
+      </c>
+      <c r="G122" s="53" t="s">
+        <v>407</v>
+      </c>
+      <c r="H122" s="52" t="s">
+        <v>406</v>
+      </c>
+      <c r="J122" s="53" t="s">
+        <v>402</v>
+      </c>
+      <c r="K122" s="53" t="s">
+        <v>404</v>
+      </c>
+      <c r="L122" s="52" t="s">
+        <v>42</v>
+      </c>
+      <c r="M122" s="53" t="s">
+        <v>418</v>
+      </c>
+      <c r="N122" s="53">
+        <v>18.420000000000002</v>
+      </c>
+      <c r="O122" s="67" t="s">
+        <v>109</v>
+      </c>
+      <c r="P122" s="67" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q122" s="53">
+        <v>0.87</v>
+      </c>
+      <c r="R122" s="53">
+        <v>0.78</v>
+      </c>
+      <c r="S122" s="56">
+        <v>83.3</v>
+      </c>
+      <c r="T122" s="56">
+        <v>0</v>
+      </c>
+      <c r="U122" s="56">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="123" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="53">
+        <v>2050</v>
+      </c>
+      <c r="B123" s="53" t="s">
+        <v>430</v>
+      </c>
+      <c r="C123" s="53" t="s">
+        <v>338</v>
+      </c>
+      <c r="D123" s="53" t="s">
+        <v>339</v>
+      </c>
+      <c r="F123" s="53" t="s">
+        <v>426</v>
+      </c>
+      <c r="G123" s="53" t="s">
+        <v>428</v>
+      </c>
+      <c r="H123" s="52" t="s">
+        <v>427</v>
+      </c>
+      <c r="I123" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="J123" s="53" t="s">
+        <v>402</v>
+      </c>
+      <c r="K123" s="53" t="s">
+        <v>404</v>
+      </c>
+      <c r="L123" s="52" t="s">
+        <v>42</v>
+      </c>
+      <c r="M123" s="53" t="s">
+        <v>431</v>
+      </c>
+      <c r="N123" s="53">
+        <v>18.420000000000002</v>
+      </c>
+      <c r="O123" s="67" t="s">
+        <v>109</v>
+      </c>
+      <c r="P123" s="67" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q123" s="53">
+        <v>0.87</v>
+      </c>
+      <c r="R123" s="53">
+        <v>0.78</v>
+      </c>
+      <c r="S123" s="56">
+        <v>83.3</v>
+      </c>
+      <c r="T123" s="56">
+        <v>0</v>
+      </c>
+      <c r="U123" s="56">
+        <v>72</v>
+      </c>
+      <c r="V123" s="53" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="121" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="68">
+    <row r="124" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="53">
         <v>2050</v>
       </c>
-      <c r="B121" s="68" t="s">
-        <v>352</v>
-      </c>
-      <c r="C121" s="68" t="s">
+      <c r="B124" s="53" t="s">
+        <v>438</v>
+      </c>
+      <c r="C124" s="53" t="s">
         <v>338</v>
       </c>
-      <c r="D121" s="68" t="s">
+      <c r="D124" s="53" t="s">
         <v>339</v>
       </c>
-      <c r="F121" s="68" t="s">
-        <v>354</v>
-      </c>
-      <c r="G121" s="68" t="s">
-        <v>347</v>
-      </c>
-      <c r="H121" s="69" t="s">
-        <v>348</v>
-      </c>
-      <c r="K121" s="68" t="s">
-        <v>355</v>
-      </c>
-      <c r="L121" s="69" t="s">
-        <v>44</v>
-      </c>
-      <c r="M121" s="68" t="s">
-        <v>357</v>
-      </c>
-      <c r="N121" s="68">
+      <c r="F124" s="53" t="s">
+        <v>448</v>
+      </c>
+      <c r="G124" s="53" t="s">
+        <v>428</v>
+      </c>
+      <c r="H124" s="52" t="s">
+        <v>427</v>
+      </c>
+      <c r="I124" s="75" t="s">
+        <v>440</v>
+      </c>
+      <c r="K124" s="53" t="s">
+        <v>404</v>
+      </c>
+      <c r="L124" s="52" t="s">
+        <v>88</v>
+      </c>
+      <c r="M124" s="53" t="s">
+        <v>439</v>
+      </c>
+      <c r="N124" s="53">
         <v>19.13</v>
       </c>
-      <c r="O121" s="70" t="s">
-        <v>109</v>
-      </c>
-      <c r="P121" s="70" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q121" s="68">
+      <c r="O124" s="67" t="s">
+        <v>109</v>
+      </c>
+      <c r="P124" s="67" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q124" s="53">
         <v>0.87</v>
       </c>
-      <c r="R121" s="68">
+      <c r="R124" s="53">
         <v>0.78</v>
       </c>
-      <c r="S121" s="71">
+      <c r="S124" s="56">
         <v>83.3</v>
       </c>
-      <c r="T121" s="71">
-        <v>0</v>
-      </c>
-      <c r="U121" s="71">
+      <c r="T124" s="56">
+        <v>0</v>
+      </c>
+      <c r="U124" s="56">
         <v>72</v>
       </c>
     </row>
-    <row r="122" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="68">
-        <v>2050</v>
-      </c>
-      <c r="B122" s="68" t="s">
-        <v>382</v>
-      </c>
-      <c r="C122" s="68" t="s">
-        <v>338</v>
-      </c>
-      <c r="D122" s="68" t="s">
-        <v>339</v>
-      </c>
-      <c r="F122" s="68" t="s">
-        <v>354</v>
-      </c>
-      <c r="G122" s="68" t="s">
-        <v>347</v>
-      </c>
-      <c r="H122" s="69" t="s">
-        <v>348</v>
-      </c>
-      <c r="K122" s="68" t="s">
-        <v>355</v>
-      </c>
-      <c r="L122" s="69" t="s">
-        <v>44</v>
-      </c>
-      <c r="M122" s="68" t="s">
-        <v>357</v>
-      </c>
-      <c r="N122" s="68">
-        <v>18.420000000000002</v>
-      </c>
-      <c r="O122" s="70" t="s">
-        <v>109</v>
-      </c>
-      <c r="P122" s="70" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q122" s="68">
-        <v>0.87</v>
-      </c>
-      <c r="R122" s="68">
-        <v>0.78</v>
-      </c>
-      <c r="S122" s="71">
-        <v>83.3</v>
-      </c>
-      <c r="T122" s="71">
-        <v>0</v>
-      </c>
-      <c r="U122" s="71">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="123" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="68">
-        <v>2050</v>
-      </c>
-      <c r="B123" s="68" t="s">
-        <v>389</v>
-      </c>
-      <c r="C123" s="68" t="s">
-        <v>338</v>
-      </c>
-      <c r="D123" s="68" t="s">
-        <v>339</v>
-      </c>
-      <c r="F123" s="68" t="s">
-        <v>386</v>
-      </c>
-      <c r="G123" s="68" t="s">
-        <v>391</v>
-      </c>
-      <c r="H123" s="69" t="s">
-        <v>393</v>
-      </c>
-      <c r="K123" s="68" t="s">
-        <v>395</v>
-      </c>
-      <c r="L123" s="69" t="s">
-        <v>44</v>
-      </c>
-      <c r="M123" s="68" t="s">
-        <v>398</v>
-      </c>
-      <c r="N123" s="68">
-        <v>18.420000000000002</v>
-      </c>
-      <c r="O123" s="70" t="s">
-        <v>109</v>
-      </c>
-      <c r="P123" s="70" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q123" s="68">
-        <v>0.87</v>
-      </c>
-      <c r="R123" s="68">
-        <v>0.78</v>
-      </c>
-      <c r="S123" s="71">
-        <v>83.3</v>
-      </c>
-      <c r="T123" s="71">
-        <v>0</v>
-      </c>
-      <c r="U123" s="71">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="124" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="68">
-        <v>2050</v>
-      </c>
-      <c r="B124" s="68" t="s">
-        <v>415</v>
-      </c>
-      <c r="C124" s="68" t="s">
-        <v>338</v>
-      </c>
-      <c r="D124" s="68" t="s">
-        <v>339</v>
-      </c>
-      <c r="F124" s="68" t="s">
-        <v>386</v>
-      </c>
-      <c r="G124" s="68" t="s">
-        <v>410</v>
-      </c>
-      <c r="H124" s="69" t="s">
-        <v>411</v>
-      </c>
-      <c r="J124" s="68" t="s">
-        <v>402</v>
-      </c>
-      <c r="K124" s="68" t="s">
-        <v>416</v>
-      </c>
-      <c r="L124" s="69" t="s">
-        <v>42</v>
-      </c>
-      <c r="M124" s="68" t="s">
-        <v>417</v>
-      </c>
-      <c r="N124" s="68">
-        <v>18.420000000000002</v>
-      </c>
-      <c r="O124" s="70" t="s">
-        <v>109</v>
-      </c>
-      <c r="P124" s="70" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q124" s="68">
-        <v>0.87</v>
-      </c>
-      <c r="R124" s="68">
-        <v>0.78</v>
-      </c>
-      <c r="S124" s="71">
-        <v>83.3</v>
-      </c>
-      <c r="T124" s="71">
-        <v>0</v>
-      </c>
-      <c r="U124" s="71">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="125" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A125" s="68">
         <v>2050</v>
       </c>
       <c r="B125" s="68" t="s">
-        <v>432</v>
+        <v>352</v>
       </c>
       <c r="C125" s="68" t="s">
         <v>338</v>
@@ -8828,31 +8889,25 @@
         <v>339</v>
       </c>
       <c r="F125" s="68" t="s">
-        <v>426</v>
+        <v>354</v>
       </c>
       <c r="G125" s="68" t="s">
-        <v>428</v>
+        <v>347</v>
       </c>
       <c r="H125" s="69" t="s">
-        <v>427</v>
-      </c>
-      <c r="I125" s="68" t="s">
-        <v>11</v>
-      </c>
-      <c r="J125" s="68" t="s">
-        <v>402</v>
+        <v>348</v>
       </c>
       <c r="K125" s="68" t="s">
-        <v>416</v>
+        <v>355</v>
       </c>
       <c r="L125" s="69" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M125" s="68" t="s">
-        <v>433</v>
+        <v>357</v>
       </c>
       <c r="N125" s="68">
-        <v>18.420000000000002</v>
+        <v>19.13</v>
       </c>
       <c r="O125" s="70" t="s">
         <v>109</v>
@@ -8875,7 +8930,352 @@
       <c r="U125" s="71">
         <v>72</v>
       </c>
-      <c r="V125" s="68" t="s">
+    </row>
+    <row r="126" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="68">
+        <v>2050</v>
+      </c>
+      <c r="B126" s="68" t="s">
+        <v>382</v>
+      </c>
+      <c r="C126" s="68" t="s">
+        <v>338</v>
+      </c>
+      <c r="D126" s="68" t="s">
+        <v>339</v>
+      </c>
+      <c r="F126" s="68" t="s">
+        <v>354</v>
+      </c>
+      <c r="G126" s="68" t="s">
+        <v>347</v>
+      </c>
+      <c r="H126" s="69" t="s">
+        <v>348</v>
+      </c>
+      <c r="K126" s="68" t="s">
+        <v>355</v>
+      </c>
+      <c r="L126" s="69" t="s">
+        <v>44</v>
+      </c>
+      <c r="M126" s="68" t="s">
+        <v>357</v>
+      </c>
+      <c r="N126" s="68">
+        <v>18.420000000000002</v>
+      </c>
+      <c r="O126" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="P126" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q126" s="68">
+        <v>0.87</v>
+      </c>
+      <c r="R126" s="68">
+        <v>0.78</v>
+      </c>
+      <c r="S126" s="71">
+        <v>83.3</v>
+      </c>
+      <c r="T126" s="71">
+        <v>0</v>
+      </c>
+      <c r="U126" s="71">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="127" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A127" s="68">
+        <v>2050</v>
+      </c>
+      <c r="B127" s="68" t="s">
+        <v>389</v>
+      </c>
+      <c r="C127" s="68" t="s">
+        <v>338</v>
+      </c>
+      <c r="D127" s="68" t="s">
+        <v>339</v>
+      </c>
+      <c r="F127" s="68" t="s">
+        <v>386</v>
+      </c>
+      <c r="G127" s="68" t="s">
+        <v>391</v>
+      </c>
+      <c r="H127" s="69" t="s">
+        <v>393</v>
+      </c>
+      <c r="K127" s="68" t="s">
+        <v>395</v>
+      </c>
+      <c r="L127" s="69" t="s">
+        <v>44</v>
+      </c>
+      <c r="M127" s="68" t="s">
+        <v>398</v>
+      </c>
+      <c r="N127" s="68">
+        <v>18.420000000000002</v>
+      </c>
+      <c r="O127" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="P127" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q127" s="68">
+        <v>0.87</v>
+      </c>
+      <c r="R127" s="68">
+        <v>0.78</v>
+      </c>
+      <c r="S127" s="71">
+        <v>83.3</v>
+      </c>
+      <c r="T127" s="71">
+        <v>0</v>
+      </c>
+      <c r="U127" s="71">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="128" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A128" s="68">
+        <v>2050</v>
+      </c>
+      <c r="B128" s="68" t="s">
+        <v>415</v>
+      </c>
+      <c r="C128" s="68" t="s">
+        <v>338</v>
+      </c>
+      <c r="D128" s="68" t="s">
+        <v>339</v>
+      </c>
+      <c r="F128" s="68" t="s">
+        <v>386</v>
+      </c>
+      <c r="G128" s="68" t="s">
+        <v>410</v>
+      </c>
+      <c r="H128" s="69" t="s">
+        <v>411</v>
+      </c>
+      <c r="J128" s="68" t="s">
+        <v>402</v>
+      </c>
+      <c r="K128" s="68" t="s">
+        <v>416</v>
+      </c>
+      <c r="L128" s="69" t="s">
+        <v>42</v>
+      </c>
+      <c r="M128" s="68" t="s">
+        <v>417</v>
+      </c>
+      <c r="N128" s="68">
+        <v>18.420000000000002</v>
+      </c>
+      <c r="O128" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="P128" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q128" s="68">
+        <v>0.87</v>
+      </c>
+      <c r="R128" s="68">
+        <v>0.78</v>
+      </c>
+      <c r="S128" s="71">
+        <v>83.3</v>
+      </c>
+      <c r="T128" s="71">
+        <v>0</v>
+      </c>
+      <c r="U128" s="71">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="129" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A129" s="68">
+        <v>2050</v>
+      </c>
+      <c r="B129" s="68" t="s">
+        <v>432</v>
+      </c>
+      <c r="C129" s="68" t="s">
+        <v>338</v>
+      </c>
+      <c r="D129" s="68" t="s">
+        <v>339</v>
+      </c>
+      <c r="F129" s="68" t="s">
+        <v>426</v>
+      </c>
+      <c r="G129" s="68" t="s">
+        <v>428</v>
+      </c>
+      <c r="H129" s="69" t="s">
+        <v>427</v>
+      </c>
+      <c r="J129" s="68" t="s">
+        <v>402</v>
+      </c>
+      <c r="K129" s="68" t="s">
+        <v>416</v>
+      </c>
+      <c r="L129" s="69" t="s">
+        <v>42</v>
+      </c>
+      <c r="M129" s="68" t="s">
+        <v>433</v>
+      </c>
+      <c r="N129" s="68">
+        <v>18.420000000000002</v>
+      </c>
+      <c r="O129" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="P129" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q129" s="68">
+        <v>0.87</v>
+      </c>
+      <c r="R129" s="68">
+        <v>0.78</v>
+      </c>
+      <c r="S129" s="71">
+        <v>83.3</v>
+      </c>
+      <c r="T129" s="71">
+        <v>0</v>
+      </c>
+      <c r="U129" s="71">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="130" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A130" s="68">
+        <v>2050</v>
+      </c>
+      <c r="B130" s="68" t="s">
+        <v>449</v>
+      </c>
+      <c r="C130" s="68" t="s">
+        <v>338</v>
+      </c>
+      <c r="D130" s="68" t="s">
+        <v>339</v>
+      </c>
+      <c r="F130" s="68" t="s">
+        <v>447</v>
+      </c>
+      <c r="G130" s="68" t="s">
+        <v>446</v>
+      </c>
+      <c r="H130" s="69" t="s">
+        <v>445</v>
+      </c>
+      <c r="K130" s="68" t="s">
+        <v>416</v>
+      </c>
+      <c r="L130" s="69" t="s">
+        <v>42</v>
+      </c>
+      <c r="M130" s="68" t="s">
+        <v>451</v>
+      </c>
+      <c r="N130" s="68">
+        <v>18.420000000000002</v>
+      </c>
+      <c r="O130" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="P130" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q130" s="68">
+        <v>0.87</v>
+      </c>
+      <c r="R130" s="68">
+        <v>0.78</v>
+      </c>
+      <c r="S130" s="71">
+        <v>83.3</v>
+      </c>
+      <c r="T130" s="71">
+        <v>0</v>
+      </c>
+      <c r="U130" s="71">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="131" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A131" s="68">
+        <v>2050</v>
+      </c>
+      <c r="B131" s="68" t="s">
+        <v>450</v>
+      </c>
+      <c r="C131" s="68" t="s">
+        <v>338</v>
+      </c>
+      <c r="D131" s="68" t="s">
+        <v>339</v>
+      </c>
+      <c r="F131" s="68" t="s">
+        <v>448</v>
+      </c>
+      <c r="G131" s="68" t="s">
+        <v>446</v>
+      </c>
+      <c r="H131" s="69" t="s">
+        <v>445</v>
+      </c>
+      <c r="I131" s="68" t="s">
+        <v>11</v>
+      </c>
+      <c r="K131" s="68" t="s">
+        <v>416</v>
+      </c>
+      <c r="L131" s="69" t="s">
+        <v>42</v>
+      </c>
+      <c r="M131" s="68" t="s">
+        <v>441</v>
+      </c>
+      <c r="N131" s="68">
+        <v>19.57</v>
+      </c>
+      <c r="O131" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="P131" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q131" s="68">
+        <v>0.87</v>
+      </c>
+      <c r="R131" s="68">
+        <v>0.78</v>
+      </c>
+      <c r="S131" s="71">
+        <v>83.3</v>
+      </c>
+      <c r="T131" s="71">
+        <v>0</v>
+      </c>
+      <c r="U131" s="71">
+        <v>72</v>
+      </c>
+      <c r="V131" s="68" t="s">
         <v>358</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update off_model run tag
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CFF8313-2D0C-4619-8C8A-5A457B0B0A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058D1375-1DE8-4C90-97C8-C4BC6BFA2529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1215" yWindow="4290" windowWidth="19710" windowHeight="9855" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
+    <workbookView xWindow="-48" yWindow="684" windowWidth="25152" windowHeight="15480" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelRuns" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1439" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1445" uniqueCount="452">
   <si>
     <t>year</t>
   </si>
@@ -2076,33 +2076,33 @@
   <dimension ref="A1:V131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C111" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C101" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A131" sqref="A131"/>
+      <selection pane="bottomRight" activeCell="K133" sqref="K133"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="7" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="42.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="42.33203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="23" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="6.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="22.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11.28515625" style="10" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="8.28515625" style="1" customWidth="1"/>
-    <col min="15" max="16" width="9.28515625" style="43"/>
-    <col min="17" max="16384" width="9.28515625" style="1"/>
+    <col min="8" max="8" width="8.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="6.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="22.33203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.33203125" style="10" customWidth="1"/>
+    <col min="13" max="13" width="17.5546875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="8.33203125" style="1" customWidth="1"/>
+    <col min="15" max="16" width="9.33203125" style="43"/>
+    <col min="17" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" s="5" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2170,7 +2170,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="2" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19">
         <v>2005</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="30">
         <v>2005</v>
       </c>
@@ -2279,7 +2279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30">
         <v>2005</v>
       </c>
@@ -2334,7 +2334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="30">
         <v>2005</v>
       </c>
@@ -2389,7 +2389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="30">
         <v>2005</v>
       </c>
@@ -2454,7 +2454,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="7" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="52">
         <v>2015</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="34">
         <v>2015</v>
       </c>
@@ -2541,7 +2541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="34">
         <v>2015</v>
       </c>
@@ -2594,7 +2594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="34">
         <v>2015</v>
       </c>
@@ -2647,7 +2647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="34">
         <v>2015</v>
       </c>
@@ -2700,7 +2700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="34">
         <v>2015</v>
       </c>
@@ -2756,7 +2756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="34">
         <v>2015</v>
       </c>
@@ -2812,7 +2812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="34">
         <v>2015</v>
       </c>
@@ -2868,7 +2868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="34">
         <v>2015</v>
       </c>
@@ -2928,7 +2928,7 @@
       </c>
       <c r="V15" s="57"/>
     </row>
-    <row r="16" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="34">
         <v>2015</v>
       </c>
@@ -2990,7 +2990,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>2023</v>
       </c>
@@ -3036,7 +3036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>2023</v>
       </c>
@@ -3082,7 +3082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>2023</v>
       </c>
@@ -3128,7 +3128,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>2023</v>
       </c>
@@ -3174,7 +3174,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>2023</v>
       </c>
@@ -3220,7 +3220,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>2023</v>
       </c>
@@ -3266,7 +3266,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>2023</v>
       </c>
@@ -3312,7 +3312,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>2023</v>
       </c>
@@ -3358,7 +3358,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>2023</v>
       </c>
@@ -3404,7 +3404,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>2023</v>
       </c>
@@ -3450,7 +3450,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>2023</v>
       </c>
@@ -3496,7 +3496,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>2023</v>
       </c>
@@ -3542,7 +3542,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>2023</v>
       </c>
@@ -3588,7 +3588,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>2023</v>
       </c>
@@ -3634,7 +3634,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>2023</v>
       </c>
@@ -3680,7 +3680,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>2023</v>
       </c>
@@ -3726,7 +3726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>2023</v>
       </c>
@@ -3772,7 +3772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>2023</v>
       </c>
@@ -3818,7 +3818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>2023</v>
       </c>
@@ -3862,7 +3862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>2023</v>
       </c>
@@ -3911,7 +3911,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>2023</v>
       </c>
@@ -3958,7 +3958,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>2023</v>
       </c>
@@ -4005,7 +4005,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>2023</v>
       </c>
@@ -4061,7 +4061,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>2023</v>
       </c>
@@ -4117,7 +4117,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>2023</v>
       </c>
@@ -4173,7 +4173,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>2023</v>
       </c>
@@ -4229,7 +4229,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>2023</v>
       </c>
@@ -4285,7 +4285,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>2023</v>
       </c>
@@ -4341,7 +4341,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>2023</v>
       </c>
@@ -4397,7 +4397,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>2023</v>
       </c>
@@ -4453,7 +4453,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>2023</v>
       </c>
@@ -4509,7 +4509,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>2023</v>
       </c>
@@ -4565,7 +4565,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>2023</v>
       </c>
@@ -4621,7 +4621,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>2023</v>
       </c>
@@ -4677,7 +4677,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>2023</v>
       </c>
@@ -4733,7 +4733,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>2023</v>
       </c>
@@ -4789,7 +4789,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>2023</v>
       </c>
@@ -4845,7 +4845,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>2023</v>
       </c>
@@ -4901,7 +4901,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>2023</v>
       </c>
@@ -4957,7 +4957,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>2023</v>
       </c>
@@ -5013,7 +5013,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>2023</v>
       </c>
@@ -5069,7 +5069,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>2023</v>
       </c>
@@ -5125,7 +5125,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>2023</v>
       </c>
@@ -5181,7 +5181,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>2023</v>
       </c>
@@ -5237,7 +5237,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>2023</v>
       </c>
@@ -5293,7 +5293,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>2023</v>
       </c>
@@ -5349,7 +5349,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>2023</v>
       </c>
@@ -5405,7 +5405,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>2023</v>
       </c>
@@ -5464,7 +5464,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>2023</v>
       </c>
@@ -5520,7 +5520,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>2023</v>
       </c>
@@ -5579,7 +5579,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>2023</v>
       </c>
@@ -5638,7 +5638,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>2023</v>
       </c>
@@ -5697,7 +5697,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>2023</v>
       </c>
@@ -5756,7 +5756,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="70" spans="1:22" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:22" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>2023</v>
       </c>
@@ -5812,7 +5812,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="71" spans="1:22" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:22" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>2023</v>
       </c>
@@ -5868,7 +5868,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>2023</v>
       </c>
@@ -5924,7 +5924,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>2023</v>
       </c>
@@ -5980,7 +5980,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>2023</v>
       </c>
@@ -6036,7 +6036,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>2023</v>
       </c>
@@ -6095,7 +6095,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>2023</v>
       </c>
@@ -6155,7 +6155,7 @@
       </c>
       <c r="V76" s="73"/>
     </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>2023</v>
       </c>
@@ -6217,7 +6217,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="78" spans="1:22" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:22" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="27">
         <v>2025</v>
       </c>
@@ -6245,7 +6245,7 @@
       <c r="T78" s="29"/>
       <c r="U78" s="29"/>
     </row>
-    <row r="79" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="15">
         <v>2035</v>
       </c>
@@ -6304,7 +6304,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="80" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="12">
         <v>2035</v>
       </c>
@@ -6360,7 +6360,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="81" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="12">
         <v>2035</v>
       </c>
@@ -6416,7 +6416,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="82" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="12">
         <v>2035</v>
       </c>
@@ -6472,7 +6472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="12">
         <v>2035</v>
       </c>
@@ -6528,7 +6528,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="84" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A84" s="12">
         <v>2035</v>
       </c>
@@ -6584,7 +6584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="12">
         <v>2035</v>
       </c>
@@ -6640,7 +6640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" s="12">
         <v>2035</v>
       </c>
@@ -6696,7 +6696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" s="12">
         <v>2035</v>
       </c>
@@ -6752,7 +6752,7 @@
         <v>41.25</v>
       </c>
     </row>
-    <row r="88" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="12">
         <v>2035</v>
       </c>
@@ -6808,7 +6808,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="89" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="12">
         <v>2035</v>
       </c>
@@ -6864,7 +6864,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="90" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90" s="12">
         <v>2035</v>
       </c>
@@ -6920,7 +6920,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="91" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" s="12">
         <v>2035</v>
       </c>
@@ -6976,7 +6976,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="92" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="12">
         <v>2035</v>
       </c>
@@ -7032,7 +7032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" s="12">
         <v>2035</v>
       </c>
@@ -7088,7 +7088,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="94" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" s="12">
         <v>2035</v>
       </c>
@@ -7144,7 +7144,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="95" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A95" s="12">
         <v>2035</v>
       </c>
@@ -7200,7 +7200,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="96" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A96" s="12">
         <v>2035</v>
       </c>
@@ -7256,7 +7256,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="97" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A97" s="12">
         <v>2035</v>
       </c>
@@ -7312,7 +7312,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="98" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" s="12">
         <v>2035</v>
       </c>
@@ -7368,7 +7368,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="99" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A99" s="12">
         <v>2035</v>
       </c>
@@ -7424,7 +7424,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="100" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A100" s="12">
         <v>2035</v>
       </c>
@@ -7480,7 +7480,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="101" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A101" s="12">
         <v>2035</v>
       </c>
@@ -7536,7 +7536,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="102" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A102" s="12">
         <v>2035</v>
       </c>
@@ -7595,7 +7595,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="103" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A103" s="12">
         <v>2035</v>
       </c>
@@ -7651,7 +7651,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="104" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A104" s="12">
         <v>2035</v>
       </c>
@@ -7716,7 +7716,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="105" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A105" s="58">
         <v>2035</v>
       </c>
@@ -7772,7 +7772,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="106" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A106" s="58">
         <v>2035</v>
       </c>
@@ -7828,7 +7828,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="107" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A107" s="58">
         <v>2035</v>
       </c>
@@ -7884,7 +7884,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="108" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A108" s="58">
         <v>2035</v>
       </c>
@@ -7943,7 +7943,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="109" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A109" s="58">
         <v>2035</v>
       </c>
@@ -8002,7 +8002,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="110" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A110" s="58">
         <v>2035</v>
       </c>
@@ -8027,6 +8027,9 @@
       <c r="I110" s="58" t="s">
         <v>11</v>
       </c>
+      <c r="J110" s="58" t="s">
+        <v>402</v>
+      </c>
       <c r="K110" s="58" t="s">
         <v>404</v>
       </c>
@@ -8064,7 +8067,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="111" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A111" s="62">
         <v>2035</v>
       </c>
@@ -8120,7 +8123,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="112" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A112" s="62">
         <v>2035</v>
       </c>
@@ -8176,7 +8179,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="113" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A113" s="62">
         <v>2035</v>
       </c>
@@ -8232,7 +8235,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="114" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A114" s="62">
         <v>2035</v>
       </c>
@@ -8291,7 +8294,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="115" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A115" s="62">
         <v>2035</v>
       </c>
@@ -8350,7 +8353,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="116" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A116" s="62">
         <v>2035</v>
       </c>
@@ -8372,6 +8375,9 @@
       <c r="H116" s="62" t="s">
         <v>445</v>
       </c>
+      <c r="J116" s="62" t="s">
+        <v>402</v>
+      </c>
       <c r="K116" s="62" t="s">
         <v>412</v>
       </c>
@@ -8406,7 +8412,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="117" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A117" s="62">
         <v>2035</v>
       </c>
@@ -8431,6 +8437,9 @@
       <c r="I117" s="62" t="s">
         <v>11</v>
       </c>
+      <c r="J117" s="62" t="s">
+        <v>402</v>
+      </c>
       <c r="K117" s="62" t="s">
         <v>412</v>
       </c>
@@ -8468,7 +8477,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="118" spans="1:22" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:22" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A118" s="24">
         <v>2050</v>
       </c>
@@ -8524,7 +8533,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="119" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A119" s="53">
         <v>2050</v>
       </c>
@@ -8580,7 +8589,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="120" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A120" s="53">
         <v>2050</v>
       </c>
@@ -8636,7 +8645,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="121" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A121" s="53">
         <v>2050</v>
       </c>
@@ -8692,7 +8701,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="122" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A122" s="53">
         <v>2050</v>
       </c>
@@ -8751,7 +8760,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="123" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A123" s="53">
         <v>2050</v>
       </c>
@@ -8816,7 +8825,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="124" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A124" s="53">
         <v>2050</v>
       </c>
@@ -8841,6 +8850,9 @@
       <c r="I124" s="75" t="s">
         <v>440</v>
       </c>
+      <c r="J124" s="53" t="s">
+        <v>402</v>
+      </c>
       <c r="K124" s="53" t="s">
         <v>404</v>
       </c>
@@ -8875,7 +8887,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="125" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A125" s="68">
         <v>2050</v>
       </c>
@@ -8931,7 +8943,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="126" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A126" s="68">
         <v>2050</v>
       </c>
@@ -8987,7 +8999,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="127" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A127" s="68">
         <v>2050</v>
       </c>
@@ -9043,7 +9055,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="128" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A128" s="68">
         <v>2050</v>
       </c>
@@ -9102,7 +9114,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="129" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A129" s="68">
         <v>2050</v>
       </c>
@@ -9161,7 +9173,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="130" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A130" s="68">
         <v>2050</v>
       </c>
@@ -9183,6 +9195,9 @@
       <c r="H130" s="69" t="s">
         <v>445</v>
       </c>
+      <c r="J130" s="68" t="s">
+        <v>402</v>
+      </c>
       <c r="K130" s="68" t="s">
         <v>416</v>
       </c>
@@ -9217,7 +9232,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="131" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A131" s="68">
         <v>2050</v>
       </c>
@@ -9241,6 +9256,9 @@
       </c>
       <c r="I131" s="68" t="s">
         <v>11</v>
+      </c>
+      <c r="J131" s="68" t="s">
+        <v>402</v>
       </c>
       <c r="K131" s="68" t="s">
         <v>416</v>

</xml_diff>

<commit_message>
Moved current tag to b series / IPAv15
and 2050_TM160_DBP_NoProject_05b is finally done
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\config_RTP2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058D1375-1DE8-4C90-97C8-C4BC6BFA2529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FB9A35-2831-4B8B-B9CF-7E861606B6CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-48" yWindow="684" windowWidth="25152" windowHeight="15480" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
+    <workbookView xWindow="6150" yWindow="4755" windowWidth="28800" windowHeight="15435" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelRuns" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1445" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1444" uniqueCount="451">
   <si>
     <t>year</t>
   </si>
@@ -1374,9 +1374,6 @@
   </si>
   <si>
     <t>https://app.asana.com/0/1182463234225195/1207094549470908/f</t>
-  </si>
-  <si>
-    <t>running</t>
   </si>
   <si>
     <t>https://app.asana.com/0/1182463234225195/1207094551343878/f</t>
@@ -1588,7 +1585,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1745,6 +1742,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2079,30 +2077,30 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C101" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K133" sqref="K133"/>
+      <selection pane="bottomRight" activeCell="I102" sqref="I102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="7" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="42.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="42.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="23" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="6.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="22.33203125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11.33203125" style="10" customWidth="1"/>
-    <col min="13" max="13" width="17.5546875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="8.33203125" style="1" customWidth="1"/>
-    <col min="15" max="16" width="9.33203125" style="43"/>
-    <col min="17" max="16384" width="9.33203125" style="1"/>
+    <col min="8" max="8" width="8.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="6.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="22.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" style="10" customWidth="1"/>
+    <col min="13" max="13" width="17.5703125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="8.28515625" style="1" customWidth="1"/>
+    <col min="15" max="16" width="9.28515625" style="43"/>
+    <col min="17" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="5" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2170,7 +2168,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="2" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="19">
         <v>2005</v>
       </c>
@@ -2223,7 +2221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="30">
         <v>2005</v>
       </c>
@@ -2279,7 +2277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="30">
         <v>2005</v>
       </c>
@@ -2334,7 +2332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="30">
         <v>2005</v>
       </c>
@@ -2389,7 +2387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="30">
         <v>2005</v>
       </c>
@@ -2454,7 +2452,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="7" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="52">
         <v>2015</v>
       </c>
@@ -2495,7 +2493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="34">
         <v>2015</v>
       </c>
@@ -2541,7 +2539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="34">
         <v>2015</v>
       </c>
@@ -2594,7 +2592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="34">
         <v>2015</v>
       </c>
@@ -2647,7 +2645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="34">
         <v>2015</v>
       </c>
@@ -2700,7 +2698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="34">
         <v>2015</v>
       </c>
@@ -2756,7 +2754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="34">
         <v>2015</v>
       </c>
@@ -2812,7 +2810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="34">
         <v>2015</v>
       </c>
@@ -2868,7 +2866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="34">
         <v>2015</v>
       </c>
@@ -2928,7 +2926,7 @@
       </c>
       <c r="V15" s="57"/>
     </row>
-    <row r="16" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="34">
         <v>2015</v>
       </c>
@@ -2990,7 +2988,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>2023</v>
       </c>
@@ -3036,7 +3034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>2023</v>
       </c>
@@ -3082,7 +3080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>2023</v>
       </c>
@@ -3128,7 +3126,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>2023</v>
       </c>
@@ -3174,7 +3172,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>2023</v>
       </c>
@@ -3220,7 +3218,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>2023</v>
       </c>
@@ -3266,7 +3264,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>2023</v>
       </c>
@@ -3312,7 +3310,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>2023</v>
       </c>
@@ -3358,7 +3356,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>2023</v>
       </c>
@@ -3404,7 +3402,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>2023</v>
       </c>
@@ -3450,7 +3448,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>2023</v>
       </c>
@@ -3496,7 +3494,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>2023</v>
       </c>
@@ -3542,7 +3540,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>2023</v>
       </c>
@@ -3588,7 +3586,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>2023</v>
       </c>
@@ -3634,7 +3632,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>2023</v>
       </c>
@@ -3680,7 +3678,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>2023</v>
       </c>
@@ -3726,7 +3724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>2023</v>
       </c>
@@ -3772,7 +3770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>2023</v>
       </c>
@@ -3818,7 +3816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>2023</v>
       </c>
@@ -3862,7 +3860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>2023</v>
       </c>
@@ -3911,7 +3909,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>2023</v>
       </c>
@@ -3958,7 +3956,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>2023</v>
       </c>
@@ -4005,7 +4003,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>2023</v>
       </c>
@@ -4061,7 +4059,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>2023</v>
       </c>
@@ -4117,7 +4115,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>2023</v>
       </c>
@@ -4173,7 +4171,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>2023</v>
       </c>
@@ -4229,7 +4227,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>2023</v>
       </c>
@@ -4285,7 +4283,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>2023</v>
       </c>
@@ -4341,7 +4339,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>2023</v>
       </c>
@@ -4397,7 +4395,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>2023</v>
       </c>
@@ -4453,7 +4451,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>2023</v>
       </c>
@@ -4509,7 +4507,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>2023</v>
       </c>
@@ -4565,7 +4563,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>2023</v>
       </c>
@@ -4621,7 +4619,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>2023</v>
       </c>
@@ -4677,7 +4675,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>2023</v>
       </c>
@@ -4733,7 +4731,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>2023</v>
       </c>
@@ -4789,7 +4787,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>2023</v>
       </c>
@@ -4845,7 +4843,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>2023</v>
       </c>
@@ -4901,7 +4899,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>2023</v>
       </c>
@@ -4957,7 +4955,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>2023</v>
       </c>
@@ -5013,7 +5011,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>2023</v>
       </c>
@@ -5069,7 +5067,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>2023</v>
       </c>
@@ -5125,7 +5123,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>2023</v>
       </c>
@@ -5181,7 +5179,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>2023</v>
       </c>
@@ -5237,7 +5235,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>2023</v>
       </c>
@@ -5293,7 +5291,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>2023</v>
       </c>
@@ -5349,7 +5347,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>2023</v>
       </c>
@@ -5405,7 +5403,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>2023</v>
       </c>
@@ -5464,7 +5462,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>2023</v>
       </c>
@@ -5520,7 +5518,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>2023</v>
       </c>
@@ -5579,7 +5577,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>2023</v>
       </c>
@@ -5638,7 +5636,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>2023</v>
       </c>
@@ -5697,7 +5695,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>2023</v>
       </c>
@@ -5756,7 +5754,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="70" spans="1:22" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:22" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>2023</v>
       </c>
@@ -5812,7 +5810,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="71" spans="1:22" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:22" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>2023</v>
       </c>
@@ -5868,7 +5866,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>2023</v>
       </c>
@@ -5924,7 +5922,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>2023</v>
       </c>
@@ -5980,7 +5978,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>2023</v>
       </c>
@@ -6036,7 +6034,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>2023</v>
       </c>
@@ -6095,7 +6093,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>2023</v>
       </c>
@@ -6155,7 +6153,7 @@
       </c>
       <c r="V76" s="73"/>
     </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>2023</v>
       </c>
@@ -6217,7 +6215,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="78" spans="1:22" s="27" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:22" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="27">
         <v>2025</v>
       </c>
@@ -6245,7 +6243,7 @@
       <c r="T78" s="29"/>
       <c r="U78" s="29"/>
     </row>
-    <row r="79" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="15">
         <v>2035</v>
       </c>
@@ -6304,7 +6302,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="80" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="12">
         <v>2035</v>
       </c>
@@ -6360,7 +6358,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="81" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="12">
         <v>2035</v>
       </c>
@@ -6416,7 +6414,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="82" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="12">
         <v>2035</v>
       </c>
@@ -6472,7 +6470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="12">
         <v>2035</v>
       </c>
@@ -6528,7 +6526,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="84" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="12">
         <v>2035</v>
       </c>
@@ -6584,7 +6582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="12">
         <v>2035</v>
       </c>
@@ -6640,7 +6638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="12">
         <v>2035</v>
       </c>
@@ -6696,7 +6694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="12">
         <v>2035</v>
       </c>
@@ -6752,7 +6750,7 @@
         <v>41.25</v>
       </c>
     </row>
-    <row r="88" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A88" s="12">
         <v>2035</v>
       </c>
@@ -6808,7 +6806,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="89" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" s="12">
         <v>2035</v>
       </c>
@@ -6864,7 +6862,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="90" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A90" s="12">
         <v>2035</v>
       </c>
@@ -6920,7 +6918,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="91" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="12">
         <v>2035</v>
       </c>
@@ -6976,7 +6974,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="92" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="12">
         <v>2035</v>
       </c>
@@ -7032,7 +7030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A93" s="12">
         <v>2035</v>
       </c>
@@ -7088,7 +7086,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="94" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A94" s="12">
         <v>2035</v>
       </c>
@@ -7144,7 +7142,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="95" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A95" s="12">
         <v>2035</v>
       </c>
@@ -7200,7 +7198,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="96" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A96" s="12">
         <v>2035</v>
       </c>
@@ -7256,7 +7254,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="97" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A97" s="12">
         <v>2035</v>
       </c>
@@ -7312,7 +7310,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="98" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="12">
         <v>2035</v>
       </c>
@@ -7368,7 +7366,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="99" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A99" s="12">
         <v>2035</v>
       </c>
@@ -7424,7 +7422,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="100" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A100" s="12">
         <v>2035</v>
       </c>
@@ -7480,7 +7478,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="101" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A101" s="12">
         <v>2035</v>
       </c>
@@ -7536,7 +7534,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="102" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A102" s="12">
         <v>2035</v>
       </c>
@@ -7558,6 +7556,9 @@
       <c r="H102" s="12" t="s">
         <v>116</v>
       </c>
+      <c r="I102" s="75" t="s">
+        <v>11</v>
+      </c>
       <c r="J102" s="12" t="s">
         <v>402</v>
       </c>
@@ -7595,7 +7596,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="103" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A103" s="12">
         <v>2035</v>
       </c>
@@ -7651,7 +7652,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="104" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A104" s="12">
         <v>2035</v>
       </c>
@@ -7673,9 +7674,6 @@
       <c r="H104" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="I104" s="12" t="s">
-        <v>11</v>
-      </c>
       <c r="J104" s="12" t="s">
         <v>402</v>
       </c>
@@ -7716,7 +7714,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="105" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A105" s="58">
         <v>2035</v>
       </c>
@@ -7772,7 +7770,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="106" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A106" s="58">
         <v>2035</v>
       </c>
@@ -7828,7 +7826,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="107" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A107" s="58">
         <v>2035</v>
       </c>
@@ -7884,7 +7882,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="108" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A108" s="58">
         <v>2035</v>
       </c>
@@ -7943,7 +7941,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="109" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A109" s="58">
         <v>2035</v>
       </c>
@@ -8002,7 +8000,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="110" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A110" s="58">
         <v>2035</v>
       </c>
@@ -8024,7 +8022,7 @@
       <c r="H110" s="58" t="s">
         <v>423</v>
       </c>
-      <c r="I110" s="58" t="s">
+      <c r="I110" s="76" t="s">
         <v>11</v>
       </c>
       <c r="J110" s="58" t="s">
@@ -8067,7 +8065,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="111" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A111" s="62">
         <v>2035</v>
       </c>
@@ -8123,7 +8121,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="112" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A112" s="62">
         <v>2035</v>
       </c>
@@ -8179,7 +8177,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="113" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A113" s="62">
         <v>2035</v>
       </c>
@@ -8235,7 +8233,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="114" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A114" s="62">
         <v>2035</v>
       </c>
@@ -8294,7 +8292,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="115" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A115" s="62">
         <v>2035</v>
       </c>
@@ -8353,12 +8351,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="116" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A116" s="62">
         <v>2035</v>
       </c>
       <c r="B116" s="62" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C116" s="63" t="s">
         <v>338</v>
@@ -8367,13 +8365,13 @@
         <v>339</v>
       </c>
       <c r="F116" s="62" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G116" s="62" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="H116" s="62" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="J116" s="62" t="s">
         <v>402</v>
@@ -8385,7 +8383,7 @@
         <v>43</v>
       </c>
       <c r="M116" s="63" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="N116" s="62">
         <v>16.82</v>
@@ -8412,12 +8410,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="117" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A117" s="62">
         <v>2035</v>
       </c>
       <c r="B117" s="62" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C117" s="63" t="s">
         <v>338</v>
@@ -8426,15 +8424,15 @@
         <v>339</v>
       </c>
       <c r="F117" s="62" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="G117" s="62" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="H117" s="62" t="s">
-        <v>445</v>
-      </c>
-      <c r="I117" s="62" t="s">
+        <v>444</v>
+      </c>
+      <c r="I117" s="76" t="s">
         <v>11</v>
       </c>
       <c r="J117" s="62" t="s">
@@ -8477,7 +8475,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="118" spans="1:22" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:22" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A118" s="24">
         <v>2050</v>
       </c>
@@ -8533,7 +8531,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="119" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A119" s="53">
         <v>2050</v>
       </c>
@@ -8589,7 +8587,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="120" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A120" s="53">
         <v>2050</v>
       </c>
@@ -8645,7 +8643,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="121" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A121" s="53">
         <v>2050</v>
       </c>
@@ -8701,7 +8699,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="122" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A122" s="53">
         <v>2050</v>
       </c>
@@ -8760,7 +8758,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="123" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A123" s="53">
         <v>2050</v>
       </c>
@@ -8782,9 +8780,6 @@
       <c r="H123" s="52" t="s">
         <v>427</v>
       </c>
-      <c r="I123" s="53" t="s">
-        <v>11</v>
-      </c>
       <c r="J123" s="53" t="s">
         <v>402</v>
       </c>
@@ -8825,7 +8820,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="124" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A124" s="53">
         <v>2050</v>
       </c>
@@ -8839,7 +8834,7 @@
         <v>339</v>
       </c>
       <c r="F124" s="53" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="G124" s="53" t="s">
         <v>428</v>
@@ -8848,7 +8843,7 @@
         <v>427</v>
       </c>
       <c r="I124" s="75" t="s">
-        <v>440</v>
+        <v>11</v>
       </c>
       <c r="J124" s="53" t="s">
         <v>402</v>
@@ -8887,7 +8882,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="125" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A125" s="68">
         <v>2050</v>
       </c>
@@ -8943,7 +8938,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="126" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A126" s="68">
         <v>2050</v>
       </c>
@@ -8999,7 +8994,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="127" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A127" s="68">
         <v>2050</v>
       </c>
@@ -9055,7 +9050,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="128" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A128" s="68">
         <v>2050</v>
       </c>
@@ -9114,7 +9109,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="129" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A129" s="68">
         <v>2050</v>
       </c>
@@ -9173,12 +9168,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="130" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A130" s="68">
         <v>2050</v>
       </c>
       <c r="B130" s="68" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C130" s="68" t="s">
         <v>338</v>
@@ -9187,13 +9182,13 @@
         <v>339</v>
       </c>
       <c r="F130" s="68" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G130" s="68" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="H130" s="69" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="J130" s="68" t="s">
         <v>402</v>
@@ -9205,7 +9200,7 @@
         <v>42</v>
       </c>
       <c r="M130" s="68" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="N130" s="68">
         <v>18.420000000000002</v>
@@ -9232,12 +9227,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="131" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A131" s="68">
         <v>2050</v>
       </c>
       <c r="B131" s="68" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C131" s="68" t="s">
         <v>338</v>
@@ -9246,15 +9241,15 @@
         <v>339</v>
       </c>
       <c r="F131" s="68" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="G131" s="68" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="H131" s="69" t="s">
-        <v>445</v>
-      </c>
-      <c r="I131" s="68" t="s">
+        <v>444</v>
+      </c>
+      <c r="I131" s="75" t="s">
         <v>11</v>
       </c>
       <c r="J131" s="68" t="s">
@@ -9267,7 +9262,7 @@
         <v>42</v>
       </c>
       <c r="M131" s="68" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="N131" s="68">
         <v>19.57</v>

</xml_diff>

<commit_message>
Move 2050 No Project to 2050_TM160_DBP_NoProject_05b
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FB9A35-2831-4B8B-B9CF-7E861606B6CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73A9C033-4F2D-4516-82AA-A06C7EF66923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6150" yWindow="4755" windowWidth="28800" windowHeight="15435" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
@@ -2074,10 +2074,10 @@
   <dimension ref="A1:V131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C101" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F101" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I102" sqref="I102"/>
+      <selection pane="bottomRight" activeCell="V124" sqref="V124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8816,9 +8816,6 @@
       <c r="U123" s="56">
         <v>72</v>
       </c>
-      <c r="V123" s="53" t="s">
-        <v>362</v>
-      </c>
     </row>
     <row r="124" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A124" s="53">
@@ -8880,6 +8877,9 @@
       </c>
       <c r="U124" s="56">
         <v>72</v>
+      </c>
+      <c r="V124" s="53" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="125" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add Plan v07b, NoProject 06b and make them current
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73A9C033-4F2D-4516-82AA-A06C7EF66923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936AC9A6-FA3B-4F59-A89E-9312BA79A9FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6150" yWindow="4755" windowWidth="28800" windowHeight="15435" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
+    <workbookView xWindow="3975" yWindow="2250" windowWidth="18300" windowHeight="9855" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelRuns" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1444" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1489" uniqueCount="466">
   <si>
     <t>year</t>
   </si>
@@ -1407,6 +1407,51 @@
   </si>
   <si>
     <t>https://app.asana.com/0/1182463234225195/1207094549470916/f</t>
+  </si>
+  <si>
+    <t>2035_TM160_DBP_NoProject_06b</t>
+  </si>
+  <si>
+    <t>Updated landuse/popsyn</t>
+  </si>
+  <si>
+    <t>M:\urban_modeling\baus\PBA50Plus\PBA50Plus_NoProject_v7</t>
+  </si>
+  <si>
+    <t>PBA50Plus_NoProject_v7</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1182463234225195/1207127651751783/f</t>
+  </si>
+  <si>
+    <t>2050_TM160_DBP_NoProject_06b</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1182463234225195/1207127941488239/f</t>
+  </si>
+  <si>
+    <t>2035_TM160_DBP_Plan_07b</t>
+  </si>
+  <si>
+    <t>Update landuse/popsyn (fix too many persons)</t>
+  </si>
+  <si>
+    <t>M:\urban_modeling\baus\PBA50Plus\PBA50Plus_DraftBlueprint\PBA50Plus_Draft_Blueprint_v6</t>
+  </si>
+  <si>
+    <t>PBA50Plus_Draft_Blueprint_v6</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1182463234225195/1207127280475842/f</t>
+  </si>
+  <si>
+    <t>2050_TM160_DBP_Plan_07b</t>
+  </si>
+  <si>
+    <t>Update landuse/popsyn (fix too many persons); tweak bike back</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1182463234225195/1207127280475846/f</t>
   </si>
 </sst>
 </file>
@@ -2071,13 +2116,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9564CC59-3725-4FDA-8BF2-0F68CB1B6F5A}">
-  <dimension ref="A1:V131"/>
+  <dimension ref="A1:V135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F101" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C114" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V124" sqref="V124"/>
+      <selection pane="bottomRight" activeCell="A135" sqref="A135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8022,9 +8067,6 @@
       <c r="H110" s="58" t="s">
         <v>423</v>
       </c>
-      <c r="I110" s="76" t="s">
-        <v>11</v>
-      </c>
       <c r="J110" s="58" t="s">
         <v>402</v>
       </c>
@@ -8061,64 +8103,67 @@
       <c r="U110" s="61">
         <v>72</v>
       </c>
-      <c r="V110" s="58" t="s">
+    </row>
+    <row r="111" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="58">
+        <v>2035</v>
+      </c>
+      <c r="B111" s="58" t="s">
+        <v>451</v>
+      </c>
+      <c r="C111" s="58" t="s">
+        <v>338</v>
+      </c>
+      <c r="D111" s="58" t="s">
+        <v>339</v>
+      </c>
+      <c r="F111" s="58" t="s">
+        <v>452</v>
+      </c>
+      <c r="G111" s="58" t="s">
+        <v>453</v>
+      </c>
+      <c r="H111" s="58" t="s">
+        <v>454</v>
+      </c>
+      <c r="I111" s="76" t="s">
+        <v>11</v>
+      </c>
+      <c r="K111" s="58" t="s">
+        <v>404</v>
+      </c>
+      <c r="L111" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="M111" s="58" t="s">
+        <v>455</v>
+      </c>
+      <c r="N111" s="58">
+        <v>17.579999999999998</v>
+      </c>
+      <c r="O111" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="P111" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q111" s="58">
+        <v>0.87</v>
+      </c>
+      <c r="R111" s="58">
+        <v>0.78</v>
+      </c>
+      <c r="S111" s="61">
+        <v>83.3</v>
+      </c>
+      <c r="T111" s="61">
+        <v>0</v>
+      </c>
+      <c r="U111" s="61">
+        <v>72</v>
+      </c>
+      <c r="V111" s="58" t="s">
         <v>361</v>
-      </c>
-    </row>
-    <row r="111" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="62">
-        <v>2035</v>
-      </c>
-      <c r="B111" s="62" t="s">
-        <v>345</v>
-      </c>
-      <c r="C111" s="63" t="s">
-        <v>338</v>
-      </c>
-      <c r="D111" s="62" t="s">
-        <v>339</v>
-      </c>
-      <c r="F111" s="62" t="s">
-        <v>346</v>
-      </c>
-      <c r="G111" s="62" t="s">
-        <v>347</v>
-      </c>
-      <c r="H111" s="62" t="s">
-        <v>348</v>
-      </c>
-      <c r="K111" s="62" t="s">
-        <v>349</v>
-      </c>
-      <c r="L111" s="64" t="s">
-        <v>129</v>
-      </c>
-      <c r="M111" s="63" t="s">
-        <v>350</v>
-      </c>
-      <c r="N111" s="62">
-        <v>17.579999999999998</v>
-      </c>
-      <c r="O111" s="65" t="s">
-        <v>109</v>
-      </c>
-      <c r="P111" s="65" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q111" s="62">
-        <v>0.87</v>
-      </c>
-      <c r="R111" s="62">
-        <v>0.78</v>
-      </c>
-      <c r="S111" s="66">
-        <v>83.3</v>
-      </c>
-      <c r="T111" s="66">
-        <v>0</v>
-      </c>
-      <c r="U111" s="66">
-        <v>72</v>
       </c>
     </row>
     <row r="112" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.2">
@@ -8126,7 +8171,7 @@
         <v>2035</v>
       </c>
       <c r="B112" s="62" t="s">
-        <v>378</v>
+        <v>345</v>
       </c>
       <c r="C112" s="63" t="s">
         <v>338</v>
@@ -8135,7 +8180,7 @@
         <v>339</v>
       </c>
       <c r="F112" s="62" t="s">
-        <v>376</v>
+        <v>346</v>
       </c>
       <c r="G112" s="62" t="s">
         <v>347</v>
@@ -8150,10 +8195,10 @@
         <v>129</v>
       </c>
       <c r="M112" s="63" t="s">
-        <v>379</v>
+        <v>350</v>
       </c>
       <c r="N112" s="62">
-        <v>16.82</v>
+        <v>17.579999999999998</v>
       </c>
       <c r="O112" s="65" t="s">
         <v>109</v>
@@ -8182,7 +8227,7 @@
         <v>2035</v>
       </c>
       <c r="B113" s="62" t="s">
-        <v>390</v>
+        <v>378</v>
       </c>
       <c r="C113" s="63" t="s">
         <v>338</v>
@@ -8191,22 +8236,22 @@
         <v>339</v>
       </c>
       <c r="F113" s="62" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="G113" s="62" t="s">
-        <v>391</v>
+        <v>347</v>
       </c>
       <c r="H113" s="62" t="s">
-        <v>393</v>
+        <v>348</v>
       </c>
       <c r="K113" s="62" t="s">
-        <v>396</v>
+        <v>349</v>
       </c>
       <c r="L113" s="64" t="s">
         <v>129</v>
       </c>
       <c r="M113" s="63" t="s">
-        <v>397</v>
+        <v>379</v>
       </c>
       <c r="N113" s="62">
         <v>16.82</v>
@@ -8238,7 +8283,7 @@
         <v>2035</v>
       </c>
       <c r="B114" s="62" t="s">
-        <v>408</v>
+        <v>390</v>
       </c>
       <c r="C114" s="63" t="s">
         <v>338</v>
@@ -8247,25 +8292,22 @@
         <v>339</v>
       </c>
       <c r="F114" s="62" t="s">
-        <v>409</v>
+        <v>386</v>
       </c>
       <c r="G114" s="62" t="s">
-        <v>410</v>
+        <v>391</v>
       </c>
       <c r="H114" s="62" t="s">
-        <v>411</v>
-      </c>
-      <c r="J114" s="62" t="s">
-        <v>402</v>
+        <v>393</v>
       </c>
       <c r="K114" s="62" t="s">
-        <v>412</v>
+        <v>396</v>
       </c>
       <c r="L114" s="64" t="s">
-        <v>43</v>
+        <v>129</v>
       </c>
       <c r="M114" s="63" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="N114" s="62">
         <v>16.82</v>
@@ -8297,7 +8339,7 @@
         <v>2035</v>
       </c>
       <c r="B115" s="62" t="s">
-        <v>425</v>
+        <v>408</v>
       </c>
       <c r="C115" s="63" t="s">
         <v>338</v>
@@ -8306,13 +8348,13 @@
         <v>339</v>
       </c>
       <c r="F115" s="62" t="s">
-        <v>426</v>
+        <v>409</v>
       </c>
       <c r="G115" s="62" t="s">
-        <v>428</v>
+        <v>410</v>
       </c>
       <c r="H115" s="62" t="s">
-        <v>427</v>
+        <v>411</v>
       </c>
       <c r="J115" s="62" t="s">
         <v>402</v>
@@ -8324,7 +8366,7 @@
         <v>43</v>
       </c>
       <c r="M115" s="63" t="s">
-        <v>429</v>
+        <v>413</v>
       </c>
       <c r="N115" s="62">
         <v>16.82</v>
@@ -8356,7 +8398,7 @@
         <v>2035</v>
       </c>
       <c r="B116" s="62" t="s">
-        <v>441</v>
+        <v>425</v>
       </c>
       <c r="C116" s="63" t="s">
         <v>338</v>
@@ -8365,13 +8407,13 @@
         <v>339</v>
       </c>
       <c r="F116" s="62" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="G116" s="62" t="s">
-        <v>445</v>
+        <v>428</v>
       </c>
       <c r="H116" s="62" t="s">
-        <v>444</v>
+        <v>427</v>
       </c>
       <c r="J116" s="62" t="s">
         <v>402</v>
@@ -8383,7 +8425,7 @@
         <v>43</v>
       </c>
       <c r="M116" s="63" t="s">
-        <v>443</v>
+        <v>429</v>
       </c>
       <c r="N116" s="62">
         <v>16.82</v>
@@ -8415,7 +8457,7 @@
         <v>2035</v>
       </c>
       <c r="B117" s="62" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C117" s="63" t="s">
         <v>338</v>
@@ -8424,7 +8466,7 @@
         <v>339</v>
       </c>
       <c r="F117" s="62" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G117" s="62" t="s">
         <v>445</v>
@@ -8432,9 +8474,6 @@
       <c r="H117" s="62" t="s">
         <v>444</v>
       </c>
-      <c r="I117" s="76" t="s">
-        <v>11</v>
-      </c>
       <c r="J117" s="62" t="s">
         <v>402</v>
       </c>
@@ -8445,10 +8484,10 @@
         <v>43</v>
       </c>
       <c r="M117" s="63" t="s">
-        <v>437</v>
+        <v>443</v>
       </c>
       <c r="N117" s="62">
-        <v>18.03</v>
+        <v>16.82</v>
       </c>
       <c r="O117" s="65" t="s">
         <v>109</v>
@@ -8471,176 +8510,182 @@
       <c r="U117" s="66">
         <v>72</v>
       </c>
-      <c r="V117" s="62" t="s">
+    </row>
+    <row r="118" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="62">
+        <v>2035</v>
+      </c>
+      <c r="B118" s="62" t="s">
+        <v>442</v>
+      </c>
+      <c r="C118" s="63" t="s">
+        <v>338</v>
+      </c>
+      <c r="D118" s="62" t="s">
+        <v>339</v>
+      </c>
+      <c r="F118" s="62" t="s">
+        <v>447</v>
+      </c>
+      <c r="G118" s="62" t="s">
+        <v>445</v>
+      </c>
+      <c r="H118" s="62" t="s">
+        <v>444</v>
+      </c>
+      <c r="J118" s="62" t="s">
+        <v>402</v>
+      </c>
+      <c r="K118" s="62" t="s">
+        <v>412</v>
+      </c>
+      <c r="L118" s="64" t="s">
+        <v>43</v>
+      </c>
+      <c r="M118" s="63" t="s">
+        <v>437</v>
+      </c>
+      <c r="N118" s="62">
+        <v>18.03</v>
+      </c>
+      <c r="O118" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="P118" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q118" s="62">
+        <v>0.87</v>
+      </c>
+      <c r="R118" s="62">
+        <v>0.78</v>
+      </c>
+      <c r="S118" s="66">
+        <v>83.3</v>
+      </c>
+      <c r="T118" s="66">
+        <v>0</v>
+      </c>
+      <c r="U118" s="66">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="119" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A119" s="62">
+        <v>2035</v>
+      </c>
+      <c r="B119" s="62" t="s">
+        <v>458</v>
+      </c>
+      <c r="C119" s="63" t="s">
+        <v>338</v>
+      </c>
+      <c r="D119" s="62" t="s">
+        <v>339</v>
+      </c>
+      <c r="F119" s="62" t="s">
+        <v>459</v>
+      </c>
+      <c r="G119" s="62" t="s">
+        <v>460</v>
+      </c>
+      <c r="H119" s="62" t="s">
+        <v>461</v>
+      </c>
+      <c r="I119" s="76" t="s">
+        <v>11</v>
+      </c>
+      <c r="K119" s="62" t="s">
+        <v>412</v>
+      </c>
+      <c r="L119" s="64" t="s">
+        <v>16</v>
+      </c>
+      <c r="M119" s="63" t="s">
+        <v>462</v>
+      </c>
+      <c r="N119" s="62">
+        <v>18.03</v>
+      </c>
+      <c r="O119" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="P119" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q119" s="62">
+        <v>0.87</v>
+      </c>
+      <c r="R119" s="62">
+        <v>0.78</v>
+      </c>
+      <c r="S119" s="66">
+        <v>83.3</v>
+      </c>
+      <c r="T119" s="66">
+        <v>0</v>
+      </c>
+      <c r="U119" s="66">
+        <v>72</v>
+      </c>
+      <c r="V119" s="62" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="118" spans="1:22" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="24">
+    <row r="120" spans="1:22" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="24">
         <v>2050</v>
       </c>
-      <c r="B118" s="24" t="s">
+      <c r="B120" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="C118" s="24" t="s">
+      <c r="C120" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="D118" s="24" t="s">
+      <c r="D120" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="F118" s="24" t="s">
+      <c r="F120" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="G118" s="24" t="s">
+      <c r="G120" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="H118" s="25" t="s">
+      <c r="H120" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="K118" s="24" t="s">
+      <c r="K120" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="L118" s="26" t="s">
+      <c r="L120" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="M118" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="N118" s="24">
+      <c r="M120" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="N120" s="24">
         <v>17.440000000000001</v>
       </c>
-      <c r="O118" s="47">
+      <c r="O120" s="47">
         <v>-0.33</v>
       </c>
-      <c r="P118" s="47">
-        <v>0</v>
-      </c>
-      <c r="Q118" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="R118" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="S118" s="72" t="s">
-        <v>109</v>
-      </c>
-      <c r="T118" s="72" t="s">
-        <v>109</v>
-      </c>
-      <c r="U118" s="72" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="119" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="53">
-        <v>2050</v>
-      </c>
-      <c r="B119" s="53" t="s">
-        <v>351</v>
-      </c>
-      <c r="C119" s="53" t="s">
-        <v>338</v>
-      </c>
-      <c r="D119" s="53" t="s">
-        <v>339</v>
-      </c>
-      <c r="F119" s="53" t="s">
-        <v>353</v>
-      </c>
-      <c r="G119" s="53" t="s">
-        <v>342</v>
-      </c>
-      <c r="H119" s="52" t="s">
-        <v>343</v>
-      </c>
-      <c r="K119" s="53" t="s">
-        <v>344</v>
-      </c>
-      <c r="L119" s="52" t="s">
-        <v>16</v>
-      </c>
-      <c r="M119" s="53" t="s">
-        <v>356</v>
-      </c>
-      <c r="N119" s="53">
-        <v>19.13</v>
-      </c>
-      <c r="O119" s="67" t="s">
-        <v>109</v>
-      </c>
-      <c r="P119" s="67" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q119" s="53">
-        <v>0.87</v>
-      </c>
-      <c r="R119" s="53">
-        <v>0.78</v>
-      </c>
-      <c r="S119" s="56">
-        <v>83.3</v>
-      </c>
-      <c r="T119" s="56">
-        <v>0</v>
-      </c>
-      <c r="U119" s="56">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="120" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="53">
-        <v>2050</v>
-      </c>
-      <c r="B120" s="53" t="s">
-        <v>380</v>
-      </c>
-      <c r="C120" s="53" t="s">
-        <v>338</v>
-      </c>
-      <c r="D120" s="53" t="s">
-        <v>339</v>
-      </c>
-      <c r="F120" s="53" t="s">
-        <v>376</v>
-      </c>
-      <c r="G120" s="53" t="s">
-        <v>342</v>
-      </c>
-      <c r="H120" s="52" t="s">
-        <v>343</v>
-      </c>
-      <c r="K120" s="53" t="s">
-        <v>344</v>
-      </c>
-      <c r="L120" s="52" t="s">
-        <v>16</v>
-      </c>
-      <c r="M120" s="53" t="s">
-        <v>381</v>
-      </c>
-      <c r="N120" s="53">
-        <v>18.420000000000002</v>
-      </c>
-      <c r="O120" s="67" t="s">
-        <v>109</v>
-      </c>
-      <c r="P120" s="67" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q120" s="53">
-        <v>0.87</v>
-      </c>
-      <c r="R120" s="53">
-        <v>0.78</v>
-      </c>
-      <c r="S120" s="56">
-        <v>83.3</v>
-      </c>
-      <c r="T120" s="56">
-        <v>0</v>
-      </c>
-      <c r="U120" s="56">
-        <v>72</v>
+      <c r="P120" s="47">
+        <v>0</v>
+      </c>
+      <c r="Q120" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="R120" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="S120" s="72" t="s">
+        <v>109</v>
+      </c>
+      <c r="T120" s="72" t="s">
+        <v>109</v>
+      </c>
+      <c r="U120" s="72" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="121" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.2">
@@ -8648,7 +8693,7 @@
         <v>2050</v>
       </c>
       <c r="B121" s="53" t="s">
-        <v>388</v>
+        <v>351</v>
       </c>
       <c r="C121" s="53" t="s">
         <v>338</v>
@@ -8657,25 +8702,25 @@
         <v>339</v>
       </c>
       <c r="F121" s="53" t="s">
-        <v>386</v>
+        <v>353</v>
       </c>
       <c r="G121" s="53" t="s">
-        <v>387</v>
+        <v>342</v>
       </c>
       <c r="H121" s="52" t="s">
-        <v>392</v>
+        <v>343</v>
       </c>
       <c r="K121" s="53" t="s">
-        <v>394</v>
+        <v>344</v>
       </c>
       <c r="L121" s="52" t="s">
         <v>16</v>
       </c>
       <c r="M121" s="53" t="s">
-        <v>400</v>
+        <v>356</v>
       </c>
       <c r="N121" s="53">
-        <v>18.420000000000002</v>
+        <v>19.13</v>
       </c>
       <c r="O121" s="67" t="s">
         <v>109</v>
@@ -8704,7 +8749,7 @@
         <v>2050</v>
       </c>
       <c r="B122" s="53" t="s">
-        <v>414</v>
+        <v>380</v>
       </c>
       <c r="C122" s="53" t="s">
         <v>338</v>
@@ -8713,25 +8758,22 @@
         <v>339</v>
       </c>
       <c r="F122" s="53" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="G122" s="53" t="s">
-        <v>407</v>
+        <v>342</v>
       </c>
       <c r="H122" s="52" t="s">
-        <v>406</v>
-      </c>
-      <c r="J122" s="53" t="s">
-        <v>402</v>
+        <v>343</v>
       </c>
       <c r="K122" s="53" t="s">
-        <v>404</v>
+        <v>344</v>
       </c>
       <c r="L122" s="52" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="M122" s="53" t="s">
-        <v>418</v>
+        <v>381</v>
       </c>
       <c r="N122" s="53">
         <v>18.420000000000002</v>
@@ -8763,7 +8805,7 @@
         <v>2050</v>
       </c>
       <c r="B123" s="53" t="s">
-        <v>430</v>
+        <v>388</v>
       </c>
       <c r="C123" s="53" t="s">
         <v>338</v>
@@ -8772,25 +8814,22 @@
         <v>339</v>
       </c>
       <c r="F123" s="53" t="s">
-        <v>426</v>
+        <v>386</v>
       </c>
       <c r="G123" s="53" t="s">
-        <v>428</v>
+        <v>387</v>
       </c>
       <c r="H123" s="52" t="s">
-        <v>427</v>
-      </c>
-      <c r="J123" s="53" t="s">
-        <v>402</v>
+        <v>392</v>
       </c>
       <c r="K123" s="53" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
       <c r="L123" s="52" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="M123" s="53" t="s">
-        <v>431</v>
+        <v>400</v>
       </c>
       <c r="N123" s="53">
         <v>18.420000000000002</v>
@@ -8822,7 +8861,7 @@
         <v>2050</v>
       </c>
       <c r="B124" s="53" t="s">
-        <v>438</v>
+        <v>414</v>
       </c>
       <c r="C124" s="53" t="s">
         <v>338</v>
@@ -8831,16 +8870,13 @@
         <v>339</v>
       </c>
       <c r="F124" s="53" t="s">
-        <v>447</v>
+        <v>386</v>
       </c>
       <c r="G124" s="53" t="s">
-        <v>428</v>
+        <v>407</v>
       </c>
       <c r="H124" s="52" t="s">
-        <v>427</v>
-      </c>
-      <c r="I124" s="75" t="s">
-        <v>11</v>
+        <v>406</v>
       </c>
       <c r="J124" s="53" t="s">
         <v>402</v>
@@ -8849,13 +8885,13 @@
         <v>404</v>
       </c>
       <c r="L124" s="52" t="s">
-        <v>88</v>
+        <v>42</v>
       </c>
       <c r="M124" s="53" t="s">
-        <v>439</v>
+        <v>418</v>
       </c>
       <c r="N124" s="53">
-        <v>19.13</v>
+        <v>18.420000000000002</v>
       </c>
       <c r="O124" s="67" t="s">
         <v>109</v>
@@ -8878,176 +8914,185 @@
       <c r="U124" s="56">
         <v>72</v>
       </c>
-      <c r="V124" s="53" t="s">
+    </row>
+    <row r="125" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="53">
+        <v>2050</v>
+      </c>
+      <c r="B125" s="53" t="s">
+        <v>430</v>
+      </c>
+      <c r="C125" s="53" t="s">
+        <v>338</v>
+      </c>
+      <c r="D125" s="53" t="s">
+        <v>339</v>
+      </c>
+      <c r="F125" s="53" t="s">
+        <v>426</v>
+      </c>
+      <c r="G125" s="53" t="s">
+        <v>428</v>
+      </c>
+      <c r="H125" s="52" t="s">
+        <v>427</v>
+      </c>
+      <c r="J125" s="53" t="s">
+        <v>402</v>
+      </c>
+      <c r="K125" s="53" t="s">
+        <v>404</v>
+      </c>
+      <c r="L125" s="52" t="s">
+        <v>42</v>
+      </c>
+      <c r="M125" s="53" t="s">
+        <v>431</v>
+      </c>
+      <c r="N125" s="53">
+        <v>18.420000000000002</v>
+      </c>
+      <c r="O125" s="67" t="s">
+        <v>109</v>
+      </c>
+      <c r="P125" s="67" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q125" s="53">
+        <v>0.87</v>
+      </c>
+      <c r="R125" s="53">
+        <v>0.78</v>
+      </c>
+      <c r="S125" s="56">
+        <v>83.3</v>
+      </c>
+      <c r="T125" s="56">
+        <v>0</v>
+      </c>
+      <c r="U125" s="56">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="126" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="53">
+        <v>2050</v>
+      </c>
+      <c r="B126" s="53" t="s">
+        <v>438</v>
+      </c>
+      <c r="C126" s="53" t="s">
+        <v>338</v>
+      </c>
+      <c r="D126" s="53" t="s">
+        <v>339</v>
+      </c>
+      <c r="F126" s="53" t="s">
+        <v>447</v>
+      </c>
+      <c r="G126" s="53" t="s">
+        <v>428</v>
+      </c>
+      <c r="H126" s="52" t="s">
+        <v>427</v>
+      </c>
+      <c r="J126" s="53" t="s">
+        <v>402</v>
+      </c>
+      <c r="K126" s="53" t="s">
+        <v>404</v>
+      </c>
+      <c r="L126" s="52" t="s">
+        <v>88</v>
+      </c>
+      <c r="M126" s="53" t="s">
+        <v>439</v>
+      </c>
+      <c r="N126" s="53">
+        <v>19.13</v>
+      </c>
+      <c r="O126" s="67" t="s">
+        <v>109</v>
+      </c>
+      <c r="P126" s="67" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q126" s="53">
+        <v>0.87</v>
+      </c>
+      <c r="R126" s="53">
+        <v>0.78</v>
+      </c>
+      <c r="S126" s="56">
+        <v>83.3</v>
+      </c>
+      <c r="T126" s="56">
+        <v>0</v>
+      </c>
+      <c r="U126" s="56">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="127" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A127" s="53">
+        <v>2050</v>
+      </c>
+      <c r="B127" s="53" t="s">
+        <v>456</v>
+      </c>
+      <c r="C127" s="53" t="s">
+        <v>338</v>
+      </c>
+      <c r="D127" s="53" t="s">
+        <v>339</v>
+      </c>
+      <c r="F127" s="53" t="s">
+        <v>452</v>
+      </c>
+      <c r="G127" s="53" t="s">
+        <v>453</v>
+      </c>
+      <c r="H127" s="52" t="s">
+        <v>454</v>
+      </c>
+      <c r="I127" s="75" t="s">
+        <v>11</v>
+      </c>
+      <c r="K127" s="53" t="s">
+        <v>404</v>
+      </c>
+      <c r="L127" s="52" t="s">
+        <v>42</v>
+      </c>
+      <c r="M127" s="53" t="s">
+        <v>457</v>
+      </c>
+      <c r="N127" s="53">
+        <v>19.13</v>
+      </c>
+      <c r="O127" s="67" t="s">
+        <v>109</v>
+      </c>
+      <c r="P127" s="67" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q127" s="53">
+        <v>0.87</v>
+      </c>
+      <c r="R127" s="53">
+        <v>0.78</v>
+      </c>
+      <c r="S127" s="56">
+        <v>83.3</v>
+      </c>
+      <c r="T127" s="56">
+        <v>0</v>
+      </c>
+      <c r="U127" s="56">
+        <v>72</v>
+      </c>
+      <c r="V127" s="53" t="s">
         <v>362</v>
-      </c>
-    </row>
-    <row r="125" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="68">
-        <v>2050</v>
-      </c>
-      <c r="B125" s="68" t="s">
-        <v>352</v>
-      </c>
-      <c r="C125" s="68" t="s">
-        <v>338</v>
-      </c>
-      <c r="D125" s="68" t="s">
-        <v>339</v>
-      </c>
-      <c r="F125" s="68" t="s">
-        <v>354</v>
-      </c>
-      <c r="G125" s="68" t="s">
-        <v>347</v>
-      </c>
-      <c r="H125" s="69" t="s">
-        <v>348</v>
-      </c>
-      <c r="K125" s="68" t="s">
-        <v>355</v>
-      </c>
-      <c r="L125" s="69" t="s">
-        <v>44</v>
-      </c>
-      <c r="M125" s="68" t="s">
-        <v>357</v>
-      </c>
-      <c r="N125" s="68">
-        <v>19.13</v>
-      </c>
-      <c r="O125" s="70" t="s">
-        <v>109</v>
-      </c>
-      <c r="P125" s="70" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q125" s="68">
-        <v>0.87</v>
-      </c>
-      <c r="R125" s="68">
-        <v>0.78</v>
-      </c>
-      <c r="S125" s="71">
-        <v>83.3</v>
-      </c>
-      <c r="T125" s="71">
-        <v>0</v>
-      </c>
-      <c r="U125" s="71">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="126" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="68">
-        <v>2050</v>
-      </c>
-      <c r="B126" s="68" t="s">
-        <v>382</v>
-      </c>
-      <c r="C126" s="68" t="s">
-        <v>338</v>
-      </c>
-      <c r="D126" s="68" t="s">
-        <v>339</v>
-      </c>
-      <c r="F126" s="68" t="s">
-        <v>354</v>
-      </c>
-      <c r="G126" s="68" t="s">
-        <v>347</v>
-      </c>
-      <c r="H126" s="69" t="s">
-        <v>348</v>
-      </c>
-      <c r="K126" s="68" t="s">
-        <v>355</v>
-      </c>
-      <c r="L126" s="69" t="s">
-        <v>44</v>
-      </c>
-      <c r="M126" s="68" t="s">
-        <v>357</v>
-      </c>
-      <c r="N126" s="68">
-        <v>18.420000000000002</v>
-      </c>
-      <c r="O126" s="70" t="s">
-        <v>109</v>
-      </c>
-      <c r="P126" s="70" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q126" s="68">
-        <v>0.87</v>
-      </c>
-      <c r="R126" s="68">
-        <v>0.78</v>
-      </c>
-      <c r="S126" s="71">
-        <v>83.3</v>
-      </c>
-      <c r="T126" s="71">
-        <v>0</v>
-      </c>
-      <c r="U126" s="71">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="127" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="68">
-        <v>2050</v>
-      </c>
-      <c r="B127" s="68" t="s">
-        <v>389</v>
-      </c>
-      <c r="C127" s="68" t="s">
-        <v>338</v>
-      </c>
-      <c r="D127" s="68" t="s">
-        <v>339</v>
-      </c>
-      <c r="F127" s="68" t="s">
-        <v>386</v>
-      </c>
-      <c r="G127" s="68" t="s">
-        <v>391</v>
-      </c>
-      <c r="H127" s="69" t="s">
-        <v>393</v>
-      </c>
-      <c r="K127" s="68" t="s">
-        <v>395</v>
-      </c>
-      <c r="L127" s="69" t="s">
-        <v>44</v>
-      </c>
-      <c r="M127" s="68" t="s">
-        <v>398</v>
-      </c>
-      <c r="N127" s="68">
-        <v>18.420000000000002</v>
-      </c>
-      <c r="O127" s="70" t="s">
-        <v>109</v>
-      </c>
-      <c r="P127" s="70" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q127" s="68">
-        <v>0.87</v>
-      </c>
-      <c r="R127" s="68">
-        <v>0.78</v>
-      </c>
-      <c r="S127" s="71">
-        <v>83.3</v>
-      </c>
-      <c r="T127" s="71">
-        <v>0</v>
-      </c>
-      <c r="U127" s="71">
-        <v>72</v>
       </c>
     </row>
     <row r="128" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
@@ -9055,7 +9100,7 @@
         <v>2050</v>
       </c>
       <c r="B128" s="68" t="s">
-        <v>415</v>
+        <v>352</v>
       </c>
       <c r="C128" s="68" t="s">
         <v>338</v>
@@ -9064,28 +9109,25 @@
         <v>339</v>
       </c>
       <c r="F128" s="68" t="s">
-        <v>386</v>
+        <v>354</v>
       </c>
       <c r="G128" s="68" t="s">
-        <v>410</v>
+        <v>347</v>
       </c>
       <c r="H128" s="69" t="s">
-        <v>411</v>
-      </c>
-      <c r="J128" s="68" t="s">
-        <v>402</v>
+        <v>348</v>
       </c>
       <c r="K128" s="68" t="s">
-        <v>416</v>
+        <v>355</v>
       </c>
       <c r="L128" s="69" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M128" s="68" t="s">
-        <v>417</v>
+        <v>357</v>
       </c>
       <c r="N128" s="68">
-        <v>18.420000000000002</v>
+        <v>19.13</v>
       </c>
       <c r="O128" s="70" t="s">
         <v>109</v>
@@ -9114,7 +9156,7 @@
         <v>2050</v>
       </c>
       <c r="B129" s="68" t="s">
-        <v>432</v>
+        <v>382</v>
       </c>
       <c r="C129" s="68" t="s">
         <v>338</v>
@@ -9123,25 +9165,22 @@
         <v>339</v>
       </c>
       <c r="F129" s="68" t="s">
-        <v>426</v>
+        <v>354</v>
       </c>
       <c r="G129" s="68" t="s">
-        <v>428</v>
+        <v>347</v>
       </c>
       <c r="H129" s="69" t="s">
-        <v>427</v>
-      </c>
-      <c r="J129" s="68" t="s">
-        <v>402</v>
+        <v>348</v>
       </c>
       <c r="K129" s="68" t="s">
-        <v>416</v>
+        <v>355</v>
       </c>
       <c r="L129" s="69" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M129" s="68" t="s">
-        <v>433</v>
+        <v>357</v>
       </c>
       <c r="N129" s="68">
         <v>18.420000000000002</v>
@@ -9173,7 +9212,7 @@
         <v>2050</v>
       </c>
       <c r="B130" s="68" t="s">
-        <v>448</v>
+        <v>389</v>
       </c>
       <c r="C130" s="68" t="s">
         <v>338</v>
@@ -9182,25 +9221,22 @@
         <v>339</v>
       </c>
       <c r="F130" s="68" t="s">
-        <v>446</v>
+        <v>386</v>
       </c>
       <c r="G130" s="68" t="s">
-        <v>445</v>
+        <v>391</v>
       </c>
       <c r="H130" s="69" t="s">
-        <v>444</v>
-      </c>
-      <c r="J130" s="68" t="s">
-        <v>402</v>
+        <v>393</v>
       </c>
       <c r="K130" s="68" t="s">
-        <v>416</v>
+        <v>395</v>
       </c>
       <c r="L130" s="69" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M130" s="68" t="s">
-        <v>450</v>
+        <v>398</v>
       </c>
       <c r="N130" s="68">
         <v>18.420000000000002</v>
@@ -9232,7 +9268,7 @@
         <v>2050</v>
       </c>
       <c r="B131" s="68" t="s">
-        <v>449</v>
+        <v>415</v>
       </c>
       <c r="C131" s="68" t="s">
         <v>338</v>
@@ -9241,16 +9277,13 @@
         <v>339</v>
       </c>
       <c r="F131" s="68" t="s">
-        <v>447</v>
+        <v>386</v>
       </c>
       <c r="G131" s="68" t="s">
-        <v>445</v>
+        <v>410</v>
       </c>
       <c r="H131" s="69" t="s">
-        <v>444</v>
-      </c>
-      <c r="I131" s="75" t="s">
-        <v>11</v>
+        <v>411</v>
       </c>
       <c r="J131" s="68" t="s">
         <v>402</v>
@@ -9262,10 +9295,10 @@
         <v>42</v>
       </c>
       <c r="M131" s="68" t="s">
-        <v>440</v>
+        <v>417</v>
       </c>
       <c r="N131" s="68">
-        <v>19.57</v>
+        <v>18.420000000000002</v>
       </c>
       <c r="O131" s="70" t="s">
         <v>109</v>
@@ -9288,7 +9321,246 @@
       <c r="U131" s="71">
         <v>72</v>
       </c>
-      <c r="V131" s="68" t="s">
+    </row>
+    <row r="132" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A132" s="68">
+        <v>2050</v>
+      </c>
+      <c r="B132" s="68" t="s">
+        <v>432</v>
+      </c>
+      <c r="C132" s="68" t="s">
+        <v>338</v>
+      </c>
+      <c r="D132" s="68" t="s">
+        <v>339</v>
+      </c>
+      <c r="F132" s="68" t="s">
+        <v>426</v>
+      </c>
+      <c r="G132" s="68" t="s">
+        <v>428</v>
+      </c>
+      <c r="H132" s="69" t="s">
+        <v>427</v>
+      </c>
+      <c r="J132" s="68" t="s">
+        <v>402</v>
+      </c>
+      <c r="K132" s="68" t="s">
+        <v>416</v>
+      </c>
+      <c r="L132" s="69" t="s">
+        <v>42</v>
+      </c>
+      <c r="M132" s="68" t="s">
+        <v>433</v>
+      </c>
+      <c r="N132" s="68">
+        <v>18.420000000000002</v>
+      </c>
+      <c r="O132" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="P132" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q132" s="68">
+        <v>0.87</v>
+      </c>
+      <c r="R132" s="68">
+        <v>0.78</v>
+      </c>
+      <c r="S132" s="71">
+        <v>83.3</v>
+      </c>
+      <c r="T132" s="71">
+        <v>0</v>
+      </c>
+      <c r="U132" s="71">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="133" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A133" s="68">
+        <v>2050</v>
+      </c>
+      <c r="B133" s="68" t="s">
+        <v>448</v>
+      </c>
+      <c r="C133" s="68" t="s">
+        <v>338</v>
+      </c>
+      <c r="D133" s="68" t="s">
+        <v>339</v>
+      </c>
+      <c r="F133" s="68" t="s">
+        <v>446</v>
+      </c>
+      <c r="G133" s="68" t="s">
+        <v>445</v>
+      </c>
+      <c r="H133" s="69" t="s">
+        <v>444</v>
+      </c>
+      <c r="J133" s="68" t="s">
+        <v>402</v>
+      </c>
+      <c r="K133" s="68" t="s">
+        <v>416</v>
+      </c>
+      <c r="L133" s="69" t="s">
+        <v>42</v>
+      </c>
+      <c r="M133" s="68" t="s">
+        <v>450</v>
+      </c>
+      <c r="N133" s="68">
+        <v>18.420000000000002</v>
+      </c>
+      <c r="O133" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="P133" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q133" s="68">
+        <v>0.87</v>
+      </c>
+      <c r="R133" s="68">
+        <v>0.78</v>
+      </c>
+      <c r="S133" s="71">
+        <v>83.3</v>
+      </c>
+      <c r="T133" s="71">
+        <v>0</v>
+      </c>
+      <c r="U133" s="71">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="134" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A134" s="68">
+        <v>2050</v>
+      </c>
+      <c r="B134" s="68" t="s">
+        <v>449</v>
+      </c>
+      <c r="C134" s="68" t="s">
+        <v>338</v>
+      </c>
+      <c r="D134" s="68" t="s">
+        <v>339</v>
+      </c>
+      <c r="F134" s="68" t="s">
+        <v>447</v>
+      </c>
+      <c r="G134" s="68" t="s">
+        <v>445</v>
+      </c>
+      <c r="H134" s="69" t="s">
+        <v>444</v>
+      </c>
+      <c r="J134" s="68" t="s">
+        <v>402</v>
+      </c>
+      <c r="K134" s="68" t="s">
+        <v>416</v>
+      </c>
+      <c r="L134" s="69" t="s">
+        <v>42</v>
+      </c>
+      <c r="M134" s="68" t="s">
+        <v>440</v>
+      </c>
+      <c r="N134" s="68">
+        <v>19.57</v>
+      </c>
+      <c r="O134" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="P134" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q134" s="68">
+        <v>0.87</v>
+      </c>
+      <c r="R134" s="68">
+        <v>0.78</v>
+      </c>
+      <c r="S134" s="71">
+        <v>83.3</v>
+      </c>
+      <c r="T134" s="71">
+        <v>0</v>
+      </c>
+      <c r="U134" s="71">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="135" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A135" s="68">
+        <v>2050</v>
+      </c>
+      <c r="B135" s="68" t="s">
+        <v>463</v>
+      </c>
+      <c r="C135" s="68" t="s">
+        <v>338</v>
+      </c>
+      <c r="D135" s="68" t="s">
+        <v>339</v>
+      </c>
+      <c r="F135" s="68" t="s">
+        <v>464</v>
+      </c>
+      <c r="G135" s="68" t="s">
+        <v>460</v>
+      </c>
+      <c r="H135" s="69" t="s">
+        <v>461</v>
+      </c>
+      <c r="I135" s="75" t="s">
+        <v>11</v>
+      </c>
+      <c r="J135" s="68" t="s">
+        <v>402</v>
+      </c>
+      <c r="K135" s="68" t="s">
+        <v>416</v>
+      </c>
+      <c r="L135" s="69" t="s">
+        <v>110</v>
+      </c>
+      <c r="M135" s="68" t="s">
+        <v>465</v>
+      </c>
+      <c r="N135" s="68">
+        <v>19.57</v>
+      </c>
+      <c r="O135" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="P135" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q135" s="68">
+        <v>0.87</v>
+      </c>
+      <c r="R135" s="68">
+        <v>0.78</v>
+      </c>
+      <c r="S135" s="71">
+        <v>83.3</v>
+      </c>
+      <c r="T135" s="71">
+        <v>0</v>
+      </c>
+      <c r="U135" s="71">
+        <v>72</v>
+      </c>
+      <c r="V135" s="68" t="s">
         <v>358</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update off-model run tag
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936AC9A6-FA3B-4F59-A89E-9312BA79A9FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E49F68-CD89-4711-AFFE-FFDF9BEAF1E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3975" yWindow="2250" windowWidth="18300" windowHeight="9855" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
+    <workbookView xWindow="1176" yWindow="948" windowWidth="23040" windowHeight="14556" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelRuns" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1489" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1492" uniqueCount="466">
   <si>
     <t>year</t>
   </si>
@@ -2119,33 +2119,33 @@
   <dimension ref="A1:V135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C114" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C93" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A135" sqref="A135"/>
+      <selection pane="bottomRight" activeCell="J112" sqref="J112"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="7" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="42.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="42.33203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="23" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="6.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="22.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11.28515625" style="10" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="8.28515625" style="1" customWidth="1"/>
-    <col min="15" max="16" width="9.28515625" style="43"/>
-    <col min="17" max="16384" width="9.28515625" style="1"/>
+    <col min="8" max="8" width="8.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="6.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="22.33203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.33203125" style="10" customWidth="1"/>
+    <col min="13" max="13" width="17.5546875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="8.33203125" style="1" customWidth="1"/>
+    <col min="15" max="16" width="9.33203125" style="43"/>
+    <col min="17" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" s="5" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2213,7 +2213,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="2" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19">
         <v>2005</v>
       </c>
@@ -2266,7 +2266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="30">
         <v>2005</v>
       </c>
@@ -2322,7 +2322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30">
         <v>2005</v>
       </c>
@@ -2377,7 +2377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="30">
         <v>2005</v>
       </c>
@@ -2432,7 +2432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="30">
         <v>2005</v>
       </c>
@@ -2497,7 +2497,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="7" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="52">
         <v>2015</v>
       </c>
@@ -2538,7 +2538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="34">
         <v>2015</v>
       </c>
@@ -2584,7 +2584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="34">
         <v>2015</v>
       </c>
@@ -2637,7 +2637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="34">
         <v>2015</v>
       </c>
@@ -2690,7 +2690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="34">
         <v>2015</v>
       </c>
@@ -2743,7 +2743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="34">
         <v>2015</v>
       </c>
@@ -2799,7 +2799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="34">
         <v>2015</v>
       </c>
@@ -2855,7 +2855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="34">
         <v>2015</v>
       </c>
@@ -2911,7 +2911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="34">
         <v>2015</v>
       </c>
@@ -2971,7 +2971,7 @@
       </c>
       <c r="V15" s="57"/>
     </row>
-    <row r="16" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="34">
         <v>2015</v>
       </c>
@@ -3033,7 +3033,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>2023</v>
       </c>
@@ -3079,7 +3079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>2023</v>
       </c>
@@ -3125,7 +3125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>2023</v>
       </c>
@@ -3171,7 +3171,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>2023</v>
       </c>
@@ -3217,7 +3217,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>2023</v>
       </c>
@@ -3263,7 +3263,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>2023</v>
       </c>
@@ -3309,7 +3309,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>2023</v>
       </c>
@@ -3355,7 +3355,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>2023</v>
       </c>
@@ -3401,7 +3401,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>2023</v>
       </c>
@@ -3447,7 +3447,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>2023</v>
       </c>
@@ -3493,7 +3493,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>2023</v>
       </c>
@@ -3539,7 +3539,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>2023</v>
       </c>
@@ -3585,7 +3585,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>2023</v>
       </c>
@@ -3631,7 +3631,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>2023</v>
       </c>
@@ -3677,7 +3677,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>2023</v>
       </c>
@@ -3723,7 +3723,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>2023</v>
       </c>
@@ -3769,7 +3769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>2023</v>
       </c>
@@ -3815,7 +3815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>2023</v>
       </c>
@@ -3861,7 +3861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>2023</v>
       </c>
@@ -3905,7 +3905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>2023</v>
       </c>
@@ -3954,7 +3954,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>2023</v>
       </c>
@@ -4001,7 +4001,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>2023</v>
       </c>
@@ -4048,7 +4048,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>2023</v>
       </c>
@@ -4104,7 +4104,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>2023</v>
       </c>
@@ -4160,7 +4160,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>2023</v>
       </c>
@@ -4216,7 +4216,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>2023</v>
       </c>
@@ -4272,7 +4272,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>2023</v>
       </c>
@@ -4328,7 +4328,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>2023</v>
       </c>
@@ -4384,7 +4384,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>2023</v>
       </c>
@@ -4440,7 +4440,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>2023</v>
       </c>
@@ -4496,7 +4496,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>2023</v>
       </c>
@@ -4552,7 +4552,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>2023</v>
       </c>
@@ -4608,7 +4608,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>2023</v>
       </c>
@@ -4664,7 +4664,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>2023</v>
       </c>
@@ -4720,7 +4720,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>2023</v>
       </c>
@@ -4776,7 +4776,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>2023</v>
       </c>
@@ -4832,7 +4832,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>2023</v>
       </c>
@@ -4888,7 +4888,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>2023</v>
       </c>
@@ -4944,7 +4944,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>2023</v>
       </c>
@@ -5000,7 +5000,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>2023</v>
       </c>
@@ -5056,7 +5056,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>2023</v>
       </c>
@@ -5112,7 +5112,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>2023</v>
       </c>
@@ -5168,7 +5168,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>2023</v>
       </c>
@@ -5224,7 +5224,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>2023</v>
       </c>
@@ -5280,7 +5280,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>2023</v>
       </c>
@@ -5336,7 +5336,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>2023</v>
       </c>
@@ -5392,7 +5392,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>2023</v>
       </c>
@@ -5448,7 +5448,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>2023</v>
       </c>
@@ -5507,7 +5507,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>2023</v>
       </c>
@@ -5563,7 +5563,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>2023</v>
       </c>
@@ -5622,7 +5622,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>2023</v>
       </c>
@@ -5681,7 +5681,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>2023</v>
       </c>
@@ -5740,7 +5740,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>2023</v>
       </c>
@@ -5799,7 +5799,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="70" spans="1:22" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:22" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>2023</v>
       </c>
@@ -5855,7 +5855,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="71" spans="1:22" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:22" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>2023</v>
       </c>
@@ -5911,7 +5911,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>2023</v>
       </c>
@@ -5967,7 +5967,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>2023</v>
       </c>
@@ -6023,7 +6023,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>2023</v>
       </c>
@@ -6079,7 +6079,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>2023</v>
       </c>
@@ -6138,7 +6138,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>2023</v>
       </c>
@@ -6198,7 +6198,7 @@
       </c>
       <c r="V76" s="73"/>
     </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>2023</v>
       </c>
@@ -6260,7 +6260,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="78" spans="1:22" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:22" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="27">
         <v>2025</v>
       </c>
@@ -6288,7 +6288,7 @@
       <c r="T78" s="29"/>
       <c r="U78" s="29"/>
     </row>
-    <row r="79" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="15">
         <v>2035</v>
       </c>
@@ -6347,7 +6347,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="80" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="12">
         <v>2035</v>
       </c>
@@ -6403,7 +6403,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="81" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="12">
         <v>2035</v>
       </c>
@@ -6459,7 +6459,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="82" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="12">
         <v>2035</v>
       </c>
@@ -6515,7 +6515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="12">
         <v>2035</v>
       </c>
@@ -6571,7 +6571,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="84" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A84" s="12">
         <v>2035</v>
       </c>
@@ -6627,7 +6627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="12">
         <v>2035</v>
       </c>
@@ -6683,7 +6683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" s="12">
         <v>2035</v>
       </c>
@@ -6739,7 +6739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" s="12">
         <v>2035</v>
       </c>
@@ -6795,7 +6795,7 @@
         <v>41.25</v>
       </c>
     </row>
-    <row r="88" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="12">
         <v>2035</v>
       </c>
@@ -6851,7 +6851,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="89" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="12">
         <v>2035</v>
       </c>
@@ -6907,7 +6907,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="90" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90" s="12">
         <v>2035</v>
       </c>
@@ -6963,7 +6963,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="91" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" s="12">
         <v>2035</v>
       </c>
@@ -7019,7 +7019,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="92" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="12">
         <v>2035</v>
       </c>
@@ -7075,7 +7075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" s="12">
         <v>2035</v>
       </c>
@@ -7131,7 +7131,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="94" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" s="12">
         <v>2035</v>
       </c>
@@ -7187,7 +7187,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="95" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A95" s="12">
         <v>2035</v>
       </c>
@@ -7243,7 +7243,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="96" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A96" s="12">
         <v>2035</v>
       </c>
@@ -7299,7 +7299,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="97" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A97" s="12">
         <v>2035</v>
       </c>
@@ -7355,7 +7355,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="98" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" s="12">
         <v>2035</v>
       </c>
@@ -7411,7 +7411,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="99" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A99" s="12">
         <v>2035</v>
       </c>
@@ -7467,7 +7467,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="100" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A100" s="12">
         <v>2035</v>
       </c>
@@ -7523,7 +7523,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="101" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A101" s="12">
         <v>2035</v>
       </c>
@@ -7579,7 +7579,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="102" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A102" s="12">
         <v>2035</v>
       </c>
@@ -7641,7 +7641,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="103" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A103" s="12">
         <v>2035</v>
       </c>
@@ -7697,7 +7697,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="104" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A104" s="12">
         <v>2035</v>
       </c>
@@ -7759,7 +7759,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="105" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A105" s="58">
         <v>2035</v>
       </c>
@@ -7815,7 +7815,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="106" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A106" s="58">
         <v>2035</v>
       </c>
@@ -7871,7 +7871,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="107" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A107" s="58">
         <v>2035</v>
       </c>
@@ -7927,7 +7927,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="108" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A108" s="58">
         <v>2035</v>
       </c>
@@ -7986,7 +7986,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="109" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A109" s="58">
         <v>2035</v>
       </c>
@@ -8045,7 +8045,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="110" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A110" s="58">
         <v>2035</v>
       </c>
@@ -8104,7 +8104,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="111" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:22" s="58" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A111" s="58">
         <v>2035</v>
       </c>
@@ -8129,6 +8129,9 @@
       <c r="I111" s="76" t="s">
         <v>11</v>
       </c>
+      <c r="J111" s="58" t="s">
+        <v>402</v>
+      </c>
       <c r="K111" s="58" t="s">
         <v>404</v>
       </c>
@@ -8166,7 +8169,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="112" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A112" s="62">
         <v>2035</v>
       </c>
@@ -8222,7 +8225,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="113" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A113" s="62">
         <v>2035</v>
       </c>
@@ -8278,7 +8281,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="114" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A114" s="62">
         <v>2035</v>
       </c>
@@ -8334,7 +8337,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="115" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A115" s="62">
         <v>2035</v>
       </c>
@@ -8393,7 +8396,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="116" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A116" s="62">
         <v>2035</v>
       </c>
@@ -8452,7 +8455,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="117" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A117" s="62">
         <v>2035</v>
       </c>
@@ -8511,7 +8514,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="118" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A118" s="62">
         <v>2035</v>
       </c>
@@ -8570,7 +8573,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="119" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:22" s="62" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A119" s="62">
         <v>2035</v>
       </c>
@@ -8595,6 +8598,9 @@
       <c r="I119" s="76" t="s">
         <v>11</v>
       </c>
+      <c r="J119" s="62" t="s">
+        <v>402</v>
+      </c>
       <c r="K119" s="62" t="s">
         <v>412</v>
       </c>
@@ -8632,7 +8638,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="120" spans="1:22" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:22" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A120" s="24">
         <v>2050</v>
       </c>
@@ -8688,7 +8694,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="121" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A121" s="53">
         <v>2050</v>
       </c>
@@ -8744,7 +8750,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="122" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A122" s="53">
         <v>2050</v>
       </c>
@@ -8800,7 +8806,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="123" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A123" s="53">
         <v>2050</v>
       </c>
@@ -8856,7 +8862,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="124" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A124" s="53">
         <v>2050</v>
       </c>
@@ -8915,7 +8921,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="125" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A125" s="53">
         <v>2050</v>
       </c>
@@ -8974,7 +8980,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="126" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A126" s="53">
         <v>2050</v>
       </c>
@@ -9033,7 +9039,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="127" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A127" s="53">
         <v>2050</v>
       </c>
@@ -9058,6 +9064,9 @@
       <c r="I127" s="75" t="s">
         <v>11</v>
       </c>
+      <c r="J127" s="53" t="s">
+        <v>402</v>
+      </c>
       <c r="K127" s="53" t="s">
         <v>404</v>
       </c>
@@ -9095,7 +9104,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="128" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A128" s="68">
         <v>2050</v>
       </c>
@@ -9151,7 +9160,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="129" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A129" s="68">
         <v>2050</v>
       </c>
@@ -9207,7 +9216,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="130" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A130" s="68">
         <v>2050</v>
       </c>
@@ -9263,7 +9272,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="131" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A131" s="68">
         <v>2050</v>
       </c>
@@ -9322,7 +9331,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="132" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A132" s="68">
         <v>2050</v>
       </c>
@@ -9381,7 +9390,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="133" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A133" s="68">
         <v>2050</v>
       </c>
@@ -9440,7 +9449,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="134" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A134" s="68">
         <v>2050</v>
       </c>
@@ -9499,7 +9508,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="135" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:22" s="68" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A135" s="68">
         <v>2050</v>
       </c>

</xml_diff>

<commit_message>
Fix typo in an older run's AOC and update current tags for 2005, 2015 runs to single run
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41D5EF8-F3BC-4663-8980-5DB8F70DAA81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EEC1FB1-FBC4-49A6-8E91-0A533B6FC73D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="17010" windowHeight="9855" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="28800" windowHeight="11385" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelRuns" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1549" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1546" uniqueCount="480">
   <si>
     <t>year</t>
   </si>
@@ -2233,10 +2233,10 @@
   <dimension ref="A1:V139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C109" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C113" sqref="C113"/>
+      <selection pane="bottomRight" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2458,9 +2458,6 @@
       <c r="H4" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="29" t="s">
-        <v>11</v>
-      </c>
       <c r="K4" s="29" t="s">
         <v>224</v>
       </c>
@@ -2513,9 +2510,6 @@
       <c r="H5" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="29" t="s">
-        <v>11</v>
-      </c>
       <c r="K5" s="29" t="s">
         <v>224</v>
       </c>
@@ -2568,7 +2562,7 @@
       <c r="H6" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="29" t="s">
+      <c r="I6" s="73" t="s">
         <v>11</v>
       </c>
       <c r="J6" s="29" t="s">
@@ -3047,9 +3041,6 @@
       <c r="H15" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="I15" s="33" t="s">
-        <v>11</v>
-      </c>
       <c r="K15" s="33" t="s">
         <v>146</v>
       </c>
@@ -3107,7 +3098,7 @@
       <c r="H16" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="I16" s="33" t="s">
+      <c r="I16" s="73" t="s">
         <v>11</v>
       </c>
       <c r="K16" s="33" t="s">
@@ -3120,7 +3111,7 @@
         <v>368</v>
       </c>
       <c r="N16" s="33">
-        <v>15.28</v>
+        <v>14.73</v>
       </c>
       <c r="O16" s="39" t="s">
         <v>109</v>

</xml_diff>

<commit_message>
Added [2035,2050]_DBP_Plan_v08b and [2035,2050]_DBP_Trend_v07b
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EEC1FB1-FBC4-49A6-8E91-0A533B6FC73D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB8B2512-AE2E-498E-B8FB-F453364F88D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="28800" windowHeight="11385" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
+    <workbookView xWindow="2190" yWindow="780" windowWidth="19335" windowHeight="11685" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelRuns" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1546" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1596" uniqueCount="495">
   <si>
     <t>year</t>
   </si>
@@ -1494,6 +1494,51 @@
   </si>
   <si>
     <t>2050 Trend</t>
+  </si>
+  <si>
+    <t>2035_TM160_DBP_Trend_07b</t>
+  </si>
+  <si>
+    <t>DBP Land Use BAUSv8</t>
+  </si>
+  <si>
+    <t>M:\urban_modeling\baus\PBA50Plus\PBA50Plus_DraftBlueprint\PBA50Plus_Draft_Blueprint_v8_znupd_nodevfix</t>
+  </si>
+  <si>
+    <t>PBA50Plus_Draft_Blueprint_v8_znupd_nodevfix</t>
+  </si>
+  <si>
+    <t>2035_TM160_DBP_Plan_08b</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1182463234225195/1207227541117519/f</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1182463234225195/1207227169631490/f</t>
+  </si>
+  <si>
+    <t>2050_TM160_DBP_Trend_07b</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1182463234225195/1207227541117524/f</t>
+  </si>
+  <si>
+    <t>2050 Trend Previous</t>
+  </si>
+  <si>
+    <t>2035 Plan Previous</t>
+  </si>
+  <si>
+    <t>2035 Trend Previous</t>
+  </si>
+  <si>
+    <t>2050 Plan Previous</t>
+  </si>
+  <si>
+    <t>2050_TM160_DBP_Plan_08b</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1182463234225195/1207227169631494/f</t>
   </si>
 </sst>
 </file>
@@ -2230,13 +2275,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9564CC59-3725-4FDA-8BF2-0F68CB1B6F5A}">
-  <dimension ref="A1:V139"/>
+  <dimension ref="A1:V143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C114" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I10" sqref="I10"/>
+      <selection pane="bottomRight" activeCell="M143" sqref="M143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2245,7 +2290,7 @@
     <col min="2" max="2" width="31.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="7" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="42.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="23" style="1" customWidth="1"/>
     <col min="8" max="8" width="8.28515625" style="1" customWidth="1"/>
@@ -8355,9 +8400,6 @@
       <c r="H113" s="83" t="s">
         <v>461</v>
       </c>
-      <c r="I113" s="74" t="s">
-        <v>11</v>
-      </c>
       <c r="K113" s="83" t="s">
         <v>404</v>
       </c>
@@ -8392,63 +8434,69 @@
         <v>72</v>
       </c>
       <c r="V113" s="83" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="114" spans="1:22" s="83" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="83">
+        <v>2035</v>
+      </c>
+      <c r="B114" s="83" t="s">
+        <v>480</v>
+      </c>
+      <c r="C114" s="83" t="s">
+        <v>338</v>
+      </c>
+      <c r="D114" s="83" t="s">
+        <v>339</v>
+      </c>
+      <c r="F114" s="83" t="s">
+        <v>481</v>
+      </c>
+      <c r="G114" s="83" t="s">
+        <v>482</v>
+      </c>
+      <c r="H114" s="83" t="s">
+        <v>483</v>
+      </c>
+      <c r="I114" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="K114" s="83" t="s">
+        <v>404</v>
+      </c>
+      <c r="L114" s="84" t="s">
+        <v>43</v>
+      </c>
+      <c r="M114" s="85" t="s">
+        <v>485</v>
+      </c>
+      <c r="N114" s="83">
+        <v>17.579999999999998</v>
+      </c>
+      <c r="O114" s="86" t="s">
+        <v>109</v>
+      </c>
+      <c r="P114" s="86" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q114" s="83">
+        <v>0.87</v>
+      </c>
+      <c r="R114" s="83">
+        <v>0.78</v>
+      </c>
+      <c r="S114" s="87">
+        <v>83.3</v>
+      </c>
+      <c r="T114" s="87">
+        <v>0</v>
+      </c>
+      <c r="U114" s="87">
+        <v>72</v>
+      </c>
+      <c r="V114" s="83" t="s">
         <v>476</v>
-      </c>
-    </row>
-    <row r="114" spans="1:22" s="60" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="60">
-        <v>2035</v>
-      </c>
-      <c r="B114" s="60" t="s">
-        <v>345</v>
-      </c>
-      <c r="C114" s="61" t="s">
-        <v>338</v>
-      </c>
-      <c r="D114" s="60" t="s">
-        <v>339</v>
-      </c>
-      <c r="F114" s="60" t="s">
-        <v>346</v>
-      </c>
-      <c r="G114" s="60" t="s">
-        <v>347</v>
-      </c>
-      <c r="H114" s="60" t="s">
-        <v>348</v>
-      </c>
-      <c r="K114" s="60" t="s">
-        <v>349</v>
-      </c>
-      <c r="L114" s="62" t="s">
-        <v>129</v>
-      </c>
-      <c r="M114" s="61" t="s">
-        <v>350</v>
-      </c>
-      <c r="N114" s="60">
-        <v>17.579999999999998</v>
-      </c>
-      <c r="O114" s="63" t="s">
-        <v>109</v>
-      </c>
-      <c r="P114" s="63" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q114" s="60">
-        <v>0.87</v>
-      </c>
-      <c r="R114" s="60">
-        <v>0.78</v>
-      </c>
-      <c r="S114" s="64">
-        <v>83.3</v>
-      </c>
-      <c r="T114" s="64">
-        <v>0</v>
-      </c>
-      <c r="U114" s="64">
-        <v>72</v>
       </c>
     </row>
     <row r="115" spans="1:22" s="60" customFormat="1" x14ac:dyDescent="0.2">
@@ -8456,7 +8504,7 @@
         <v>2035</v>
       </c>
       <c r="B115" s="60" t="s">
-        <v>378</v>
+        <v>345</v>
       </c>
       <c r="C115" s="61" t="s">
         <v>338</v>
@@ -8465,7 +8513,7 @@
         <v>339</v>
       </c>
       <c r="F115" s="60" t="s">
-        <v>376</v>
+        <v>346</v>
       </c>
       <c r="G115" s="60" t="s">
         <v>347</v>
@@ -8480,10 +8528,10 @@
         <v>129</v>
       </c>
       <c r="M115" s="61" t="s">
-        <v>379</v>
+        <v>350</v>
       </c>
       <c r="N115" s="60">
-        <v>16.82</v>
+        <v>17.579999999999998</v>
       </c>
       <c r="O115" s="63" t="s">
         <v>109</v>
@@ -8512,7 +8560,7 @@
         <v>2035</v>
       </c>
       <c r="B116" s="60" t="s">
-        <v>390</v>
+        <v>378</v>
       </c>
       <c r="C116" s="61" t="s">
         <v>338</v>
@@ -8521,22 +8569,22 @@
         <v>339</v>
       </c>
       <c r="F116" s="60" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="G116" s="60" t="s">
-        <v>391</v>
+        <v>347</v>
       </c>
       <c r="H116" s="60" t="s">
-        <v>393</v>
+        <v>348</v>
       </c>
       <c r="K116" s="60" t="s">
-        <v>396</v>
+        <v>349</v>
       </c>
       <c r="L116" s="62" t="s">
         <v>129</v>
       </c>
       <c r="M116" s="61" t="s">
-        <v>397</v>
+        <v>379</v>
       </c>
       <c r="N116" s="60">
         <v>16.82</v>
@@ -8568,7 +8616,7 @@
         <v>2035</v>
       </c>
       <c r="B117" s="60" t="s">
-        <v>408</v>
+        <v>390</v>
       </c>
       <c r="C117" s="61" t="s">
         <v>338</v>
@@ -8577,25 +8625,22 @@
         <v>339</v>
       </c>
       <c r="F117" s="60" t="s">
-        <v>409</v>
+        <v>386</v>
       </c>
       <c r="G117" s="60" t="s">
-        <v>410</v>
+        <v>391</v>
       </c>
       <c r="H117" s="60" t="s">
-        <v>411</v>
-      </c>
-      <c r="J117" s="60" t="s">
-        <v>402</v>
+        <v>393</v>
       </c>
       <c r="K117" s="60" t="s">
-        <v>412</v>
+        <v>396</v>
       </c>
       <c r="L117" s="62" t="s">
-        <v>43</v>
+        <v>129</v>
       </c>
       <c r="M117" s="61" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="N117" s="60">
         <v>16.82</v>
@@ -8627,7 +8672,7 @@
         <v>2035</v>
       </c>
       <c r="B118" s="60" t="s">
-        <v>425</v>
+        <v>408</v>
       </c>
       <c r="C118" s="61" t="s">
         <v>338</v>
@@ -8636,13 +8681,13 @@
         <v>339</v>
       </c>
       <c r="F118" s="60" t="s">
-        <v>426</v>
+        <v>409</v>
       </c>
       <c r="G118" s="60" t="s">
-        <v>428</v>
+        <v>410</v>
       </c>
       <c r="H118" s="60" t="s">
-        <v>427</v>
+        <v>411</v>
       </c>
       <c r="J118" s="60" t="s">
         <v>402</v>
@@ -8654,7 +8699,7 @@
         <v>43</v>
       </c>
       <c r="M118" s="61" t="s">
-        <v>429</v>
+        <v>413</v>
       </c>
       <c r="N118" s="60">
         <v>16.82</v>
@@ -8686,7 +8731,7 @@
         <v>2035</v>
       </c>
       <c r="B119" s="60" t="s">
-        <v>441</v>
+        <v>425</v>
       </c>
       <c r="C119" s="61" t="s">
         <v>338</v>
@@ -8695,13 +8740,13 @@
         <v>339</v>
       </c>
       <c r="F119" s="60" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="G119" s="60" t="s">
-        <v>445</v>
+        <v>428</v>
       </c>
       <c r="H119" s="60" t="s">
-        <v>444</v>
+        <v>427</v>
       </c>
       <c r="J119" s="60" t="s">
         <v>402</v>
@@ -8713,7 +8758,7 @@
         <v>43</v>
       </c>
       <c r="M119" s="61" t="s">
-        <v>443</v>
+        <v>429</v>
       </c>
       <c r="N119" s="60">
         <v>16.82</v>
@@ -8745,7 +8790,7 @@
         <v>2035</v>
       </c>
       <c r="B120" s="60" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C120" s="61" t="s">
         <v>338</v>
@@ -8754,7 +8799,7 @@
         <v>339</v>
       </c>
       <c r="F120" s="60" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G120" s="60" t="s">
         <v>445</v>
@@ -8772,10 +8817,10 @@
         <v>43</v>
       </c>
       <c r="M120" s="61" t="s">
-        <v>437</v>
+        <v>443</v>
       </c>
       <c r="N120" s="60">
-        <v>18.03</v>
+        <v>16.82</v>
       </c>
       <c r="O120" s="63" t="s">
         <v>109</v>
@@ -8804,7 +8849,7 @@
         <v>2035</v>
       </c>
       <c r="B121" s="60" t="s">
-        <v>458</v>
+        <v>442</v>
       </c>
       <c r="C121" s="61" t="s">
         <v>338</v>
@@ -8813,16 +8858,13 @@
         <v>339</v>
       </c>
       <c r="F121" s="60" t="s">
-        <v>459</v>
+        <v>447</v>
       </c>
       <c r="G121" s="60" t="s">
-        <v>460</v>
+        <v>445</v>
       </c>
       <c r="H121" s="60" t="s">
-        <v>461</v>
-      </c>
-      <c r="I121" s="74" t="s">
-        <v>11</v>
+        <v>444</v>
       </c>
       <c r="J121" s="60" t="s">
         <v>402</v>
@@ -8831,10 +8873,10 @@
         <v>412</v>
       </c>
       <c r="L121" s="62" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="M121" s="61" t="s">
-        <v>462</v>
+        <v>437</v>
       </c>
       <c r="N121" s="60">
         <v>18.03</v>
@@ -8860,238 +8902,250 @@
       <c r="U121" s="64">
         <v>72</v>
       </c>
-      <c r="V121" s="60" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="122" spans="1:22" s="79" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="79">
-        <v>2050</v>
-      </c>
-      <c r="B122" s="79" t="s">
-        <v>471</v>
-      </c>
-      <c r="C122" s="79" t="s">
-        <v>113</v>
-      </c>
-      <c r="D122" s="79" t="s">
-        <v>244</v>
-      </c>
-      <c r="F122" s="79" t="s">
-        <v>467</v>
-      </c>
-      <c r="G122" s="79" t="s">
-        <v>468</v>
-      </c>
-      <c r="H122" s="80" t="s">
-        <v>469</v>
-      </c>
-      <c r="I122" s="74" t="s">
-        <v>11</v>
-      </c>
-      <c r="K122" s="79" t="s">
-        <v>472</v>
-      </c>
-      <c r="L122" s="80" t="s">
-        <v>110</v>
-      </c>
-      <c r="M122" s="79" t="s">
-        <v>109</v>
-      </c>
-      <c r="N122" s="79">
-        <v>17.440000000000001</v>
-      </c>
-      <c r="O122" s="81">
-        <v>-0.33</v>
-      </c>
-      <c r="P122" s="81">
-        <v>0</v>
-      </c>
-      <c r="Q122" s="81" t="s">
-        <v>109</v>
-      </c>
-      <c r="R122" s="81" t="s">
-        <v>109</v>
-      </c>
-      <c r="S122" s="82" t="s">
-        <v>109</v>
-      </c>
-      <c r="T122" s="82" t="s">
-        <v>109</v>
-      </c>
-      <c r="U122" s="82" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="123" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="23">
-        <v>2050</v>
-      </c>
-      <c r="B123" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="C123" s="23" t="s">
-        <v>113</v>
-      </c>
-      <c r="D123" s="23" t="s">
-        <v>244</v>
-      </c>
-      <c r="F123" s="23" t="s">
-        <v>114</v>
-      </c>
-      <c r="G123" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="H123" s="24" t="s">
-        <v>116</v>
+    </row>
+    <row r="122" spans="1:22" s="60" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="60">
+        <v>2035</v>
+      </c>
+      <c r="B122" s="60" t="s">
+        <v>458</v>
+      </c>
+      <c r="C122" s="61" t="s">
+        <v>338</v>
+      </c>
+      <c r="D122" s="60" t="s">
+        <v>339</v>
+      </c>
+      <c r="F122" s="60" t="s">
+        <v>459</v>
+      </c>
+      <c r="G122" s="60" t="s">
+        <v>460</v>
+      </c>
+      <c r="H122" s="60" t="s">
+        <v>461</v>
+      </c>
+      <c r="J122" s="60" t="s">
+        <v>402</v>
+      </c>
+      <c r="K122" s="60" t="s">
+        <v>412</v>
+      </c>
+      <c r="L122" s="62" t="s">
+        <v>16</v>
+      </c>
+      <c r="M122" s="61" t="s">
+        <v>462</v>
+      </c>
+      <c r="N122" s="60">
+        <v>18.03</v>
+      </c>
+      <c r="O122" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="P122" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q122" s="60">
+        <v>0.87</v>
+      </c>
+      <c r="R122" s="60">
+        <v>0.78</v>
+      </c>
+      <c r="S122" s="64">
+        <v>83.3</v>
+      </c>
+      <c r="T122" s="64">
+        <v>0</v>
+      </c>
+      <c r="U122" s="64">
+        <v>72</v>
+      </c>
+      <c r="V122" s="60" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="123" spans="1:22" s="60" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="60">
+        <v>2035</v>
+      </c>
+      <c r="B123" s="60" t="s">
+        <v>484</v>
+      </c>
+      <c r="C123" s="61" t="s">
+        <v>338</v>
+      </c>
+      <c r="D123" s="60" t="s">
+        <v>339</v>
+      </c>
+      <c r="F123" s="60" t="s">
+        <v>481</v>
+      </c>
+      <c r="G123" s="60" t="s">
+        <v>482</v>
+      </c>
+      <c r="H123" s="60" t="s">
+        <v>483</v>
       </c>
       <c r="I123" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="K123" s="23" t="s">
+      <c r="J123" s="60" t="s">
+        <v>402</v>
+      </c>
+      <c r="K123" s="60" t="s">
+        <v>412</v>
+      </c>
+      <c r="L123" s="62" t="s">
+        <v>16</v>
+      </c>
+      <c r="M123" s="61" t="s">
+        <v>486</v>
+      </c>
+      <c r="N123" s="60">
+        <v>18.03</v>
+      </c>
+      <c r="O123" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="P123" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q123" s="60">
+        <v>0.87</v>
+      </c>
+      <c r="R123" s="60">
+        <v>0.78</v>
+      </c>
+      <c r="S123" s="64">
+        <v>83.3</v>
+      </c>
+      <c r="T123" s="64">
+        <v>0</v>
+      </c>
+      <c r="U123" s="64">
+        <v>72</v>
+      </c>
+      <c r="V123" s="60" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="124" spans="1:22" s="79" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="79">
+        <v>2050</v>
+      </c>
+      <c r="B124" s="79" t="s">
+        <v>471</v>
+      </c>
+      <c r="C124" s="79" t="s">
+        <v>113</v>
+      </c>
+      <c r="D124" s="79" t="s">
+        <v>244</v>
+      </c>
+      <c r="F124" s="79" t="s">
+        <v>467</v>
+      </c>
+      <c r="G124" s="79" t="s">
+        <v>468</v>
+      </c>
+      <c r="H124" s="80" t="s">
+        <v>469</v>
+      </c>
+      <c r="I124" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="K124" s="79" t="s">
+        <v>472</v>
+      </c>
+      <c r="L124" s="80" t="s">
+        <v>110</v>
+      </c>
+      <c r="M124" s="79" t="s">
+        <v>109</v>
+      </c>
+      <c r="N124" s="79">
+        <v>17.440000000000001</v>
+      </c>
+      <c r="O124" s="81">
+        <v>-0.33</v>
+      </c>
+      <c r="P124" s="81">
+        <v>0</v>
+      </c>
+      <c r="Q124" s="81" t="s">
+        <v>109</v>
+      </c>
+      <c r="R124" s="81" t="s">
+        <v>109</v>
+      </c>
+      <c r="S124" s="82" t="s">
+        <v>109</v>
+      </c>
+      <c r="T124" s="82" t="s">
+        <v>109</v>
+      </c>
+      <c r="U124" s="82" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="125" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="23">
+        <v>2050</v>
+      </c>
+      <c r="B125" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="C125" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="D125" s="23" t="s">
+        <v>244</v>
+      </c>
+      <c r="F125" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="G125" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="H125" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="I125" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="K125" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="L123" s="24" t="s">
+      <c r="L125" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="M123" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="N123" s="23">
+      <c r="M125" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="N125" s="23">
         <v>17.440000000000001</v>
       </c>
-      <c r="O123" s="45">
+      <c r="O125" s="45">
         <v>-0.33</v>
       </c>
-      <c r="P123" s="45">
-        <v>0</v>
-      </c>
-      <c r="Q123" s="45" t="s">
-        <v>109</v>
-      </c>
-      <c r="R123" s="45" t="s">
-        <v>109</v>
-      </c>
-      <c r="S123" s="70" t="s">
-        <v>109</v>
-      </c>
-      <c r="T123" s="70" t="s">
-        <v>109</v>
-      </c>
-      <c r="U123" s="70" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="124" spans="1:22" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="51">
-        <v>2050</v>
-      </c>
-      <c r="B124" s="51" t="s">
-        <v>351</v>
-      </c>
-      <c r="C124" s="51" t="s">
-        <v>338</v>
-      </c>
-      <c r="D124" s="51" t="s">
-        <v>339</v>
-      </c>
-      <c r="F124" s="51" t="s">
-        <v>353</v>
-      </c>
-      <c r="G124" s="51" t="s">
-        <v>342</v>
-      </c>
-      <c r="H124" s="50" t="s">
-        <v>343</v>
-      </c>
-      <c r="K124" s="51" t="s">
-        <v>344</v>
-      </c>
-      <c r="L124" s="50" t="s">
-        <v>16</v>
-      </c>
-      <c r="M124" s="51" t="s">
-        <v>356</v>
-      </c>
-      <c r="N124" s="51">
-        <v>19.13</v>
-      </c>
-      <c r="O124" s="65" t="s">
-        <v>109</v>
-      </c>
-      <c r="P124" s="65" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q124" s="51">
-        <v>0.87</v>
-      </c>
-      <c r="R124" s="51">
-        <v>0.78</v>
-      </c>
-      <c r="S124" s="54">
-        <v>83.3</v>
-      </c>
-      <c r="T124" s="54">
-        <v>0</v>
-      </c>
-      <c r="U124" s="54">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="125" spans="1:22" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="51">
-        <v>2050</v>
-      </c>
-      <c r="B125" s="51" t="s">
-        <v>380</v>
-      </c>
-      <c r="C125" s="51" t="s">
-        <v>338</v>
-      </c>
-      <c r="D125" s="51" t="s">
-        <v>339</v>
-      </c>
-      <c r="F125" s="51" t="s">
-        <v>376</v>
-      </c>
-      <c r="G125" s="51" t="s">
-        <v>342</v>
-      </c>
-      <c r="H125" s="50" t="s">
-        <v>343</v>
-      </c>
-      <c r="K125" s="51" t="s">
-        <v>344</v>
-      </c>
-      <c r="L125" s="50" t="s">
-        <v>16</v>
-      </c>
-      <c r="M125" s="51" t="s">
-        <v>381</v>
-      </c>
-      <c r="N125" s="51">
-        <v>18.420000000000002</v>
-      </c>
-      <c r="O125" s="65" t="s">
-        <v>109</v>
-      </c>
-      <c r="P125" s="65" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q125" s="51">
-        <v>0.87</v>
-      </c>
-      <c r="R125" s="51">
-        <v>0.78</v>
-      </c>
-      <c r="S125" s="54">
-        <v>83.3</v>
-      </c>
-      <c r="T125" s="54">
-        <v>0</v>
-      </c>
-      <c r="U125" s="54">
-        <v>72</v>
+      <c r="P125" s="45">
+        <v>0</v>
+      </c>
+      <c r="Q125" s="45" t="s">
+        <v>109</v>
+      </c>
+      <c r="R125" s="45" t="s">
+        <v>109</v>
+      </c>
+      <c r="S125" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="T125" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="U125" s="70" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="126" spans="1:22" s="51" customFormat="1" x14ac:dyDescent="0.2">
@@ -9099,7 +9153,7 @@
         <v>2050</v>
       </c>
       <c r="B126" s="51" t="s">
-        <v>388</v>
+        <v>351</v>
       </c>
       <c r="C126" s="51" t="s">
         <v>338</v>
@@ -9108,25 +9162,25 @@
         <v>339</v>
       </c>
       <c r="F126" s="51" t="s">
-        <v>386</v>
+        <v>353</v>
       </c>
       <c r="G126" s="51" t="s">
-        <v>387</v>
+        <v>342</v>
       </c>
       <c r="H126" s="50" t="s">
-        <v>392</v>
+        <v>343</v>
       </c>
       <c r="K126" s="51" t="s">
-        <v>394</v>
+        <v>344</v>
       </c>
       <c r="L126" s="50" t="s">
         <v>16</v>
       </c>
       <c r="M126" s="51" t="s">
-        <v>400</v>
+        <v>356</v>
       </c>
       <c r="N126" s="51">
-        <v>18.420000000000002</v>
+        <v>19.13</v>
       </c>
       <c r="O126" s="65" t="s">
         <v>109</v>
@@ -9155,7 +9209,7 @@
         <v>2050</v>
       </c>
       <c r="B127" s="51" t="s">
-        <v>414</v>
+        <v>380</v>
       </c>
       <c r="C127" s="51" t="s">
         <v>338</v>
@@ -9164,25 +9218,22 @@
         <v>339</v>
       </c>
       <c r="F127" s="51" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="G127" s="51" t="s">
-        <v>407</v>
+        <v>342</v>
       </c>
       <c r="H127" s="50" t="s">
-        <v>406</v>
-      </c>
-      <c r="J127" s="51" t="s">
-        <v>402</v>
+        <v>343</v>
       </c>
       <c r="K127" s="51" t="s">
-        <v>404</v>
+        <v>344</v>
       </c>
       <c r="L127" s="50" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="M127" s="51" t="s">
-        <v>418</v>
+        <v>381</v>
       </c>
       <c r="N127" s="51">
         <v>18.420000000000002</v>
@@ -9214,7 +9265,7 @@
         <v>2050</v>
       </c>
       <c r="B128" s="51" t="s">
-        <v>430</v>
+        <v>388</v>
       </c>
       <c r="C128" s="51" t="s">
         <v>338</v>
@@ -9223,25 +9274,22 @@
         <v>339</v>
       </c>
       <c r="F128" s="51" t="s">
-        <v>426</v>
+        <v>386</v>
       </c>
       <c r="G128" s="51" t="s">
-        <v>428</v>
+        <v>387</v>
       </c>
       <c r="H128" s="50" t="s">
-        <v>427</v>
-      </c>
-      <c r="J128" s="51" t="s">
-        <v>402</v>
+        <v>392</v>
       </c>
       <c r="K128" s="51" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
       <c r="L128" s="50" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="M128" s="51" t="s">
-        <v>431</v>
+        <v>400</v>
       </c>
       <c r="N128" s="51">
         <v>18.420000000000002</v>
@@ -9273,7 +9321,7 @@
         <v>2050</v>
       </c>
       <c r="B129" s="51" t="s">
-        <v>438</v>
+        <v>414</v>
       </c>
       <c r="C129" s="51" t="s">
         <v>338</v>
@@ -9282,13 +9330,13 @@
         <v>339</v>
       </c>
       <c r="F129" s="51" t="s">
-        <v>447</v>
+        <v>386</v>
       </c>
       <c r="G129" s="51" t="s">
-        <v>428</v>
+        <v>407</v>
       </c>
       <c r="H129" s="50" t="s">
-        <v>427</v>
+        <v>406</v>
       </c>
       <c r="J129" s="51" t="s">
         <v>402</v>
@@ -9297,13 +9345,13 @@
         <v>404</v>
       </c>
       <c r="L129" s="50" t="s">
-        <v>88</v>
+        <v>42</v>
       </c>
       <c r="M129" s="51" t="s">
-        <v>439</v>
+        <v>418</v>
       </c>
       <c r="N129" s="51">
-        <v>19.13</v>
+        <v>18.420000000000002</v>
       </c>
       <c r="O129" s="65" t="s">
         <v>109</v>
@@ -9332,7 +9380,7 @@
         <v>2050</v>
       </c>
       <c r="B130" s="51" t="s">
-        <v>456</v>
+        <v>430</v>
       </c>
       <c r="C130" s="51" t="s">
         <v>338</v>
@@ -9341,16 +9389,13 @@
         <v>339</v>
       </c>
       <c r="F130" s="51" t="s">
-        <v>452</v>
+        <v>426</v>
       </c>
       <c r="G130" s="51" t="s">
-        <v>453</v>
+        <v>428</v>
       </c>
       <c r="H130" s="50" t="s">
-        <v>454</v>
-      </c>
-      <c r="I130" s="73" t="s">
-        <v>11</v>
+        <v>427</v>
       </c>
       <c r="J130" s="51" t="s">
         <v>402</v>
@@ -9362,10 +9407,10 @@
         <v>42</v>
       </c>
       <c r="M130" s="51" t="s">
-        <v>457</v>
+        <v>431</v>
       </c>
       <c r="N130" s="51">
-        <v>19.13</v>
+        <v>18.420000000000002</v>
       </c>
       <c r="O130" s="65" t="s">
         <v>109</v>
@@ -9388,240 +9433,255 @@
       <c r="U130" s="54">
         <v>72</v>
       </c>
-      <c r="V130" s="51" t="s">
+    </row>
+    <row r="131" spans="1:22" s="51" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A131" s="51">
+        <v>2050</v>
+      </c>
+      <c r="B131" s="51" t="s">
+        <v>438</v>
+      </c>
+      <c r="C131" s="51" t="s">
+        <v>338</v>
+      </c>
+      <c r="D131" s="51" t="s">
+        <v>339</v>
+      </c>
+      <c r="F131" s="51" t="s">
+        <v>447</v>
+      </c>
+      <c r="G131" s="51" t="s">
+        <v>428</v>
+      </c>
+      <c r="H131" s="50" t="s">
+        <v>427</v>
+      </c>
+      <c r="J131" s="51" t="s">
+        <v>402</v>
+      </c>
+      <c r="K131" s="51" t="s">
+        <v>404</v>
+      </c>
+      <c r="L131" s="50" t="s">
+        <v>88</v>
+      </c>
+      <c r="M131" s="51" t="s">
+        <v>439</v>
+      </c>
+      <c r="N131" s="51">
+        <v>19.13</v>
+      </c>
+      <c r="O131" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="P131" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q131" s="51">
+        <v>0.87</v>
+      </c>
+      <c r="R131" s="51">
+        <v>0.78</v>
+      </c>
+      <c r="S131" s="54">
+        <v>83.3</v>
+      </c>
+      <c r="T131" s="54">
+        <v>0</v>
+      </c>
+      <c r="U131" s="54">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="132" spans="1:22" s="51" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A132" s="51">
+        <v>2050</v>
+      </c>
+      <c r="B132" s="51" t="s">
+        <v>456</v>
+      </c>
+      <c r="C132" s="51" t="s">
+        <v>338</v>
+      </c>
+      <c r="D132" s="51" t="s">
+        <v>339</v>
+      </c>
+      <c r="F132" s="51" t="s">
+        <v>452</v>
+      </c>
+      <c r="G132" s="51" t="s">
+        <v>453</v>
+      </c>
+      <c r="H132" s="50" t="s">
+        <v>454</v>
+      </c>
+      <c r="I132" s="73" t="s">
+        <v>11</v>
+      </c>
+      <c r="J132" s="51" t="s">
+        <v>402</v>
+      </c>
+      <c r="K132" s="51" t="s">
+        <v>404</v>
+      </c>
+      <c r="L132" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="M132" s="51" t="s">
+        <v>457</v>
+      </c>
+      <c r="N132" s="51">
+        <v>19.13</v>
+      </c>
+      <c r="O132" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="P132" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q132" s="51">
+        <v>0.87</v>
+      </c>
+      <c r="R132" s="51">
+        <v>0.78</v>
+      </c>
+      <c r="S132" s="54">
+        <v>83.3</v>
+      </c>
+      <c r="T132" s="54">
+        <v>0</v>
+      </c>
+      <c r="U132" s="54">
+        <v>72</v>
+      </c>
+      <c r="V132" s="51" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="131" spans="1:22" s="88" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A131" s="89">
+    <row r="133" spans="1:22" s="88" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A133" s="89">
         <v>2050</v>
       </c>
-      <c r="B131" s="89" t="s">
+      <c r="B133" s="89" t="s">
         <v>477</v>
       </c>
-      <c r="C131" s="89" t="s">
+      <c r="C133" s="89" t="s">
         <v>338</v>
       </c>
-      <c r="D131" s="89" t="s">
+      <c r="D133" s="89" t="s">
         <v>339</v>
       </c>
-      <c r="E131" s="89"/>
-      <c r="F131" s="89" t="s">
+      <c r="E133" s="89"/>
+      <c r="F133" s="89" t="s">
         <v>474</v>
       </c>
-      <c r="G131" s="89" t="s">
+      <c r="G133" s="89" t="s">
         <v>460</v>
       </c>
-      <c r="H131" s="90" t="s">
+      <c r="H133" s="90" t="s">
         <v>461</v>
       </c>
-      <c r="I131" s="74" t="s">
+      <c r="I133" s="89"/>
+      <c r="J133" s="89"/>
+      <c r="K133" s="89" t="s">
+        <v>404</v>
+      </c>
+      <c r="L133" s="90" t="s">
+        <v>42</v>
+      </c>
+      <c r="M133" s="93" t="s">
+        <v>478</v>
+      </c>
+      <c r="N133" s="89">
+        <v>19.13</v>
+      </c>
+      <c r="O133" s="91" t="s">
+        <v>109</v>
+      </c>
+      <c r="P133" s="91" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q133" s="89">
+        <v>0.87</v>
+      </c>
+      <c r="R133" s="89">
+        <v>0.78</v>
+      </c>
+      <c r="S133" s="92">
+        <v>83.3</v>
+      </c>
+      <c r="T133" s="92">
+        <v>0</v>
+      </c>
+      <c r="U133" s="92">
+        <v>72</v>
+      </c>
+      <c r="V133" s="89" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="134" spans="1:22" s="88" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A134" s="89">
+        <v>2050</v>
+      </c>
+      <c r="B134" s="89" t="s">
+        <v>487</v>
+      </c>
+      <c r="C134" s="89" t="s">
+        <v>338</v>
+      </c>
+      <c r="D134" s="89" t="s">
+        <v>339</v>
+      </c>
+      <c r="E134" s="89"/>
+      <c r="F134" s="89" t="s">
+        <v>481</v>
+      </c>
+      <c r="G134" s="89" t="s">
+        <v>482</v>
+      </c>
+      <c r="H134" s="90" t="s">
+        <v>483</v>
+      </c>
+      <c r="I134" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="J131" s="89"/>
-      <c r="K131" s="89" t="s">
+      <c r="J134" s="89"/>
+      <c r="K134" s="89" t="s">
         <v>404</v>
       </c>
-      <c r="L131" s="90" t="s">
+      <c r="L134" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="M131" s="93" t="s">
-        <v>478</v>
-      </c>
-      <c r="N131" s="89">
+      <c r="M134" s="93" t="s">
+        <v>488</v>
+      </c>
+      <c r="N134" s="89">
         <v>19.13</v>
       </c>
-      <c r="O131" s="91" t="s">
-        <v>109</v>
-      </c>
-      <c r="P131" s="91" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q131" s="89">
+      <c r="O134" s="91" t="s">
+        <v>109</v>
+      </c>
+      <c r="P134" s="91" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q134" s="89">
         <v>0.87</v>
       </c>
-      <c r="R131" s="89">
+      <c r="R134" s="89">
         <v>0.78</v>
       </c>
-      <c r="S131" s="92">
+      <c r="S134" s="92">
         <v>83.3</v>
       </c>
-      <c r="T131" s="92">
-        <v>0</v>
-      </c>
-      <c r="U131" s="92">
+      <c r="T134" s="92">
+        <v>0</v>
+      </c>
+      <c r="U134" s="92">
         <v>72</v>
       </c>
-      <c r="V131" s="89" t="s">
+      <c r="V134" s="89" t="s">
         <v>479</v>
-      </c>
-    </row>
-    <row r="132" spans="1:22" s="66" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A132" s="66">
-        <v>2050</v>
-      </c>
-      <c r="B132" s="66" t="s">
-        <v>352</v>
-      </c>
-      <c r="C132" s="66" t="s">
-        <v>338</v>
-      </c>
-      <c r="D132" s="66" t="s">
-        <v>339</v>
-      </c>
-      <c r="F132" s="66" t="s">
-        <v>354</v>
-      </c>
-      <c r="G132" s="66" t="s">
-        <v>347</v>
-      </c>
-      <c r="H132" s="67" t="s">
-        <v>348</v>
-      </c>
-      <c r="K132" s="66" t="s">
-        <v>355</v>
-      </c>
-      <c r="L132" s="67" t="s">
-        <v>44</v>
-      </c>
-      <c r="M132" s="66" t="s">
-        <v>357</v>
-      </c>
-      <c r="N132" s="66">
-        <v>19.13</v>
-      </c>
-      <c r="O132" s="68" t="s">
-        <v>109</v>
-      </c>
-      <c r="P132" s="68" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q132" s="66">
-        <v>0.87</v>
-      </c>
-      <c r="R132" s="66">
-        <v>0.78</v>
-      </c>
-      <c r="S132" s="69">
-        <v>83.3</v>
-      </c>
-      <c r="T132" s="69">
-        <v>0</v>
-      </c>
-      <c r="U132" s="69">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="133" spans="1:22" s="66" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A133" s="66">
-        <v>2050</v>
-      </c>
-      <c r="B133" s="66" t="s">
-        <v>382</v>
-      </c>
-      <c r="C133" s="66" t="s">
-        <v>338</v>
-      </c>
-      <c r="D133" s="66" t="s">
-        <v>339</v>
-      </c>
-      <c r="F133" s="66" t="s">
-        <v>354</v>
-      </c>
-      <c r="G133" s="66" t="s">
-        <v>347</v>
-      </c>
-      <c r="H133" s="67" t="s">
-        <v>348</v>
-      </c>
-      <c r="K133" s="66" t="s">
-        <v>355</v>
-      </c>
-      <c r="L133" s="67" t="s">
-        <v>44</v>
-      </c>
-      <c r="M133" s="66" t="s">
-        <v>357</v>
-      </c>
-      <c r="N133" s="66">
-        <v>18.420000000000002</v>
-      </c>
-      <c r="O133" s="68" t="s">
-        <v>109</v>
-      </c>
-      <c r="P133" s="68" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q133" s="66">
-        <v>0.87</v>
-      </c>
-      <c r="R133" s="66">
-        <v>0.78</v>
-      </c>
-      <c r="S133" s="69">
-        <v>83.3</v>
-      </c>
-      <c r="T133" s="69">
-        <v>0</v>
-      </c>
-      <c r="U133" s="69">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="134" spans="1:22" s="66" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A134" s="66">
-        <v>2050</v>
-      </c>
-      <c r="B134" s="66" t="s">
-        <v>389</v>
-      </c>
-      <c r="C134" s="66" t="s">
-        <v>338</v>
-      </c>
-      <c r="D134" s="66" t="s">
-        <v>339</v>
-      </c>
-      <c r="F134" s="66" t="s">
-        <v>386</v>
-      </c>
-      <c r="G134" s="66" t="s">
-        <v>391</v>
-      </c>
-      <c r="H134" s="67" t="s">
-        <v>393</v>
-      </c>
-      <c r="K134" s="66" t="s">
-        <v>395</v>
-      </c>
-      <c r="L134" s="67" t="s">
-        <v>44</v>
-      </c>
-      <c r="M134" s="66" t="s">
-        <v>398</v>
-      </c>
-      <c r="N134" s="66">
-        <v>18.420000000000002</v>
-      </c>
-      <c r="O134" s="68" t="s">
-        <v>109</v>
-      </c>
-      <c r="P134" s="68" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q134" s="66">
-        <v>0.87</v>
-      </c>
-      <c r="R134" s="66">
-        <v>0.78</v>
-      </c>
-      <c r="S134" s="69">
-        <v>83.3</v>
-      </c>
-      <c r="T134" s="69">
-        <v>0</v>
-      </c>
-      <c r="U134" s="69">
-        <v>72</v>
       </c>
     </row>
     <row r="135" spans="1:22" s="66" customFormat="1" x14ac:dyDescent="0.2">
@@ -9629,7 +9689,7 @@
         <v>2050</v>
       </c>
       <c r="B135" s="66" t="s">
-        <v>415</v>
+        <v>352</v>
       </c>
       <c r="C135" s="66" t="s">
         <v>338</v>
@@ -9638,28 +9698,25 @@
         <v>339</v>
       </c>
       <c r="F135" s="66" t="s">
-        <v>386</v>
+        <v>354</v>
       </c>
       <c r="G135" s="66" t="s">
-        <v>410</v>
+        <v>347</v>
       </c>
       <c r="H135" s="67" t="s">
-        <v>411</v>
-      </c>
-      <c r="J135" s="66" t="s">
-        <v>402</v>
+        <v>348</v>
       </c>
       <c r="K135" s="66" t="s">
-        <v>416</v>
+        <v>355</v>
       </c>
       <c r="L135" s="67" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M135" s="66" t="s">
-        <v>417</v>
+        <v>357</v>
       </c>
       <c r="N135" s="66">
-        <v>18.420000000000002</v>
+        <v>19.13</v>
       </c>
       <c r="O135" s="68" t="s">
         <v>109</v>
@@ -9688,7 +9745,7 @@
         <v>2050</v>
       </c>
       <c r="B136" s="66" t="s">
-        <v>432</v>
+        <v>382</v>
       </c>
       <c r="C136" s="66" t="s">
         <v>338</v>
@@ -9697,25 +9754,22 @@
         <v>339</v>
       </c>
       <c r="F136" s="66" t="s">
-        <v>426</v>
+        <v>354</v>
       </c>
       <c r="G136" s="66" t="s">
-        <v>428</v>
+        <v>347</v>
       </c>
       <c r="H136" s="67" t="s">
-        <v>427</v>
-      </c>
-      <c r="J136" s="66" t="s">
-        <v>402</v>
+        <v>348</v>
       </c>
       <c r="K136" s="66" t="s">
-        <v>416</v>
+        <v>355</v>
       </c>
       <c r="L136" s="67" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M136" s="66" t="s">
-        <v>433</v>
+        <v>357</v>
       </c>
       <c r="N136" s="66">
         <v>18.420000000000002</v>
@@ -9747,7 +9801,7 @@
         <v>2050</v>
       </c>
       <c r="B137" s="66" t="s">
-        <v>448</v>
+        <v>389</v>
       </c>
       <c r="C137" s="66" t="s">
         <v>338</v>
@@ -9756,25 +9810,22 @@
         <v>339</v>
       </c>
       <c r="F137" s="66" t="s">
-        <v>446</v>
+        <v>386</v>
       </c>
       <c r="G137" s="66" t="s">
-        <v>445</v>
+        <v>391</v>
       </c>
       <c r="H137" s="67" t="s">
-        <v>444</v>
-      </c>
-      <c r="J137" s="66" t="s">
-        <v>402</v>
+        <v>393</v>
       </c>
       <c r="K137" s="66" t="s">
-        <v>416</v>
+        <v>395</v>
       </c>
       <c r="L137" s="67" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M137" s="66" t="s">
-        <v>450</v>
+        <v>398</v>
       </c>
       <c r="N137" s="66">
         <v>18.420000000000002</v>
@@ -9806,7 +9857,7 @@
         <v>2050</v>
       </c>
       <c r="B138" s="66" t="s">
-        <v>449</v>
+        <v>415</v>
       </c>
       <c r="C138" s="66" t="s">
         <v>338</v>
@@ -9815,13 +9866,13 @@
         <v>339</v>
       </c>
       <c r="F138" s="66" t="s">
-        <v>447</v>
+        <v>386</v>
       </c>
       <c r="G138" s="66" t="s">
-        <v>445</v>
+        <v>410</v>
       </c>
       <c r="H138" s="67" t="s">
-        <v>444</v>
+        <v>411</v>
       </c>
       <c r="J138" s="66" t="s">
         <v>402</v>
@@ -9833,10 +9884,10 @@
         <v>42</v>
       </c>
       <c r="M138" s="66" t="s">
-        <v>440</v>
+        <v>417</v>
       </c>
       <c r="N138" s="66">
-        <v>19.57</v>
+        <v>18.420000000000002</v>
       </c>
       <c r="O138" s="68" t="s">
         <v>109</v>
@@ -9865,7 +9916,7 @@
         <v>2050</v>
       </c>
       <c r="B139" s="66" t="s">
-        <v>463</v>
+        <v>432</v>
       </c>
       <c r="C139" s="66" t="s">
         <v>338</v>
@@ -9874,16 +9925,13 @@
         <v>339</v>
       </c>
       <c r="F139" s="66" t="s">
-        <v>464</v>
+        <v>426</v>
       </c>
       <c r="G139" s="66" t="s">
-        <v>460</v>
+        <v>428</v>
       </c>
       <c r="H139" s="67" t="s">
-        <v>461</v>
-      </c>
-      <c r="I139" s="73" t="s">
-        <v>11</v>
+        <v>427</v>
       </c>
       <c r="J139" s="66" t="s">
         <v>402</v>
@@ -9892,13 +9940,13 @@
         <v>416</v>
       </c>
       <c r="L139" s="67" t="s">
-        <v>110</v>
+        <v>42</v>
       </c>
       <c r="M139" s="66" t="s">
-        <v>465</v>
+        <v>433</v>
       </c>
       <c r="N139" s="66">
-        <v>19.57</v>
+        <v>18.420000000000002</v>
       </c>
       <c r="O139" s="68" t="s">
         <v>109</v>
@@ -9921,7 +9969,249 @@
       <c r="U139" s="69">
         <v>72</v>
       </c>
-      <c r="V139" s="66" t="s">
+    </row>
+    <row r="140" spans="1:22" s="66" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A140" s="66">
+        <v>2050</v>
+      </c>
+      <c r="B140" s="66" t="s">
+        <v>448</v>
+      </c>
+      <c r="C140" s="66" t="s">
+        <v>338</v>
+      </c>
+      <c r="D140" s="66" t="s">
+        <v>339</v>
+      </c>
+      <c r="F140" s="66" t="s">
+        <v>446</v>
+      </c>
+      <c r="G140" s="66" t="s">
+        <v>445</v>
+      </c>
+      <c r="H140" s="67" t="s">
+        <v>444</v>
+      </c>
+      <c r="J140" s="66" t="s">
+        <v>402</v>
+      </c>
+      <c r="K140" s="66" t="s">
+        <v>416</v>
+      </c>
+      <c r="L140" s="67" t="s">
+        <v>42</v>
+      </c>
+      <c r="M140" s="66" t="s">
+        <v>450</v>
+      </c>
+      <c r="N140" s="66">
+        <v>18.420000000000002</v>
+      </c>
+      <c r="O140" s="68" t="s">
+        <v>109</v>
+      </c>
+      <c r="P140" s="68" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q140" s="66">
+        <v>0.87</v>
+      </c>
+      <c r="R140" s="66">
+        <v>0.78</v>
+      </c>
+      <c r="S140" s="69">
+        <v>83.3</v>
+      </c>
+      <c r="T140" s="69">
+        <v>0</v>
+      </c>
+      <c r="U140" s="69">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="141" spans="1:22" s="66" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A141" s="66">
+        <v>2050</v>
+      </c>
+      <c r="B141" s="66" t="s">
+        <v>449</v>
+      </c>
+      <c r="C141" s="66" t="s">
+        <v>338</v>
+      </c>
+      <c r="D141" s="66" t="s">
+        <v>339</v>
+      </c>
+      <c r="F141" s="66" t="s">
+        <v>447</v>
+      </c>
+      <c r="G141" s="66" t="s">
+        <v>445</v>
+      </c>
+      <c r="H141" s="67" t="s">
+        <v>444</v>
+      </c>
+      <c r="J141" s="66" t="s">
+        <v>402</v>
+      </c>
+      <c r="K141" s="66" t="s">
+        <v>416</v>
+      </c>
+      <c r="L141" s="67" t="s">
+        <v>42</v>
+      </c>
+      <c r="M141" s="66" t="s">
+        <v>440</v>
+      </c>
+      <c r="N141" s="66">
+        <v>19.57</v>
+      </c>
+      <c r="O141" s="68" t="s">
+        <v>109</v>
+      </c>
+      <c r="P141" s="68" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q141" s="66">
+        <v>0.87</v>
+      </c>
+      <c r="R141" s="66">
+        <v>0.78</v>
+      </c>
+      <c r="S141" s="69">
+        <v>83.3</v>
+      </c>
+      <c r="T141" s="69">
+        <v>0</v>
+      </c>
+      <c r="U141" s="69">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="142" spans="1:22" s="66" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A142" s="66">
+        <v>2050</v>
+      </c>
+      <c r="B142" s="66" t="s">
+        <v>463</v>
+      </c>
+      <c r="C142" s="66" t="s">
+        <v>338</v>
+      </c>
+      <c r="D142" s="66" t="s">
+        <v>339</v>
+      </c>
+      <c r="F142" s="66" t="s">
+        <v>464</v>
+      </c>
+      <c r="G142" s="66" t="s">
+        <v>460</v>
+      </c>
+      <c r="H142" s="67" t="s">
+        <v>461</v>
+      </c>
+      <c r="J142" s="66" t="s">
+        <v>402</v>
+      </c>
+      <c r="K142" s="66" t="s">
+        <v>416</v>
+      </c>
+      <c r="L142" s="67" t="s">
+        <v>110</v>
+      </c>
+      <c r="M142" s="66" t="s">
+        <v>465</v>
+      </c>
+      <c r="N142" s="66">
+        <v>19.57</v>
+      </c>
+      <c r="O142" s="68" t="s">
+        <v>109</v>
+      </c>
+      <c r="P142" s="68" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q142" s="66">
+        <v>0.87</v>
+      </c>
+      <c r="R142" s="66">
+        <v>0.78</v>
+      </c>
+      <c r="S142" s="69">
+        <v>83.3</v>
+      </c>
+      <c r="T142" s="69">
+        <v>0</v>
+      </c>
+      <c r="U142" s="69">
+        <v>72</v>
+      </c>
+      <c r="V142" s="66" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="143" spans="1:22" s="66" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A143" s="66">
+        <v>2050</v>
+      </c>
+      <c r="B143" s="66" t="s">
+        <v>493</v>
+      </c>
+      <c r="C143" s="66" t="s">
+        <v>338</v>
+      </c>
+      <c r="D143" s="66" t="s">
+        <v>339</v>
+      </c>
+      <c r="F143" s="66" t="s">
+        <v>481</v>
+      </c>
+      <c r="G143" s="66" t="s">
+        <v>482</v>
+      </c>
+      <c r="H143" s="67" t="s">
+        <v>483</v>
+      </c>
+      <c r="I143" s="73" t="s">
+        <v>11</v>
+      </c>
+      <c r="J143" s="66" t="s">
+        <v>402</v>
+      </c>
+      <c r="K143" s="66" t="s">
+        <v>416</v>
+      </c>
+      <c r="L143" s="67" t="s">
+        <v>110</v>
+      </c>
+      <c r="M143" s="66" t="s">
+        <v>494</v>
+      </c>
+      <c r="N143" s="66">
+        <v>19.57</v>
+      </c>
+      <c r="O143" s="68" t="s">
+        <v>109</v>
+      </c>
+      <c r="P143" s="68" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q143" s="66">
+        <v>0.87</v>
+      </c>
+      <c r="R143" s="66">
+        <v>0.78</v>
+      </c>
+      <c r="S143" s="69">
+        <v>83.3</v>
+      </c>
+      <c r="T143" s="69">
+        <v>0</v>
+      </c>
+      <c r="U143" s="69">
+        <v>72</v>
+      </c>
+      <c r="V143" s="66" t="s">
         <v>358</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Leave previous DBP/Trend runs as current
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB8B2512-AE2E-498E-B8FB-F453364F88D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D7A6F83-003B-4D95-B6E2-CDBD6B16FA53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2190" yWindow="780" windowWidth="19335" windowHeight="11685" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1596" uniqueCount="495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1600" uniqueCount="495">
   <si>
     <t>year</t>
   </si>
@@ -2278,10 +2278,10 @@
   <dimension ref="A1:V143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C114" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C110" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M143" sqref="M143"/>
+      <selection pane="bottomRight" activeCell="I111" sqref="I111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8276,6 +8276,9 @@
       <c r="H111" s="56" t="s">
         <v>423</v>
       </c>
+      <c r="I111" s="74" t="s">
+        <v>11</v>
+      </c>
       <c r="J111" s="56" t="s">
         <v>402</v>
       </c>
@@ -8400,6 +8403,9 @@
       <c r="H113" s="83" t="s">
         <v>461</v>
       </c>
+      <c r="I113" s="74" t="s">
+        <v>11</v>
+      </c>
       <c r="K113" s="83" t="s">
         <v>404</v>
       </c>
@@ -9581,7 +9587,9 @@
       <c r="H133" s="90" t="s">
         <v>461</v>
       </c>
-      <c r="I133" s="89"/>
+      <c r="I133" s="73" t="s">
+        <v>11</v>
+      </c>
       <c r="J133" s="89"/>
       <c r="K133" s="89" t="s">
         <v>404</v>
@@ -10109,6 +10117,9 @@
       </c>
       <c r="H142" s="67" t="s">
         <v>461</v>
+      </c>
+      <c r="I142" s="73" t="s">
+        <v>11</v>
       </c>
       <c r="J142" s="66" t="s">
         <v>402</v>

</xml_diff>

<commit_message>
Move alias for 2023, 2035 IPA
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\config_RTP2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDB85F37-F986-456D-B9D0-FD5825AAE72E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E94E5B-E097-4991-A0B0-ED3E2C9177C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="1116" windowWidth="23412" windowHeight="15972" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
+    <workbookView xWindow="4575" yWindow="1515" windowWidth="33180" windowHeight="10770" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelRuns" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1602" uniqueCount="495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1601" uniqueCount="495">
   <si>
     <t>year</t>
   </si>
@@ -2278,33 +2278,33 @@
   <dimension ref="A1:V143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C107" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C119" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J122" sqref="J122"/>
+      <selection pane="bottomRight" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="7" style="1" customWidth="1"/>
-    <col min="5" max="5" width="7.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="42.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="42.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="23" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="6.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="22.33203125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11.33203125" style="10" customWidth="1"/>
-    <col min="13" max="13" width="17.5546875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="8.33203125" style="1" customWidth="1"/>
-    <col min="15" max="16" width="9.33203125" style="41"/>
-    <col min="17" max="16384" width="9.33203125" style="1"/>
+    <col min="8" max="8" width="8.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="6.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="22.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" style="10" customWidth="1"/>
+    <col min="13" max="13" width="17.5703125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="8.28515625" style="1" customWidth="1"/>
+    <col min="15" max="16" width="9.28515625" style="41"/>
+    <col min="17" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="5" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2372,7 +2372,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="2" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18">
         <v>2005</v>
       </c>
@@ -2425,7 +2425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:22" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="28">
         <v>2005</v>
       </c>
@@ -2481,7 +2481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:22" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="28">
         <v>2005</v>
       </c>
@@ -2533,7 +2533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:22" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="28">
         <v>2005</v>
       </c>
@@ -2585,7 +2585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:22" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="28">
         <v>2005</v>
       </c>
@@ -2650,7 +2650,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="7" spans="1:22" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" s="51" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="50">
         <v>2015</v>
       </c>
@@ -2691,7 +2691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:22" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="32">
         <v>2015</v>
       </c>
@@ -2737,7 +2737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:22" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="32">
         <v>2015</v>
       </c>
@@ -2790,7 +2790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:22" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="32">
         <v>2015</v>
       </c>
@@ -2843,7 +2843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:22" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="32">
         <v>2015</v>
       </c>
@@ -2896,7 +2896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:22" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="32">
         <v>2015</v>
       </c>
@@ -2952,7 +2952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:22" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="32">
         <v>2015</v>
       </c>
@@ -3008,7 +3008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:22" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="32">
         <v>2015</v>
       </c>
@@ -3064,7 +3064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:22" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="32">
         <v>2015</v>
       </c>
@@ -3121,7 +3121,7 @@
       </c>
       <c r="V15" s="55"/>
     </row>
-    <row r="16" spans="1:22" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="32">
         <v>2015</v>
       </c>
@@ -3183,7 +3183,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>2023</v>
       </c>
@@ -3229,7 +3229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>2023</v>
       </c>
@@ -3275,7 +3275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>2023</v>
       </c>
@@ -3321,7 +3321,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>2023</v>
       </c>
@@ -3367,7 +3367,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>2023</v>
       </c>
@@ -3413,7 +3413,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>2023</v>
       </c>
@@ -3459,7 +3459,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>2023</v>
       </c>
@@ -3505,7 +3505,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>2023</v>
       </c>
@@ -3551,7 +3551,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>2023</v>
       </c>
@@ -3597,7 +3597,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>2023</v>
       </c>
@@ -3643,7 +3643,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>2023</v>
       </c>
@@ -3689,7 +3689,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>2023</v>
       </c>
@@ -3735,7 +3735,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>2023</v>
       </c>
@@ -3781,7 +3781,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>2023</v>
       </c>
@@ -3827,7 +3827,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>2023</v>
       </c>
@@ -3873,7 +3873,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>2023</v>
       </c>
@@ -3919,7 +3919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>2023</v>
       </c>
@@ -3965,7 +3965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>2023</v>
       </c>
@@ -4011,7 +4011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>2023</v>
       </c>
@@ -4055,7 +4055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>2023</v>
       </c>
@@ -4104,7 +4104,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>2023</v>
       </c>
@@ -4151,7 +4151,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>2023</v>
       </c>
@@ -4198,7 +4198,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>2023</v>
       </c>
@@ -4254,7 +4254,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>2023</v>
       </c>
@@ -4310,7 +4310,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>2023</v>
       </c>
@@ -4366,7 +4366,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>2023</v>
       </c>
@@ -4422,7 +4422,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>2023</v>
       </c>
@@ -4478,7 +4478,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>2023</v>
       </c>
@@ -4534,7 +4534,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>2023</v>
       </c>
@@ -4590,7 +4590,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>2023</v>
       </c>
@@ -4646,7 +4646,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>2023</v>
       </c>
@@ -4702,7 +4702,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>2023</v>
       </c>
@@ -4758,7 +4758,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>2023</v>
       </c>
@@ -4814,7 +4814,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>2023</v>
       </c>
@@ -4870,7 +4870,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>2023</v>
       </c>
@@ -4926,7 +4926,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>2023</v>
       </c>
@@ -4982,7 +4982,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>2023</v>
       </c>
@@ -5038,7 +5038,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>2023</v>
       </c>
@@ -5094,7 +5094,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>2023</v>
       </c>
@@ -5150,7 +5150,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>2023</v>
       </c>
@@ -5206,7 +5206,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>2023</v>
       </c>
@@ -5262,7 +5262,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>2023</v>
       </c>
@@ -5318,7 +5318,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>2023</v>
       </c>
@@ -5374,7 +5374,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>2023</v>
       </c>
@@ -5430,7 +5430,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>2023</v>
       </c>
@@ -5486,7 +5486,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>2023</v>
       </c>
@@ -5542,7 +5542,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>2023</v>
       </c>
@@ -5598,7 +5598,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>2023</v>
       </c>
@@ -5657,7 +5657,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>2023</v>
       </c>
@@ -5713,7 +5713,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>2023</v>
       </c>
@@ -5772,7 +5772,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>2023</v>
       </c>
@@ -5831,7 +5831,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>2023</v>
       </c>
@@ -5890,7 +5890,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>2023</v>
       </c>
@@ -5949,7 +5949,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="70" spans="1:22" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:22" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>2023</v>
       </c>
@@ -6005,7 +6005,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="71" spans="1:22" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:22" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>2023</v>
       </c>
@@ -6061,7 +6061,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>2023</v>
       </c>
@@ -6117,7 +6117,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>2023</v>
       </c>
@@ -6173,7 +6173,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>2023</v>
       </c>
@@ -6229,7 +6229,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>2023</v>
       </c>
@@ -6288,7 +6288,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>2023</v>
       </c>
@@ -6346,9 +6346,11 @@
       <c r="U76" s="6">
         <v>72</v>
       </c>
-      <c r="V76" s="71"/>
-    </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V76" s="71" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="77" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>2023</v>
       </c>
@@ -6370,9 +6372,6 @@
       <c r="H77" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I77" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="K77" s="1" t="s">
         <v>291</v>
       </c>
@@ -6406,11 +6405,8 @@
       <c r="U77" s="6">
         <v>72</v>
       </c>
-      <c r="V77" s="71" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="78" spans="1:22" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="78" spans="1:22" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="25">
         <v>2025</v>
       </c>
@@ -6438,7 +6434,7 @@
       <c r="T78" s="27"/>
       <c r="U78" s="27"/>
     </row>
-    <row r="79" spans="1:22" s="75" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:22" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="75">
         <v>2035</v>
       </c>
@@ -6497,7 +6493,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="80" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="15">
         <v>2035</v>
       </c>
@@ -6556,7 +6552,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="81" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="12">
         <v>2035</v>
       </c>
@@ -6612,7 +6608,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="82" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="12">
         <v>2035</v>
       </c>
@@ -6668,7 +6664,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="83" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="12">
         <v>2035</v>
       </c>
@@ -6724,7 +6720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="12">
         <v>2035</v>
       </c>
@@ -6780,7 +6776,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="85" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="12">
         <v>2035</v>
       </c>
@@ -6836,7 +6832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="12">
         <v>2035</v>
       </c>
@@ -6892,7 +6888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="12">
         <v>2035</v>
       </c>
@@ -6948,7 +6944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A88" s="12">
         <v>2035</v>
       </c>
@@ -7004,7 +7000,7 @@
         <v>41.25</v>
       </c>
     </row>
-    <row r="89" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" s="12">
         <v>2035</v>
       </c>
@@ -7060,7 +7056,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="90" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A90" s="12">
         <v>2035</v>
       </c>
@@ -7116,7 +7112,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="91" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="12">
         <v>2035</v>
       </c>
@@ -7172,7 +7168,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="92" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="12">
         <v>2035</v>
       </c>
@@ -7228,7 +7224,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="93" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A93" s="12">
         <v>2035</v>
       </c>
@@ -7284,7 +7280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A94" s="12">
         <v>2035</v>
       </c>
@@ -7340,7 +7336,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="95" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A95" s="12">
         <v>2035</v>
       </c>
@@ -7396,7 +7392,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="96" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A96" s="12">
         <v>2035</v>
       </c>
@@ -7452,7 +7448,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="97" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A97" s="12">
         <v>2035</v>
       </c>
@@ -7508,7 +7504,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="98" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="12">
         <v>2035</v>
       </c>
@@ -7564,7 +7560,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="99" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A99" s="12">
         <v>2035</v>
       </c>
@@ -7620,7 +7616,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="100" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A100" s="12">
         <v>2035</v>
       </c>
@@ -7676,7 +7672,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="101" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A101" s="12">
         <v>2035</v>
       </c>
@@ -7732,7 +7728,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="102" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A102" s="12">
         <v>2035</v>
       </c>
@@ -7788,7 +7784,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="103" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A103" s="12">
         <v>2035</v>
       </c>
@@ -7849,8 +7845,11 @@
       <c r="U103" s="14">
         <v>75</v>
       </c>
-    </row>
-    <row r="104" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="V103" s="12" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="104" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A104" s="12">
         <v>2035</v>
       </c>
@@ -7906,7 +7905,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="105" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A105" s="12">
         <v>2035</v>
       </c>
@@ -7964,11 +7963,8 @@
       <c r="U105" s="14">
         <v>75</v>
       </c>
-      <c r="V105" s="12" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="106" spans="1:22" s="56" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="106" spans="1:22" s="56" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A106" s="56">
         <v>2035</v>
       </c>
@@ -8024,7 +8020,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="107" spans="1:22" s="56" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:22" s="56" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A107" s="56">
         <v>2035</v>
       </c>
@@ -8080,7 +8076,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="108" spans="1:22" s="56" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:22" s="56" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A108" s="56">
         <v>2035</v>
       </c>
@@ -8136,7 +8132,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="109" spans="1:22" s="56" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:22" s="56" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A109" s="56">
         <v>2035</v>
       </c>
@@ -8195,7 +8191,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="110" spans="1:22" s="56" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:22" s="56" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A110" s="56">
         <v>2035</v>
       </c>
@@ -8254,7 +8250,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="111" spans="1:22" s="56" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:22" s="56" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A111" s="56">
         <v>2035</v>
       </c>
@@ -8316,7 +8312,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="112" spans="1:22" s="56" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:22" s="56" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A112" s="56">
         <v>2035</v>
       </c>
@@ -8381,7 +8377,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="113" spans="1:22" s="83" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:22" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A113" s="83">
         <v>2035</v>
       </c>
@@ -8443,7 +8439,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="114" spans="1:22" s="83" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:22" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A114" s="83">
         <v>2035</v>
       </c>
@@ -8508,7 +8504,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="115" spans="1:22" s="60" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:22" s="60" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A115" s="60">
         <v>2035</v>
       </c>
@@ -8564,7 +8560,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="116" spans="1:22" s="60" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:22" s="60" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A116" s="60">
         <v>2035</v>
       </c>
@@ -8620,7 +8616,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="117" spans="1:22" s="60" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:22" s="60" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A117" s="60">
         <v>2035</v>
       </c>
@@ -8676,7 +8672,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="118" spans="1:22" s="60" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:22" s="60" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A118" s="60">
         <v>2035</v>
       </c>
@@ -8735,7 +8731,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="119" spans="1:22" s="60" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:22" s="60" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A119" s="60">
         <v>2035</v>
       </c>
@@ -8794,7 +8790,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="120" spans="1:22" s="60" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:22" s="60" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A120" s="60">
         <v>2035</v>
       </c>
@@ -8853,7 +8849,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="121" spans="1:22" s="60" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:22" s="60" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A121" s="60">
         <v>2035</v>
       </c>
@@ -8912,7 +8908,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="122" spans="1:22" s="60" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:22" s="60" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A122" s="60">
         <v>2035</v>
       </c>
@@ -8974,7 +8970,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="123" spans="1:22" s="60" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:22" s="60" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A123" s="60">
         <v>2035</v>
       </c>
@@ -9039,7 +9035,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="124" spans="1:22" s="79" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:22" s="79" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A124" s="79">
         <v>2050</v>
       </c>
@@ -9098,7 +9094,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="125" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A125" s="23">
         <v>2050</v>
       </c>
@@ -9157,7 +9153,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="126" spans="1:22" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:22" s="51" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A126" s="51">
         <v>2050</v>
       </c>
@@ -9213,7 +9209,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="127" spans="1:22" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:22" s="51" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A127" s="51">
         <v>2050</v>
       </c>
@@ -9269,7 +9265,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="128" spans="1:22" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:22" s="51" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A128" s="51">
         <v>2050</v>
       </c>
@@ -9325,7 +9321,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="129" spans="1:22" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:22" s="51" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A129" s="51">
         <v>2050</v>
       </c>
@@ -9384,7 +9380,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="130" spans="1:22" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:22" s="51" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A130" s="51">
         <v>2050</v>
       </c>
@@ -9443,7 +9439,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="131" spans="1:22" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:22" s="51" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A131" s="51">
         <v>2050</v>
       </c>
@@ -9502,7 +9498,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="132" spans="1:22" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:22" s="51" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A132" s="51">
         <v>2050</v>
       </c>
@@ -9567,7 +9563,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="133" spans="1:22" s="88" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:22" s="88" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A133" s="89">
         <v>2050</v>
       </c>
@@ -9631,7 +9627,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="134" spans="1:22" s="88" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:22" s="88" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A134" s="89">
         <v>2050</v>
       </c>
@@ -9697,7 +9693,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="135" spans="1:22" s="66" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:22" s="66" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A135" s="66">
         <v>2050</v>
       </c>
@@ -9753,7 +9749,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="136" spans="1:22" s="66" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:22" s="66" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A136" s="66">
         <v>2050</v>
       </c>
@@ -9809,7 +9805,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="137" spans="1:22" s="66" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:22" s="66" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A137" s="66">
         <v>2050</v>
       </c>
@@ -9865,7 +9861,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="138" spans="1:22" s="66" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:22" s="66" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A138" s="66">
         <v>2050</v>
       </c>
@@ -9924,7 +9920,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="139" spans="1:22" s="66" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:22" s="66" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A139" s="66">
         <v>2050</v>
       </c>
@@ -9983,7 +9979,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="140" spans="1:22" s="66" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:22" s="66" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A140" s="66">
         <v>2050</v>
       </c>
@@ -10042,7 +10038,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="141" spans="1:22" s="66" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:22" s="66" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A141" s="66">
         <v>2050</v>
       </c>
@@ -10101,7 +10097,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="142" spans="1:22" s="66" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:22" s="66" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A142" s="66">
         <v>2050</v>
       </c>
@@ -10166,7 +10162,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="143" spans="1:22" s="66" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:22" s="66" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A143" s="66">
         <v>2050</v>
       </c>

</xml_diff>

<commit_message>
Add [2035,2050]_TM160_DBP_Plan_08b_[ZeroTrnHes, PBA50network, PBA50lupop]
</commit_message>
<xml_diff>
--- a/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
+++ b/utilities/RTP/config_RTP2025/ModelRuns_RTP2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\travel-model-one\utilities\RTP\config_RTP2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC82010-8836-41BC-8B3C-1AB5E65FF4E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6BD8C48-0C2A-4EDD-BE8C-7A4C9E11CA78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5565" yWindow="2595" windowWidth="28800" windowHeight="15435" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
+    <workbookView xWindow="9900" yWindow="2550" windowWidth="28170" windowHeight="17310" xr2:uid="{1F9DB3D6-6479-4470-B3F5-B9ED0E0652FB}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelRuns" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1591" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1661" uniqueCount="499">
   <si>
     <t>year</t>
   </si>
@@ -1521,6 +1521,36 @@
   </si>
   <si>
     <t>https://app.asana.com/0/1182463234225195/1207227169631494/f</t>
+  </si>
+  <si>
+    <t>2035_TM160_DBP_Plan_08b_ZeroTrnHes</t>
+  </si>
+  <si>
+    <t>2035_TM160_DBP_Plan_08b_PBA50network</t>
+  </si>
+  <si>
+    <t>2035_TM160_DBP_Plan_08b_PBA50lupop</t>
+  </si>
+  <si>
+    <t>DBP run with zero transit hesitancy</t>
+  </si>
+  <si>
+    <t>DBP run with PBA50 network</t>
+  </si>
+  <si>
+    <t>DBP run with PBA50 landuse/pop</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/0/1207403425432857/f</t>
+  </si>
+  <si>
+    <t>2050_TM160_DBP_Plan_08b_ZeroTrnHes</t>
+  </si>
+  <si>
+    <t>2050_TM160_DBP_Plan_08b_PBA50network</t>
+  </si>
+  <si>
+    <t>2050_TM160_DBP_Plan_08b_PBA50lupop</t>
   </si>
 </sst>
 </file>
@@ -1736,7 +1766,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1928,6 +1958,13 @@
     <xf numFmtId="2" fontId="9" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2257,19 +2294,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9564CC59-3725-4FDA-8BF2-0F68CB1B6F5A}">
-  <dimension ref="A1:V143"/>
+  <dimension ref="A1:V149"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F104" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G106" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I143" sqref="I143"/>
+      <selection pane="bottomRight" activeCell="S148" sqref="S148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="37.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="7" style="1" customWidth="1"/>
     <col min="5" max="5" width="7.85546875" style="1" customWidth="1"/>
@@ -9002,290 +9039,293 @@
         <v>359</v>
       </c>
     </row>
-    <row r="124" spans="1:22" s="79" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="79">
-        <v>2050</v>
-      </c>
-      <c r="B124" s="79" t="s">
-        <v>469</v>
-      </c>
-      <c r="C124" s="79" t="s">
-        <v>113</v>
-      </c>
-      <c r="D124" s="79" t="s">
-        <v>244</v>
-      </c>
-      <c r="F124" s="79" t="s">
-        <v>465</v>
-      </c>
-      <c r="G124" s="79" t="s">
-        <v>466</v>
-      </c>
-      <c r="H124" s="80" t="s">
-        <v>467</v>
+    <row r="124" spans="1:22" s="60" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="60">
+        <v>2035</v>
+      </c>
+      <c r="B124" s="60" t="s">
+        <v>489</v>
+      </c>
+      <c r="C124" s="61" t="s">
+        <v>338</v>
+      </c>
+      <c r="D124" s="60" t="s">
+        <v>339</v>
+      </c>
+      <c r="F124" s="60" t="s">
+        <v>492</v>
+      </c>
+      <c r="G124" s="60" t="s">
+        <v>480</v>
       </c>
       <c r="I124" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="K124" s="79" t="s">
-        <v>470</v>
-      </c>
-      <c r="L124" s="80" t="s">
-        <v>110</v>
-      </c>
-      <c r="M124" s="79" t="s">
-        <v>109</v>
-      </c>
-      <c r="N124" s="79">
-        <v>17.440000000000001</v>
-      </c>
-      <c r="O124" s="81">
-        <v>-0.33</v>
-      </c>
-      <c r="P124" s="81">
-        <v>0</v>
-      </c>
-      <c r="Q124" s="81" t="s">
-        <v>109</v>
-      </c>
-      <c r="R124" s="81" t="s">
-        <v>109</v>
-      </c>
-      <c r="S124" s="82" t="s">
-        <v>109</v>
-      </c>
-      <c r="T124" s="82" t="s">
-        <v>109</v>
-      </c>
-      <c r="U124" s="82" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="125" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="23">
-        <v>2050</v>
-      </c>
-      <c r="B125" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r=